<commit_message>
- extracted data from `10.1016/j.intermet.2023.108089`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B918FF2-DEF2-BA42-9865-F28472CCD823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E514E45-0525-334B-9B7B-B252AF329243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="760" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2260" yWindow="10480" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="82">
   <si>
     <t>Metadata</t>
   </si>
@@ -317,6 +317,63 @@
   </si>
   <si>
     <t>Col5</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>hardness</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>BM+CIP+S</t>
+  </si>
+  <si>
+    <t>Al25 Li25 Mg12.5 Ti37.5</t>
+  </si>
+  <si>
+    <t>(Al25 Li25 Mg12.5 Ti37.5)0.8 Sc20</t>
+  </si>
+  <si>
+    <t>(Al25 Li25 Mg12.5 Ti37.5)0.95 Sc5</t>
+  </si>
+  <si>
+    <t>(Al25 Li25 Mg12.5 Ti37.5)0.9 Sc10</t>
+  </si>
+  <si>
+    <t>(Al25 Li25 Mg12.5 Ti37.5)0.9 Sc15</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2023.108089</t>
+  </si>
+  <si>
+    <t>D024+L10+gamma</t>
+  </si>
+  <si>
+    <t>HCP+gamma</t>
+  </si>
+  <si>
+    <t>C15+D024+L10+gamma</t>
+  </si>
+  <si>
+    <t>C15+D024+L10+gamma+HCP</t>
+  </si>
+  <si>
+    <t>D024+L10+gamma+HCP</t>
+  </si>
+  <si>
+    <t>ball milled with steel balls for 30h then cold pressed at 2GPa for 2min and sintered at 550*C for 2h and slowly cooled; D024 is β-AlTi3; L10 is α-AlTi; gamma is Al12Mg17; C15 is Al2Sc</t>
+  </si>
+  <si>
+    <t>ball milled with steel balls for 30h then cold pressed at 2GPa for 2min and sintered at 650*C for 2h and slowly cooled; D024 is β-AlTi3; L10 is α-AlTi; gamma is Al12Mg17; C15 is Al2Sc</t>
   </si>
 </sst>
 </file>
@@ -1649,8 +1706,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1970,254 +2027,722 @@
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="24"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="B10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="4"/>
+      <c r="I10" s="43">
+        <v>298</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2790</v>
+      </c>
       <c r="K10" s="4"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="9"/>
+      <c r="L10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="24"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="B11" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="4"/>
+      <c r="I11" s="43">
+        <v>298</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2820</v>
+      </c>
       <c r="K11" s="4"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="9"/>
+      <c r="L11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="24"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="B12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="4"/>
+      <c r="I12" s="43">
+        <v>298</v>
+      </c>
+      <c r="J12" s="4">
+        <v>2770</v>
+      </c>
       <c r="K12" s="4"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="9"/>
+      <c r="L12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="24"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="B13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="4"/>
+      <c r="I13" s="43">
+        <v>298</v>
+      </c>
+      <c r="J13" s="4">
+        <v>2650</v>
+      </c>
       <c r="K13" s="4"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="9"/>
+      <c r="L13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="24"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="B14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="4"/>
+      <c r="I14" s="43">
+        <v>298</v>
+      </c>
+      <c r="J14" s="4">
+        <v>2880</v>
+      </c>
       <c r="K14" s="4"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="9"/>
+      <c r="L14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="24"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="42"/>
+      <c r="I15" s="43">
+        <v>298</v>
+      </c>
+      <c r="J15" s="4">
+        <f>P15*9807000</f>
+        <v>1772854205.6074688</v>
+      </c>
+      <c r="K15" s="4">
+        <f>R15*9807000</f>
+        <v>73323364.485984281</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="O15" s="44"/>
+      <c r="P15" s="6">
+        <v>180.77436582109399</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>188.25100133511299</v>
+      </c>
+      <c r="R15" s="6">
+        <f>Q15-P15</f>
+        <v>7.4766355140189944</v>
+      </c>
     </row>
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="24"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="9"/>
+      <c r="B16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="42"/>
+      <c r="I16" s="43">
+        <v>298</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" ref="J16:J24" si="0">P16*9807000</f>
+        <v>1919500934.5794377</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" ref="K16:K24" si="1">R16*9807000</f>
+        <v>73323364.48597452</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="O16" s="44"/>
-    </row>
-    <row r="17" spans="1:17" ht="18.75" customHeight="1">
+      <c r="P16" s="6">
+        <v>195.72763684913201</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>203.20427236315001</v>
+      </c>
+      <c r="R16" s="6">
+        <f t="shared" ref="R16:R24" si="2">Q16-P16</f>
+        <v>7.4766355140179996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="18.75" customHeight="1">
       <c r="A17" s="24"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="9"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
-    </row>
-    <row r="18" spans="1:17" ht="18.75" customHeight="1">
+      <c r="B17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="42"/>
+      <c r="I17" s="43">
+        <v>298</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="0"/>
+        <v>2186607476.6355085</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="1"/>
+        <v>109985046.72897168</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P17" s="46">
+        <v>222.963951935914</v>
+      </c>
+      <c r="Q17" s="46">
+        <v>234.17890520694201</v>
+      </c>
+      <c r="R17" s="6">
+        <f t="shared" si="2"/>
+        <v>11.214953271028008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="18.75" customHeight="1">
       <c r="A18" s="24"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="B18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="1:17" ht="18.75" customHeight="1">
+      <c r="I18" s="43">
+        <v>298</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="0"/>
+        <v>2328016822.4299021</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="1"/>
+        <v>151884112.14953405</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P18" s="6">
+        <v>237.38317757009301</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>252.87049399198901</v>
+      </c>
+      <c r="R18" s="6">
+        <f t="shared" si="2"/>
+        <v>15.487316421895997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="18.75" customHeight="1">
       <c r="A19" s="24"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="9"/>
-    </row>
-    <row r="20" spans="1:17" ht="18.75" customHeight="1">
+      <c r="B19" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="43">
+        <v>298</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="0"/>
+        <v>3726398130.8411212</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="1"/>
+        <v>83798130.8411147</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P19" s="6">
+        <v>379.97329773030702</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>388.51802403204198</v>
+      </c>
+      <c r="R19" s="6">
+        <f t="shared" si="2"/>
+        <v>8.5447263017349542</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="18.75" customHeight="1">
       <c r="A20" s="24"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="B20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="9"/>
-    </row>
-    <row r="21" spans="1:17" ht="18.75" customHeight="1">
+      <c r="I20" s="43">
+        <v>298</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="0"/>
+        <v>2747007476.6355071</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" si="1"/>
+        <v>115222429.90654664</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P20" s="6">
+        <v>280.10680907877099</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>291.85580774365798</v>
+      </c>
+      <c r="R20" s="6">
+        <f t="shared" si="2"/>
+        <v>11.748998664886983</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="18.75" customHeight="1">
       <c r="A21" s="24"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="B21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H21" s="42"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="9"/>
-    </row>
-    <row r="22" spans="1:17" ht="18.75" customHeight="1">
+      <c r="I21" s="43">
+        <v>298</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="0"/>
+        <v>2930315887.8504634</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="1"/>
+        <v>120459813.08411185</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P21" s="6">
+        <v>298.79839786381802</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>311.08144192256299</v>
+      </c>
+      <c r="R21" s="6">
+        <f t="shared" si="2"/>
+        <v>12.283044058744963</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="18.75" customHeight="1">
       <c r="A22" s="24"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="B22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H22" s="42"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="9"/>
-    </row>
-    <row r="23" spans="1:17" ht="18.75" customHeight="1">
+      <c r="I22" s="43">
+        <v>298</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="0"/>
+        <v>3008876635.5140128</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="1"/>
+        <v>115222429.90654664</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P22" s="6">
+        <v>306.809078771695</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>318.55807743658198</v>
+      </c>
+      <c r="R22" s="6">
+        <f t="shared" si="2"/>
+        <v>11.748998664886983</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="18.75" customHeight="1">
       <c r="A23" s="24"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="B23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H23" s="42"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="9"/>
-    </row>
-    <row r="24" spans="1:17" ht="18.75" customHeight="1">
+      <c r="I23" s="43">
+        <v>298</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="0"/>
+        <v>3160760747.663547</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" si="1"/>
+        <v>109985046.72897141</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P23" s="6">
+        <v>322.29639519359102</v>
+      </c>
+      <c r="Q23" s="6">
+        <v>333.511348464619</v>
+      </c>
+      <c r="R23" s="6">
+        <f t="shared" si="2"/>
+        <v>11.21495327102798</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="18.75" customHeight="1">
       <c r="A24" s="24"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="9"/>
-    </row>
-    <row r="25" spans="1:17" ht="18.75" customHeight="1">
+      <c r="B24" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="43">
+        <v>298</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="0"/>
+        <v>5779452336.4485941</v>
+      </c>
+      <c r="K24" s="4">
+        <f t="shared" si="1"/>
+        <v>136171962.61681807</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="P24" s="6">
+        <v>589.31909212283006</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>603.20427236315004</v>
+      </c>
+      <c r="R24" s="6">
+        <f t="shared" si="2"/>
+        <v>13.885180240319983</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="18.75" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="9"/>
       <c r="C25" s="2"/>
@@ -2233,7 +2758,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="9"/>
     </row>
-    <row r="26" spans="1:17" ht="18.75" customHeight="1">
+    <row r="26" spans="1:18" ht="18.75" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="9"/>
       <c r="C26" s="2"/>
@@ -2249,7 +2774,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="9"/>
     </row>
-    <row r="27" spans="1:17" ht="18.75" customHeight="1">
+    <row r="27" spans="1:18" ht="18.75" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="9"/>
       <c r="C27" s="2"/>
@@ -2265,7 +2790,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="9"/>
     </row>
-    <row r="28" spans="1:17" ht="18.75" customHeight="1">
+    <row r="28" spans="1:18" ht="18.75" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="9"/>
       <c r="C28" s="2"/>
@@ -2281,7 +2806,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="9"/>
     </row>
-    <row r="29" spans="1:17" ht="18.75" customHeight="1">
+    <row r="29" spans="1:18" ht="18.75" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="9"/>
       <c r="C29" s="2"/>
@@ -2297,7 +2822,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="9"/>
     </row>
-    <row r="30" spans="1:17" ht="18.75" customHeight="1">
+    <row r="30" spans="1:18" ht="18.75" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="9"/>
       <c r="C30" s="2"/>
@@ -2313,7 +2838,7 @@
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
     </row>
-    <row r="31" spans="1:17" ht="18.75" customHeight="1">
+    <row r="31" spans="1:18" ht="18.75" customHeight="1">
       <c r="A31" s="24"/>
       <c r="B31" s="9"/>
       <c r="C31" s="2"/>
@@ -2329,7 +2854,7 @@
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
     </row>
-    <row r="32" spans="1:17" ht="18.75" customHeight="1">
+    <row r="32" spans="1:18" ht="18.75" customHeight="1">
       <c r="A32" s="24"/>
       <c r="B32" s="9"/>
       <c r="C32" s="2"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2021.161924`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E514E45-0525-334B-9B7B-B252AF329243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C786CEE8-F346-824B-9EFC-A90818426459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="10480" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="10860" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="97">
   <si>
     <t>Metadata</t>
   </si>
@@ -325,6 +325,33 @@
     <t>hardness</t>
   </si>
   <si>
+    <t>FCC</t>
+  </si>
+  <si>
+    <t>nanohardness</t>
+  </si>
+  <si>
+    <t>reduced elastic modulus</t>
+  </si>
+  <si>
+    <t>saturation magnetization</t>
+  </si>
+  <si>
+    <t>coercivity</t>
+  </si>
+  <si>
+    <t>A/m</t>
+  </si>
+  <si>
+    <t>FCC+BCC</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>BM+SPS</t>
+  </si>
+  <si>
     <t>kg/m^3</t>
   </si>
   <si>
@@ -332,6 +359,9 @@
   </si>
   <si>
     <t>F5</t>
+  </si>
+  <si>
+    <t>T6</t>
   </si>
   <si>
     <t>BM+CIP+S</t>
@@ -374,6 +404,21 @@
   </si>
   <si>
     <t>ball milled with steel balls for 30h then cold pressed at 2GPa for 2min and sintered at 650*C for 2h and slowly cooled; D024 is β-AlTi3; L10 is α-AlTi; gamma is Al12Mg17; C15 is Al2Sc</t>
+  </si>
+  <si>
+    <t>NiCoCrFe</t>
+  </si>
+  <si>
+    <t>NiCoCrFeZr0.4</t>
+  </si>
+  <si>
+    <t>milled untill SS and SPSed at 1173K for 45min under 45MPa</t>
+  </si>
+  <si>
+    <t>Am^2/kg</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2021.161924</t>
   </si>
 </sst>
 </file>
@@ -1706,8 +1751,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="75" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2028,16 +2073,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="9" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>63</v>
@@ -2054,29 +2099,29 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="9" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>63</v>
@@ -2093,29 +2138,29 @@
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="9" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>63</v>
@@ -2132,29 +2177,29 @@
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>63</v>
@@ -2171,29 +2216,29 @@
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>63</v>
@@ -2210,29 +2255,29 @@
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="9" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>64</v>
@@ -2256,10 +2301,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="6">
@@ -2276,16 +2321,16 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="9" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>64</v>
@@ -2298,21 +2343,21 @@
         <v>298</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" ref="J16:J24" si="0">P16*9807000</f>
+        <f t="shared" ref="J16:J28" si="0">P16*9807000</f>
         <v>1919500934.5794377</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" ref="K16:K24" si="1">R16*9807000</f>
+        <f t="shared" ref="K16:K28" si="1">R16*9807000</f>
         <v>73323364.48597452</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="O16" s="44"/>
       <c r="P16" s="6">
@@ -2329,16 +2374,16 @@
     <row r="17" spans="1:18" ht="18.75" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="9" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>64</v>
@@ -2362,10 +2407,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="P17" s="46">
         <v>222.963951935914</v>
@@ -2381,16 +2426,16 @@
     <row r="18" spans="1:18" ht="18.75" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>64</v>
@@ -2414,10 +2459,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="P18" s="6">
         <v>237.38317757009301</v>
@@ -2433,16 +2478,16 @@
     <row r="19" spans="1:18" ht="18.75" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="9" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>64</v>
@@ -2466,10 +2511,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="P19" s="6">
         <v>379.97329773030702</v>
@@ -2485,16 +2530,16 @@
     <row r="20" spans="1:18" ht="18.75" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>64</v>
@@ -2518,10 +2563,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="P20" s="6">
         <v>280.10680907877099</v>
@@ -2537,16 +2582,16 @@
     <row r="21" spans="1:18" ht="18.75" customHeight="1">
       <c r="A21" s="24"/>
       <c r="B21" s="9" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>64</v>
@@ -2570,10 +2615,10 @@
         <v>33</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="P21" s="6">
         <v>298.79839786381802</v>
@@ -2589,16 +2634,16 @@
     <row r="22" spans="1:18" ht="18.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>64</v>
@@ -2622,10 +2667,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="P22" s="6">
         <v>306.809078771695</v>
@@ -2641,16 +2686,16 @@
     <row r="23" spans="1:18" ht="18.75" customHeight="1">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>64</v>
@@ -2674,10 +2719,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="P23" s="6">
         <v>322.29639519359102</v>
@@ -2693,16 +2738,16 @@
     <row r="24" spans="1:18" ht="18.75" customHeight="1">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>64</v>
@@ -2726,10 +2771,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="P24" s="6">
         <v>589.31909212283006</v>
@@ -2744,163 +2789,425 @@
     </row>
     <row r="25" spans="1:18" ht="18.75" customHeight="1">
       <c r="A25" s="24"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="B25" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H25" s="42"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="9"/>
+      <c r="I25" s="43">
+        <v>298</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="0"/>
+        <v>6099954000</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="1"/>
+        <v>68649000</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="P25" s="6">
+        <v>622</v>
+      </c>
+      <c r="R25">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:18" ht="18.75" customHeight="1">
       <c r="A26" s="24"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="B26" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H26" s="42"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="9"/>
+      <c r="I26" s="43">
+        <v>298</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" si="0"/>
+        <v>8120196000</v>
+      </c>
+      <c r="K26" s="4">
+        <f t="shared" si="1"/>
+        <v>98070000</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="P26" s="6">
+        <v>828</v>
+      </c>
+      <c r="R26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:18" ht="18.75" customHeight="1">
       <c r="A27" s="24"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="9"/>
+      <c r="B27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="43">
+        <v>298</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="0"/>
+        <v>6590304000</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" si="1"/>
+        <v>68649000</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N27" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="P27" s="6">
+        <v>672</v>
+      </c>
+      <c r="R27">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="1:18" ht="18.75" customHeight="1">
       <c r="A28" s="24"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="B28" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H28" s="42"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="9"/>
+      <c r="I28" s="43">
+        <v>298</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="0"/>
+        <v>8286915000</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="1"/>
+        <v>98070000</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N28" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="P28" s="6">
+        <v>845</v>
+      </c>
+      <c r="R28">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="1:18" ht="18.75" customHeight="1">
       <c r="A29" s="24"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="B29" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H29" s="42"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="4"/>
+      <c r="I29" s="43">
+        <v>298</v>
+      </c>
+      <c r="J29" s="4">
+        <v>181500000000</v>
+      </c>
       <c r="K29" s="4"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="9"/>
+      <c r="L29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N29" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="30" spans="1:18" ht="18.75" customHeight="1">
       <c r="A30" s="24"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="B30" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H30" s="42"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="4"/>
+      <c r="I30" s="43">
+        <v>298</v>
+      </c>
+      <c r="J30" s="4">
+        <v>189600000000</v>
+      </c>
       <c r="K30" s="4"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
+      <c r="L30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N30" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="31" spans="1:18" ht="18.75" customHeight="1">
       <c r="A31" s="24"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="B31" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H31" s="42"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="4"/>
+      <c r="I31" s="43">
+        <v>298</v>
+      </c>
+      <c r="J31" s="4">
+        <v>83</v>
+      </c>
       <c r="K31" s="4"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
+      <c r="L31" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N31" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="32" spans="1:18" ht="18.75" customHeight="1">
       <c r="A32" s="24"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="B32" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H32" s="42"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="4"/>
+      <c r="I32" s="43">
+        <v>298</v>
+      </c>
+      <c r="J32" s="4">
+        <v>70</v>
+      </c>
       <c r="K32" s="4"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
+      <c r="L32" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N32" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="33" spans="1:14" ht="18.75" customHeight="1">
       <c r="A33" s="24"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="B33" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H33" s="42"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="4"/>
+      <c r="I33" s="43">
+        <v>298</v>
+      </c>
+      <c r="J33" s="4">
+        <f>79.577472*9</f>
+        <v>716.19724799999995</v>
+      </c>
       <c r="K33" s="4"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
+      <c r="L33" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M33" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N33" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="34" spans="1:14" ht="18.75" customHeight="1">
       <c r="A34" s="24"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="B34" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H34" s="42"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="4"/>
+      <c r="I34" s="43">
+        <v>298</v>
+      </c>
+      <c r="J34" s="4">
+        <f>79.577472*21</f>
+        <v>1671.1269119999999</v>
+      </c>
       <c r="K34" s="4"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
+      <c r="L34" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N34" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="35" spans="1:14" ht="18.75" customHeight="1">
       <c r="A35" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s12613-019-1771-3`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C786CEE8-F346-824B-9EFC-A90818426459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1079CF75-AB3B-D54A-8E2F-88235D00DEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="10860" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="101">
   <si>
     <t>Metadata</t>
   </si>
@@ -419,6 +419,18 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2021.161924</t>
+  </si>
+  <si>
+    <t>AlCoCrCuFeNiTi</t>
+  </si>
+  <si>
+    <t>milled for 10h then pressed under 1.5GPa and sintered in vacuum at 1473K for 3h</t>
+  </si>
+  <si>
+    <t>FCC+FCC+BCC+B2+sigma</t>
+  </si>
+  <si>
+    <t>10.1007/s12613-019-1771-3</t>
   </si>
 </sst>
 </file>
@@ -1751,8 +1763,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3131,7 +3143,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="18.75" customHeight="1">
+    <row r="33" spans="1:17" ht="18.75" customHeight="1">
       <c r="A33" s="24"/>
       <c r="B33" s="9" t="s">
         <v>92</v>
@@ -3170,7 +3182,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="18.75" customHeight="1">
+    <row r="34" spans="1:17" ht="18.75" customHeight="1">
       <c r="A34" s="24"/>
       <c r="B34" s="9" t="s">
         <v>93</v>
@@ -3209,23 +3221,53 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18.75" customHeight="1">
+    <row r="35" spans="1:17" ht="18.75" customHeight="1">
       <c r="A35" s="24"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="B35" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H35" s="42"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="9"/>
+      <c r="I35" s="43">
+        <v>298</v>
+      </c>
+      <c r="J35" s="4">
+        <f t="shared" ref="J35:K35" si="3">P35*9807000</f>
+        <v>5903814000</v>
+      </c>
+      <c r="K35" s="4">
+        <f t="shared" si="3"/>
+        <v>431508000</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-    </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1">
+      <c r="N35" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="P35" s="6">
+        <v>602</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="18.75" customHeight="1">
       <c r="A36" s="24"/>
       <c r="B36" s="9"/>
       <c r="C36" s="2"/>
@@ -3241,7 +3283,7 @@
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
     </row>
-    <row r="37" spans="1:14" ht="18.75" customHeight="1">
+    <row r="37" spans="1:17" ht="18.75" customHeight="1">
       <c r="A37" s="24"/>
       <c r="B37" s="9"/>
       <c r="C37" s="2"/>
@@ -3257,7 +3299,7 @@
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
     </row>
-    <row r="38" spans="1:14" ht="18.75" customHeight="1">
+    <row r="38" spans="1:17" ht="18.75" customHeight="1">
       <c r="A38" s="24"/>
       <c r="B38" s="9"/>
       <c r="C38" s="2"/>
@@ -3273,7 +3315,7 @@
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1">
+    <row r="39" spans="1:17" ht="18.75" customHeight="1">
       <c r="A39" s="24"/>
       <c r="B39" s="44"/>
       <c r="C39" s="42"/>
@@ -3288,7 +3330,7 @@
       <c r="M39" s="44"/>
       <c r="N39" s="44"/>
     </row>
-    <row r="40" spans="1:14" ht="18.75" customHeight="1">
+    <row r="40" spans="1:17" ht="18.75" customHeight="1">
       <c r="A40" s="24"/>
       <c r="B40" s="44"/>
       <c r="C40" s="42"/>
@@ -3302,7 +3344,7 @@
       <c r="M40" s="44"/>
       <c r="N40" s="44"/>
     </row>
-    <row r="41" spans="1:14" ht="18.75" customHeight="1">
+    <row r="41" spans="1:17" ht="18.75" customHeight="1">
       <c r="A41" s="24"/>
       <c r="B41" s="44"/>
       <c r="C41" s="42"/>
@@ -3316,7 +3358,7 @@
       <c r="M41" s="44"/>
       <c r="N41" s="44"/>
     </row>
-    <row r="42" spans="1:14" ht="18.75" customHeight="1">
+    <row r="42" spans="1:17" ht="18.75" customHeight="1">
       <c r="A42" s="24"/>
       <c r="B42" s="44"/>
       <c r="C42" s="42"/>
@@ -3330,7 +3372,7 @@
       <c r="M42" s="44"/>
       <c r="N42" s="44"/>
     </row>
-    <row r="43" spans="1:14" ht="18" customHeight="1">
+    <row r="43" spans="1:17" ht="18" customHeight="1">
       <c r="A43" s="24"/>
       <c r="B43" s="44"/>
       <c r="C43" s="42"/>
@@ -3344,7 +3386,7 @@
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
     </row>
-    <row r="44" spans="1:14" ht="18" customHeight="1">
+    <row r="44" spans="1:17" ht="18" customHeight="1">
       <c r="A44" s="24"/>
       <c r="B44" s="44"/>
       <c r="C44" s="42"/>
@@ -3359,7 +3401,7 @@
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
     </row>
-    <row r="45" spans="1:14" ht="18" customHeight="1">
+    <row r="45" spans="1:17" ht="18" customHeight="1">
       <c r="A45" s="24"/>
       <c r="B45" s="44"/>
       <c r="C45" s="42"/>
@@ -3374,7 +3416,7 @@
       <c r="M45" s="44"/>
       <c r="N45" s="44"/>
     </row>
-    <row r="46" spans="1:14" ht="18" customHeight="1">
+    <row r="46" spans="1:17" ht="18" customHeight="1">
       <c r="A46" s="24"/>
       <c r="B46" s="44"/>
       <c r="C46" s="42"/>
@@ -3389,7 +3431,7 @@
       <c r="M46" s="44"/>
       <c r="N46" s="44"/>
     </row>
-    <row r="47" spans="1:14" ht="18" customHeight="1">
+    <row r="47" spans="1:17" ht="18" customHeight="1">
       <c r="A47" s="24"/>
       <c r="B47" s="44"/>
       <c r="C47" s="42"/>
@@ -3404,7 +3446,7 @@
       <c r="M47" s="44"/>
       <c r="N47" s="44"/>
     </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1">
+    <row r="48" spans="1:17" ht="18" customHeight="1">
       <c r="A48" s="24"/>
       <c r="B48" s="44"/>
       <c r="C48" s="42"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.actamat.2016.11.046`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1079CF75-AB3B-D54A-8E2F-88235D00DEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D5B46B-824D-E643-B7D9-49F32BD289E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="10860" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="5360" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="112">
   <si>
     <t>Metadata</t>
   </si>
@@ -343,6 +343,9 @@
     <t>A/m</t>
   </si>
   <si>
+    <t>F10</t>
+  </si>
+  <si>
     <t>FCC+BCC</t>
   </si>
   <si>
@@ -362,6 +365,9 @@
   </si>
   <si>
     <t>T6</t>
+  </si>
+  <si>
+    <t>F11</t>
   </si>
   <si>
     <t>BM+CIP+S</t>
@@ -431,6 +437,33 @@
   </si>
   <si>
     <t>10.1007/s12613-019-1771-3</t>
+  </si>
+  <si>
+    <t>AlCoCrCuFeNi</t>
+  </si>
+  <si>
+    <t>milled for 60h then SPS at 1023K under 80MPa for 15min</t>
+  </si>
+  <si>
+    <t>vickers load 100g</t>
+  </si>
+  <si>
+    <t>vickers load 300g</t>
+  </si>
+  <si>
+    <t>vickers load 500g</t>
+  </si>
+  <si>
+    <t>peak load 1mN</t>
+  </si>
+  <si>
+    <t>peak load 8mN</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2016.11.046</t>
+  </si>
+  <si>
+    <t>FCC+B2</t>
   </si>
 </sst>
 </file>
@@ -1763,8 +1796,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2085,16 +2118,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>63</v>
@@ -2111,29 +2144,29 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>63</v>
@@ -2150,29 +2183,29 @@
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>63</v>
@@ -2189,29 +2222,29 @@
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>63</v>
@@ -2228,29 +2261,29 @@
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>63</v>
@@ -2267,29 +2300,29 @@
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>64</v>
@@ -2313,10 +2346,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="6">
@@ -2333,16 +2366,16 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>64</v>
@@ -2366,10 +2399,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O16" s="44"/>
       <c r="P16" s="6">
@@ -2386,16 +2419,16 @@
     <row r="17" spans="1:18" ht="18.75" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>64</v>
@@ -2419,10 +2452,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P17" s="46">
         <v>222.963951935914</v>
@@ -2438,16 +2471,16 @@
     <row r="18" spans="1:18" ht="18.75" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>64</v>
@@ -2471,10 +2504,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P18" s="6">
         <v>237.38317757009301</v>
@@ -2490,16 +2523,16 @@
     <row r="19" spans="1:18" ht="18.75" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>64</v>
@@ -2523,10 +2556,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P19" s="6">
         <v>379.97329773030702</v>
@@ -2542,16 +2575,16 @@
     <row r="20" spans="1:18" ht="18.75" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>64</v>
@@ -2575,10 +2608,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P20" s="6">
         <v>280.10680907877099</v>
@@ -2594,16 +2627,16 @@
     <row r="21" spans="1:18" ht="18.75" customHeight="1">
       <c r="A21" s="24"/>
       <c r="B21" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>64</v>
@@ -2627,10 +2660,10 @@
         <v>33</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P21" s="6">
         <v>298.79839786381802</v>
@@ -2646,16 +2679,16 @@
     <row r="22" spans="1:18" ht="18.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>64</v>
@@ -2679,10 +2712,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P22" s="6">
         <v>306.809078771695</v>
@@ -2698,16 +2731,16 @@
     <row r="23" spans="1:18" ht="18.75" customHeight="1">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>64</v>
@@ -2731,10 +2764,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P23" s="6">
         <v>322.29639519359102</v>
@@ -2750,16 +2783,16 @@
     <row r="24" spans="1:18" ht="18.75" customHeight="1">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>64</v>
@@ -2783,10 +2816,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P24" s="6">
         <v>589.31909212283006</v>
@@ -2802,16 +2835,16 @@
     <row r="25" spans="1:18" ht="18.75" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>64</v>
@@ -2835,10 +2868,10 @@
         <v>33</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="P25" s="6">
         <v>622</v>
@@ -2850,16 +2883,16 @@
     <row r="26" spans="1:18" ht="18.75" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>64</v>
@@ -2883,10 +2916,10 @@
         <v>33</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="P26" s="6">
         <v>828</v>
@@ -2898,16 +2931,16 @@
     <row r="27" spans="1:18" ht="18.75" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>66</v>
@@ -2931,10 +2964,10 @@
         <v>33</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="P27" s="6">
         <v>672</v>
@@ -2946,16 +2979,16 @@
     <row r="28" spans="1:18" ht="18.75" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>66</v>
@@ -2979,10 +3012,10 @@
         <v>33</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="P28" s="6">
         <v>845</v>
@@ -2994,16 +3027,16 @@
     <row r="29" spans="1:18" ht="18.75" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>67</v>
@@ -3023,25 +3056,25 @@
         <v>33</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="18.75" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>67</v>
@@ -3061,25 +3094,25 @@
         <v>33</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="18.75" customHeight="1">
       <c r="A31" s="24"/>
       <c r="B31" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>68</v>
@@ -3096,28 +3129,28 @@
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="18.75" customHeight="1">
       <c r="A32" s="24"/>
       <c r="B32" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>68</v>
@@ -3134,28 +3167,28 @@
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="18.75" customHeight="1">
       <c r="A33" s="24"/>
       <c r="B33" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>69</v>
@@ -3176,25 +3209,25 @@
         <v>70</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" customHeight="1">
       <c r="A34" s="24"/>
       <c r="B34" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>69</v>
@@ -3215,25 +3248,25 @@
         <v>70</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="18.75" customHeight="1">
       <c r="A35" s="24"/>
       <c r="B35" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E35" s="44" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>64</v>
@@ -3258,7 +3291,7 @@
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="P35" s="6">
         <v>602</v>
@@ -3269,108 +3302,287 @@
     </row>
     <row r="36" spans="1:17" ht="18.75" customHeight="1">
       <c r="A36" s="24"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="B36" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H36" s="42"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="4"/>
+      <c r="I36" s="43">
+        <v>298</v>
+      </c>
+      <c r="J36" s="4">
+        <v>7120</v>
+      </c>
       <c r="K36" s="4"/>
-      <c r="L36" s="9"/>
+      <c r="L36" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
+      <c r="N36" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="37" spans="1:17" ht="18.75" customHeight="1">
       <c r="A37" s="24"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
+      <c r="B37" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="I37" s="43">
+        <v>298</v>
+      </c>
+      <c r="J37" s="4">
+        <v>6501267427.1229401</v>
+      </c>
+      <c r="K37" s="4">
+        <v>177439797.21166</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M37" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N37" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="38" spans="1:17" ht="18.75" customHeight="1">
       <c r="A38" s="24"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
+      <c r="B38" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H38" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="I38" s="43">
+        <v>298</v>
+      </c>
+      <c r="J38" s="4">
+        <v>6599493029.1508198</v>
+      </c>
+      <c r="K38" s="4">
+        <v>123574144.48669</v>
+      </c>
+      <c r="L38" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N38" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="39" spans="1:17" ht="18.75" customHeight="1">
       <c r="A39" s="24"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="44"/>
-      <c r="N39" s="44"/>
+      <c r="B39" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="I39" s="43">
+        <v>298</v>
+      </c>
+      <c r="J39" s="4">
+        <v>6501267427.1229401</v>
+      </c>
+      <c r="K39" s="4">
+        <v>98225602.027880207</v>
+      </c>
+      <c r="L39" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M39" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="N39" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="40" spans="1:17" ht="18.75" customHeight="1">
       <c r="A40" s="24"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="44"/>
-      <c r="N40" s="44"/>
+      <c r="B40" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="I40" s="43">
+        <v>298</v>
+      </c>
+      <c r="J40" s="42">
+        <v>8014267185.4734097</v>
+      </c>
+      <c r="K40" s="3">
+        <v>269779507.13358998</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M40" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="N40" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="41" spans="1:17" ht="18.75" customHeight="1">
       <c r="A41" s="24"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="44"/>
-      <c r="M41" s="44"/>
-      <c r="N41" s="44"/>
+      <c r="B41" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" s="43">
+        <v>298</v>
+      </c>
+      <c r="J41" s="42">
+        <v>8162127107.6523895</v>
+      </c>
+      <c r="K41" s="3">
+        <v>233463035.01945999</v>
+      </c>
+      <c r="L41" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M41" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="N41" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="42" spans="1:17" ht="18.75" customHeight="1">
       <c r="A42" s="24"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="J42" s="3"/>
+      <c r="B42" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F42" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="I42" s="43">
+        <v>298</v>
+      </c>
+      <c r="J42" s="3">
+        <v>172000000000</v>
+      </c>
       <c r="K42" s="4"/>
-      <c r="L42" s="44"/>
+      <c r="L42" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="M42" s="44"/>
-      <c r="N42" s="44"/>
+      <c r="N42" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="43" spans="1:17" ht="18" customHeight="1">
       <c r="A43" s="24"/>
@@ -3396,8 +3608,7 @@
       <c r="G44" s="42"/>
       <c r="H44" s="42"/>
       <c r="J44" s="3"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="44"/>
+      <c r="L44" s="4"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
     </row>
@@ -3411,8 +3622,7 @@
       <c r="G45" s="42"/>
       <c r="H45" s="42"/>
       <c r="J45" s="3"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="44"/>
+      <c r="L45" s="4"/>
       <c r="M45" s="44"/>
       <c r="N45" s="44"/>
     </row>
@@ -3426,8 +3636,7 @@
       <c r="G46" s="42"/>
       <c r="H46" s="42"/>
       <c r="J46" s="3"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="44"/>
+      <c r="L46" s="4"/>
       <c r="M46" s="44"/>
       <c r="N46" s="44"/>
     </row>
@@ -3441,7 +3650,6 @@
       <c r="G47" s="42"/>
       <c r="H47" s="42"/>
       <c r="J47" s="3"/>
-      <c r="K47" s="4"/>
       <c r="L47" s="44"/>
       <c r="M47" s="44"/>
       <c r="N47" s="44"/>
@@ -3456,7 +3664,6 @@
       <c r="G48" s="42"/>
       <c r="H48" s="42"/>
       <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
       <c r="L48" s="52"/>
       <c r="M48" s="44"/>
       <c r="N48" s="44"/>
@@ -3471,7 +3678,6 @@
       <c r="G49" s="42"/>
       <c r="H49" s="42"/>
       <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
       <c r="L49" s="52"/>
       <c r="M49" s="44"/>
       <c r="N49" s="44"/>
@@ -3484,7 +3690,7 @@
       <c r="E50" s="42"/>
       <c r="F50" s="42"/>
       <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="52"/>
@@ -3499,7 +3705,7 @@
       <c r="E51" s="42"/>
       <c r="F51" s="42"/>
       <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
+      <c r="I51" s="42"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="52"/>
@@ -3514,7 +3720,6 @@
       <c r="E52" s="42"/>
       <c r="F52" s="42"/>
       <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="44"/>
@@ -3529,7 +3734,6 @@
       <c r="E53" s="42"/>
       <c r="F53" s="42"/>
       <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="44"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.matchemphys.2005.01.001`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D5B46B-824D-E643-B7D9-49F32BD289E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A45A54-C1B5-9548-BF96-7157960B89FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="5360" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="118">
   <si>
     <t>Metadata</t>
   </si>
@@ -355,6 +355,9 @@
     <t>BM+SPS</t>
   </si>
   <si>
+    <t>AAM</t>
+  </si>
+  <si>
     <t>kg/m^3</t>
   </si>
   <si>
@@ -464,6 +467,21 @@
   </si>
   <si>
     <t>FCC+B2</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchemphys.2005.01.001</t>
+  </si>
+  <si>
+    <t>FeCoNiCr</t>
+  </si>
+  <si>
+    <t>FeCoNiCrCu0.5</t>
+  </si>
+  <si>
+    <t>FeCoNiCrCu</t>
+  </si>
+  <si>
+    <t>FCC+FCC</t>
   </si>
 </sst>
 </file>
@@ -1796,8 +1814,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2118,16 +2136,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>63</v>
@@ -2144,29 +2162,29 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>63</v>
@@ -2183,29 +2201,29 @@
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>63</v>
@@ -2222,29 +2240,29 @@
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>63</v>
@@ -2261,29 +2279,29 @@
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>63</v>
@@ -2300,29 +2318,29 @@
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>64</v>
@@ -2346,10 +2364,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="6">
@@ -2366,16 +2384,16 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>64</v>
@@ -2399,10 +2417,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O16" s="44"/>
       <c r="P16" s="6">
@@ -2419,16 +2437,16 @@
     <row r="17" spans="1:18" ht="18.75" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>64</v>
@@ -2452,10 +2470,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P17" s="46">
         <v>222.963951935914</v>
@@ -2471,16 +2489,16 @@
     <row r="18" spans="1:18" ht="18.75" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>64</v>
@@ -2504,10 +2522,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P18" s="6">
         <v>237.38317757009301</v>
@@ -2523,16 +2541,16 @@
     <row r="19" spans="1:18" ht="18.75" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>64</v>
@@ -2556,10 +2574,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P19" s="6">
         <v>379.97329773030702</v>
@@ -2575,16 +2593,16 @@
     <row r="20" spans="1:18" ht="18.75" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>64</v>
@@ -2608,10 +2626,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P20" s="6">
         <v>280.10680907877099</v>
@@ -2627,16 +2645,16 @@
     <row r="21" spans="1:18" ht="18.75" customHeight="1">
       <c r="A21" s="24"/>
       <c r="B21" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>64</v>
@@ -2660,10 +2678,10 @@
         <v>33</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P21" s="6">
         <v>298.79839786381802</v>
@@ -2679,16 +2697,16 @@
     <row r="22" spans="1:18" ht="18.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>64</v>
@@ -2712,10 +2730,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P22" s="6">
         <v>306.809078771695</v>
@@ -2731,16 +2749,16 @@
     <row r="23" spans="1:18" ht="18.75" customHeight="1">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>64</v>
@@ -2764,10 +2782,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P23" s="6">
         <v>322.29639519359102</v>
@@ -2783,16 +2801,16 @@
     <row r="24" spans="1:18" ht="18.75" customHeight="1">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>64</v>
@@ -2816,10 +2834,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P24" s="6">
         <v>589.31909212283006</v>
@@ -2835,7 +2853,7 @@
     <row r="25" spans="1:18" ht="18.75" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>72</v>
@@ -2844,7 +2862,7 @@
         <v>74</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>64</v>
@@ -2871,7 +2889,7 @@
         <v>73</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P25" s="6">
         <v>622</v>
@@ -2883,7 +2901,7 @@
     <row r="26" spans="1:18" ht="18.75" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>65</v>
@@ -2892,7 +2910,7 @@
         <v>74</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>64</v>
@@ -2919,7 +2937,7 @@
         <v>73</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P26" s="6">
         <v>828</v>
@@ -2931,7 +2949,7 @@
     <row r="27" spans="1:18" ht="18.75" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>72</v>
@@ -2940,7 +2958,7 @@
         <v>74</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>66</v>
@@ -2967,7 +2985,7 @@
         <v>73</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P27" s="6">
         <v>672</v>
@@ -2979,7 +2997,7 @@
     <row r="28" spans="1:18" ht="18.75" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>65</v>
@@ -2988,7 +3006,7 @@
         <v>74</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>66</v>
@@ -3015,7 +3033,7 @@
         <v>73</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P28" s="6">
         <v>845</v>
@@ -3027,7 +3045,7 @@
     <row r="29" spans="1:18" ht="18.75" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>72</v>
@@ -3036,7 +3054,7 @@
         <v>74</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>67</v>
@@ -3059,13 +3077,13 @@
         <v>73</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="18.75" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>65</v>
@@ -3074,7 +3092,7 @@
         <v>74</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>67</v>
@@ -3097,13 +3115,13 @@
         <v>73</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="18.75" customHeight="1">
       <c r="A31" s="24"/>
       <c r="B31" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>72</v>
@@ -3112,7 +3130,7 @@
         <v>74</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>68</v>
@@ -3129,19 +3147,19 @@
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="18.75" customHeight="1">
       <c r="A32" s="24"/>
       <c r="B32" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>65</v>
@@ -3150,7 +3168,7 @@
         <v>74</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>68</v>
@@ -3167,19 +3185,19 @@
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="18.75" customHeight="1">
       <c r="A33" s="24"/>
       <c r="B33" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>72</v>
@@ -3188,7 +3206,7 @@
         <v>74</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>69</v>
@@ -3209,16 +3227,16 @@
         <v>70</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" customHeight="1">
       <c r="A34" s="24"/>
       <c r="B34" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>65</v>
@@ -3227,7 +3245,7 @@
         <v>74</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>69</v>
@@ -3248,25 +3266,25 @@
         <v>70</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="18.75" customHeight="1">
       <c r="A35" s="24"/>
       <c r="B35" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="44" t="s">
         <v>101</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>100</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>64</v>
@@ -3291,7 +3309,7 @@
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P35" s="6">
         <v>602</v>
@@ -3303,16 +3321,16 @@
     <row r="36" spans="1:17" ht="18.75" customHeight="1">
       <c r="A36" s="24"/>
       <c r="B36" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>63</v>
@@ -3329,26 +3347,26 @@
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="18.75" customHeight="1">
       <c r="A37" s="24"/>
       <c r="B37" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>64</v>
@@ -3357,7 +3375,7 @@
         <v>29</v>
       </c>
       <c r="H37" s="42" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I37" s="43">
         <v>298</v>
@@ -3375,22 +3393,22 @@
         <v>71</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="18.75" customHeight="1">
       <c r="A38" s="24"/>
       <c r="B38" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>64</v>
@@ -3399,7 +3417,7 @@
         <v>29</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I38" s="43">
         <v>298</v>
@@ -3417,22 +3435,22 @@
         <v>71</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="18.75" customHeight="1">
       <c r="A39" s="24"/>
       <c r="B39" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>64</v>
@@ -3441,7 +3459,7 @@
         <v>29</v>
       </c>
       <c r="H39" s="42" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I39" s="43">
         <v>298</v>
@@ -3459,22 +3477,22 @@
         <v>71</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="18.75" customHeight="1">
       <c r="A40" s="24"/>
       <c r="B40" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>66</v>
@@ -3483,7 +3501,7 @@
         <v>29</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I40" s="43">
         <v>298</v>
@@ -3498,25 +3516,25 @@
         <v>33</v>
       </c>
       <c r="M40" s="44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="18.75" customHeight="1">
       <c r="A41" s="24"/>
       <c r="B41" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>66</v>
@@ -3525,7 +3543,7 @@
         <v>29</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I41" s="43">
         <v>298</v>
@@ -3540,25 +3558,25 @@
         <v>33</v>
       </c>
       <c r="M41" s="44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="18.75" customHeight="1">
       <c r="A42" s="24"/>
       <c r="B42" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>67</v>
@@ -3567,7 +3585,7 @@
         <v>29</v>
       </c>
       <c r="H42" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I42" s="43">
         <v>298</v>
@@ -3581,14 +3599,20 @@
       </c>
       <c r="M42" s="44"/>
       <c r="N42" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="18" customHeight="1">
       <c r="A43" s="24"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
+      <c r="B43" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="E43" s="42"/>
       <c r="G43" s="42"/>
       <c r="H43" s="42"/>
@@ -3596,13 +3620,21 @@
       <c r="K43" s="4"/>
       <c r="L43" s="44"/>
       <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
+      <c r="N43" s="44" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="44" spans="1:17" ht="18" customHeight="1">
       <c r="A44" s="24"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
+      <c r="B44" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="E44" s="42"/>
       <c r="F44" s="42"/>
       <c r="G44" s="42"/>
@@ -3610,13 +3642,21 @@
       <c r="J44" s="3"/>
       <c r="L44" s="4"/>
       <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
+      <c r="N44" s="44" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="45" spans="1:17" ht="18" customHeight="1">
       <c r="A45" s="24"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
+      <c r="B45" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="E45" s="42"/>
       <c r="F45" s="42"/>
       <c r="G45" s="42"/>
@@ -3624,7 +3664,9 @@
       <c r="J45" s="3"/>
       <c r="L45" s="4"/>
       <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
+      <c r="N45" s="44" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="46" spans="1:17" ht="18" customHeight="1">
       <c r="A46" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s11661-006-0234-4` (Yeh2004 paper!!)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A45A54-C1B5-9548-BF96-7157960B89FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FED1B4C-6563-6C4D-81C3-6E9E4D99959C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="5360" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15340" yWindow="7860" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="132">
   <si>
     <t>Metadata</t>
   </si>
@@ -319,10 +319,22 @@
     <t>Col5</t>
   </si>
   <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
     <t>density</t>
   </si>
   <si>
     <t>hardness</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>SD</t>
   </si>
   <si>
     <t>FCC</t>
@@ -356,6 +368,9 @@
   </si>
   <si>
     <t>AAM</t>
+  </si>
+  <si>
+    <t>BCC+FCC</t>
   </si>
   <si>
     <t>kg/m^3</t>
@@ -482,6 +497,33 @@
   </si>
   <si>
     <t>FCC+FCC</t>
+  </si>
+  <si>
+    <t>10.1007/s11661-006-0234-4</t>
+  </si>
+  <si>
+    <t>CuCoNiCrFe</t>
+  </si>
+  <si>
+    <t>CuCoNiCrAl0.5Fe</t>
+  </si>
+  <si>
+    <t>Cu0.5CoNiCrAl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CuCoNiCrAlFeTiV</t>
+  </si>
+  <si>
+    <t>CuCoNiCrAlFeTiV</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>two major phases</t>
+  </si>
+  <si>
+    <t>major BCC phase</t>
   </si>
 </sst>
 </file>
@@ -1814,8 +1856,8 @@
   </sheetPr>
   <dimension ref="A1:T862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" topLeftCell="G33" zoomScale="75" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2136,19 +2178,19 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="9" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>29</v>
@@ -2162,32 +2204,32 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>29</v>
@@ -2201,32 +2243,32 @@
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="9" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>29</v>
@@ -2240,32 +2282,32 @@
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>29</v>
@@ -2279,32 +2321,32 @@
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>29</v>
@@ -2318,32 +2360,32 @@
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="9" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>29</v>
@@ -2364,10 +2406,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="6">
@@ -2384,19 +2426,19 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>29</v>
@@ -2417,10 +2459,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O16" s="44"/>
       <c r="P16" s="6">
@@ -2437,19 +2479,19 @@
     <row r="17" spans="1:18" ht="18.75" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="9" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>29</v>
@@ -2470,10 +2512,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P17" s="46">
         <v>222.963951935914</v>
@@ -2489,19 +2531,19 @@
     <row r="18" spans="1:18" ht="18.75" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>29</v>
@@ -2522,10 +2564,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P18" s="6">
         <v>237.38317757009301</v>
@@ -2541,19 +2583,19 @@
     <row r="19" spans="1:18" ht="18.75" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>29</v>
@@ -2574,10 +2616,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P19" s="6">
         <v>379.97329773030702</v>
@@ -2593,19 +2635,19 @@
     <row r="20" spans="1:18" ht="18.75" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>29</v>
@@ -2626,10 +2668,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P20" s="6">
         <v>280.10680907877099</v>
@@ -2645,19 +2687,19 @@
     <row r="21" spans="1:18" ht="18.75" customHeight="1">
       <c r="A21" s="24"/>
       <c r="B21" s="9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>29</v>
@@ -2678,10 +2720,10 @@
         <v>33</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P21" s="6">
         <v>298.79839786381802</v>
@@ -2697,19 +2739,19 @@
     <row r="22" spans="1:18" ht="18.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>29</v>
@@ -2730,10 +2772,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P22" s="6">
         <v>306.809078771695</v>
@@ -2749,19 +2791,19 @@
     <row r="23" spans="1:18" ht="18.75" customHeight="1">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>29</v>
@@ -2782,10 +2824,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P23" s="6">
         <v>322.29639519359102</v>
@@ -2801,19 +2843,19 @@
     <row r="24" spans="1:18" ht="18.75" customHeight="1">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>29</v>
@@ -2834,10 +2876,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P24" s="6">
         <v>589.31909212283006</v>
@@ -2853,19 +2895,19 @@
     <row r="25" spans="1:18" ht="18.75" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="9" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>29</v>
@@ -2886,10 +2928,10 @@
         <v>33</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="P25" s="6">
         <v>622</v>
@@ -2901,19 +2943,19 @@
     <row r="26" spans="1:18" ht="18.75" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>29</v>
@@ -2934,10 +2976,10 @@
         <v>33</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="P26" s="6">
         <v>828</v>
@@ -2949,19 +2991,19 @@
     <row r="27" spans="1:18" ht="18.75" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="9" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>29</v>
@@ -2982,10 +3024,10 @@
         <v>33</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="P27" s="6">
         <v>672</v>
@@ -2997,19 +3039,19 @@
     <row r="28" spans="1:18" ht="18.75" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>29</v>
@@ -3030,10 +3072,10 @@
         <v>33</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="P28" s="6">
         <v>845</v>
@@ -3045,19 +3087,19 @@
     <row r="29" spans="1:18" ht="18.75" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="9" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>29</v>
@@ -3074,28 +3116,28 @@
         <v>33</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="18.75" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>29</v>
@@ -3112,28 +3154,28 @@
         <v>33</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="18.75" customHeight="1">
       <c r="A31" s="24"/>
       <c r="B31" s="9" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>29</v>
@@ -3147,31 +3189,31 @@
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="9" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="18.75" customHeight="1">
       <c r="A32" s="24"/>
       <c r="B32" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>29</v>
@@ -3185,31 +3227,31 @@
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="9" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="18.75" customHeight="1">
       <c r="A33" s="24"/>
       <c r="B33" s="9" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>29</v>
@@ -3224,31 +3266,31 @@
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="9" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" customHeight="1">
       <c r="A34" s="24"/>
       <c r="B34" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>29</v>
@@ -3263,31 +3305,31 @@
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="9" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="18.75" customHeight="1">
       <c r="A35" s="24"/>
       <c r="B35" s="9" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E35" s="44" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>29</v>
@@ -3309,7 +3351,7 @@
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="P35" s="6">
         <v>602</v>
@@ -3321,19 +3363,19 @@
     <row r="36" spans="1:17" ht="18.75" customHeight="1">
       <c r="A36" s="24"/>
       <c r="B36" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>29</v>
@@ -3347,35 +3389,35 @@
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="9" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="18.75" customHeight="1">
       <c r="A37" s="24"/>
       <c r="B37" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H37" s="42" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="I37" s="43">
         <v>298</v>
@@ -3390,34 +3432,34 @@
         <v>33</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="18.75" customHeight="1">
       <c r="A38" s="24"/>
       <c r="B38" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="I38" s="43">
         <v>298</v>
@@ -3432,34 +3474,34 @@
         <v>33</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="18.75" customHeight="1">
       <c r="A39" s="24"/>
       <c r="B39" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H39" s="42" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I39" s="43">
         <v>298</v>
@@ -3474,34 +3516,34 @@
         <v>33</v>
       </c>
       <c r="M39" s="44" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="18.75" customHeight="1">
       <c r="A40" s="24"/>
       <c r="B40" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F40" s="48" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="I40" s="43">
         <v>298</v>
@@ -3516,34 +3558,34 @@
         <v>33</v>
       </c>
       <c r="M40" s="44" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="18.75" customHeight="1">
       <c r="A41" s="24"/>
       <c r="B41" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F41" s="48" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="I41" s="43">
         <v>298</v>
@@ -3558,34 +3600,34 @@
         <v>33</v>
       </c>
       <c r="M41" s="44" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="18.75" customHeight="1">
       <c r="A42" s="24"/>
       <c r="B42" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F42" s="48" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H42" s="42" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="I42" s="43">
         <v>298</v>
@@ -3599,19 +3641,19 @@
       </c>
       <c r="M42" s="44"/>
       <c r="N42" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="18" customHeight="1">
       <c r="A43" s="24"/>
       <c r="B43" s="44" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D43" s="42" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E43" s="42"/>
       <c r="G43" s="42"/>
@@ -3621,19 +3663,19 @@
       <c r="L43" s="44"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="18" customHeight="1">
       <c r="A44" s="24"/>
       <c r="B44" s="44" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D44" s="42" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E44" s="42"/>
       <c r="F44" s="42"/>
@@ -3643,19 +3685,19 @@
       <c r="L44" s="4"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="18" customHeight="1">
       <c r="A45" s="24"/>
       <c r="B45" s="44" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D45" s="42" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E45" s="42"/>
       <c r="F45" s="42"/>
@@ -3665,96 +3707,250 @@
       <c r="L45" s="4"/>
       <c r="M45" s="44"/>
       <c r="N45" s="44" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="18" customHeight="1">
       <c r="A46" s="24"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
+      <c r="B46" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>63</v>
+      </c>
       <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
+      <c r="F46" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G46" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H46" s="42"/>
-      <c r="J46" s="3"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="44"/>
+      <c r="I46" s="49">
+        <v>298</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" ref="J46:J51" si="4">P46*9807000</f>
+        <v>1304331000</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M46" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N46" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="P46" s="6">
+        <v>133</v>
+      </c>
     </row>
     <row r="47" spans="1:17" ht="18" customHeight="1">
       <c r="A47" s="24"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
+      <c r="B47" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>63</v>
+      </c>
       <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42"/>
+      <c r="F47" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G47" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H47" s="42"/>
-      <c r="J47" s="3"/>
-      <c r="L47" s="44"/>
-      <c r="M47" s="44"/>
-      <c r="N47" s="44"/>
+      <c r="I47" s="49">
+        <v>298</v>
+      </c>
+      <c r="J47" s="4">
+        <f t="shared" si="4"/>
+        <v>2039856000</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M47" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N47" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="P47" s="6">
+        <v>208</v>
+      </c>
     </row>
     <row r="48" spans="1:17" ht="18" customHeight="1">
       <c r="A48" s="24"/>
-      <c r="B48" s="44"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
+      <c r="B48" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="F48" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G48" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H48" s="42"/>
-      <c r="J48" s="4"/>
-      <c r="L48" s="52"/>
-      <c r="M48" s="44"/>
-      <c r="N48" s="44"/>
-    </row>
-    <row r="49" spans="1:14" ht="18" customHeight="1">
+      <c r="I48" s="49">
+        <v>298</v>
+      </c>
+      <c r="J48" s="4">
+        <f t="shared" si="4"/>
+        <v>4864272000</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M48" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N48" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="P48" s="6">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="18" customHeight="1">
       <c r="A49" s="24"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
+      <c r="B49" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="F49" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H49" s="42"/>
-      <c r="J49" s="4"/>
-      <c r="L49" s="52"/>
-      <c r="M49" s="44"/>
-      <c r="N49" s="44"/>
-    </row>
-    <row r="50" spans="1:14" ht="18" customHeight="1">
+      <c r="I49" s="49">
+        <v>298</v>
+      </c>
+      <c r="J49" s="4">
+        <f t="shared" si="4"/>
+        <v>8002512000</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M49" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N49" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="P49" s="6">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="18" customHeight="1">
       <c r="A50" s="24"/>
-      <c r="B50" s="44"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="52"/>
-      <c r="M50" s="44"/>
-      <c r="N50" s="44"/>
-    </row>
-    <row r="51" spans="1:14" ht="18" customHeight="1">
+      <c r="B50" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="F50" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H50" s="42"/>
+      <c r="I50" s="49">
+        <v>298</v>
+      </c>
+      <c r="J50" s="4">
+        <f t="shared" si="4"/>
+        <v>5491920000</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M50" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N50" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="P50" s="6">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="18" customHeight="1">
       <c r="A51" s="24"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
+      <c r="B51" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>129</v>
+      </c>
       <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="52"/>
-      <c r="M51" s="44"/>
-      <c r="N51" s="44"/>
-    </row>
-    <row r="52" spans="1:14" ht="18" customHeight="1">
+      <c r="F51" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G51" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H51" s="42"/>
+      <c r="I51" s="49">
+        <v>298</v>
+      </c>
+      <c r="J51" s="4">
+        <f t="shared" si="4"/>
+        <v>6531462000</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M51" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="N51" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="P51" s="6">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="18" customHeight="1">
       <c r="A52" s="24"/>
       <c r="B52" s="44"/>
       <c r="C52" s="42"/>
@@ -3768,7 +3964,7 @@
       <c r="M52" s="44"/>
       <c r="N52" s="44"/>
     </row>
-    <row r="53" spans="1:14" ht="18" customHeight="1">
+    <row r="53" spans="1:16" ht="18" customHeight="1">
       <c r="A53" s="24"/>
       <c r="B53" s="44"/>
       <c r="C53" s="42"/>
@@ -3782,7 +3978,7 @@
       <c r="M53" s="44"/>
       <c r="N53" s="44"/>
     </row>
-    <row r="54" spans="1:14" ht="18" customHeight="1">
+    <row r="54" spans="1:16" ht="18" customHeight="1">
       <c r="A54" s="24"/>
       <c r="B54" s="44"/>
       <c r="C54" s="42"/>
@@ -3797,7 +3993,7 @@
       <c r="M54" s="44"/>
       <c r="N54" s="44"/>
     </row>
-    <row r="55" spans="1:14" ht="18" customHeight="1">
+    <row r="55" spans="1:16" ht="18" customHeight="1">
       <c r="A55" s="24"/>
       <c r="B55" s="44"/>
       <c r="C55" s="42"/>
@@ -3812,7 +4008,7 @@
       <c r="M55" s="44"/>
       <c r="N55" s="44"/>
     </row>
-    <row r="56" spans="1:14" ht="18" customHeight="1">
+    <row r="56" spans="1:16" ht="18" customHeight="1">
       <c r="A56" s="24"/>
       <c r="B56" s="44"/>
       <c r="C56" s="42"/>
@@ -3827,7 +4023,7 @@
       <c r="M56" s="44"/>
       <c r="N56" s="44"/>
     </row>
-    <row r="57" spans="1:14" ht="18" customHeight="1">
+    <row r="57" spans="1:16" ht="18" customHeight="1">
       <c r="A57" s="24"/>
       <c r="B57" s="44"/>
       <c r="C57" s="42"/>
@@ -3842,7 +4038,7 @@
       <c r="M57" s="44"/>
       <c r="N57" s="44"/>
     </row>
-    <row r="58" spans="1:14" ht="18" customHeight="1">
+    <row r="58" spans="1:16" ht="18" customHeight="1">
       <c r="A58" s="24"/>
       <c r="B58" s="44"/>
       <c r="C58" s="42"/>
@@ -3857,7 +4053,7 @@
       <c r="M58" s="44"/>
       <c r="N58" s="44"/>
     </row>
-    <row r="59" spans="1:14" ht="18" customHeight="1">
+    <row r="59" spans="1:16" ht="18" customHeight="1">
       <c r="A59" s="24"/>
       <c r="B59" s="44"/>
       <c r="C59" s="42"/>
@@ -3872,7 +4068,7 @@
       <c r="M59" s="44"/>
       <c r="N59" s="44"/>
     </row>
-    <row r="60" spans="1:14" ht="18" customHeight="1">
+    <row r="60" spans="1:16" ht="18" customHeight="1">
       <c r="A60" s="24"/>
       <c r="B60" s="44"/>
       <c r="C60" s="42"/>
@@ -3888,7 +4084,7 @@
       <c r="M60" s="44"/>
       <c r="N60" s="44"/>
     </row>
-    <row r="61" spans="1:14" ht="18" customHeight="1">
+    <row r="61" spans="1:16" ht="18" customHeight="1">
       <c r="A61" s="24"/>
       <c r="B61" s="44"/>
       <c r="C61" s="42"/>
@@ -3904,7 +4100,7 @@
       <c r="M61" s="44"/>
       <c r="N61" s="44"/>
     </row>
-    <row r="62" spans="1:14" ht="18" customHeight="1">
+    <row r="62" spans="1:16" ht="18" customHeight="1">
       <c r="A62" s="24"/>
       <c r="B62" s="44"/>
       <c r="C62" s="42"/>
@@ -3920,7 +4116,7 @@
       <c r="M62" s="44"/>
       <c r="N62" s="44"/>
     </row>
-    <row r="63" spans="1:14" ht="18" customHeight="1">
+    <row r="63" spans="1:16" ht="18" customHeight="1">
       <c r="A63" s="24"/>
       <c r="B63" s="44"/>
       <c r="C63" s="42"/>
@@ -3936,7 +4132,7 @@
       <c r="M63" s="44"/>
       <c r="N63" s="44"/>
     </row>
-    <row r="64" spans="1:14" ht="18" customHeight="1">
+    <row r="64" spans="1:16" ht="18" customHeight="1">
       <c r="A64" s="24"/>
       <c r="B64" s="44"/>
       <c r="C64" s="42"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2003.10.257` (Cantor2004 paper!!)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FED1B4C-6563-6C4D-81C3-6E9E4D99959C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F696153-1017-314E-BF55-60592E8202C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15340" yWindow="7860" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="7760" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="btblfn1" localSheetId="0">Sheet1!$I$754</definedName>
+    <definedName name="btblfn1" localSheetId="0">Sheet1!$I$753</definedName>
     <definedName name="btblfn2" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="148">
   <si>
     <t>Metadata</t>
   </si>
@@ -379,6 +379,9 @@
     <t>T3</t>
   </si>
   <si>
+    <t>MS</t>
+  </si>
+  <si>
     <t>F5</t>
   </si>
   <si>
@@ -524,6 +527,51 @@
   </si>
   <si>
     <t>major BCC phase</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2003.10.257</t>
+  </si>
+  <si>
+    <t>Fe20Cr20Mn20Ni20Co20</t>
+  </si>
+  <si>
+    <t>MnCrFeCoNiCuAgWMoNbAlCdSnPbZnMg</t>
+  </si>
+  <si>
+    <t>MnCrFeCoNiCuAgWMoNbAlCdSnPbBiZnGeSiSbMg</t>
+  </si>
+  <si>
+    <t>FCC+5?</t>
+  </si>
+  <si>
+    <t>VIM</t>
+  </si>
+  <si>
+    <t>Fe Cr Mn Ni Co Nb</t>
+  </si>
+  <si>
+    <t>Fe Cr Mn Ni Co Ge</t>
+  </si>
+  <si>
+    <t>Fe Cr Mn Ni Co Cu</t>
+  </si>
+  <si>
+    <t>Fe Cr Mn Ni Co Ti</t>
+  </si>
+  <si>
+    <t>Fe Cr Mn Ni Co V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">very brittle; not tested mechanically but used to derrive candidates based on FCC solid solution </t>
+  </si>
+  <si>
+    <t>FCC+BCC+FCC</t>
+  </si>
+  <si>
+    <t>FCC+?</t>
+  </si>
+  <si>
+    <t>the Cantor alloy</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1548,6 +1596,9 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1854,16 +1905,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T862"/>
+  <dimension ref="A1:T861"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G33" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.1640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" style="48" bestFit="1" customWidth="1"/>
@@ -2178,16 +2229,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>65</v>
@@ -2210,23 +2261,23 @@
         <v>82</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>65</v>
@@ -2249,23 +2300,23 @@
         <v>82</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>65</v>
@@ -2288,23 +2339,23 @@
         <v>82</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>65</v>
@@ -2327,23 +2378,23 @@
         <v>82</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>65</v>
@@ -2366,23 +2417,23 @@
         <v>82</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>66</v>
@@ -2406,10 +2457,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="6">
@@ -2426,16 +2477,16 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>66</v>
@@ -2459,10 +2510,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O16" s="44"/>
       <c r="P16" s="6">
@@ -2479,16 +2530,16 @@
     <row r="17" spans="1:18" ht="18.75" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>66</v>
@@ -2512,10 +2563,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P17" s="46">
         <v>222.963951935914</v>
@@ -2531,16 +2582,16 @@
     <row r="18" spans="1:18" ht="18.75" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>66</v>
@@ -2564,10 +2615,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P18" s="6">
         <v>237.38317757009301</v>
@@ -2583,16 +2634,16 @@
     <row r="19" spans="1:18" ht="18.75" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>66</v>
@@ -2616,10 +2667,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P19" s="6">
         <v>379.97329773030702</v>
@@ -2635,16 +2686,16 @@
     <row r="20" spans="1:18" ht="18.75" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>66</v>
@@ -2668,10 +2719,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P20" s="6">
         <v>280.10680907877099</v>
@@ -2687,16 +2738,16 @@
     <row r="21" spans="1:18" ht="18.75" customHeight="1">
       <c r="A21" s="24"/>
       <c r="B21" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>66</v>
@@ -2720,10 +2771,10 @@
         <v>33</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P21" s="6">
         <v>298.79839786381802</v>
@@ -2739,16 +2790,16 @@
     <row r="22" spans="1:18" ht="18.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>66</v>
@@ -2772,10 +2823,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P22" s="6">
         <v>306.809078771695</v>
@@ -2791,16 +2842,16 @@
     <row r="23" spans="1:18" ht="18.75" customHeight="1">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>66</v>
@@ -2824,10 +2875,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P23" s="6">
         <v>322.29639519359102</v>
@@ -2843,16 +2894,16 @@
     <row r="24" spans="1:18" ht="18.75" customHeight="1">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>66</v>
@@ -2876,10 +2927,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P24" s="6">
         <v>589.31909212283006</v>
@@ -2895,7 +2946,7 @@
     <row r="25" spans="1:18" ht="18.75" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>76</v>
@@ -2904,7 +2955,7 @@
         <v>78</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>66</v>
@@ -2931,7 +2982,7 @@
         <v>77</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P25" s="6">
         <v>622</v>
@@ -2943,7 +2994,7 @@
     <row r="26" spans="1:18" ht="18.75" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>69</v>
@@ -2952,7 +3003,7 @@
         <v>78</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>66</v>
@@ -2979,7 +3030,7 @@
         <v>77</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P26" s="6">
         <v>828</v>
@@ -2991,7 +3042,7 @@
     <row r="27" spans="1:18" ht="18.75" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>76</v>
@@ -3000,7 +3051,7 @@
         <v>78</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>70</v>
@@ -3027,7 +3078,7 @@
         <v>77</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P27" s="6">
         <v>672</v>
@@ -3039,7 +3090,7 @@
     <row r="28" spans="1:18" ht="18.75" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>69</v>
@@ -3048,7 +3099,7 @@
         <v>78</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>70</v>
@@ -3075,7 +3126,7 @@
         <v>77</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P28" s="6">
         <v>845</v>
@@ -3087,7 +3138,7 @@
     <row r="29" spans="1:18" ht="18.75" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>76</v>
@@ -3096,7 +3147,7 @@
         <v>78</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>71</v>
@@ -3119,13 +3170,13 @@
         <v>77</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="18.75" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>69</v>
@@ -3134,7 +3185,7 @@
         <v>78</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>71</v>
@@ -3157,13 +3208,13 @@
         <v>77</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="18.75" customHeight="1">
       <c r="A31" s="24"/>
       <c r="B31" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>76</v>
@@ -3172,7 +3223,7 @@
         <v>78</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>72</v>
@@ -3189,19 +3240,19 @@
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="18.75" customHeight="1">
       <c r="A32" s="24"/>
       <c r="B32" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>69</v>
@@ -3210,7 +3261,7 @@
         <v>78</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>72</v>
@@ -3227,19 +3278,19 @@
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="18.75" customHeight="1">
       <c r="A33" s="24"/>
       <c r="B33" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>76</v>
@@ -3248,7 +3299,7 @@
         <v>78</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>73</v>
@@ -3269,16 +3320,16 @@
         <v>74</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" customHeight="1">
       <c r="A34" s="24"/>
       <c r="B34" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>69</v>
@@ -3287,7 +3338,7 @@
         <v>78</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>73</v>
@@ -3308,25 +3359,25 @@
         <v>74</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="18.75" customHeight="1">
       <c r="A35" s="24"/>
       <c r="B35" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="44" t="s">
         <v>107</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>106</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>66</v>
@@ -3351,7 +3402,7 @@
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P35" s="6">
         <v>602</v>
@@ -3363,16 +3414,16 @@
     <row r="36" spans="1:17" ht="18.75" customHeight="1">
       <c r="A36" s="24"/>
       <c r="B36" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>65</v>
@@ -3393,22 +3444,22 @@
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="18.75" customHeight="1">
       <c r="A37" s="24"/>
       <c r="B37" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>66</v>
@@ -3417,7 +3468,7 @@
         <v>29</v>
       </c>
       <c r="H37" s="42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I37" s="43">
         <v>298</v>
@@ -3435,22 +3486,22 @@
         <v>75</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="18.75" customHeight="1">
       <c r="A38" s="24"/>
       <c r="B38" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>66</v>
@@ -3459,7 +3510,7 @@
         <v>29</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I38" s="43">
         <v>298</v>
@@ -3477,22 +3528,22 @@
         <v>75</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="18.75" customHeight="1">
       <c r="A39" s="24"/>
       <c r="B39" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>66</v>
@@ -3501,7 +3552,7 @@
         <v>29</v>
       </c>
       <c r="H39" s="42" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I39" s="43">
         <v>298</v>
@@ -3519,22 +3570,22 @@
         <v>75</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="18.75" customHeight="1">
       <c r="A40" s="24"/>
       <c r="B40" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>70</v>
@@ -3543,7 +3594,7 @@
         <v>29</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I40" s="43">
         <v>298</v>
@@ -3558,25 +3609,25 @@
         <v>33</v>
       </c>
       <c r="M40" s="44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="18.75" customHeight="1">
       <c r="A41" s="24"/>
       <c r="B41" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>70</v>
@@ -3585,7 +3636,7 @@
         <v>29</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I41" s="43">
         <v>298</v>
@@ -3600,25 +3651,25 @@
         <v>33</v>
       </c>
       <c r="M41" s="44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="18.75" customHeight="1">
       <c r="A42" s="24"/>
       <c r="B42" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>71</v>
@@ -3627,7 +3678,7 @@
         <v>29</v>
       </c>
       <c r="H42" s="42" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I42" s="43">
         <v>298</v>
@@ -3641,13 +3692,13 @@
       </c>
       <c r="M42" s="44"/>
       <c r="N42" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="18" customHeight="1">
       <c r="A43" s="24"/>
       <c r="B43" s="44" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C43" s="42" t="s">
         <v>69</v>
@@ -3663,13 +3714,13 @@
       <c r="L43" s="44"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="18" customHeight="1">
       <c r="A44" s="24"/>
       <c r="B44" s="44" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C44" s="42" t="s">
         <v>69</v>
@@ -3685,16 +3736,16 @@
       <c r="L44" s="4"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="18" customHeight="1">
       <c r="A45" s="24"/>
       <c r="B45" s="44" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D45" s="42" t="s">
         <v>79</v>
@@ -3707,13 +3758,13 @@
       <c r="L45" s="4"/>
       <c r="M45" s="44"/>
       <c r="N45" s="44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="18" customHeight="1">
       <c r="A46" s="24"/>
       <c r="B46" s="44" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C46" s="42" t="s">
         <v>69</v>
@@ -3743,7 +3794,7 @@
         <v>67</v>
       </c>
       <c r="N46" s="44" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P46" s="6">
         <v>133</v>
@@ -3752,7 +3803,7 @@
     <row r="47" spans="1:17" ht="18" customHeight="1">
       <c r="A47" s="24"/>
       <c r="B47" s="44" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C47" s="42" t="s">
         <v>69</v>
@@ -3782,7 +3833,7 @@
         <v>67</v>
       </c>
       <c r="N47" s="44" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P47" s="6">
         <v>208</v>
@@ -3791,7 +3842,7 @@
     <row r="48" spans="1:17" ht="18" customHeight="1">
       <c r="A48" s="24"/>
       <c r="B48" s="44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C48" s="42" t="s">
         <v>80</v>
@@ -3800,7 +3851,7 @@
         <v>63</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F48" s="42" t="s">
         <v>66</v>
@@ -3823,7 +3874,7 @@
         <v>67</v>
       </c>
       <c r="N48" s="44" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P48" s="6">
         <v>496</v>
@@ -3832,7 +3883,7 @@
     <row r="49" spans="1:16" ht="18" customHeight="1">
       <c r="A49" s="24"/>
       <c r="B49" s="44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C49" s="42" t="s">
         <v>80</v>
@@ -3841,7 +3892,7 @@
         <v>68</v>
       </c>
       <c r="E49" s="42" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F49" s="42" t="s">
         <v>66</v>
@@ -3864,7 +3915,7 @@
         <v>67</v>
       </c>
       <c r="N49" s="44" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P49" s="6">
         <v>816</v>
@@ -3873,7 +3924,7 @@
     <row r="50" spans="1:16" ht="18" customHeight="1">
       <c r="A50" s="24"/>
       <c r="B50" s="44" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C50" s="42" t="s">
         <v>80</v>
@@ -3882,7 +3933,7 @@
         <v>63</v>
       </c>
       <c r="E50" s="42" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F50" s="42" t="s">
         <v>66</v>
@@ -3905,7 +3956,7 @@
         <v>67</v>
       </c>
       <c r="N50" s="44" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P50" s="6">
         <v>560</v>
@@ -3914,13 +3965,13 @@
     <row r="51" spans="1:16" ht="18" customHeight="1">
       <c r="A51" s="24"/>
       <c r="B51" s="44" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C51" s="42" t="s">
         <v>64</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E51" s="42"/>
       <c r="F51" s="42" t="s">
@@ -3944,7 +3995,7 @@
         <v>67</v>
       </c>
       <c r="N51" s="44" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P51" s="6">
         <v>666</v>
@@ -3952,38 +4003,67 @@
     </row>
     <row r="52" spans="1:16" ht="18" customHeight="1">
       <c r="A52" s="24"/>
-      <c r="B52" s="44"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
+      <c r="B52" s="128" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E52" s="42" t="s">
+        <v>144</v>
+      </c>
       <c r="F52" s="42"/>
       <c r="G52" s="42"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="44"/>
       <c r="M52" s="44"/>
-      <c r="N52" s="44"/>
+      <c r="N52" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="53" spans="1:16" ht="18" customHeight="1">
       <c r="A53" s="24"/>
-      <c r="B53" s="44"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
+      <c r="B53" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E53" s="42" t="s">
+        <v>144</v>
+      </c>
       <c r="F53" s="42"/>
       <c r="G53" s="42"/>
+      <c r="H53" s="42"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="44"/>
       <c r="M53" s="44"/>
-      <c r="N53" s="44"/>
+      <c r="N53" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="54" spans="1:16" ht="18" customHeight="1">
       <c r="A54" s="24"/>
-      <c r="B54" s="44"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
+      <c r="B54" s="128" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E54" s="42" t="s">
+        <v>144</v>
+      </c>
       <c r="F54" s="42"/>
       <c r="G54" s="42"/>
       <c r="H54" s="42"/>
@@ -3991,29 +4071,49 @@
       <c r="K54" s="4"/>
       <c r="L54" s="44"/>
       <c r="M54" s="44"/>
-      <c r="N54" s="44"/>
+      <c r="N54" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="55" spans="1:16" ht="18" customHeight="1">
       <c r="A55" s="24"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="42"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
+      <c r="B55" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" s="42" t="s">
+        <v>144</v>
+      </c>
       <c r="F55" s="42"/>
       <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
+      <c r="I55" s="3"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="44"/>
       <c r="M55" s="44"/>
-      <c r="N55" s="44"/>
+      <c r="N55" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="56" spans="1:16" ht="18" customHeight="1">
       <c r="A56" s="24"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="44"/>
+      <c r="B56" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E56" s="44" t="s">
+        <v>147</v>
+      </c>
       <c r="F56" s="42"/>
       <c r="G56" s="42"/>
       <c r="I56" s="3"/>
@@ -4021,13 +4121,21 @@
       <c r="K56" s="4"/>
       <c r="L56" s="44"/>
       <c r="M56" s="44"/>
-      <c r="N56" s="44"/>
+      <c r="N56" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="57" spans="1:16" ht="18" customHeight="1">
       <c r="A57" s="24"/>
-      <c r="B57" s="44"/>
-      <c r="C57" s="42"/>
-      <c r="D57" s="42"/>
+      <c r="B57" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="42" t="s">
+        <v>138</v>
+      </c>
       <c r="E57" s="44"/>
       <c r="F57" s="42"/>
       <c r="G57" s="42"/>
@@ -4036,13 +4144,21 @@
       <c r="K57" s="4"/>
       <c r="L57" s="44"/>
       <c r="M57" s="44"/>
-      <c r="N57" s="44"/>
+      <c r="N57" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="58" spans="1:16" ht="18" customHeight="1">
       <c r="A58" s="24"/>
-      <c r="B58" s="44"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
+      <c r="B58" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>138</v>
+      </c>
       <c r="E58" s="44"/>
       <c r="F58" s="42"/>
       <c r="G58" s="42"/>
@@ -4051,28 +4167,45 @@
       <c r="K58" s="4"/>
       <c r="L58" s="44"/>
       <c r="M58" s="44"/>
-      <c r="N58" s="44"/>
+      <c r="N58" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="59" spans="1:16" ht="18" customHeight="1">
       <c r="A59" s="24"/>
-      <c r="B59" s="44"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="42"/>
+      <c r="B59" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>138</v>
+      </c>
       <c r="E59" s="44"/>
       <c r="F59" s="42"/>
       <c r="G59" s="42"/>
+      <c r="H59" s="42"/>
       <c r="I59" s="3"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="44"/>
       <c r="M59" s="44"/>
-      <c r="N59" s="44"/>
+      <c r="N59" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="60" spans="1:16" ht="18" customHeight="1">
       <c r="A60" s="24"/>
-      <c r="B60" s="44"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="42"/>
+      <c r="B60" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="42" t="s">
+        <v>138</v>
+      </c>
       <c r="E60" s="44"/>
       <c r="F60" s="42"/>
       <c r="G60" s="42"/>
@@ -4082,13 +4215,21 @@
       <c r="K60" s="4"/>
       <c r="L60" s="44"/>
       <c r="M60" s="44"/>
-      <c r="N60" s="44"/>
+      <c r="N60" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="61" spans="1:16" ht="18" customHeight="1">
       <c r="A61" s="24"/>
-      <c r="B61" s="44"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
+      <c r="B61" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="D61" s="42" t="s">
+        <v>138</v>
+      </c>
       <c r="E61" s="44"/>
       <c r="F61" s="42"/>
       <c r="G61" s="42"/>
@@ -4098,7 +4239,9 @@
       <c r="K61" s="4"/>
       <c r="L61" s="44"/>
       <c r="M61" s="44"/>
-      <c r="N61" s="44"/>
+      <c r="N61" s="44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="62" spans="1:16" ht="18" customHeight="1">
       <c r="A62" s="24"/>
@@ -5158,7 +5301,7 @@
     </row>
     <row r="128" spans="1:14" ht="18" customHeight="1">
       <c r="A128" s="24"/>
-      <c r="B128" s="44"/>
+      <c r="B128" s="52"/>
       <c r="C128" s="42"/>
       <c r="D128" s="42"/>
       <c r="E128" s="44"/>
@@ -5174,7 +5317,7 @@
     </row>
     <row r="129" spans="1:14" ht="18" customHeight="1">
       <c r="A129" s="24"/>
-      <c r="B129" s="52"/>
+      <c r="B129" s="44"/>
       <c r="C129" s="42"/>
       <c r="D129" s="42"/>
       <c r="E129" s="44"/>
@@ -5206,7 +5349,7 @@
     </row>
     <row r="131" spans="1:14" ht="18" customHeight="1">
       <c r="A131" s="24"/>
-      <c r="B131" s="44"/>
+      <c r="B131" s="52"/>
       <c r="C131" s="42"/>
       <c r="D131" s="42"/>
       <c r="E131" s="44"/>
@@ -5222,7 +5365,7 @@
     </row>
     <row r="132" spans="1:14" ht="18" customHeight="1">
       <c r="A132" s="24"/>
-      <c r="B132" s="52"/>
+      <c r="B132" s="44"/>
       <c r="C132" s="42"/>
       <c r="D132" s="42"/>
       <c r="E132" s="44"/>
@@ -5254,7 +5397,7 @@
     </row>
     <row r="134" spans="1:14" ht="18" customHeight="1">
       <c r="A134" s="24"/>
-      <c r="B134" s="44"/>
+      <c r="B134" s="52"/>
       <c r="C134" s="42"/>
       <c r="D134" s="42"/>
       <c r="E134" s="44"/>
@@ -5270,7 +5413,7 @@
     </row>
     <row r="135" spans="1:14" ht="18" customHeight="1">
       <c r="A135" s="24"/>
-      <c r="B135" s="52"/>
+      <c r="B135" s="44"/>
       <c r="C135" s="42"/>
       <c r="D135" s="42"/>
       <c r="E135" s="44"/>
@@ -5302,7 +5445,7 @@
     </row>
     <row r="137" spans="1:14" ht="18" customHeight="1">
       <c r="A137" s="24"/>
-      <c r="B137" s="44"/>
+      <c r="B137" s="52"/>
       <c r="C137" s="42"/>
       <c r="D137" s="42"/>
       <c r="E137" s="44"/>
@@ -5318,7 +5461,7 @@
     </row>
     <row r="138" spans="1:14" ht="18" customHeight="1">
       <c r="A138" s="24"/>
-      <c r="B138" s="52"/>
+      <c r="B138" s="44"/>
       <c r="C138" s="42"/>
       <c r="D138" s="42"/>
       <c r="E138" s="44"/>
@@ -5350,7 +5493,7 @@
     </row>
     <row r="140" spans="1:14" ht="18" customHeight="1">
       <c r="A140" s="24"/>
-      <c r="B140" s="44"/>
+      <c r="B140" s="52"/>
       <c r="C140" s="42"/>
       <c r="D140" s="42"/>
       <c r="E140" s="44"/>
@@ -5366,7 +5509,7 @@
     </row>
     <row r="141" spans="1:14" ht="18" customHeight="1">
       <c r="A141" s="24"/>
-      <c r="B141" s="52"/>
+      <c r="B141" s="44"/>
       <c r="C141" s="42"/>
       <c r="D141" s="42"/>
       <c r="E141" s="44"/>
@@ -5454,7 +5597,6 @@
       <c r="G146" s="42"/>
       <c r="H146" s="42"/>
       <c r="I146" s="3"/>
-      <c r="J146" s="4"/>
       <c r="K146" s="4"/>
       <c r="L146" s="44"/>
       <c r="M146" s="44"/>
@@ -5462,7 +5604,7 @@
     </row>
     <row r="147" spans="1:14" ht="18" customHeight="1">
       <c r="A147" s="24"/>
-      <c r="B147" s="44"/>
+      <c r="B147" s="52"/>
       <c r="C147" s="42"/>
       <c r="D147" s="42"/>
       <c r="E147" s="44"/>
@@ -5470,6 +5612,7 @@
       <c r="G147" s="42"/>
       <c r="H147" s="42"/>
       <c r="I147" s="3"/>
+      <c r="J147" s="4"/>
       <c r="K147" s="4"/>
       <c r="L147" s="44"/>
       <c r="M147" s="44"/>
@@ -5509,7 +5652,7 @@
     </row>
     <row r="150" spans="1:14" ht="18" customHeight="1">
       <c r="A150" s="24"/>
-      <c r="B150" s="52"/>
+      <c r="B150" s="44"/>
       <c r="C150" s="42"/>
       <c r="D150" s="42"/>
       <c r="E150" s="44"/>
@@ -5605,7 +5748,7 @@
     </row>
     <row r="156" spans="1:14" ht="18" customHeight="1">
       <c r="A156" s="24"/>
-      <c r="B156" s="44"/>
+      <c r="B156" s="52"/>
       <c r="C156" s="42"/>
       <c r="D156" s="42"/>
       <c r="E156" s="44"/>
@@ -5653,7 +5796,7 @@
     </row>
     <row r="159" spans="1:14" ht="18" customHeight="1">
       <c r="A159" s="24"/>
-      <c r="B159" s="52"/>
+      <c r="B159" s="44"/>
       <c r="C159" s="42"/>
       <c r="D159" s="42"/>
       <c r="E159" s="44"/>
@@ -5749,7 +5892,7 @@
     </row>
     <row r="165" spans="1:14" ht="18" customHeight="1">
       <c r="A165" s="24"/>
-      <c r="B165" s="44"/>
+      <c r="B165" s="52"/>
       <c r="C165" s="42"/>
       <c r="D165" s="42"/>
       <c r="E165" s="44"/>
@@ -5797,7 +5940,7 @@
     </row>
     <row r="168" spans="1:14" ht="18" customHeight="1">
       <c r="A168" s="24"/>
-      <c r="B168" s="52"/>
+      <c r="B168" s="44"/>
       <c r="C168" s="42"/>
       <c r="D168" s="42"/>
       <c r="E168" s="44"/>
@@ -6493,9 +6636,6 @@
       <c r="G211" s="42"/>
       <c r="H211" s="42"/>
       <c r="I211" s="3"/>
-      <c r="J211" s="4"/>
-      <c r="K211" s="4"/>
-      <c r="L211" s="44"/>
       <c r="M211" s="44"/>
       <c r="N211" s="44"/>
     </row>
@@ -6509,6 +6649,9 @@
       <c r="G212" s="42"/>
       <c r="H212" s="42"/>
       <c r="I212" s="3"/>
+      <c r="J212" s="4"/>
+      <c r="K212" s="4"/>
+      <c r="L212" s="44"/>
       <c r="M212" s="44"/>
       <c r="N212" s="44"/>
     </row>
@@ -6698,7 +6841,7 @@
       <c r="G224" s="42"/>
       <c r="H224" s="42"/>
       <c r="I224" s="3"/>
-      <c r="J224" s="4"/>
+      <c r="J224" s="42"/>
       <c r="K224" s="4"/>
       <c r="L224" s="44"/>
       <c r="M224" s="44"/>
@@ -6890,7 +7033,7 @@
       <c r="G236" s="42"/>
       <c r="H236" s="42"/>
       <c r="I236" s="3"/>
-      <c r="J236" s="42"/>
+      <c r="J236" s="4"/>
       <c r="K236" s="4"/>
       <c r="L236" s="44"/>
       <c r="M236" s="44"/>
@@ -7235,10 +7378,9 @@
     <row r="258" spans="1:14" ht="18" customHeight="1">
       <c r="A258" s="24"/>
       <c r="B258" s="44"/>
-      <c r="C258" s="42"/>
-      <c r="D258" s="42"/>
-      <c r="E258" s="44"/>
-      <c r="F258" s="42"/>
+      <c r="C258" s="2"/>
+      <c r="D258" s="2"/>
+      <c r="F258" s="2"/>
       <c r="G258" s="42"/>
       <c r="H258" s="42"/>
       <c r="I258" s="3"/>
@@ -7510,7 +7652,7 @@
       <c r="D276" s="2"/>
       <c r="F276" s="2"/>
       <c r="G276" s="42"/>
-      <c r="H276" s="42"/>
+      <c r="H276" s="2"/>
       <c r="I276" s="3"/>
       <c r="J276" s="4"/>
       <c r="K276" s="4"/>
@@ -7776,10 +7918,9 @@
     <row r="294" spans="1:14" ht="18" customHeight="1">
       <c r="A294" s="24"/>
       <c r="B294" s="44"/>
-      <c r="C294" s="2"/>
       <c r="D294" s="2"/>
       <c r="F294" s="2"/>
-      <c r="G294" s="42"/>
+      <c r="G294" s="2"/>
       <c r="H294" s="2"/>
       <c r="I294" s="3"/>
       <c r="J294" s="4"/>
@@ -7915,7 +8056,7 @@
       <c r="N303" s="44"/>
     </row>
     <row r="304" spans="1:14" ht="18" customHeight="1">
-      <c r="A304" s="24"/>
+      <c r="A304" s="44"/>
       <c r="B304" s="44"/>
       <c r="D304" s="2"/>
       <c r="F304" s="2"/>
@@ -8035,7 +8176,6 @@
       <c r="H312" s="2"/>
       <c r="I312" s="3"/>
       <c r="J312" s="4"/>
-      <c r="K312" s="4"/>
       <c r="L312" s="44"/>
       <c r="M312" s="44"/>
       <c r="N312" s="44"/>
@@ -8049,6 +8189,7 @@
       <c r="H313" s="2"/>
       <c r="I313" s="3"/>
       <c r="J313" s="4"/>
+      <c r="K313" s="4"/>
       <c r="L313" s="44"/>
       <c r="M313" s="44"/>
       <c r="N313" s="44"/>
@@ -8196,6 +8337,7 @@
     <row r="324" spans="1:14" ht="18" customHeight="1">
       <c r="A324" s="44"/>
       <c r="B324" s="44"/>
+      <c r="C324" s="2"/>
       <c r="D324" s="2"/>
       <c r="F324" s="2"/>
       <c r="G324" s="2"/>
@@ -8308,7 +8450,7 @@
       <c r="I331" s="3"/>
       <c r="J331" s="4"/>
       <c r="K331" s="4"/>
-      <c r="L331" s="44"/>
+      <c r="L331" s="52"/>
       <c r="M331" s="44"/>
       <c r="N331" s="44"/>
     </row>
@@ -8323,7 +8465,7 @@
       <c r="I332" s="3"/>
       <c r="J332" s="4"/>
       <c r="K332" s="4"/>
-      <c r="L332" s="52"/>
+      <c r="L332" s="44"/>
       <c r="M332" s="44"/>
       <c r="N332" s="44"/>
     </row>
@@ -8412,9 +8554,8 @@
       <c r="H338" s="2"/>
       <c r="I338" s="3"/>
       <c r="J338" s="4"/>
-      <c r="K338" s="4"/>
       <c r="L338" s="44"/>
-      <c r="M338" s="44"/>
+      <c r="M338" s="4"/>
       <c r="N338" s="44"/>
     </row>
     <row r="339" spans="1:14" ht="18" customHeight="1">
@@ -8511,8 +8652,9 @@
       <c r="H345" s="2"/>
       <c r="I345" s="3"/>
       <c r="J345" s="4"/>
+      <c r="K345" s="4"/>
       <c r="L345" s="44"/>
-      <c r="M345" s="4"/>
+      <c r="M345" s="44"/>
       <c r="N345" s="44"/>
     </row>
     <row r="346" spans="1:14" ht="18" customHeight="1">
@@ -8563,8 +8705,6 @@
     <row r="349" spans="1:14" ht="18" customHeight="1">
       <c r="A349" s="44"/>
       <c r="B349" s="44"/>
-      <c r="C349" s="2"/>
-      <c r="D349" s="2"/>
       <c r="F349" s="2"/>
       <c r="G349" s="2"/>
       <c r="H349" s="2"/>
@@ -8591,6 +8731,8 @@
     <row r="351" spans="1:14" ht="18" customHeight="1">
       <c r="A351" s="44"/>
       <c r="B351" s="44"/>
+      <c r="C351" s="2"/>
+      <c r="D351" s="2"/>
       <c r="F351" s="2"/>
       <c r="G351" s="2"/>
       <c r="H351" s="2"/>
@@ -8606,6 +8748,7 @@
       <c r="B352" s="44"/>
       <c r="C352" s="2"/>
       <c r="D352" s="2"/>
+      <c r="E352" s="53"/>
       <c r="F352" s="2"/>
       <c r="G352" s="2"/>
       <c r="H352" s="2"/>
@@ -8717,7 +8860,6 @@
       <c r="B359" s="44"/>
       <c r="C359" s="2"/>
       <c r="D359" s="2"/>
-      <c r="E359" s="53"/>
       <c r="F359" s="2"/>
       <c r="G359" s="2"/>
       <c r="H359" s="2"/>
@@ -8733,6 +8875,7 @@
       <c r="B360" s="44"/>
       <c r="C360" s="2"/>
       <c r="D360" s="2"/>
+      <c r="E360" s="53"/>
       <c r="F360" s="2"/>
       <c r="G360" s="2"/>
       <c r="H360" s="2"/>
@@ -8796,7 +8939,6 @@
       <c r="B364" s="44"/>
       <c r="C364" s="2"/>
       <c r="D364" s="2"/>
-      <c r="E364" s="53"/>
       <c r="F364" s="2"/>
       <c r="G364" s="2"/>
       <c r="H364" s="2"/>
@@ -8812,6 +8954,7 @@
       <c r="B365" s="44"/>
       <c r="C365" s="2"/>
       <c r="D365" s="2"/>
+      <c r="E365" s="53"/>
       <c r="F365" s="2"/>
       <c r="G365" s="2"/>
       <c r="H365" s="2"/>
@@ -8875,7 +9018,6 @@
       <c r="B369" s="44"/>
       <c r="C369" s="2"/>
       <c r="D369" s="2"/>
-      <c r="E369" s="53"/>
       <c r="F369" s="2"/>
       <c r="G369" s="2"/>
       <c r="H369" s="2"/>
@@ -8891,6 +9033,7 @@
       <c r="B370" s="44"/>
       <c r="C370" s="2"/>
       <c r="D370" s="2"/>
+      <c r="E370" s="53"/>
       <c r="F370" s="2"/>
       <c r="G370" s="2"/>
       <c r="H370" s="2"/>
@@ -8970,7 +9113,6 @@
       <c r="B375" s="44"/>
       <c r="C375" s="2"/>
       <c r="D375" s="2"/>
-      <c r="E375" s="53"/>
       <c r="F375" s="2"/>
       <c r="G375" s="2"/>
       <c r="H375" s="2"/>
@@ -9061,6 +9203,7 @@
       <c r="B381" s="44"/>
       <c r="C381" s="2"/>
       <c r="D381" s="2"/>
+      <c r="E381" s="53"/>
       <c r="F381" s="2"/>
       <c r="G381" s="2"/>
       <c r="H381" s="2"/>
@@ -9076,7 +9219,6 @@
       <c r="B382" s="44"/>
       <c r="C382" s="2"/>
       <c r="D382" s="2"/>
-      <c r="E382" s="53"/>
       <c r="F382" s="2"/>
       <c r="G382" s="2"/>
       <c r="H382" s="2"/>
@@ -9167,6 +9309,7 @@
       <c r="B388" s="44"/>
       <c r="C388" s="2"/>
       <c r="D388" s="2"/>
+      <c r="E388" s="53"/>
       <c r="F388" s="2"/>
       <c r="G388" s="2"/>
       <c r="H388" s="2"/>
@@ -9182,7 +9325,6 @@
       <c r="B389" s="44"/>
       <c r="C389" s="2"/>
       <c r="D389" s="2"/>
-      <c r="E389" s="53"/>
       <c r="F389" s="2"/>
       <c r="G389" s="2"/>
       <c r="H389" s="2"/>
@@ -9273,6 +9415,7 @@
       <c r="B395" s="44"/>
       <c r="C395" s="2"/>
       <c r="D395" s="2"/>
+      <c r="E395" s="53"/>
       <c r="F395" s="2"/>
       <c r="G395" s="2"/>
       <c r="H395" s="2"/>
@@ -9288,7 +9431,6 @@
       <c r="B396" s="44"/>
       <c r="C396" s="2"/>
       <c r="D396" s="2"/>
-      <c r="E396" s="53"/>
       <c r="F396" s="2"/>
       <c r="G396" s="2"/>
       <c r="H396" s="2"/>
@@ -9324,7 +9466,6 @@
       <c r="H398" s="2"/>
       <c r="I398" s="3"/>
       <c r="J398" s="4"/>
-      <c r="K398" s="4"/>
       <c r="L398" s="44"/>
       <c r="M398" s="44"/>
       <c r="N398" s="44"/>
@@ -9339,6 +9480,7 @@
       <c r="H399" s="2"/>
       <c r="I399" s="3"/>
       <c r="J399" s="4"/>
+      <c r="K399" s="4"/>
       <c r="L399" s="44"/>
       <c r="M399" s="44"/>
       <c r="N399" s="44"/>
@@ -9378,6 +9520,7 @@
       <c r="B402" s="44"/>
       <c r="C402" s="2"/>
       <c r="D402" s="2"/>
+      <c r="E402" s="53"/>
       <c r="F402" s="2"/>
       <c r="G402" s="2"/>
       <c r="H402" s="2"/>
@@ -9393,7 +9536,6 @@
       <c r="B403" s="44"/>
       <c r="C403" s="2"/>
       <c r="D403" s="2"/>
-      <c r="E403" s="53"/>
       <c r="F403" s="2"/>
       <c r="G403" s="2"/>
       <c r="H403" s="2"/>
@@ -9779,7 +9921,7 @@
       <c r="M428" s="44"/>
       <c r="N428" s="44"/>
     </row>
-    <row r="429" spans="1:14" ht="18" customHeight="1">
+    <row r="429" spans="1:14">
       <c r="A429" s="44"/>
       <c r="B429" s="44"/>
       <c r="C429" s="2"/>
@@ -9788,8 +9930,6 @@
       <c r="G429" s="2"/>
       <c r="H429" s="2"/>
       <c r="I429" s="3"/>
-      <c r="J429" s="4"/>
-      <c r="K429" s="4"/>
       <c r="L429" s="44"/>
       <c r="M429" s="44"/>
       <c r="N429" s="44"/>
@@ -9828,7 +9968,6 @@
       <c r="F432" s="2"/>
       <c r="G432" s="2"/>
       <c r="H432" s="2"/>
-      <c r="I432" s="3"/>
       <c r="L432" s="44"/>
       <c r="M432" s="44"/>
       <c r="N432" s="44"/>
@@ -9913,8 +10052,7 @@
       <c r="F439" s="2"/>
       <c r="G439" s="2"/>
       <c r="H439" s="2"/>
-      <c r="L439" s="44"/>
-      <c r="M439" s="44"/>
+      <c r="I439" s="3"/>
       <c r="N439" s="44"/>
     </row>
     <row r="440" spans="1:14">
@@ -10145,7 +10283,6 @@
       <c r="F460" s="2"/>
       <c r="G460" s="2"/>
       <c r="H460" s="2"/>
-      <c r="I460" s="3"/>
       <c r="N460" s="44"/>
     </row>
     <row r="461" spans="1:14">
@@ -10216,6 +10353,7 @@
       <c r="F467" s="2"/>
       <c r="G467" s="2"/>
       <c r="H467" s="2"/>
+      <c r="I467" s="3"/>
       <c r="N467" s="44"/>
     </row>
     <row r="468" spans="1:14">
@@ -10259,7 +10397,6 @@
       <c r="F471" s="2"/>
       <c r="G471" s="2"/>
       <c r="H471" s="2"/>
-      <c r="I471" s="3"/>
       <c r="N471" s="44"/>
     </row>
     <row r="472" spans="1:14">
@@ -10283,14 +10420,9 @@
       <c r="N473" s="44"/>
     </row>
     <row r="474" spans="1:14">
-      <c r="A474" s="44"/>
       <c r="B474" s="44"/>
-      <c r="C474" s="2"/>
-      <c r="D474" s="2"/>
-      <c r="F474" s="2"/>
-      <c r="G474" s="2"/>
-      <c r="H474" s="2"/>
-      <c r="N474" s="44"/>
+      <c r="J474" s="4"/>
+      <c r="K474" s="4"/>
     </row>
     <row r="475" spans="1:14">
       <c r="B475" s="44"/>
@@ -10322,54 +10454,52 @@
       <c r="J480" s="4"/>
       <c r="K480" s="4"/>
     </row>
-    <row r="481" spans="2:11">
+    <row r="481" spans="2:2">
       <c r="B481" s="44"/>
-      <c r="J481" s="4"/>
-      <c r="K481" s="4"/>
-    </row>
-    <row r="482" spans="2:11">
+    </row>
+    <row r="482" spans="2:2">
       <c r="B482" s="44"/>
     </row>
-    <row r="483" spans="2:11">
+    <row r="483" spans="2:2">
       <c r="B483" s="44"/>
     </row>
-    <row r="484" spans="2:11">
+    <row r="484" spans="2:2">
       <c r="B484" s="44"/>
     </row>
-    <row r="485" spans="2:11">
+    <row r="485" spans="2:2">
       <c r="B485" s="44"/>
     </row>
-    <row r="486" spans="2:11">
+    <row r="486" spans="2:2">
       <c r="B486" s="44"/>
     </row>
-    <row r="487" spans="2:11">
+    <row r="487" spans="2:2">
       <c r="B487" s="44"/>
     </row>
-    <row r="488" spans="2:11">
+    <row r="488" spans="2:2">
       <c r="B488" s="44"/>
     </row>
-    <row r="489" spans="2:11">
+    <row r="489" spans="2:2">
       <c r="B489" s="44"/>
     </row>
-    <row r="490" spans="2:11">
+    <row r="490" spans="2:2">
       <c r="B490" s="44"/>
     </row>
-    <row r="491" spans="2:11">
+    <row r="491" spans="2:2">
       <c r="B491" s="44"/>
     </row>
-    <row r="492" spans="2:11">
+    <row r="492" spans="2:2">
       <c r="B492" s="44"/>
     </row>
-    <row r="493" spans="2:11">
+    <row r="493" spans="2:2">
       <c r="B493" s="44"/>
     </row>
-    <row r="494" spans="2:11">
+    <row r="494" spans="2:2">
       <c r="B494" s="44"/>
     </row>
-    <row r="495" spans="2:11">
+    <row r="495" spans="2:2">
       <c r="B495" s="44"/>
     </row>
-    <row r="496" spans="2:11">
+    <row r="496" spans="2:2">
       <c r="B496" s="44"/>
     </row>
     <row r="497" spans="2:11">
@@ -10413,6 +10543,8 @@
     </row>
     <row r="510" spans="2:11">
       <c r="B510" s="44"/>
+      <c r="J510" s="4"/>
+      <c r="K510" s="4"/>
     </row>
     <row r="511" spans="2:11">
       <c r="B511" s="44"/>
@@ -10436,8 +10568,6 @@
     </row>
     <row r="515" spans="2:11">
       <c r="B515" s="44"/>
-      <c r="J515" s="4"/>
-      <c r="K515" s="4"/>
     </row>
     <row r="516" spans="2:11">
       <c r="B516" s="44"/>
@@ -10558,6 +10688,10 @@
     </row>
     <row r="555" spans="2:17">
       <c r="B555" s="44"/>
+      <c r="J555" s="4"/>
+      <c r="K555" s="4"/>
+      <c r="P555" s="50"/>
+      <c r="Q555" s="50"/>
     </row>
     <row r="556" spans="2:17">
       <c r="B556" s="44"/>
@@ -10589,10 +10723,7 @@
     </row>
     <row r="560" spans="2:17">
       <c r="B560" s="44"/>
-      <c r="J560" s="4"/>
-      <c r="K560" s="4"/>
-      <c r="P560" s="50"/>
-      <c r="Q560" s="50"/>
+      <c r="P560"/>
     </row>
     <row r="561" spans="2:16">
       <c r="B561" s="44"/>
@@ -10611,8 +10742,8 @@
       <c r="P564"/>
     </row>
     <row r="565" spans="2:16">
-      <c r="B565" s="44"/>
-      <c r="P565"/>
+      <c r="B565" s="54"/>
+      <c r="C565" s="54"/>
     </row>
     <row r="566" spans="2:16">
       <c r="B566" s="54"/>
@@ -10683,8 +10814,11 @@
       <c r="C582" s="54"/>
     </row>
     <row r="583" spans="1:5">
-      <c r="B583" s="54"/>
-      <c r="C583" s="54"/>
+      <c r="A583" s="52"/>
+      <c r="B583" s="55"/>
+      <c r="C583" s="55"/>
+      <c r="D583" s="56"/>
+      <c r="E583" s="55"/>
     </row>
     <row r="584" spans="1:5">
       <c r="A584" s="52"/>
@@ -10722,11 +10856,8 @@
       <c r="E588" s="55"/>
     </row>
     <row r="589" spans="1:5">
-      <c r="A589" s="52"/>
-      <c r="B589" s="55"/>
-      <c r="C589" s="55"/>
-      <c r="D589" s="56"/>
-      <c r="E589" s="55"/>
+      <c r="B589" s="54"/>
+      <c r="C589" s="54"/>
     </row>
     <row r="590" spans="1:5">
       <c r="B590" s="54"/>
@@ -10773,8 +10904,11 @@
       <c r="C600" s="54"/>
     </row>
     <row r="601" spans="1:9">
-      <c r="B601" s="54"/>
-      <c r="C601" s="54"/>
+      <c r="A601" s="52"/>
+      <c r="B601" s="55"/>
+      <c r="C601" s="55"/>
+      <c r="D601" s="56"/>
+      <c r="E601" s="55"/>
     </row>
     <row r="602" spans="1:9">
       <c r="A602" s="52"/>
@@ -10817,6 +10951,9 @@
       <c r="C607" s="55"/>
       <c r="D607" s="56"/>
       <c r="E607" s="55"/>
+      <c r="F607" s="56"/>
+      <c r="H607" s="56"/>
+      <c r="I607" s="57"/>
     </row>
     <row r="608" spans="1:9">
       <c r="A608" s="52"/>
@@ -10989,14 +11126,8 @@
       <c r="I624" s="57"/>
     </row>
     <row r="625" spans="1:14">
-      <c r="A625" s="52"/>
       <c r="B625" s="55"/>
-      <c r="C625" s="55"/>
-      <c r="D625" s="56"/>
       <c r="E625" s="55"/>
-      <c r="F625" s="56"/>
-      <c r="H625" s="56"/>
-      <c r="I625" s="57"/>
     </row>
     <row r="626" spans="1:14">
       <c r="B626" s="55"/>
@@ -11018,9 +11149,21 @@
       <c r="B630" s="55"/>
       <c r="E630" s="55"/>
     </row>
-    <row r="631" spans="1:14">
-      <c r="B631" s="55"/>
-      <c r="E631" s="55"/>
+    <row r="631" spans="1:14" ht="16">
+      <c r="A631" s="58"/>
+      <c r="B631" s="59"/>
+      <c r="C631" s="58"/>
+      <c r="D631" s="58"/>
+      <c r="E631" s="59"/>
+      <c r="F631" s="59"/>
+      <c r="G631" s="59"/>
+      <c r="H631" s="60"/>
+      <c r="I631" s="61"/>
+      <c r="J631" s="62"/>
+      <c r="K631" s="62"/>
+      <c r="L631" s="59"/>
+      <c r="M631" s="59"/>
+      <c r="N631" s="63"/>
     </row>
     <row r="632" spans="1:14" ht="16">
       <c r="A632" s="58"/>
@@ -11116,10 +11259,9 @@
       <c r="K637" s="62"/>
       <c r="L637" s="59"/>
       <c r="M637" s="59"/>
-      <c r="N637" s="63"/>
+      <c r="N637" s="80"/>
     </row>
     <row r="638" spans="1:14" ht="16">
-      <c r="A638" s="58"/>
       <c r="B638" s="59"/>
       <c r="C638" s="58"/>
       <c r="D638" s="58"/>
@@ -11128,10 +11270,6 @@
       <c r="G638" s="59"/>
       <c r="H638" s="60"/>
       <c r="I638" s="61"/>
-      <c r="J638" s="62"/>
-      <c r="K638" s="62"/>
-      <c r="L638" s="59"/>
-      <c r="M638" s="59"/>
       <c r="N638" s="80"/>
     </row>
     <row r="639" spans="1:14" ht="16">
@@ -11190,6 +11328,7 @@
       <c r="N643" s="80"/>
     </row>
     <row r="644" spans="1:18" ht="16">
+      <c r="A644" s="58"/>
       <c r="B644" s="59"/>
       <c r="C644" s="58"/>
       <c r="D644" s="58"/>
@@ -11198,7 +11337,11 @@
       <c r="G644" s="59"/>
       <c r="H644" s="60"/>
       <c r="I644" s="61"/>
-      <c r="N644" s="80"/>
+      <c r="J644" s="62"/>
+      <c r="K644" s="62"/>
+      <c r="L644" s="59"/>
+      <c r="M644" s="59"/>
+      <c r="N644" s="81"/>
     </row>
     <row r="645" spans="1:18" ht="16">
       <c r="A645" s="58"/>
@@ -11240,13 +11383,11 @@
       <c r="E647" s="59"/>
       <c r="F647" s="59"/>
       <c r="G647" s="59"/>
-      <c r="H647" s="60"/>
-      <c r="I647" s="61"/>
-      <c r="J647" s="62"/>
-      <c r="K647" s="62"/>
       <c r="L647" s="59"/>
       <c r="M647" s="59"/>
       <c r="N647" s="81"/>
+      <c r="P647" s="65"/>
+      <c r="R647" s="65"/>
     </row>
     <row r="648" spans="1:18" ht="16">
       <c r="A648" s="58"/>
@@ -11354,10 +11495,10 @@
       <c r="E655" s="59"/>
       <c r="F655" s="59"/>
       <c r="G655" s="59"/>
+      <c r="J655" s="51"/>
       <c r="L655" s="59"/>
       <c r="M655" s="59"/>
       <c r="N655" s="81"/>
-      <c r="P655" s="65"/>
       <c r="R655" s="65"/>
     </row>
     <row r="656" spans="1:18" ht="16">
@@ -11410,11 +11551,18 @@
       <c r="E659" s="59"/>
       <c r="F659" s="59"/>
       <c r="G659" s="59"/>
-      <c r="J659" s="51"/>
+      <c r="H659" s="60"/>
+      <c r="I659" s="61"/>
+      <c r="J659" s="62"/>
+      <c r="K659" s="62"/>
       <c r="L659" s="59"/>
       <c r="M659" s="59"/>
       <c r="N659" s="81"/>
-      <c r="R659" s="65"/>
+      <c r="O659" s="70"/>
+      <c r="P659" s="71"/>
+      <c r="Q659" s="71"/>
+      <c r="R659" s="70"/>
+      <c r="S659" s="70"/>
     </row>
     <row r="660" spans="1:19" ht="16">
       <c r="A660" s="58"/>
@@ -11485,17 +11633,17 @@
       <c r="C663" s="58"/>
       <c r="D663" s="58"/>
       <c r="E663" s="59"/>
-      <c r="F663" s="59"/>
+      <c r="F663" s="72"/>
       <c r="G663" s="59"/>
       <c r="H663" s="60"/>
       <c r="I663" s="61"/>
-      <c r="J663" s="62"/>
-      <c r="K663" s="62"/>
-      <c r="L663" s="59"/>
-      <c r="M663" s="59"/>
+      <c r="J663" s="73"/>
+      <c r="K663" s="75"/>
+      <c r="L663" s="74"/>
+      <c r="M663" s="74"/>
       <c r="N663" s="81"/>
       <c r="O663" s="70"/>
-      <c r="P663" s="71"/>
+      <c r="P663" s="75"/>
       <c r="Q663" s="71"/>
       <c r="R663" s="70"/>
       <c r="S663" s="70"/>
@@ -11511,7 +11659,7 @@
       <c r="H664" s="60"/>
       <c r="I664" s="61"/>
       <c r="J664" s="73"/>
-      <c r="K664" s="75"/>
+      <c r="K664" s="73"/>
       <c r="L664" s="74"/>
       <c r="M664" s="74"/>
       <c r="N664" s="81"/>
@@ -11572,7 +11720,7 @@
       <c r="F667" s="72"/>
       <c r="G667" s="59"/>
       <c r="H667" s="60"/>
-      <c r="I667" s="61"/>
+      <c r="I667" s="76"/>
       <c r="J667" s="73"/>
       <c r="K667" s="73"/>
       <c r="L667" s="74"/>
@@ -11824,7 +11972,7 @@
       <c r="F679" s="72"/>
       <c r="G679" s="59"/>
       <c r="H679" s="60"/>
-      <c r="I679" s="76"/>
+      <c r="I679" s="61"/>
       <c r="J679" s="73"/>
       <c r="K679" s="73"/>
       <c r="L679" s="74"/>
@@ -11908,7 +12056,7 @@
       <c r="F683" s="72"/>
       <c r="G683" s="59"/>
       <c r="H683" s="60"/>
-      <c r="I683" s="61"/>
+      <c r="I683" s="76"/>
       <c r="J683" s="73"/>
       <c r="K683" s="73"/>
       <c r="L683" s="74"/>
@@ -12036,7 +12184,7 @@
       <c r="H689" s="60"/>
       <c r="I689" s="76"/>
       <c r="J689" s="73"/>
-      <c r="K689" s="73"/>
+      <c r="K689" s="82"/>
       <c r="L689" s="74"/>
       <c r="M689" s="74"/>
       <c r="N689" s="81"/>
@@ -12057,7 +12205,7 @@
       <c r="H690" s="60"/>
       <c r="I690" s="76"/>
       <c r="J690" s="73"/>
-      <c r="K690" s="82"/>
+      <c r="K690" s="70"/>
       <c r="L690" s="74"/>
       <c r="M690" s="74"/>
       <c r="N690" s="81"/>
@@ -12078,7 +12226,7 @@
       <c r="H691" s="60"/>
       <c r="I691" s="76"/>
       <c r="J691" s="73"/>
-      <c r="K691" s="70"/>
+      <c r="K691" s="75"/>
       <c r="L691" s="74"/>
       <c r="M691" s="74"/>
       <c r="N691" s="81"/>
@@ -12152,22 +12300,22 @@
       <c r="S694" s="70"/>
     </row>
     <row r="695" spans="1:19" ht="16">
-      <c r="A695" s="58"/>
-      <c r="B695" s="59"/>
-      <c r="C695" s="58"/>
-      <c r="D695" s="58"/>
-      <c r="E695" s="59"/>
-      <c r="F695" s="72"/>
-      <c r="G695" s="59"/>
+      <c r="A695" s="66"/>
+      <c r="B695" s="67"/>
+      <c r="C695" s="66"/>
+      <c r="D695" s="66"/>
+      <c r="E695" s="67"/>
+      <c r="F695" s="77"/>
+      <c r="G695" s="67"/>
       <c r="H695" s="60"/>
-      <c r="I695" s="76"/>
-      <c r="J695" s="73"/>
-      <c r="K695" s="75"/>
+      <c r="I695" s="68"/>
+      <c r="J695" s="75"/>
+      <c r="K695" s="70"/>
       <c r="L695" s="74"/>
       <c r="M695" s="74"/>
       <c r="N695" s="81"/>
       <c r="O695" s="70"/>
-      <c r="P695" s="75"/>
+      <c r="P695" s="71"/>
       <c r="Q695" s="71"/>
       <c r="R695" s="70"/>
       <c r="S695" s="70"/>
@@ -12183,7 +12331,7 @@
       <c r="H696" s="60"/>
       <c r="I696" s="68"/>
       <c r="J696" s="75"/>
-      <c r="K696" s="70"/>
+      <c r="K696" s="75"/>
       <c r="L696" s="74"/>
       <c r="M696" s="74"/>
       <c r="N696" s="81"/>
@@ -12244,8 +12392,8 @@
       <c r="F699" s="77"/>
       <c r="G699" s="67"/>
       <c r="H699" s="60"/>
-      <c r="I699" s="68"/>
-      <c r="J699" s="75"/>
+      <c r="I699" s="78"/>
+      <c r="J699" s="71"/>
       <c r="K699" s="75"/>
       <c r="L699" s="74"/>
       <c r="M699" s="74"/>
@@ -12267,7 +12415,7 @@
       <c r="H700" s="60"/>
       <c r="I700" s="78"/>
       <c r="J700" s="71"/>
-      <c r="K700" s="75"/>
+      <c r="K700" s="70"/>
       <c r="L700" s="74"/>
       <c r="M700" s="74"/>
       <c r="N700" s="81"/>
@@ -12288,7 +12436,7 @@
       <c r="H701" s="60"/>
       <c r="I701" s="78"/>
       <c r="J701" s="71"/>
-      <c r="K701" s="70"/>
+      <c r="K701" s="75"/>
       <c r="L701" s="74"/>
       <c r="M701" s="74"/>
       <c r="N701" s="81"/>
@@ -12372,7 +12520,7 @@
       <c r="H705" s="60"/>
       <c r="I705" s="78"/>
       <c r="J705" s="71"/>
-      <c r="K705" s="75"/>
+      <c r="K705" s="70"/>
       <c r="L705" s="74"/>
       <c r="M705" s="74"/>
       <c r="N705" s="81"/>
@@ -12393,7 +12541,7 @@
       <c r="H706" s="60"/>
       <c r="I706" s="78"/>
       <c r="J706" s="71"/>
-      <c r="K706" s="70"/>
+      <c r="K706" s="75"/>
       <c r="L706" s="74"/>
       <c r="M706" s="74"/>
       <c r="N706" s="81"/>
@@ -12477,7 +12625,7 @@
       <c r="H710" s="60"/>
       <c r="I710" s="78"/>
       <c r="J710" s="71"/>
-      <c r="K710" s="75"/>
+      <c r="K710" s="73"/>
       <c r="L710" s="74"/>
       <c r="M710" s="74"/>
       <c r="N710" s="81"/>
@@ -12488,16 +12636,16 @@
       <c r="S710" s="70"/>
     </row>
     <row r="711" spans="1:19" ht="16">
-      <c r="A711" s="66"/>
-      <c r="B711" s="67"/>
-      <c r="C711" s="66"/>
-      <c r="D711" s="66"/>
-      <c r="E711" s="67"/>
-      <c r="F711" s="77"/>
-      <c r="G711" s="67"/>
+      <c r="A711" s="58"/>
+      <c r="B711" s="59"/>
+      <c r="C711" s="58"/>
+      <c r="D711" s="58"/>
+      <c r="E711" s="59"/>
+      <c r="F711" s="59"/>
+      <c r="G711" s="59"/>
       <c r="H711" s="60"/>
-      <c r="I711" s="78"/>
-      <c r="J711" s="71"/>
+      <c r="I711" s="61"/>
+      <c r="J711" s="73"/>
       <c r="K711" s="73"/>
       <c r="L711" s="74"/>
       <c r="M711" s="74"/>
@@ -12581,13 +12729,13 @@
       <c r="G715" s="59"/>
       <c r="H715" s="60"/>
       <c r="I715" s="61"/>
-      <c r="J715" s="73"/>
-      <c r="K715" s="73"/>
-      <c r="L715" s="74"/>
-      <c r="M715" s="74"/>
-      <c r="N715" s="81"/>
+      <c r="J715" s="62"/>
+      <c r="K715" s="62"/>
+      <c r="L715" s="59"/>
+      <c r="M715" s="59"/>
+      <c r="N715" s="69"/>
       <c r="O715" s="70"/>
-      <c r="P715" s="71"/>
+      <c r="P715" s="75"/>
       <c r="Q715" s="71"/>
       <c r="R715" s="70"/>
       <c r="S715" s="70"/>
@@ -12713,7 +12861,7 @@
       <c r="M721" s="59"/>
       <c r="N721" s="69"/>
       <c r="O721" s="70"/>
-      <c r="P721" s="75"/>
+      <c r="P721" s="71"/>
       <c r="Q721" s="71"/>
       <c r="R721" s="70"/>
       <c r="S721" s="70"/>
@@ -12740,7 +12888,7 @@
       <c r="S722" s="70"/>
     </row>
     <row r="723" spans="1:19" ht="16">
-      <c r="A723" s="58"/>
+      <c r="A723" s="79"/>
       <c r="B723" s="59"/>
       <c r="C723" s="58"/>
       <c r="D723" s="58"/>
@@ -12750,12 +12898,12 @@
       <c r="H723" s="60"/>
       <c r="I723" s="61"/>
       <c r="J723" s="62"/>
-      <c r="K723" s="62"/>
+      <c r="K723" s="73"/>
       <c r="L723" s="59"/>
       <c r="M723" s="59"/>
       <c r="N723" s="69"/>
       <c r="O723" s="70"/>
-      <c r="P723" s="71"/>
+      <c r="P723" s="75"/>
       <c r="Q723" s="71"/>
       <c r="R723" s="70"/>
       <c r="S723" s="70"/>
@@ -12797,7 +12945,7 @@
       <c r="M725" s="59"/>
       <c r="N725" s="69"/>
       <c r="O725" s="70"/>
-      <c r="P725" s="75"/>
+      <c r="P725" s="71"/>
       <c r="Q725" s="71"/>
       <c r="R725" s="70"/>
       <c r="S725" s="70"/>
@@ -12833,9 +12981,9 @@
       <c r="G727" s="59"/>
       <c r="H727" s="60"/>
       <c r="I727" s="61"/>
-      <c r="J727" s="62"/>
+      <c r="J727" s="71"/>
       <c r="K727" s="73"/>
-      <c r="L727" s="59"/>
+      <c r="L727" s="74"/>
       <c r="M727" s="59"/>
       <c r="N727" s="69"/>
       <c r="O727" s="70"/>
@@ -13001,13 +13149,13 @@
       <c r="G735" s="59"/>
       <c r="H735" s="60"/>
       <c r="I735" s="61"/>
-      <c r="J735" s="71"/>
+      <c r="J735" s="73"/>
       <c r="K735" s="73"/>
       <c r="L735" s="74"/>
-      <c r="M735" s="59"/>
+      <c r="M735" s="74"/>
       <c r="N735" s="69"/>
       <c r="O735" s="70"/>
-      <c r="P735" s="71"/>
+      <c r="P735" s="75"/>
       <c r="Q735" s="71"/>
       <c r="R735" s="70"/>
       <c r="S735" s="70"/>
@@ -13106,13 +13254,13 @@
       <c r="G740" s="59"/>
       <c r="H740" s="60"/>
       <c r="I740" s="61"/>
-      <c r="J740" s="73"/>
+      <c r="J740" s="71"/>
       <c r="K740" s="73"/>
       <c r="L740" s="74"/>
       <c r="M740" s="74"/>
       <c r="N740" s="69"/>
       <c r="O740" s="70"/>
-      <c r="P740" s="75"/>
+      <c r="P740" s="71"/>
       <c r="Q740" s="71"/>
       <c r="R740" s="70"/>
       <c r="S740" s="70"/>
@@ -13127,7 +13275,7 @@
       <c r="G741" s="59"/>
       <c r="H741" s="60"/>
       <c r="I741" s="61"/>
-      <c r="J741" s="71"/>
+      <c r="J741" s="75"/>
       <c r="K741" s="73"/>
       <c r="L741" s="74"/>
       <c r="M741" s="74"/>
@@ -13159,26 +13307,16 @@
       <c r="R742" s="70"/>
       <c r="S742" s="70"/>
     </row>
-    <row r="743" spans="1:19" ht="16">
-      <c r="A743" s="79"/>
+    <row r="743" spans="1:19" s="58" customFormat="1" ht="16">
       <c r="B743" s="59"/>
-      <c r="C743" s="58"/>
-      <c r="D743" s="58"/>
       <c r="E743" s="59"/>
       <c r="F743" s="59"/>
       <c r="G743" s="59"/>
       <c r="H743" s="60"/>
-      <c r="I743" s="61"/>
-      <c r="J743" s="75"/>
-      <c r="K743" s="73"/>
-      <c r="L743" s="74"/>
-      <c r="M743" s="74"/>
-      <c r="N743" s="69"/>
-      <c r="O743" s="70"/>
-      <c r="P743" s="71"/>
-      <c r="Q743" s="71"/>
-      <c r="R743" s="70"/>
-      <c r="S743" s="70"/>
+      <c r="J743" s="62"/>
+      <c r="K743" s="62"/>
+      <c r="L743" s="59"/>
+      <c r="M743" s="59"/>
     </row>
     <row r="744" spans="1:19" s="58" customFormat="1" ht="16">
       <c r="B744" s="59"/>
@@ -13191,16 +13329,26 @@
       <c r="L744" s="59"/>
       <c r="M744" s="59"/>
     </row>
-    <row r="745" spans="1:19" s="58" customFormat="1" ht="16">
+    <row r="745" spans="1:19" ht="16">
+      <c r="A745" s="58"/>
       <c r="B745" s="59"/>
+      <c r="C745" s="58"/>
+      <c r="D745" s="58"/>
       <c r="E745" s="59"/>
       <c r="F745" s="59"/>
       <c r="G745" s="59"/>
       <c r="H745" s="60"/>
-      <c r="J745" s="62"/>
-      <c r="K745" s="62"/>
+      <c r="I745" s="76"/>
+      <c r="J745" s="83"/>
+      <c r="K745" s="73"/>
       <c r="L745" s="59"/>
       <c r="M745" s="59"/>
+      <c r="N745" s="58"/>
+      <c r="O745" s="70"/>
+      <c r="P745" s="71"/>
+      <c r="Q745" s="71"/>
+      <c r="R745" s="70"/>
+      <c r="S745" s="70"/>
     </row>
     <row r="746" spans="1:19" ht="16">
       <c r="A746" s="58"/>
@@ -13224,7 +13372,7 @@
       <c r="S746" s="70"/>
     </row>
     <row r="747" spans="1:19" ht="16">
-      <c r="A747" s="58"/>
+      <c r="A747" s="79"/>
       <c r="B747" s="59"/>
       <c r="C747" s="58"/>
       <c r="D747" s="58"/>
@@ -13232,11 +13380,11 @@
       <c r="F747" s="59"/>
       <c r="G747" s="59"/>
       <c r="H747" s="60"/>
-      <c r="I747" s="76"/>
-      <c r="J747" s="83"/>
+      <c r="I747" s="58"/>
+      <c r="J747" s="84"/>
       <c r="K747" s="73"/>
       <c r="L747" s="59"/>
-      <c r="M747" s="59"/>
+      <c r="M747" s="74"/>
       <c r="N747" s="58"/>
       <c r="O747" s="70"/>
       <c r="P747" s="71"/>
@@ -13274,8 +13422,8 @@
       <c r="F749" s="59"/>
       <c r="G749" s="59"/>
       <c r="H749" s="60"/>
-      <c r="I749" s="58"/>
-      <c r="J749" s="84"/>
+      <c r="I749" s="76"/>
+      <c r="J749" s="83"/>
       <c r="K749" s="73"/>
       <c r="L749" s="59"/>
       <c r="M749" s="74"/>
@@ -13316,10 +13464,10 @@
       <c r="F751" s="59"/>
       <c r="G751" s="59"/>
       <c r="H751" s="60"/>
-      <c r="I751" s="76"/>
-      <c r="J751" s="83"/>
+      <c r="I751" s="58"/>
+      <c r="J751" s="70"/>
       <c r="K751" s="73"/>
-      <c r="L751" s="59"/>
+      <c r="L751" s="74"/>
       <c r="M751" s="74"/>
       <c r="N751" s="58"/>
       <c r="O751" s="70"/>
@@ -13358,8 +13506,8 @@
       <c r="F753" s="59"/>
       <c r="G753" s="59"/>
       <c r="H753" s="60"/>
-      <c r="I753" s="58"/>
-      <c r="J753" s="70"/>
+      <c r="I753" s="76"/>
+      <c r="J753" s="75"/>
       <c r="K753" s="73"/>
       <c r="L753" s="74"/>
       <c r="M753" s="74"/>
@@ -13392,7 +13540,7 @@
       <c r="S754" s="70"/>
     </row>
     <row r="755" spans="1:19" ht="16">
-      <c r="A755" s="79"/>
+      <c r="A755" s="58"/>
       <c r="B755" s="59"/>
       <c r="C755" s="58"/>
       <c r="D755" s="58"/>
@@ -13400,12 +13548,12 @@
       <c r="F755" s="59"/>
       <c r="G755" s="59"/>
       <c r="H755" s="60"/>
-      <c r="I755" s="76"/>
-      <c r="J755" s="75"/>
-      <c r="K755" s="73"/>
-      <c r="L755" s="74"/>
-      <c r="M755" s="74"/>
-      <c r="N755" s="58"/>
+      <c r="I755" s="61"/>
+      <c r="J755" s="62"/>
+      <c r="K755" s="62"/>
+      <c r="L755" s="59"/>
+      <c r="M755" s="59"/>
+      <c r="N755" s="64"/>
       <c r="O755" s="70"/>
       <c r="P755" s="71"/>
       <c r="Q755" s="71"/>
@@ -13469,11 +13617,6 @@
       <c r="L758" s="59"/>
       <c r="M758" s="59"/>
       <c r="N758" s="64"/>
-      <c r="O758" s="70"/>
-      <c r="P758" s="71"/>
-      <c r="Q758" s="71"/>
-      <c r="R758" s="70"/>
-      <c r="S758" s="70"/>
     </row>
     <row r="759" spans="1:19" ht="16">
       <c r="A759" s="58"/>
@@ -13548,11 +13691,7 @@
       <c r="F763" s="59"/>
       <c r="G763" s="59"/>
       <c r="H763" s="60"/>
-      <c r="I763" s="61"/>
-      <c r="J763" s="62"/>
-      <c r="K763" s="62"/>
       <c r="L763" s="59"/>
-      <c r="M763" s="59"/>
       <c r="N763" s="64"/>
     </row>
     <row r="764" spans="1:19" ht="16">
@@ -13615,7 +13754,7 @@
       <c r="L768" s="59"/>
       <c r="N768" s="64"/>
     </row>
-    <row r="769" spans="1:14" ht="16">
+    <row r="769" spans="1:16" ht="16">
       <c r="A769" s="58"/>
       <c r="B769" s="59"/>
       <c r="C769" s="58"/>
@@ -13627,7 +13766,7 @@
       <c r="L769" s="59"/>
       <c r="N769" s="64"/>
     </row>
-    <row r="770" spans="1:14" ht="16">
+    <row r="770" spans="1:16" ht="16">
       <c r="A770" s="58"/>
       <c r="B770" s="59"/>
       <c r="C770" s="58"/>
@@ -13639,19 +13778,23 @@
       <c r="L770" s="59"/>
       <c r="N770" s="64"/>
     </row>
-    <row r="771" spans="1:14" ht="16">
+    <row r="771" spans="1:16" ht="16">
       <c r="A771" s="58"/>
       <c r="B771" s="59"/>
-      <c r="C771" s="58"/>
+      <c r="C771" s="59"/>
       <c r="D771" s="58"/>
       <c r="E771" s="59"/>
       <c r="F771" s="59"/>
       <c r="G771" s="59"/>
       <c r="H771" s="60"/>
+      <c r="I771" s="61"/>
+      <c r="J771" s="62"/>
+      <c r="K771" s="62"/>
       <c r="L771" s="59"/>
+      <c r="M771" s="59"/>
       <c r="N771" s="64"/>
     </row>
-    <row r="772" spans="1:14" ht="16">
+    <row r="772" spans="1:16" ht="16">
       <c r="A772" s="58"/>
       <c r="B772" s="59"/>
       <c r="C772" s="59"/>
@@ -13665,9 +13808,9 @@
       <c r="K772" s="62"/>
       <c r="L772" s="59"/>
       <c r="M772" s="59"/>
-      <c r="N772" s="64"/>
-    </row>
-    <row r="773" spans="1:14" ht="16">
+      <c r="N772" s="58"/>
+    </row>
+    <row r="773" spans="1:16" ht="16">
       <c r="A773" s="58"/>
       <c r="B773" s="59"/>
       <c r="C773" s="59"/>
@@ -13683,7 +13826,7 @@
       <c r="M773" s="59"/>
       <c r="N773" s="58"/>
     </row>
-    <row r="774" spans="1:14" ht="16">
+    <row r="774" spans="1:16" ht="16">
       <c r="A774" s="58"/>
       <c r="B774" s="59"/>
       <c r="C774" s="59"/>
@@ -13699,7 +13842,7 @@
       <c r="M774" s="59"/>
       <c r="N774" s="58"/>
     </row>
-    <row r="775" spans="1:14" ht="16">
+    <row r="775" spans="1:16" ht="16">
       <c r="A775" s="58"/>
       <c r="B775" s="59"/>
       <c r="C775" s="59"/>
@@ -13715,7 +13858,7 @@
       <c r="M775" s="59"/>
       <c r="N775" s="58"/>
     </row>
-    <row r="776" spans="1:14" ht="16">
+    <row r="776" spans="1:16" ht="16">
       <c r="A776" s="58"/>
       <c r="B776" s="59"/>
       <c r="C776" s="59"/>
@@ -13729,9 +13872,9 @@
       <c r="K776" s="62"/>
       <c r="L776" s="59"/>
       <c r="M776" s="59"/>
-      <c r="N776" s="58"/>
-    </row>
-    <row r="777" spans="1:14" ht="16">
+      <c r="N776" s="64"/>
+    </row>
+    <row r="777" spans="1:16" ht="16">
       <c r="A777" s="58"/>
       <c r="B777" s="59"/>
       <c r="C777" s="59"/>
@@ -13747,7 +13890,7 @@
       <c r="M777" s="59"/>
       <c r="N777" s="64"/>
     </row>
-    <row r="778" spans="1:14" ht="16">
+    <row r="778" spans="1:16" ht="16">
       <c r="A778" s="58"/>
       <c r="B778" s="59"/>
       <c r="C778" s="59"/>
@@ -13763,7 +13906,7 @@
       <c r="M778" s="59"/>
       <c r="N778" s="64"/>
     </row>
-    <row r="779" spans="1:14" ht="16">
+    <row r="779" spans="1:16" ht="16">
       <c r="A779" s="58"/>
       <c r="B779" s="59"/>
       <c r="C779" s="59"/>
@@ -13773,13 +13916,10 @@
       <c r="G779" s="59"/>
       <c r="H779" s="60"/>
       <c r="I779" s="61"/>
-      <c r="J779" s="62"/>
-      <c r="K779" s="62"/>
       <c r="L779" s="59"/>
-      <c r="M779" s="59"/>
       <c r="N779" s="64"/>
     </row>
-    <row r="780" spans="1:14" ht="16">
+    <row r="780" spans="1:16" ht="16">
       <c r="A780" s="58"/>
       <c r="B780" s="59"/>
       <c r="C780" s="59"/>
@@ -13792,7 +13932,7 @@
       <c r="L780" s="59"/>
       <c r="N780" s="64"/>
     </row>
-    <row r="781" spans="1:14" ht="16">
+    <row r="781" spans="1:16" ht="16">
       <c r="A781" s="58"/>
       <c r="B781" s="59"/>
       <c r="C781" s="59"/>
@@ -13805,7 +13945,7 @@
       <c r="L781" s="59"/>
       <c r="N781" s="64"/>
     </row>
-    <row r="782" spans="1:14" ht="16">
+    <row r="782" spans="1:16" ht="16">
       <c r="A782" s="58"/>
       <c r="B782" s="59"/>
       <c r="C782" s="59"/>
@@ -13815,10 +13955,9 @@
       <c r="G782" s="59"/>
       <c r="H782" s="60"/>
       <c r="I782" s="61"/>
-      <c r="L782" s="59"/>
       <c r="N782" s="64"/>
     </row>
-    <row r="783" spans="1:14" ht="16">
+    <row r="783" spans="1:16" ht="16">
       <c r="A783" s="58"/>
       <c r="B783" s="59"/>
       <c r="C783" s="59"/>
@@ -13830,7 +13969,7 @@
       <c r="I783" s="61"/>
       <c r="N783" s="64"/>
     </row>
-    <row r="784" spans="1:14" ht="16">
+    <row r="784" spans="1:16" ht="16">
       <c r="A784" s="58"/>
       <c r="B784" s="59"/>
       <c r="C784" s="59"/>
@@ -13841,21 +13980,19 @@
       <c r="H784" s="60"/>
       <c r="I784" s="61"/>
       <c r="N784" s="64"/>
-    </row>
-    <row r="785" spans="1:16" ht="16">
-      <c r="A785" s="58"/>
-      <c r="B785" s="59"/>
-      <c r="C785" s="59"/>
-      <c r="D785" s="58"/>
-      <c r="E785" s="59"/>
-      <c r="F785" s="59"/>
-      <c r="G785" s="59"/>
-      <c r="H785" s="60"/>
-      <c r="I785" s="61"/>
-      <c r="N785" s="64"/>
-      <c r="P785" s="71"/>
-    </row>
-    <row r="786" spans="1:16" ht="16">
+      <c r="P784" s="71"/>
+    </row>
+    <row r="785" spans="2:16" ht="16">
+      <c r="B785" s="85"/>
+      <c r="C785" s="70"/>
+      <c r="D785" s="70"/>
+      <c r="E785" s="70"/>
+      <c r="F785" s="86"/>
+      <c r="G785" s="85"/>
+      <c r="H785" s="72"/>
+      <c r="P785" s="75"/>
+    </row>
+    <row r="786" spans="2:16" ht="16">
       <c r="B786" s="85"/>
       <c r="C786" s="70"/>
       <c r="D786" s="70"/>
@@ -13865,7 +14002,7 @@
       <c r="H786" s="72"/>
       <c r="P786" s="75"/>
     </row>
-    <row r="787" spans="1:16" ht="16">
+    <row r="787" spans="2:16" ht="16">
       <c r="B787" s="85"/>
       <c r="C787" s="70"/>
       <c r="D787" s="70"/>
@@ -13875,7 +14012,7 @@
       <c r="H787" s="72"/>
       <c r="P787" s="75"/>
     </row>
-    <row r="788" spans="1:16" ht="16">
+    <row r="788" spans="2:16" ht="16">
       <c r="B788" s="85"/>
       <c r="C788" s="70"/>
       <c r="D788" s="70"/>
@@ -13885,7 +14022,7 @@
       <c r="H788" s="72"/>
       <c r="P788" s="75"/>
     </row>
-    <row r="789" spans="1:16" ht="16">
+    <row r="789" spans="2:16" ht="16">
       <c r="B789" s="85"/>
       <c r="C789" s="70"/>
       <c r="D789" s="70"/>
@@ -13895,7 +14032,7 @@
       <c r="H789" s="72"/>
       <c r="P789" s="75"/>
     </row>
-    <row r="790" spans="1:16" ht="16">
+    <row r="790" spans="2:16" ht="16">
       <c r="B790" s="85"/>
       <c r="C790" s="70"/>
       <c r="D790" s="70"/>
@@ -13905,7 +14042,7 @@
       <c r="H790" s="72"/>
       <c r="P790" s="75"/>
     </row>
-    <row r="791" spans="1:16" ht="16">
+    <row r="791" spans="2:16" ht="16">
       <c r="B791" s="85"/>
       <c r="C791" s="70"/>
       <c r="D791" s="70"/>
@@ -13915,7 +14052,7 @@
       <c r="H791" s="72"/>
       <c r="P791" s="75"/>
     </row>
-    <row r="792" spans="1:16" ht="16">
+    <row r="792" spans="2:16" ht="16">
       <c r="B792" s="85"/>
       <c r="C792" s="70"/>
       <c r="D792" s="70"/>
@@ -13925,7 +14062,7 @@
       <c r="H792" s="72"/>
       <c r="P792" s="75"/>
     </row>
-    <row r="793" spans="1:16" ht="16">
+    <row r="793" spans="2:16" ht="16">
       <c r="B793" s="85"/>
       <c r="C793" s="70"/>
       <c r="D793" s="70"/>
@@ -13935,42 +14072,37 @@
       <c r="H793" s="72"/>
       <c r="P793" s="75"/>
     </row>
-    <row r="794" spans="1:16" ht="16">
-      <c r="B794" s="85"/>
-      <c r="C794" s="70"/>
-      <c r="D794" s="70"/>
-      <c r="E794" s="70"/>
-      <c r="F794" s="86"/>
+    <row r="794" spans="2:16" ht="16">
+      <c r="B794" s="88"/>
+      <c r="E794" s="87"/>
       <c r="G794" s="85"/>
-      <c r="H794" s="72"/>
-      <c r="P794" s="75"/>
-    </row>
-    <row r="795" spans="1:16" ht="16">
+    </row>
+    <row r="795" spans="2:16" ht="16">
       <c r="B795" s="88"/>
       <c r="E795" s="87"/>
       <c r="G795" s="85"/>
     </row>
-    <row r="796" spans="1:16" ht="16">
+    <row r="796" spans="2:16" ht="16">
       <c r="B796" s="88"/>
       <c r="E796" s="87"/>
       <c r="G796" s="85"/>
     </row>
-    <row r="797" spans="1:16" ht="16">
+    <row r="797" spans="2:16" ht="16">
       <c r="B797" s="88"/>
       <c r="E797" s="87"/>
       <c r="G797" s="85"/>
     </row>
-    <row r="798" spans="1:16" ht="16">
+    <row r="798" spans="2:16" ht="16">
       <c r="B798" s="88"/>
       <c r="E798" s="87"/>
       <c r="G798" s="85"/>
     </row>
-    <row r="799" spans="1:16" ht="16">
+    <row r="799" spans="2:16" ht="16">
       <c r="B799" s="88"/>
       <c r="E799" s="87"/>
       <c r="G799" s="85"/>
     </row>
-    <row r="800" spans="1:16" ht="16">
+    <row r="800" spans="2:16" ht="16">
       <c r="B800" s="88"/>
       <c r="E800" s="87"/>
       <c r="G800" s="85"/>
@@ -14066,7 +14198,7 @@
       <c r="G818" s="85"/>
     </row>
     <row r="819" spans="2:7" ht="16">
-      <c r="B819" s="88"/>
+      <c r="B819" s="67"/>
       <c r="E819" s="87"/>
       <c r="G819" s="85"/>
     </row>
@@ -14076,7 +14208,7 @@
       <c r="G820" s="85"/>
     </row>
     <row r="821" spans="2:7" ht="16">
-      <c r="B821" s="67"/>
+      <c r="B821" s="88"/>
       <c r="E821" s="87"/>
       <c r="G821" s="85"/>
     </row>
@@ -14086,7 +14218,7 @@
       <c r="G822" s="85"/>
     </row>
     <row r="823" spans="2:7" ht="16">
-      <c r="B823" s="88"/>
+      <c r="B823" s="67"/>
       <c r="E823" s="87"/>
       <c r="G823" s="85"/>
     </row>
@@ -14096,7 +14228,7 @@
       <c r="G824" s="85"/>
     </row>
     <row r="825" spans="2:7" ht="16">
-      <c r="B825" s="67"/>
+      <c r="B825" s="88"/>
       <c r="E825" s="87"/>
       <c r="G825" s="85"/>
     </row>
@@ -14106,7 +14238,7 @@
       <c r="G826" s="85"/>
     </row>
     <row r="827" spans="2:7" ht="16">
-      <c r="B827" s="88"/>
+      <c r="B827" s="67"/>
       <c r="E827" s="87"/>
       <c r="G827" s="85"/>
     </row>
@@ -14116,7 +14248,7 @@
       <c r="G828" s="85"/>
     </row>
     <row r="829" spans="2:7" ht="16">
-      <c r="B829" s="67"/>
+      <c r="B829" s="88"/>
       <c r="E829" s="87"/>
       <c r="G829" s="85"/>
     </row>
@@ -14126,7 +14258,7 @@
       <c r="G830" s="85"/>
     </row>
     <row r="831" spans="2:7" ht="16">
-      <c r="B831" s="88"/>
+      <c r="B831" s="67"/>
       <c r="E831" s="87"/>
       <c r="G831" s="85"/>
     </row>
@@ -14137,8 +14269,13 @@
     </row>
     <row r="833" spans="2:9" ht="16">
       <c r="B833" s="67"/>
-      <c r="E833" s="87"/>
-      <c r="G833" s="85"/>
+      <c r="C833" s="56"/>
+      <c r="D833" s="56"/>
+      <c r="E833" s="66"/>
+      <c r="F833" s="56"/>
+      <c r="G833" s="67"/>
+      <c r="H833" s="56"/>
+      <c r="I833" s="57"/>
     </row>
     <row r="834" spans="2:9" ht="16">
       <c r="B834" s="67"/>
@@ -14212,13 +14349,6 @@
     </row>
     <row r="841" spans="2:9" ht="16">
       <c r="B841" s="67"/>
-      <c r="C841" s="56"/>
-      <c r="D841" s="56"/>
-      <c r="E841" s="66"/>
-      <c r="F841" s="56"/>
-      <c r="G841" s="67"/>
-      <c r="H841" s="56"/>
-      <c r="I841" s="57"/>
     </row>
     <row r="842" spans="2:9" ht="16">
       <c r="B842" s="67"/>
@@ -14279,9 +14409,6 @@
     </row>
     <row r="861" spans="2:2" ht="16">
       <c r="B861" s="67"/>
-    </row>
-    <row r="862" spans="2:2" ht="16">
-      <c r="B862" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
- extracted structural data from `10.1063/1.110520` (MG work cited by Cantor)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F696153-1017-314E-BF55-60592E8202C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFE7D9D-53ED-8048-B138-0E932B22FE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="7760" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="4560" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="152">
   <si>
     <t>Metadata</t>
   </si>
@@ -572,6 +572,18 @@
   </si>
   <si>
     <t>the Cantor alloy</t>
+  </si>
+  <si>
+    <t>Zr41.2Ti13.8Cu12.5Ni10.0Be22.5</t>
+  </si>
+  <si>
+    <t>amorphous</t>
+  </si>
+  <si>
+    <t>glassy state retained upon slow 10K/s cooling; extremely ductile at 99.9% rolling reduction</t>
+  </si>
+  <si>
+    <t>10.1063/1.110520</t>
   </si>
 </sst>
 </file>
@@ -1907,8 +1919,8 @@
   </sheetPr>
   <dimension ref="A1:T861"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4245,19 +4257,39 @@
     </row>
     <row r="62" spans="1:16" ht="18" customHeight="1">
       <c r="A62" s="24"/>
-      <c r="B62" s="44"/>
-      <c r="C62" s="42"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="44"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
+      <c r="B62" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="D62" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E62" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="F62" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G62" s="42" t="s">
+        <v>29</v>
+      </c>
       <c r="H62" s="42"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="4"/>
+      <c r="I62" s="49">
+        <v>298</v>
+      </c>
+      <c r="J62" s="4">
+        <v>5738000000</v>
+      </c>
       <c r="K62" s="4"/>
-      <c r="L62" s="44"/>
+      <c r="L62" s="44" t="s">
+        <v>33</v>
+      </c>
       <c r="M62" s="44"/>
-      <c r="N62" s="44"/>
+      <c r="N62" s="44" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="63" spans="1:16" ht="18" customHeight="1">
       <c r="A63" s="24"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/S0925-8388(02)00928-3` (MG reporting supersaturated BCC SS)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AB7CA4-852E-F54E-A9B1-50F6955DF63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7CA505-FCDE-BD4A-A03F-1A3B83C308FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="7800" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="176">
   <si>
     <t>Metadata</t>
   </si>
@@ -400,6 +400,9 @@
     <t>T6</t>
   </si>
   <si>
+    <t>MA</t>
+  </si>
+  <si>
     <t>F11</t>
   </si>
   <si>
@@ -641,6 +644,18 @@
   </si>
   <si>
     <t>10.1063/1.122980</t>
+  </si>
+  <si>
+    <t>Ta55Zr10Ni10Al10Cu15</t>
+  </si>
+  <si>
+    <t>ball milled for 1080ks</t>
+  </si>
+  <si>
+    <t>ball milled for 130ks; supersaturated BCC solid solution reported</t>
+  </si>
+  <si>
+    <t>10.1016/S0925-8388(02)00928-3</t>
   </si>
 </sst>
 </file>
@@ -1976,8 +1991,8 @@
   </sheetPr>
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O82" sqref="O82"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2298,16 +2313,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>65</v>
@@ -2330,23 +2345,23 @@
         <v>85</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>65</v>
@@ -2369,23 +2384,23 @@
         <v>85</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>65</v>
@@ -2408,23 +2423,23 @@
         <v>85</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>65</v>
@@ -2447,23 +2462,23 @@
         <v>85</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>65</v>
@@ -2486,23 +2501,23 @@
         <v>85</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>68</v>
@@ -2529,7 +2544,7 @@
         <v>87</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="6">
@@ -2546,16 +2561,16 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>68</v>
@@ -2582,7 +2597,7 @@
         <v>87</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O16" s="44"/>
       <c r="P16" s="6">
@@ -2599,16 +2614,16 @@
     <row r="17" spans="1:18" ht="18.75" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>68</v>
@@ -2635,7 +2650,7 @@
         <v>87</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P17" s="46">
         <v>222.963951935914</v>
@@ -2651,16 +2666,16 @@
     <row r="18" spans="1:18" ht="18.75" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>68</v>
@@ -2687,7 +2702,7 @@
         <v>87</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P18" s="6">
         <v>237.38317757009301</v>
@@ -2703,16 +2718,16 @@
     <row r="19" spans="1:18" ht="18.75" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>68</v>
@@ -2739,7 +2754,7 @@
         <v>87</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P19" s="6">
         <v>379.97329773030702</v>
@@ -2755,16 +2770,16 @@
     <row r="20" spans="1:18" ht="18.75" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>68</v>
@@ -2791,7 +2806,7 @@
         <v>87</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P20" s="6">
         <v>280.10680907877099</v>
@@ -2807,16 +2822,16 @@
     <row r="21" spans="1:18" ht="18.75" customHeight="1">
       <c r="A21" s="24"/>
       <c r="B21" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>68</v>
@@ -2843,7 +2858,7 @@
         <v>87</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P21" s="6">
         <v>298.79839786381802</v>
@@ -2859,16 +2874,16 @@
     <row r="22" spans="1:18" ht="18.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>68</v>
@@ -2895,7 +2910,7 @@
         <v>87</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P22" s="6">
         <v>306.809078771695</v>
@@ -2911,16 +2926,16 @@
     <row r="23" spans="1:18" ht="18.75" customHeight="1">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>68</v>
@@ -2947,7 +2962,7 @@
         <v>87</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P23" s="6">
         <v>322.29639519359102</v>
@@ -2963,16 +2978,16 @@
     <row r="24" spans="1:18" ht="18.75" customHeight="1">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>68</v>
@@ -2999,7 +3014,7 @@
         <v>87</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P24" s="6">
         <v>589.31909212283006</v>
@@ -3015,7 +3030,7 @@
     <row r="25" spans="1:18" ht="18.75" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>78</v>
@@ -3024,7 +3039,7 @@
         <v>80</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>68</v>
@@ -3051,7 +3066,7 @@
         <v>79</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="P25" s="6">
         <v>622</v>
@@ -3063,7 +3078,7 @@
     <row r="26" spans="1:18" ht="18.75" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>71</v>
@@ -3072,7 +3087,7 @@
         <v>80</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>68</v>
@@ -3099,7 +3114,7 @@
         <v>79</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="P26" s="6">
         <v>828</v>
@@ -3111,7 +3126,7 @@
     <row r="27" spans="1:18" ht="18.75" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>78</v>
@@ -3120,7 +3135,7 @@
         <v>80</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>72</v>
@@ -3147,7 +3162,7 @@
         <v>79</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="P27" s="6">
         <v>672</v>
@@ -3159,7 +3174,7 @@
     <row r="28" spans="1:18" ht="18.75" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>71</v>
@@ -3168,7 +3183,7 @@
         <v>80</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>72</v>
@@ -3195,7 +3210,7 @@
         <v>79</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="P28" s="6">
         <v>845</v>
@@ -3207,7 +3222,7 @@
     <row r="29" spans="1:18" ht="18.75" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>78</v>
@@ -3216,7 +3231,7 @@
         <v>80</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>73</v>
@@ -3239,13 +3254,13 @@
         <v>79</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="18.75" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>71</v>
@@ -3254,7 +3269,7 @@
         <v>80</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>73</v>
@@ -3277,13 +3292,13 @@
         <v>79</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="18.75" customHeight="1">
       <c r="A31" s="24"/>
       <c r="B31" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>78</v>
@@ -3292,7 +3307,7 @@
         <v>80</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>74</v>
@@ -3309,19 +3324,19 @@
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M31" s="9" t="s">
         <v>89</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="18.75" customHeight="1">
       <c r="A32" s="24"/>
       <c r="B32" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>71</v>
@@ -3330,7 +3345,7 @@
         <v>80</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>74</v>
@@ -3347,19 +3362,19 @@
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M32" s="9" t="s">
         <v>89</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="18.75" customHeight="1">
       <c r="A33" s="24"/>
       <c r="B33" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>78</v>
@@ -3368,7 +3383,7 @@
         <v>80</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>75</v>
@@ -3392,13 +3407,13 @@
         <v>89</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" customHeight="1">
       <c r="A34" s="24"/>
       <c r="B34" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>71</v>
@@ -3407,7 +3422,7 @@
         <v>80</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>75</v>
@@ -3431,22 +3446,22 @@
         <v>89</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="18.75" customHeight="1">
       <c r="A35" s="24"/>
       <c r="B35" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="44" t="s">
         <v>113</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>112</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>68</v>
@@ -3471,7 +3486,7 @@
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="P35" s="6">
         <v>602</v>
@@ -3483,16 +3498,16 @@
     <row r="36" spans="1:17" ht="18.75" customHeight="1">
       <c r="A36" s="24"/>
       <c r="B36" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>65</v>
@@ -3513,22 +3528,22 @@
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="18.75" customHeight="1">
       <c r="A37" s="24"/>
       <c r="B37" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>68</v>
@@ -3537,7 +3552,7 @@
         <v>29</v>
       </c>
       <c r="H37" s="42" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I37" s="43">
         <v>298</v>
@@ -3555,22 +3570,22 @@
         <v>77</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="18.75" customHeight="1">
       <c r="A38" s="24"/>
       <c r="B38" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>68</v>
@@ -3579,7 +3594,7 @@
         <v>29</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I38" s="43">
         <v>298</v>
@@ -3597,22 +3612,22 @@
         <v>77</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="18.75" customHeight="1">
       <c r="A39" s="24"/>
       <c r="B39" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>68</v>
@@ -3621,7 +3636,7 @@
         <v>29</v>
       </c>
       <c r="H39" s="42" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I39" s="43">
         <v>298</v>
@@ -3639,22 +3654,22 @@
         <v>77</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="18.75" customHeight="1">
       <c r="A40" s="24"/>
       <c r="B40" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>72</v>
@@ -3663,7 +3678,7 @@
         <v>29</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I40" s="43">
         <v>298</v>
@@ -3678,25 +3693,25 @@
         <v>33</v>
       </c>
       <c r="M40" s="44" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="18.75" customHeight="1">
       <c r="A41" s="24"/>
       <c r="B41" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>72</v>
@@ -3705,7 +3720,7 @@
         <v>29</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I41" s="43">
         <v>298</v>
@@ -3720,25 +3735,25 @@
         <v>33</v>
       </c>
       <c r="M41" s="44" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="18.75" customHeight="1">
       <c r="A42" s="24"/>
       <c r="B42" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>73</v>
@@ -3747,7 +3762,7 @@
         <v>29</v>
       </c>
       <c r="H42" s="42" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I42" s="43">
         <v>298</v>
@@ -3761,13 +3776,13 @@
       </c>
       <c r="M42" s="44"/>
       <c r="N42" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="18" customHeight="1">
       <c r="A43" s="24"/>
       <c r="B43" s="44" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C43" s="42" t="s">
         <v>71</v>
@@ -3783,13 +3798,13 @@
       <c r="L43" s="44"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="18" customHeight="1">
       <c r="A44" s="24"/>
       <c r="B44" s="44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C44" s="42" t="s">
         <v>71</v>
@@ -3805,16 +3820,16 @@
       <c r="L44" s="4"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="18" customHeight="1">
       <c r="A45" s="24"/>
       <c r="B45" s="44" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D45" s="42" t="s">
         <v>81</v>
@@ -3827,13 +3842,13 @@
       <c r="L45" s="4"/>
       <c r="M45" s="44"/>
       <c r="N45" s="44" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="18" customHeight="1">
       <c r="A46" s="24"/>
       <c r="B46" s="44" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C46" s="42" t="s">
         <v>71</v>
@@ -3863,7 +3878,7 @@
         <v>69</v>
       </c>
       <c r="N46" s="44" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P46" s="6">
         <v>133</v>
@@ -3872,7 +3887,7 @@
     <row r="47" spans="1:17" ht="18" customHeight="1">
       <c r="A47" s="24"/>
       <c r="B47" s="44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C47" s="42" t="s">
         <v>71</v>
@@ -3902,7 +3917,7 @@
         <v>69</v>
       </c>
       <c r="N47" s="44" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P47" s="6">
         <v>208</v>
@@ -3911,7 +3926,7 @@
     <row r="48" spans="1:17" ht="18" customHeight="1">
       <c r="A48" s="24"/>
       <c r="B48" s="44" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C48" s="42" t="s">
         <v>82</v>
@@ -3920,7 +3935,7 @@
         <v>63</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F48" s="42" t="s">
         <v>68</v>
@@ -3943,7 +3958,7 @@
         <v>69</v>
       </c>
       <c r="N48" s="44" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P48" s="6">
         <v>496</v>
@@ -3952,7 +3967,7 @@
     <row r="49" spans="1:16" ht="18" customHeight="1">
       <c r="A49" s="24"/>
       <c r="B49" s="44" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C49" s="42" t="s">
         <v>82</v>
@@ -3961,7 +3976,7 @@
         <v>70</v>
       </c>
       <c r="E49" s="42" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F49" s="42" t="s">
         <v>68</v>
@@ -3984,7 +3999,7 @@
         <v>69</v>
       </c>
       <c r="N49" s="44" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P49" s="6">
         <v>816</v>
@@ -3993,7 +4008,7 @@
     <row r="50" spans="1:16" ht="18" customHeight="1">
       <c r="A50" s="24"/>
       <c r="B50" s="44" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C50" s="42" t="s">
         <v>82</v>
@@ -4002,7 +4017,7 @@
         <v>63</v>
       </c>
       <c r="E50" s="42" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F50" s="42" t="s">
         <v>68</v>
@@ -4025,7 +4040,7 @@
         <v>69</v>
       </c>
       <c r="N50" s="44" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P50" s="6">
         <v>560</v>
@@ -4034,13 +4049,13 @@
     <row r="51" spans="1:16" ht="18" customHeight="1">
       <c r="A51" s="24"/>
       <c r="B51" s="44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C51" s="42" t="s">
         <v>64</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E51" s="42"/>
       <c r="F51" s="42" t="s">
@@ -4064,7 +4079,7 @@
         <v>69</v>
       </c>
       <c r="N51" s="44" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P51" s="6">
         <v>666</v>
@@ -4073,16 +4088,16 @@
     <row r="52" spans="1:16" ht="18" customHeight="1">
       <c r="A52" s="24"/>
       <c r="B52" s="128" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C52" s="42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D52" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E52" s="42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F52" s="42"/>
       <c r="G52" s="42"/>
@@ -4091,22 +4106,22 @@
       <c r="L52" s="44"/>
       <c r="M52" s="44"/>
       <c r="N52" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="18" customHeight="1">
       <c r="A53" s="24"/>
       <c r="B53" s="44" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E53" s="42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F53" s="42"/>
       <c r="G53" s="42"/>
@@ -4116,22 +4131,22 @@
       <c r="L53" s="44"/>
       <c r="M53" s="44"/>
       <c r="N53" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="18" customHeight="1">
       <c r="A54" s="24"/>
       <c r="B54" s="128" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D54" s="42" t="s">
         <v>86</v>
       </c>
       <c r="E54" s="42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F54" s="42"/>
       <c r="G54" s="42"/>
@@ -4141,22 +4156,22 @@
       <c r="L54" s="44"/>
       <c r="M54" s="44"/>
       <c r="N54" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="18" customHeight="1">
       <c r="A55" s="24"/>
       <c r="B55" s="44" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C55" s="42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D55" s="42" t="s">
         <v>86</v>
       </c>
       <c r="E55" s="42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F55" s="42"/>
       <c r="G55" s="42"/>
@@ -4166,22 +4181,22 @@
       <c r="L55" s="44"/>
       <c r="M55" s="44"/>
       <c r="N55" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="18" customHeight="1">
       <c r="A56" s="24"/>
       <c r="B56" s="44" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C56" s="42" t="s">
         <v>71</v>
       </c>
       <c r="D56" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E56" s="44" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F56" s="42"/>
       <c r="G56" s="42"/>
@@ -4191,19 +4206,19 @@
       <c r="L56" s="44"/>
       <c r="M56" s="44"/>
       <c r="N56" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="18" customHeight="1">
       <c r="A57" s="24"/>
       <c r="B57" s="44" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C57" s="42" t="s">
         <v>71</v>
       </c>
       <c r="D57" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E57" s="44"/>
       <c r="F57" s="42"/>
@@ -4214,19 +4229,19 @@
       <c r="L57" s="44"/>
       <c r="M57" s="44"/>
       <c r="N57" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="18" customHeight="1">
       <c r="A58" s="24"/>
       <c r="B58" s="44" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C58" s="42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D58" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E58" s="44"/>
       <c r="F58" s="42"/>
@@ -4237,19 +4252,19 @@
       <c r="L58" s="44"/>
       <c r="M58" s="44"/>
       <c r="N58" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="18" customHeight="1">
       <c r="A59" s="24"/>
       <c r="B59" s="44" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C59" s="42" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D59" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E59" s="44"/>
       <c r="F59" s="42"/>
@@ -4261,19 +4276,19 @@
       <c r="L59" s="44"/>
       <c r="M59" s="44"/>
       <c r="N59" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="18" customHeight="1">
       <c r="A60" s="24"/>
       <c r="B60" s="44" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C60" s="42" t="s">
         <v>78</v>
       </c>
       <c r="D60" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E60" s="44"/>
       <c r="F60" s="42"/>
@@ -4285,19 +4300,19 @@
       <c r="L60" s="44"/>
       <c r="M60" s="44"/>
       <c r="N60" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="18" customHeight="1">
       <c r="A61" s="24"/>
       <c r="B61" s="44" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C61" s="42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D61" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E61" s="44"/>
       <c r="F61" s="42"/>
@@ -4309,22 +4324,22 @@
       <c r="L61" s="44"/>
       <c r="M61" s="44"/>
       <c r="N61" s="44" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="18" customHeight="1">
       <c r="A62" s="24"/>
       <c r="B62" s="44" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C62" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E62" s="44" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F62" s="42" t="s">
         <v>68</v>
@@ -4345,19 +4360,19 @@
       </c>
       <c r="M62" s="44"/>
       <c r="N62" s="44" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="18" customHeight="1">
       <c r="A63" s="24"/>
       <c r="B63" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E63" s="44"/>
       <c r="F63" s="42"/>
@@ -4369,19 +4384,19 @@
       <c r="L63" s="44"/>
       <c r="M63" s="44"/>
       <c r="N63" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="18" customHeight="1">
       <c r="A64" s="24"/>
       <c r="B64" s="44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C64" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D64" s="42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E64" s="44"/>
       <c r="F64" s="42"/>
@@ -4393,22 +4408,22 @@
       <c r="L64" s="44"/>
       <c r="M64" s="44"/>
       <c r="N64" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="18" customHeight="1">
       <c r="A65" s="24"/>
       <c r="B65" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C65" s="42" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E65" s="42" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F65" s="42"/>
       <c r="G65" s="42"/>
@@ -4419,22 +4434,22 @@
       <c r="L65" s="44"/>
       <c r="M65" s="44"/>
       <c r="N65" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="18" customHeight="1">
       <c r="A66" s="24"/>
       <c r="B66" s="44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C66" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D66" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="E66" s="44" t="s">
         <v>165</v>
-      </c>
-      <c r="E66" s="44" t="s">
-        <v>164</v>
       </c>
       <c r="F66" s="42"/>
       <c r="G66" s="42"/>
@@ -4445,19 +4460,19 @@
       <c r="L66" s="44"/>
       <c r="M66" s="44"/>
       <c r="N66" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="18" customHeight="1">
       <c r="A67" s="24"/>
       <c r="B67" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C67" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F67" s="42" t="s">
         <v>68</v>
@@ -4466,7 +4481,7 @@
         <v>29</v>
       </c>
       <c r="H67" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I67" s="49">
         <v>298</v>
@@ -4481,7 +4496,7 @@
       </c>
       <c r="M67" s="44"/>
       <c r="N67" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P67" s="6">
         <v>510</v>
@@ -4490,16 +4505,16 @@
     <row r="68" spans="1:16" ht="18" customHeight="1">
       <c r="A68" s="24"/>
       <c r="B68" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C68" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D68" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E68" s="44" t="s">
         <v>165</v>
-      </c>
-      <c r="E68" s="44" t="s">
-        <v>164</v>
       </c>
       <c r="F68" s="42" t="s">
         <v>68</v>
@@ -4508,7 +4523,7 @@
         <v>29</v>
       </c>
       <c r="H68" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I68" s="49">
         <v>298</v>
@@ -4523,7 +4538,7 @@
       </c>
       <c r="M68" s="44"/>
       <c r="N68" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P68" s="6">
         <v>530</v>
@@ -4532,16 +4547,16 @@
     <row r="69" spans="1:16" ht="18" customHeight="1">
       <c r="A69" s="24"/>
       <c r="B69" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C69" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D69" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E69" s="44" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F69" s="42" t="s">
         <v>68</v>
@@ -4550,7 +4565,7 @@
         <v>29</v>
       </c>
       <c r="H69" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I69" s="49">
         <v>298</v>
@@ -4565,7 +4580,7 @@
       </c>
       <c r="M69" s="44"/>
       <c r="N69" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P69" s="6">
         <v>590</v>
@@ -4574,16 +4589,16 @@
     <row r="70" spans="1:16" ht="18" customHeight="1">
       <c r="A70" s="24"/>
       <c r="B70" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C70" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D70" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E70" s="44" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F70" s="42" t="s">
         <v>68</v>
@@ -4592,7 +4607,7 @@
         <v>29</v>
       </c>
       <c r="H70" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I70" s="49">
         <v>298</v>
@@ -4607,7 +4622,7 @@
       </c>
       <c r="M70" s="44"/>
       <c r="N70" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P70" s="6">
         <v>660</v>
@@ -4616,13 +4631,13 @@
     <row r="71" spans="1:16" ht="18" customHeight="1">
       <c r="A71" s="24"/>
       <c r="B71" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F71" s="42" t="s">
         <v>88</v>
@@ -4631,7 +4646,7 @@
         <v>29</v>
       </c>
       <c r="H71" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I71" s="49">
         <v>298</v>
@@ -4645,22 +4660,22 @@
       </c>
       <c r="M71" s="44"/>
       <c r="N71" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="18" customHeight="1">
       <c r="A72" s="24"/>
       <c r="B72" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D72" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E72" s="44" t="s">
         <v>165</v>
-      </c>
-      <c r="E72" s="44" t="s">
-        <v>164</v>
       </c>
       <c r="F72" s="42" t="s">
         <v>88</v>
@@ -4669,7 +4684,7 @@
         <v>29</v>
       </c>
       <c r="H72" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I72" s="49">
         <v>298</v>
@@ -4683,22 +4698,22 @@
       </c>
       <c r="M72" s="44"/>
       <c r="N72" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="18" customHeight="1">
       <c r="A73" s="24"/>
       <c r="B73" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D73" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E73" s="44" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F73" s="42" t="s">
         <v>88</v>
@@ -4707,7 +4722,7 @@
         <v>29</v>
       </c>
       <c r="H73" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I73" s="49">
         <v>298</v>
@@ -4721,22 +4736,22 @@
       </c>
       <c r="M73" s="44"/>
       <c r="N73" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="1:16" ht="18" customHeight="1">
       <c r="A74" s="24"/>
       <c r="B74" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D74" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E74" s="44" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F74" s="42" t="s">
         <v>88</v>
@@ -4745,7 +4760,7 @@
         <v>29</v>
       </c>
       <c r="H74" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I74" s="49">
         <v>298</v>
@@ -4759,22 +4774,22 @@
       </c>
       <c r="M74" s="44"/>
       <c r="N74" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="18" customHeight="1">
       <c r="A75" s="24"/>
       <c r="B75" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D75" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E75" s="44" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F75" s="42" t="s">
         <v>88</v>
@@ -4783,7 +4798,7 @@
         <v>29</v>
       </c>
       <c r="H75" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I75" s="49">
         <v>298</v>
@@ -4797,28 +4812,28 @@
       </c>
       <c r="M75" s="44"/>
       <c r="N75" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="18" customHeight="1">
       <c r="A76" s="24"/>
       <c r="B76" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C76" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D76" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F76" s="42" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G76" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H76" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I76" s="49">
         <v>298</v>
@@ -4832,31 +4847,31 @@
       </c>
       <c r="M76" s="44"/>
       <c r="N76" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="18" customHeight="1">
       <c r="A77" s="24"/>
       <c r="B77" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C77" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D77" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E77" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="E77" s="44" t="s">
-        <v>164</v>
-      </c>
       <c r="F77" s="42" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G77" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H77" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I77" s="49">
         <v>298</v>
@@ -4870,31 +4885,31 @@
       </c>
       <c r="M77" s="44"/>
       <c r="N77" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:16" ht="18" customHeight="1">
       <c r="A78" s="24"/>
       <c r="B78" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C78" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D78" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E78" s="44" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F78" s="42" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G78" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H78" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I78" s="49">
         <v>298</v>
@@ -4908,31 +4923,31 @@
       </c>
       <c r="M78" s="44"/>
       <c r="N78" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:16" ht="18" customHeight="1">
       <c r="A79" s="24"/>
       <c r="B79" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C79" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D79" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E79" s="44" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F79" s="42" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G79" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H79" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I79" s="49">
         <v>298</v>
@@ -4946,31 +4961,31 @@
       </c>
       <c r="M79" s="44"/>
       <c r="N79" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:16" ht="18" customHeight="1">
       <c r="A80" s="24"/>
       <c r="B80" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C80" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D80" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E80" s="44" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F80" s="42" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G80" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H80" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I80" s="49">
         <v>298</v>
@@ -4984,19 +4999,19 @@
       </c>
       <c r="M80" s="44"/>
       <c r="N80" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="18" customHeight="1">
       <c r="A81" s="24"/>
       <c r="B81" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C81" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D81" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F81" s="42" t="s">
         <v>84</v>
@@ -5005,7 +5020,7 @@
         <v>29</v>
       </c>
       <c r="H81" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I81" s="49">
         <v>298</v>
@@ -5019,22 +5034,22 @@
       </c>
       <c r="M81" s="44"/>
       <c r="N81" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="18" customHeight="1">
       <c r="A82" s="24"/>
       <c r="B82" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C82" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D82" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E82" s="44" t="s">
         <v>165</v>
-      </c>
-      <c r="E82" s="44" t="s">
-        <v>164</v>
       </c>
       <c r="F82" s="42" t="s">
         <v>84</v>
@@ -5043,7 +5058,7 @@
         <v>29</v>
       </c>
       <c r="H82" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I82" s="49">
         <v>298</v>
@@ -5057,22 +5072,22 @@
       </c>
       <c r="M82" s="44"/>
       <c r="N82" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="18" customHeight="1">
       <c r="A83" s="24"/>
       <c r="B83" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C83" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D83" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E83" s="44" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F83" s="42" t="s">
         <v>84</v>
@@ -5081,7 +5096,7 @@
         <v>29</v>
       </c>
       <c r="H83" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I83" s="49">
         <v>298</v>
@@ -5095,22 +5110,22 @@
       </c>
       <c r="M83" s="44"/>
       <c r="N83" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="18" customHeight="1">
       <c r="A84" s="24"/>
       <c r="B84" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C84" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D84" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E84" s="44" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F84" s="42" t="s">
         <v>84</v>
@@ -5119,7 +5134,7 @@
         <v>29</v>
       </c>
       <c r="H84" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I84" s="49">
         <v>298</v>
@@ -5133,19 +5148,19 @@
       </c>
       <c r="M84" s="44"/>
       <c r="N84" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="18" customHeight="1">
       <c r="A85" s="24"/>
       <c r="B85" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C85" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D85" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F85" s="42" t="s">
         <v>66</v>
@@ -5154,7 +5169,7 @@
         <v>29</v>
       </c>
       <c r="H85" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I85" s="49">
         <v>298</v>
@@ -5168,22 +5183,22 @@
       </c>
       <c r="M85" s="44"/>
       <c r="N85" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="18" customHeight="1">
       <c r="A86" s="24"/>
       <c r="B86" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C86" s="42" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D86" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E86" s="44" t="s">
         <v>165</v>
-      </c>
-      <c r="E86" s="44" t="s">
-        <v>164</v>
       </c>
       <c r="F86" s="42" t="s">
         <v>66</v>
@@ -5192,7 +5207,7 @@
         <v>29</v>
       </c>
       <c r="H86" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I86" s="49">
         <v>298</v>
@@ -5206,22 +5221,22 @@
       </c>
       <c r="M86" s="44"/>
       <c r="N86" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="18" customHeight="1">
       <c r="A87" s="24"/>
       <c r="B87" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C87" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D87" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E87" s="44" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F87" s="42" t="s">
         <v>66</v>
@@ -5230,7 +5245,7 @@
         <v>29</v>
       </c>
       <c r="H87" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I87" s="49">
         <v>298</v>
@@ -5244,22 +5259,22 @@
       </c>
       <c r="M87" s="44"/>
       <c r="N87" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="18" customHeight="1">
       <c r="A88" s="24"/>
       <c r="B88" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D88" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E88" s="44" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F88" s="42" t="s">
         <v>66</v>
@@ -5268,7 +5283,7 @@
         <v>29</v>
       </c>
       <c r="H88" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I88" s="49">
         <v>298</v>
@@ -5282,22 +5297,22 @@
       </c>
       <c r="M88" s="44"/>
       <c r="N88" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="18" customHeight="1">
       <c r="A89" s="24"/>
       <c r="B89" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C89" s="42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D89" s="42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E89" s="44" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F89" s="42" t="s">
         <v>66</v>
@@ -5306,7 +5321,7 @@
         <v>29</v>
       </c>
       <c r="H89" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I89" s="49">
         <v>298</v>
@@ -5320,15 +5335,23 @@
       </c>
       <c r="M89" s="44"/>
       <c r="N89" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="18" customHeight="1">
       <c r="A90" s="24"/>
-      <c r="B90" s="44"/>
-      <c r="C90" s="42"/>
-      <c r="D90" s="42"/>
-      <c r="E90" s="44"/>
+      <c r="B90" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C90" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D90" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E90" s="44" t="s">
+        <v>174</v>
+      </c>
       <c r="F90" s="42"/>
       <c r="G90" s="42"/>
       <c r="H90" s="42"/>
@@ -5337,14 +5360,24 @@
       <c r="K90" s="4"/>
       <c r="L90" s="44"/>
       <c r="M90" s="44"/>
-      <c r="N90" s="44"/>
+      <c r="N90" s="44" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="91" spans="1:14" ht="18" customHeight="1">
       <c r="A91" s="24"/>
-      <c r="B91" s="44"/>
-      <c r="C91" s="42"/>
-      <c r="D91" s="42"/>
-      <c r="E91" s="44"/>
+      <c r="B91" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C91" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D91" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E91" s="44" t="s">
+        <v>173</v>
+      </c>
       <c r="F91" s="42"/>
       <c r="G91" s="42"/>
       <c r="H91" s="42"/>
@@ -5353,7 +5386,9 @@
       <c r="K91" s="4"/>
       <c r="L91" s="44"/>
       <c r="M91" s="44"/>
-      <c r="N91" s="44"/>
+      <c r="N91" s="44" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="92" spans="1:14" ht="18" customHeight="1">
       <c r="A92" s="24"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/S0142-9612(03)00440-X` (earlier HEAs from 2023)
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7CA505-FCDE-BD4A-A03F-1A3B83C308FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3B46C9-0AD1-7243-8B79-21558326C99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="7800" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="4740" windowWidth="31760" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="190">
   <si>
     <t>Metadata</t>
   </si>
@@ -379,6 +379,9 @@
     <t>BCC+FCC</t>
   </si>
   <si>
+    <t>UCS</t>
+  </si>
+  <si>
     <t>kg/m^3</t>
   </si>
   <si>
@@ -388,12 +391,18 @@
     <t>T3</t>
   </si>
   <si>
+    <t>T1</t>
+  </si>
+  <si>
     <t>MS</t>
   </si>
   <si>
     <t>F5</t>
   </si>
   <si>
+    <t>strain rate 1e-4/s</t>
+  </si>
+  <si>
     <t>youngs modulus</t>
   </si>
   <si>
@@ -406,6 +415,9 @@
     <t>F11</t>
   </si>
   <si>
+    <t>AAM+A</t>
+  </si>
+  <si>
     <t>strain rate 3e-4/s</t>
   </si>
   <si>
@@ -656,6 +668,36 @@
   </si>
   <si>
     <t>10.1016/S0925-8388(02)00928-3</t>
+  </si>
+  <si>
+    <t>10.1016/S0142-9612(03)00440-X</t>
+  </si>
+  <si>
+    <t>Ti60Cu14Ni12Sn4Mo10</t>
+  </si>
+  <si>
+    <t>Ti60Cu14Ni12Sn4Nb10</t>
+  </si>
+  <si>
+    <t>Ti60Cu14Ni12Sn4Mo12Ta10</t>
+  </si>
+  <si>
+    <t>Ti60Cu14Ni12Sn4Mo13Ta10</t>
+  </si>
+  <si>
+    <t>Ti60Cu14Ni12Sn4Mo14Ta10</t>
+  </si>
+  <si>
+    <t>AAM+Q</t>
+  </si>
+  <si>
+    <t>annealed at 973K for 10min</t>
+  </si>
+  <si>
+    <t>BCC+?</t>
+  </si>
+  <si>
+    <t>BCC+HCP+?</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1683,6 +1725,9 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1991,8 +2036,8 @@
   </sheetPr>
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2313,16 +2358,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>65</v>
@@ -2339,29 +2384,29 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="9" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>65</v>
@@ -2378,29 +2423,29 @@
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>65</v>
@@ -2417,29 +2462,29 @@
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>65</v>
@@ -2456,29 +2501,29 @@
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>65</v>
@@ -2495,29 +2540,29 @@
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>68</v>
@@ -2541,10 +2586,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="6">
@@ -2561,16 +2606,16 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="9" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>68</v>
@@ -2594,10 +2639,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O16" s="44"/>
       <c r="P16" s="6">
@@ -2614,16 +2659,16 @@
     <row r="17" spans="1:18" ht="18.75" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>68</v>
@@ -2647,10 +2692,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P17" s="46">
         <v>222.963951935914</v>
@@ -2666,16 +2711,16 @@
     <row r="18" spans="1:18" ht="18.75" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>68</v>
@@ -2699,10 +2744,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P18" s="6">
         <v>237.38317757009301</v>
@@ -2718,16 +2763,16 @@
     <row r="19" spans="1:18" ht="18.75" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="9" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>68</v>
@@ -2751,10 +2796,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P19" s="6">
         <v>379.97329773030702</v>
@@ -2770,16 +2815,16 @@
     <row r="20" spans="1:18" ht="18.75" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>68</v>
@@ -2803,10 +2848,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P20" s="6">
         <v>280.10680907877099</v>
@@ -2822,16 +2867,16 @@
     <row r="21" spans="1:18" ht="18.75" customHeight="1">
       <c r="A21" s="24"/>
       <c r="B21" s="9" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>68</v>
@@ -2855,10 +2900,10 @@
         <v>33</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P21" s="6">
         <v>298.79839786381802</v>
@@ -2874,16 +2919,16 @@
     <row r="22" spans="1:18" ht="18.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>68</v>
@@ -2907,10 +2952,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P22" s="6">
         <v>306.809078771695</v>
@@ -2926,16 +2971,16 @@
     <row r="23" spans="1:18" ht="18.75" customHeight="1">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>68</v>
@@ -2959,10 +3004,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P23" s="6">
         <v>322.29639519359102</v>
@@ -2978,16 +3023,16 @@
     <row r="24" spans="1:18" ht="18.75" customHeight="1">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>68</v>
@@ -3011,10 +3056,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P24" s="6">
         <v>589.31909212283006</v>
@@ -3030,7 +3075,7 @@
     <row r="25" spans="1:18" ht="18.75" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>78</v>
@@ -3039,7 +3084,7 @@
         <v>80</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>68</v>
@@ -3066,7 +3111,7 @@
         <v>79</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="P25" s="6">
         <v>622</v>
@@ -3078,7 +3123,7 @@
     <row r="26" spans="1:18" ht="18.75" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>71</v>
@@ -3087,7 +3132,7 @@
         <v>80</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>68</v>
@@ -3114,7 +3159,7 @@
         <v>79</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="P26" s="6">
         <v>828</v>
@@ -3126,7 +3171,7 @@
     <row r="27" spans="1:18" ht="18.75" customHeight="1">
       <c r="A27" s="24"/>
       <c r="B27" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>78</v>
@@ -3135,7 +3180,7 @@
         <v>80</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>72</v>
@@ -3162,7 +3207,7 @@
         <v>79</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="P27" s="6">
         <v>672</v>
@@ -3174,7 +3219,7 @@
     <row r="28" spans="1:18" ht="18.75" customHeight="1">
       <c r="A28" s="24"/>
       <c r="B28" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>71</v>
@@ -3183,7 +3228,7 @@
         <v>80</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>72</v>
@@ -3210,7 +3255,7 @@
         <v>79</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="P28" s="6">
         <v>845</v>
@@ -3222,7 +3267,7 @@
     <row r="29" spans="1:18" ht="18.75" customHeight="1">
       <c r="A29" s="24"/>
       <c r="B29" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>78</v>
@@ -3231,7 +3276,7 @@
         <v>80</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>73</v>
@@ -3254,13 +3299,13 @@
         <v>79</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="18.75" customHeight="1">
       <c r="A30" s="24"/>
       <c r="B30" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>71</v>
@@ -3269,7 +3314,7 @@
         <v>80</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>73</v>
@@ -3292,13 +3337,13 @@
         <v>79</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="18.75" customHeight="1">
       <c r="A31" s="24"/>
       <c r="B31" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>78</v>
@@ -3307,7 +3352,7 @@
         <v>80</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>74</v>
@@ -3324,19 +3369,19 @@
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="9" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="18.75" customHeight="1">
       <c r="A32" s="24"/>
       <c r="B32" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>71</v>
@@ -3345,7 +3390,7 @@
         <v>80</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>74</v>
@@ -3362,19 +3407,19 @@
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="9" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="18.75" customHeight="1">
       <c r="A33" s="24"/>
       <c r="B33" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>78</v>
@@ -3383,7 +3428,7 @@
         <v>80</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>75</v>
@@ -3404,16 +3449,16 @@
         <v>76</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" customHeight="1">
       <c r="A34" s="24"/>
       <c r="B34" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>71</v>
@@ -3422,7 +3467,7 @@
         <v>80</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>75</v>
@@ -3443,25 +3488,25 @@
         <v>76</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="18.75" customHeight="1">
       <c r="A35" s="24"/>
       <c r="B35" s="9" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E35" s="44" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>68</v>
@@ -3486,7 +3531,7 @@
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="P35" s="6">
         <v>602</v>
@@ -3498,16 +3543,16 @@
     <row r="36" spans="1:17" ht="18.75" customHeight="1">
       <c r="A36" s="24"/>
       <c r="B36" s="9" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>65</v>
@@ -3524,26 +3569,26 @@
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="18.75" customHeight="1">
       <c r="A37" s="24"/>
       <c r="B37" s="9" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>68</v>
@@ -3552,7 +3597,7 @@
         <v>29</v>
       </c>
       <c r="H37" s="42" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I37" s="43">
         <v>298</v>
@@ -3570,22 +3615,22 @@
         <v>77</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="18.75" customHeight="1">
       <c r="A38" s="24"/>
       <c r="B38" s="9" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>68</v>
@@ -3594,7 +3639,7 @@
         <v>29</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I38" s="43">
         <v>298</v>
@@ -3612,22 +3657,22 @@
         <v>77</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="18.75" customHeight="1">
       <c r="A39" s="24"/>
       <c r="B39" s="9" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>68</v>
@@ -3636,7 +3681,7 @@
         <v>29</v>
       </c>
       <c r="H39" s="42" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="I39" s="43">
         <v>298</v>
@@ -3654,22 +3699,22 @@
         <v>77</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="18.75" customHeight="1">
       <c r="A40" s="24"/>
       <c r="B40" s="9" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>72</v>
@@ -3678,7 +3723,7 @@
         <v>29</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I40" s="43">
         <v>298</v>
@@ -3693,25 +3738,25 @@
         <v>33</v>
       </c>
       <c r="M40" s="44" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="18.75" customHeight="1">
       <c r="A41" s="24"/>
       <c r="B41" s="9" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>72</v>
@@ -3720,7 +3765,7 @@
         <v>29</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I41" s="43">
         <v>298</v>
@@ -3735,25 +3780,25 @@
         <v>33</v>
       </c>
       <c r="M41" s="44" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="18.75" customHeight="1">
       <c r="A42" s="24"/>
       <c r="B42" s="9" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>73</v>
@@ -3762,7 +3807,7 @@
         <v>29</v>
       </c>
       <c r="H42" s="42" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I42" s="43">
         <v>298</v>
@@ -3776,13 +3821,13 @@
       </c>
       <c r="M42" s="44"/>
       <c r="N42" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="18" customHeight="1">
       <c r="A43" s="24"/>
       <c r="B43" s="44" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C43" s="42" t="s">
         <v>71</v>
@@ -3798,13 +3843,13 @@
       <c r="L43" s="44"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="18" customHeight="1">
       <c r="A44" s="24"/>
       <c r="B44" s="44" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C44" s="42" t="s">
         <v>71</v>
@@ -3820,16 +3865,16 @@
       <c r="L44" s="4"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="18" customHeight="1">
       <c r="A45" s="24"/>
       <c r="B45" s="44" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D45" s="42" t="s">
         <v>81</v>
@@ -3842,13 +3887,13 @@
       <c r="L45" s="4"/>
       <c r="M45" s="44"/>
       <c r="N45" s="44" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="18" customHeight="1">
       <c r="A46" s="24"/>
       <c r="B46" s="44" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C46" s="42" t="s">
         <v>71</v>
@@ -3878,7 +3923,7 @@
         <v>69</v>
       </c>
       <c r="N46" s="44" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P46" s="6">
         <v>133</v>
@@ -3887,7 +3932,7 @@
     <row r="47" spans="1:17" ht="18" customHeight="1">
       <c r="A47" s="24"/>
       <c r="B47" s="44" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C47" s="42" t="s">
         <v>71</v>
@@ -3917,7 +3962,7 @@
         <v>69</v>
       </c>
       <c r="N47" s="44" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P47" s="6">
         <v>208</v>
@@ -3926,7 +3971,7 @@
     <row r="48" spans="1:17" ht="18" customHeight="1">
       <c r="A48" s="24"/>
       <c r="B48" s="44" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C48" s="42" t="s">
         <v>82</v>
@@ -3935,7 +3980,7 @@
         <v>63</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F48" s="42" t="s">
         <v>68</v>
@@ -3958,7 +4003,7 @@
         <v>69</v>
       </c>
       <c r="N48" s="44" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P48" s="6">
         <v>496</v>
@@ -3967,7 +4012,7 @@
     <row r="49" spans="1:16" ht="18" customHeight="1">
       <c r="A49" s="24"/>
       <c r="B49" s="44" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C49" s="42" t="s">
         <v>82</v>
@@ -3976,7 +4021,7 @@
         <v>70</v>
       </c>
       <c r="E49" s="42" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F49" s="42" t="s">
         <v>68</v>
@@ -3999,7 +4044,7 @@
         <v>69</v>
       </c>
       <c r="N49" s="44" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P49" s="6">
         <v>816</v>
@@ -4008,7 +4053,7 @@
     <row r="50" spans="1:16" ht="18" customHeight="1">
       <c r="A50" s="24"/>
       <c r="B50" s="44" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C50" s="42" t="s">
         <v>82</v>
@@ -4017,7 +4062,7 @@
         <v>63</v>
       </c>
       <c r="E50" s="42" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F50" s="42" t="s">
         <v>68</v>
@@ -4040,7 +4085,7 @@
         <v>69</v>
       </c>
       <c r="N50" s="44" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P50" s="6">
         <v>560</v>
@@ -4049,13 +4094,13 @@
     <row r="51" spans="1:16" ht="18" customHeight="1">
       <c r="A51" s="24"/>
       <c r="B51" s="44" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C51" s="42" t="s">
         <v>64</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E51" s="42"/>
       <c r="F51" s="42" t="s">
@@ -4079,7 +4124,7 @@
         <v>69</v>
       </c>
       <c r="N51" s="44" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P51" s="6">
         <v>666</v>
@@ -4088,16 +4133,16 @@
     <row r="52" spans="1:16" ht="18" customHeight="1">
       <c r="A52" s="24"/>
       <c r="B52" s="128" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C52" s="42" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D52" s="42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E52" s="42" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F52" s="42"/>
       <c r="G52" s="42"/>
@@ -4106,22 +4151,22 @@
       <c r="L52" s="44"/>
       <c r="M52" s="44"/>
       <c r="N52" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="18" customHeight="1">
       <c r="A53" s="24"/>
       <c r="B53" s="44" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E53" s="42" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F53" s="42"/>
       <c r="G53" s="42"/>
@@ -4131,22 +4176,22 @@
       <c r="L53" s="44"/>
       <c r="M53" s="44"/>
       <c r="N53" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="18" customHeight="1">
       <c r="A54" s="24"/>
       <c r="B54" s="128" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E54" s="42" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F54" s="42"/>
       <c r="G54" s="42"/>
@@ -4156,22 +4201,22 @@
       <c r="L54" s="44"/>
       <c r="M54" s="44"/>
       <c r="N54" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="18" customHeight="1">
       <c r="A55" s="24"/>
       <c r="B55" s="44" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C55" s="42" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D55" s="42" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E55" s="42" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F55" s="42"/>
       <c r="G55" s="42"/>
@@ -4181,22 +4226,22 @@
       <c r="L55" s="44"/>
       <c r="M55" s="44"/>
       <c r="N55" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="18" customHeight="1">
       <c r="A56" s="24"/>
       <c r="B56" s="44" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C56" s="42" t="s">
         <v>71</v>
       </c>
       <c r="D56" s="42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E56" s="44" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F56" s="42"/>
       <c r="G56" s="42"/>
@@ -4206,19 +4251,19 @@
       <c r="L56" s="44"/>
       <c r="M56" s="44"/>
       <c r="N56" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="18" customHeight="1">
       <c r="A57" s="24"/>
       <c r="B57" s="44" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C57" s="42" t="s">
         <v>71</v>
       </c>
       <c r="D57" s="42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E57" s="44"/>
       <c r="F57" s="42"/>
@@ -4229,19 +4274,19 @@
       <c r="L57" s="44"/>
       <c r="M57" s="44"/>
       <c r="N57" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="18" customHeight="1">
       <c r="A58" s="24"/>
       <c r="B58" s="44" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C58" s="42" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D58" s="42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E58" s="44"/>
       <c r="F58" s="42"/>
@@ -4252,19 +4297,19 @@
       <c r="L58" s="44"/>
       <c r="M58" s="44"/>
       <c r="N58" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="18" customHeight="1">
       <c r="A59" s="24"/>
       <c r="B59" s="44" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C59" s="42" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D59" s="42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E59" s="44"/>
       <c r="F59" s="42"/>
@@ -4276,19 +4321,19 @@
       <c r="L59" s="44"/>
       <c r="M59" s="44"/>
       <c r="N59" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="18" customHeight="1">
       <c r="A60" s="24"/>
       <c r="B60" s="44" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C60" s="42" t="s">
         <v>78</v>
       </c>
       <c r="D60" s="42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E60" s="44"/>
       <c r="F60" s="42"/>
@@ -4300,19 +4345,19 @@
       <c r="L60" s="44"/>
       <c r="M60" s="44"/>
       <c r="N60" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="18" customHeight="1">
       <c r="A61" s="24"/>
       <c r="B61" s="44" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C61" s="42" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D61" s="42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E61" s="44"/>
       <c r="F61" s="42"/>
@@ -4324,22 +4369,22 @@
       <c r="L61" s="44"/>
       <c r="M61" s="44"/>
       <c r="N61" s="44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="18" customHeight="1">
       <c r="A62" s="24"/>
       <c r="B62" s="44" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C62" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E62" s="44" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="F62" s="42" t="s">
         <v>68</v>
@@ -4360,19 +4405,19 @@
       </c>
       <c r="M62" s="44"/>
       <c r="N62" s="44" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="18" customHeight="1">
       <c r="A63" s="24"/>
       <c r="B63" s="44" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E63" s="44"/>
       <c r="F63" s="42"/>
@@ -4384,19 +4429,19 @@
       <c r="L63" s="44"/>
       <c r="M63" s="44"/>
       <c r="N63" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="18" customHeight="1">
       <c r="A64" s="24"/>
       <c r="B64" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C64" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="C64" s="42" t="s">
-        <v>155</v>
-      </c>
       <c r="D64" s="42" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E64" s="44"/>
       <c r="F64" s="42"/>
@@ -4408,22 +4453,22 @@
       <c r="L64" s="44"/>
       <c r="M64" s="44"/>
       <c r="N64" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="18" customHeight="1">
       <c r="A65" s="24"/>
       <c r="B65" s="44" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C65" s="42" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E65" s="42" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F65" s="42"/>
       <c r="G65" s="42"/>
@@ -4434,22 +4479,22 @@
       <c r="L65" s="44"/>
       <c r="M65" s="44"/>
       <c r="N65" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="18" customHeight="1">
       <c r="A66" s="24"/>
       <c r="B66" s="44" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C66" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E66" s="44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F66" s="42"/>
       <c r="G66" s="42"/>
@@ -4460,19 +4505,19 @@
       <c r="L66" s="44"/>
       <c r="M66" s="44"/>
       <c r="N66" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="18" customHeight="1">
       <c r="A67" s="24"/>
       <c r="B67" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C67" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F67" s="42" t="s">
         <v>68</v>
@@ -4481,7 +4526,7 @@
         <v>29</v>
       </c>
       <c r="H67" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I67" s="49">
         <v>298</v>
@@ -4494,9 +4539,11 @@
       <c r="L67" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M67" s="44"/>
+      <c r="M67" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N67" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="P67" s="6">
         <v>510</v>
@@ -4505,16 +4552,16 @@
     <row r="68" spans="1:16" ht="18" customHeight="1">
       <c r="A68" s="24"/>
       <c r="B68" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C68" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D68" s="42" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E68" s="44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F68" s="42" t="s">
         <v>68</v>
@@ -4523,7 +4570,7 @@
         <v>29</v>
       </c>
       <c r="H68" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I68" s="49">
         <v>298</v>
@@ -4536,9 +4583,11 @@
       <c r="L68" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M68" s="44"/>
+      <c r="M68" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N68" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="P68" s="6">
         <v>530</v>
@@ -4547,16 +4596,16 @@
     <row r="69" spans="1:16" ht="18" customHeight="1">
       <c r="A69" s="24"/>
       <c r="B69" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C69" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D69" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E69" s="44" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F69" s="42" t="s">
         <v>68</v>
@@ -4565,7 +4614,7 @@
         <v>29</v>
       </c>
       <c r="H69" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I69" s="49">
         <v>298</v>
@@ -4578,9 +4627,11 @@
       <c r="L69" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M69" s="44"/>
+      <c r="M69" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N69" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="P69" s="6">
         <v>590</v>
@@ -4589,16 +4640,16 @@
     <row r="70" spans="1:16" ht="18" customHeight="1">
       <c r="A70" s="24"/>
       <c r="B70" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C70" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D70" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E70" s="44" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F70" s="42" t="s">
         <v>68</v>
@@ -4607,7 +4658,7 @@
         <v>29</v>
       </c>
       <c r="H70" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I70" s="49">
         <v>298</v>
@@ -4620,9 +4671,11 @@
       <c r="L70" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M70" s="44"/>
+      <c r="M70" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N70" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="P70" s="6">
         <v>660</v>
@@ -4631,22 +4684,22 @@
     <row r="71" spans="1:16" ht="18" customHeight="1">
       <c r="A71" s="24"/>
       <c r="B71" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F71" s="42" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G71" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H71" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I71" s="49">
         <v>298</v>
@@ -4658,33 +4711,35 @@
       <c r="L71" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M71" s="44"/>
+      <c r="M71" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N71" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="18" customHeight="1">
       <c r="A72" s="24"/>
       <c r="B72" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D72" s="42" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E72" s="44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F72" s="42" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G72" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H72" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I72" s="49">
         <v>298</v>
@@ -4696,33 +4751,35 @@
       <c r="L72" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M72" s="44"/>
+      <c r="M72" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N72" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="18" customHeight="1">
       <c r="A73" s="24"/>
       <c r="B73" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D73" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E73" s="44" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F73" s="42" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G73" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H73" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I73" s="49">
         <v>298</v>
@@ -4734,33 +4791,35 @@
       <c r="L73" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M73" s="44"/>
+      <c r="M73" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N73" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:16" ht="18" customHeight="1">
       <c r="A74" s="24"/>
       <c r="B74" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D74" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E74" s="44" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F74" s="42" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G74" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H74" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I74" s="49">
         <v>298</v>
@@ -4772,33 +4831,35 @@
       <c r="L74" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M74" s="44"/>
+      <c r="M74" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N74" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="18" customHeight="1">
       <c r="A75" s="24"/>
       <c r="B75" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D75" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E75" s="44" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F75" s="42" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G75" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H75" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I75" s="49">
         <v>298</v>
@@ -4810,30 +4871,32 @@
       <c r="L75" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M75" s="44"/>
+      <c r="M75" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N75" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="18" customHeight="1">
       <c r="A76" s="24"/>
       <c r="B76" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C76" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D76" s="48" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F76" s="42" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G76" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H76" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I76" s="49">
         <v>298</v>
@@ -4845,33 +4908,35 @@
       <c r="L76" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M76" s="44"/>
+      <c r="M76" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N76" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="18" customHeight="1">
       <c r="A77" s="24"/>
       <c r="B77" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C77" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D77" s="42" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E77" s="44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F77" s="42" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G77" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H77" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I77" s="49">
         <v>298</v>
@@ -4883,33 +4948,35 @@
       <c r="L77" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M77" s="44"/>
+      <c r="M77" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N77" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:16" ht="18" customHeight="1">
       <c r="A78" s="24"/>
       <c r="B78" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C78" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D78" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E78" s="44" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F78" s="42" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G78" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H78" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I78" s="49">
         <v>298</v>
@@ -4921,33 +4988,35 @@
       <c r="L78" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M78" s="44"/>
+      <c r="M78" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N78" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:16" ht="18" customHeight="1">
       <c r="A79" s="24"/>
       <c r="B79" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C79" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D79" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E79" s="44" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F79" s="42" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G79" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H79" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I79" s="49">
         <v>298</v>
@@ -4959,33 +5028,35 @@
       <c r="L79" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M79" s="44"/>
+      <c r="M79" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N79" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:16" ht="18" customHeight="1">
       <c r="A80" s="24"/>
       <c r="B80" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C80" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D80" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E80" s="44" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F80" s="42" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G80" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H80" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I80" s="49">
         <v>298</v>
@@ -4997,30 +5068,32 @@
       <c r="L80" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M80" s="44"/>
+      <c r="M80" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N80" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="18" customHeight="1">
       <c r="A81" s="24"/>
       <c r="B81" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C81" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D81" s="48" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F81" s="42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G81" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H81" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I81" s="49">
         <v>298</v>
@@ -5032,33 +5105,35 @@
       <c r="L81" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M81" s="44"/>
+      <c r="M81" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N81" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="18" customHeight="1">
       <c r="A82" s="24"/>
       <c r="B82" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C82" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D82" s="42" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E82" s="44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F82" s="42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G82" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H82" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I82" s="49">
         <v>298</v>
@@ -5070,33 +5145,35 @@
       <c r="L82" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M82" s="44"/>
+      <c r="M82" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N82" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="18" customHeight="1">
       <c r="A83" s="24"/>
       <c r="B83" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C83" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D83" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E83" s="44" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F83" s="42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G83" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H83" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I83" s="49">
         <v>298</v>
@@ -5108,33 +5185,35 @@
       <c r="L83" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M83" s="44"/>
+      <c r="M83" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N83" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="18" customHeight="1">
       <c r="A84" s="24"/>
       <c r="B84" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C84" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D84" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E84" s="44" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F84" s="42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G84" s="42" t="s">
         <v>29</v>
       </c>
       <c r="H84" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I84" s="49">
         <v>298</v>
@@ -5146,21 +5225,23 @@
       <c r="L84" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M84" s="44"/>
+      <c r="M84" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N84" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="18" customHeight="1">
       <c r="A85" s="24"/>
       <c r="B85" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C85" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D85" s="48" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F85" s="42" t="s">
         <v>66</v>
@@ -5169,7 +5250,7 @@
         <v>29</v>
       </c>
       <c r="H85" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I85" s="49">
         <v>298</v>
@@ -5181,24 +5262,26 @@
       <c r="L85" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="M85" s="44"/>
+      <c r="M85" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N85" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="18" customHeight="1">
       <c r="A86" s="24"/>
       <c r="B86" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C86" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D86" s="42" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E86" s="44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F86" s="42" t="s">
         <v>66</v>
@@ -5207,7 +5290,7 @@
         <v>29</v>
       </c>
       <c r="H86" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I86" s="49">
         <v>298</v>
@@ -5219,24 +5302,26 @@
       <c r="L86" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="M86" s="44"/>
+      <c r="M86" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N86" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="18" customHeight="1">
       <c r="A87" s="24"/>
       <c r="B87" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C87" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D87" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E87" s="44" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F87" s="42" t="s">
         <v>66</v>
@@ -5245,7 +5330,7 @@
         <v>29</v>
       </c>
       <c r="H87" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I87" s="49">
         <v>298</v>
@@ -5257,24 +5342,26 @@
       <c r="L87" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="M87" s="44"/>
+      <c r="M87" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N87" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="18" customHeight="1">
       <c r="A88" s="24"/>
       <c r="B88" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D88" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E88" s="44" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F88" s="42" t="s">
         <v>66</v>
@@ -5283,7 +5370,7 @@
         <v>29</v>
       </c>
       <c r="H88" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I88" s="49">
         <v>298</v>
@@ -5295,24 +5382,26 @@
       <c r="L88" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="M88" s="44"/>
+      <c r="M88" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N88" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="18" customHeight="1">
       <c r="A89" s="24"/>
       <c r="B89" s="44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C89" s="42" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D89" s="42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E89" s="44" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F89" s="42" t="s">
         <v>66</v>
@@ -5321,7 +5410,7 @@
         <v>29</v>
       </c>
       <c r="H89" s="42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I89" s="49">
         <v>298</v>
@@ -5333,24 +5422,26 @@
       <c r="L89" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="M89" s="44"/>
+      <c r="M89" s="44" t="s">
+        <v>87</v>
+      </c>
       <c r="N89" s="44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="18" customHeight="1">
       <c r="A90" s="24"/>
       <c r="B90" s="44" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C90" s="42" t="s">
         <v>64</v>
       </c>
       <c r="D90" s="42" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E90" s="44" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F90" s="42"/>
       <c r="G90" s="42"/>
@@ -5361,22 +5452,22 @@
       <c r="L90" s="44"/>
       <c r="M90" s="44"/>
       <c r="N90" s="44" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="18" customHeight="1">
       <c r="A91" s="24"/>
       <c r="B91" s="44" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C91" s="42" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D91" s="42" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E91" s="44" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F91" s="42"/>
       <c r="G91" s="42"/>
@@ -5387,392 +5478,914 @@
       <c r="L91" s="44"/>
       <c r="M91" s="44"/>
       <c r="N91" s="44" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="18" customHeight="1">
       <c r="A92" s="24"/>
-      <c r="B92" s="44"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="42"/>
+      <c r="B92" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="C92" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="D92" s="42" t="s">
+        <v>81</v>
+      </c>
       <c r="E92" s="44"/>
-      <c r="F92" s="42"/>
-      <c r="G92" s="42"/>
-      <c r="H92" s="42"/>
-      <c r="I92" s="3"/>
-      <c r="J92" s="4"/>
+      <c r="F92" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G92" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H92" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I92" s="3">
+        <v>298</v>
+      </c>
+      <c r="J92" s="4">
+        <v>103000000000</v>
+      </c>
       <c r="K92" s="4"/>
-      <c r="L92" s="44"/>
-      <c r="M92" s="44"/>
-      <c r="N92" s="44"/>
+      <c r="L92" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M92" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N92" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="93" spans="1:14" ht="18" customHeight="1">
       <c r="A93" s="24"/>
-      <c r="B93" s="44"/>
-      <c r="C93" s="42"/>
-      <c r="D93" s="42"/>
+      <c r="B93" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="D93" s="42" t="s">
+        <v>81</v>
+      </c>
       <c r="E93" s="44"/>
-      <c r="F93" s="42"/>
-      <c r="G93" s="42"/>
-      <c r="H93" s="42"/>
-      <c r="I93" s="3"/>
-      <c r="J93" s="4"/>
+      <c r="F93" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G93" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H93" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I93" s="3">
+        <v>298</v>
+      </c>
+      <c r="J93" s="4">
+        <v>59000000000</v>
+      </c>
       <c r="K93" s="4"/>
-      <c r="L93" s="44"/>
-      <c r="M93" s="44"/>
-      <c r="N93" s="44"/>
+      <c r="L93" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M93" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N93" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="94" spans="1:14" ht="18" customHeight="1">
       <c r="A94" s="24"/>
-      <c r="B94" s="44"/>
-      <c r="C94" s="42"/>
-      <c r="D94" s="42"/>
+      <c r="B94" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="D94" s="42" t="s">
+        <v>81</v>
+      </c>
       <c r="E94" s="44"/>
-      <c r="F94" s="42"/>
-      <c r="G94" s="42"/>
-      <c r="H94" s="42"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="4"/>
+      <c r="F94" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G94" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H94" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I94" s="3">
+        <v>298</v>
+      </c>
+      <c r="J94" s="4">
+        <v>71000000000</v>
+      </c>
       <c r="K94" s="4"/>
-      <c r="L94" s="44"/>
-      <c r="M94" s="44"/>
-      <c r="N94" s="44"/>
+      <c r="L94" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M94" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N94" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="95" spans="1:14" ht="18" customHeight="1">
       <c r="A95" s="24"/>
-      <c r="B95" s="44"/>
-      <c r="C95" s="42"/>
-      <c r="D95" s="42"/>
+      <c r="B95" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="C95" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="D95" s="42" t="s">
+        <v>186</v>
+      </c>
       <c r="E95" s="44"/>
-      <c r="F95" s="42"/>
-      <c r="G95" s="42"/>
-      <c r="H95" s="42"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="4"/>
+      <c r="F95" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G95" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H95" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I95" s="3">
+        <v>298</v>
+      </c>
+      <c r="J95" s="4">
+        <v>69000000000</v>
+      </c>
       <c r="K95" s="4"/>
-      <c r="L95" s="44"/>
-      <c r="M95" s="44"/>
-      <c r="N95" s="44"/>
+      <c r="L95" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M95" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N95" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="96" spans="1:14" ht="18" customHeight="1">
       <c r="A96" s="24"/>
-      <c r="B96" s="44"/>
-      <c r="C96" s="42"/>
-      <c r="D96" s="42"/>
+      <c r="B96" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C96" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="D96" s="42" t="s">
+        <v>186</v>
+      </c>
       <c r="E96" s="44"/>
-      <c r="F96" s="42"/>
-      <c r="G96" s="42"/>
-      <c r="H96" s="42"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="4"/>
+      <c r="F96" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G96" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H96" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I96" s="3">
+        <v>298</v>
+      </c>
+      <c r="J96" s="4">
+        <v>73000000000</v>
+      </c>
       <c r="K96" s="4"/>
-      <c r="L96" s="44"/>
-      <c r="M96" s="44"/>
-      <c r="N96" s="44"/>
+      <c r="L96" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M96" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N96" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="97" spans="1:14" ht="18" customHeight="1">
       <c r="A97" s="24"/>
-      <c r="B97" s="44"/>
+      <c r="B97" s="44" t="s">
+        <v>185</v>
+      </c>
       <c r="C97" s="42"/>
-      <c r="D97" s="42"/>
-      <c r="E97" s="44"/>
-      <c r="F97" s="42"/>
-      <c r="G97" s="42"/>
-      <c r="H97" s="42"/>
-      <c r="I97" s="3"/>
-      <c r="J97" s="4"/>
+      <c r="D97" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E97" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="F97" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G97" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H97" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I97" s="3">
+        <v>298</v>
+      </c>
+      <c r="J97" s="4">
+        <v>96000000000</v>
+      </c>
       <c r="K97" s="4"/>
-      <c r="L97" s="44"/>
-      <c r="M97" s="44"/>
-      <c r="N97" s="44"/>
+      <c r="L97" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M97" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N97" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="98" spans="1:14" ht="18" customHeight="1">
       <c r="A98" s="24"/>
-      <c r="B98" s="44"/>
-      <c r="C98" s="42"/>
-      <c r="D98" s="42"/>
+      <c r="B98" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="C98" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="D98" s="42" t="s">
+        <v>81</v>
+      </c>
       <c r="E98" s="44"/>
-      <c r="F98" s="42"/>
-      <c r="G98" s="42"/>
-      <c r="H98" s="42"/>
-      <c r="I98" s="3"/>
-      <c r="J98" s="4"/>
+      <c r="F98" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G98" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I98" s="3">
+        <v>298</v>
+      </c>
+      <c r="J98" s="4">
+        <v>1169000000</v>
+      </c>
       <c r="K98" s="4"/>
-      <c r="L98" s="44"/>
-      <c r="M98" s="44"/>
-      <c r="N98" s="44"/>
+      <c r="L98" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M98" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N98" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="99" spans="1:14" ht="18" customHeight="1">
       <c r="A99" s="24"/>
-      <c r="B99" s="44"/>
-      <c r="C99" s="42"/>
-      <c r="D99" s="42"/>
+      <c r="B99" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="D99" s="42" t="s">
+        <v>81</v>
+      </c>
       <c r="E99" s="44"/>
-      <c r="F99" s="42"/>
-      <c r="G99" s="42"/>
-      <c r="H99" s="42"/>
-      <c r="I99" s="3"/>
-      <c r="J99" s="4"/>
+      <c r="F99" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G99" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H99" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I99" s="3">
+        <v>298</v>
+      </c>
+      <c r="J99" s="4">
+        <v>1052000000</v>
+      </c>
       <c r="K99" s="4"/>
-      <c r="L99" s="44"/>
-      <c r="M99" s="44"/>
-      <c r="N99" s="44"/>
+      <c r="L99" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M99" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N99" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="100" spans="1:14" ht="18" customHeight="1">
       <c r="A100" s="24"/>
-      <c r="B100" s="44"/>
-      <c r="C100" s="42"/>
-      <c r="D100" s="42"/>
+      <c r="B100" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C100" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="D100" s="42" t="s">
+        <v>81</v>
+      </c>
       <c r="E100" s="44"/>
-      <c r="F100" s="42"/>
-      <c r="G100" s="42"/>
-      <c r="H100" s="42"/>
-      <c r="I100" s="3"/>
-      <c r="J100" s="4"/>
+      <c r="F100" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G100" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H100" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I100" s="3">
+        <v>298</v>
+      </c>
+      <c r="J100" s="4">
+        <v>1037000000</v>
+      </c>
       <c r="K100" s="4"/>
-      <c r="L100" s="44"/>
-      <c r="M100" s="44"/>
-      <c r="N100" s="44"/>
+      <c r="L100" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M100" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N100" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="101" spans="1:14" ht="18" customHeight="1">
       <c r="A101" s="24"/>
-      <c r="B101" s="44"/>
-      <c r="C101" s="42"/>
-      <c r="D101" s="42"/>
+      <c r="B101" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="C101" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="D101" s="42" t="s">
+        <v>186</v>
+      </c>
       <c r="E101" s="44"/>
-      <c r="F101" s="42"/>
-      <c r="G101" s="42"/>
-      <c r="H101" s="42"/>
-      <c r="I101" s="3"/>
-      <c r="J101" s="4"/>
+      <c r="F101" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G101" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H101" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I101" s="3">
+        <v>298</v>
+      </c>
+      <c r="J101" s="4">
+        <v>1755000000</v>
+      </c>
       <c r="K101" s="4"/>
-      <c r="L101" s="44"/>
-      <c r="M101" s="44"/>
-      <c r="N101" s="44"/>
+      <c r="L101" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M101" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N101" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="102" spans="1:14" ht="18" customHeight="1">
       <c r="A102" s="24"/>
-      <c r="B102" s="44"/>
-      <c r="C102" s="42"/>
-      <c r="D102" s="42"/>
+      <c r="B102" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C102" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="D102" s="42" t="s">
+        <v>186</v>
+      </c>
       <c r="E102" s="44"/>
-      <c r="F102" s="42"/>
-      <c r="G102" s="42"/>
-      <c r="H102" s="42"/>
-      <c r="I102" s="3"/>
-      <c r="J102" s="4"/>
+      <c r="F102" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G102" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H102" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I102" s="3">
+        <v>298</v>
+      </c>
+      <c r="J102" s="4">
+        <v>1525000000</v>
+      </c>
       <c r="K102" s="4"/>
-      <c r="L102" s="44"/>
-      <c r="M102" s="44"/>
-      <c r="N102" s="44"/>
+      <c r="L102" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M102" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N102" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="103" spans="1:14" ht="18" customHeight="1">
       <c r="A103" s="24"/>
-      <c r="B103" s="44"/>
+      <c r="B103" s="44" t="s">
+        <v>185</v>
+      </c>
       <c r="C103" s="42"/>
-      <c r="D103" s="42"/>
-      <c r="E103" s="44"/>
-      <c r="F103" s="42"/>
-      <c r="G103" s="42"/>
-      <c r="H103" s="42"/>
-      <c r="I103" s="3"/>
-      <c r="J103" s="4"/>
+      <c r="D103" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E103" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="F103" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G103" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H103" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I103" s="3">
+        <v>298</v>
+      </c>
+      <c r="J103" s="4">
+        <v>1770000000</v>
+      </c>
       <c r="K103" s="4"/>
-      <c r="L103" s="44"/>
-      <c r="M103" s="44"/>
-      <c r="N103" s="44"/>
+      <c r="L103" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M103" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N103" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="104" spans="1:14" ht="18" customHeight="1">
       <c r="A104" s="24"/>
-      <c r="B104" s="44"/>
-      <c r="C104" s="42"/>
-      <c r="D104" s="42"/>
-      <c r="E104" s="44"/>
-      <c r="F104" s="42"/>
-      <c r="G104" s="42"/>
-      <c r="H104" s="42"/>
-      <c r="I104" s="3"/>
-      <c r="J104" s="4"/>
+      <c r="B104" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="C104" s="129" t="s">
+        <v>188</v>
+      </c>
+      <c r="D104" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="E104" s="52"/>
+      <c r="F104" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G104" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H104" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I104" s="3">
+        <v>298</v>
+      </c>
+      <c r="J104" s="4">
+        <v>2578000000</v>
+      </c>
       <c r="K104" s="4"/>
-      <c r="L104" s="44"/>
-      <c r="M104" s="44"/>
-      <c r="N104" s="44"/>
+      <c r="L104" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M104" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N104" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="105" spans="1:14" ht="18" customHeight="1">
       <c r="A105" s="24"/>
-      <c r="B105" s="44"/>
-      <c r="C105" s="42"/>
-      <c r="D105" s="42"/>
-      <c r="E105" s="44"/>
-      <c r="F105" s="42"/>
-      <c r="G105" s="42"/>
-      <c r="H105" s="42"/>
-      <c r="I105" s="3"/>
-      <c r="J105" s="4"/>
+      <c r="B105" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="C105" s="129" t="s">
+        <v>189</v>
+      </c>
+      <c r="D105" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="E105" s="52"/>
+      <c r="F105" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G105" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H105" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I105" s="3">
+        <v>298</v>
+      </c>
+      <c r="J105" s="4">
+        <v>2345000000</v>
+      </c>
       <c r="K105" s="4"/>
-      <c r="L105" s="44"/>
-      <c r="M105" s="44"/>
-      <c r="N105" s="44"/>
+      <c r="L105" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M105" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N105" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="106" spans="1:14" ht="18" customHeight="1">
       <c r="A106" s="24"/>
-      <c r="B106" s="44"/>
-      <c r="C106" s="42"/>
-      <c r="D106" s="42"/>
-      <c r="E106" s="44"/>
-      <c r="F106" s="42"/>
-      <c r="G106" s="42"/>
-      <c r="H106" s="42"/>
-      <c r="I106" s="3"/>
-      <c r="J106" s="4"/>
+      <c r="B106" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="C106" s="129" t="s">
+        <v>189</v>
+      </c>
+      <c r="D106" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="E106" s="52"/>
+      <c r="F106" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G106" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H106" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I106" s="3">
+        <v>298</v>
+      </c>
+      <c r="J106" s="4">
+        <v>2196000000</v>
+      </c>
       <c r="K106" s="4"/>
-      <c r="L106" s="44"/>
-      <c r="M106" s="44"/>
-      <c r="N106" s="44"/>
+      <c r="L106" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M106" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N106" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="107" spans="1:14" ht="18" customHeight="1">
       <c r="A107" s="24"/>
-      <c r="B107" s="44"/>
-      <c r="C107" s="42"/>
-      <c r="D107" s="42"/>
-      <c r="E107" s="44"/>
-      <c r="F107" s="42"/>
-      <c r="G107" s="42"/>
-      <c r="H107" s="42"/>
-      <c r="I107" s="3"/>
-      <c r="J107" s="4"/>
+      <c r="B107" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="C107" s="129" t="s">
+        <v>188</v>
+      </c>
+      <c r="D107" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="E107" s="52"/>
+      <c r="F107" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G107" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H107" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I107" s="3">
+        <v>298</v>
+      </c>
+      <c r="J107" s="4">
+        <v>2440000000</v>
+      </c>
       <c r="K107" s="4"/>
-      <c r="L107" s="44"/>
-      <c r="M107" s="44"/>
-      <c r="N107" s="44"/>
+      <c r="L107" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M107" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N107" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="108" spans="1:14" ht="18" customHeight="1">
       <c r="A108" s="24"/>
-      <c r="B108" s="44"/>
-      <c r="C108" s="42"/>
-      <c r="D108" s="42"/>
-      <c r="E108" s="44"/>
-      <c r="F108" s="42"/>
-      <c r="G108" s="42"/>
-      <c r="H108" s="42"/>
-      <c r="I108" s="3"/>
-      <c r="J108" s="4"/>
+      <c r="B108" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C108" s="129" t="s">
+        <v>188</v>
+      </c>
+      <c r="D108" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="E108" s="52"/>
+      <c r="F108" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G108" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H108" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I108" s="3">
+        <v>298</v>
+      </c>
+      <c r="J108" s="4">
+        <v>2282000000</v>
+      </c>
       <c r="K108" s="4"/>
-      <c r="L108" s="44"/>
-      <c r="M108" s="44"/>
-      <c r="N108" s="44"/>
+      <c r="L108" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M108" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N108" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="109" spans="1:14" ht="18" customHeight="1">
       <c r="A109" s="24"/>
-      <c r="B109" s="44"/>
-      <c r="C109" s="42"/>
-      <c r="D109" s="42"/>
-      <c r="E109" s="44"/>
-      <c r="F109" s="42"/>
-      <c r="G109" s="42"/>
-      <c r="H109" s="42"/>
-      <c r="I109" s="3"/>
-      <c r="J109" s="4"/>
+      <c r="B109" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C109" s="129"/>
+      <c r="D109" s="129" t="s">
+        <v>95</v>
+      </c>
+      <c r="E109" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="F109" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G109" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H109" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I109" s="3">
+        <v>298</v>
+      </c>
+      <c r="J109" s="4">
+        <v>2285000000</v>
+      </c>
       <c r="K109" s="4"/>
-      <c r="L109" s="44"/>
-      <c r="M109" s="44"/>
-      <c r="N109" s="44"/>
+      <c r="L109" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M109" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="N109" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="110" spans="1:14" ht="18" customHeight="1">
       <c r="A110" s="24"/>
-      <c r="B110" s="44"/>
-      <c r="C110" s="42"/>
-      <c r="D110" s="42"/>
-      <c r="E110" s="44"/>
-      <c r="F110" s="42"/>
-      <c r="G110" s="42"/>
-      <c r="H110" s="42"/>
-      <c r="I110" s="3"/>
-      <c r="J110" s="4"/>
-      <c r="K110" s="4"/>
-      <c r="L110" s="44"/>
-      <c r="M110" s="44"/>
-      <c r="N110" s="44"/>
+      <c r="B110" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="C110" s="129" t="s">
+        <v>188</v>
+      </c>
+      <c r="D110" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="E110" s="52"/>
+      <c r="F110" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G110" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H110" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I110" s="3">
+        <v>298</v>
+      </c>
+      <c r="J110" s="4">
+        <v>18.798181818181799</v>
+      </c>
+      <c r="L110" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="M110" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="N110" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="111" spans="1:14" ht="18" customHeight="1">
       <c r="A111" s="24"/>
-      <c r="B111" s="44"/>
-      <c r="C111" s="42"/>
-      <c r="D111" s="42"/>
-      <c r="E111" s="44"/>
-      <c r="F111" s="42"/>
-      <c r="G111" s="42"/>
-      <c r="H111" s="42"/>
-      <c r="I111" s="3"/>
-      <c r="J111" s="4"/>
-      <c r="K111" s="4"/>
-      <c r="L111" s="44"/>
-      <c r="M111" s="44"/>
-      <c r="N111" s="44"/>
+      <c r="B111" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="C111" s="129" t="s">
+        <v>189</v>
+      </c>
+      <c r="D111" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="E111" s="52"/>
+      <c r="F111" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G111" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H111" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I111" s="3">
+        <v>298</v>
+      </c>
+      <c r="J111" s="4">
+        <v>22.416363636363599</v>
+      </c>
+      <c r="L111" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="M111" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="N111" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="112" spans="1:14" ht="18" customHeight="1">
       <c r="A112" s="24"/>
-      <c r="B112" s="44"/>
-      <c r="C112" s="42"/>
-      <c r="D112" s="42"/>
-      <c r="E112" s="44"/>
-      <c r="F112" s="42"/>
-      <c r="G112" s="42"/>
-      <c r="H112" s="42"/>
-      <c r="I112" s="3"/>
-      <c r="J112" s="4"/>
-      <c r="K112" s="4"/>
-      <c r="L112" s="44"/>
-      <c r="M112" s="44"/>
-      <c r="N112" s="44"/>
+      <c r="B112" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="C112" s="129" t="s">
+        <v>189</v>
+      </c>
+      <c r="D112" s="129" t="s">
+        <v>81</v>
+      </c>
+      <c r="E112" s="52"/>
+      <c r="F112" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G112" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H112" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I112" s="3">
+        <v>298</v>
+      </c>
+      <c r="J112" s="4">
+        <v>16.798181818181799</v>
+      </c>
+      <c r="L112" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="M112" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="N112" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="113" spans="1:14" ht="18" customHeight="1">
       <c r="A113" s="24"/>
-      <c r="B113" s="44"/>
-      <c r="C113" s="42"/>
-      <c r="D113" s="42"/>
-      <c r="E113" s="44"/>
-      <c r="F113" s="42"/>
-      <c r="G113" s="42"/>
-      <c r="H113" s="42"/>
-      <c r="I113" s="3"/>
-      <c r="J113" s="4"/>
-      <c r="K113" s="4"/>
-      <c r="L113" s="44"/>
-      <c r="M113" s="44"/>
-      <c r="N113" s="44"/>
+      <c r="B113" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="C113" s="129" t="s">
+        <v>188</v>
+      </c>
+      <c r="D113" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="E113" s="52"/>
+      <c r="F113" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G113" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H113" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I113" s="3">
+        <v>298</v>
+      </c>
+      <c r="J113" s="4">
+        <v>7.0336363636363597</v>
+      </c>
+      <c r="L113" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="M113" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="N113" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="114" spans="1:14" ht="18" customHeight="1">
       <c r="A114" s="24"/>
-      <c r="B114" s="44"/>
-      <c r="C114" s="42"/>
-      <c r="D114" s="42"/>
-      <c r="E114" s="44"/>
-      <c r="F114" s="42"/>
-      <c r="G114" s="42"/>
-      <c r="H114" s="42"/>
-      <c r="I114" s="3"/>
-      <c r="J114" s="4"/>
-      <c r="K114" s="4"/>
-      <c r="L114" s="44"/>
-      <c r="M114" s="44"/>
-      <c r="N114" s="44"/>
+      <c r="B114" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C114" s="129" t="s">
+        <v>188</v>
+      </c>
+      <c r="D114" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="E114" s="52"/>
+      <c r="F114" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G114" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H114" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I114" s="3">
+        <v>298</v>
+      </c>
+      <c r="J114" s="4">
+        <v>8.07</v>
+      </c>
+      <c r="L114" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="M114" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="N114" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="115" spans="1:14" ht="18" customHeight="1">
       <c r="A115" s="24"/>
-      <c r="B115" s="44"/>
-      <c r="C115" s="42"/>
-      <c r="D115" s="42"/>
-      <c r="E115" s="44"/>
-      <c r="F115" s="42"/>
-      <c r="G115" s="42"/>
-      <c r="H115" s="42"/>
-      <c r="I115" s="3"/>
-      <c r="J115" s="4"/>
-      <c r="K115" s="4"/>
-      <c r="L115" s="44"/>
-      <c r="M115" s="44"/>
-      <c r="N115" s="44"/>
+      <c r="B115" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C115" s="129"/>
+      <c r="D115" s="129" t="s">
+        <v>95</v>
+      </c>
+      <c r="E115" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="F115" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G115" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H115" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I115" s="3">
+        <v>298</v>
+      </c>
+      <c r="J115" s="4">
+        <v>3.5609090909090901</v>
+      </c>
+      <c r="L115" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="M115" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="N115" s="44" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="116" spans="1:14" ht="18" customHeight="1">
       <c r="A116" s="24"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.jallcom.2016.10.286`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B752A7F3-7E7E-8949-9791-57C76C038B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18654C9D-EC42-7949-A0F1-9E534977F4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6820" yWindow="760" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="240">
   <si>
     <r>
       <rPr>
@@ -775,6 +775,72 @@
   <si>
     <t>10.1016/j.jallcom.2021.163388</t>
   </si>
+  <si>
+    <t>B27 is YNi (oP8-FeB-b); Y2Ni17 has structure (hP38-Th2Ni17); YCo3 has structure (hR36-PuNi3)</t>
+  </si>
+  <si>
+    <t>CoCrFeNiY</t>
+  </si>
+  <si>
+    <t>BCC+B27+Y2Ni17+YCo3</t>
+  </si>
+  <si>
+    <t>chi has structure (cI58-Ti5Re24); D024 aka eta-Ni3Ti has structure (hP16-TiNi3)</t>
+  </si>
+  <si>
+    <t>chi+C14+D024</t>
+  </si>
+  <si>
+    <t>CoCrFeNiTi</t>
+  </si>
+  <si>
+    <t>CoCrFeNiZr</t>
+  </si>
+  <si>
+    <t>CoCrFeNiHf</t>
+  </si>
+  <si>
+    <t>CoCrFeNiV</t>
+  </si>
+  <si>
+    <t>CoCrFeNiNb</t>
+  </si>
+  <si>
+    <t>CoCrFeNiTa</t>
+  </si>
+  <si>
+    <t>CoCrFeNiMo</t>
+  </si>
+  <si>
+    <t>CoCrFeNiW</t>
+  </si>
+  <si>
+    <t>BCC+C15</t>
+  </si>
+  <si>
+    <t>BCC+C36</t>
+  </si>
+  <si>
+    <t>FCC+sigma</t>
+  </si>
+  <si>
+    <t>FCC+C14</t>
+  </si>
+  <si>
+    <t>CoCr2FeNi</t>
+  </si>
+  <si>
+    <t>D85 aka mu is (hR39-W6Fe7)</t>
+  </si>
+  <si>
+    <t>FCC+D85</t>
+  </si>
+  <si>
+    <t>VAM</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2016.10.286</t>
+  </si>
 </sst>
 </file>
 
@@ -936,7 +1002,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1559,11 +1625,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1920,6 +1997,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3082,8 +3163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A92" zoomScale="86" workbookViewId="0">
-      <selection activeCell="M136" sqref="M136"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="86" workbookViewId="0">
+      <selection activeCell="M145" sqref="M145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -8602,10 +8683,18 @@
     </row>
     <row r="132" spans="1:20" ht="18" customHeight="1">
       <c r="A132" s="64"/>
-      <c r="B132" s="73"/>
-      <c r="C132" s="68"/>
-      <c r="D132" s="68"/>
-      <c r="E132" s="73"/>
+      <c r="B132" s="148" t="s">
+        <v>219</v>
+      </c>
+      <c r="C132" s="150" t="s">
+        <v>220</v>
+      </c>
+      <c r="D132" s="149" t="s">
+        <v>238</v>
+      </c>
+      <c r="E132" s="149" t="s">
+        <v>218</v>
+      </c>
       <c r="F132" s="68"/>
       <c r="G132" s="68"/>
       <c r="H132" s="68"/>
@@ -8614,7 +8703,9 @@
       <c r="K132" s="70"/>
       <c r="L132" s="68"/>
       <c r="M132" s="68"/>
-      <c r="N132" s="68"/>
+      <c r="N132" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O132" s="9"/>
       <c r="P132" s="4"/>
       <c r="Q132" s="4"/>
@@ -8624,10 +8715,18 @@
     </row>
     <row r="133" spans="1:20" ht="18" customHeight="1">
       <c r="A133" s="64"/>
-      <c r="B133" s="73"/>
-      <c r="C133" s="68"/>
-      <c r="D133" s="68"/>
-      <c r="E133" s="73"/>
+      <c r="B133" s="148" t="s">
+        <v>223</v>
+      </c>
+      <c r="C133" s="149" t="s">
+        <v>222</v>
+      </c>
+      <c r="D133" s="149" t="s">
+        <v>238</v>
+      </c>
+      <c r="E133" s="148" t="s">
+        <v>221</v>
+      </c>
       <c r="F133" s="68"/>
       <c r="G133" s="68"/>
       <c r="H133" s="68"/>
@@ -8636,7 +8735,9 @@
       <c r="K133" s="70"/>
       <c r="L133" s="68"/>
       <c r="M133" s="68"/>
-      <c r="N133" s="68"/>
+      <c r="N133" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O133" s="9"/>
       <c r="P133" s="4"/>
       <c r="Q133" s="4"/>
@@ -8646,9 +8747,15 @@
     </row>
     <row r="134" spans="1:20" ht="18" customHeight="1">
       <c r="A134" s="64"/>
-      <c r="B134" s="73"/>
-      <c r="C134" s="68"/>
-      <c r="D134" s="68"/>
+      <c r="B134" s="148" t="s">
+        <v>224</v>
+      </c>
+      <c r="C134" s="149" t="s">
+        <v>231</v>
+      </c>
+      <c r="D134" s="149" t="s">
+        <v>238</v>
+      </c>
       <c r="E134" s="73"/>
       <c r="F134" s="68"/>
       <c r="G134" s="68"/>
@@ -8658,7 +8765,9 @@
       <c r="K134" s="70"/>
       <c r="L134" s="68"/>
       <c r="M134" s="68"/>
-      <c r="N134" s="68"/>
+      <c r="N134" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O134" s="9"/>
       <c r="P134" s="4"/>
       <c r="Q134" s="4"/>
@@ -8668,9 +8777,15 @@
     </row>
     <row r="135" spans="1:20" ht="18" customHeight="1">
       <c r="A135" s="64"/>
-      <c r="B135" s="73"/>
-      <c r="C135" s="68"/>
-      <c r="D135" s="68"/>
+      <c r="B135" s="148" t="s">
+        <v>225</v>
+      </c>
+      <c r="C135" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="D135" s="149" t="s">
+        <v>238</v>
+      </c>
       <c r="E135" s="73"/>
       <c r="F135" s="68"/>
       <c r="G135" s="68"/>
@@ -8680,7 +8795,9 @@
       <c r="K135" s="70"/>
       <c r="L135" s="68"/>
       <c r="M135" s="68"/>
-      <c r="N135" s="68"/>
+      <c r="N135" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O135" s="9"/>
       <c r="P135" s="4"/>
       <c r="Q135" s="4"/>
@@ -8690,9 +8807,15 @@
     </row>
     <row r="136" spans="1:20" ht="18" customHeight="1">
       <c r="A136" s="64"/>
-      <c r="B136" s="73"/>
-      <c r="C136" s="68"/>
-      <c r="D136" s="68"/>
+      <c r="B136" s="148" t="s">
+        <v>226</v>
+      </c>
+      <c r="C136" s="149" t="s">
+        <v>233</v>
+      </c>
+      <c r="D136" s="149" t="s">
+        <v>238</v>
+      </c>
       <c r="E136" s="73"/>
       <c r="F136" s="68"/>
       <c r="G136" s="68"/>
@@ -8702,7 +8825,9 @@
       <c r="K136" s="70"/>
       <c r="L136" s="68"/>
       <c r="M136" s="68"/>
-      <c r="N136" s="68"/>
+      <c r="N136" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O136" s="9"/>
       <c r="P136" s="4"/>
       <c r="Q136" s="4"/>
@@ -8712,9 +8837,15 @@
     </row>
     <row r="137" spans="1:20" ht="18" customHeight="1">
       <c r="A137" s="64"/>
-      <c r="B137" s="73"/>
-      <c r="C137" s="68"/>
-      <c r="D137" s="68"/>
+      <c r="B137" s="148" t="s">
+        <v>227</v>
+      </c>
+      <c r="C137" s="149" t="s">
+        <v>234</v>
+      </c>
+      <c r="D137" s="149" t="s">
+        <v>238</v>
+      </c>
       <c r="E137" s="73"/>
       <c r="F137" s="68"/>
       <c r="G137" s="68"/>
@@ -8724,7 +8855,9 @@
       <c r="K137" s="70"/>
       <c r="L137" s="68"/>
       <c r="M137" s="68"/>
-      <c r="N137" s="68"/>
+      <c r="N137" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O137" s="9"/>
       <c r="P137" s="4"/>
       <c r="Q137" s="4"/>
@@ -8734,9 +8867,15 @@
     </row>
     <row r="138" spans="1:20" ht="18" customHeight="1">
       <c r="A138" s="64"/>
-      <c r="B138" s="73"/>
-      <c r="C138" s="68"/>
-      <c r="D138" s="68"/>
+      <c r="B138" s="148" t="s">
+        <v>228</v>
+      </c>
+      <c r="C138" s="149" t="s">
+        <v>234</v>
+      </c>
+      <c r="D138" s="149" t="s">
+        <v>238</v>
+      </c>
       <c r="E138" s="73"/>
       <c r="F138" s="68"/>
       <c r="G138" s="68"/>
@@ -8746,7 +8885,9 @@
       <c r="K138" s="70"/>
       <c r="L138" s="68"/>
       <c r="M138" s="68"/>
-      <c r="N138" s="68"/>
+      <c r="N138" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O138" s="9"/>
       <c r="P138" s="4"/>
       <c r="Q138" s="4"/>
@@ -8756,9 +8897,15 @@
     </row>
     <row r="139" spans="1:20" ht="18" customHeight="1">
       <c r="A139" s="64"/>
-      <c r="B139" s="73"/>
-      <c r="C139" s="68"/>
-      <c r="D139" s="68"/>
+      <c r="B139" s="148" t="s">
+        <v>235</v>
+      </c>
+      <c r="C139" s="149" t="s">
+        <v>83</v>
+      </c>
+      <c r="D139" s="149" t="s">
+        <v>238</v>
+      </c>
       <c r="E139" s="73"/>
       <c r="F139" s="68"/>
       <c r="G139" s="68"/>
@@ -8768,7 +8915,9 @@
       <c r="K139" s="70"/>
       <c r="L139" s="68"/>
       <c r="M139" s="68"/>
-      <c r="N139" s="68"/>
+      <c r="N139" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O139" s="9"/>
       <c r="P139" s="4"/>
       <c r="Q139" s="4"/>
@@ -8778,9 +8927,15 @@
     </row>
     <row r="140" spans="1:20" ht="18" customHeight="1">
       <c r="A140" s="64"/>
-      <c r="B140" s="73"/>
-      <c r="C140" s="68"/>
-      <c r="D140" s="68"/>
+      <c r="B140" s="148" t="s">
+        <v>229</v>
+      </c>
+      <c r="C140" s="149" t="s">
+        <v>233</v>
+      </c>
+      <c r="D140" s="149" t="s">
+        <v>238</v>
+      </c>
       <c r="E140" s="73"/>
       <c r="F140" s="68"/>
       <c r="G140" s="68"/>
@@ -8790,7 +8945,9 @@
       <c r="K140" s="70"/>
       <c r="L140" s="68"/>
       <c r="M140" s="68"/>
-      <c r="N140" s="68"/>
+      <c r="N140" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O140" s="9"/>
       <c r="P140" s="4"/>
       <c r="Q140" s="4"/>
@@ -8800,10 +8957,18 @@
     </row>
     <row r="141" spans="1:20" ht="18" customHeight="1">
       <c r="A141" s="64"/>
-      <c r="B141" s="73"/>
-      <c r="C141" s="68"/>
-      <c r="D141" s="68"/>
-      <c r="E141" s="73"/>
+      <c r="B141" s="148" t="s">
+        <v>230</v>
+      </c>
+      <c r="C141" s="149" t="s">
+        <v>237</v>
+      </c>
+      <c r="D141" s="149" t="s">
+        <v>238</v>
+      </c>
+      <c r="E141" s="151" t="s">
+        <v>236</v>
+      </c>
       <c r="F141" s="68"/>
       <c r="G141" s="68"/>
       <c r="H141" s="68"/>
@@ -8812,7 +8977,9 @@
       <c r="K141" s="70"/>
       <c r="L141" s="68"/>
       <c r="M141" s="68"/>
-      <c r="N141" s="68"/>
+      <c r="N141" s="149" t="s">
+        <v>239</v>
+      </c>
       <c r="O141" s="9"/>
       <c r="P141" s="4"/>
       <c r="Q141" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2020.155929`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18654C9D-EC42-7949-A0F1-9E534977F4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705BD1A4-B83F-2F4C-9066-83DE12716536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="760" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9280" yWindow="800" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="248">
   <si>
     <r>
       <rPr>
@@ -841,6 +841,30 @@
   <si>
     <t>10.1016/j.jallcom.2016.10.286</t>
   </si>
+  <si>
+    <t>FeCr1.2Ni1.5Al</t>
+  </si>
+  <si>
+    <t>FeCr1.2Ni1.1Al</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2020.155929</t>
+  </si>
+  <si>
+    <t>FeCr1.2Ni1.3Al</t>
+  </si>
+  <si>
+    <t>minor B2 phase could have been missed by others</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>minimum compressive ductility</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
 </sst>
 </file>
 
@@ -1640,7 +1664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2001,6 +2025,7 @@
     <xf numFmtId="3" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3163,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="86" workbookViewId="0">
-      <selection activeCell="M145" sqref="M145"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A129" zoomScale="86" workbookViewId="0">
+      <selection activeCell="G168" sqref="G168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -8989,19 +9014,41 @@
     </row>
     <row r="142" spans="1:20" ht="18" customHeight="1">
       <c r="A142" s="64"/>
-      <c r="B142" s="73"/>
-      <c r="C142" s="68"/>
-      <c r="D142" s="68"/>
-      <c r="E142" s="73"/>
-      <c r="F142" s="68"/>
-      <c r="G142" s="68"/>
+      <c r="B142" s="148" t="s">
+        <v>241</v>
+      </c>
+      <c r="C142" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D142" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E142" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F142" s="149" t="s">
+        <v>67</v>
+      </c>
+      <c r="G142" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H142" s="68"/>
-      <c r="I142" s="83"/>
-      <c r="J142" s="70"/>
+      <c r="I142" s="83">
+        <v>298</v>
+      </c>
+      <c r="J142" s="70">
+        <v>6600</v>
+      </c>
       <c r="K142" s="70"/>
-      <c r="L142" s="68"/>
-      <c r="M142" s="68"/>
-      <c r="N142" s="68"/>
+      <c r="L142" s="149" t="s">
+        <v>68</v>
+      </c>
+      <c r="M142" s="149" t="s">
+        <v>86</v>
+      </c>
+      <c r="N142" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O142" s="9"/>
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
@@ -9011,19 +9058,41 @@
     </row>
     <row r="143" spans="1:20" ht="18" customHeight="1">
       <c r="A143" s="64"/>
-      <c r="B143" s="73"/>
-      <c r="C143" s="68"/>
-      <c r="D143" s="68"/>
-      <c r="E143" s="73"/>
-      <c r="F143" s="68"/>
-      <c r="G143" s="68"/>
+      <c r="B143" s="148" t="s">
+        <v>243</v>
+      </c>
+      <c r="C143" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D143" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E143" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F143" s="149" t="s">
+        <v>67</v>
+      </c>
+      <c r="G143" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H143" s="68"/>
-      <c r="I143" s="83"/>
-      <c r="J143" s="70"/>
+      <c r="I143" s="83">
+        <v>298</v>
+      </c>
+      <c r="J143" s="70">
+        <v>6740</v>
+      </c>
       <c r="K143" s="70"/>
-      <c r="L143" s="68"/>
-      <c r="M143" s="68"/>
-      <c r="N143" s="68"/>
+      <c r="L143" s="149" t="s">
+        <v>68</v>
+      </c>
+      <c r="M143" s="149" t="s">
+        <v>86</v>
+      </c>
+      <c r="N143" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O143" s="9"/>
       <c r="P143" s="4"/>
       <c r="Q143" s="4"/>
@@ -9033,19 +9102,41 @@
     </row>
     <row r="144" spans="1:20" ht="18" customHeight="1">
       <c r="A144" s="64"/>
-      <c r="B144" s="73"/>
-      <c r="C144" s="68"/>
-      <c r="D144" s="68"/>
-      <c r="E144" s="73"/>
-      <c r="F144" s="68"/>
-      <c r="G144" s="68"/>
+      <c r="B144" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C144" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D144" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E144" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F144" s="149" t="s">
+        <v>67</v>
+      </c>
+      <c r="G144" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H144" s="68"/>
-      <c r="I144" s="83"/>
-      <c r="J144" s="4"/>
+      <c r="I144" s="83">
+        <v>298</v>
+      </c>
+      <c r="J144" s="4">
+        <v>6850</v>
+      </c>
       <c r="K144" s="70"/>
-      <c r="L144" s="68"/>
-      <c r="M144" s="68"/>
-      <c r="N144" s="68"/>
+      <c r="L144" s="149" t="s">
+        <v>68</v>
+      </c>
+      <c r="M144" s="149" t="s">
+        <v>86</v>
+      </c>
+      <c r="N144" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O144" s="9"/>
       <c r="P144" s="4"/>
       <c r="Q144" s="4"/>
@@ -9055,21 +9146,46 @@
     </row>
     <row r="145" spans="1:20" ht="18" customHeight="1">
       <c r="A145" s="64"/>
-      <c r="B145" s="73"/>
-      <c r="C145" s="68"/>
-      <c r="D145" s="68"/>
-      <c r="E145" s="73"/>
-      <c r="F145" s="68"/>
-      <c r="G145" s="68"/>
+      <c r="B145" s="148" t="s">
+        <v>241</v>
+      </c>
+      <c r="C145" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D145" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E145" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F145" s="149" t="s">
+        <v>77</v>
+      </c>
+      <c r="G145" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H145" s="68"/>
-      <c r="I145" s="83"/>
-      <c r="J145" s="70"/>
+      <c r="I145" s="83">
+        <v>298</v>
+      </c>
+      <c r="J145" s="70">
+        <f t="shared" ref="J145:J147" si="4">P145*9807000</f>
+        <v>4506316500</v>
+      </c>
       <c r="K145" s="70"/>
-      <c r="L145" s="68"/>
-      <c r="M145" s="68"/>
-      <c r="N145" s="68"/>
+      <c r="L145" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M145" s="149" t="s">
+        <v>86</v>
+      </c>
+      <c r="N145" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O145" s="9"/>
-      <c r="P145" s="4"/>
+      <c r="P145" s="4">
+        <v>459.5</v>
+      </c>
       <c r="Q145" s="4"/>
       <c r="R145" s="9"/>
       <c r="S145" s="9"/>
@@ -9077,21 +9193,46 @@
     </row>
     <row r="146" spans="1:20" ht="18" customHeight="1">
       <c r="A146" s="64"/>
-      <c r="B146" s="73"/>
-      <c r="C146" s="68"/>
-      <c r="D146" s="68"/>
-      <c r="E146" s="73"/>
-      <c r="F146" s="68"/>
-      <c r="G146" s="68"/>
+      <c r="B146" s="148" t="s">
+        <v>243</v>
+      </c>
+      <c r="C146" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D146" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E146" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F146" s="149" t="s">
+        <v>77</v>
+      </c>
+      <c r="G146" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H146" s="68"/>
-      <c r="I146" s="83"/>
-      <c r="J146" s="70"/>
+      <c r="I146" s="83">
+        <v>298</v>
+      </c>
+      <c r="J146" s="70">
+        <f t="shared" si="4"/>
+        <v>4597521600</v>
+      </c>
       <c r="K146" s="70"/>
-      <c r="L146" s="68"/>
-      <c r="M146" s="68"/>
-      <c r="N146" s="68"/>
+      <c r="L146" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M146" s="149" t="s">
+        <v>86</v>
+      </c>
+      <c r="N146" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O146" s="9"/>
-      <c r="P146" s="4"/>
+      <c r="P146" s="4">
+        <v>468.8</v>
+      </c>
       <c r="Q146" s="4"/>
       <c r="R146" s="9"/>
       <c r="S146" s="9"/>
@@ -9099,21 +9240,46 @@
     </row>
     <row r="147" spans="1:20" ht="18" customHeight="1">
       <c r="A147" s="64"/>
-      <c r="B147" s="73"/>
-      <c r="C147" s="68"/>
-      <c r="D147" s="68"/>
-      <c r="E147" s="73"/>
-      <c r="F147" s="68"/>
-      <c r="G147" s="68"/>
+      <c r="B147" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C147" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D147" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E147" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F147" s="149" t="s">
+        <v>77</v>
+      </c>
+      <c r="G147" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H147" s="68"/>
-      <c r="I147" s="83"/>
-      <c r="J147" s="70"/>
+      <c r="I147" s="83">
+        <v>298</v>
+      </c>
+      <c r="J147" s="70">
+        <f t="shared" si="4"/>
+        <v>4704417900</v>
+      </c>
       <c r="K147" s="70"/>
-      <c r="L147" s="68"/>
-      <c r="M147" s="68"/>
-      <c r="N147" s="68"/>
+      <c r="L147" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M147" s="149" t="s">
+        <v>86</v>
+      </c>
+      <c r="N147" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O147" s="9"/>
-      <c r="P147" s="4"/>
+      <c r="P147" s="4">
+        <v>479.7</v>
+      </c>
       <c r="Q147" s="4"/>
       <c r="R147" s="9"/>
       <c r="S147" s="9"/>
@@ -9121,19 +9287,41 @@
     </row>
     <row r="148" spans="1:20" ht="18" customHeight="1">
       <c r="A148" s="64"/>
-      <c r="B148" s="73"/>
-      <c r="C148" s="68"/>
-      <c r="D148" s="68"/>
-      <c r="E148" s="73"/>
-      <c r="F148" s="68"/>
-      <c r="G148" s="68"/>
+      <c r="B148" s="148" t="s">
+        <v>241</v>
+      </c>
+      <c r="C148" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D148" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E148" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F148" s="149" t="s">
+        <v>189</v>
+      </c>
+      <c r="G148" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H148" s="68"/>
-      <c r="I148" s="83"/>
-      <c r="J148" s="70"/>
+      <c r="I148" s="83">
+        <v>298</v>
+      </c>
+      <c r="J148" s="70">
+        <v>2783000000</v>
+      </c>
       <c r="K148" s="70"/>
-      <c r="L148" s="68"/>
-      <c r="M148" s="68"/>
-      <c r="N148" s="68"/>
+      <c r="L148" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M148" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N148" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O148" s="9"/>
       <c r="P148" s="4"/>
       <c r="Q148" s="4"/>
@@ -9143,19 +9331,41 @@
     </row>
     <row r="149" spans="1:20" ht="18" customHeight="1">
       <c r="A149" s="64"/>
-      <c r="B149" s="73"/>
-      <c r="C149" s="68"/>
-      <c r="D149" s="68"/>
-      <c r="E149" s="73"/>
-      <c r="F149" s="68"/>
-      <c r="G149" s="68"/>
+      <c r="B149" s="148" t="s">
+        <v>243</v>
+      </c>
+      <c r="C149" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D149" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E149" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F149" s="149" t="s">
+        <v>189</v>
+      </c>
+      <c r="G149" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H149" s="68"/>
-      <c r="I149" s="83"/>
-      <c r="J149" s="70"/>
+      <c r="I149" s="83">
+        <v>298</v>
+      </c>
+      <c r="J149" s="70">
+        <v>3069000000</v>
+      </c>
       <c r="K149" s="70"/>
-      <c r="L149" s="68"/>
-      <c r="M149" s="68"/>
-      <c r="N149" s="68"/>
+      <c r="L149" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M149" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N149" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O149" s="9"/>
       <c r="P149" s="4"/>
       <c r="Q149" s="4"/>
@@ -9165,19 +9375,41 @@
     </row>
     <row r="150" spans="1:20" ht="18" customHeight="1">
       <c r="A150" s="64"/>
-      <c r="B150" s="73"/>
-      <c r="C150" s="68"/>
-      <c r="D150" s="68"/>
-      <c r="E150" s="73"/>
-      <c r="F150" s="68"/>
-      <c r="G150" s="68"/>
+      <c r="B150" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C150" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D150" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E150" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F150" s="149" t="s">
+        <v>189</v>
+      </c>
+      <c r="G150" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H150" s="68"/>
-      <c r="I150" s="83"/>
-      <c r="J150" s="70"/>
+      <c r="I150" s="83">
+        <v>298</v>
+      </c>
+      <c r="J150" s="70">
+        <v>3184000000</v>
+      </c>
       <c r="K150" s="70"/>
-      <c r="L150" s="68"/>
-      <c r="M150" s="68"/>
-      <c r="N150" s="68"/>
+      <c r="L150" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M150" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N150" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O150" s="9"/>
       <c r="P150" s="4"/>
       <c r="Q150" s="4"/>
@@ -9187,19 +9419,41 @@
     </row>
     <row r="151" spans="1:20" ht="18" customHeight="1">
       <c r="A151" s="64"/>
-      <c r="B151" s="73"/>
-      <c r="C151" s="68"/>
-      <c r="D151" s="68"/>
-      <c r="E151" s="73"/>
-      <c r="F151" s="68"/>
-      <c r="G151" s="68"/>
+      <c r="B151" s="148" t="s">
+        <v>241</v>
+      </c>
+      <c r="C151" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D151" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E151" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F151" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G151" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H151" s="68"/>
-      <c r="I151" s="83"/>
-      <c r="J151" s="70"/>
+      <c r="I151" s="83">
+        <v>298</v>
+      </c>
+      <c r="J151" s="70">
+        <v>1348000000</v>
+      </c>
       <c r="K151" s="70"/>
-      <c r="L151" s="68"/>
-      <c r="M151" s="68"/>
-      <c r="N151" s="68"/>
+      <c r="L151" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M151" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N151" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O151" s="9"/>
       <c r="P151" s="4"/>
       <c r="Q151" s="4"/>
@@ -9209,19 +9463,41 @@
     </row>
     <row r="152" spans="1:20" ht="18" customHeight="1">
       <c r="A152" s="64"/>
-      <c r="B152" s="73"/>
-      <c r="C152" s="68"/>
-      <c r="D152" s="68"/>
-      <c r="E152" s="73"/>
-      <c r="F152" s="68"/>
-      <c r="G152" s="68"/>
+      <c r="B152" s="148" t="s">
+        <v>243</v>
+      </c>
+      <c r="C152" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D152" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E152" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F152" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G152" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H152" s="68"/>
-      <c r="I152" s="83"/>
-      <c r="J152" s="70"/>
+      <c r="I152" s="83">
+        <v>298</v>
+      </c>
+      <c r="J152" s="70">
+        <v>1413000000</v>
+      </c>
       <c r="K152" s="70"/>
-      <c r="L152" s="68"/>
-      <c r="M152" s="68"/>
-      <c r="N152" s="68"/>
+      <c r="L152" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M152" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N152" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O152" s="9"/>
       <c r="P152" s="4"/>
       <c r="Q152" s="4"/>
@@ -9231,19 +9507,41 @@
     </row>
     <row r="153" spans="1:20" ht="18" customHeight="1">
       <c r="A153" s="64"/>
-      <c r="B153" s="73"/>
-      <c r="C153" s="68"/>
-      <c r="D153" s="68"/>
-      <c r="E153" s="73"/>
-      <c r="F153" s="68"/>
-      <c r="G153" s="68"/>
+      <c r="B153" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C153" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D153" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E153" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F153" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G153" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H153" s="68"/>
-      <c r="I153" s="83"/>
-      <c r="J153" s="70"/>
+      <c r="I153" s="83">
+        <v>298</v>
+      </c>
+      <c r="J153" s="70">
+        <v>1459000000</v>
+      </c>
       <c r="K153" s="70"/>
-      <c r="L153" s="68"/>
-      <c r="M153" s="68"/>
-      <c r="N153" s="68"/>
+      <c r="L153" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M153" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N153" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O153" s="9"/>
       <c r="P153" s="4"/>
       <c r="Q153" s="4"/>
@@ -9253,19 +9551,41 @@
     </row>
     <row r="154" spans="1:20" ht="18" customHeight="1">
       <c r="A154" s="64"/>
-      <c r="B154" s="73"/>
-      <c r="C154" s="68"/>
-      <c r="D154" s="68"/>
-      <c r="E154" s="73"/>
-      <c r="F154" s="68"/>
-      <c r="G154" s="68"/>
+      <c r="B154" s="148" t="s">
+        <v>241</v>
+      </c>
+      <c r="C154" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D154" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E154" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F154" s="149" t="s">
+        <v>170</v>
+      </c>
+      <c r="G154" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H154" s="68"/>
-      <c r="I154" s="83"/>
-      <c r="J154" s="70"/>
+      <c r="I154" s="83">
+        <v>298</v>
+      </c>
+      <c r="J154" s="70">
+        <v>33.9</v>
+      </c>
       <c r="K154" s="70"/>
-      <c r="L154" s="68"/>
-      <c r="M154" s="68"/>
-      <c r="N154" s="68"/>
+      <c r="L154" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M154" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N154" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O154" s="9"/>
       <c r="P154" s="4"/>
       <c r="Q154" s="4"/>
@@ -9275,19 +9595,41 @@
     </row>
     <row r="155" spans="1:20" ht="18" customHeight="1">
       <c r="A155" s="64"/>
-      <c r="B155" s="73"/>
-      <c r="C155" s="68"/>
-      <c r="D155" s="68"/>
-      <c r="E155" s="73"/>
-      <c r="F155" s="68"/>
-      <c r="G155" s="68"/>
+      <c r="B155" s="148" t="s">
+        <v>243</v>
+      </c>
+      <c r="C155" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D155" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E155" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F155" s="149" t="s">
+        <v>170</v>
+      </c>
+      <c r="G155" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H155" s="68"/>
-      <c r="I155" s="83"/>
-      <c r="J155" s="70"/>
+      <c r="I155" s="83">
+        <v>298</v>
+      </c>
+      <c r="J155" s="70">
+        <v>35.9</v>
+      </c>
       <c r="K155" s="70"/>
-      <c r="L155" s="68"/>
-      <c r="M155" s="68"/>
-      <c r="N155" s="68"/>
+      <c r="L155" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M155" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N155" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O155" s="9"/>
       <c r="P155" s="4"/>
       <c r="Q155" s="4"/>
@@ -9297,19 +9639,41 @@
     </row>
     <row r="156" spans="1:20" ht="18" customHeight="1">
       <c r="A156" s="64"/>
-      <c r="B156" s="73"/>
-      <c r="C156" s="68"/>
-      <c r="D156" s="68"/>
-      <c r="E156" s="73"/>
-      <c r="F156" s="68"/>
-      <c r="G156" s="68"/>
+      <c r="B156" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C156" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D156" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E156" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F156" s="149" t="s">
+        <v>170</v>
+      </c>
+      <c r="G156" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H156" s="68"/>
-      <c r="I156" s="83"/>
-      <c r="J156" s="70"/>
+      <c r="I156" s="83">
+        <v>298</v>
+      </c>
+      <c r="J156" s="70">
+        <v>36.6</v>
+      </c>
       <c r="K156" s="70"/>
-      <c r="L156" s="68"/>
-      <c r="M156" s="68"/>
-      <c r="N156" s="68"/>
+      <c r="L156" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M156" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N156" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O156" s="9"/>
       <c r="P156" s="4"/>
       <c r="Q156" s="4"/>
@@ -9319,19 +9683,41 @@
     </row>
     <row r="157" spans="1:20" ht="18" customHeight="1">
       <c r="A157" s="64"/>
-      <c r="B157" s="73"/>
-      <c r="C157" s="68"/>
-      <c r="D157" s="68"/>
-      <c r="E157" s="73"/>
-      <c r="F157" s="68"/>
-      <c r="G157" s="68"/>
+      <c r="B157" s="148" t="s">
+        <v>241</v>
+      </c>
+      <c r="C157" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D157" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E157" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F157" s="149" t="s">
+        <v>189</v>
+      </c>
+      <c r="G157" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H157" s="68"/>
-      <c r="I157" s="83"/>
-      <c r="J157" s="70"/>
+      <c r="I157" s="152">
+        <v>1173</v>
+      </c>
+      <c r="J157" s="70">
+        <v>281000000</v>
+      </c>
       <c r="K157" s="70"/>
-      <c r="L157" s="68"/>
-      <c r="M157" s="68"/>
-      <c r="N157" s="68"/>
+      <c r="L157" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M157" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N157" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O157" s="9"/>
       <c r="P157" s="4"/>
       <c r="Q157" s="4"/>
@@ -9341,19 +9727,41 @@
     </row>
     <row r="158" spans="1:20" ht="18" customHeight="1">
       <c r="A158" s="64"/>
-      <c r="B158" s="73"/>
-      <c r="C158" s="68"/>
-      <c r="D158" s="68"/>
-      <c r="E158" s="73"/>
-      <c r="F158" s="68"/>
-      <c r="G158" s="68"/>
+      <c r="B158" s="148" t="s">
+        <v>243</v>
+      </c>
+      <c r="C158" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D158" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E158" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F158" s="149" t="s">
+        <v>189</v>
+      </c>
+      <c r="G158" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H158" s="68"/>
-      <c r="I158" s="83"/>
-      <c r="J158" s="70"/>
+      <c r="I158" s="152">
+        <v>1173</v>
+      </c>
+      <c r="J158" s="70">
+        <v>255000000</v>
+      </c>
       <c r="K158" s="70"/>
-      <c r="L158" s="68"/>
-      <c r="M158" s="68"/>
-      <c r="N158" s="68"/>
+      <c r="L158" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M158" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N158" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O158" s="9"/>
       <c r="P158" s="4"/>
       <c r="Q158" s="4"/>
@@ -9363,19 +9771,41 @@
     </row>
     <row r="159" spans="1:20" ht="18" customHeight="1">
       <c r="A159" s="64"/>
-      <c r="B159" s="73"/>
-      <c r="C159" s="68"/>
-      <c r="D159" s="68"/>
-      <c r="E159" s="73"/>
-      <c r="F159" s="68"/>
-      <c r="G159" s="68"/>
+      <c r="B159" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C159" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D159" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E159" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F159" s="149" t="s">
+        <v>189</v>
+      </c>
+      <c r="G159" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H159" s="68"/>
-      <c r="I159" s="83"/>
-      <c r="J159" s="70"/>
+      <c r="I159" s="152">
+        <v>1173</v>
+      </c>
+      <c r="J159" s="70">
+        <v>218000000</v>
+      </c>
       <c r="K159" s="70"/>
-      <c r="L159" s="68"/>
-      <c r="M159" s="68"/>
-      <c r="N159" s="68"/>
+      <c r="L159" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M159" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N159" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O159" s="9"/>
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
@@ -9385,19 +9815,41 @@
     </row>
     <row r="160" spans="1:20" ht="18" customHeight="1">
       <c r="A160" s="64"/>
-      <c r="B160" s="73"/>
-      <c r="C160" s="68"/>
-      <c r="D160" s="68"/>
-      <c r="E160" s="73"/>
-      <c r="F160" s="68"/>
-      <c r="G160" s="68"/>
+      <c r="B160" s="148" t="s">
+        <v>241</v>
+      </c>
+      <c r="C160" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D160" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E160" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F160" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G160" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H160" s="68"/>
-      <c r="I160" s="83"/>
-      <c r="J160" s="70"/>
+      <c r="I160" s="152">
+        <v>1173</v>
+      </c>
+      <c r="J160" s="70">
+        <v>45</v>
+      </c>
       <c r="K160" s="70"/>
-      <c r="L160" s="68"/>
-      <c r="M160" s="68"/>
-      <c r="N160" s="68"/>
+      <c r="L160" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M160" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N160" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O160" s="9"/>
       <c r="P160" s="4"/>
       <c r="Q160" s="4"/>
@@ -9407,19 +9859,41 @@
     </row>
     <row r="161" spans="1:20" ht="18" customHeight="1">
       <c r="A161" s="64"/>
-      <c r="B161" s="73"/>
-      <c r="C161" s="68"/>
-      <c r="D161" s="68"/>
-      <c r="E161" s="73"/>
-      <c r="F161" s="68"/>
-      <c r="G161" s="68"/>
+      <c r="B161" s="148" t="s">
+        <v>243</v>
+      </c>
+      <c r="C161" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D161" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E161" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F161" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G161" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H161" s="68"/>
-      <c r="I161" s="83"/>
-      <c r="J161" s="70"/>
+      <c r="I161" s="152">
+        <v>1173</v>
+      </c>
+      <c r="J161" s="70">
+        <v>45</v>
+      </c>
       <c r="K161" s="70"/>
-      <c r="L161" s="68"/>
-      <c r="M161" s="68"/>
-      <c r="N161" s="68"/>
+      <c r="L161" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M161" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N161" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O161" s="9"/>
       <c r="P161" s="4"/>
       <c r="Q161" s="4"/>
@@ -9429,19 +9903,41 @@
     </row>
     <row r="162" spans="1:20" ht="18" customHeight="1">
       <c r="A162" s="64"/>
-      <c r="B162" s="73"/>
-      <c r="C162" s="68"/>
-      <c r="D162" s="68"/>
-      <c r="E162" s="73"/>
-      <c r="F162" s="68"/>
-      <c r="G162" s="68"/>
+      <c r="B162" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C162" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D162" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E162" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F162" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G162" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H162" s="68"/>
-      <c r="I162" s="83"/>
-      <c r="J162" s="70"/>
+      <c r="I162" s="152">
+        <v>1173</v>
+      </c>
+      <c r="J162" s="70">
+        <v>45</v>
+      </c>
       <c r="K162" s="70"/>
-      <c r="L162" s="68"/>
-      <c r="M162" s="68"/>
-      <c r="N162" s="68"/>
+      <c r="L162" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M162" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N162" s="149" t="s">
+        <v>242</v>
+      </c>
       <c r="O162" s="9"/>
       <c r="P162" s="4"/>
       <c r="Q162" s="4"/>
@@ -9451,10 +9947,10 @@
     </row>
     <row r="163" spans="1:20" ht="18" customHeight="1">
       <c r="A163" s="64"/>
-      <c r="B163" s="73"/>
-      <c r="C163" s="68"/>
-      <c r="D163" s="68"/>
-      <c r="E163" s="73"/>
+      <c r="B163" s="148"/>
+      <c r="C163" s="149"/>
+      <c r="D163" s="149"/>
+      <c r="E163" s="148"/>
       <c r="F163" s="68"/>
       <c r="G163" s="68"/>
       <c r="H163" s="68"/>
@@ -9473,10 +9969,10 @@
     </row>
     <row r="164" spans="1:20" ht="18" customHeight="1">
       <c r="A164" s="64"/>
-      <c r="B164" s="73"/>
-      <c r="C164" s="68"/>
-      <c r="D164" s="68"/>
-      <c r="E164" s="73"/>
+      <c r="B164" s="148"/>
+      <c r="C164" s="149"/>
+      <c r="D164" s="149"/>
+      <c r="E164" s="148"/>
       <c r="F164" s="68"/>
       <c r="G164" s="68"/>
       <c r="H164" s="68"/>
@@ -9495,10 +9991,10 @@
     </row>
     <row r="165" spans="1:20" ht="18" customHeight="1">
       <c r="A165" s="64"/>
-      <c r="B165" s="73"/>
-      <c r="C165" s="68"/>
-      <c r="D165" s="68"/>
-      <c r="E165" s="73"/>
+      <c r="B165" s="148"/>
+      <c r="C165" s="149"/>
+      <c r="D165" s="149"/>
+      <c r="E165" s="148"/>
       <c r="F165" s="68"/>
       <c r="G165" s="68"/>
       <c r="H165" s="68"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2024.178025`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705BD1A4-B83F-2F4C-9066-83DE12716536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4333FD0D-0E52-7647-834F-188146040A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9280" yWindow="800" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="259">
   <si>
     <r>
       <rPr>
@@ -864,6 +864,39 @@
   </si>
   <si>
     <t>F7</t>
+  </si>
+  <si>
+    <t>solidus temperature</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>liquidus temperature</t>
+  </si>
+  <si>
+    <t>electrical resistivity</t>
+  </si>
+  <si>
+    <t>Ohm m</t>
+  </si>
+  <si>
+    <t>W/(m K)</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>thermal conductivity</t>
+  </si>
+  <si>
+    <t>CTE</t>
+  </si>
+  <si>
+    <t>K^-1</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2024.178025</t>
   </si>
 </sst>
 </file>
@@ -3188,8 +3221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A129" zoomScale="86" workbookViewId="0">
-      <selection activeCell="G168" sqref="G168"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B139" zoomScale="86" workbookViewId="0">
+      <selection activeCell="G182" sqref="G182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -9947,19 +9980,37 @@
     </row>
     <row r="163" spans="1:20" ht="18" customHeight="1">
       <c r="A163" s="64"/>
-      <c r="B163" s="148"/>
-      <c r="C163" s="149"/>
-      <c r="D163" s="149"/>
-      <c r="E163" s="148"/>
-      <c r="F163" s="68"/>
-      <c r="G163" s="68"/>
+      <c r="B163" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C163" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D163" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E163" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F163" s="149" t="s">
+        <v>248</v>
+      </c>
+      <c r="G163" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H163" s="68"/>
-      <c r="I163" s="83"/>
-      <c r="J163" s="70"/>
+      <c r="J163" s="83">
+        <f>1348+273</f>
+        <v>1621</v>
+      </c>
       <c r="K163" s="70"/>
-      <c r="L163" s="68"/>
+      <c r="L163" s="149" t="s">
+        <v>249</v>
+      </c>
       <c r="M163" s="68"/>
-      <c r="N163" s="68"/>
+      <c r="N163" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O163" s="9"/>
       <c r="P163" s="4"/>
       <c r="Q163" s="4"/>
@@ -9969,19 +10020,38 @@
     </row>
     <row r="164" spans="1:20" ht="18" customHeight="1">
       <c r="A164" s="64"/>
-      <c r="B164" s="148"/>
-      <c r="C164" s="149"/>
-      <c r="D164" s="149"/>
-      <c r="E164" s="148"/>
-      <c r="F164" s="68"/>
-      <c r="G164" s="68"/>
+      <c r="B164" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C164" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D164" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E164" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F164" s="149" t="s">
+        <v>250</v>
+      </c>
+      <c r="G164" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H164" s="68"/>
       <c r="I164" s="83"/>
-      <c r="J164" s="70"/>
+      <c r="J164" s="70">
+        <f>273+1382</f>
+        <v>1655</v>
+      </c>
       <c r="K164" s="70"/>
-      <c r="L164" s="68"/>
+      <c r="L164" s="149" t="s">
+        <v>249</v>
+      </c>
       <c r="M164" s="68"/>
-      <c r="N164" s="68"/>
+      <c r="N164" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O164" s="9"/>
       <c r="P164" s="4"/>
       <c r="Q164" s="4"/>
@@ -9991,19 +10061,39 @@
     </row>
     <row r="165" spans="1:20" ht="18" customHeight="1">
       <c r="A165" s="64"/>
-      <c r="B165" s="148"/>
-      <c r="C165" s="149"/>
-      <c r="D165" s="149"/>
-      <c r="E165" s="148"/>
-      <c r="F165" s="68"/>
-      <c r="G165" s="68"/>
+      <c r="B165" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C165" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D165" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E165" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F165" s="149" t="s">
+        <v>251</v>
+      </c>
+      <c r="G165" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H165" s="68"/>
-      <c r="I165" s="83"/>
-      <c r="J165" s="70"/>
+      <c r="I165" s="83">
+        <v>298</v>
+      </c>
+      <c r="J165" s="70">
+        <v>5.4000000000000002E-7</v>
+      </c>
       <c r="K165" s="70"/>
-      <c r="L165" s="68"/>
+      <c r="L165" s="149" t="s">
+        <v>252</v>
+      </c>
       <c r="M165" s="68"/>
-      <c r="N165" s="68"/>
+      <c r="N165" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O165" s="9"/>
       <c r="P165" s="4"/>
       <c r="Q165" s="4"/>
@@ -10013,19 +10103,41 @@
     </row>
     <row r="166" spans="1:20" ht="18" customHeight="1">
       <c r="A166" s="64"/>
-      <c r="B166" s="73"/>
-      <c r="C166" s="68"/>
-      <c r="D166" s="68"/>
-      <c r="E166" s="73"/>
-      <c r="F166" s="68"/>
-      <c r="G166" s="68"/>
+      <c r="B166" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C166" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D166" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E166" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F166" s="149" t="s">
+        <v>255</v>
+      </c>
+      <c r="G166" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H166" s="68"/>
-      <c r="I166" s="83"/>
-      <c r="J166" s="70"/>
+      <c r="I166" s="83">
+        <v>298</v>
+      </c>
+      <c r="J166" s="70">
+        <v>13.14</v>
+      </c>
       <c r="K166" s="70"/>
-      <c r="L166" s="68"/>
-      <c r="M166" s="68"/>
-      <c r="N166" s="68"/>
+      <c r="L166" s="149" t="s">
+        <v>253</v>
+      </c>
+      <c r="M166" s="149" t="s">
+        <v>254</v>
+      </c>
+      <c r="N166" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O166" s="9"/>
       <c r="P166" s="4"/>
       <c r="Q166" s="4"/>
@@ -10035,19 +10147,41 @@
     </row>
     <row r="167" spans="1:20" ht="18" customHeight="1">
       <c r="A167" s="64"/>
-      <c r="B167" s="73"/>
-      <c r="C167" s="68"/>
-      <c r="D167" s="68"/>
-      <c r="E167" s="73"/>
-      <c r="F167" s="68"/>
-      <c r="G167" s="68"/>
+      <c r="B167" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C167" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D167" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E167" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F167" s="149" t="s">
+        <v>255</v>
+      </c>
+      <c r="G167" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H167" s="68"/>
-      <c r="I167" s="83"/>
-      <c r="J167" s="70"/>
+      <c r="I167" s="83">
+        <v>500</v>
+      </c>
+      <c r="J167" s="70">
+        <v>16.89</v>
+      </c>
       <c r="K167" s="70"/>
-      <c r="L167" s="68"/>
-      <c r="M167" s="68"/>
-      <c r="N167" s="68"/>
+      <c r="L167" s="149" t="s">
+        <v>253</v>
+      </c>
+      <c r="M167" s="149" t="s">
+        <v>254</v>
+      </c>
+      <c r="N167" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O167" s="9"/>
       <c r="P167" s="4"/>
       <c r="Q167" s="4"/>
@@ -10057,19 +10191,41 @@
     </row>
     <row r="168" spans="1:20" ht="18" customHeight="1">
       <c r="A168" s="64"/>
-      <c r="B168" s="73"/>
-      <c r="C168" s="68"/>
-      <c r="D168" s="68"/>
-      <c r="E168" s="73"/>
-      <c r="F168" s="68"/>
-      <c r="G168" s="68"/>
+      <c r="B168" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C168" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D168" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E168" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F168" s="149" t="s">
+        <v>255</v>
+      </c>
+      <c r="G168" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H168" s="68"/>
-      <c r="I168" s="83"/>
-      <c r="J168" s="70"/>
+      <c r="I168" s="83">
+        <v>700</v>
+      </c>
+      <c r="J168" s="70">
+        <v>21.67</v>
+      </c>
       <c r="K168" s="70"/>
-      <c r="L168" s="68"/>
-      <c r="M168" s="68"/>
-      <c r="N168" s="68"/>
+      <c r="L168" s="149" t="s">
+        <v>253</v>
+      </c>
+      <c r="M168" s="149" t="s">
+        <v>254</v>
+      </c>
+      <c r="N168" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O168" s="9"/>
       <c r="P168" s="4"/>
       <c r="Q168" s="4"/>
@@ -10079,19 +10235,41 @@
     </row>
     <row r="169" spans="1:20" ht="18" customHeight="1">
       <c r="A169" s="64"/>
-      <c r="B169" s="73"/>
-      <c r="C169" s="68"/>
-      <c r="D169" s="68"/>
-      <c r="E169" s="73"/>
-      <c r="F169" s="68"/>
-      <c r="G169" s="68"/>
+      <c r="B169" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C169" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D169" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E169" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F169" s="149" t="s">
+        <v>255</v>
+      </c>
+      <c r="G169" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H169" s="68"/>
-      <c r="I169" s="83"/>
-      <c r="J169" s="70"/>
+      <c r="I169" s="83">
+        <v>900</v>
+      </c>
+      <c r="J169" s="70">
+        <v>26.13</v>
+      </c>
       <c r="K169" s="70"/>
-      <c r="L169" s="68"/>
-      <c r="M169" s="68"/>
-      <c r="N169" s="68"/>
+      <c r="L169" s="149" t="s">
+        <v>253</v>
+      </c>
+      <c r="M169" s="149" t="s">
+        <v>254</v>
+      </c>
+      <c r="N169" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O169" s="9"/>
       <c r="P169" s="4"/>
       <c r="Q169" s="4"/>
@@ -10101,19 +10279,41 @@
     </row>
     <row r="170" spans="1:20" ht="18" customHeight="1">
       <c r="A170" s="64"/>
-      <c r="B170" s="73"/>
-      <c r="C170" s="68"/>
-      <c r="D170" s="68"/>
-      <c r="E170" s="73"/>
-      <c r="F170" s="68"/>
-      <c r="G170" s="68"/>
+      <c r="B170" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C170" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D170" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E170" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F170" s="149" t="s">
+        <v>255</v>
+      </c>
+      <c r="G170" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H170" s="68"/>
-      <c r="I170" s="83"/>
-      <c r="J170" s="70"/>
+      <c r="I170" s="83">
+        <v>1173</v>
+      </c>
+      <c r="J170" s="70">
+        <v>29.37</v>
+      </c>
       <c r="K170" s="70"/>
-      <c r="L170" s="68"/>
-      <c r="M170" s="68"/>
-      <c r="N170" s="68"/>
+      <c r="L170" s="149" t="s">
+        <v>253</v>
+      </c>
+      <c r="M170" s="149" t="s">
+        <v>254</v>
+      </c>
+      <c r="N170" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O170" s="9"/>
       <c r="P170" s="4"/>
       <c r="Q170" s="4"/>
@@ -10123,19 +10323,41 @@
     </row>
     <row r="171" spans="1:20" ht="18" customHeight="1">
       <c r="A171" s="64"/>
-      <c r="B171" s="73"/>
-      <c r="C171" s="68"/>
-      <c r="D171" s="68"/>
-      <c r="E171" s="73"/>
-      <c r="F171" s="68"/>
-      <c r="G171" s="68"/>
+      <c r="B171" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C171" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D171" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E171" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F171" s="149" t="s">
+        <v>256</v>
+      </c>
+      <c r="G171" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H171" s="68"/>
-      <c r="I171" s="83"/>
-      <c r="J171" s="70"/>
+      <c r="I171" s="83">
+        <v>300</v>
+      </c>
+      <c r="J171" s="70">
+        <v>1.04E-5</v>
+      </c>
       <c r="K171" s="70"/>
-      <c r="L171" s="68"/>
-      <c r="M171" s="68"/>
-      <c r="N171" s="68"/>
+      <c r="L171" s="149" t="s">
+        <v>257</v>
+      </c>
+      <c r="M171" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="N171" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O171" s="9"/>
       <c r="P171" s="4"/>
       <c r="Q171" s="4"/>
@@ -10145,19 +10367,41 @@
     </row>
     <row r="172" spans="1:20" ht="18" customHeight="1">
       <c r="A172" s="64"/>
-      <c r="B172" s="73"/>
-      <c r="C172" s="68"/>
-      <c r="D172" s="68"/>
-      <c r="E172" s="73"/>
-      <c r="F172" s="68"/>
-      <c r="G172" s="68"/>
+      <c r="B172" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C172" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D172" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E172" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F172" s="149" t="s">
+        <v>256</v>
+      </c>
+      <c r="G172" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H172" s="68"/>
-      <c r="I172" s="83"/>
-      <c r="J172" s="70"/>
+      <c r="I172" s="83">
+        <v>400</v>
+      </c>
+      <c r="J172" s="70">
+        <v>1.119E-5</v>
+      </c>
       <c r="K172" s="70"/>
-      <c r="L172" s="68"/>
-      <c r="M172" s="68"/>
-      <c r="N172" s="68"/>
+      <c r="L172" s="149" t="s">
+        <v>257</v>
+      </c>
+      <c r="M172" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="N172" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O172" s="9"/>
       <c r="P172" s="4"/>
       <c r="Q172" s="4"/>
@@ -10167,19 +10411,41 @@
     </row>
     <row r="173" spans="1:20" ht="18" customHeight="1">
       <c r="A173" s="64"/>
-      <c r="B173" s="73"/>
-      <c r="C173" s="68"/>
-      <c r="D173" s="68"/>
-      <c r="E173" s="73"/>
-      <c r="F173" s="68"/>
-      <c r="G173" s="68"/>
+      <c r="B173" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C173" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D173" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E173" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F173" s="149" t="s">
+        <v>256</v>
+      </c>
+      <c r="G173" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H173" s="68"/>
-      <c r="I173" s="83"/>
-      <c r="J173" s="70"/>
+      <c r="I173" s="83">
+        <v>600</v>
+      </c>
+      <c r="J173" s="70">
+        <v>1.224E-5</v>
+      </c>
       <c r="K173" s="70"/>
-      <c r="L173" s="68"/>
-      <c r="M173" s="68"/>
-      <c r="N173" s="68"/>
+      <c r="L173" s="149" t="s">
+        <v>257</v>
+      </c>
+      <c r="M173" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="N173" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O173" s="9"/>
       <c r="P173" s="4"/>
       <c r="Q173" s="4"/>
@@ -10189,19 +10455,41 @@
     </row>
     <row r="174" spans="1:20" ht="18" customHeight="1">
       <c r="A174" s="64"/>
-      <c r="B174" s="73"/>
-      <c r="C174" s="68"/>
-      <c r="D174" s="68"/>
-      <c r="E174" s="73"/>
-      <c r="F174" s="68"/>
-      <c r="G174" s="68"/>
+      <c r="B174" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C174" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D174" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E174" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F174" s="149" t="s">
+        <v>256</v>
+      </c>
+      <c r="G174" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H174" s="68"/>
-      <c r="I174" s="83"/>
-      <c r="J174" s="70"/>
+      <c r="I174" s="83">
+        <v>800</v>
+      </c>
+      <c r="J174" s="70">
+        <v>1.2619999999999999E-5</v>
+      </c>
       <c r="K174" s="70"/>
-      <c r="L174" s="68"/>
-      <c r="M174" s="68"/>
-      <c r="N174" s="68"/>
+      <c r="L174" s="149" t="s">
+        <v>257</v>
+      </c>
+      <c r="M174" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="N174" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O174" s="9"/>
       <c r="P174" s="4"/>
       <c r="Q174" s="4"/>
@@ -10211,19 +10499,41 @@
     </row>
     <row r="175" spans="1:20" ht="18" customHeight="1">
       <c r="A175" s="64"/>
-      <c r="B175" s="73"/>
-      <c r="C175" s="68"/>
-      <c r="D175" s="68"/>
-      <c r="E175" s="73"/>
-      <c r="F175" s="68"/>
-      <c r="G175" s="68"/>
+      <c r="B175" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C175" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D175" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E175" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F175" s="149" t="s">
+        <v>256</v>
+      </c>
+      <c r="G175" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H175" s="68"/>
-      <c r="I175" s="83"/>
-      <c r="J175" s="70"/>
+      <c r="I175" s="83">
+        <v>1000</v>
+      </c>
+      <c r="J175" s="70">
+        <v>1.2989999999999999E-5</v>
+      </c>
       <c r="K175" s="70"/>
-      <c r="L175" s="68"/>
-      <c r="M175" s="68"/>
-      <c r="N175" s="68"/>
+      <c r="L175" s="149" t="s">
+        <v>257</v>
+      </c>
+      <c r="M175" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="N175" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O175" s="9"/>
       <c r="P175" s="4"/>
       <c r="Q175" s="4"/>
@@ -10233,19 +10543,41 @@
     </row>
     <row r="176" spans="1:20" ht="18" customHeight="1">
       <c r="A176" s="64"/>
-      <c r="B176" s="73"/>
-      <c r="C176" s="68"/>
-      <c r="D176" s="68"/>
-      <c r="E176" s="73"/>
-      <c r="F176" s="68"/>
-      <c r="G176" s="68"/>
+      <c r="B176" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="C176" s="149" t="s">
+        <v>210</v>
+      </c>
+      <c r="D176" s="149" t="s">
+        <v>113</v>
+      </c>
+      <c r="E176" s="148" t="s">
+        <v>244</v>
+      </c>
+      <c r="F176" s="149" t="s">
+        <v>256</v>
+      </c>
+      <c r="G176" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H176" s="68"/>
-      <c r="I176" s="83"/>
-      <c r="J176" s="70"/>
+      <c r="I176" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J176" s="70">
+        <v>1.508E-5</v>
+      </c>
       <c r="K176" s="70"/>
-      <c r="L176" s="68"/>
-      <c r="M176" s="68"/>
-      <c r="N176" s="68"/>
+      <c r="L176" s="149" t="s">
+        <v>257</v>
+      </c>
+      <c r="M176" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="N176" s="149" t="s">
+        <v>258</v>
+      </c>
       <c r="O176" s="9"/>
       <c r="P176" s="4"/>
       <c r="Q176" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2023.144870`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4333FD0D-0E52-7647-834F-188146040A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F7A8FB-9945-EF4A-A216-709FF567F5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9280" yWindow="800" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="4080" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="269">
   <si>
     <r>
       <rPr>
@@ -897,6 +897,36 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2024.178025</t>
+  </si>
+  <si>
+    <t>Nb70 Ti18 W12</t>
+  </si>
+  <si>
+    <t>NTW</t>
+  </si>
+  <si>
+    <t>NTW-R</t>
+  </si>
+  <si>
+    <t>NTW-RA</t>
+  </si>
+  <si>
+    <t>Nb65 Ti18 W12 Re5</t>
+  </si>
+  <si>
+    <t>Nb64 Ti18 W12 Re5 Al1</t>
+  </si>
+  <si>
+    <t>helium pycnometry</t>
+  </si>
+  <si>
+    <t>VAM+HIP</t>
+  </si>
+  <si>
+    <t>HIPed at 1673K under 207MPa for 3h</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2023.144870</t>
   </si>
 </sst>
 </file>
@@ -1697,7 +1727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2059,6 +2089,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3221,8 +3254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B139" zoomScale="86" workbookViewId="0">
-      <selection activeCell="G182" sqref="G182"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D169" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N214" sqref="N214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -10586,20 +10619,46 @@
       <c r="T176" s="9"/>
     </row>
     <row r="177" spans="1:20" ht="18" customHeight="1">
-      <c r="A177" s="64"/>
-      <c r="B177" s="73"/>
-      <c r="C177" s="68"/>
-      <c r="D177" s="68"/>
-      <c r="E177" s="73"/>
-      <c r="F177" s="68"/>
-      <c r="G177" s="68"/>
-      <c r="H177" s="68"/>
-      <c r="I177" s="83"/>
-      <c r="J177" s="70"/>
+      <c r="A177" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B177" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C177" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D177" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E177" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F177" s="149" t="s">
+        <v>67</v>
+      </c>
+      <c r="G177" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="H177" s="149" t="s">
+        <v>265</v>
+      </c>
+      <c r="I177" s="83">
+        <v>298</v>
+      </c>
+      <c r="J177" s="70">
+        <v>8900</v>
+      </c>
       <c r="K177" s="70"/>
-      <c r="L177" s="68"/>
-      <c r="M177" s="68"/>
-      <c r="N177" s="68"/>
+      <c r="L177" s="149" t="s">
+        <v>68</v>
+      </c>
+      <c r="M177" s="149" t="s">
+        <v>69</v>
+      </c>
+      <c r="N177" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O177" s="9"/>
       <c r="P177" s="4"/>
       <c r="Q177" s="4"/>
@@ -10608,20 +10667,46 @@
       <c r="T177" s="9"/>
     </row>
     <row r="178" spans="1:20" ht="18" customHeight="1">
-      <c r="A178" s="64"/>
-      <c r="B178" s="73"/>
-      <c r="C178" s="68"/>
-      <c r="D178" s="68"/>
-      <c r="E178" s="73"/>
-      <c r="F178" s="68"/>
-      <c r="G178" s="68"/>
-      <c r="H178" s="68"/>
-      <c r="I178" s="83"/>
-      <c r="J178" s="70"/>
+      <c r="A178" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B178" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C178" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D178" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E178" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F178" s="149" t="s">
+        <v>67</v>
+      </c>
+      <c r="G178" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="H178" s="149" t="s">
+        <v>265</v>
+      </c>
+      <c r="I178" s="83">
+        <v>298</v>
+      </c>
+      <c r="J178" s="70">
+        <v>9460</v>
+      </c>
       <c r="K178" s="70"/>
-      <c r="L178" s="68"/>
-      <c r="M178" s="68"/>
-      <c r="N178" s="68"/>
+      <c r="L178" s="149" t="s">
+        <v>68</v>
+      </c>
+      <c r="M178" s="149" t="s">
+        <v>69</v>
+      </c>
+      <c r="N178" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O178" s="9"/>
       <c r="P178" s="4"/>
       <c r="Q178" s="4"/>
@@ -10630,20 +10715,46 @@
       <c r="T178" s="9"/>
     </row>
     <row r="179" spans="1:20" ht="18" customHeight="1">
-      <c r="A179" s="64"/>
-      <c r="B179" s="73"/>
-      <c r="C179" s="68"/>
-      <c r="D179" s="68"/>
-      <c r="E179" s="73"/>
-      <c r="F179" s="68"/>
-      <c r="G179" s="68"/>
-      <c r="H179" s="68"/>
-      <c r="I179" s="83"/>
-      <c r="J179" s="70"/>
+      <c r="A179" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B179" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C179" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D179" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E179" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F179" s="149" t="s">
+        <v>67</v>
+      </c>
+      <c r="G179" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="H179" s="149" t="s">
+        <v>265</v>
+      </c>
+      <c r="I179" s="83">
+        <v>298</v>
+      </c>
+      <c r="J179" s="70">
+        <v>9460</v>
+      </c>
       <c r="K179" s="70"/>
-      <c r="L179" s="68"/>
-      <c r="M179" s="68"/>
-      <c r="N179" s="68"/>
+      <c r="L179" s="149" t="s">
+        <v>68</v>
+      </c>
+      <c r="M179" s="149" t="s">
+        <v>69</v>
+      </c>
+      <c r="N179" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O179" s="9"/>
       <c r="P179" s="4"/>
       <c r="Q179" s="4"/>
@@ -10652,20 +10763,44 @@
       <c r="T179" s="9"/>
     </row>
     <row r="180" spans="1:20" ht="18" customHeight="1">
-      <c r="A180" s="64"/>
-      <c r="B180" s="73"/>
-      <c r="C180" s="68"/>
-      <c r="D180" s="68"/>
-      <c r="E180" s="73"/>
-      <c r="F180" s="68"/>
-      <c r="G180" s="68"/>
+      <c r="A180" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B180" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C180" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D180" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E180" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F180" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G180" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H180" s="68"/>
-      <c r="I180" s="83"/>
-      <c r="J180" s="70"/>
+      <c r="I180" s="83">
+        <v>298</v>
+      </c>
+      <c r="J180" s="70">
+        <v>874000000</v>
+      </c>
       <c r="K180" s="70"/>
-      <c r="L180" s="68"/>
-      <c r="M180" s="68"/>
-      <c r="N180" s="68"/>
+      <c r="L180" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M180" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N180" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O180" s="9"/>
       <c r="P180" s="4"/>
       <c r="Q180" s="4"/>
@@ -10674,20 +10809,44 @@
       <c r="T180" s="9"/>
     </row>
     <row r="181" spans="1:20" ht="18" customHeight="1">
-      <c r="A181" s="64"/>
-      <c r="B181" s="73"/>
-      <c r="C181" s="68"/>
-      <c r="D181" s="68"/>
-      <c r="E181" s="73"/>
-      <c r="F181" s="68"/>
-      <c r="G181" s="68"/>
+      <c r="A181" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B181" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C181" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D181" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E181" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F181" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G181" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H181" s="68"/>
-      <c r="I181" s="83"/>
-      <c r="J181" s="70"/>
+      <c r="I181" s="83">
+        <v>298</v>
+      </c>
+      <c r="J181" s="70">
+        <v>1000000000</v>
+      </c>
       <c r="K181" s="70"/>
-      <c r="L181" s="68"/>
-      <c r="M181" s="68"/>
-      <c r="N181" s="68"/>
+      <c r="L181" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M181" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N181" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O181" s="9"/>
       <c r="P181" s="4"/>
       <c r="Q181" s="4"/>
@@ -10696,20 +10855,44 @@
       <c r="T181" s="9"/>
     </row>
     <row r="182" spans="1:20" ht="18" customHeight="1">
-      <c r="A182" s="64"/>
-      <c r="B182" s="73"/>
-      <c r="C182" s="68"/>
-      <c r="D182" s="68"/>
-      <c r="E182" s="73"/>
-      <c r="F182" s="68"/>
-      <c r="G182" s="68"/>
+      <c r="A182" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B182" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C182" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D182" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E182" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F182" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G182" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H182" s="68"/>
-      <c r="I182" s="83"/>
-      <c r="J182" s="70"/>
+      <c r="I182" s="83">
+        <v>298</v>
+      </c>
+      <c r="J182" s="70">
+        <v>924000000</v>
+      </c>
       <c r="K182" s="70"/>
-      <c r="L182" s="68"/>
-      <c r="M182" s="68"/>
-      <c r="N182" s="68"/>
+      <c r="L182" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M182" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N182" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O182" s="9"/>
       <c r="P182" s="4"/>
       <c r="Q182" s="4"/>
@@ -10718,20 +10901,44 @@
       <c r="T182" s="9"/>
     </row>
     <row r="183" spans="1:20" ht="18" customHeight="1">
-      <c r="A183" s="64"/>
-      <c r="B183" s="73"/>
-      <c r="C183" s="68"/>
-      <c r="D183" s="68"/>
-      <c r="E183" s="73"/>
-      <c r="F183" s="68"/>
-      <c r="G183" s="68"/>
+      <c r="A183" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B183" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C183" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D183" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E183" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F183" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G183" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H183" s="68"/>
-      <c r="I183" s="83"/>
-      <c r="J183" s="70"/>
+      <c r="I183" s="83">
+        <v>873</v>
+      </c>
+      <c r="J183" s="70">
+        <v>430000000</v>
+      </c>
       <c r="K183" s="70"/>
-      <c r="L183" s="68"/>
-      <c r="M183" s="68"/>
-      <c r="N183" s="68"/>
+      <c r="L183" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M183" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N183" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O183" s="9"/>
       <c r="P183" s="4"/>
       <c r="Q183" s="4"/>
@@ -10740,20 +10947,44 @@
       <c r="T183" s="9"/>
     </row>
     <row r="184" spans="1:20" ht="18" customHeight="1">
-      <c r="A184" s="64"/>
-      <c r="B184" s="73"/>
-      <c r="C184" s="68"/>
-      <c r="D184" s="68"/>
-      <c r="E184" s="73"/>
-      <c r="F184" s="68"/>
-      <c r="G184" s="68"/>
+      <c r="A184" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B184" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C184" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D184" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E184" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F184" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G184" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H184" s="68"/>
-      <c r="I184" s="83"/>
-      <c r="J184" s="70"/>
+      <c r="I184" s="83">
+        <v>873</v>
+      </c>
+      <c r="J184" s="70">
+        <v>520000000</v>
+      </c>
       <c r="K184" s="70"/>
-      <c r="L184" s="68"/>
-      <c r="M184" s="68"/>
-      <c r="N184" s="68"/>
+      <c r="L184" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M184" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N184" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O184" s="9"/>
       <c r="P184" s="4"/>
       <c r="Q184" s="4"/>
@@ -10762,20 +10993,44 @@
       <c r="T184" s="9"/>
     </row>
     <row r="185" spans="1:20" ht="18" customHeight="1">
-      <c r="A185" s="64"/>
-      <c r="B185" s="73"/>
-      <c r="C185" s="68"/>
-      <c r="D185" s="68"/>
-      <c r="E185" s="73"/>
-      <c r="F185" s="68"/>
-      <c r="G185" s="68"/>
+      <c r="A185" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B185" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C185" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D185" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E185" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F185" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G185" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H185" s="68"/>
-      <c r="I185" s="83"/>
-      <c r="J185" s="70"/>
+      <c r="I185" s="83">
+        <v>873</v>
+      </c>
+      <c r="J185" s="70">
+        <v>604000000</v>
+      </c>
       <c r="K185" s="70"/>
-      <c r="L185" s="68"/>
-      <c r="M185" s="68"/>
-      <c r="N185" s="68"/>
+      <c r="L185" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M185" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N185" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O185" s="9"/>
       <c r="P185" s="4"/>
       <c r="Q185" s="4"/>
@@ -10784,20 +11039,44 @@
       <c r="T185" s="9"/>
     </row>
     <row r="186" spans="1:20" ht="18" customHeight="1">
-      <c r="A186" s="64"/>
-      <c r="B186" s="73"/>
-      <c r="C186" s="68"/>
-      <c r="D186" s="68"/>
-      <c r="E186" s="73"/>
-      <c r="F186" s="68"/>
-      <c r="G186" s="68"/>
+      <c r="A186" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B186" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C186" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D186" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E186" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F186" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G186" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H186" s="68"/>
-      <c r="I186" s="83"/>
-      <c r="J186" s="70"/>
+      <c r="I186" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J186" s="70">
+        <v>404000000</v>
+      </c>
       <c r="K186" s="70"/>
-      <c r="L186" s="68"/>
-      <c r="M186" s="68"/>
-      <c r="N186" s="68"/>
+      <c r="L186" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M186" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N186" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O186" s="9"/>
       <c r="P186" s="4"/>
       <c r="Q186" s="4"/>
@@ -10806,20 +11085,44 @@
       <c r="T186" s="9"/>
     </row>
     <row r="187" spans="1:20" ht="18" customHeight="1">
-      <c r="A187" s="64"/>
-      <c r="B187" s="73"/>
-      <c r="C187" s="68"/>
-      <c r="D187" s="68"/>
-      <c r="E187" s="73"/>
-      <c r="F187" s="68"/>
-      <c r="G187" s="68"/>
+      <c r="A187" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B187" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C187" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D187" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E187" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F187" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G187" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H187" s="68"/>
-      <c r="I187" s="83"/>
-      <c r="J187" s="70"/>
+      <c r="I187" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J187" s="70">
+        <v>455000000</v>
+      </c>
       <c r="K187" s="70"/>
-      <c r="L187" s="68"/>
-      <c r="M187" s="68"/>
-      <c r="N187" s="68"/>
+      <c r="L187" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M187" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N187" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O187" s="9"/>
       <c r="P187" s="4"/>
       <c r="Q187" s="4"/>
@@ -10828,20 +11131,44 @@
       <c r="T187" s="9"/>
     </row>
     <row r="188" spans="1:20" ht="18" customHeight="1">
-      <c r="A188" s="64"/>
-      <c r="B188" s="73"/>
-      <c r="C188" s="68"/>
-      <c r="D188" s="68"/>
-      <c r="E188" s="73"/>
-      <c r="F188" s="68"/>
-      <c r="G188" s="68"/>
+      <c r="A188" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B188" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C188" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D188" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E188" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F188" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G188" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H188" s="68"/>
-      <c r="I188" s="83"/>
-      <c r="J188" s="70"/>
+      <c r="I188" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J188" s="70">
+        <v>513000000</v>
+      </c>
       <c r="K188" s="70"/>
-      <c r="L188" s="68"/>
-      <c r="M188" s="68"/>
-      <c r="N188" s="68"/>
+      <c r="L188" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M188" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N188" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O188" s="9"/>
       <c r="P188" s="4"/>
       <c r="Q188" s="4"/>
@@ -10850,20 +11177,44 @@
       <c r="T188" s="9"/>
     </row>
     <row r="189" spans="1:20" ht="18" customHeight="1">
-      <c r="A189" s="64"/>
-      <c r="B189" s="73"/>
-      <c r="C189" s="68"/>
-      <c r="D189" s="68"/>
-      <c r="E189" s="73"/>
-      <c r="F189" s="68"/>
-      <c r="G189" s="68"/>
+      <c r="A189" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B189" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C189" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D189" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E189" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F189" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G189" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H189" s="68"/>
-      <c r="I189" s="83"/>
-      <c r="J189" s="70"/>
+      <c r="I189" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J189" s="70">
+        <v>353000000</v>
+      </c>
       <c r="K189" s="70"/>
-      <c r="L189" s="68"/>
-      <c r="M189" s="68"/>
-      <c r="N189" s="68"/>
+      <c r="L189" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M189" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N189" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O189" s="9"/>
       <c r="P189" s="4"/>
       <c r="Q189" s="4"/>
@@ -10872,20 +11223,44 @@
       <c r="T189" s="9"/>
     </row>
     <row r="190" spans="1:20" ht="18" customHeight="1">
-      <c r="A190" s="64"/>
-      <c r="B190" s="73"/>
-      <c r="C190" s="68"/>
-      <c r="D190" s="68"/>
-      <c r="E190" s="73"/>
-      <c r="F190" s="68"/>
-      <c r="G190" s="68"/>
+      <c r="A190" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B190" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C190" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D190" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E190" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F190" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G190" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H190" s="68"/>
-      <c r="I190" s="83"/>
-      <c r="J190" s="70"/>
+      <c r="I190" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J190" s="70">
+        <v>412000000</v>
+      </c>
       <c r="K190" s="70"/>
-      <c r="L190" s="68"/>
-      <c r="M190" s="68"/>
-      <c r="N190" s="68"/>
+      <c r="L190" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M190" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N190" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O190" s="9"/>
       <c r="P190" s="4"/>
       <c r="Q190" s="4"/>
@@ -10894,20 +11269,44 @@
       <c r="T190" s="9"/>
     </row>
     <row r="191" spans="1:20" ht="18" customHeight="1">
-      <c r="A191" s="64"/>
-      <c r="B191" s="73"/>
-      <c r="C191" s="68"/>
-      <c r="D191" s="68"/>
-      <c r="E191" s="73"/>
-      <c r="F191" s="68"/>
-      <c r="G191" s="68"/>
+      <c r="A191" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B191" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C191" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D191" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E191" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F191" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G191" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H191" s="68"/>
-      <c r="I191" s="83"/>
-      <c r="J191" s="70"/>
+      <c r="I191" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J191" s="70">
+        <v>452000000</v>
+      </c>
       <c r="K191" s="70"/>
-      <c r="L191" s="68"/>
-      <c r="M191" s="68"/>
-      <c r="N191" s="68"/>
+      <c r="L191" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M191" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N191" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O191" s="9"/>
       <c r="P191" s="4"/>
       <c r="Q191" s="4"/>
@@ -10916,20 +11315,44 @@
       <c r="T191" s="9"/>
     </row>
     <row r="192" spans="1:20" ht="18" customHeight="1">
-      <c r="A192" s="64"/>
-      <c r="B192" s="73"/>
-      <c r="C192" s="68"/>
-      <c r="D192" s="68"/>
-      <c r="E192" s="73"/>
-      <c r="F192" s="68"/>
-      <c r="G192" s="68"/>
+      <c r="A192" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B192" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C192" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D192" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E192" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F192" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G192" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H192" s="68"/>
-      <c r="I192" s="83"/>
-      <c r="J192" s="70"/>
+      <c r="I192" s="83">
+        <v>1473</v>
+      </c>
+      <c r="J192" s="70">
+        <v>202000000</v>
+      </c>
       <c r="K192" s="70"/>
-      <c r="L192" s="68"/>
-      <c r="M192" s="68"/>
-      <c r="N192" s="68"/>
+      <c r="L192" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M192" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N192" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O192" s="9"/>
       <c r="P192" s="4"/>
       <c r="Q192" s="4"/>
@@ -10938,20 +11361,44 @@
       <c r="T192" s="9"/>
     </row>
     <row r="193" spans="1:20" ht="18" customHeight="1">
-      <c r="A193" s="64"/>
-      <c r="B193" s="73"/>
-      <c r="C193" s="68"/>
-      <c r="D193" s="68"/>
-      <c r="E193" s="73"/>
-      <c r="F193" s="68"/>
-      <c r="G193" s="68"/>
+      <c r="A193" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B193" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C193" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D193" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E193" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F193" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G193" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H193" s="68"/>
-      <c r="I193" s="83"/>
-      <c r="J193" s="70"/>
+      <c r="I193" s="83">
+        <v>1474</v>
+      </c>
+      <c r="J193" s="70">
+        <v>337000000</v>
+      </c>
       <c r="K193" s="70"/>
-      <c r="L193" s="68"/>
-      <c r="M193" s="68"/>
-      <c r="N193" s="68"/>
+      <c r="L193" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M193" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N193" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O193" s="9"/>
       <c r="P193" s="4"/>
       <c r="Q193" s="4"/>
@@ -10960,20 +11407,44 @@
       <c r="T193" s="9"/>
     </row>
     <row r="194" spans="1:20" ht="18" customHeight="1">
-      <c r="A194" s="64"/>
-      <c r="B194" s="73"/>
-      <c r="C194" s="68"/>
-      <c r="D194" s="68"/>
-      <c r="E194" s="73"/>
-      <c r="F194" s="68"/>
-      <c r="G194" s="68"/>
+      <c r="A194" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B194" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C194" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D194" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E194" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F194" s="149" t="s">
+        <v>169</v>
+      </c>
+      <c r="G194" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H194" s="68"/>
-      <c r="I194" s="83"/>
-      <c r="J194" s="70"/>
+      <c r="I194" s="83">
+        <v>1475</v>
+      </c>
+      <c r="J194" s="70">
+        <v>373000000</v>
+      </c>
       <c r="K194" s="70"/>
-      <c r="L194" s="68"/>
-      <c r="M194" s="68"/>
-      <c r="N194" s="68"/>
+      <c r="L194" s="149" t="s">
+        <v>33</v>
+      </c>
+      <c r="M194" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="N194" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O194" s="9"/>
       <c r="P194" s="4"/>
       <c r="Q194" s="4"/>
@@ -10982,20 +11453,44 @@
       <c r="T194" s="9"/>
     </row>
     <row r="195" spans="1:20" ht="18" customHeight="1">
-      <c r="A195" s="64"/>
-      <c r="B195" s="73"/>
-      <c r="C195" s="68"/>
-      <c r="D195" s="68"/>
-      <c r="E195" s="73"/>
-      <c r="F195" s="68"/>
-      <c r="G195" s="68"/>
+      <c r="A195" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B195" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C195" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D195" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E195" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F195" s="149" t="s">
+        <v>170</v>
+      </c>
+      <c r="G195" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H195" s="68"/>
-      <c r="I195" s="83"/>
-      <c r="J195" s="70"/>
+      <c r="I195" s="83">
+        <v>298</v>
+      </c>
+      <c r="J195" s="70">
+        <v>59</v>
+      </c>
       <c r="K195" s="70"/>
-      <c r="L195" s="68"/>
-      <c r="M195" s="68"/>
-      <c r="N195" s="68"/>
+      <c r="L195" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M195" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N195" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O195" s="9"/>
       <c r="P195" s="4"/>
       <c r="Q195" s="4"/>
@@ -11004,20 +11499,44 @@
       <c r="T195" s="9"/>
     </row>
     <row r="196" spans="1:20" ht="18" customHeight="1">
-      <c r="A196" s="64"/>
-      <c r="B196" s="73"/>
-      <c r="C196" s="68"/>
-      <c r="D196" s="68"/>
-      <c r="E196" s="73"/>
-      <c r="F196" s="68"/>
-      <c r="G196" s="68"/>
+      <c r="A196" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B196" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C196" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D196" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E196" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F196" s="149" t="s">
+        <v>170</v>
+      </c>
+      <c r="G196" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H196" s="68"/>
-      <c r="I196" s="83"/>
-      <c r="J196" s="70"/>
+      <c r="I196" s="83">
+        <v>298</v>
+      </c>
+      <c r="J196" s="70">
+        <v>26</v>
+      </c>
       <c r="K196" s="70"/>
-      <c r="L196" s="68"/>
-      <c r="M196" s="68"/>
-      <c r="N196" s="68"/>
+      <c r="L196" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M196" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N196" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O196" s="9"/>
       <c r="P196" s="4"/>
       <c r="Q196" s="4"/>
@@ -11026,20 +11545,44 @@
       <c r="T196" s="9"/>
     </row>
     <row r="197" spans="1:20" ht="18" customHeight="1">
-      <c r="A197" s="64"/>
-      <c r="B197" s="73"/>
-      <c r="C197" s="68"/>
-      <c r="D197" s="68"/>
-      <c r="E197" s="73"/>
-      <c r="F197" s="68"/>
-      <c r="G197" s="68"/>
+      <c r="A197" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B197" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C197" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D197" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E197" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F197" s="149" t="s">
+        <v>170</v>
+      </c>
+      <c r="G197" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H197" s="68"/>
-      <c r="I197" s="83"/>
-      <c r="J197" s="70"/>
+      <c r="I197" s="83">
+        <v>298</v>
+      </c>
+      <c r="J197" s="70">
+        <v>18</v>
+      </c>
       <c r="K197" s="70"/>
-      <c r="L197" s="68"/>
-      <c r="M197" s="68"/>
-      <c r="N197" s="68"/>
+      <c r="L197" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M197" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N197" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O197" s="9"/>
       <c r="P197" s="4"/>
       <c r="Q197" s="4"/>
@@ -11048,20 +11591,44 @@
       <c r="T197" s="9"/>
     </row>
     <row r="198" spans="1:20" ht="18" customHeight="1">
-      <c r="A198" s="64"/>
-      <c r="B198" s="73"/>
-      <c r="C198" s="68"/>
-      <c r="D198" s="68"/>
-      <c r="E198" s="73"/>
-      <c r="F198" s="68"/>
-      <c r="G198" s="68"/>
+      <c r="A198" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B198" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C198" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D198" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E198" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F198" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G198" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H198" s="68"/>
-      <c r="I198" s="83"/>
-      <c r="J198" s="70"/>
+      <c r="I198" s="83">
+        <v>873</v>
+      </c>
+      <c r="J198" s="70">
+        <v>50</v>
+      </c>
       <c r="K198" s="70"/>
-      <c r="L198" s="68"/>
-      <c r="M198" s="68"/>
-      <c r="N198" s="68"/>
+      <c r="L198" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M198" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N198" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O198" s="9"/>
       <c r="P198" s="4"/>
       <c r="Q198" s="4"/>
@@ -11070,20 +11637,44 @@
       <c r="T198" s="9"/>
     </row>
     <row r="199" spans="1:20" ht="18" customHeight="1">
-      <c r="A199" s="64"/>
-      <c r="B199" s="73"/>
-      <c r="C199" s="68"/>
-      <c r="D199" s="68"/>
-      <c r="E199" s="73"/>
-      <c r="F199" s="68"/>
-      <c r="G199" s="68"/>
+      <c r="A199" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B199" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C199" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D199" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E199" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F199" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G199" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H199" s="68"/>
-      <c r="I199" s="83"/>
-      <c r="J199" s="70"/>
+      <c r="I199" s="83">
+        <v>873</v>
+      </c>
+      <c r="J199" s="70">
+        <v>50</v>
+      </c>
       <c r="K199" s="70"/>
-      <c r="L199" s="68"/>
-      <c r="M199" s="68"/>
-      <c r="N199" s="68"/>
+      <c r="L199" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M199" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N199" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O199" s="9"/>
       <c r="P199" s="4"/>
       <c r="Q199" s="4"/>
@@ -11092,20 +11683,44 @@
       <c r="T199" s="9"/>
     </row>
     <row r="200" spans="1:20" ht="18" customHeight="1">
-      <c r="A200" s="64"/>
-      <c r="B200" s="73"/>
-      <c r="C200" s="68"/>
-      <c r="D200" s="68"/>
-      <c r="E200" s="73"/>
-      <c r="F200" s="68"/>
-      <c r="G200" s="68"/>
+      <c r="A200" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B200" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C200" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D200" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E200" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F200" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G200" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H200" s="68"/>
-      <c r="I200" s="83"/>
-      <c r="J200" s="70"/>
+      <c r="I200" s="83">
+        <v>873</v>
+      </c>
+      <c r="J200" s="70">
+        <v>50</v>
+      </c>
       <c r="K200" s="70"/>
-      <c r="L200" s="68"/>
-      <c r="M200" s="68"/>
-      <c r="N200" s="68"/>
+      <c r="L200" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M200" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N200" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O200" s="9"/>
       <c r="P200" s="4"/>
       <c r="Q200" s="4"/>
@@ -11114,20 +11729,44 @@
       <c r="T200" s="9"/>
     </row>
     <row r="201" spans="1:20" ht="18" customHeight="1">
-      <c r="A201" s="64"/>
-      <c r="B201" s="73"/>
-      <c r="C201" s="68"/>
-      <c r="D201" s="68"/>
-      <c r="E201" s="73"/>
-      <c r="F201" s="68"/>
-      <c r="G201" s="68"/>
+      <c r="A201" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B201" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C201" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D201" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E201" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F201" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G201" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H201" s="68"/>
-      <c r="I201" s="83"/>
-      <c r="J201" s="70"/>
+      <c r="I201" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J201" s="70">
+        <v>50</v>
+      </c>
       <c r="K201" s="70"/>
-      <c r="L201" s="68"/>
-      <c r="M201" s="68"/>
-      <c r="N201" s="68"/>
+      <c r="L201" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M201" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N201" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O201" s="9"/>
       <c r="P201" s="4"/>
       <c r="Q201" s="4"/>
@@ -11136,20 +11775,44 @@
       <c r="T201" s="9"/>
     </row>
     <row r="202" spans="1:20" ht="18" customHeight="1">
-      <c r="A202" s="64"/>
-      <c r="B202" s="73"/>
-      <c r="C202" s="68"/>
-      <c r="D202" s="68"/>
-      <c r="E202" s="73"/>
-      <c r="F202" s="68"/>
-      <c r="G202" s="68"/>
+      <c r="A202" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B202" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C202" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D202" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E202" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F202" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G202" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H202" s="68"/>
-      <c r="I202" s="83"/>
-      <c r="J202" s="70"/>
+      <c r="I202" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J202" s="70">
+        <v>50</v>
+      </c>
       <c r="K202" s="70"/>
-      <c r="L202" s="68"/>
-      <c r="M202" s="68"/>
-      <c r="N202" s="68"/>
+      <c r="L202" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M202" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N202" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O202" s="9"/>
       <c r="P202" s="4"/>
       <c r="Q202" s="4"/>
@@ -11158,20 +11821,44 @@
       <c r="T202" s="9"/>
     </row>
     <row r="203" spans="1:20" ht="18" customHeight="1">
-      <c r="A203" s="64"/>
-      <c r="B203" s="73"/>
-      <c r="C203" s="68"/>
-      <c r="D203" s="68"/>
-      <c r="E203" s="73"/>
-      <c r="F203" s="68"/>
-      <c r="G203" s="68"/>
+      <c r="A203" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B203" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C203" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D203" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E203" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F203" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G203" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H203" s="68"/>
-      <c r="I203" s="83"/>
-      <c r="J203" s="70"/>
+      <c r="I203" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J203" s="70">
+        <v>50</v>
+      </c>
       <c r="K203" s="70"/>
-      <c r="L203" s="68"/>
-      <c r="M203" s="68"/>
-      <c r="N203" s="68"/>
+      <c r="L203" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M203" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N203" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O203" s="9"/>
       <c r="P203" s="4"/>
       <c r="Q203" s="4"/>
@@ -11180,20 +11867,44 @@
       <c r="T203" s="9"/>
     </row>
     <row r="204" spans="1:20" ht="18" customHeight="1">
-      <c r="A204" s="64"/>
-      <c r="B204" s="73"/>
-      <c r="C204" s="68"/>
-      <c r="D204" s="68"/>
-      <c r="E204" s="73"/>
-      <c r="F204" s="68"/>
-      <c r="G204" s="68"/>
+      <c r="A204" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B204" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C204" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D204" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E204" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F204" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G204" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H204" s="68"/>
-      <c r="I204" s="83"/>
-      <c r="J204" s="70"/>
+      <c r="I204" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J204" s="70">
+        <v>50</v>
+      </c>
       <c r="K204" s="70"/>
-      <c r="L204" s="68"/>
-      <c r="M204" s="68"/>
-      <c r="N204" s="68"/>
+      <c r="L204" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M204" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N204" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O204" s="9"/>
       <c r="P204" s="4"/>
       <c r="Q204" s="4"/>
@@ -11202,20 +11913,44 @@
       <c r="T204" s="9"/>
     </row>
     <row r="205" spans="1:20" ht="18" customHeight="1">
-      <c r="A205" s="64"/>
-      <c r="B205" s="73"/>
-      <c r="C205" s="68"/>
-      <c r="D205" s="68"/>
-      <c r="E205" s="73"/>
-      <c r="F205" s="68"/>
-      <c r="G205" s="68"/>
+      <c r="A205" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B205" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C205" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D205" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E205" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F205" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G205" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H205" s="68"/>
-      <c r="I205" s="83"/>
-      <c r="J205" s="70"/>
+      <c r="I205" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J205" s="70">
+        <v>50</v>
+      </c>
       <c r="K205" s="70"/>
-      <c r="L205" s="68"/>
-      <c r="M205" s="68"/>
-      <c r="N205" s="68"/>
+      <c r="L205" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M205" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N205" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O205" s="9"/>
       <c r="P205" s="4"/>
       <c r="Q205" s="4"/>
@@ -11224,20 +11959,44 @@
       <c r="T205" s="9"/>
     </row>
     <row r="206" spans="1:20" ht="18" customHeight="1">
-      <c r="A206" s="64"/>
-      <c r="B206" s="73"/>
-      <c r="C206" s="68"/>
-      <c r="D206" s="68"/>
-      <c r="E206" s="73"/>
-      <c r="F206" s="68"/>
-      <c r="G206" s="68"/>
+      <c r="A206" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B206" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C206" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D206" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E206" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F206" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G206" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H206" s="68"/>
-      <c r="I206" s="83"/>
-      <c r="J206" s="70"/>
+      <c r="I206" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J206" s="70">
+        <v>50</v>
+      </c>
       <c r="K206" s="70"/>
-      <c r="L206" s="68"/>
-      <c r="M206" s="68"/>
-      <c r="N206" s="68"/>
+      <c r="L206" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M206" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N206" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O206" s="9"/>
       <c r="P206" s="4"/>
       <c r="Q206" s="4"/>
@@ -11246,20 +12005,44 @@
       <c r="T206" s="9"/>
     </row>
     <row r="207" spans="1:20" ht="18" customHeight="1">
-      <c r="A207" s="64"/>
-      <c r="B207" s="73"/>
-      <c r="C207" s="68"/>
-      <c r="D207" s="68"/>
-      <c r="E207" s="73"/>
-      <c r="F207" s="68"/>
-      <c r="G207" s="68"/>
+      <c r="A207" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="B207" s="148" t="s">
+        <v>259</v>
+      </c>
+      <c r="C207" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D207" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E207" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F207" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G207" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H207" s="68"/>
-      <c r="I207" s="83"/>
-      <c r="J207" s="70"/>
+      <c r="I207" s="83">
+        <v>1473</v>
+      </c>
+      <c r="J207" s="70">
+        <v>50</v>
+      </c>
       <c r="K207" s="70"/>
-      <c r="L207" s="68"/>
-      <c r="M207" s="68"/>
-      <c r="N207" s="68"/>
+      <c r="L207" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M207" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N207" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O207" s="9"/>
       <c r="P207" s="4"/>
       <c r="Q207" s="4"/>
@@ -11268,20 +12051,44 @@
       <c r="T207" s="9"/>
     </row>
     <row r="208" spans="1:20" ht="18" customHeight="1">
-      <c r="A208" s="64"/>
-      <c r="B208" s="73"/>
-      <c r="C208" s="68"/>
-      <c r="D208" s="68"/>
-      <c r="E208" s="73"/>
-      <c r="F208" s="68"/>
-      <c r="G208" s="68"/>
+      <c r="A208" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="B208" s="148" t="s">
+        <v>263</v>
+      </c>
+      <c r="C208" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D208" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E208" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F208" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G208" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H208" s="68"/>
-      <c r="I208" s="83"/>
-      <c r="J208" s="70"/>
+      <c r="I208" s="83">
+        <v>1474</v>
+      </c>
+      <c r="J208" s="70">
+        <v>50</v>
+      </c>
       <c r="K208" s="70"/>
-      <c r="L208" s="68"/>
-      <c r="M208" s="68"/>
-      <c r="N208" s="68"/>
+      <c r="L208" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M208" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N208" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O208" s="9"/>
       <c r="P208" s="4"/>
       <c r="Q208" s="4"/>
@@ -11290,20 +12097,44 @@
       <c r="T208" s="9"/>
     </row>
     <row r="209" spans="1:20" ht="18" customHeight="1">
-      <c r="A209" s="64"/>
-      <c r="B209" s="73"/>
-      <c r="C209" s="68"/>
-      <c r="D209" s="68"/>
-      <c r="E209" s="73"/>
-      <c r="F209" s="68"/>
-      <c r="G209" s="68"/>
+      <c r="A209" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="B209" s="148" t="s">
+        <v>264</v>
+      </c>
+      <c r="C209" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="D209" s="149" t="s">
+        <v>266</v>
+      </c>
+      <c r="E209" s="148" t="s">
+        <v>267</v>
+      </c>
+      <c r="F209" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="G209" s="149" t="s">
+        <v>29</v>
+      </c>
       <c r="H209" s="68"/>
-      <c r="I209" s="83"/>
-      <c r="J209" s="4"/>
+      <c r="I209" s="83">
+        <v>1475</v>
+      </c>
+      <c r="J209" s="70">
+        <v>50</v>
+      </c>
       <c r="K209" s="4"/>
-      <c r="L209" s="4"/>
-      <c r="M209" s="68"/>
-      <c r="N209" s="68"/>
+      <c r="L209" s="149" t="s">
+        <v>171</v>
+      </c>
+      <c r="M209" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="N209" s="149" t="s">
+        <v>268</v>
+      </c>
       <c r="O209" s="9"/>
       <c r="P209" s="4"/>
       <c r="Q209" s="4"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1557/mrc.2017.7`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F7A8FB-9945-EF4A-A216-709FF567F5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B949C8-FAAF-FF4C-A680-AD27D7C9DFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="4080" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="760" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="271">
   <si>
     <r>
       <rPr>
@@ -927,6 +927,12 @@
   </si>
   <si>
     <t>10.1016/j.msea.2023.144870</t>
+  </si>
+  <si>
+    <t>10.1557/mrc.2017.7</t>
+  </si>
+  <si>
+    <t>CrMoNbReTaVW</t>
   </si>
 </sst>
 </file>
@@ -1969,6 +1975,69 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2028,69 +2097,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="16" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3254,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D169" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N214" sqref="N214"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E184" zoomScale="86" workbookViewId="0">
+      <selection activeCell="H194" sqref="H194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3312,19 +3318,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="112"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="119"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="139"/>
+      <c r="M2" s="139"/>
+      <c r="N2" s="142"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3340,17 +3346,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="123"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="145"/>
+      <c r="K3" s="145"/>
+      <c r="L3" s="143"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="146"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3391,43 +3397,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="147" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="126" t="s">
+      <c r="D5" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="126" t="s">
+      <c r="E5" s="149" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="126" t="s">
+      <c r="F5" s="149" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="126" t="s">
+      <c r="G5" s="149" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="127" t="s">
+      <c r="H5" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="126" t="s">
+      <c r="I5" s="149" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="126" t="s">
+      <c r="J5" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="126" t="s">
+      <c r="K5" s="149" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="126" t="s">
+      <c r="L5" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="126" t="s">
+      <c r="M5" s="149" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="126" t="s">
+      <c r="N5" s="149" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="131" t="s">
+      <c r="O5" s="117" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3443,19 +3449,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="125"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="130"/>
-      <c r="K6" s="130"/>
-      <c r="L6" s="125"/>
-      <c r="M6" s="125"/>
-      <c r="N6" s="125"/>
-      <c r="O6" s="132"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="148"/>
+      <c r="E6" s="148"/>
+      <c r="F6" s="148"/>
+      <c r="G6" s="148"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="152"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
+      <c r="N6" s="148"/>
+      <c r="O6" s="118"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3505,7 +3511,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="133"/>
+      <c r="O7" s="119"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -3520,35 +3526,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="134" t="s">
+      <c r="B8" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="135"/>
-      <c r="D8" s="135"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="137" t="s">
+      <c r="C8" s="121"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="138"/>
-      <c r="H8" s="138"/>
-      <c r="I8" s="139"/>
-      <c r="J8" s="140"/>
-      <c r="K8" s="140"/>
-      <c r="L8" s="141"/>
-      <c r="M8" s="142" t="s">
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="127"/>
+      <c r="M8" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="143"/>
+      <c r="N8" s="129"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="144" t="s">
+      <c r="P8" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="145"/>
-      <c r="R8" s="146"/>
-      <c r="S8" s="146"/>
-      <c r="T8" s="147"/>
+      <c r="Q8" s="131"/>
+      <c r="R8" s="132"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="133"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="38" t="s">
@@ -8296,16 +8302,16 @@
     </row>
     <row r="117" spans="1:20" ht="18" customHeight="1">
       <c r="A117" s="64"/>
-      <c r="B117" s="148" t="s">
+      <c r="B117" s="111" t="s">
         <v>194</v>
       </c>
-      <c r="C117" s="149" t="s">
+      <c r="C117" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="D117" s="149" t="s">
+      <c r="D117" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E117" s="148" t="s">
+      <c r="E117" s="111" t="s">
         <v>201</v>
       </c>
       <c r="F117" s="68"/>
@@ -8316,7 +8322,7 @@
       <c r="K117" s="70"/>
       <c r="L117" s="68"/>
       <c r="M117" s="68"/>
-      <c r="N117" s="149" t="s">
+      <c r="N117" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O117" s="9"/>
@@ -8328,16 +8334,16 @@
     </row>
     <row r="118" spans="1:20" ht="18" customHeight="1">
       <c r="A118" s="64"/>
-      <c r="B118" s="148" t="s">
+      <c r="B118" s="111" t="s">
         <v>194</v>
       </c>
-      <c r="C118" s="149" t="s">
+      <c r="C118" s="112" t="s">
         <v>203</v>
       </c>
-      <c r="D118" s="149" t="s">
+      <c r="D118" s="112" t="s">
         <v>195</v>
       </c>
-      <c r="E118" s="148" t="s">
+      <c r="E118" s="111" t="s">
         <v>204</v>
       </c>
       <c r="F118" s="68"/>
@@ -8348,7 +8354,7 @@
       <c r="K118" s="70"/>
       <c r="L118" s="68"/>
       <c r="M118" s="68"/>
-      <c r="N118" s="149" t="s">
+      <c r="N118" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O118" s="9"/>
@@ -8360,16 +8366,16 @@
     </row>
     <row r="119" spans="1:20" ht="18" customHeight="1">
       <c r="A119" s="64"/>
-      <c r="B119" s="148" t="s">
+      <c r="B119" s="111" t="s">
         <v>194</v>
       </c>
-      <c r="C119" s="149" t="s">
+      <c r="C119" s="112" t="s">
         <v>203</v>
       </c>
-      <c r="D119" s="149" t="s">
+      <c r="D119" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="E119" s="148" t="s">
+      <c r="E119" s="111" t="s">
         <v>206</v>
       </c>
       <c r="F119" s="68"/>
@@ -8380,7 +8386,7 @@
       <c r="K119" s="70"/>
       <c r="L119" s="68"/>
       <c r="M119" s="68"/>
-      <c r="N119" s="149" t="s">
+      <c r="N119" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O119" s="9"/>
@@ -8392,16 +8398,16 @@
     </row>
     <row r="120" spans="1:20" ht="18" customHeight="1">
       <c r="A120" s="64"/>
-      <c r="B120" s="148" t="s">
+      <c r="B120" s="111" t="s">
         <v>194</v>
       </c>
-      <c r="C120" s="149" t="s">
+      <c r="C120" s="112" t="s">
         <v>205</v>
       </c>
-      <c r="D120" s="149" t="s">
+      <c r="D120" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="E120" s="148" t="s">
+      <c r="E120" s="111" t="s">
         <v>207</v>
       </c>
       <c r="F120" s="68"/>
@@ -8412,7 +8418,7 @@
       <c r="K120" s="70"/>
       <c r="L120" s="68"/>
       <c r="M120" s="68"/>
-      <c r="N120" s="149" t="s">
+      <c r="N120" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O120" s="9"/>
@@ -8424,16 +8430,16 @@
     </row>
     <row r="121" spans="1:20" ht="18" customHeight="1">
       <c r="A121" s="64"/>
-      <c r="B121" s="148" t="s">
+      <c r="B121" s="111" t="s">
         <v>194</v>
       </c>
-      <c r="C121" s="149" t="s">
+      <c r="C121" s="112" t="s">
         <v>203</v>
       </c>
-      <c r="D121" s="149" t="s">
+      <c r="D121" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="E121" s="148" t="s">
+      <c r="E121" s="111" t="s">
         <v>208</v>
       </c>
       <c r="F121" s="68"/>
@@ -8444,7 +8450,7 @@
       <c r="K121" s="70"/>
       <c r="L121" s="68"/>
       <c r="M121" s="68"/>
-      <c r="N121" s="149" t="s">
+      <c r="N121" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O121" s="9"/>
@@ -8456,16 +8462,16 @@
     </row>
     <row r="122" spans="1:20" ht="18" customHeight="1">
       <c r="A122" s="64"/>
-      <c r="B122" s="148" t="s">
+      <c r="B122" s="111" t="s">
         <v>209</v>
       </c>
-      <c r="C122" s="149" t="s">
+      <c r="C122" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D122" s="149" t="s">
+      <c r="D122" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E122" s="148" t="s">
+      <c r="E122" s="111" t="s">
         <v>211</v>
       </c>
       <c r="F122" s="68"/>
@@ -8476,7 +8482,7 @@
       <c r="K122" s="70"/>
       <c r="L122" s="68"/>
       <c r="M122" s="68"/>
-      <c r="N122" s="149" t="s">
+      <c r="N122" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O122" s="9"/>
@@ -8488,16 +8494,16 @@
     </row>
     <row r="123" spans="1:20" ht="18" customHeight="1">
       <c r="A123" s="64"/>
-      <c r="B123" s="148" t="s">
+      <c r="B123" s="111" t="s">
         <v>209</v>
       </c>
-      <c r="C123" s="149" t="s">
+      <c r="C123" s="112" t="s">
         <v>212</v>
       </c>
-      <c r="D123" s="149" t="s">
+      <c r="D123" s="112" t="s">
         <v>195</v>
       </c>
-      <c r="E123" s="148" t="s">
+      <c r="E123" s="111" t="s">
         <v>196</v>
       </c>
       <c r="F123" s="68"/>
@@ -8508,7 +8514,7 @@
       <c r="K123" s="70"/>
       <c r="L123" s="68"/>
       <c r="M123" s="68"/>
-      <c r="N123" s="149" t="s">
+      <c r="N123" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O123" s="9"/>
@@ -8520,16 +8526,16 @@
     </row>
     <row r="124" spans="1:20" ht="18" customHeight="1">
       <c r="A124" s="64"/>
-      <c r="B124" s="148" t="s">
+      <c r="B124" s="111" t="s">
         <v>209</v>
       </c>
-      <c r="C124" s="149" t="s">
+      <c r="C124" s="112" t="s">
         <v>213</v>
       </c>
-      <c r="D124" s="149" t="s">
+      <c r="D124" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="E124" s="148" t="s">
+      <c r="E124" s="111" t="s">
         <v>198</v>
       </c>
       <c r="F124" s="68"/>
@@ -8540,7 +8546,7 @@
       <c r="K124" s="70"/>
       <c r="L124" s="68"/>
       <c r="M124" s="68"/>
-      <c r="N124" s="149" t="s">
+      <c r="N124" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O124" s="9"/>
@@ -8552,16 +8558,16 @@
     </row>
     <row r="125" spans="1:20" ht="18" customHeight="1">
       <c r="A125" s="64"/>
-      <c r="B125" s="148" t="s">
+      <c r="B125" s="111" t="s">
         <v>209</v>
       </c>
-      <c r="C125" s="149" t="s">
+      <c r="C125" s="112" t="s">
         <v>213</v>
       </c>
-      <c r="D125" s="149" t="s">
+      <c r="D125" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="E125" s="148" t="s">
+      <c r="E125" s="111" t="s">
         <v>199</v>
       </c>
       <c r="F125" s="68"/>
@@ -8572,7 +8578,7 @@
       <c r="K125" s="70"/>
       <c r="L125" s="68"/>
       <c r="M125" s="68"/>
-      <c r="N125" s="149" t="s">
+      <c r="N125" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O125" s="9"/>
@@ -8584,16 +8590,16 @@
     </row>
     <row r="126" spans="1:20" ht="18" customHeight="1">
       <c r="A126" s="64"/>
-      <c r="B126" s="148" t="s">
+      <c r="B126" s="111" t="s">
         <v>209</v>
       </c>
-      <c r="C126" s="149" t="s">
+      <c r="C126" s="112" t="s">
         <v>214</v>
       </c>
-      <c r="D126" s="149" t="s">
+      <c r="D126" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="E126" s="148" t="s">
+      <c r="E126" s="111" t="s">
         <v>200</v>
       </c>
       <c r="F126" s="68"/>
@@ -8604,7 +8610,7 @@
       <c r="K126" s="70"/>
       <c r="L126" s="68"/>
       <c r="M126" s="68"/>
-      <c r="N126" s="149" t="s">
+      <c r="N126" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O126" s="9"/>
@@ -8616,13 +8622,13 @@
     </row>
     <row r="127" spans="1:20" ht="18" customHeight="1">
       <c r="A127" s="64"/>
-      <c r="B127" s="148" t="s">
+      <c r="B127" s="111" t="s">
         <v>215</v>
       </c>
-      <c r="C127" s="149" t="s">
+      <c r="C127" s="112" t="s">
         <v>214</v>
       </c>
-      <c r="D127" s="149" t="s">
+      <c r="D127" s="112" t="s">
         <v>113</v>
       </c>
       <c r="E127" s="73"/>
@@ -8634,7 +8640,7 @@
       <c r="K127" s="70"/>
       <c r="L127" s="68"/>
       <c r="M127" s="68"/>
-      <c r="N127" s="149" t="s">
+      <c r="N127" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O127" s="9"/>
@@ -8646,16 +8652,16 @@
     </row>
     <row r="128" spans="1:20" ht="18" customHeight="1">
       <c r="A128" s="64"/>
-      <c r="B128" s="148" t="s">
+      <c r="B128" s="111" t="s">
         <v>215</v>
       </c>
-      <c r="C128" s="149" t="s">
+      <c r="C128" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="D128" s="149" t="s">
+      <c r="D128" s="112" t="s">
         <v>195</v>
       </c>
-      <c r="E128" s="148" t="s">
+      <c r="E128" s="111" t="s">
         <v>196</v>
       </c>
       <c r="F128" s="68"/>
@@ -8666,7 +8672,7 @@
       <c r="K128" s="70"/>
       <c r="L128" s="68"/>
       <c r="M128" s="68"/>
-      <c r="N128" s="149" t="s">
+      <c r="N128" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O128" s="9"/>
@@ -8678,16 +8684,16 @@
     </row>
     <row r="129" spans="1:20" ht="18" customHeight="1">
       <c r="A129" s="64"/>
-      <c r="B129" s="148" t="s">
+      <c r="B129" s="111" t="s">
         <v>215</v>
       </c>
-      <c r="C129" s="149" t="s">
+      <c r="C129" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="D129" s="149" t="s">
+      <c r="D129" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="E129" s="148" t="s">
+      <c r="E129" s="111" t="s">
         <v>198</v>
       </c>
       <c r="F129" s="68"/>
@@ -8698,7 +8704,7 @@
       <c r="K129" s="70"/>
       <c r="L129" s="68"/>
       <c r="M129" s="68"/>
-      <c r="N129" s="149" t="s">
+      <c r="N129" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O129" s="9"/>
@@ -8710,16 +8716,16 @@
     </row>
     <row r="130" spans="1:20" ht="18" customHeight="1">
       <c r="A130" s="64"/>
-      <c r="B130" s="148" t="s">
+      <c r="B130" s="111" t="s">
         <v>215</v>
       </c>
-      <c r="C130" s="149" t="s">
+      <c r="C130" s="112" t="s">
         <v>216</v>
       </c>
-      <c r="D130" s="149" t="s">
+      <c r="D130" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="E130" s="148" t="s">
+      <c r="E130" s="111" t="s">
         <v>199</v>
       </c>
       <c r="F130" s="68"/>
@@ -8730,7 +8736,7 @@
       <c r="K130" s="70"/>
       <c r="L130" s="68"/>
       <c r="M130" s="68"/>
-      <c r="N130" s="149" t="s">
+      <c r="N130" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O130" s="9"/>
@@ -8742,16 +8748,16 @@
     </row>
     <row r="131" spans="1:20" ht="18" customHeight="1">
       <c r="A131" s="64"/>
-      <c r="B131" s="148" t="s">
+      <c r="B131" s="111" t="s">
         <v>215</v>
       </c>
-      <c r="C131" s="149" t="s">
+      <c r="C131" s="112" t="s">
         <v>216</v>
       </c>
-      <c r="D131" s="149" t="s">
+      <c r="D131" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="E131" s="148" t="s">
+      <c r="E131" s="111" t="s">
         <v>200</v>
       </c>
       <c r="F131" s="68"/>
@@ -8762,7 +8768,7 @@
       <c r="K131" s="70"/>
       <c r="L131" s="68"/>
       <c r="M131" s="68"/>
-      <c r="N131" s="149" t="s">
+      <c r="N131" s="112" t="s">
         <v>217</v>
       </c>
       <c r="O131" s="9"/>
@@ -8774,16 +8780,16 @@
     </row>
     <row r="132" spans="1:20" ht="18" customHeight="1">
       <c r="A132" s="64"/>
-      <c r="B132" s="148" t="s">
+      <c r="B132" s="111" t="s">
         <v>219</v>
       </c>
-      <c r="C132" s="150" t="s">
+      <c r="C132" s="113" t="s">
         <v>220</v>
       </c>
-      <c r="D132" s="149" t="s">
+      <c r="D132" s="112" t="s">
         <v>238</v>
       </c>
-      <c r="E132" s="149" t="s">
+      <c r="E132" s="112" t="s">
         <v>218</v>
       </c>
       <c r="F132" s="68"/>
@@ -8794,7 +8800,7 @@
       <c r="K132" s="70"/>
       <c r="L132" s="68"/>
       <c r="M132" s="68"/>
-      <c r="N132" s="149" t="s">
+      <c r="N132" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O132" s="9"/>
@@ -8806,16 +8812,16 @@
     </row>
     <row r="133" spans="1:20" ht="18" customHeight="1">
       <c r="A133" s="64"/>
-      <c r="B133" s="148" t="s">
+      <c r="B133" s="111" t="s">
         <v>223</v>
       </c>
-      <c r="C133" s="149" t="s">
+      <c r="C133" s="112" t="s">
         <v>222</v>
       </c>
-      <c r="D133" s="149" t="s">
+      <c r="D133" s="112" t="s">
         <v>238</v>
       </c>
-      <c r="E133" s="148" t="s">
+      <c r="E133" s="111" t="s">
         <v>221</v>
       </c>
       <c r="F133" s="68"/>
@@ -8826,7 +8832,7 @@
       <c r="K133" s="70"/>
       <c r="L133" s="68"/>
       <c r="M133" s="68"/>
-      <c r="N133" s="149" t="s">
+      <c r="N133" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O133" s="9"/>
@@ -8838,13 +8844,13 @@
     </row>
     <row r="134" spans="1:20" ht="18" customHeight="1">
       <c r="A134" s="64"/>
-      <c r="B134" s="148" t="s">
+      <c r="B134" s="111" t="s">
         <v>224</v>
       </c>
-      <c r="C134" s="149" t="s">
+      <c r="C134" s="112" t="s">
         <v>231</v>
       </c>
-      <c r="D134" s="149" t="s">
+      <c r="D134" s="112" t="s">
         <v>238</v>
       </c>
       <c r="E134" s="73"/>
@@ -8856,7 +8862,7 @@
       <c r="K134" s="70"/>
       <c r="L134" s="68"/>
       <c r="M134" s="68"/>
-      <c r="N134" s="149" t="s">
+      <c r="N134" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O134" s="9"/>
@@ -8868,13 +8874,13 @@
     </row>
     <row r="135" spans="1:20" ht="18" customHeight="1">
       <c r="A135" s="64"/>
-      <c r="B135" s="148" t="s">
+      <c r="B135" s="111" t="s">
         <v>225</v>
       </c>
-      <c r="C135" s="149" t="s">
+      <c r="C135" s="112" t="s">
         <v>232</v>
       </c>
-      <c r="D135" s="149" t="s">
+      <c r="D135" s="112" t="s">
         <v>238</v>
       </c>
       <c r="E135" s="73"/>
@@ -8886,7 +8892,7 @@
       <c r="K135" s="70"/>
       <c r="L135" s="68"/>
       <c r="M135" s="68"/>
-      <c r="N135" s="149" t="s">
+      <c r="N135" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O135" s="9"/>
@@ -8898,13 +8904,13 @@
     </row>
     <row r="136" spans="1:20" ht="18" customHeight="1">
       <c r="A136" s="64"/>
-      <c r="B136" s="148" t="s">
+      <c r="B136" s="111" t="s">
         <v>226</v>
       </c>
-      <c r="C136" s="149" t="s">
+      <c r="C136" s="112" t="s">
         <v>233</v>
       </c>
-      <c r="D136" s="149" t="s">
+      <c r="D136" s="112" t="s">
         <v>238</v>
       </c>
       <c r="E136" s="73"/>
@@ -8916,7 +8922,7 @@
       <c r="K136" s="70"/>
       <c r="L136" s="68"/>
       <c r="M136" s="68"/>
-      <c r="N136" s="149" t="s">
+      <c r="N136" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O136" s="9"/>
@@ -8928,13 +8934,13 @@
     </row>
     <row r="137" spans="1:20" ht="18" customHeight="1">
       <c r="A137" s="64"/>
-      <c r="B137" s="148" t="s">
+      <c r="B137" s="111" t="s">
         <v>227</v>
       </c>
-      <c r="C137" s="149" t="s">
+      <c r="C137" s="112" t="s">
         <v>234</v>
       </c>
-      <c r="D137" s="149" t="s">
+      <c r="D137" s="112" t="s">
         <v>238</v>
       </c>
       <c r="E137" s="73"/>
@@ -8946,7 +8952,7 @@
       <c r="K137" s="70"/>
       <c r="L137" s="68"/>
       <c r="M137" s="68"/>
-      <c r="N137" s="149" t="s">
+      <c r="N137" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O137" s="9"/>
@@ -8958,13 +8964,13 @@
     </row>
     <row r="138" spans="1:20" ht="18" customHeight="1">
       <c r="A138" s="64"/>
-      <c r="B138" s="148" t="s">
+      <c r="B138" s="111" t="s">
         <v>228</v>
       </c>
-      <c r="C138" s="149" t="s">
+      <c r="C138" s="112" t="s">
         <v>234</v>
       </c>
-      <c r="D138" s="149" t="s">
+      <c r="D138" s="112" t="s">
         <v>238</v>
       </c>
       <c r="E138" s="73"/>
@@ -8976,7 +8982,7 @@
       <c r="K138" s="70"/>
       <c r="L138" s="68"/>
       <c r="M138" s="68"/>
-      <c r="N138" s="149" t="s">
+      <c r="N138" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O138" s="9"/>
@@ -8988,13 +8994,13 @@
     </row>
     <row r="139" spans="1:20" ht="18" customHeight="1">
       <c r="A139" s="64"/>
-      <c r="B139" s="148" t="s">
+      <c r="B139" s="111" t="s">
         <v>235</v>
       </c>
-      <c r="C139" s="149" t="s">
+      <c r="C139" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="D139" s="149" t="s">
+      <c r="D139" s="112" t="s">
         <v>238</v>
       </c>
       <c r="E139" s="73"/>
@@ -9006,7 +9012,7 @@
       <c r="K139" s="70"/>
       <c r="L139" s="68"/>
       <c r="M139" s="68"/>
-      <c r="N139" s="149" t="s">
+      <c r="N139" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O139" s="9"/>
@@ -9018,13 +9024,13 @@
     </row>
     <row r="140" spans="1:20" ht="18" customHeight="1">
       <c r="A140" s="64"/>
-      <c r="B140" s="148" t="s">
+      <c r="B140" s="111" t="s">
         <v>229</v>
       </c>
-      <c r="C140" s="149" t="s">
+      <c r="C140" s="112" t="s">
         <v>233</v>
       </c>
-      <c r="D140" s="149" t="s">
+      <c r="D140" s="112" t="s">
         <v>238</v>
       </c>
       <c r="E140" s="73"/>
@@ -9036,7 +9042,7 @@
       <c r="K140" s="70"/>
       <c r="L140" s="68"/>
       <c r="M140" s="68"/>
-      <c r="N140" s="149" t="s">
+      <c r="N140" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O140" s="9"/>
@@ -9048,16 +9054,16 @@
     </row>
     <row r="141" spans="1:20" ht="18" customHeight="1">
       <c r="A141" s="64"/>
-      <c r="B141" s="148" t="s">
+      <c r="B141" s="111" t="s">
         <v>230</v>
       </c>
-      <c r="C141" s="149" t="s">
+      <c r="C141" s="112" t="s">
         <v>237</v>
       </c>
-      <c r="D141" s="149" t="s">
+      <c r="D141" s="112" t="s">
         <v>238</v>
       </c>
-      <c r="E141" s="151" t="s">
+      <c r="E141" s="114" t="s">
         <v>236</v>
       </c>
       <c r="F141" s="68"/>
@@ -9068,7 +9074,7 @@
       <c r="K141" s="70"/>
       <c r="L141" s="68"/>
       <c r="M141" s="68"/>
-      <c r="N141" s="149" t="s">
+      <c r="N141" s="112" t="s">
         <v>239</v>
       </c>
       <c r="O141" s="9"/>
@@ -9080,22 +9086,22 @@
     </row>
     <row r="142" spans="1:20" ht="18" customHeight="1">
       <c r="A142" s="64"/>
-      <c r="B142" s="148" t="s">
+      <c r="B142" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C142" s="149" t="s">
+      <c r="C142" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D142" s="149" t="s">
+      <c r="D142" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E142" s="148" t="s">
+      <c r="E142" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F142" s="149" t="s">
+      <c r="F142" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="G142" s="149" t="s">
+      <c r="G142" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H142" s="68"/>
@@ -9106,13 +9112,13 @@
         <v>6600</v>
       </c>
       <c r="K142" s="70"/>
-      <c r="L142" s="149" t="s">
+      <c r="L142" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="M142" s="149" t="s">
+      <c r="M142" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="N142" s="149" t="s">
+      <c r="N142" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O142" s="9"/>
@@ -9124,22 +9130,22 @@
     </row>
     <row r="143" spans="1:20" ht="18" customHeight="1">
       <c r="A143" s="64"/>
-      <c r="B143" s="148" t="s">
+      <c r="B143" s="111" t="s">
         <v>243</v>
       </c>
-      <c r="C143" s="149" t="s">
+      <c r="C143" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D143" s="149" t="s">
+      <c r="D143" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E143" s="148" t="s">
+      <c r="E143" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F143" s="149" t="s">
+      <c r="F143" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="G143" s="149" t="s">
+      <c r="G143" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H143" s="68"/>
@@ -9150,13 +9156,13 @@
         <v>6740</v>
       </c>
       <c r="K143" s="70"/>
-      <c r="L143" s="149" t="s">
+      <c r="L143" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="M143" s="149" t="s">
+      <c r="M143" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="N143" s="149" t="s">
+      <c r="N143" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O143" s="9"/>
@@ -9168,22 +9174,22 @@
     </row>
     <row r="144" spans="1:20" ht="18" customHeight="1">
       <c r="A144" s="64"/>
-      <c r="B144" s="148" t="s">
+      <c r="B144" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C144" s="149" t="s">
+      <c r="C144" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D144" s="149" t="s">
+      <c r="D144" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E144" s="148" t="s">
+      <c r="E144" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F144" s="149" t="s">
+      <c r="F144" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="G144" s="149" t="s">
+      <c r="G144" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H144" s="68"/>
@@ -9194,13 +9200,13 @@
         <v>6850</v>
       </c>
       <c r="K144" s="70"/>
-      <c r="L144" s="149" t="s">
+      <c r="L144" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="M144" s="149" t="s">
+      <c r="M144" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="N144" s="149" t="s">
+      <c r="N144" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O144" s="9"/>
@@ -9212,22 +9218,22 @@
     </row>
     <row r="145" spans="1:20" ht="18" customHeight="1">
       <c r="A145" s="64"/>
-      <c r="B145" s="148" t="s">
+      <c r="B145" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C145" s="149" t="s">
+      <c r="C145" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D145" s="149" t="s">
+      <c r="D145" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E145" s="148" t="s">
+      <c r="E145" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F145" s="149" t="s">
+      <c r="F145" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="G145" s="149" t="s">
+      <c r="G145" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H145" s="68"/>
@@ -9239,13 +9245,13 @@
         <v>4506316500</v>
       </c>
       <c r="K145" s="70"/>
-      <c r="L145" s="149" t="s">
+      <c r="L145" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M145" s="149" t="s">
+      <c r="M145" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="N145" s="149" t="s">
+      <c r="N145" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O145" s="9"/>
@@ -9259,22 +9265,22 @@
     </row>
     <row r="146" spans="1:20" ht="18" customHeight="1">
       <c r="A146" s="64"/>
-      <c r="B146" s="148" t="s">
+      <c r="B146" s="111" t="s">
         <v>243</v>
       </c>
-      <c r="C146" s="149" t="s">
+      <c r="C146" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D146" s="149" t="s">
+      <c r="D146" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E146" s="148" t="s">
+      <c r="E146" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F146" s="149" t="s">
+      <c r="F146" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="G146" s="149" t="s">
+      <c r="G146" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H146" s="68"/>
@@ -9286,13 +9292,13 @@
         <v>4597521600</v>
       </c>
       <c r="K146" s="70"/>
-      <c r="L146" s="149" t="s">
+      <c r="L146" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M146" s="149" t="s">
+      <c r="M146" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="N146" s="149" t="s">
+      <c r="N146" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O146" s="9"/>
@@ -9306,22 +9312,22 @@
     </row>
     <row r="147" spans="1:20" ht="18" customHeight="1">
       <c r="A147" s="64"/>
-      <c r="B147" s="148" t="s">
+      <c r="B147" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C147" s="149" t="s">
+      <c r="C147" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D147" s="149" t="s">
+      <c r="D147" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E147" s="148" t="s">
+      <c r="E147" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F147" s="149" t="s">
+      <c r="F147" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="G147" s="149" t="s">
+      <c r="G147" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H147" s="68"/>
@@ -9333,13 +9339,13 @@
         <v>4704417900</v>
       </c>
       <c r="K147" s="70"/>
-      <c r="L147" s="149" t="s">
+      <c r="L147" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M147" s="149" t="s">
+      <c r="M147" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="N147" s="149" t="s">
+      <c r="N147" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O147" s="9"/>
@@ -9353,22 +9359,22 @@
     </row>
     <row r="148" spans="1:20" ht="18" customHeight="1">
       <c r="A148" s="64"/>
-      <c r="B148" s="148" t="s">
+      <c r="B148" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C148" s="149" t="s">
+      <c r="C148" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D148" s="149" t="s">
+      <c r="D148" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E148" s="148" t="s">
+      <c r="E148" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F148" s="149" t="s">
+      <c r="F148" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="G148" s="149" t="s">
+      <c r="G148" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H148" s="68"/>
@@ -9379,13 +9385,13 @@
         <v>2783000000</v>
       </c>
       <c r="K148" s="70"/>
-      <c r="L148" s="149" t="s">
+      <c r="L148" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M148" s="149" t="s">
+      <c r="M148" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N148" s="149" t="s">
+      <c r="N148" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O148" s="9"/>
@@ -9397,22 +9403,22 @@
     </row>
     <row r="149" spans="1:20" ht="18" customHeight="1">
       <c r="A149" s="64"/>
-      <c r="B149" s="148" t="s">
+      <c r="B149" s="111" t="s">
         <v>243</v>
       </c>
-      <c r="C149" s="149" t="s">
+      <c r="C149" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D149" s="149" t="s">
+      <c r="D149" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E149" s="148" t="s">
+      <c r="E149" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F149" s="149" t="s">
+      <c r="F149" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="G149" s="149" t="s">
+      <c r="G149" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H149" s="68"/>
@@ -9423,13 +9429,13 @@
         <v>3069000000</v>
       </c>
       <c r="K149" s="70"/>
-      <c r="L149" s="149" t="s">
+      <c r="L149" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M149" s="149" t="s">
+      <c r="M149" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N149" s="149" t="s">
+      <c r="N149" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O149" s="9"/>
@@ -9441,22 +9447,22 @@
     </row>
     <row r="150" spans="1:20" ht="18" customHeight="1">
       <c r="A150" s="64"/>
-      <c r="B150" s="148" t="s">
+      <c r="B150" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C150" s="149" t="s">
+      <c r="C150" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D150" s="149" t="s">
+      <c r="D150" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E150" s="148" t="s">
+      <c r="E150" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F150" s="149" t="s">
+      <c r="F150" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="G150" s="149" t="s">
+      <c r="G150" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H150" s="68"/>
@@ -9467,13 +9473,13 @@
         <v>3184000000</v>
       </c>
       <c r="K150" s="70"/>
-      <c r="L150" s="149" t="s">
+      <c r="L150" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M150" s="149" t="s">
+      <c r="M150" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N150" s="149" t="s">
+      <c r="N150" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O150" s="9"/>
@@ -9485,22 +9491,22 @@
     </row>
     <row r="151" spans="1:20" ht="18" customHeight="1">
       <c r="A151" s="64"/>
-      <c r="B151" s="148" t="s">
+      <c r="B151" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C151" s="149" t="s">
+      <c r="C151" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D151" s="149" t="s">
+      <c r="D151" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E151" s="148" t="s">
+      <c r="E151" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F151" s="149" t="s">
+      <c r="F151" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G151" s="149" t="s">
+      <c r="G151" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H151" s="68"/>
@@ -9511,13 +9517,13 @@
         <v>1348000000</v>
       </c>
       <c r="K151" s="70"/>
-      <c r="L151" s="149" t="s">
+      <c r="L151" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M151" s="149" t="s">
+      <c r="M151" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N151" s="149" t="s">
+      <c r="N151" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O151" s="9"/>
@@ -9529,22 +9535,22 @@
     </row>
     <row r="152" spans="1:20" ht="18" customHeight="1">
       <c r="A152" s="64"/>
-      <c r="B152" s="148" t="s">
+      <c r="B152" s="111" t="s">
         <v>243</v>
       </c>
-      <c r="C152" s="149" t="s">
+      <c r="C152" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D152" s="149" t="s">
+      <c r="D152" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E152" s="148" t="s">
+      <c r="E152" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F152" s="149" t="s">
+      <c r="F152" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G152" s="149" t="s">
+      <c r="G152" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H152" s="68"/>
@@ -9555,13 +9561,13 @@
         <v>1413000000</v>
       </c>
       <c r="K152" s="70"/>
-      <c r="L152" s="149" t="s">
+      <c r="L152" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M152" s="149" t="s">
+      <c r="M152" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N152" s="149" t="s">
+      <c r="N152" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O152" s="9"/>
@@ -9573,22 +9579,22 @@
     </row>
     <row r="153" spans="1:20" ht="18" customHeight="1">
       <c r="A153" s="64"/>
-      <c r="B153" s="148" t="s">
+      <c r="B153" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C153" s="149" t="s">
+      <c r="C153" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D153" s="149" t="s">
+      <c r="D153" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E153" s="148" t="s">
+      <c r="E153" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F153" s="149" t="s">
+      <c r="F153" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G153" s="149" t="s">
+      <c r="G153" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H153" s="68"/>
@@ -9599,13 +9605,13 @@
         <v>1459000000</v>
       </c>
       <c r="K153" s="70"/>
-      <c r="L153" s="149" t="s">
+      <c r="L153" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M153" s="149" t="s">
+      <c r="M153" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N153" s="149" t="s">
+      <c r="N153" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O153" s="9"/>
@@ -9617,22 +9623,22 @@
     </row>
     <row r="154" spans="1:20" ht="18" customHeight="1">
       <c r="A154" s="64"/>
-      <c r="B154" s="148" t="s">
+      <c r="B154" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C154" s="149" t="s">
+      <c r="C154" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D154" s="149" t="s">
+      <c r="D154" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E154" s="148" t="s">
+      <c r="E154" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F154" s="149" t="s">
+      <c r="F154" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="G154" s="149" t="s">
+      <c r="G154" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H154" s="68"/>
@@ -9643,13 +9649,13 @@
         <v>33.9</v>
       </c>
       <c r="K154" s="70"/>
-      <c r="L154" s="149" t="s">
+      <c r="L154" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M154" s="149" t="s">
+      <c r="M154" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N154" s="149" t="s">
+      <c r="N154" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O154" s="9"/>
@@ -9661,22 +9667,22 @@
     </row>
     <row r="155" spans="1:20" ht="18" customHeight="1">
       <c r="A155" s="64"/>
-      <c r="B155" s="148" t="s">
+      <c r="B155" s="111" t="s">
         <v>243</v>
       </c>
-      <c r="C155" s="149" t="s">
+      <c r="C155" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D155" s="149" t="s">
+      <c r="D155" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E155" s="148" t="s">
+      <c r="E155" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F155" s="149" t="s">
+      <c r="F155" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="G155" s="149" t="s">
+      <c r="G155" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H155" s="68"/>
@@ -9687,13 +9693,13 @@
         <v>35.9</v>
       </c>
       <c r="K155" s="70"/>
-      <c r="L155" s="149" t="s">
+      <c r="L155" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M155" s="149" t="s">
+      <c r="M155" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N155" s="149" t="s">
+      <c r="N155" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O155" s="9"/>
@@ -9705,22 +9711,22 @@
     </row>
     <row r="156" spans="1:20" ht="18" customHeight="1">
       <c r="A156" s="64"/>
-      <c r="B156" s="148" t="s">
+      <c r="B156" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C156" s="149" t="s">
+      <c r="C156" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D156" s="149" t="s">
+      <c r="D156" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E156" s="148" t="s">
+      <c r="E156" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F156" s="149" t="s">
+      <c r="F156" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="G156" s="149" t="s">
+      <c r="G156" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H156" s="68"/>
@@ -9731,13 +9737,13 @@
         <v>36.6</v>
       </c>
       <c r="K156" s="70"/>
-      <c r="L156" s="149" t="s">
+      <c r="L156" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M156" s="149" t="s">
+      <c r="M156" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N156" s="149" t="s">
+      <c r="N156" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O156" s="9"/>
@@ -9749,39 +9755,39 @@
     </row>
     <row r="157" spans="1:20" ht="18" customHeight="1">
       <c r="A157" s="64"/>
-      <c r="B157" s="148" t="s">
+      <c r="B157" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C157" s="149" t="s">
+      <c r="C157" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D157" s="149" t="s">
+      <c r="D157" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E157" s="148" t="s">
+      <c r="E157" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F157" s="149" t="s">
+      <c r="F157" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="G157" s="149" t="s">
+      <c r="G157" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H157" s="68"/>
-      <c r="I157" s="152">
+      <c r="I157" s="115">
         <v>1173</v>
       </c>
       <c r="J157" s="70">
         <v>281000000</v>
       </c>
       <c r="K157" s="70"/>
-      <c r="L157" s="149" t="s">
+      <c r="L157" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M157" s="149" t="s">
+      <c r="M157" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N157" s="149" t="s">
+      <c r="N157" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O157" s="9"/>
@@ -9793,39 +9799,39 @@
     </row>
     <row r="158" spans="1:20" ht="18" customHeight="1">
       <c r="A158" s="64"/>
-      <c r="B158" s="148" t="s">
+      <c r="B158" s="111" t="s">
         <v>243</v>
       </c>
-      <c r="C158" s="149" t="s">
+      <c r="C158" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D158" s="149" t="s">
+      <c r="D158" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E158" s="148" t="s">
+      <c r="E158" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F158" s="149" t="s">
+      <c r="F158" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="G158" s="149" t="s">
+      <c r="G158" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H158" s="68"/>
-      <c r="I158" s="152">
+      <c r="I158" s="115">
         <v>1173</v>
       </c>
       <c r="J158" s="70">
         <v>255000000</v>
       </c>
       <c r="K158" s="70"/>
-      <c r="L158" s="149" t="s">
+      <c r="L158" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M158" s="149" t="s">
+      <c r="M158" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N158" s="149" t="s">
+      <c r="N158" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O158" s="9"/>
@@ -9837,39 +9843,39 @@
     </row>
     <row r="159" spans="1:20" ht="18" customHeight="1">
       <c r="A159" s="64"/>
-      <c r="B159" s="148" t="s">
+      <c r="B159" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C159" s="149" t="s">
+      <c r="C159" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D159" s="149" t="s">
+      <c r="D159" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E159" s="148" t="s">
+      <c r="E159" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F159" s="149" t="s">
+      <c r="F159" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="G159" s="149" t="s">
+      <c r="G159" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H159" s="68"/>
-      <c r="I159" s="152">
+      <c r="I159" s="115">
         <v>1173</v>
       </c>
       <c r="J159" s="70">
         <v>218000000</v>
       </c>
       <c r="K159" s="70"/>
-      <c r="L159" s="149" t="s">
+      <c r="L159" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M159" s="149" t="s">
+      <c r="M159" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N159" s="149" t="s">
+      <c r="N159" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O159" s="9"/>
@@ -9881,39 +9887,39 @@
     </row>
     <row r="160" spans="1:20" ht="18" customHeight="1">
       <c r="A160" s="64"/>
-      <c r="B160" s="148" t="s">
+      <c r="B160" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C160" s="149" t="s">
+      <c r="C160" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D160" s="149" t="s">
+      <c r="D160" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E160" s="148" t="s">
+      <c r="E160" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F160" s="149" t="s">
+      <c r="F160" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G160" s="149" t="s">
+      <c r="G160" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H160" s="68"/>
-      <c r="I160" s="152">
+      <c r="I160" s="115">
         <v>1173</v>
       </c>
       <c r="J160" s="70">
         <v>45</v>
       </c>
       <c r="K160" s="70"/>
-      <c r="L160" s="149" t="s">
+      <c r="L160" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M160" s="149" t="s">
+      <c r="M160" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N160" s="149" t="s">
+      <c r="N160" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O160" s="9"/>
@@ -9925,39 +9931,39 @@
     </row>
     <row r="161" spans="1:20" ht="18" customHeight="1">
       <c r="A161" s="64"/>
-      <c r="B161" s="148" t="s">
+      <c r="B161" s="111" t="s">
         <v>243</v>
       </c>
-      <c r="C161" s="149" t="s">
+      <c r="C161" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D161" s="149" t="s">
+      <c r="D161" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E161" s="148" t="s">
+      <c r="E161" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F161" s="149" t="s">
+      <c r="F161" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G161" s="149" t="s">
+      <c r="G161" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H161" s="68"/>
-      <c r="I161" s="152">
+      <c r="I161" s="115">
         <v>1173</v>
       </c>
       <c r="J161" s="70">
         <v>45</v>
       </c>
       <c r="K161" s="70"/>
-      <c r="L161" s="149" t="s">
+      <c r="L161" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M161" s="149" t="s">
+      <c r="M161" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N161" s="149" t="s">
+      <c r="N161" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O161" s="9"/>
@@ -9969,39 +9975,39 @@
     </row>
     <row r="162" spans="1:20" ht="18" customHeight="1">
       <c r="A162" s="64"/>
-      <c r="B162" s="148" t="s">
+      <c r="B162" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C162" s="149" t="s">
+      <c r="C162" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D162" s="149" t="s">
+      <c r="D162" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E162" s="148" t="s">
+      <c r="E162" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F162" s="149" t="s">
+      <c r="F162" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G162" s="149" t="s">
+      <c r="G162" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H162" s="68"/>
-      <c r="I162" s="152">
+      <c r="I162" s="115">
         <v>1173</v>
       </c>
       <c r="J162" s="70">
         <v>45</v>
       </c>
       <c r="K162" s="70"/>
-      <c r="L162" s="149" t="s">
+      <c r="L162" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M162" s="149" t="s">
+      <c r="M162" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N162" s="149" t="s">
+      <c r="N162" s="112" t="s">
         <v>242</v>
       </c>
       <c r="O162" s="9"/>
@@ -10013,22 +10019,22 @@
     </row>
     <row r="163" spans="1:20" ht="18" customHeight="1">
       <c r="A163" s="64"/>
-      <c r="B163" s="148" t="s">
+      <c r="B163" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C163" s="149" t="s">
+      <c r="C163" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D163" s="149" t="s">
+      <c r="D163" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E163" s="148" t="s">
+      <c r="E163" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F163" s="149" t="s">
+      <c r="F163" s="112" t="s">
         <v>248</v>
       </c>
-      <c r="G163" s="149" t="s">
+      <c r="G163" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H163" s="68"/>
@@ -10037,11 +10043,11 @@
         <v>1621</v>
       </c>
       <c r="K163" s="70"/>
-      <c r="L163" s="149" t="s">
+      <c r="L163" s="112" t="s">
         <v>249</v>
       </c>
       <c r="M163" s="68"/>
-      <c r="N163" s="149" t="s">
+      <c r="N163" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O163" s="9"/>
@@ -10053,22 +10059,22 @@
     </row>
     <row r="164" spans="1:20" ht="18" customHeight="1">
       <c r="A164" s="64"/>
-      <c r="B164" s="148" t="s">
+      <c r="B164" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C164" s="149" t="s">
+      <c r="C164" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D164" s="149" t="s">
+      <c r="D164" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E164" s="148" t="s">
+      <c r="E164" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F164" s="149" t="s">
+      <c r="F164" s="112" t="s">
         <v>250</v>
       </c>
-      <c r="G164" s="149" t="s">
+      <c r="G164" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H164" s="68"/>
@@ -10078,11 +10084,11 @@
         <v>1655</v>
       </c>
       <c r="K164" s="70"/>
-      <c r="L164" s="149" t="s">
+      <c r="L164" s="112" t="s">
         <v>249</v>
       </c>
       <c r="M164" s="68"/>
-      <c r="N164" s="149" t="s">
+      <c r="N164" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O164" s="9"/>
@@ -10094,22 +10100,22 @@
     </row>
     <row r="165" spans="1:20" ht="18" customHeight="1">
       <c r="A165" s="64"/>
-      <c r="B165" s="148" t="s">
+      <c r="B165" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C165" s="149" t="s">
+      <c r="C165" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D165" s="149" t="s">
+      <c r="D165" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E165" s="148" t="s">
+      <c r="E165" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F165" s="149" t="s">
+      <c r="F165" s="112" t="s">
         <v>251</v>
       </c>
-      <c r="G165" s="149" t="s">
+      <c r="G165" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H165" s="68"/>
@@ -10120,11 +10126,11 @@
         <v>5.4000000000000002E-7</v>
       </c>
       <c r="K165" s="70"/>
-      <c r="L165" s="149" t="s">
+      <c r="L165" s="112" t="s">
         <v>252</v>
       </c>
       <c r="M165" s="68"/>
-      <c r="N165" s="149" t="s">
+      <c r="N165" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O165" s="9"/>
@@ -10136,22 +10142,22 @@
     </row>
     <row r="166" spans="1:20" ht="18" customHeight="1">
       <c r="A166" s="64"/>
-      <c r="B166" s="148" t="s">
+      <c r="B166" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C166" s="149" t="s">
+      <c r="C166" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D166" s="149" t="s">
+      <c r="D166" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E166" s="148" t="s">
+      <c r="E166" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F166" s="149" t="s">
+      <c r="F166" s="112" t="s">
         <v>255</v>
       </c>
-      <c r="G166" s="149" t="s">
+      <c r="G166" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H166" s="68"/>
@@ -10162,13 +10168,13 @@
         <v>13.14</v>
       </c>
       <c r="K166" s="70"/>
-      <c r="L166" s="149" t="s">
+      <c r="L166" s="112" t="s">
         <v>253</v>
       </c>
-      <c r="M166" s="149" t="s">
+      <c r="M166" s="112" t="s">
         <v>254</v>
       </c>
-      <c r="N166" s="149" t="s">
+      <c r="N166" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O166" s="9"/>
@@ -10180,22 +10186,22 @@
     </row>
     <row r="167" spans="1:20" ht="18" customHeight="1">
       <c r="A167" s="64"/>
-      <c r="B167" s="148" t="s">
+      <c r="B167" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C167" s="149" t="s">
+      <c r="C167" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D167" s="149" t="s">
+      <c r="D167" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E167" s="148" t="s">
+      <c r="E167" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F167" s="149" t="s">
+      <c r="F167" s="112" t="s">
         <v>255</v>
       </c>
-      <c r="G167" s="149" t="s">
+      <c r="G167" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H167" s="68"/>
@@ -10206,13 +10212,13 @@
         <v>16.89</v>
       </c>
       <c r="K167" s="70"/>
-      <c r="L167" s="149" t="s">
+      <c r="L167" s="112" t="s">
         <v>253</v>
       </c>
-      <c r="M167" s="149" t="s">
+      <c r="M167" s="112" t="s">
         <v>254</v>
       </c>
-      <c r="N167" s="149" t="s">
+      <c r="N167" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O167" s="9"/>
@@ -10224,22 +10230,22 @@
     </row>
     <row r="168" spans="1:20" ht="18" customHeight="1">
       <c r="A168" s="64"/>
-      <c r="B168" s="148" t="s">
+      <c r="B168" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C168" s="149" t="s">
+      <c r="C168" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D168" s="149" t="s">
+      <c r="D168" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E168" s="148" t="s">
+      <c r="E168" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F168" s="149" t="s">
+      <c r="F168" s="112" t="s">
         <v>255</v>
       </c>
-      <c r="G168" s="149" t="s">
+      <c r="G168" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H168" s="68"/>
@@ -10250,13 +10256,13 @@
         <v>21.67</v>
       </c>
       <c r="K168" s="70"/>
-      <c r="L168" s="149" t="s">
+      <c r="L168" s="112" t="s">
         <v>253</v>
       </c>
-      <c r="M168" s="149" t="s">
+      <c r="M168" s="112" t="s">
         <v>254</v>
       </c>
-      <c r="N168" s="149" t="s">
+      <c r="N168" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O168" s="9"/>
@@ -10268,22 +10274,22 @@
     </row>
     <row r="169" spans="1:20" ht="18" customHeight="1">
       <c r="A169" s="64"/>
-      <c r="B169" s="148" t="s">
+      <c r="B169" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C169" s="149" t="s">
+      <c r="C169" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D169" s="149" t="s">
+      <c r="D169" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E169" s="148" t="s">
+      <c r="E169" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F169" s="149" t="s">
+      <c r="F169" s="112" t="s">
         <v>255</v>
       </c>
-      <c r="G169" s="149" t="s">
+      <c r="G169" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H169" s="68"/>
@@ -10294,13 +10300,13 @@
         <v>26.13</v>
       </c>
       <c r="K169" s="70"/>
-      <c r="L169" s="149" t="s">
+      <c r="L169" s="112" t="s">
         <v>253</v>
       </c>
-      <c r="M169" s="149" t="s">
+      <c r="M169" s="112" t="s">
         <v>254</v>
       </c>
-      <c r="N169" s="149" t="s">
+      <c r="N169" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O169" s="9"/>
@@ -10312,22 +10318,22 @@
     </row>
     <row r="170" spans="1:20" ht="18" customHeight="1">
       <c r="A170" s="64"/>
-      <c r="B170" s="148" t="s">
+      <c r="B170" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C170" s="149" t="s">
+      <c r="C170" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D170" s="149" t="s">
+      <c r="D170" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E170" s="148" t="s">
+      <c r="E170" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F170" s="149" t="s">
+      <c r="F170" s="112" t="s">
         <v>255</v>
       </c>
-      <c r="G170" s="149" t="s">
+      <c r="G170" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H170" s="68"/>
@@ -10338,13 +10344,13 @@
         <v>29.37</v>
       </c>
       <c r="K170" s="70"/>
-      <c r="L170" s="149" t="s">
+      <c r="L170" s="112" t="s">
         <v>253</v>
       </c>
-      <c r="M170" s="149" t="s">
+      <c r="M170" s="112" t="s">
         <v>254</v>
       </c>
-      <c r="N170" s="149" t="s">
+      <c r="N170" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O170" s="9"/>
@@ -10356,22 +10362,22 @@
     </row>
     <row r="171" spans="1:20" ht="18" customHeight="1">
       <c r="A171" s="64"/>
-      <c r="B171" s="148" t="s">
+      <c r="B171" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C171" s="149" t="s">
+      <c r="C171" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D171" s="149" t="s">
+      <c r="D171" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E171" s="148" t="s">
+      <c r="E171" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F171" s="149" t="s">
+      <c r="F171" s="112" t="s">
         <v>256</v>
       </c>
-      <c r="G171" s="149" t="s">
+      <c r="G171" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H171" s="68"/>
@@ -10382,13 +10388,13 @@
         <v>1.04E-5</v>
       </c>
       <c r="K171" s="70"/>
-      <c r="L171" s="149" t="s">
+      <c r="L171" s="112" t="s">
         <v>257</v>
       </c>
-      <c r="M171" s="149" t="s">
+      <c r="M171" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="N171" s="149" t="s">
+      <c r="N171" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O171" s="9"/>
@@ -10400,22 +10406,22 @@
     </row>
     <row r="172" spans="1:20" ht="18" customHeight="1">
       <c r="A172" s="64"/>
-      <c r="B172" s="148" t="s">
+      <c r="B172" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C172" s="149" t="s">
+      <c r="C172" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D172" s="149" t="s">
+      <c r="D172" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E172" s="148" t="s">
+      <c r="E172" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F172" s="149" t="s">
+      <c r="F172" s="112" t="s">
         <v>256</v>
       </c>
-      <c r="G172" s="149" t="s">
+      <c r="G172" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H172" s="68"/>
@@ -10426,13 +10432,13 @@
         <v>1.119E-5</v>
       </c>
       <c r="K172" s="70"/>
-      <c r="L172" s="149" t="s">
+      <c r="L172" s="112" t="s">
         <v>257</v>
       </c>
-      <c r="M172" s="149" t="s">
+      <c r="M172" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="N172" s="149" t="s">
+      <c r="N172" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O172" s="9"/>
@@ -10444,22 +10450,22 @@
     </row>
     <row r="173" spans="1:20" ht="18" customHeight="1">
       <c r="A173" s="64"/>
-      <c r="B173" s="148" t="s">
+      <c r="B173" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C173" s="149" t="s">
+      <c r="C173" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D173" s="149" t="s">
+      <c r="D173" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E173" s="148" t="s">
+      <c r="E173" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F173" s="149" t="s">
+      <c r="F173" s="112" t="s">
         <v>256</v>
       </c>
-      <c r="G173" s="149" t="s">
+      <c r="G173" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H173" s="68"/>
@@ -10470,13 +10476,13 @@
         <v>1.224E-5</v>
       </c>
       <c r="K173" s="70"/>
-      <c r="L173" s="149" t="s">
+      <c r="L173" s="112" t="s">
         <v>257</v>
       </c>
-      <c r="M173" s="149" t="s">
+      <c r="M173" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="N173" s="149" t="s">
+      <c r="N173" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O173" s="9"/>
@@ -10488,22 +10494,22 @@
     </row>
     <row r="174" spans="1:20" ht="18" customHeight="1">
       <c r="A174" s="64"/>
-      <c r="B174" s="148" t="s">
+      <c r="B174" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C174" s="149" t="s">
+      <c r="C174" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D174" s="149" t="s">
+      <c r="D174" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E174" s="148" t="s">
+      <c r="E174" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F174" s="149" t="s">
+      <c r="F174" s="112" t="s">
         <v>256</v>
       </c>
-      <c r="G174" s="149" t="s">
+      <c r="G174" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H174" s="68"/>
@@ -10514,13 +10520,13 @@
         <v>1.2619999999999999E-5</v>
       </c>
       <c r="K174" s="70"/>
-      <c r="L174" s="149" t="s">
+      <c r="L174" s="112" t="s">
         <v>257</v>
       </c>
-      <c r="M174" s="149" t="s">
+      <c r="M174" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="N174" s="149" t="s">
+      <c r="N174" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O174" s="9"/>
@@ -10532,22 +10538,22 @@
     </row>
     <row r="175" spans="1:20" ht="18" customHeight="1">
       <c r="A175" s="64"/>
-      <c r="B175" s="148" t="s">
+      <c r="B175" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C175" s="149" t="s">
+      <c r="C175" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D175" s="149" t="s">
+      <c r="D175" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E175" s="148" t="s">
+      <c r="E175" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F175" s="149" t="s">
+      <c r="F175" s="112" t="s">
         <v>256</v>
       </c>
-      <c r="G175" s="149" t="s">
+      <c r="G175" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H175" s="68"/>
@@ -10558,13 +10564,13 @@
         <v>1.2989999999999999E-5</v>
       </c>
       <c r="K175" s="70"/>
-      <c r="L175" s="149" t="s">
+      <c r="L175" s="112" t="s">
         <v>257</v>
       </c>
-      <c r="M175" s="149" t="s">
+      <c r="M175" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="N175" s="149" t="s">
+      <c r="N175" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O175" s="9"/>
@@ -10576,22 +10582,22 @@
     </row>
     <row r="176" spans="1:20" ht="18" customHeight="1">
       <c r="A176" s="64"/>
-      <c r="B176" s="148" t="s">
+      <c r="B176" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="C176" s="149" t="s">
+      <c r="C176" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="D176" s="149" t="s">
+      <c r="D176" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="E176" s="148" t="s">
+      <c r="E176" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="F176" s="149" t="s">
+      <c r="F176" s="112" t="s">
         <v>256</v>
       </c>
-      <c r="G176" s="149" t="s">
+      <c r="G176" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H176" s="68"/>
@@ -10602,13 +10608,13 @@
         <v>1.508E-5</v>
       </c>
       <c r="K176" s="70"/>
-      <c r="L176" s="149" t="s">
+      <c r="L176" s="112" t="s">
         <v>257</v>
       </c>
-      <c r="M176" s="149" t="s">
+      <c r="M176" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="N176" s="149" t="s">
+      <c r="N176" s="112" t="s">
         <v>258</v>
       </c>
       <c r="O176" s="9"/>
@@ -10619,28 +10625,28 @@
       <c r="T176" s="9"/>
     </row>
     <row r="177" spans="1:20" ht="18" customHeight="1">
-      <c r="A177" s="153" t="s">
+      <c r="A177" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B177" s="148" t="s">
+      <c r="B177" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C177" s="149" t="s">
+      <c r="C177" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D177" s="149" t="s">
+      <c r="D177" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E177" s="148" t="s">
+      <c r="E177" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F177" s="149" t="s">
+      <c r="F177" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="G177" s="149" t="s">
+      <c r="G177" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="H177" s="149" t="s">
+      <c r="H177" s="112" t="s">
         <v>265</v>
       </c>
       <c r="I177" s="83">
@@ -10650,13 +10656,13 @@
         <v>8900</v>
       </c>
       <c r="K177" s="70"/>
-      <c r="L177" s="149" t="s">
+      <c r="L177" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="M177" s="149" t="s">
+      <c r="M177" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="N177" s="149" t="s">
+      <c r="N177" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O177" s="9"/>
@@ -10667,28 +10673,28 @@
       <c r="T177" s="9"/>
     </row>
     <row r="178" spans="1:20" ht="18" customHeight="1">
-      <c r="A178" s="153" t="s">
+      <c r="A178" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B178" s="148" t="s">
+      <c r="B178" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C178" s="149" t="s">
+      <c r="C178" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D178" s="149" t="s">
+      <c r="D178" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E178" s="148" t="s">
+      <c r="E178" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F178" s="149" t="s">
+      <c r="F178" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="G178" s="149" t="s">
+      <c r="G178" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="H178" s="149" t="s">
+      <c r="H178" s="112" t="s">
         <v>265</v>
       </c>
       <c r="I178" s="83">
@@ -10698,13 +10704,13 @@
         <v>9460</v>
       </c>
       <c r="K178" s="70"/>
-      <c r="L178" s="149" t="s">
+      <c r="L178" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="M178" s="149" t="s">
+      <c r="M178" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="N178" s="149" t="s">
+      <c r="N178" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O178" s="9"/>
@@ -10715,28 +10721,28 @@
       <c r="T178" s="9"/>
     </row>
     <row r="179" spans="1:20" ht="18" customHeight="1">
-      <c r="A179" s="153" t="s">
+      <c r="A179" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B179" s="148" t="s">
+      <c r="B179" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C179" s="149" t="s">
+      <c r="C179" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D179" s="149" t="s">
+      <c r="D179" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E179" s="148" t="s">
+      <c r="E179" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F179" s="149" t="s">
+      <c r="F179" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="G179" s="149" t="s">
+      <c r="G179" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="H179" s="149" t="s">
+      <c r="H179" s="112" t="s">
         <v>265</v>
       </c>
       <c r="I179" s="83">
@@ -10746,13 +10752,13 @@
         <v>9460</v>
       </c>
       <c r="K179" s="70"/>
-      <c r="L179" s="149" t="s">
+      <c r="L179" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="M179" s="149" t="s">
+      <c r="M179" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="N179" s="149" t="s">
+      <c r="N179" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O179" s="9"/>
@@ -10763,25 +10769,25 @@
       <c r="T179" s="9"/>
     </row>
     <row r="180" spans="1:20" ht="18" customHeight="1">
-      <c r="A180" s="153" t="s">
+      <c r="A180" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B180" s="148" t="s">
+      <c r="B180" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C180" s="149" t="s">
+      <c r="C180" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D180" s="149" t="s">
+      <c r="D180" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E180" s="148" t="s">
+      <c r="E180" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F180" s="149" t="s">
+      <c r="F180" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G180" s="149" t="s">
+      <c r="G180" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H180" s="68"/>
@@ -10792,13 +10798,13 @@
         <v>874000000</v>
       </c>
       <c r="K180" s="70"/>
-      <c r="L180" s="149" t="s">
+      <c r="L180" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M180" s="149" t="s">
+      <c r="M180" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N180" s="149" t="s">
+      <c r="N180" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O180" s="9"/>
@@ -10809,25 +10815,25 @@
       <c r="T180" s="9"/>
     </row>
     <row r="181" spans="1:20" ht="18" customHeight="1">
-      <c r="A181" s="153" t="s">
+      <c r="A181" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B181" s="148" t="s">
+      <c r="B181" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C181" s="149" t="s">
+      <c r="C181" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D181" s="149" t="s">
+      <c r="D181" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E181" s="148" t="s">
+      <c r="E181" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F181" s="149" t="s">
+      <c r="F181" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G181" s="149" t="s">
+      <c r="G181" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H181" s="68"/>
@@ -10838,13 +10844,13 @@
         <v>1000000000</v>
       </c>
       <c r="K181" s="70"/>
-      <c r="L181" s="149" t="s">
+      <c r="L181" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M181" s="149" t="s">
+      <c r="M181" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N181" s="149" t="s">
+      <c r="N181" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O181" s="9"/>
@@ -10855,25 +10861,25 @@
       <c r="T181" s="9"/>
     </row>
     <row r="182" spans="1:20" ht="18" customHeight="1">
-      <c r="A182" s="153" t="s">
+      <c r="A182" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B182" s="148" t="s">
+      <c r="B182" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C182" s="149" t="s">
+      <c r="C182" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D182" s="149" t="s">
+      <c r="D182" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E182" s="148" t="s">
+      <c r="E182" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F182" s="149" t="s">
+      <c r="F182" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G182" s="149" t="s">
+      <c r="G182" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H182" s="68"/>
@@ -10884,13 +10890,13 @@
         <v>924000000</v>
       </c>
       <c r="K182" s="70"/>
-      <c r="L182" s="149" t="s">
+      <c r="L182" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M182" s="149" t="s">
+      <c r="M182" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N182" s="149" t="s">
+      <c r="N182" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O182" s="9"/>
@@ -10901,25 +10907,25 @@
       <c r="T182" s="9"/>
     </row>
     <row r="183" spans="1:20" ht="18" customHeight="1">
-      <c r="A183" s="153" t="s">
+      <c r="A183" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B183" s="148" t="s">
+      <c r="B183" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C183" s="149" t="s">
+      <c r="C183" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D183" s="149" t="s">
+      <c r="D183" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E183" s="148" t="s">
+      <c r="E183" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F183" s="149" t="s">
+      <c r="F183" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G183" s="149" t="s">
+      <c r="G183" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H183" s="68"/>
@@ -10930,13 +10936,13 @@
         <v>430000000</v>
       </c>
       <c r="K183" s="70"/>
-      <c r="L183" s="149" t="s">
+      <c r="L183" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M183" s="149" t="s">
+      <c r="M183" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N183" s="149" t="s">
+      <c r="N183" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O183" s="9"/>
@@ -10947,25 +10953,25 @@
       <c r="T183" s="9"/>
     </row>
     <row r="184" spans="1:20" ht="18" customHeight="1">
-      <c r="A184" s="153" t="s">
+      <c r="A184" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B184" s="148" t="s">
+      <c r="B184" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C184" s="149" t="s">
+      <c r="C184" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D184" s="149" t="s">
+      <c r="D184" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E184" s="148" t="s">
+      <c r="E184" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F184" s="149" t="s">
+      <c r="F184" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G184" s="149" t="s">
+      <c r="G184" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H184" s="68"/>
@@ -10976,13 +10982,13 @@
         <v>520000000</v>
       </c>
       <c r="K184" s="70"/>
-      <c r="L184" s="149" t="s">
+      <c r="L184" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M184" s="149" t="s">
+      <c r="M184" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N184" s="149" t="s">
+      <c r="N184" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O184" s="9"/>
@@ -10993,25 +10999,25 @@
       <c r="T184" s="9"/>
     </row>
     <row r="185" spans="1:20" ht="18" customHeight="1">
-      <c r="A185" s="153" t="s">
+      <c r="A185" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B185" s="148" t="s">
+      <c r="B185" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C185" s="149" t="s">
+      <c r="C185" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D185" s="149" t="s">
+      <c r="D185" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E185" s="148" t="s">
+      <c r="E185" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F185" s="149" t="s">
+      <c r="F185" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G185" s="149" t="s">
+      <c r="G185" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H185" s="68"/>
@@ -11022,13 +11028,13 @@
         <v>604000000</v>
       </c>
       <c r="K185" s="70"/>
-      <c r="L185" s="149" t="s">
+      <c r="L185" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M185" s="149" t="s">
+      <c r="M185" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N185" s="149" t="s">
+      <c r="N185" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O185" s="9"/>
@@ -11039,25 +11045,25 @@
       <c r="T185" s="9"/>
     </row>
     <row r="186" spans="1:20" ht="18" customHeight="1">
-      <c r="A186" s="153" t="s">
+      <c r="A186" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B186" s="148" t="s">
+      <c r="B186" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C186" s="149" t="s">
+      <c r="C186" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D186" s="149" t="s">
+      <c r="D186" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E186" s="148" t="s">
+      <c r="E186" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F186" s="149" t="s">
+      <c r="F186" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G186" s="149" t="s">
+      <c r="G186" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H186" s="68"/>
@@ -11068,13 +11074,13 @@
         <v>404000000</v>
       </c>
       <c r="K186" s="70"/>
-      <c r="L186" s="149" t="s">
+      <c r="L186" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M186" s="149" t="s">
+      <c r="M186" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N186" s="149" t="s">
+      <c r="N186" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O186" s="9"/>
@@ -11085,25 +11091,25 @@
       <c r="T186" s="9"/>
     </row>
     <row r="187" spans="1:20" ht="18" customHeight="1">
-      <c r="A187" s="153" t="s">
+      <c r="A187" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B187" s="148" t="s">
+      <c r="B187" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C187" s="149" t="s">
+      <c r="C187" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D187" s="149" t="s">
+      <c r="D187" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E187" s="148" t="s">
+      <c r="E187" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F187" s="149" t="s">
+      <c r="F187" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G187" s="149" t="s">
+      <c r="G187" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H187" s="68"/>
@@ -11114,13 +11120,13 @@
         <v>455000000</v>
       </c>
       <c r="K187" s="70"/>
-      <c r="L187" s="149" t="s">
+      <c r="L187" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M187" s="149" t="s">
+      <c r="M187" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N187" s="149" t="s">
+      <c r="N187" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O187" s="9"/>
@@ -11131,25 +11137,25 @@
       <c r="T187" s="9"/>
     </row>
     <row r="188" spans="1:20" ht="18" customHeight="1">
-      <c r="A188" s="153" t="s">
+      <c r="A188" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B188" s="148" t="s">
+      <c r="B188" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C188" s="149" t="s">
+      <c r="C188" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D188" s="149" t="s">
+      <c r="D188" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E188" s="148" t="s">
+      <c r="E188" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F188" s="149" t="s">
+      <c r="F188" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G188" s="149" t="s">
+      <c r="G188" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H188" s="68"/>
@@ -11160,13 +11166,13 @@
         <v>513000000</v>
       </c>
       <c r="K188" s="70"/>
-      <c r="L188" s="149" t="s">
+      <c r="L188" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M188" s="149" t="s">
+      <c r="M188" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N188" s="149" t="s">
+      <c r="N188" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O188" s="9"/>
@@ -11177,25 +11183,25 @@
       <c r="T188" s="9"/>
     </row>
     <row r="189" spans="1:20" ht="18" customHeight="1">
-      <c r="A189" s="153" t="s">
+      <c r="A189" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B189" s="148" t="s">
+      <c r="B189" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C189" s="149" t="s">
+      <c r="C189" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D189" s="149" t="s">
+      <c r="D189" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E189" s="148" t="s">
+      <c r="E189" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F189" s="149" t="s">
+      <c r="F189" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G189" s="149" t="s">
+      <c r="G189" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H189" s="68"/>
@@ -11206,13 +11212,13 @@
         <v>353000000</v>
       </c>
       <c r="K189" s="70"/>
-      <c r="L189" s="149" t="s">
+      <c r="L189" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M189" s="149" t="s">
+      <c r="M189" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N189" s="149" t="s">
+      <c r="N189" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O189" s="9"/>
@@ -11223,25 +11229,25 @@
       <c r="T189" s="9"/>
     </row>
     <row r="190" spans="1:20" ht="18" customHeight="1">
-      <c r="A190" s="153" t="s">
+      <c r="A190" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B190" s="148" t="s">
+      <c r="B190" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C190" s="149" t="s">
+      <c r="C190" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D190" s="149" t="s">
+      <c r="D190" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E190" s="148" t="s">
+      <c r="E190" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F190" s="149" t="s">
+      <c r="F190" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G190" s="149" t="s">
+      <c r="G190" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H190" s="68"/>
@@ -11252,13 +11258,13 @@
         <v>412000000</v>
       </c>
       <c r="K190" s="70"/>
-      <c r="L190" s="149" t="s">
+      <c r="L190" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M190" s="149" t="s">
+      <c r="M190" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N190" s="149" t="s">
+      <c r="N190" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O190" s="9"/>
@@ -11269,25 +11275,25 @@
       <c r="T190" s="9"/>
     </row>
     <row r="191" spans="1:20" ht="18" customHeight="1">
-      <c r="A191" s="153" t="s">
+      <c r="A191" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B191" s="148" t="s">
+      <c r="B191" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C191" s="149" t="s">
+      <c r="C191" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D191" s="149" t="s">
+      <c r="D191" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E191" s="148" t="s">
+      <c r="E191" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F191" s="149" t="s">
+      <c r="F191" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G191" s="149" t="s">
+      <c r="G191" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H191" s="68"/>
@@ -11298,13 +11304,13 @@
         <v>452000000</v>
       </c>
       <c r="K191" s="70"/>
-      <c r="L191" s="149" t="s">
+      <c r="L191" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M191" s="149" t="s">
+      <c r="M191" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N191" s="149" t="s">
+      <c r="N191" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O191" s="9"/>
@@ -11315,25 +11321,25 @@
       <c r="T191" s="9"/>
     </row>
     <row r="192" spans="1:20" ht="18" customHeight="1">
-      <c r="A192" s="153" t="s">
+      <c r="A192" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B192" s="148" t="s">
+      <c r="B192" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C192" s="149" t="s">
+      <c r="C192" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D192" s="149" t="s">
+      <c r="D192" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E192" s="148" t="s">
+      <c r="E192" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F192" s="149" t="s">
+      <c r="F192" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G192" s="149" t="s">
+      <c r="G192" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H192" s="68"/>
@@ -11344,13 +11350,13 @@
         <v>202000000</v>
       </c>
       <c r="K192" s="70"/>
-      <c r="L192" s="149" t="s">
+      <c r="L192" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M192" s="149" t="s">
+      <c r="M192" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N192" s="149" t="s">
+      <c r="N192" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O192" s="9"/>
@@ -11361,25 +11367,25 @@
       <c r="T192" s="9"/>
     </row>
     <row r="193" spans="1:20" ht="18" customHeight="1">
-      <c r="A193" s="153" t="s">
+      <c r="A193" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B193" s="148" t="s">
+      <c r="B193" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C193" s="149" t="s">
+      <c r="C193" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D193" s="149" t="s">
+      <c r="D193" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E193" s="148" t="s">
+      <c r="E193" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F193" s="149" t="s">
+      <c r="F193" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G193" s="149" t="s">
+      <c r="G193" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H193" s="68"/>
@@ -11390,13 +11396,13 @@
         <v>337000000</v>
       </c>
       <c r="K193" s="70"/>
-      <c r="L193" s="149" t="s">
+      <c r="L193" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M193" s="149" t="s">
+      <c r="M193" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N193" s="149" t="s">
+      <c r="N193" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O193" s="9"/>
@@ -11407,25 +11413,25 @@
       <c r="T193" s="9"/>
     </row>
     <row r="194" spans="1:20" ht="18" customHeight="1">
-      <c r="A194" s="153" t="s">
+      <c r="A194" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B194" s="148" t="s">
+      <c r="B194" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C194" s="149" t="s">
+      <c r="C194" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D194" s="149" t="s">
+      <c r="D194" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E194" s="148" t="s">
+      <c r="E194" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F194" s="149" t="s">
+      <c r="F194" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G194" s="149" t="s">
+      <c r="G194" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H194" s="68"/>
@@ -11436,13 +11442,13 @@
         <v>373000000</v>
       </c>
       <c r="K194" s="70"/>
-      <c r="L194" s="149" t="s">
+      <c r="L194" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="M194" s="149" t="s">
+      <c r="M194" s="112" t="s">
         <v>245</v>
       </c>
-      <c r="N194" s="149" t="s">
+      <c r="N194" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O194" s="9"/>
@@ -11453,25 +11459,25 @@
       <c r="T194" s="9"/>
     </row>
     <row r="195" spans="1:20" ht="18" customHeight="1">
-      <c r="A195" s="153" t="s">
+      <c r="A195" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B195" s="148" t="s">
+      <c r="B195" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C195" s="149" t="s">
+      <c r="C195" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D195" s="149" t="s">
+      <c r="D195" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E195" s="148" t="s">
+      <c r="E195" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F195" s="149" t="s">
+      <c r="F195" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="G195" s="149" t="s">
+      <c r="G195" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H195" s="68"/>
@@ -11482,13 +11488,13 @@
         <v>59</v>
       </c>
       <c r="K195" s="70"/>
-      <c r="L195" s="149" t="s">
+      <c r="L195" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M195" s="149" t="s">
+      <c r="M195" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N195" s="149" t="s">
+      <c r="N195" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O195" s="9"/>
@@ -11499,25 +11505,25 @@
       <c r="T195" s="9"/>
     </row>
     <row r="196" spans="1:20" ht="18" customHeight="1">
-      <c r="A196" s="153" t="s">
+      <c r="A196" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B196" s="148" t="s">
+      <c r="B196" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C196" s="149" t="s">
+      <c r="C196" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D196" s="149" t="s">
+      <c r="D196" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E196" s="148" t="s">
+      <c r="E196" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F196" s="149" t="s">
+      <c r="F196" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="G196" s="149" t="s">
+      <c r="G196" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H196" s="68"/>
@@ -11528,13 +11534,13 @@
         <v>26</v>
       </c>
       <c r="K196" s="70"/>
-      <c r="L196" s="149" t="s">
+      <c r="L196" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M196" s="149" t="s">
+      <c r="M196" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N196" s="149" t="s">
+      <c r="N196" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O196" s="9"/>
@@ -11545,25 +11551,25 @@
       <c r="T196" s="9"/>
     </row>
     <row r="197" spans="1:20" ht="18" customHeight="1">
-      <c r="A197" s="153" t="s">
+      <c r="A197" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B197" s="148" t="s">
+      <c r="B197" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C197" s="149" t="s">
+      <c r="C197" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D197" s="149" t="s">
+      <c r="D197" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E197" s="148" t="s">
+      <c r="E197" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F197" s="149" t="s">
+      <c r="F197" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="G197" s="149" t="s">
+      <c r="G197" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H197" s="68"/>
@@ -11574,13 +11580,13 @@
         <v>18</v>
       </c>
       <c r="K197" s="70"/>
-      <c r="L197" s="149" t="s">
+      <c r="L197" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M197" s="149" t="s">
+      <c r="M197" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N197" s="149" t="s">
+      <c r="N197" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O197" s="9"/>
@@ -11591,25 +11597,25 @@
       <c r="T197" s="9"/>
     </row>
     <row r="198" spans="1:20" ht="18" customHeight="1">
-      <c r="A198" s="153" t="s">
+      <c r="A198" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B198" s="148" t="s">
+      <c r="B198" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C198" s="149" t="s">
+      <c r="C198" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D198" s="149" t="s">
+      <c r="D198" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E198" s="148" t="s">
+      <c r="E198" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F198" s="149" t="s">
+      <c r="F198" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G198" s="149" t="s">
+      <c r="G198" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H198" s="68"/>
@@ -11620,13 +11626,13 @@
         <v>50</v>
       </c>
       <c r="K198" s="70"/>
-      <c r="L198" s="149" t="s">
+      <c r="L198" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M198" s="149" t="s">
+      <c r="M198" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N198" s="149" t="s">
+      <c r="N198" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O198" s="9"/>
@@ -11637,25 +11643,25 @@
       <c r="T198" s="9"/>
     </row>
     <row r="199" spans="1:20" ht="18" customHeight="1">
-      <c r="A199" s="153" t="s">
+      <c r="A199" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B199" s="148" t="s">
+      <c r="B199" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C199" s="149" t="s">
+      <c r="C199" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D199" s="149" t="s">
+      <c r="D199" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E199" s="148" t="s">
+      <c r="E199" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F199" s="149" t="s">
+      <c r="F199" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G199" s="149" t="s">
+      <c r="G199" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H199" s="68"/>
@@ -11666,13 +11672,13 @@
         <v>50</v>
       </c>
       <c r="K199" s="70"/>
-      <c r="L199" s="149" t="s">
+      <c r="L199" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M199" s="149" t="s">
+      <c r="M199" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N199" s="149" t="s">
+      <c r="N199" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O199" s="9"/>
@@ -11683,25 +11689,25 @@
       <c r="T199" s="9"/>
     </row>
     <row r="200" spans="1:20" ht="18" customHeight="1">
-      <c r="A200" s="153" t="s">
+      <c r="A200" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B200" s="148" t="s">
+      <c r="B200" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C200" s="149" t="s">
+      <c r="C200" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D200" s="149" t="s">
+      <c r="D200" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E200" s="148" t="s">
+      <c r="E200" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F200" s="149" t="s">
+      <c r="F200" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G200" s="149" t="s">
+      <c r="G200" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H200" s="68"/>
@@ -11712,13 +11718,13 @@
         <v>50</v>
       </c>
       <c r="K200" s="70"/>
-      <c r="L200" s="149" t="s">
+      <c r="L200" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M200" s="149" t="s">
+      <c r="M200" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N200" s="149" t="s">
+      <c r="N200" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O200" s="9"/>
@@ -11729,25 +11735,25 @@
       <c r="T200" s="9"/>
     </row>
     <row r="201" spans="1:20" ht="18" customHeight="1">
-      <c r="A201" s="153" t="s">
+      <c r="A201" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B201" s="148" t="s">
+      <c r="B201" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C201" s="149" t="s">
+      <c r="C201" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D201" s="149" t="s">
+      <c r="D201" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E201" s="148" t="s">
+      <c r="E201" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F201" s="149" t="s">
+      <c r="F201" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G201" s="149" t="s">
+      <c r="G201" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H201" s="68"/>
@@ -11758,13 +11764,13 @@
         <v>50</v>
       </c>
       <c r="K201" s="70"/>
-      <c r="L201" s="149" t="s">
+      <c r="L201" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M201" s="149" t="s">
+      <c r="M201" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N201" s="149" t="s">
+      <c r="N201" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O201" s="9"/>
@@ -11775,25 +11781,25 @@
       <c r="T201" s="9"/>
     </row>
     <row r="202" spans="1:20" ht="18" customHeight="1">
-      <c r="A202" s="153" t="s">
+      <c r="A202" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B202" s="148" t="s">
+      <c r="B202" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C202" s="149" t="s">
+      <c r="C202" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D202" s="149" t="s">
+      <c r="D202" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E202" s="148" t="s">
+      <c r="E202" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F202" s="149" t="s">
+      <c r="F202" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G202" s="149" t="s">
+      <c r="G202" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H202" s="68"/>
@@ -11804,13 +11810,13 @@
         <v>50</v>
       </c>
       <c r="K202" s="70"/>
-      <c r="L202" s="149" t="s">
+      <c r="L202" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M202" s="149" t="s">
+      <c r="M202" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N202" s="149" t="s">
+      <c r="N202" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O202" s="9"/>
@@ -11821,25 +11827,25 @@
       <c r="T202" s="9"/>
     </row>
     <row r="203" spans="1:20" ht="18" customHeight="1">
-      <c r="A203" s="153" t="s">
+      <c r="A203" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B203" s="148" t="s">
+      <c r="B203" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C203" s="149" t="s">
+      <c r="C203" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D203" s="149" t="s">
+      <c r="D203" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E203" s="148" t="s">
+      <c r="E203" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F203" s="149" t="s">
+      <c r="F203" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G203" s="149" t="s">
+      <c r="G203" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H203" s="68"/>
@@ -11850,13 +11856,13 @@
         <v>50</v>
       </c>
       <c r="K203" s="70"/>
-      <c r="L203" s="149" t="s">
+      <c r="L203" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M203" s="149" t="s">
+      <c r="M203" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N203" s="149" t="s">
+      <c r="N203" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O203" s="9"/>
@@ -11867,25 +11873,25 @@
       <c r="T203" s="9"/>
     </row>
     <row r="204" spans="1:20" ht="18" customHeight="1">
-      <c r="A204" s="153" t="s">
+      <c r="A204" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B204" s="148" t="s">
+      <c r="B204" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C204" s="149" t="s">
+      <c r="C204" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D204" s="149" t="s">
+      <c r="D204" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E204" s="148" t="s">
+      <c r="E204" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F204" s="149" t="s">
+      <c r="F204" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G204" s="149" t="s">
+      <c r="G204" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H204" s="68"/>
@@ -11896,13 +11902,13 @@
         <v>50</v>
       </c>
       <c r="K204" s="70"/>
-      <c r="L204" s="149" t="s">
+      <c r="L204" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M204" s="149" t="s">
+      <c r="M204" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N204" s="149" t="s">
+      <c r="N204" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O204" s="9"/>
@@ -11913,25 +11919,25 @@
       <c r="T204" s="9"/>
     </row>
     <row r="205" spans="1:20" ht="18" customHeight="1">
-      <c r="A205" s="153" t="s">
+      <c r="A205" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B205" s="148" t="s">
+      <c r="B205" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C205" s="149" t="s">
+      <c r="C205" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D205" s="149" t="s">
+      <c r="D205" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E205" s="148" t="s">
+      <c r="E205" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F205" s="149" t="s">
+      <c r="F205" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G205" s="149" t="s">
+      <c r="G205" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H205" s="68"/>
@@ -11942,13 +11948,13 @@
         <v>50</v>
       </c>
       <c r="K205" s="70"/>
-      <c r="L205" s="149" t="s">
+      <c r="L205" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M205" s="149" t="s">
+      <c r="M205" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N205" s="149" t="s">
+      <c r="N205" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O205" s="9"/>
@@ -11959,25 +11965,25 @@
       <c r="T205" s="9"/>
     </row>
     <row r="206" spans="1:20" ht="18" customHeight="1">
-      <c r="A206" s="153" t="s">
+      <c r="A206" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B206" s="148" t="s">
+      <c r="B206" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C206" s="149" t="s">
+      <c r="C206" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D206" s="149" t="s">
+      <c r="D206" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E206" s="148" t="s">
+      <c r="E206" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F206" s="149" t="s">
+      <c r="F206" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G206" s="149" t="s">
+      <c r="G206" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H206" s="68"/>
@@ -11988,13 +11994,13 @@
         <v>50</v>
       </c>
       <c r="K206" s="70"/>
-      <c r="L206" s="149" t="s">
+      <c r="L206" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M206" s="149" t="s">
+      <c r="M206" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N206" s="149" t="s">
+      <c r="N206" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O206" s="9"/>
@@ -12005,25 +12011,25 @@
       <c r="T206" s="9"/>
     </row>
     <row r="207" spans="1:20" ht="18" customHeight="1">
-      <c r="A207" s="153" t="s">
+      <c r="A207" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="B207" s="148" t="s">
+      <c r="B207" s="111" t="s">
         <v>259</v>
       </c>
-      <c r="C207" s="149" t="s">
+      <c r="C207" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D207" s="149" t="s">
+      <c r="D207" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E207" s="148" t="s">
+      <c r="E207" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F207" s="149" t="s">
+      <c r="F207" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G207" s="149" t="s">
+      <c r="G207" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H207" s="68"/>
@@ -12034,13 +12040,13 @@
         <v>50</v>
       </c>
       <c r="K207" s="70"/>
-      <c r="L207" s="149" t="s">
+      <c r="L207" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M207" s="149" t="s">
+      <c r="M207" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N207" s="149" t="s">
+      <c r="N207" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O207" s="9"/>
@@ -12051,25 +12057,25 @@
       <c r="T207" s="9"/>
     </row>
     <row r="208" spans="1:20" ht="18" customHeight="1">
-      <c r="A208" s="153" t="s">
+      <c r="A208" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B208" s="148" t="s">
+      <c r="B208" s="111" t="s">
         <v>263</v>
       </c>
-      <c r="C208" s="149" t="s">
+      <c r="C208" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D208" s="149" t="s">
+      <c r="D208" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E208" s="148" t="s">
+      <c r="E208" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F208" s="149" t="s">
+      <c r="F208" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G208" s="149" t="s">
+      <c r="G208" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H208" s="68"/>
@@ -12080,13 +12086,13 @@
         <v>50</v>
       </c>
       <c r="K208" s="70"/>
-      <c r="L208" s="149" t="s">
+      <c r="L208" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M208" s="149" t="s">
+      <c r="M208" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N208" s="149" t="s">
+      <c r="N208" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O208" s="9"/>
@@ -12097,25 +12103,25 @@
       <c r="T208" s="9"/>
     </row>
     <row r="209" spans="1:20" ht="18" customHeight="1">
-      <c r="A209" s="153" t="s">
+      <c r="A209" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="B209" s="148" t="s">
+      <c r="B209" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="C209" s="149" t="s">
+      <c r="C209" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="D209" s="149" t="s">
+      <c r="D209" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="E209" s="148" t="s">
+      <c r="E209" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="F209" s="149" t="s">
+      <c r="F209" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="G209" s="149" t="s">
+      <c r="G209" s="112" t="s">
         <v>29</v>
       </c>
       <c r="H209" s="68"/>
@@ -12126,13 +12132,13 @@
         <v>50</v>
       </c>
       <c r="K209" s="4"/>
-      <c r="L209" s="149" t="s">
+      <c r="L209" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="M209" s="149" t="s">
+      <c r="M209" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="N209" s="149" t="s">
+      <c r="N209" s="112" t="s">
         <v>268</v>
       </c>
       <c r="O209" s="9"/>
@@ -12144,9 +12150,15 @@
     </row>
     <row r="210" spans="1:20" ht="18" customHeight="1">
       <c r="A210" s="64"/>
-      <c r="B210" s="73"/>
-      <c r="C210" s="68"/>
-      <c r="D210" s="68"/>
+      <c r="B210" s="111" t="s">
+        <v>270</v>
+      </c>
+      <c r="C210" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D210" s="112" t="s">
+        <v>238</v>
+      </c>
       <c r="E210" s="73"/>
       <c r="F210" s="68"/>
       <c r="G210" s="68"/>
@@ -12156,7 +12168,9 @@
       <c r="K210" s="70"/>
       <c r="L210" s="68"/>
       <c r="M210" s="68"/>
-      <c r="N210" s="68"/>
+      <c r="N210" s="112" t="s">
+        <v>269</v>
+      </c>
       <c r="O210" s="9"/>
       <c r="P210" s="4"/>
       <c r="Q210" s="4"/>
@@ -26444,11 +26458,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -26463,6 +26472,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.jallcom.2012.12.095`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B949C8-FAAF-FF4C-A680-AD27D7C9DFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78CB0BA-BAC8-CA46-BB2C-EF2E843DF6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="760" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="278">
   <si>
     <r>
       <rPr>
@@ -933,6 +933,27 @@
   </si>
   <si>
     <t>CrMoNbReTaVW</t>
+  </si>
+  <si>
+    <t>6C</t>
+  </si>
+  <si>
+    <t>7C</t>
+  </si>
+  <si>
+    <t>8C</t>
+  </si>
+  <si>
+    <t>AlCoCrCuFeNiW</t>
+  </si>
+  <si>
+    <t>AlCoCrCuFeNiWZr</t>
+  </si>
+  <si>
+    <t>mechanical alloying through high energy ball milling for 60h</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2012.12.095</t>
   </si>
 </sst>
 </file>
@@ -3260,8 +3281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E184" zoomScale="86" workbookViewId="0">
-      <selection activeCell="H194" sqref="H194"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A187" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N218" sqref="N218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -12179,11 +12200,21 @@
       <c r="T210" s="9"/>
     </row>
     <row r="211" spans="1:20" ht="18" customHeight="1">
-      <c r="A211" s="64"/>
-      <c r="B211" s="73"/>
-      <c r="C211" s="68"/>
-      <c r="D211" s="68"/>
-      <c r="E211" s="73"/>
+      <c r="A211" s="116" t="s">
+        <v>271</v>
+      </c>
+      <c r="B211" s="111" t="s">
+        <v>101</v>
+      </c>
+      <c r="C211" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D211" s="112" t="s">
+        <v>173</v>
+      </c>
+      <c r="E211" s="111" t="s">
+        <v>276</v>
+      </c>
       <c r="F211" s="68"/>
       <c r="G211" s="68"/>
       <c r="H211" s="68"/>
@@ -12192,7 +12223,9 @@
       <c r="K211" s="70"/>
       <c r="L211" s="68"/>
       <c r="M211" s="68"/>
-      <c r="N211" s="68"/>
+      <c r="N211" s="112" t="s">
+        <v>277</v>
+      </c>
       <c r="O211" s="9"/>
       <c r="P211" s="4"/>
       <c r="Q211" s="4"/>
@@ -12201,11 +12234,21 @@
       <c r="T211" s="9"/>
     </row>
     <row r="212" spans="1:20" ht="18" customHeight="1">
-      <c r="A212" s="64"/>
-      <c r="B212" s="73"/>
-      <c r="C212" s="68"/>
-      <c r="D212" s="68"/>
-      <c r="E212" s="73"/>
+      <c r="A212" s="116" t="s">
+        <v>272</v>
+      </c>
+      <c r="B212" s="111" t="s">
+        <v>274</v>
+      </c>
+      <c r="C212" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D212" s="112" t="s">
+        <v>173</v>
+      </c>
+      <c r="E212" s="111" t="s">
+        <v>276</v>
+      </c>
       <c r="F212" s="68"/>
       <c r="G212" s="68"/>
       <c r="H212" s="68"/>
@@ -12214,7 +12257,9 @@
       <c r="K212" s="70"/>
       <c r="L212" s="68"/>
       <c r="M212" s="68"/>
-      <c r="N212" s="68"/>
+      <c r="N212" s="112" t="s">
+        <v>277</v>
+      </c>
       <c r="O212" s="9"/>
       <c r="P212" s="4"/>
       <c r="Q212" s="4"/>
@@ -12223,11 +12268,21 @@
       <c r="T212" s="9"/>
     </row>
     <row r="213" spans="1:20" ht="18" customHeight="1">
-      <c r="A213" s="64"/>
-      <c r="B213" s="73"/>
-      <c r="C213" s="68"/>
-      <c r="D213" s="68"/>
-      <c r="E213" s="73"/>
+      <c r="A213" s="116" t="s">
+        <v>273</v>
+      </c>
+      <c r="B213" s="111" t="s">
+        <v>275</v>
+      </c>
+      <c r="C213" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D213" s="112" t="s">
+        <v>173</v>
+      </c>
+      <c r="E213" s="111" t="s">
+        <v>276</v>
+      </c>
       <c r="F213" s="68"/>
       <c r="G213" s="68"/>
       <c r="H213" s="68"/>
@@ -12236,7 +12291,9 @@
       <c r="K213" s="70"/>
       <c r="L213" s="68"/>
       <c r="M213" s="68"/>
-      <c r="N213" s="68"/>
+      <c r="N213" s="112" t="s">
+        <v>277</v>
+      </c>
       <c r="O213" s="9"/>
       <c r="P213" s="4"/>
       <c r="Q213" s="4"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1080/10426914.2021.2006217`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78CB0BA-BAC8-CA46-BB2C-EF2E843DF6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6034F631-F8E5-B24D-B555-B08E64303F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="760" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="286">
   <si>
     <r>
       <rPr>
@@ -954,6 +954,30 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2012.12.095</t>
+  </si>
+  <si>
+    <t>5C</t>
+  </si>
+  <si>
+    <t>FeCrCuMnTi</t>
+  </si>
+  <si>
+    <t>FeCrCuMnTiV</t>
+  </si>
+  <si>
+    <t>FeCrCuMnTiVZn</t>
+  </si>
+  <si>
+    <t>MA+SR</t>
+  </si>
+  <si>
+    <t>mechanical alloying through high energy ball milling for 25h</t>
+  </si>
+  <si>
+    <t>FCC+BCC+HCP</t>
+  </si>
+  <si>
+    <t>10.1080/10426914.2021.2006217</t>
   </si>
 </sst>
 </file>
@@ -3281,8 +3305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A187" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N218" sqref="N218"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A186" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N220" sqref="N220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -12302,11 +12326,21 @@
       <c r="T213" s="9"/>
     </row>
     <row r="214" spans="1:20" ht="18" customHeight="1">
-      <c r="A214" s="64"/>
-      <c r="B214" s="73"/>
-      <c r="C214" s="68"/>
-      <c r="D214" s="68"/>
-      <c r="E214" s="73"/>
+      <c r="A214" s="116" t="s">
+        <v>278</v>
+      </c>
+      <c r="B214" s="111" t="s">
+        <v>279</v>
+      </c>
+      <c r="C214" s="112" t="s">
+        <v>284</v>
+      </c>
+      <c r="D214" s="112" t="s">
+        <v>282</v>
+      </c>
+      <c r="E214" s="111" t="s">
+        <v>283</v>
+      </c>
       <c r="F214" s="68"/>
       <c r="G214" s="68"/>
       <c r="H214" s="68"/>
@@ -12315,7 +12349,9 @@
       <c r="K214" s="70"/>
       <c r="L214" s="68"/>
       <c r="M214" s="68"/>
-      <c r="N214" s="68"/>
+      <c r="N214" s="112" t="s">
+        <v>285</v>
+      </c>
       <c r="O214" s="9"/>
       <c r="P214" s="4"/>
       <c r="Q214" s="4"/>
@@ -12324,11 +12360,21 @@
       <c r="T214" s="9"/>
     </row>
     <row r="215" spans="1:20" ht="18" customHeight="1">
-      <c r="A215" s="64"/>
-      <c r="B215" s="73"/>
-      <c r="C215" s="68"/>
-      <c r="D215" s="68"/>
-      <c r="E215" s="73"/>
+      <c r="A215" s="116" t="s">
+        <v>271</v>
+      </c>
+      <c r="B215" s="111" t="s">
+        <v>280</v>
+      </c>
+      <c r="C215" s="112" t="s">
+        <v>284</v>
+      </c>
+      <c r="D215" s="112" t="s">
+        <v>282</v>
+      </c>
+      <c r="E215" s="111" t="s">
+        <v>283</v>
+      </c>
       <c r="F215" s="68"/>
       <c r="G215" s="68"/>
       <c r="H215" s="68"/>
@@ -12337,7 +12383,9 @@
       <c r="K215" s="70"/>
       <c r="L215" s="68"/>
       <c r="M215" s="68"/>
-      <c r="N215" s="68"/>
+      <c r="N215" s="112" t="s">
+        <v>285</v>
+      </c>
       <c r="O215" s="9"/>
       <c r="P215" s="4"/>
       <c r="Q215" s="4"/>
@@ -12346,11 +12394,21 @@
       <c r="T215" s="9"/>
     </row>
     <row r="216" spans="1:20" ht="18" customHeight="1">
-      <c r="A216" s="64"/>
-      <c r="B216" s="73"/>
-      <c r="C216" s="68"/>
-      <c r="D216" s="68"/>
-      <c r="E216" s="73"/>
+      <c r="A216" s="116" t="s">
+        <v>272</v>
+      </c>
+      <c r="B216" s="111" t="s">
+        <v>281</v>
+      </c>
+      <c r="C216" s="112" t="s">
+        <v>284</v>
+      </c>
+      <c r="D216" s="112" t="s">
+        <v>282</v>
+      </c>
+      <c r="E216" s="111" t="s">
+        <v>283</v>
+      </c>
       <c r="F216" s="68"/>
       <c r="G216" s="68"/>
       <c r="H216" s="68"/>
@@ -12359,7 +12417,9 @@
       <c r="K216" s="70"/>
       <c r="L216" s="68"/>
       <c r="M216" s="68"/>
-      <c r="N216" s="68"/>
+      <c r="N216" s="112" t="s">
+        <v>285</v>
+      </c>
       <c r="O216" s="9"/>
       <c r="P216" s="4"/>
       <c r="Q216" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2024.146887`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6034F631-F8E5-B24D-B555-B08E64303F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E4650B-9565-9540-BDFC-8C0750D8A05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="760" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="291">
   <si>
     <r>
       <rPr>
@@ -978,6 +978,21 @@
   </si>
   <si>
     <t>10.1080/10426914.2021.2006217</t>
+  </si>
+  <si>
+    <t>Ni48.6 Al10.3 Co17 Cr7.5 Fe9 Ti5.8 Ta0.6 Mo0.8 W0.4</t>
+  </si>
+  <si>
+    <t>FCC+L12</t>
+  </si>
+  <si>
+    <t>F7b</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2024.146887</t>
+  </si>
+  <si>
+    <t>strain rate 1e-2/s</t>
   </si>
 </sst>
 </file>
@@ -1778,7 +1793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2143,6 +2158,7 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3305,8 +3321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A186" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N220" sqref="N220"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A190" zoomScale="86" workbookViewId="0">
+      <selection activeCell="K232" sqref="K232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -12429,21 +12445,46 @@
     </row>
     <row r="217" spans="1:20" ht="18" customHeight="1">
       <c r="A217" s="64"/>
-      <c r="B217" s="73"/>
-      <c r="C217" s="68"/>
-      <c r="D217" s="68"/>
+      <c r="B217" s="111" t="s">
+        <v>286</v>
+      </c>
+      <c r="C217" s="112" t="s">
+        <v>287</v>
+      </c>
+      <c r="D217" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E217" s="73"/>
-      <c r="F217" s="68"/>
-      <c r="G217" s="68"/>
-      <c r="H217" s="68"/>
-      <c r="I217" s="83"/>
-      <c r="J217" s="70"/>
+      <c r="F217" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G217" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H217" s="112" t="s">
+        <v>290</v>
+      </c>
+      <c r="I217" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J217" s="70">
+        <f>P217*1000000</f>
+        <v>1175177304.96453</v>
+      </c>
       <c r="K217" s="70"/>
-      <c r="L217" s="68"/>
-      <c r="M217" s="68"/>
-      <c r="N217" s="68"/>
+      <c r="L217" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M217" s="112" t="s">
+        <v>288</v>
+      </c>
+      <c r="N217" s="112" t="s">
+        <v>289</v>
+      </c>
       <c r="O217" s="9"/>
-      <c r="P217" s="4"/>
+      <c r="P217" s="4">
+        <v>1175.1773049645301</v>
+      </c>
       <c r="Q217" s="4"/>
       <c r="R217" s="9"/>
       <c r="S217" s="9"/>
@@ -12451,21 +12492,46 @@
     </row>
     <row r="218" spans="1:20" ht="18" customHeight="1">
       <c r="A218" s="64"/>
-      <c r="B218" s="73"/>
-      <c r="C218" s="68"/>
-      <c r="D218" s="68"/>
+      <c r="B218" s="111" t="s">
+        <v>286</v>
+      </c>
+      <c r="C218" s="112" t="s">
+        <v>287</v>
+      </c>
+      <c r="D218" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E218" s="73"/>
-      <c r="F218" s="68"/>
-      <c r="G218" s="68"/>
-      <c r="H218" s="68"/>
-      <c r="I218" s="83"/>
-      <c r="J218" s="70"/>
+      <c r="F218" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G218" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H218" s="112" t="s">
+        <v>290</v>
+      </c>
+      <c r="I218" s="83">
+        <v>1173</v>
+      </c>
+      <c r="J218" s="70">
+        <f t="shared" ref="J218:J221" si="5">P218*1000000</f>
+        <v>664539007.0921979</v>
+      </c>
       <c r="K218" s="70"/>
-      <c r="L218" s="68"/>
-      <c r="M218" s="68"/>
-      <c r="N218" s="68"/>
+      <c r="L218" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M218" s="112" t="s">
+        <v>288</v>
+      </c>
+      <c r="N218" s="112" t="s">
+        <v>289</v>
+      </c>
       <c r="O218" s="9"/>
-      <c r="P218" s="4"/>
+      <c r="P218" s="4">
+        <v>664.53900709219795</v>
+      </c>
       <c r="Q218" s="4"/>
       <c r="R218" s="9"/>
       <c r="S218" s="9"/>
@@ -12473,21 +12539,46 @@
     </row>
     <row r="219" spans="1:20" ht="18" customHeight="1">
       <c r="A219" s="64"/>
-      <c r="B219" s="73"/>
-      <c r="C219" s="68"/>
-      <c r="D219" s="68"/>
+      <c r="B219" s="111" t="s">
+        <v>286</v>
+      </c>
+      <c r="C219" s="112" t="s">
+        <v>287</v>
+      </c>
+      <c r="D219" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E219" s="73"/>
-      <c r="F219" s="68"/>
-      <c r="G219" s="68"/>
-      <c r="H219" s="68"/>
-      <c r="I219" s="83"/>
-      <c r="J219" s="70"/>
+      <c r="F219" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G219" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H219" s="112" t="s">
+        <v>290</v>
+      </c>
+      <c r="I219" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J219" s="70">
+        <f t="shared" si="5"/>
+        <v>412765957.44680798</v>
+      </c>
       <c r="K219" s="70"/>
-      <c r="L219" s="68"/>
-      <c r="M219" s="68"/>
-      <c r="N219" s="68"/>
+      <c r="L219" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M219" s="112" t="s">
+        <v>288</v>
+      </c>
+      <c r="N219" s="112" t="s">
+        <v>289</v>
+      </c>
       <c r="O219" s="9"/>
-      <c r="P219" s="4"/>
+      <c r="P219" s="4">
+        <v>412.76595744680799</v>
+      </c>
       <c r="Q219" s="4"/>
       <c r="R219" s="9"/>
       <c r="S219" s="9"/>
@@ -12495,21 +12586,46 @@
     </row>
     <row r="220" spans="1:20" ht="18" customHeight="1">
       <c r="A220" s="64"/>
-      <c r="B220" s="73"/>
-      <c r="C220" s="68"/>
-      <c r="D220" s="68"/>
+      <c r="B220" s="111" t="s">
+        <v>286</v>
+      </c>
+      <c r="C220" s="112" t="s">
+        <v>287</v>
+      </c>
+      <c r="D220" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E220" s="73"/>
-      <c r="F220" s="68"/>
-      <c r="G220" s="68"/>
-      <c r="H220" s="68"/>
-      <c r="I220" s="83"/>
-      <c r="J220" s="70"/>
+      <c r="F220" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G220" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H220" s="112" t="s">
+        <v>290</v>
+      </c>
+      <c r="I220" s="154">
+        <v>1323</v>
+      </c>
+      <c r="J220" s="70">
+        <f t="shared" si="5"/>
+        <v>274468085.10638303</v>
+      </c>
       <c r="K220" s="70"/>
-      <c r="L220" s="68"/>
-      <c r="M220" s="68"/>
-      <c r="N220" s="68"/>
+      <c r="L220" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M220" s="112" t="s">
+        <v>288</v>
+      </c>
+      <c r="N220" s="112" t="s">
+        <v>289</v>
+      </c>
       <c r="O220" s="9"/>
-      <c r="P220" s="4"/>
+      <c r="P220" s="4">
+        <v>274.468085106383</v>
+      </c>
       <c r="Q220" s="4"/>
       <c r="R220" s="9"/>
       <c r="S220" s="9"/>
@@ -12517,21 +12633,46 @@
     </row>
     <row r="221" spans="1:20" ht="18" customHeight="1">
       <c r="A221" s="64"/>
-      <c r="B221" s="73"/>
-      <c r="C221" s="68"/>
-      <c r="D221" s="68"/>
+      <c r="B221" s="111" t="s">
+        <v>286</v>
+      </c>
+      <c r="C221" s="112" t="s">
+        <v>287</v>
+      </c>
+      <c r="D221" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E221" s="73"/>
-      <c r="F221" s="68"/>
-      <c r="G221" s="68"/>
-      <c r="H221" s="68"/>
-      <c r="I221" s="83"/>
-      <c r="J221" s="70"/>
+      <c r="F221" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G221" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H221" s="112" t="s">
+        <v>290</v>
+      </c>
+      <c r="I221" s="83">
+        <v>1373</v>
+      </c>
+      <c r="J221" s="70">
+        <f t="shared" si="5"/>
+        <v>182269503.54609901</v>
+      </c>
       <c r="K221" s="70"/>
-      <c r="L221" s="68"/>
-      <c r="M221" s="68"/>
-      <c r="N221" s="68"/>
+      <c r="L221" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M221" s="112" t="s">
+        <v>288</v>
+      </c>
+      <c r="N221" s="112" t="s">
+        <v>289</v>
+      </c>
       <c r="O221" s="9"/>
-      <c r="P221" s="4"/>
+      <c r="P221" s="4">
+        <v>182.269503546099</v>
+      </c>
       <c r="Q221" s="4"/>
       <c r="R221" s="9"/>
       <c r="S221" s="9"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2023.168975`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E4650B-9565-9540-BDFC-8C0750D8A05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5E6F29-D34D-1B40-B4DB-0AC062FA0F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="760" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3640" yWindow="3540" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="301">
   <si>
     <r>
       <rPr>
@@ -41,6 +41,7 @@
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Metadata</t>
     </r>
@@ -102,6 +103,7 @@
         <sz val="11"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>T</t>
     </r>
@@ -110,6 +112,7 @@
         <sz val="8"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">able </t>
     </r>
@@ -118,6 +121,7 @@
         <sz val="11"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>/ F</t>
     </r>
@@ -126,6 +130,7 @@
         <sz val="8"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">igure </t>
     </r>
@@ -134,6 +139,7 @@
         <sz val="11"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>/ A</t>
     </r>
@@ -142,6 +148,7 @@
         <sz val="8"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>ppendix</t>
     </r>
@@ -150,6 +157,7 @@
         <sz val="11"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> P</t>
     </r>
@@ -166,6 +174,7 @@
         <sz val="11"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> / S</t>
     </r>
@@ -174,6 +183,7 @@
         <sz val="8"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>upplemental</t>
     </r>
@@ -993,6 +1003,36 @@
   </si>
   <si>
     <t>strain rate 1e-2/s</t>
+  </si>
+  <si>
+    <t>CoCrFeNiNb0.25Ta0.20</t>
+  </si>
+  <si>
+    <t>CoCrFeNiTa0.25Hf0.25</t>
+  </si>
+  <si>
+    <t>CoCrFeNiNb0.15Zr0.15Hf0.15</t>
+  </si>
+  <si>
+    <t>CoCrFeNiZr0.17Hf0.16Ta0.16</t>
+  </si>
+  <si>
+    <t>FCC+C15</t>
+  </si>
+  <si>
+    <t>melting temperature</t>
+  </si>
+  <si>
+    <t>cooling DSC</t>
+  </si>
+  <si>
+    <t>eutectic alloy; lamellar microstructure</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2023.168975</t>
   </si>
 </sst>
 </file>
@@ -1013,32 +1053,38 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="13"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color indexed="13"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -1049,12 +1095,14 @@
       <sz val="10"/>
       <color indexed="13"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1065,22 +1113,26 @@
       <sz val="12"/>
       <color indexed="20"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="21"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="21"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="21"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2047,57 +2099,7 @@
     <xf numFmtId="3" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2158,7 +2160,57 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3321,8 +3373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A190" zoomScale="86" workbookViewId="0">
-      <selection activeCell="K232" sqref="K232"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E211" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N242" sqref="N242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3379,19 +3431,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="134" t="s">
+      <c r="D2" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="135"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="139"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="141"/>
-      <c r="K2" s="141"/>
-      <c r="L2" s="139"/>
-      <c r="M2" s="139"/>
-      <c r="N2" s="142"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="126"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3407,17 +3459,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="145"/>
-      <c r="K3" s="145"/>
-      <c r="L3" s="143"/>
-      <c r="M3" s="143"/>
-      <c r="N3" s="146"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="129"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127"/>
+      <c r="N3" s="130"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3458,43 +3510,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="149" t="s">
+      <c r="D5" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="149" t="s">
+      <c r="E5" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="149" t="s">
+      <c r="F5" s="133" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="149" t="s">
+      <c r="G5" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="150" t="s">
+      <c r="H5" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="149" t="s">
+      <c r="I5" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="149" t="s">
+      <c r="J5" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="149" t="s">
+      <c r="K5" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="149" t="s">
+      <c r="L5" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="149" t="s">
+      <c r="M5" s="133" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="149" t="s">
+      <c r="N5" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="117" t="s">
+      <c r="O5" s="138" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3510,19 +3562,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="148"/>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="151"/>
-      <c r="I6" s="152"/>
-      <c r="J6" s="153"/>
-      <c r="K6" s="153"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="118"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="137"/>
+      <c r="K6" s="137"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="139"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3572,7 +3624,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="119"/>
+      <c r="O7" s="140"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -3587,35 +3639,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="120" t="s">
+      <c r="B8" s="141" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="123" t="s">
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="143"/>
+      <c r="F8" s="144" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="125"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="126"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="128" t="s">
+      <c r="G8" s="145"/>
+      <c r="H8" s="145"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="147"/>
+      <c r="K8" s="147"/>
+      <c r="L8" s="148"/>
+      <c r="M8" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="129"/>
+      <c r="N8" s="150"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="130" t="s">
+      <c r="P8" s="151" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="132"/>
-      <c r="S8" s="132"/>
-      <c r="T8" s="133"/>
+      <c r="Q8" s="152"/>
+      <c r="R8" s="153"/>
+      <c r="S8" s="153"/>
+      <c r="T8" s="154"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="38" t="s">
@@ -12605,7 +12657,7 @@
       <c r="H220" s="112" t="s">
         <v>290</v>
       </c>
-      <c r="I220" s="154">
+      <c r="I220" s="117">
         <v>1323</v>
       </c>
       <c r="J220" s="70">
@@ -12680,19 +12732,41 @@
     </row>
     <row r="222" spans="1:20" ht="18" customHeight="1">
       <c r="A222" s="64"/>
-      <c r="B222" s="73"/>
-      <c r="C222" s="68"/>
-      <c r="D222" s="68"/>
-      <c r="E222" s="73"/>
-      <c r="F222" s="68"/>
-      <c r="G222" s="68"/>
-      <c r="H222" s="68"/>
+      <c r="B222" s="111" t="s">
+        <v>291</v>
+      </c>
+      <c r="C222" s="112" t="s">
+        <v>234</v>
+      </c>
+      <c r="D222" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E222" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F222" s="112" t="s">
+        <v>296</v>
+      </c>
+      <c r="G222" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H222" s="112" t="s">
+        <v>297</v>
+      </c>
       <c r="I222" s="83"/>
-      <c r="J222" s="80"/>
+      <c r="J222" s="80">
+        <v>1525</v>
+      </c>
       <c r="K222" s="70"/>
-      <c r="L222" s="68"/>
-      <c r="M222" s="68"/>
-      <c r="N222" s="68"/>
+      <c r="L222" s="112" t="s">
+        <v>249</v>
+      </c>
+      <c r="M222" s="112" t="s">
+        <v>254</v>
+      </c>
+      <c r="N222" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O222" s="9"/>
       <c r="P222" s="4"/>
       <c r="Q222" s="4"/>
@@ -12702,19 +12776,41 @@
     </row>
     <row r="223" spans="1:20" ht="18" customHeight="1">
       <c r="A223" s="64"/>
-      <c r="B223" s="73"/>
-      <c r="C223" s="68"/>
-      <c r="D223" s="68"/>
-      <c r="E223" s="73"/>
-      <c r="F223" s="68"/>
-      <c r="G223" s="68"/>
-      <c r="H223" s="68"/>
+      <c r="B223" s="111" t="s">
+        <v>292</v>
+      </c>
+      <c r="C223" s="112" t="s">
+        <v>234</v>
+      </c>
+      <c r="D223" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E223" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F223" s="112" t="s">
+        <v>296</v>
+      </c>
+      <c r="G223" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H223" s="112" t="s">
+        <v>297</v>
+      </c>
       <c r="I223" s="83"/>
-      <c r="J223" s="80"/>
+      <c r="J223" s="80">
+        <v>1512</v>
+      </c>
       <c r="K223" s="70"/>
-      <c r="L223" s="68"/>
-      <c r="M223" s="68"/>
-      <c r="N223" s="68"/>
+      <c r="L223" s="112" t="s">
+        <v>249</v>
+      </c>
+      <c r="M223" s="112" t="s">
+        <v>254</v>
+      </c>
+      <c r="N223" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O223" s="9"/>
       <c r="P223" s="4"/>
       <c r="Q223" s="4"/>
@@ -12724,19 +12820,41 @@
     </row>
     <row r="224" spans="1:20" ht="18" customHeight="1">
       <c r="A224" s="64"/>
-      <c r="B224" s="73"/>
-      <c r="C224" s="68"/>
-      <c r="D224" s="68"/>
-      <c r="E224" s="73"/>
-      <c r="F224" s="68"/>
-      <c r="G224" s="68"/>
-      <c r="H224" s="68"/>
+      <c r="B224" s="111" t="s">
+        <v>293</v>
+      </c>
+      <c r="C224" s="112" t="s">
+        <v>295</v>
+      </c>
+      <c r="D224" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E224" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F224" s="112" t="s">
+        <v>296</v>
+      </c>
+      <c r="G224" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H224" s="112" t="s">
+        <v>297</v>
+      </c>
       <c r="I224" s="83"/>
-      <c r="J224" s="80"/>
+      <c r="J224" s="80">
+        <v>1489</v>
+      </c>
       <c r="K224" s="70"/>
-      <c r="L224" s="68"/>
-      <c r="M224" s="68"/>
-      <c r="N224" s="68"/>
+      <c r="L224" s="112" t="s">
+        <v>249</v>
+      </c>
+      <c r="M224" s="112" t="s">
+        <v>254</v>
+      </c>
+      <c r="N224" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O224" s="9"/>
       <c r="P224" s="4"/>
       <c r="Q224" s="4"/>
@@ -12746,19 +12864,41 @@
     </row>
     <row r="225" spans="1:20" ht="18" customHeight="1">
       <c r="A225" s="64"/>
-      <c r="B225" s="73"/>
-      <c r="C225" s="68"/>
-      <c r="D225" s="68"/>
-      <c r="E225" s="73"/>
-      <c r="F225" s="68"/>
-      <c r="G225" s="68"/>
-      <c r="H225" s="68"/>
+      <c r="B225" s="111" t="s">
+        <v>294</v>
+      </c>
+      <c r="C225" s="112" t="s">
+        <v>295</v>
+      </c>
+      <c r="D225" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E225" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F225" s="112" t="s">
+        <v>296</v>
+      </c>
+      <c r="G225" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H225" s="112" t="s">
+        <v>297</v>
+      </c>
       <c r="I225" s="83"/>
-      <c r="J225" s="80"/>
+      <c r="J225" s="80">
+        <v>1482</v>
+      </c>
       <c r="K225" s="70"/>
-      <c r="L225" s="68"/>
-      <c r="M225" s="68"/>
-      <c r="N225" s="68"/>
+      <c r="L225" s="112" t="s">
+        <v>249</v>
+      </c>
+      <c r="M225" s="112" t="s">
+        <v>254</v>
+      </c>
+      <c r="N225" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O225" s="9"/>
       <c r="P225" s="4"/>
       <c r="Q225" s="4"/>
@@ -12768,21 +12908,48 @@
     </row>
     <row r="226" spans="1:20" ht="18" customHeight="1">
       <c r="A226" s="64"/>
-      <c r="B226" s="73"/>
-      <c r="C226" s="68"/>
-      <c r="D226" s="68"/>
-      <c r="E226" s="73"/>
-      <c r="F226" s="68"/>
-      <c r="G226" s="68"/>
-      <c r="H226" s="68"/>
-      <c r="I226" s="83"/>
-      <c r="J226" s="80"/>
+      <c r="B226" s="111" t="s">
+        <v>291</v>
+      </c>
+      <c r="C226" s="112" t="s">
+        <v>234</v>
+      </c>
+      <c r="D226" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E226" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F226" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G226" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H226" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I226" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J226" s="80">
+        <f>P226*1000000</f>
+        <v>593253968.253968</v>
+      </c>
       <c r="K226" s="70"/>
-      <c r="L226" s="68"/>
-      <c r="M226" s="68"/>
-      <c r="N226" s="68"/>
+      <c r="L226" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M226" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N226" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O226" s="9"/>
-      <c r="P226" s="4"/>
+      <c r="P226" s="4">
+        <v>593.25396825396797</v>
+      </c>
       <c r="Q226" s="4"/>
       <c r="R226" s="9"/>
       <c r="S226" s="9"/>
@@ -12790,21 +12957,48 @@
     </row>
     <row r="227" spans="1:20" ht="18" customHeight="1">
       <c r="A227" s="64"/>
-      <c r="B227" s="73"/>
-      <c r="C227" s="68"/>
-      <c r="D227" s="68"/>
-      <c r="E227" s="73"/>
-      <c r="F227" s="68"/>
-      <c r="G227" s="68"/>
-      <c r="H227" s="68"/>
-      <c r="I227" s="83"/>
-      <c r="J227" s="80"/>
+      <c r="B227" s="111" t="s">
+        <v>292</v>
+      </c>
+      <c r="C227" s="112" t="s">
+        <v>234</v>
+      </c>
+      <c r="D227" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E227" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F227" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G227" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H227" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I227" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J227" s="80">
+        <f t="shared" ref="J227:J237" si="6">P227*1000000</f>
+        <v>659722222.22222197</v>
+      </c>
       <c r="K227" s="70"/>
-      <c r="L227" s="68"/>
-      <c r="M227" s="68"/>
-      <c r="N227" s="68"/>
+      <c r="L227" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M227" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N227" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O227" s="9"/>
-      <c r="P227" s="4"/>
+      <c r="P227" s="4">
+        <v>659.72222222222194</v>
+      </c>
       <c r="Q227" s="4"/>
       <c r="R227" s="9"/>
       <c r="S227" s="9"/>
@@ -12812,21 +13006,48 @@
     </row>
     <row r="228" spans="1:20" ht="18" customHeight="1">
       <c r="A228" s="64"/>
-      <c r="B228" s="73"/>
-      <c r="C228" s="68"/>
-      <c r="D228" s="68"/>
-      <c r="E228" s="73"/>
-      <c r="F228" s="68"/>
-      <c r="G228" s="68"/>
-      <c r="H228" s="68"/>
-      <c r="I228" s="83"/>
-      <c r="J228" s="80"/>
+      <c r="B228" s="111" t="s">
+        <v>293</v>
+      </c>
+      <c r="C228" s="112" t="s">
+        <v>295</v>
+      </c>
+      <c r="D228" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E228" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F228" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G228" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H228" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I228" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J228" s="80">
+        <f t="shared" si="6"/>
+        <v>441468253.96825397</v>
+      </c>
       <c r="K228" s="70"/>
-      <c r="L228" s="68"/>
-      <c r="M228" s="68"/>
-      <c r="N228" s="68"/>
+      <c r="L228" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M228" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N228" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O228" s="9"/>
-      <c r="P228" s="4"/>
+      <c r="P228" s="4">
+        <v>441.46825396825398</v>
+      </c>
       <c r="Q228" s="4"/>
       <c r="R228" s="9"/>
       <c r="S228" s="9"/>
@@ -12834,21 +13055,48 @@
     </row>
     <row r="229" spans="1:20" ht="18" customHeight="1">
       <c r="A229" s="64"/>
-      <c r="B229" s="73"/>
-      <c r="C229" s="68"/>
-      <c r="D229" s="68"/>
-      <c r="E229" s="73"/>
-      <c r="F229" s="68"/>
-      <c r="G229" s="68"/>
-      <c r="H229" s="68"/>
-      <c r="I229" s="83"/>
-      <c r="J229" s="80"/>
+      <c r="B229" s="111" t="s">
+        <v>294</v>
+      </c>
+      <c r="C229" s="112" t="s">
+        <v>295</v>
+      </c>
+      <c r="D229" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E229" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F229" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G229" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H229" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I229" s="83">
+        <v>1073</v>
+      </c>
+      <c r="J229" s="80">
+        <f t="shared" si="6"/>
+        <v>503968253.96825397</v>
+      </c>
       <c r="K229" s="70"/>
-      <c r="L229" s="68"/>
-      <c r="M229" s="68"/>
-      <c r="N229" s="68"/>
+      <c r="L229" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M229" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N229" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O229" s="9"/>
-      <c r="P229" s="4"/>
+      <c r="P229" s="4">
+        <v>503.96825396825398</v>
+      </c>
       <c r="Q229" s="4"/>
       <c r="R229" s="9"/>
       <c r="S229" s="9"/>
@@ -12856,21 +13104,48 @@
     </row>
     <row r="230" spans="1:20" ht="18" customHeight="1">
       <c r="A230" s="64"/>
-      <c r="B230" s="73"/>
-      <c r="C230" s="68"/>
-      <c r="D230" s="68"/>
-      <c r="E230" s="73"/>
-      <c r="F230" s="68"/>
-      <c r="G230" s="68"/>
-      <c r="H230" s="68"/>
-      <c r="I230" s="83"/>
-      <c r="J230" s="80"/>
+      <c r="B230" s="111" t="s">
+        <v>291</v>
+      </c>
+      <c r="C230" s="112" t="s">
+        <v>234</v>
+      </c>
+      <c r="D230" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E230" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F230" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G230" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H230" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I230" s="83">
+        <v>1173</v>
+      </c>
+      <c r="J230" s="80">
+        <f t="shared" si="6"/>
+        <v>272817460.31746</v>
+      </c>
       <c r="K230" s="70"/>
-      <c r="L230" s="68"/>
-      <c r="M230" s="68"/>
-      <c r="N230" s="68"/>
+      <c r="L230" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M230" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N230" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O230" s="9"/>
-      <c r="P230" s="4"/>
+      <c r="P230" s="4">
+        <v>272.81746031746002</v>
+      </c>
       <c r="Q230" s="4"/>
       <c r="R230" s="9"/>
       <c r="S230" s="9"/>
@@ -12878,21 +13153,48 @@
     </row>
     <row r="231" spans="1:20" ht="18" customHeight="1">
       <c r="A231" s="64"/>
-      <c r="B231" s="73"/>
-      <c r="C231" s="68"/>
-      <c r="D231" s="68"/>
-      <c r="E231" s="73"/>
-      <c r="F231" s="68"/>
-      <c r="G231" s="68"/>
-      <c r="H231" s="68"/>
-      <c r="I231" s="83"/>
-      <c r="J231" s="80"/>
+      <c r="B231" s="111" t="s">
+        <v>292</v>
+      </c>
+      <c r="C231" s="112" t="s">
+        <v>234</v>
+      </c>
+      <c r="D231" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E231" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F231" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G231" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H231" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I231" s="83">
+        <v>1173</v>
+      </c>
+      <c r="J231" s="80">
+        <f t="shared" si="6"/>
+        <v>258928571.42857099</v>
+      </c>
       <c r="K231" s="70"/>
-      <c r="L231" s="68"/>
-      <c r="M231" s="68"/>
-      <c r="N231" s="68"/>
+      <c r="L231" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M231" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N231" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O231" s="9"/>
-      <c r="P231" s="4"/>
+      <c r="P231" s="4">
+        <v>258.92857142857099</v>
+      </c>
       <c r="Q231" s="4"/>
       <c r="R231" s="9"/>
       <c r="S231" s="9"/>
@@ -12900,21 +13202,48 @@
     </row>
     <row r="232" spans="1:20" ht="18" customHeight="1">
       <c r="A232" s="64"/>
-      <c r="B232" s="73"/>
-      <c r="C232" s="68"/>
-      <c r="D232" s="68"/>
-      <c r="E232" s="73"/>
-      <c r="F232" s="68"/>
-      <c r="G232" s="68"/>
-      <c r="H232" s="68"/>
-      <c r="I232" s="83"/>
-      <c r="J232" s="80"/>
+      <c r="B232" s="111" t="s">
+        <v>293</v>
+      </c>
+      <c r="C232" s="112" t="s">
+        <v>295</v>
+      </c>
+      <c r="D232" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E232" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F232" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G232" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H232" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I232" s="83">
+        <v>1173</v>
+      </c>
+      <c r="J232" s="80">
+        <f t="shared" si="6"/>
+        <v>272817460.31746</v>
+      </c>
       <c r="K232" s="70"/>
-      <c r="L232" s="68"/>
-      <c r="M232" s="68"/>
-      <c r="N232" s="68"/>
+      <c r="L232" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M232" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N232" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O232" s="9"/>
-      <c r="P232" s="4"/>
+      <c r="P232" s="4">
+        <v>272.81746031746002</v>
+      </c>
       <c r="Q232" s="4"/>
       <c r="R232" s="9"/>
       <c r="S232" s="9"/>
@@ -12922,21 +13251,48 @@
     </row>
     <row r="233" spans="1:20" ht="18" customHeight="1">
       <c r="A233" s="64"/>
-      <c r="B233" s="73"/>
-      <c r="C233" s="68"/>
-      <c r="D233" s="68"/>
-      <c r="E233" s="73"/>
-      <c r="F233" s="68"/>
-      <c r="G233" s="68"/>
-      <c r="H233" s="68"/>
-      <c r="I233" s="83"/>
-      <c r="J233" s="80"/>
+      <c r="B233" s="111" t="s">
+        <v>294</v>
+      </c>
+      <c r="C233" s="112" t="s">
+        <v>295</v>
+      </c>
+      <c r="D233" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E233" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F233" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G233" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H233" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I233" s="83">
+        <v>1173</v>
+      </c>
+      <c r="J233" s="80">
+        <f t="shared" si="6"/>
+        <v>280753968.253968</v>
+      </c>
       <c r="K233" s="70"/>
-      <c r="L233" s="68"/>
-      <c r="M233" s="68"/>
-      <c r="N233" s="68"/>
+      <c r="L233" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M233" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N233" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O233" s="9"/>
-      <c r="P233" s="4"/>
+      <c r="P233" s="4">
+        <v>280.75396825396803</v>
+      </c>
       <c r="Q233" s="4"/>
       <c r="R233" s="9"/>
       <c r="S233" s="9"/>
@@ -12944,21 +13300,48 @@
     </row>
     <row r="234" spans="1:20" ht="18" customHeight="1">
       <c r="A234" s="64"/>
-      <c r="B234" s="73"/>
-      <c r="C234" s="68"/>
-      <c r="D234" s="68"/>
-      <c r="E234" s="73"/>
-      <c r="F234" s="68"/>
-      <c r="G234" s="68"/>
-      <c r="H234" s="68"/>
-      <c r="I234" s="83"/>
-      <c r="J234" s="70"/>
+      <c r="B234" s="111" t="s">
+        <v>291</v>
+      </c>
+      <c r="C234" s="112" t="s">
+        <v>234</v>
+      </c>
+      <c r="D234" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E234" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F234" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G234" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H234" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I234" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J234" s="80">
+        <f t="shared" si="6"/>
+        <v>141865079.36507899</v>
+      </c>
       <c r="K234" s="70"/>
-      <c r="L234" s="68"/>
-      <c r="M234" s="68"/>
-      <c r="N234" s="68"/>
+      <c r="L234" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M234" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N234" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O234" s="9"/>
-      <c r="P234" s="4"/>
+      <c r="P234" s="4">
+        <v>141.865079365079</v>
+      </c>
       <c r="Q234" s="4"/>
       <c r="R234" s="9"/>
       <c r="S234" s="9"/>
@@ -12966,21 +13349,48 @@
     </row>
     <row r="235" spans="1:20" ht="18" customHeight="1">
       <c r="A235" s="64"/>
-      <c r="B235" s="73"/>
-      <c r="C235" s="68"/>
-      <c r="D235" s="68"/>
-      <c r="E235" s="73"/>
-      <c r="F235" s="68"/>
-      <c r="G235" s="68"/>
-      <c r="H235" s="68"/>
-      <c r="I235" s="83"/>
-      <c r="J235" s="70"/>
+      <c r="B235" s="111" t="s">
+        <v>292</v>
+      </c>
+      <c r="C235" s="112" t="s">
+        <v>234</v>
+      </c>
+      <c r="D235" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E235" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F235" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G235" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H235" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I235" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J235" s="80">
+        <f t="shared" si="6"/>
+        <v>140873015.87301499</v>
+      </c>
       <c r="K235" s="70"/>
-      <c r="L235" s="68"/>
-      <c r="M235" s="68"/>
-      <c r="N235" s="68"/>
+      <c r="L235" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M235" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N235" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O235" s="9"/>
-      <c r="P235" s="4"/>
+      <c r="P235" s="4">
+        <v>140.87301587301499</v>
+      </c>
       <c r="Q235" s="4"/>
       <c r="R235" s="9"/>
       <c r="S235" s="9"/>
@@ -12988,21 +13398,48 @@
     </row>
     <row r="236" spans="1:20" ht="18" customHeight="1">
       <c r="A236" s="64"/>
-      <c r="B236" s="73"/>
-      <c r="C236" s="68"/>
-      <c r="D236" s="68"/>
-      <c r="E236" s="73"/>
-      <c r="F236" s="68"/>
-      <c r="G236" s="68"/>
-      <c r="H236" s="68"/>
-      <c r="I236" s="83"/>
-      <c r="J236" s="70"/>
+      <c r="B236" s="111" t="s">
+        <v>293</v>
+      </c>
+      <c r="C236" s="112" t="s">
+        <v>295</v>
+      </c>
+      <c r="D236" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E236" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F236" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G236" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H236" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I236" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J236" s="80">
+        <f t="shared" si="6"/>
+        <v>153769841.26984102</v>
+      </c>
       <c r="K236" s="70"/>
-      <c r="L236" s="68"/>
-      <c r="M236" s="68"/>
-      <c r="N236" s="68"/>
+      <c r="L236" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M236" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N236" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O236" s="9"/>
-      <c r="P236" s="4"/>
+      <c r="P236" s="4">
+        <v>153.76984126984101</v>
+      </c>
       <c r="Q236" s="4"/>
       <c r="R236" s="9"/>
       <c r="S236" s="9"/>
@@ -13010,21 +13447,48 @@
     </row>
     <row r="237" spans="1:20" ht="18" customHeight="1">
       <c r="A237" s="64"/>
-      <c r="B237" s="73"/>
-      <c r="C237" s="68"/>
-      <c r="D237" s="68"/>
-      <c r="E237" s="73"/>
-      <c r="F237" s="68"/>
-      <c r="G237" s="68"/>
-      <c r="H237" s="68"/>
-      <c r="I237" s="83"/>
-      <c r="J237" s="70"/>
+      <c r="B237" s="111" t="s">
+        <v>294</v>
+      </c>
+      <c r="C237" s="112" t="s">
+        <v>295</v>
+      </c>
+      <c r="D237" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="E237" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F237" s="112" t="s">
+        <v>189</v>
+      </c>
+      <c r="G237" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H237" s="112" t="s">
+        <v>192</v>
+      </c>
+      <c r="I237" s="83">
+        <v>1273</v>
+      </c>
+      <c r="J237" s="80">
+        <f t="shared" si="6"/>
+        <v>140873015.87301499</v>
+      </c>
       <c r="K237" s="70"/>
-      <c r="L237" s="68"/>
-      <c r="M237" s="68"/>
-      <c r="N237" s="68"/>
+      <c r="L237" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M237" s="112" t="s">
+        <v>299</v>
+      </c>
+      <c r="N237" s="112" t="s">
+        <v>300</v>
+      </c>
       <c r="O237" s="9"/>
-      <c r="P237" s="4"/>
+      <c r="P237" s="4">
+        <v>140.87301587301499</v>
+      </c>
       <c r="Q237" s="4"/>
       <c r="R237" s="9"/>
       <c r="S237" s="9"/>
@@ -19515,7 +19979,7 @@
       <c r="N532" s="4"/>
       <c r="O532" s="9"/>
       <c r="P532" s="4"/>
-      <c r="Q532" s="4"/>
+      <c r="Q532" s="86"/>
       <c r="R532" s="9"/>
       <c r="S532" s="9"/>
       <c r="T532" s="9"/>
@@ -19537,7 +20001,7 @@
       <c r="N533" s="4"/>
       <c r="O533" s="9"/>
       <c r="P533" s="4"/>
-      <c r="Q533" s="4"/>
+      <c r="Q533" s="86"/>
       <c r="R533" s="9"/>
       <c r="S533" s="9"/>
       <c r="T533" s="9"/>
@@ -19559,7 +20023,7 @@
       <c r="N534" s="4"/>
       <c r="O534" s="9"/>
       <c r="P534" s="4"/>
-      <c r="Q534" s="4"/>
+      <c r="Q534" s="86"/>
       <c r="R534" s="9"/>
       <c r="S534" s="9"/>
       <c r="T534" s="9"/>
@@ -19581,7 +20045,7 @@
       <c r="N535" s="4"/>
       <c r="O535" s="9"/>
       <c r="P535" s="4"/>
-      <c r="Q535" s="4"/>
+      <c r="Q535" s="86"/>
       <c r="R535" s="9"/>
       <c r="S535" s="9"/>
       <c r="T535" s="9"/>
@@ -19603,7 +20067,7 @@
       <c r="N536" s="4"/>
       <c r="O536" s="9"/>
       <c r="P536" s="4"/>
-      <c r="Q536" s="4"/>
+      <c r="Q536" s="86"/>
       <c r="R536" s="9"/>
       <c r="S536" s="9"/>
       <c r="T536" s="9"/>
@@ -19977,7 +20441,7 @@
       <c r="N553" s="4"/>
       <c r="O553" s="9"/>
       <c r="P553" s="86"/>
-      <c r="Q553" s="86"/>
+      <c r="Q553" s="4"/>
       <c r="R553" s="9"/>
       <c r="S553" s="9"/>
       <c r="T553" s="9"/>
@@ -19999,7 +20463,7 @@
       <c r="N554" s="4"/>
       <c r="O554" s="9"/>
       <c r="P554" s="86"/>
-      <c r="Q554" s="86"/>
+      <c r="Q554" s="4"/>
       <c r="R554" s="9"/>
       <c r="S554" s="9"/>
       <c r="T554" s="9"/>
@@ -20021,7 +20485,7 @@
       <c r="N555" s="4"/>
       <c r="O555" s="9"/>
       <c r="P555" s="86"/>
-      <c r="Q555" s="86"/>
+      <c r="Q555" s="4"/>
       <c r="R555" s="9"/>
       <c r="S555" s="9"/>
       <c r="T555" s="9"/>
@@ -20043,7 +20507,7 @@
       <c r="N556" s="4"/>
       <c r="O556" s="9"/>
       <c r="P556" s="86"/>
-      <c r="Q556" s="86"/>
+      <c r="Q556" s="4"/>
       <c r="R556" s="9"/>
       <c r="S556" s="9"/>
       <c r="T556" s="9"/>
@@ -20065,7 +20529,7 @@
       <c r="N557" s="4"/>
       <c r="O557" s="9"/>
       <c r="P557" s="86"/>
-      <c r="Q557" s="86"/>
+      <c r="Q557" s="4"/>
       <c r="R557" s="9"/>
       <c r="S557" s="9"/>
       <c r="T557" s="9"/>
@@ -21803,7 +22267,7 @@
       <c r="N636" s="94"/>
       <c r="O636" s="9"/>
       <c r="P636" s="4"/>
-      <c r="Q636" s="4"/>
+      <c r="Q636" s="98"/>
       <c r="R636" s="9"/>
       <c r="S636" s="9"/>
       <c r="T636" s="9"/>
@@ -21825,7 +22289,7 @@
       <c r="N637" s="94"/>
       <c r="O637" s="9"/>
       <c r="P637" s="4"/>
-      <c r="Q637" s="4"/>
+      <c r="Q637" s="98"/>
       <c r="R637" s="9"/>
       <c r="S637" s="9"/>
       <c r="T637" s="9"/>
@@ -21847,7 +22311,7 @@
       <c r="N638" s="94"/>
       <c r="O638" s="9"/>
       <c r="P638" s="4"/>
-      <c r="Q638" s="4"/>
+      <c r="Q638" s="98"/>
       <c r="R638" s="9"/>
       <c r="S638" s="9"/>
       <c r="T638" s="9"/>
@@ -21869,7 +22333,7 @@
       <c r="N639" s="94"/>
       <c r="O639" s="9"/>
       <c r="P639" s="4"/>
-      <c r="Q639" s="4"/>
+      <c r="Q639" s="98"/>
       <c r="R639" s="9"/>
       <c r="S639" s="9"/>
       <c r="T639" s="9"/>
@@ -21891,7 +22355,7 @@
       <c r="N640" s="94"/>
       <c r="O640" s="9"/>
       <c r="P640" s="4"/>
-      <c r="Q640" s="4"/>
+      <c r="Q640" s="98"/>
       <c r="R640" s="9"/>
       <c r="S640" s="9"/>
       <c r="T640" s="9"/>
@@ -21913,7 +22377,7 @@
       <c r="N641" s="94"/>
       <c r="O641" s="9"/>
       <c r="P641" s="4"/>
-      <c r="Q641" s="4"/>
+      <c r="Q641" s="98"/>
       <c r="R641" s="9"/>
       <c r="S641" s="9"/>
       <c r="T641" s="9"/>
@@ -21935,7 +22399,7 @@
       <c r="N642" s="87"/>
       <c r="O642" s="9"/>
       <c r="P642" s="4"/>
-      <c r="Q642" s="4"/>
+      <c r="Q642" s="98"/>
       <c r="R642" s="9"/>
       <c r="S642" s="9"/>
       <c r="T642" s="9"/>
@@ -21957,7 +22421,7 @@
       <c r="N643" s="87"/>
       <c r="O643" s="9"/>
       <c r="P643" s="4"/>
-      <c r="Q643" s="4"/>
+      <c r="Q643" s="98"/>
       <c r="R643" s="9"/>
       <c r="S643" s="9"/>
       <c r="T643" s="9"/>
@@ -21979,7 +22443,7 @@
       <c r="N644" s="87"/>
       <c r="O644" s="9"/>
       <c r="P644" s="4"/>
-      <c r="Q644" s="4"/>
+      <c r="Q644" s="98"/>
       <c r="R644" s="9"/>
       <c r="S644" s="9"/>
       <c r="T644" s="9"/>
@@ -22001,7 +22465,7 @@
       <c r="N645" s="87"/>
       <c r="O645" s="9"/>
       <c r="P645" s="95"/>
-      <c r="Q645" s="4"/>
+      <c r="Q645" s="98"/>
       <c r="R645" s="96"/>
       <c r="S645" s="9"/>
       <c r="T645" s="9"/>
@@ -22023,7 +22487,7 @@
       <c r="N646" s="87"/>
       <c r="O646" s="9"/>
       <c r="P646" s="95"/>
-      <c r="Q646" s="4"/>
+      <c r="Q646" s="98"/>
       <c r="R646" s="96"/>
       <c r="S646" s="9"/>
       <c r="T646" s="9"/>
@@ -22045,7 +22509,7 @@
       <c r="N647" s="87"/>
       <c r="O647" s="9"/>
       <c r="P647" s="95"/>
-      <c r="Q647" s="4"/>
+      <c r="Q647" s="98"/>
       <c r="R647" s="96"/>
       <c r="S647" s="9"/>
       <c r="T647" s="9"/>
@@ -22067,7 +22531,7 @@
       <c r="N648" s="87"/>
       <c r="O648" s="9"/>
       <c r="P648" s="95"/>
-      <c r="Q648" s="4"/>
+      <c r="Q648" s="98"/>
       <c r="R648" s="96"/>
       <c r="S648" s="9"/>
       <c r="T648" s="9"/>
@@ -22089,7 +22553,7 @@
       <c r="N649" s="87"/>
       <c r="O649" s="9"/>
       <c r="P649" s="95"/>
-      <c r="Q649" s="4"/>
+      <c r="Q649" s="98"/>
       <c r="R649" s="96"/>
       <c r="S649" s="9"/>
       <c r="T649" s="9"/>
@@ -22111,7 +22575,7 @@
       <c r="N650" s="87"/>
       <c r="O650" s="9"/>
       <c r="P650" s="95"/>
-      <c r="Q650" s="4"/>
+      <c r="Q650" s="98"/>
       <c r="R650" s="96"/>
       <c r="S650" s="9"/>
       <c r="T650" s="9"/>
@@ -22133,7 +22597,7 @@
       <c r="N651" s="87"/>
       <c r="O651" s="9"/>
       <c r="P651" s="95"/>
-      <c r="Q651" s="4"/>
+      <c r="Q651" s="98"/>
       <c r="R651" s="96"/>
       <c r="S651" s="9"/>
       <c r="T651" s="9"/>
@@ -22155,7 +22619,7 @@
       <c r="N652" s="87"/>
       <c r="O652" s="9"/>
       <c r="P652" s="95"/>
-      <c r="Q652" s="4"/>
+      <c r="Q652" s="98"/>
       <c r="R652" s="96"/>
       <c r="S652" s="9"/>
       <c r="T652" s="9"/>
@@ -22177,7 +22641,7 @@
       <c r="N653" s="87"/>
       <c r="O653" s="9"/>
       <c r="P653" s="4"/>
-      <c r="Q653" s="4"/>
+      <c r="Q653" s="98"/>
       <c r="R653" s="96"/>
       <c r="S653" s="9"/>
       <c r="T653" s="9"/>
@@ -22199,7 +22663,7 @@
       <c r="N654" s="87"/>
       <c r="O654" s="9"/>
       <c r="P654" s="4"/>
-      <c r="Q654" s="4"/>
+      <c r="Q654" s="98"/>
       <c r="R654" s="96"/>
       <c r="S654" s="9"/>
       <c r="T654" s="9"/>
@@ -22221,7 +22685,7 @@
       <c r="N655" s="87"/>
       <c r="O655" s="9"/>
       <c r="P655" s="4"/>
-      <c r="Q655" s="4"/>
+      <c r="Q655" s="98"/>
       <c r="R655" s="96"/>
       <c r="S655" s="9"/>
       <c r="T655" s="9"/>
@@ -22243,7 +22707,7 @@
       <c r="N656" s="87"/>
       <c r="O656" s="9"/>
       <c r="P656" s="4"/>
-      <c r="Q656" s="4"/>
+      <c r="Q656" s="98"/>
       <c r="R656" s="96"/>
       <c r="S656" s="9"/>
       <c r="T656" s="9"/>
@@ -23651,7 +24115,7 @@
       <c r="N720" s="87"/>
       <c r="O720" s="97"/>
       <c r="P720" s="98"/>
-      <c r="Q720" s="98"/>
+      <c r="Q720" s="4"/>
       <c r="R720" s="97"/>
       <c r="S720" s="97"/>
       <c r="T720" s="9"/>
@@ -23673,7 +24137,7 @@
       <c r="N721" s="87"/>
       <c r="O721" s="97"/>
       <c r="P721" s="101"/>
-      <c r="Q721" s="98"/>
+      <c r="Q721" s="4"/>
       <c r="R721" s="97"/>
       <c r="S721" s="97"/>
       <c r="T721" s="9"/>
@@ -23981,7 +24445,7 @@
       <c r="N735" s="87"/>
       <c r="O735" s="97"/>
       <c r="P735" s="101"/>
-      <c r="Q735" s="98"/>
+      <c r="Q735" s="4"/>
       <c r="R735" s="97"/>
       <c r="S735" s="97"/>
       <c r="T735" s="9"/>
@@ -24003,7 +24467,7 @@
       <c r="N736" s="87"/>
       <c r="O736" s="97"/>
       <c r="P736" s="101"/>
-      <c r="Q736" s="98"/>
+      <c r="Q736" s="4"/>
       <c r="R736" s="97"/>
       <c r="S736" s="97"/>
       <c r="T736" s="9"/>
@@ -24025,7 +24489,7 @@
       <c r="N737" s="87"/>
       <c r="O737" s="97"/>
       <c r="P737" s="101"/>
-      <c r="Q737" s="98"/>
+      <c r="Q737" s="4"/>
       <c r="R737" s="97"/>
       <c r="S737" s="97"/>
       <c r="T737" s="9"/>
@@ -24047,7 +24511,7 @@
       <c r="N738" s="87"/>
       <c r="O738" s="97"/>
       <c r="P738" s="98"/>
-      <c r="Q738" s="98"/>
+      <c r="Q738" s="4"/>
       <c r="R738" s="97"/>
       <c r="S738" s="97"/>
       <c r="T738" s="9"/>
@@ -24069,7 +24533,7 @@
       <c r="N739" s="87"/>
       <c r="O739" s="97"/>
       <c r="P739" s="98"/>
-      <c r="Q739" s="98"/>
+      <c r="Q739" s="4"/>
       <c r="R739" s="97"/>
       <c r="S739" s="97"/>
       <c r="T739" s="9"/>
@@ -24091,7 +24555,7 @@
       <c r="N740" s="87"/>
       <c r="O740" s="97"/>
       <c r="P740" s="98"/>
-      <c r="Q740" s="98"/>
+      <c r="Q740" s="4"/>
       <c r="R740" s="97"/>
       <c r="S740" s="97"/>
       <c r="T740" s="9"/>
@@ -24157,7 +24621,7 @@
       <c r="N743" s="87"/>
       <c r="O743" s="97"/>
       <c r="P743" s="98"/>
-      <c r="Q743" s="98"/>
+      <c r="Q743" s="4"/>
       <c r="R743" s="97"/>
       <c r="S743" s="97"/>
       <c r="T743" s="9"/>
@@ -24179,7 +24643,7 @@
       <c r="N744" s="87"/>
       <c r="O744" s="97"/>
       <c r="P744" s="98"/>
-      <c r="Q744" s="98"/>
+      <c r="Q744" s="4"/>
       <c r="R744" s="97"/>
       <c r="S744" s="97"/>
       <c r="T744" s="9"/>
@@ -24201,7 +24665,7 @@
       <c r="N745" s="87"/>
       <c r="O745" s="97"/>
       <c r="P745" s="98"/>
-      <c r="Q745" s="98"/>
+      <c r="Q745" s="4"/>
       <c r="R745" s="97"/>
       <c r="S745" s="97"/>
       <c r="T745" s="9"/>
@@ -24223,7 +24687,7 @@
       <c r="N746" s="87"/>
       <c r="O746" s="97"/>
       <c r="P746" s="98"/>
-      <c r="Q746" s="98"/>
+      <c r="Q746" s="4"/>
       <c r="R746" s="97"/>
       <c r="S746" s="97"/>
       <c r="T746" s="9"/>
@@ -24245,7 +24709,7 @@
       <c r="N747" s="87"/>
       <c r="O747" s="97"/>
       <c r="P747" s="98"/>
-      <c r="Q747" s="98"/>
+      <c r="Q747" s="4"/>
       <c r="R747" s="97"/>
       <c r="S747" s="97"/>
       <c r="T747" s="9"/>
@@ -24267,7 +24731,7 @@
       <c r="N748" s="87"/>
       <c r="O748" s="97"/>
       <c r="P748" s="98"/>
-      <c r="Q748" s="98"/>
+      <c r="Q748" s="4"/>
       <c r="R748" s="97"/>
       <c r="S748" s="97"/>
       <c r="T748" s="9"/>
@@ -24289,7 +24753,7 @@
       <c r="N749" s="87"/>
       <c r="O749" s="97"/>
       <c r="P749" s="98"/>
-      <c r="Q749" s="98"/>
+      <c r="Q749" s="4"/>
       <c r="R749" s="97"/>
       <c r="S749" s="97"/>
       <c r="T749" s="9"/>
@@ -24311,7 +24775,7 @@
       <c r="N750" s="87"/>
       <c r="O750" s="97"/>
       <c r="P750" s="98"/>
-      <c r="Q750" s="98"/>
+      <c r="Q750" s="4"/>
       <c r="R750" s="97"/>
       <c r="S750" s="97"/>
       <c r="T750" s="9"/>
@@ -24333,7 +24797,7 @@
       <c r="N751" s="87"/>
       <c r="O751" s="97"/>
       <c r="P751" s="98"/>
-      <c r="Q751" s="98"/>
+      <c r="Q751" s="4"/>
       <c r="R751" s="97"/>
       <c r="S751" s="97"/>
       <c r="T751" s="9"/>
@@ -24355,7 +24819,7 @@
       <c r="N752" s="87"/>
       <c r="O752" s="97"/>
       <c r="P752" s="98"/>
-      <c r="Q752" s="98"/>
+      <c r="Q752" s="4"/>
       <c r="R752" s="97"/>
       <c r="S752" s="97"/>
       <c r="T752" s="9"/>
@@ -24377,7 +24841,7 @@
       <c r="N753" s="109"/>
       <c r="O753" s="97"/>
       <c r="P753" s="98"/>
-      <c r="Q753" s="98"/>
+      <c r="Q753" s="4"/>
       <c r="R753" s="97"/>
       <c r="S753" s="97"/>
       <c r="T753" s="9"/>
@@ -24399,7 +24863,7 @@
       <c r="N754" s="109"/>
       <c r="O754" s="97"/>
       <c r="P754" s="98"/>
-      <c r="Q754" s="98"/>
+      <c r="Q754" s="4"/>
       <c r="R754" s="97"/>
       <c r="S754" s="97"/>
       <c r="T754" s="9"/>
@@ -24421,7 +24885,7 @@
       <c r="N755" s="109"/>
       <c r="O755" s="97"/>
       <c r="P755" s="98"/>
-      <c r="Q755" s="98"/>
+      <c r="Q755" s="4"/>
       <c r="R755" s="97"/>
       <c r="S755" s="97"/>
       <c r="T755" s="9"/>
@@ -26269,7 +26733,6 @@
       <c r="N839" s="4"/>
       <c r="O839" s="9"/>
       <c r="P839" s="4"/>
-      <c r="Q839" s="4"/>
       <c r="R839" s="9"/>
       <c r="S839" s="9"/>
       <c r="T839" s="9"/>
@@ -26291,7 +26754,6 @@
       <c r="N840" s="4"/>
       <c r="O840" s="9"/>
       <c r="P840" s="4"/>
-      <c r="Q840" s="4"/>
       <c r="R840" s="9"/>
       <c r="S840" s="9"/>
       <c r="T840" s="9"/>
@@ -26313,7 +26775,6 @@
       <c r="N841" s="4"/>
       <c r="O841" s="9"/>
       <c r="P841" s="4"/>
-      <c r="Q841" s="4"/>
       <c r="R841" s="9"/>
       <c r="S841" s="9"/>
       <c r="T841" s="9"/>
@@ -26335,7 +26796,6 @@
       <c r="N842" s="4"/>
       <c r="O842" s="9"/>
       <c r="P842" s="4"/>
-      <c r="Q842" s="4"/>
       <c r="R842" s="9"/>
       <c r="S842" s="9"/>
       <c r="T842" s="9"/>
@@ -26357,7 +26817,6 @@
       <c r="N843" s="4"/>
       <c r="O843" s="9"/>
       <c r="P843" s="4"/>
-      <c r="Q843" s="4"/>
       <c r="R843" s="9"/>
       <c r="S843" s="9"/>
       <c r="T843" s="9"/>
@@ -26379,7 +26838,6 @@
       <c r="N844" s="4"/>
       <c r="O844" s="9"/>
       <c r="P844" s="4"/>
-      <c r="Q844" s="4"/>
       <c r="R844" s="9"/>
       <c r="S844" s="9"/>
       <c r="T844" s="9"/>
@@ -26401,7 +26859,6 @@
       <c r="N845" s="4"/>
       <c r="O845" s="9"/>
       <c r="P845" s="4"/>
-      <c r="Q845" s="4"/>
       <c r="R845" s="9"/>
       <c r="S845" s="9"/>
       <c r="T845" s="9"/>
@@ -26423,7 +26880,6 @@
       <c r="N846" s="4"/>
       <c r="O846" s="9"/>
       <c r="P846" s="4"/>
-      <c r="Q846" s="4"/>
       <c r="R846" s="9"/>
       <c r="S846" s="9"/>
       <c r="T846" s="9"/>
@@ -26445,7 +26901,6 @@
       <c r="N847" s="4"/>
       <c r="O847" s="9"/>
       <c r="P847" s="4"/>
-      <c r="Q847" s="4"/>
       <c r="R847" s="9"/>
       <c r="S847" s="9"/>
       <c r="T847" s="9"/>
@@ -26467,7 +26922,6 @@
       <c r="N848" s="4"/>
       <c r="O848" s="9"/>
       <c r="P848" s="4"/>
-      <c r="Q848" s="4"/>
       <c r="R848" s="9"/>
       <c r="S848" s="9"/>
       <c r="T848" s="9"/>
@@ -26489,7 +26943,6 @@
       <c r="N849" s="4"/>
       <c r="O849" s="9"/>
       <c r="P849" s="4"/>
-      <c r="Q849" s="4"/>
       <c r="R849" s="9"/>
       <c r="S849" s="9"/>
       <c r="T849" s="9"/>
@@ -26511,7 +26964,6 @@
       <c r="N850" s="4"/>
       <c r="O850" s="9"/>
       <c r="P850" s="4"/>
-      <c r="Q850" s="4"/>
       <c r="R850" s="9"/>
       <c r="S850" s="9"/>
       <c r="T850" s="9"/>
@@ -26533,7 +26985,6 @@
       <c r="N851" s="4"/>
       <c r="O851" s="9"/>
       <c r="P851" s="4"/>
-      <c r="Q851" s="4"/>
       <c r="R851" s="9"/>
       <c r="S851" s="9"/>
       <c r="T851" s="9"/>
@@ -26555,7 +27006,6 @@
       <c r="N852" s="4"/>
       <c r="O852" s="9"/>
       <c r="P852" s="4"/>
-      <c r="Q852" s="4"/>
       <c r="R852" s="9"/>
       <c r="S852" s="9"/>
       <c r="T852" s="9"/>
@@ -26577,7 +27027,6 @@
       <c r="N853" s="4"/>
       <c r="O853" s="9"/>
       <c r="P853" s="4"/>
-      <c r="Q853" s="4"/>
       <c r="R853" s="9"/>
       <c r="S853" s="9"/>
       <c r="T853" s="9"/>
@@ -26599,7 +27048,6 @@
       <c r="N854" s="4"/>
       <c r="O854" s="9"/>
       <c r="P854" s="4"/>
-      <c r="Q854" s="4"/>
       <c r="R854" s="9"/>
       <c r="S854" s="9"/>
       <c r="T854" s="9"/>
@@ -26621,7 +27069,6 @@
       <c r="N855" s="4"/>
       <c r="O855" s="9"/>
       <c r="P855" s="4"/>
-      <c r="Q855" s="4"/>
       <c r="R855" s="9"/>
       <c r="S855" s="9"/>
       <c r="T855" s="9"/>
@@ -26643,7 +27090,6 @@
       <c r="N856" s="4"/>
       <c r="O856" s="9"/>
       <c r="P856" s="4"/>
-      <c r="Q856" s="4"/>
       <c r="R856" s="9"/>
       <c r="S856" s="9"/>
       <c r="T856" s="9"/>
@@ -26665,7 +27111,6 @@
       <c r="N857" s="4"/>
       <c r="O857" s="9"/>
       <c r="P857" s="4"/>
-      <c r="Q857" s="4"/>
       <c r="R857" s="9"/>
       <c r="S857" s="9"/>
       <c r="T857" s="9"/>
@@ -26687,7 +27132,6 @@
       <c r="N858" s="4"/>
       <c r="O858" s="9"/>
       <c r="P858" s="4"/>
-      <c r="Q858" s="4"/>
       <c r="R858" s="9"/>
       <c r="S858" s="9"/>
       <c r="T858" s="9"/>
@@ -26709,13 +27153,17 @@
       <c r="N859" s="4"/>
       <c r="O859" s="9"/>
       <c r="P859" s="4"/>
-      <c r="Q859" s="4"/>
       <c r="R859" s="9"/>
       <c r="S859" s="9"/>
       <c r="T859" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -26730,11 +27178,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matchemphys.2024.130114`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5E6F29-D34D-1B40-B4DB-0AC062FA0F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65F868A-1F7B-074E-AF02-669F60CBF640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="3540" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4540" yWindow="6080" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="306">
   <si>
     <r>
       <rPr>
@@ -1033,6 +1033,21 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2023.168975</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchemphys.2024.130114</t>
+  </si>
+  <si>
+    <t>Ti35 Zr35 Nb20 Ta5 Ag5</t>
+  </si>
+  <si>
+    <t>MA+CIP+S</t>
+  </si>
+  <si>
+    <t>BioHEA 1; mechanical alloying for 2h followed by CIP under 700MPa and 2h sintering in Ar at 1573K</t>
+  </si>
+  <si>
+    <t>BCC+BCC</t>
   </si>
 </sst>
 </file>
@@ -3373,8 +3388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E211" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N242" sqref="N242"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A223" zoomScale="86" workbookViewId="0">
+      <selection activeCell="M252" sqref="M252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -13496,19 +13511,39 @@
     </row>
     <row r="238" spans="1:20" ht="18" customHeight="1">
       <c r="A238" s="64"/>
-      <c r="B238" s="73"/>
-      <c r="C238" s="68"/>
-      <c r="D238" s="68"/>
-      <c r="E238" s="73"/>
-      <c r="F238" s="68"/>
-      <c r="G238" s="68"/>
+      <c r="B238" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="C238" s="112" t="s">
+        <v>305</v>
+      </c>
+      <c r="D238" s="112" t="s">
+        <v>303</v>
+      </c>
+      <c r="E238" s="111" t="s">
+        <v>304</v>
+      </c>
+      <c r="F238" s="112" t="s">
+        <v>67</v>
+      </c>
+      <c r="G238" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H238" s="68"/>
-      <c r="I238" s="83"/>
-      <c r="J238" s="70"/>
+      <c r="I238" s="83">
+        <v>298</v>
+      </c>
+      <c r="J238" s="70">
+        <v>6255</v>
+      </c>
       <c r="K238" s="70"/>
-      <c r="L238" s="68"/>
+      <c r="L238" s="112" t="s">
+        <v>68</v>
+      </c>
       <c r="M238" s="68"/>
-      <c r="N238" s="68"/>
+      <c r="N238" s="112" t="s">
+        <v>301</v>
+      </c>
       <c r="O238" s="9"/>
       <c r="P238" s="4"/>
       <c r="Q238" s="4"/>
@@ -13518,19 +13553,39 @@
     </row>
     <row r="239" spans="1:20" ht="18" customHeight="1">
       <c r="A239" s="64"/>
-      <c r="B239" s="73"/>
-      <c r="C239" s="68"/>
-      <c r="D239" s="68"/>
-      <c r="E239" s="73"/>
-      <c r="F239" s="68"/>
-      <c r="G239" s="68"/>
+      <c r="B239" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="C239" s="112" t="s">
+        <v>305</v>
+      </c>
+      <c r="D239" s="112" t="s">
+        <v>303</v>
+      </c>
+      <c r="E239" s="111" t="s">
+        <v>304</v>
+      </c>
+      <c r="F239" s="112" t="s">
+        <v>67</v>
+      </c>
+      <c r="G239" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H239" s="68"/>
-      <c r="I239" s="83"/>
-      <c r="J239" s="70"/>
+      <c r="I239" s="83">
+        <v>298</v>
+      </c>
+      <c r="J239" s="70">
+        <v>6508</v>
+      </c>
       <c r="K239" s="70"/>
-      <c r="L239" s="68"/>
+      <c r="L239" s="112" t="s">
+        <v>68</v>
+      </c>
       <c r="M239" s="68"/>
-      <c r="N239" s="68"/>
+      <c r="N239" s="112" t="s">
+        <v>301</v>
+      </c>
       <c r="O239" s="9"/>
       <c r="P239" s="4"/>
       <c r="Q239" s="4"/>
@@ -13540,19 +13595,41 @@
     </row>
     <row r="240" spans="1:20" ht="18" customHeight="1">
       <c r="A240" s="64"/>
-      <c r="B240" s="73"/>
-      <c r="C240" s="68"/>
-      <c r="D240" s="68"/>
-      <c r="E240" s="73"/>
-      <c r="F240" s="68"/>
-      <c r="G240" s="68"/>
+      <c r="B240" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="C240" s="112" t="s">
+        <v>305</v>
+      </c>
+      <c r="D240" s="112" t="s">
+        <v>303</v>
+      </c>
+      <c r="E240" s="111" t="s">
+        <v>304</v>
+      </c>
+      <c r="F240" s="112" t="s">
+        <v>91</v>
+      </c>
+      <c r="G240" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H240" s="68"/>
-      <c r="I240" s="83"/>
-      <c r="J240" s="70"/>
-      <c r="K240" s="70"/>
-      <c r="L240" s="68"/>
+      <c r="I240" s="83">
+        <v>298</v>
+      </c>
+      <c r="J240" s="70">
+        <v>87900000000</v>
+      </c>
+      <c r="K240" s="70">
+        <v>6300000000</v>
+      </c>
+      <c r="L240" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M240" s="68"/>
-      <c r="N240" s="68"/>
+      <c r="N240" s="112" t="s">
+        <v>301</v>
+      </c>
       <c r="O240" s="9"/>
       <c r="P240" s="4"/>
       <c r="Q240" s="4"/>
@@ -13562,19 +13639,41 @@
     </row>
     <row r="241" spans="1:20" ht="18" customHeight="1">
       <c r="A241" s="64"/>
-      <c r="B241" s="73"/>
-      <c r="C241" s="68"/>
-      <c r="D241" s="68"/>
-      <c r="E241" s="73"/>
-      <c r="F241" s="68"/>
-      <c r="G241" s="68"/>
+      <c r="B241" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="C241" s="112" t="s">
+        <v>305</v>
+      </c>
+      <c r="D241" s="112" t="s">
+        <v>303</v>
+      </c>
+      <c r="E241" s="111" t="s">
+        <v>304</v>
+      </c>
+      <c r="F241" s="112" t="s">
+        <v>91</v>
+      </c>
+      <c r="G241" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H241" s="68"/>
-      <c r="I241" s="83"/>
-      <c r="J241" s="70"/>
-      <c r="K241" s="70"/>
-      <c r="L241" s="68"/>
+      <c r="I241" s="83">
+        <v>298</v>
+      </c>
+      <c r="J241" s="70">
+        <v>113300000000</v>
+      </c>
+      <c r="K241" s="70">
+        <v>13100000000</v>
+      </c>
+      <c r="L241" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M241" s="68"/>
-      <c r="N241" s="68"/>
+      <c r="N241" s="112" t="s">
+        <v>301</v>
+      </c>
       <c r="O241" s="9"/>
       <c r="P241" s="4"/>
       <c r="Q241" s="4"/>
@@ -13584,19 +13683,39 @@
     </row>
     <row r="242" spans="1:20" ht="18" customHeight="1">
       <c r="A242" s="64"/>
-      <c r="B242" s="73"/>
-      <c r="C242" s="68"/>
-      <c r="D242" s="68"/>
-      <c r="E242" s="73"/>
-      <c r="F242" s="68"/>
-      <c r="G242" s="68"/>
+      <c r="B242" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="C242" s="112" t="s">
+        <v>305</v>
+      </c>
+      <c r="D242" s="112" t="s">
+        <v>303</v>
+      </c>
+      <c r="E242" s="111" t="s">
+        <v>304</v>
+      </c>
+      <c r="F242" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="G242" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H242" s="68"/>
-      <c r="I242" s="83"/>
-      <c r="J242" s="70"/>
+      <c r="I242" s="83">
+        <v>298</v>
+      </c>
+      <c r="J242" s="70">
+        <v>3930000000</v>
+      </c>
       <c r="K242" s="70"/>
-      <c r="L242" s="68"/>
+      <c r="L242" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M242" s="68"/>
-      <c r="N242" s="68"/>
+      <c r="N242" s="112" t="s">
+        <v>301</v>
+      </c>
       <c r="O242" s="9"/>
       <c r="P242" s="4"/>
       <c r="Q242" s="4"/>
@@ -13606,19 +13725,39 @@
     </row>
     <row r="243" spans="1:20" ht="18" customHeight="1">
       <c r="A243" s="64"/>
-      <c r="B243" s="73"/>
-      <c r="C243" s="68"/>
-      <c r="D243" s="68"/>
-      <c r="E243" s="73"/>
-      <c r="F243" s="68"/>
-      <c r="G243" s="68"/>
+      <c r="B243" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="C243" s="112" t="s">
+        <v>305</v>
+      </c>
+      <c r="D243" s="112" t="s">
+        <v>303</v>
+      </c>
+      <c r="E243" s="111" t="s">
+        <v>304</v>
+      </c>
+      <c r="F243" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="G243" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H243" s="68"/>
-      <c r="I243" s="83"/>
-      <c r="J243" s="70"/>
+      <c r="I243" s="83">
+        <v>298</v>
+      </c>
+      <c r="J243" s="70">
+        <v>5188000000</v>
+      </c>
       <c r="K243" s="70"/>
-      <c r="L243" s="68"/>
+      <c r="L243" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M243" s="68"/>
-      <c r="N243" s="68"/>
+      <c r="N243" s="112" t="s">
+        <v>301</v>
+      </c>
       <c r="O243" s="9"/>
       <c r="P243" s="4"/>
       <c r="Q243" s="4"/>
@@ -13633,7 +13772,7 @@
       <c r="D244" s="68"/>
       <c r="E244" s="73"/>
       <c r="F244" s="68"/>
-      <c r="G244" s="68"/>
+      <c r="G244" s="112"/>
       <c r="H244" s="68"/>
       <c r="I244" s="83"/>
       <c r="J244" s="70"/>
@@ -13655,7 +13794,7 @@
       <c r="D245" s="68"/>
       <c r="E245" s="73"/>
       <c r="F245" s="68"/>
-      <c r="G245" s="68"/>
+      <c r="G245" s="112"/>
       <c r="H245" s="68"/>
       <c r="I245" s="83"/>
       <c r="J245" s="70"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jmrt.2024.06.209`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65F868A-1F7B-074E-AF02-669F60CBF640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5B946B-BD78-7740-8F8A-663E4A2BD3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="6080" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11080" yWindow="6300" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="313">
   <si>
     <r>
       <rPr>
@@ -1048,6 +1048,27 @@
   </si>
   <si>
     <t>BCC+BCC</t>
+  </si>
+  <si>
+    <t>CoCrFeNiCe0.1</t>
+  </si>
+  <si>
+    <t>CoCrFeNiCe0.3</t>
+  </si>
+  <si>
+    <t>CoCrFeNiCe0.5</t>
+  </si>
+  <si>
+    <t>CoCrFeNi</t>
+  </si>
+  <si>
+    <t>FCC+CeNi3</t>
+  </si>
+  <si>
+    <t>FCC+CeNi3+FCC</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmrt.2024.06.209</t>
   </si>
 </sst>
 </file>
@@ -3388,8 +3409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A223" zoomScale="86" workbookViewId="0">
-      <selection activeCell="M252" sqref="M252"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A231" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N251" sqref="N251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -13767,88 +13788,200 @@
     </row>
     <row r="244" spans="1:20" ht="18" customHeight="1">
       <c r="A244" s="64"/>
-      <c r="B244" s="73"/>
-      <c r="C244" s="68"/>
-      <c r="D244" s="68"/>
+      <c r="B244" s="111" t="s">
+        <v>309</v>
+      </c>
+      <c r="C244" s="112" t="s">
+        <v>89</v>
+      </c>
+      <c r="D244" s="112" t="s">
+        <v>134</v>
+      </c>
       <c r="E244" s="73"/>
-      <c r="F244" s="68"/>
-      <c r="G244" s="112"/>
+      <c r="F244" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="G244" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H244" s="68"/>
-      <c r="I244" s="83"/>
-      <c r="J244" s="70"/>
-      <c r="K244" s="70"/>
-      <c r="L244" s="68"/>
-      <c r="M244" s="68"/>
-      <c r="N244" s="68"/>
+      <c r="I244" s="83">
+        <v>298</v>
+      </c>
+      <c r="J244" s="70">
+        <f t="shared" ref="J244:K247" si="7">P244*9807000</f>
+        <v>1321983600</v>
+      </c>
+      <c r="K244" s="70">
+        <f t="shared" si="7"/>
+        <v>52957800</v>
+      </c>
+      <c r="L244" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M244" s="112" t="s">
+        <v>254</v>
+      </c>
+      <c r="N244" s="112" t="s">
+        <v>312</v>
+      </c>
       <c r="O244" s="9"/>
-      <c r="P244" s="4"/>
-      <c r="Q244" s="4"/>
+      <c r="P244" s="4">
+        <v>134.80000000000001</v>
+      </c>
+      <c r="Q244" s="4">
+        <v>5.4</v>
+      </c>
       <c r="R244" s="9"/>
       <c r="S244" s="9"/>
       <c r="T244" s="9"/>
     </row>
     <row r="245" spans="1:20" ht="18" customHeight="1">
       <c r="A245" s="64"/>
-      <c r="B245" s="73"/>
-      <c r="C245" s="68"/>
-      <c r="D245" s="68"/>
+      <c r="B245" s="111" t="s">
+        <v>306</v>
+      </c>
+      <c r="C245" s="112" t="s">
+        <v>310</v>
+      </c>
+      <c r="D245" s="112" t="s">
+        <v>134</v>
+      </c>
       <c r="E245" s="73"/>
-      <c r="F245" s="68"/>
-      <c r="G245" s="112"/>
+      <c r="F245" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="G245" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H245" s="68"/>
-      <c r="I245" s="83"/>
-      <c r="J245" s="70"/>
-      <c r="K245" s="70"/>
-      <c r="L245" s="68"/>
-      <c r="M245" s="68"/>
-      <c r="N245" s="68"/>
+      <c r="I245" s="83">
+        <v>298</v>
+      </c>
+      <c r="J245" s="70">
+        <f t="shared" si="7"/>
+        <v>1995724500</v>
+      </c>
+      <c r="K245" s="70">
+        <f t="shared" si="7"/>
+        <v>40208700</v>
+      </c>
+      <c r="L245" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M245" s="112" t="s">
+        <v>254</v>
+      </c>
+      <c r="N245" s="112" t="s">
+        <v>312</v>
+      </c>
       <c r="O245" s="9"/>
-      <c r="P245" s="4"/>
-      <c r="Q245" s="4"/>
+      <c r="P245" s="4">
+        <v>203.5</v>
+      </c>
+      <c r="Q245" s="4">
+        <v>4.0999999999999996</v>
+      </c>
       <c r="R245" s="9"/>
       <c r="S245" s="9"/>
       <c r="T245" s="9"/>
     </row>
     <row r="246" spans="1:20" ht="18" customHeight="1">
       <c r="A246" s="64"/>
-      <c r="B246" s="73"/>
-      <c r="C246" s="68"/>
-      <c r="D246" s="68"/>
+      <c r="B246" s="111" t="s">
+        <v>307</v>
+      </c>
+      <c r="C246" s="112" t="s">
+        <v>310</v>
+      </c>
+      <c r="D246" s="112" t="s">
+        <v>134</v>
+      </c>
       <c r="E246" s="73"/>
-      <c r="F246" s="68"/>
-      <c r="G246" s="68"/>
+      <c r="F246" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="G246" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H246" s="68"/>
-      <c r="I246" s="83"/>
-      <c r="J246" s="70"/>
-      <c r="K246" s="70"/>
-      <c r="L246" s="68"/>
-      <c r="M246" s="68"/>
-      <c r="N246" s="68"/>
+      <c r="I246" s="83">
+        <v>298</v>
+      </c>
+      <c r="J246" s="70">
+        <f t="shared" si="7"/>
+        <v>3274557300</v>
+      </c>
+      <c r="K246" s="70">
+        <f t="shared" si="7"/>
+        <v>167699700</v>
+      </c>
+      <c r="L246" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M246" s="112" t="s">
+        <v>254</v>
+      </c>
+      <c r="N246" s="112" t="s">
+        <v>312</v>
+      </c>
       <c r="O246" s="9"/>
-      <c r="P246" s="4"/>
-      <c r="Q246" s="4"/>
+      <c r="P246" s="4">
+        <v>333.9</v>
+      </c>
+      <c r="Q246" s="4">
+        <v>17.100000000000001</v>
+      </c>
       <c r="R246" s="9"/>
       <c r="S246" s="9"/>
       <c r="T246" s="9"/>
     </row>
     <row r="247" spans="1:20" ht="18" customHeight="1">
       <c r="A247" s="64"/>
-      <c r="B247" s="73"/>
-      <c r="C247" s="68"/>
-      <c r="D247" s="68"/>
+      <c r="B247" s="111" t="s">
+        <v>308</v>
+      </c>
+      <c r="C247" s="112" t="s">
+        <v>311</v>
+      </c>
+      <c r="D247" s="112" t="s">
+        <v>134</v>
+      </c>
       <c r="E247" s="73"/>
-      <c r="F247" s="68"/>
-      <c r="G247" s="68"/>
+      <c r="F247" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="G247" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H247" s="68"/>
-      <c r="I247" s="83"/>
-      <c r="J247" s="70"/>
-      <c r="K247" s="70"/>
-      <c r="L247" s="68"/>
-      <c r="M247" s="68"/>
-      <c r="N247" s="68"/>
+      <c r="I247" s="83">
+        <v>298</v>
+      </c>
+      <c r="J247" s="70">
+        <f t="shared" si="7"/>
+        <v>3752158200</v>
+      </c>
+      <c r="K247" s="70">
+        <f t="shared" si="7"/>
+        <v>170641800</v>
+      </c>
+      <c r="L247" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M247" s="112" t="s">
+        <v>254</v>
+      </c>
+      <c r="N247" s="112" t="s">
+        <v>312</v>
+      </c>
       <c r="O247" s="9"/>
-      <c r="P247" s="4"/>
-      <c r="Q247" s="4"/>
+      <c r="P247" s="4">
+        <v>382.6</v>
+      </c>
+      <c r="Q247" s="4">
+        <v>17.399999999999999</v>
+      </c>
       <c r="R247" s="9"/>
       <c r="S247" s="9"/>
       <c r="T247" s="9"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jmst.2024.01.046`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5B946B-BD78-7740-8F8A-663E4A2BD3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8B2456-5E36-3E40-A86C-F4DEEB70C537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11080" yWindow="6300" windowWidth="27740" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="331">
   <si>
     <r>
       <rPr>
@@ -1069,6 +1069,60 @@
   </si>
   <si>
     <t>10.1016/j.jmrt.2024.06.209</t>
+  </si>
+  <si>
+    <t>Nb0.5TiZrV0.5</t>
+  </si>
+  <si>
+    <t>(Nb16.67 Ti33.33 Zr33.33 V16.67)0.995 Ce0.005</t>
+  </si>
+  <si>
+    <t>(Nb16.67 Ti33.33 Zr33.33 V16.67)0.99 Ce0.01</t>
+  </si>
+  <si>
+    <t>0.005Ce</t>
+  </si>
+  <si>
+    <t>0.01Ce</t>
+  </si>
+  <si>
+    <t>0Ce</t>
+  </si>
+  <si>
+    <t>BCC+C32</t>
+  </si>
+  <si>
+    <t>C32 is Ce-rich omega-like phase formed in RHEAs</t>
+  </si>
+  <si>
+    <t>tensile yield stress</t>
+  </si>
+  <si>
+    <t>tensile ductility</t>
+  </si>
+  <si>
+    <t>UTS</t>
+  </si>
+  <si>
+    <t>F5a</t>
+  </si>
+  <si>
+    <t>F5b</t>
+  </si>
+  <si>
+    <t>estimated tensile ductility</t>
+  </si>
+  <si>
+    <t>(Nb16.67 Ti33.33 Zr33.33 V16.67)0.97 Ce0.03</t>
+  </si>
+  <si>
+    <t>(Nb16.67 Ti33.33 Zr33.33 V16.67)0.95 Ce0.05</t>
+  </si>
+  <si>
+    <t>manufactured and tested but not fully discussed in the manuscript due to near-zero ductility</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmst.2024.01.046</t>
   </si>
 </sst>
 </file>
@@ -1881,7 +1935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2247,6 +2301,9 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3409,8 +3466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A231" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N251" sqref="N251"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A235" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N264" sqref="N264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -13987,20 +14044,42 @@
       <c r="T247" s="9"/>
     </row>
     <row r="248" spans="1:20" ht="18" customHeight="1">
-      <c r="A248" s="64"/>
-      <c r="B248" s="73"/>
-      <c r="C248" s="68"/>
-      <c r="D248" s="68"/>
+      <c r="A248" s="116" t="s">
+        <v>318</v>
+      </c>
+      <c r="B248" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="C248" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D248" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E248" s="73"/>
-      <c r="F248" s="68"/>
-      <c r="G248" s="68"/>
+      <c r="F248" s="112" t="s">
+        <v>321</v>
+      </c>
+      <c r="G248" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H248" s="68"/>
-      <c r="I248" s="83"/>
-      <c r="J248" s="70"/>
+      <c r="I248" s="83">
+        <v>298</v>
+      </c>
+      <c r="J248" s="70">
+        <v>985400000</v>
+      </c>
       <c r="K248" s="70"/>
-      <c r="L248" s="68"/>
-      <c r="M248" s="68"/>
-      <c r="N248" s="68"/>
+      <c r="L248" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M248" s="112" t="s">
+        <v>324</v>
+      </c>
+      <c r="N248" s="112" t="s">
+        <v>330</v>
+      </c>
       <c r="O248" s="9"/>
       <c r="P248" s="4"/>
       <c r="Q248" s="4"/>
@@ -14009,20 +14088,42 @@
       <c r="T248" s="9"/>
     </row>
     <row r="249" spans="1:20" ht="18" customHeight="1">
-      <c r="A249" s="64"/>
-      <c r="B249" s="73"/>
-      <c r="C249" s="68"/>
-      <c r="D249" s="68"/>
+      <c r="A249" s="116" t="s">
+        <v>316</v>
+      </c>
+      <c r="B249" s="111" t="s">
+        <v>314</v>
+      </c>
+      <c r="C249" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D249" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E249" s="73"/>
-      <c r="F249" s="68"/>
-      <c r="G249" s="68"/>
+      <c r="F249" s="112" t="s">
+        <v>321</v>
+      </c>
+      <c r="G249" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H249" s="68"/>
-      <c r="I249" s="83"/>
-      <c r="J249" s="70"/>
+      <c r="I249" s="83">
+        <v>298</v>
+      </c>
+      <c r="J249" s="70">
+        <v>963800000</v>
+      </c>
       <c r="K249" s="70"/>
-      <c r="L249" s="68"/>
-      <c r="M249" s="68"/>
-      <c r="N249" s="68"/>
+      <c r="L249" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M249" s="112" t="s">
+        <v>324</v>
+      </c>
+      <c r="N249" s="112" t="s">
+        <v>330</v>
+      </c>
       <c r="O249" s="9"/>
       <c r="P249" s="4"/>
       <c r="Q249" s="4"/>
@@ -14031,20 +14132,44 @@
       <c r="T249" s="9"/>
     </row>
     <row r="250" spans="1:20" ht="18" customHeight="1">
-      <c r="A250" s="64"/>
-      <c r="B250" s="73"/>
-      <c r="C250" s="68"/>
-      <c r="D250" s="68"/>
-      <c r="E250" s="73"/>
-      <c r="F250" s="68"/>
-      <c r="G250" s="68"/>
+      <c r="A250" s="116" t="s">
+        <v>317</v>
+      </c>
+      <c r="B250" s="111" t="s">
+        <v>315</v>
+      </c>
+      <c r="C250" s="112" t="s">
+        <v>319</v>
+      </c>
+      <c r="D250" s="112" t="s">
+        <v>113</v>
+      </c>
+      <c r="E250" s="111" t="s">
+        <v>320</v>
+      </c>
+      <c r="F250" s="112" t="s">
+        <v>321</v>
+      </c>
+      <c r="G250" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H250" s="68"/>
-      <c r="I250" s="83"/>
-      <c r="J250" s="70"/>
+      <c r="I250" s="83">
+        <v>298</v>
+      </c>
+      <c r="J250" s="70">
+        <v>979000000</v>
+      </c>
       <c r="K250" s="70"/>
-      <c r="L250" s="68"/>
-      <c r="M250" s="68"/>
-      <c r="N250" s="68"/>
+      <c r="L250" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M250" s="112" t="s">
+        <v>324</v>
+      </c>
+      <c r="N250" s="112" t="s">
+        <v>330</v>
+      </c>
       <c r="O250" s="9"/>
       <c r="P250" s="4"/>
       <c r="Q250" s="4"/>
@@ -14053,86 +14178,173 @@
       <c r="T250" s="9"/>
     </row>
     <row r="251" spans="1:20" ht="18" customHeight="1">
-      <c r="A251" s="64"/>
-      <c r="B251" s="73"/>
-      <c r="C251" s="68"/>
-      <c r="D251" s="68"/>
+      <c r="A251" s="116" t="s">
+        <v>318</v>
+      </c>
+      <c r="B251" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="C251" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D251" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E251" s="73"/>
-      <c r="F251" s="68"/>
-      <c r="G251" s="68"/>
+      <c r="F251" s="112" t="s">
+        <v>323</v>
+      </c>
+      <c r="G251" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H251" s="68"/>
-      <c r="I251" s="83"/>
-      <c r="J251" s="70"/>
-      <c r="K251" s="70"/>
-      <c r="L251" s="68"/>
-      <c r="M251" s="68"/>
-      <c r="N251" s="68"/>
-      <c r="O251" s="9"/>
+      <c r="I251" s="83">
+        <v>298</v>
+      </c>
+      <c r="J251" s="70">
+        <v>1018000000</v>
+      </c>
+      <c r="K251" s="68"/>
+      <c r="L251" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M251" s="112" t="s">
+        <v>325</v>
+      </c>
+      <c r="N251" s="112" t="s">
+        <v>330</v>
+      </c>
+      <c r="O251" s="4"/>
       <c r="P251" s="4"/>
-      <c r="Q251" s="4"/>
+      <c r="Q251" s="9"/>
       <c r="R251" s="9"/>
       <c r="S251" s="9"/>
-      <c r="T251" s="9"/>
     </row>
     <row r="252" spans="1:20" ht="18" customHeight="1">
-      <c r="A252" s="64"/>
-      <c r="B252" s="73"/>
-      <c r="C252" s="68"/>
-      <c r="D252" s="68"/>
+      <c r="A252" s="116" t="s">
+        <v>316</v>
+      </c>
+      <c r="B252" s="111" t="s">
+        <v>314</v>
+      </c>
+      <c r="C252" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D252" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E252" s="73"/>
-      <c r="F252" s="68"/>
-      <c r="G252" s="68"/>
+      <c r="F252" s="112" t="s">
+        <v>323</v>
+      </c>
+      <c r="G252" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H252" s="68"/>
-      <c r="I252" s="83"/>
-      <c r="J252" s="70"/>
-      <c r="K252" s="70"/>
-      <c r="L252" s="68"/>
-      <c r="M252" s="68"/>
-      <c r="N252" s="68"/>
-      <c r="O252" s="9"/>
+      <c r="I252" s="83">
+        <v>298</v>
+      </c>
+      <c r="J252" s="70">
+        <v>1009000000</v>
+      </c>
+      <c r="K252" s="68"/>
+      <c r="L252" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M252" s="112" t="s">
+        <v>325</v>
+      </c>
+      <c r="N252" s="112" t="s">
+        <v>330</v>
+      </c>
+      <c r="O252" s="4"/>
       <c r="P252" s="4"/>
-      <c r="Q252" s="4"/>
+      <c r="Q252" s="9"/>
       <c r="R252" s="9"/>
       <c r="S252" s="9"/>
-      <c r="T252" s="9"/>
     </row>
     <row r="253" spans="1:20" ht="18" customHeight="1">
-      <c r="A253" s="64"/>
-      <c r="B253" s="73"/>
-      <c r="C253" s="68"/>
-      <c r="D253" s="68"/>
-      <c r="E253" s="73"/>
-      <c r="F253" s="68"/>
-      <c r="G253" s="68"/>
+      <c r="A253" s="116" t="s">
+        <v>317</v>
+      </c>
+      <c r="B253" s="111" t="s">
+        <v>315</v>
+      </c>
+      <c r="C253" s="112" t="s">
+        <v>319</v>
+      </c>
+      <c r="D253" s="112" t="s">
+        <v>113</v>
+      </c>
+      <c r="E253" s="111" t="s">
+        <v>320</v>
+      </c>
+      <c r="F253" s="112" t="s">
+        <v>323</v>
+      </c>
+      <c r="G253" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H253" s="68"/>
-      <c r="I253" s="83"/>
-      <c r="J253" s="70"/>
-      <c r="K253" s="70"/>
-      <c r="L253" s="68"/>
-      <c r="M253" s="68"/>
-      <c r="N253" s="68"/>
-      <c r="O253" s="9"/>
+      <c r="I253" s="83">
+        <v>298</v>
+      </c>
+      <c r="J253" s="70">
+        <v>1000000000</v>
+      </c>
+      <c r="K253" s="68"/>
+      <c r="L253" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M253" s="112" t="s">
+        <v>325</v>
+      </c>
+      <c r="N253" s="112" t="s">
+        <v>330</v>
+      </c>
+      <c r="O253" s="4"/>
       <c r="P253" s="4"/>
-      <c r="Q253" s="4"/>
+      <c r="Q253" s="9"/>
       <c r="R253" s="9"/>
       <c r="S253" s="9"/>
-      <c r="T253" s="9"/>
     </row>
     <row r="254" spans="1:20" ht="18" customHeight="1">
-      <c r="A254" s="64"/>
-      <c r="B254" s="73"/>
-      <c r="C254" s="68"/>
-      <c r="D254" s="68"/>
+      <c r="A254" s="116" t="s">
+        <v>318</v>
+      </c>
+      <c r="B254" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="C254" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D254" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E254" s="73"/>
-      <c r="F254" s="68"/>
-      <c r="G254" s="68"/>
+      <c r="F254" s="112" t="s">
+        <v>322</v>
+      </c>
+      <c r="G254" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H254" s="68"/>
-      <c r="I254" s="83"/>
-      <c r="J254" s="70"/>
-      <c r="K254" s="70"/>
-      <c r="L254" s="68"/>
+      <c r="I254" s="83">
+        <v>298</v>
+      </c>
+      <c r="J254" s="70">
+        <v>4.32</v>
+      </c>
+      <c r="K254" s="70">
+        <v>0.34</v>
+      </c>
+      <c r="L254" s="112" t="s">
+        <v>171</v>
+      </c>
       <c r="M254" s="68"/>
-      <c r="N254" s="68"/>
+      <c r="N254" s="112" t="s">
+        <v>330</v>
+      </c>
       <c r="O254" s="9"/>
       <c r="P254" s="4"/>
       <c r="Q254" s="4"/>
@@ -14141,20 +14353,42 @@
       <c r="T254" s="9"/>
     </row>
     <row r="255" spans="1:20" ht="18" customHeight="1">
-      <c r="A255" s="64"/>
-      <c r="B255" s="73"/>
-      <c r="C255" s="68"/>
-      <c r="D255" s="68"/>
+      <c r="A255" s="116" t="s">
+        <v>316</v>
+      </c>
+      <c r="B255" s="111" t="s">
+        <v>314</v>
+      </c>
+      <c r="C255" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D255" s="112" t="s">
+        <v>113</v>
+      </c>
       <c r="E255" s="73"/>
-      <c r="F255" s="68"/>
-      <c r="G255" s="68"/>
+      <c r="F255" s="112" t="s">
+        <v>322</v>
+      </c>
+      <c r="G255" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H255" s="68"/>
-      <c r="I255" s="83"/>
-      <c r="J255" s="70"/>
-      <c r="K255" s="70"/>
-      <c r="L255" s="68"/>
+      <c r="I255" s="83">
+        <v>298</v>
+      </c>
+      <c r="J255" s="70">
+        <v>7.15</v>
+      </c>
+      <c r="K255" s="70">
+        <v>0.41</v>
+      </c>
+      <c r="L255" s="112" t="s">
+        <v>171</v>
+      </c>
       <c r="M255" s="68"/>
-      <c r="N255" s="68"/>
+      <c r="N255" s="112" t="s">
+        <v>330</v>
+      </c>
       <c r="O255" s="9"/>
       <c r="P255" s="4"/>
       <c r="Q255" s="4"/>
@@ -14163,20 +14397,44 @@
       <c r="T255" s="9"/>
     </row>
     <row r="256" spans="1:20" ht="18" customHeight="1">
-      <c r="A256" s="64"/>
-      <c r="B256" s="73"/>
-      <c r="C256" s="4"/>
-      <c r="D256" s="4"/>
-      <c r="E256" s="9"/>
-      <c r="F256" s="4"/>
-      <c r="G256" s="68"/>
+      <c r="A256" s="116" t="s">
+        <v>317</v>
+      </c>
+      <c r="B256" s="111" t="s">
+        <v>315</v>
+      </c>
+      <c r="C256" s="112" t="s">
+        <v>319</v>
+      </c>
+      <c r="D256" s="112" t="s">
+        <v>113</v>
+      </c>
+      <c r="E256" s="111" t="s">
+        <v>320</v>
+      </c>
+      <c r="F256" s="112" t="s">
+        <v>322</v>
+      </c>
+      <c r="G256" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H256" s="68"/>
-      <c r="I256" s="83"/>
-      <c r="J256" s="70"/>
-      <c r="K256" s="70"/>
-      <c r="L256" s="68"/>
+      <c r="I256" s="83">
+        <v>298</v>
+      </c>
+      <c r="J256" s="70">
+        <v>2.29</v>
+      </c>
+      <c r="K256" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L256" s="112" t="s">
+        <v>171</v>
+      </c>
       <c r="M256" s="68"/>
-      <c r="N256" s="68"/>
+      <c r="N256" s="112" t="s">
+        <v>330</v>
+      </c>
       <c r="O256" s="9"/>
       <c r="P256" s="4"/>
       <c r="Q256" s="4"/>
@@ -14186,19 +14444,37 @@
     </row>
     <row r="257" spans="1:20" ht="18" customHeight="1">
       <c r="A257" s="64"/>
-      <c r="B257" s="73"/>
+      <c r="B257" s="111" t="s">
+        <v>327</v>
+      </c>
       <c r="C257" s="4"/>
-      <c r="D257" s="4"/>
-      <c r="E257" s="9"/>
-      <c r="F257" s="4"/>
-      <c r="G257" s="68"/>
+      <c r="D257" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="E257" s="157" t="s">
+        <v>329</v>
+      </c>
+      <c r="F257" s="155" t="s">
+        <v>326</v>
+      </c>
+      <c r="G257" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H257" s="68"/>
-      <c r="I257" s="83"/>
-      <c r="J257" s="70"/>
+      <c r="I257" s="83">
+        <v>298</v>
+      </c>
+      <c r="J257" s="156">
+        <v>0</v>
+      </c>
       <c r="K257" s="70"/>
-      <c r="L257" s="68"/>
+      <c r="L257" s="112" t="s">
+        <v>171</v>
+      </c>
       <c r="M257" s="68"/>
-      <c r="N257" s="68"/>
+      <c r="N257" s="112" t="s">
+        <v>330</v>
+      </c>
       <c r="O257" s="9"/>
       <c r="P257" s="4"/>
       <c r="Q257" s="4"/>
@@ -14208,19 +14484,37 @@
     </row>
     <row r="258" spans="1:20" ht="18" customHeight="1">
       <c r="A258" s="64"/>
-      <c r="B258" s="73"/>
+      <c r="B258" s="111" t="s">
+        <v>328</v>
+      </c>
       <c r="C258" s="4"/>
-      <c r="D258" s="4"/>
-      <c r="E258" s="9"/>
-      <c r="F258" s="4"/>
-      <c r="G258" s="68"/>
+      <c r="D258" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="E258" s="157" t="s">
+        <v>329</v>
+      </c>
+      <c r="F258" s="155" t="s">
+        <v>326</v>
+      </c>
+      <c r="G258" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H258" s="68"/>
-      <c r="I258" s="83"/>
-      <c r="J258" s="70"/>
+      <c r="I258" s="83">
+        <v>298</v>
+      </c>
+      <c r="J258" s="70">
+        <v>0</v>
+      </c>
       <c r="K258" s="70"/>
-      <c r="L258" s="68"/>
+      <c r="L258" s="112" t="s">
+        <v>171</v>
+      </c>
       <c r="M258" s="68"/>
-      <c r="N258" s="68"/>
+      <c r="N258" s="112" t="s">
+        <v>330</v>
+      </c>
       <c r="O258" s="9"/>
       <c r="P258" s="4"/>
       <c r="Q258" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matchar.2018.06.012`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8B2456-5E36-3E40-A86C-F4DEEB70C537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29637F5E-8B37-8A4C-81EE-86F9D160CC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="4460" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="338">
   <si>
     <r>
       <rPr>
@@ -1123,6 +1123,27 @@
   </si>
   <si>
     <t>10.1016/j.jmst.2024.01.046</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchar.2018.06.012</t>
+  </si>
+  <si>
+    <t>HfZrTiNb0.2</t>
+  </si>
+  <si>
+    <t>HfZrTiNb0.4</t>
+  </si>
+  <si>
+    <t>HfZrTiNb0.6</t>
+  </si>
+  <si>
+    <t>HfZrTiNb1</t>
+  </si>
+  <si>
+    <t>C32 is omega-like phase formed in RHEAs</t>
+  </si>
+  <si>
+    <t>F3</t>
   </si>
 </sst>
 </file>
@@ -3466,8 +3487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A235" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N264" sqref="N264"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C249" zoomScale="86" workbookViewId="0">
+      <selection activeCell="M275" sqref="M275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -14524,19 +14545,41 @@
     </row>
     <row r="259" spans="1:20" ht="18" customHeight="1">
       <c r="A259" s="64"/>
-      <c r="B259" s="73"/>
-      <c r="C259" s="4"/>
-      <c r="D259" s="4"/>
-      <c r="E259" s="9"/>
-      <c r="F259" s="4"/>
-      <c r="G259" s="68"/>
+      <c r="B259" s="111" t="s">
+        <v>332</v>
+      </c>
+      <c r="C259" s="155" t="s">
+        <v>319</v>
+      </c>
+      <c r="D259" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="E259" s="111" t="s">
+        <v>336</v>
+      </c>
+      <c r="F259" s="155" t="s">
+        <v>169</v>
+      </c>
+      <c r="G259" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H259" s="68"/>
-      <c r="I259" s="83"/>
-      <c r="J259" s="70"/>
-      <c r="K259" s="70"/>
-      <c r="L259" s="68"/>
+      <c r="I259" s="83">
+        <v>298</v>
+      </c>
+      <c r="J259" s="70">
+        <v>1005000000</v>
+      </c>
+      <c r="K259" s="70">
+        <v>5000000</v>
+      </c>
+      <c r="L259" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M259" s="68"/>
-      <c r="N259" s="68"/>
+      <c r="N259" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O259" s="9"/>
       <c r="P259" s="4"/>
       <c r="Q259" s="4"/>
@@ -14546,19 +14589,39 @@
     </row>
     <row r="260" spans="1:20" ht="18" customHeight="1">
       <c r="A260" s="64"/>
-      <c r="B260" s="73"/>
-      <c r="C260" s="4"/>
-      <c r="D260" s="4"/>
+      <c r="B260" s="111" t="s">
+        <v>333</v>
+      </c>
+      <c r="C260" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D260" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E260" s="9"/>
-      <c r="F260" s="4"/>
-      <c r="G260" s="68"/>
+      <c r="F260" s="155" t="s">
+        <v>169</v>
+      </c>
+      <c r="G260" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H260" s="68"/>
-      <c r="I260" s="83"/>
-      <c r="J260" s="70"/>
-      <c r="K260" s="70"/>
-      <c r="L260" s="68"/>
+      <c r="I260" s="83">
+        <v>298</v>
+      </c>
+      <c r="J260" s="70">
+        <v>670000000</v>
+      </c>
+      <c r="K260" s="70">
+        <v>8000000</v>
+      </c>
+      <c r="L260" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M260" s="68"/>
-      <c r="N260" s="68"/>
+      <c r="N260" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O260" s="9"/>
       <c r="P260" s="4"/>
       <c r="Q260" s="4"/>
@@ -14568,19 +14631,39 @@
     </row>
     <row r="261" spans="1:20" ht="18" customHeight="1">
       <c r="A261" s="64"/>
-      <c r="B261" s="73"/>
-      <c r="C261" s="4"/>
-      <c r="D261" s="4"/>
+      <c r="B261" s="111" t="s">
+        <v>334</v>
+      </c>
+      <c r="C261" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D261" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E261" s="9"/>
-      <c r="F261" s="4"/>
-      <c r="G261" s="68"/>
+      <c r="F261" s="155" t="s">
+        <v>169</v>
+      </c>
+      <c r="G261" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H261" s="68"/>
-      <c r="I261" s="83"/>
-      <c r="J261" s="70"/>
-      <c r="K261" s="70"/>
-      <c r="L261" s="68"/>
+      <c r="I261" s="83">
+        <v>298</v>
+      </c>
+      <c r="J261" s="70">
+        <v>660000000</v>
+      </c>
+      <c r="K261" s="70">
+        <v>5000000</v>
+      </c>
+      <c r="L261" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M261" s="68"/>
-      <c r="N261" s="68"/>
+      <c r="N261" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O261" s="9"/>
       <c r="P261" s="4"/>
       <c r="Q261" s="4"/>
@@ -14590,19 +14673,39 @@
     </row>
     <row r="262" spans="1:20" ht="18" customHeight="1">
       <c r="A262" s="64"/>
-      <c r="B262" s="73"/>
-      <c r="C262" s="4"/>
-      <c r="D262" s="4"/>
+      <c r="B262" s="111" t="s">
+        <v>335</v>
+      </c>
+      <c r="C262" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D262" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E262" s="9"/>
-      <c r="F262" s="4"/>
-      <c r="G262" s="68"/>
+      <c r="F262" s="155" t="s">
+        <v>169</v>
+      </c>
+      <c r="G262" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H262" s="68"/>
-      <c r="I262" s="83"/>
-      <c r="J262" s="70"/>
-      <c r="K262" s="70"/>
-      <c r="L262" s="68"/>
+      <c r="I262" s="83">
+        <v>298</v>
+      </c>
+      <c r="J262" s="70">
+        <v>645000000</v>
+      </c>
+      <c r="K262" s="70">
+        <v>5000000</v>
+      </c>
+      <c r="L262" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M262" s="68"/>
-      <c r="N262" s="68"/>
+      <c r="N262" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O262" s="9"/>
       <c r="P262" s="4"/>
       <c r="Q262" s="4"/>
@@ -14612,19 +14715,41 @@
     </row>
     <row r="263" spans="1:20" ht="18" customHeight="1">
       <c r="A263" s="64"/>
-      <c r="B263" s="73"/>
-      <c r="C263" s="4"/>
-      <c r="D263" s="4"/>
-      <c r="E263" s="9"/>
-      <c r="F263" s="4"/>
-      <c r="G263" s="68"/>
+      <c r="B263" s="111" t="s">
+        <v>332</v>
+      </c>
+      <c r="C263" s="155" t="s">
+        <v>319</v>
+      </c>
+      <c r="D263" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="E263" s="111" t="s">
+        <v>336</v>
+      </c>
+      <c r="F263" s="155" t="s">
+        <v>189</v>
+      </c>
+      <c r="G263" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H263" s="68"/>
-      <c r="I263" s="83"/>
-      <c r="J263" s="70"/>
+      <c r="I263" s="83">
+        <v>298</v>
+      </c>
+      <c r="J263" s="70">
+        <v>1069000000</v>
+      </c>
       <c r="K263" s="70"/>
-      <c r="L263" s="68"/>
-      <c r="M263" s="68"/>
-      <c r="N263" s="68"/>
+      <c r="L263" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M263" s="112" t="s">
+        <v>337</v>
+      </c>
+      <c r="N263" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O263" s="9"/>
       <c r="P263" s="4"/>
       <c r="Q263" s="4"/>
@@ -14634,19 +14759,39 @@
     </row>
     <row r="264" spans="1:20" ht="18" customHeight="1">
       <c r="A264" s="64"/>
-      <c r="B264" s="73"/>
-      <c r="C264" s="4"/>
-      <c r="D264" s="4"/>
+      <c r="B264" s="111" t="s">
+        <v>333</v>
+      </c>
+      <c r="C264" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D264" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E264" s="9"/>
-      <c r="F264" s="4"/>
-      <c r="G264" s="68"/>
+      <c r="F264" s="155" t="s">
+        <v>189</v>
+      </c>
+      <c r="G264" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H264" s="68"/>
-      <c r="I264" s="83"/>
-      <c r="J264" s="70"/>
+      <c r="I264" s="83">
+        <v>298</v>
+      </c>
+      <c r="J264" s="70">
+        <v>897000000</v>
+      </c>
       <c r="K264" s="70"/>
-      <c r="L264" s="68"/>
-      <c r="M264" s="68"/>
-      <c r="N264" s="68"/>
+      <c r="L264" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M264" s="112" t="s">
+        <v>337</v>
+      </c>
+      <c r="N264" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O264" s="9"/>
       <c r="P264" s="4"/>
       <c r="Q264" s="4"/>
@@ -14656,19 +14801,39 @@
     </row>
     <row r="265" spans="1:20" ht="18" customHeight="1">
       <c r="A265" s="64"/>
-      <c r="B265" s="73"/>
-      <c r="C265" s="4"/>
-      <c r="D265" s="4"/>
+      <c r="B265" s="111" t="s">
+        <v>334</v>
+      </c>
+      <c r="C265" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D265" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E265" s="9"/>
-      <c r="F265" s="4"/>
-      <c r="G265" s="68"/>
+      <c r="F265" s="155" t="s">
+        <v>189</v>
+      </c>
+      <c r="G265" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H265" s="68"/>
-      <c r="I265" s="83"/>
-      <c r="J265" s="70"/>
+      <c r="I265" s="83">
+        <v>298</v>
+      </c>
+      <c r="J265" s="70">
+        <v>932000000</v>
+      </c>
       <c r="K265" s="70"/>
-      <c r="L265" s="68"/>
-      <c r="M265" s="68"/>
-      <c r="N265" s="68"/>
+      <c r="L265" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M265" s="112" t="s">
+        <v>337</v>
+      </c>
+      <c r="N265" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O265" s="9"/>
       <c r="P265" s="4"/>
       <c r="Q265" s="4"/>
@@ -14678,19 +14843,39 @@
     </row>
     <row r="266" spans="1:20" ht="18" customHeight="1">
       <c r="A266" s="64"/>
-      <c r="B266" s="73"/>
-      <c r="C266" s="4"/>
-      <c r="D266" s="4"/>
+      <c r="B266" s="111" t="s">
+        <v>335</v>
+      </c>
+      <c r="C266" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D266" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E266" s="9"/>
-      <c r="F266" s="4"/>
-      <c r="G266" s="68"/>
+      <c r="F266" s="155" t="s">
+        <v>189</v>
+      </c>
+      <c r="G266" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H266" s="68"/>
-      <c r="I266" s="83"/>
-      <c r="J266" s="70"/>
+      <c r="I266" s="83">
+        <v>298</v>
+      </c>
+      <c r="J266" s="70">
+        <v>941000000</v>
+      </c>
       <c r="K266" s="70"/>
-      <c r="L266" s="68"/>
-      <c r="M266" s="68"/>
-      <c r="N266" s="68"/>
+      <c r="L266" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M266" s="112" t="s">
+        <v>337</v>
+      </c>
+      <c r="N266" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O266" s="9"/>
       <c r="P266" s="4"/>
       <c r="Q266" s="4"/>
@@ -14700,19 +14885,41 @@
     </row>
     <row r="267" spans="1:20" ht="18" customHeight="1">
       <c r="A267" s="64"/>
-      <c r="B267" s="73"/>
-      <c r="C267" s="4"/>
-      <c r="D267" s="4"/>
-      <c r="E267" s="9"/>
-      <c r="F267" s="4"/>
-      <c r="G267" s="68"/>
+      <c r="B267" s="111" t="s">
+        <v>332</v>
+      </c>
+      <c r="C267" s="155" t="s">
+        <v>319</v>
+      </c>
+      <c r="D267" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="E267" s="111" t="s">
+        <v>336</v>
+      </c>
+      <c r="F267" s="155" t="s">
+        <v>170</v>
+      </c>
+      <c r="G267" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H267" s="68"/>
-      <c r="I267" s="83"/>
-      <c r="J267" s="70"/>
+      <c r="I267" s="83">
+        <v>298</v>
+      </c>
+      <c r="J267" s="70">
+        <v>27.6</v>
+      </c>
       <c r="K267" s="70"/>
-      <c r="L267" s="68"/>
-      <c r="M267" s="68"/>
-      <c r="N267" s="68"/>
+      <c r="L267" s="112" t="s">
+        <v>171</v>
+      </c>
+      <c r="M267" s="112" t="s">
+        <v>337</v>
+      </c>
+      <c r="N267" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O267" s="9"/>
       <c r="P267" s="4"/>
       <c r="Q267" s="4"/>
@@ -14722,19 +14929,39 @@
     </row>
     <row r="268" spans="1:20" ht="18" customHeight="1">
       <c r="A268" s="64"/>
-      <c r="B268" s="73"/>
-      <c r="C268" s="4"/>
-      <c r="D268" s="4"/>
+      <c r="B268" s="111" t="s">
+        <v>333</v>
+      </c>
+      <c r="C268" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D268" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E268" s="9"/>
-      <c r="F268" s="4"/>
-      <c r="G268" s="68"/>
+      <c r="F268" s="155" t="s">
+        <v>170</v>
+      </c>
+      <c r="G268" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H268" s="68"/>
-      <c r="I268" s="83"/>
-      <c r="J268" s="70"/>
+      <c r="I268" s="83">
+        <v>298</v>
+      </c>
+      <c r="J268" s="70">
+        <v>36.6</v>
+      </c>
       <c r="K268" s="70"/>
-      <c r="L268" s="68"/>
-      <c r="M268" s="68"/>
-      <c r="N268" s="68"/>
+      <c r="L268" s="112" t="s">
+        <v>171</v>
+      </c>
+      <c r="M268" s="112" t="s">
+        <v>337</v>
+      </c>
+      <c r="N268" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O268" s="9"/>
       <c r="P268" s="4"/>
       <c r="Q268" s="4"/>
@@ -14744,19 +14971,39 @@
     </row>
     <row r="269" spans="1:20" ht="18" customHeight="1">
       <c r="A269" s="64"/>
-      <c r="B269" s="73"/>
-      <c r="C269" s="4"/>
-      <c r="D269" s="4"/>
+      <c r="B269" s="111" t="s">
+        <v>334</v>
+      </c>
+      <c r="C269" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D269" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E269" s="9"/>
-      <c r="F269" s="4"/>
-      <c r="G269" s="68"/>
+      <c r="F269" s="155" t="s">
+        <v>246</v>
+      </c>
+      <c r="G269" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H269" s="68"/>
-      <c r="I269" s="83"/>
-      <c r="J269" s="70"/>
+      <c r="I269" s="83">
+        <v>298</v>
+      </c>
+      <c r="J269" s="70">
+        <v>70</v>
+      </c>
       <c r="K269" s="70"/>
-      <c r="L269" s="68"/>
-      <c r="M269" s="68"/>
-      <c r="N269" s="68"/>
+      <c r="L269" s="112" t="s">
+        <v>171</v>
+      </c>
+      <c r="M269" s="112" t="s">
+        <v>337</v>
+      </c>
+      <c r="N269" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O269" s="9"/>
       <c r="P269" s="4"/>
       <c r="Q269" s="4"/>
@@ -14766,19 +15013,39 @@
     </row>
     <row r="270" spans="1:20" ht="18" customHeight="1">
       <c r="A270" s="64"/>
-      <c r="B270" s="73"/>
-      <c r="C270" s="4"/>
-      <c r="D270" s="4"/>
+      <c r="B270" s="111" t="s">
+        <v>335</v>
+      </c>
+      <c r="C270" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D270" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E270" s="9"/>
-      <c r="F270" s="4"/>
-      <c r="G270" s="68"/>
+      <c r="F270" s="155" t="s">
+        <v>246</v>
+      </c>
+      <c r="G270" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H270" s="68"/>
-      <c r="I270" s="83"/>
-      <c r="J270" s="70"/>
+      <c r="I270" s="83">
+        <v>298</v>
+      </c>
+      <c r="J270" s="70">
+        <v>70</v>
+      </c>
       <c r="K270" s="70"/>
-      <c r="L270" s="68"/>
-      <c r="M270" s="68"/>
-      <c r="N270" s="68"/>
+      <c r="L270" s="112" t="s">
+        <v>171</v>
+      </c>
+      <c r="M270" s="112" t="s">
+        <v>337</v>
+      </c>
+      <c r="N270" s="112" t="s">
+        <v>331</v>
+      </c>
       <c r="O270" s="9"/>
       <c r="P270" s="4"/>
       <c r="Q270" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2018.01.331`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29637F5E-8B37-8A4C-81EE-86F9D160CC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CE054F-3B90-F44A-BED0-271B1B2A7CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="4460" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="4100" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2263" uniqueCount="343">
   <si>
     <r>
       <rPr>
@@ -1144,6 +1144,21 @@
   </si>
   <si>
     <t>F3</t>
+  </si>
+  <si>
+    <t>CeGdTbDyHo</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>HCP+C19</t>
+  </si>
+  <si>
+    <t>curie temperature</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2018.01.331</t>
   </si>
 </sst>
 </file>
@@ -1956,7 +1971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2325,6 +2340,7 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3487,8 +3503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C249" zoomScale="86" workbookViewId="0">
-      <selection activeCell="M275" sqref="M275"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E257" zoomScale="86" workbookViewId="0">
+      <selection activeCell="M283" sqref="M283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -15055,19 +15071,35 @@
     </row>
     <row r="271" spans="1:20" ht="18" customHeight="1">
       <c r="A271" s="64"/>
-      <c r="B271" s="73"/>
-      <c r="C271" s="4"/>
-      <c r="D271" s="4"/>
+      <c r="B271" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="C271" s="155" t="s">
+        <v>340</v>
+      </c>
+      <c r="D271" s="155" t="s">
+        <v>339</v>
+      </c>
       <c r="E271" s="9"/>
-      <c r="F271" s="4"/>
-      <c r="G271" s="68"/>
+      <c r="F271" s="155" t="s">
+        <v>341</v>
+      </c>
+      <c r="G271" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H271" s="68"/>
       <c r="I271" s="83"/>
-      <c r="J271" s="70"/>
+      <c r="J271" s="70">
+        <v>140</v>
+      </c>
       <c r="K271" s="70"/>
-      <c r="L271" s="68"/>
+      <c r="L271" s="112" t="s">
+        <v>249</v>
+      </c>
       <c r="M271" s="68"/>
-      <c r="N271" s="68"/>
+      <c r="N271" s="112" t="s">
+        <v>342</v>
+      </c>
       <c r="O271" s="9"/>
       <c r="P271" s="4"/>
       <c r="Q271" s="4"/>
@@ -15077,19 +15109,37 @@
     </row>
     <row r="272" spans="1:20" ht="18" customHeight="1">
       <c r="A272" s="64"/>
-      <c r="B272" s="73"/>
-      <c r="C272" s="4"/>
-      <c r="D272" s="4"/>
+      <c r="B272" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="C272" s="155" t="s">
+        <v>340</v>
+      </c>
+      <c r="D272" s="155" t="s">
+        <v>339</v>
+      </c>
       <c r="E272" s="9"/>
-      <c r="F272" s="4"/>
-      <c r="G272" s="68"/>
+      <c r="F272" s="155" t="s">
+        <v>251</v>
+      </c>
+      <c r="G272" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H272" s="68"/>
-      <c r="I272" s="83"/>
-      <c r="J272" s="70"/>
+      <c r="I272" s="83">
+        <v>2</v>
+      </c>
+      <c r="J272" s="70">
+        <v>8.1999999999999998E-7</v>
+      </c>
       <c r="K272" s="70"/>
-      <c r="L272" s="68"/>
+      <c r="L272" s="112" t="s">
+        <v>252</v>
+      </c>
       <c r="M272" s="68"/>
-      <c r="N272" s="68"/>
+      <c r="N272" s="112" t="s">
+        <v>342</v>
+      </c>
       <c r="O272" s="9"/>
       <c r="P272" s="4"/>
       <c r="Q272" s="4"/>
@@ -15099,19 +15149,37 @@
     </row>
     <row r="273" spans="1:20" ht="18" customHeight="1">
       <c r="A273" s="64"/>
-      <c r="B273" s="73"/>
-      <c r="C273" s="4"/>
-      <c r="D273" s="4"/>
+      <c r="B273" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="C273" s="155" t="s">
+        <v>340</v>
+      </c>
+      <c r="D273" s="155" t="s">
+        <v>339</v>
+      </c>
       <c r="E273" s="9"/>
-      <c r="F273" s="4"/>
-      <c r="G273" s="68"/>
+      <c r="F273" s="155" t="s">
+        <v>251</v>
+      </c>
+      <c r="G273" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H273" s="68"/>
-      <c r="I273" s="83"/>
-      <c r="J273" s="70"/>
+      <c r="I273" s="117">
+        <v>140</v>
+      </c>
+      <c r="J273" s="158">
+        <v>1.17E-6</v>
+      </c>
       <c r="K273" s="70"/>
-      <c r="L273" s="68"/>
+      <c r="L273" s="113" t="s">
+        <v>252</v>
+      </c>
       <c r="M273" s="68"/>
-      <c r="N273" s="68"/>
+      <c r="N273" s="112" t="s">
+        <v>342</v>
+      </c>
       <c r="O273" s="9"/>
       <c r="P273" s="4"/>
       <c r="Q273" s="4"/>
@@ -15121,19 +15189,37 @@
     </row>
     <row r="274" spans="1:20" ht="18" customHeight="1">
       <c r="A274" s="64"/>
-      <c r="B274" s="73"/>
-      <c r="C274" s="4"/>
-      <c r="D274" s="4"/>
+      <c r="B274" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="C274" s="155" t="s">
+        <v>340</v>
+      </c>
+      <c r="D274" s="155" t="s">
+        <v>339</v>
+      </c>
       <c r="E274" s="9"/>
-      <c r="F274" s="4"/>
-      <c r="G274" s="68"/>
-      <c r="H274" s="4"/>
-      <c r="I274" s="83"/>
-      <c r="J274" s="70"/>
+      <c r="F274" s="155" t="s">
+        <v>251</v>
+      </c>
+      <c r="G274" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H274" s="68"/>
+      <c r="I274" s="83">
+        <v>300</v>
+      </c>
+      <c r="J274" s="70">
+        <v>1.2699999999999999E-6</v>
+      </c>
       <c r="K274" s="70"/>
-      <c r="L274" s="68"/>
+      <c r="L274" s="112" t="s">
+        <v>252</v>
+      </c>
       <c r="M274" s="68"/>
-      <c r="N274" s="68"/>
+      <c r="N274" s="112" t="s">
+        <v>342</v>
+      </c>
       <c r="O274" s="9"/>
       <c r="P274" s="4"/>
       <c r="Q274" s="4"/>
@@ -15900,7 +15986,7 @@
       <c r="H309" s="4"/>
       <c r="I309" s="83"/>
       <c r="J309" s="70"/>
-      <c r="K309" s="70"/>
+      <c r="K309" s="4"/>
       <c r="L309" s="68"/>
       <c r="M309" s="68"/>
       <c r="N309" s="68"/>
@@ -15922,7 +16008,7 @@
       <c r="H310" s="4"/>
       <c r="I310" s="83"/>
       <c r="J310" s="70"/>
-      <c r="K310" s="4"/>
+      <c r="K310" s="70"/>
       <c r="L310" s="68"/>
       <c r="M310" s="68"/>
       <c r="N310" s="68"/>
@@ -16472,7 +16558,7 @@
       <c r="H335" s="4"/>
       <c r="I335" s="83"/>
       <c r="J335" s="70"/>
-      <c r="K335" s="70"/>
+      <c r="K335" s="4"/>
       <c r="L335" s="68"/>
       <c r="M335" s="68"/>
       <c r="N335" s="68"/>
@@ -16626,7 +16712,7 @@
       <c r="H342" s="4"/>
       <c r="I342" s="83"/>
       <c r="J342" s="70"/>
-      <c r="K342" s="4"/>
+      <c r="K342" s="70"/>
       <c r="L342" s="68"/>
       <c r="M342" s="70"/>
       <c r="N342" s="68"/>
@@ -17792,7 +17878,7 @@
       <c r="H395" s="4"/>
       <c r="I395" s="83"/>
       <c r="J395" s="70"/>
-      <c r="K395" s="70"/>
+      <c r="K395" s="4"/>
       <c r="L395" s="68"/>
       <c r="M395" s="68"/>
       <c r="N395" s="68"/>
@@ -17814,7 +17900,7 @@
       <c r="H396" s="4"/>
       <c r="I396" s="83"/>
       <c r="J396" s="70"/>
-      <c r="K396" s="4"/>
+      <c r="K396" s="70"/>
       <c r="L396" s="68"/>
       <c r="M396" s="68"/>
       <c r="N396" s="68"/>
@@ -18474,7 +18560,7 @@
       <c r="H426" s="4"/>
       <c r="I426" s="83"/>
       <c r="J426" s="70"/>
-      <c r="K426" s="70"/>
+      <c r="K426" s="4"/>
       <c r="L426" s="68"/>
       <c r="M426" s="68"/>
       <c r="N426" s="68"/>
@@ -19464,7 +19550,7 @@
       <c r="H471" s="4"/>
       <c r="I471" s="4"/>
       <c r="J471" s="4"/>
-      <c r="K471" s="4"/>
+      <c r="K471" s="70"/>
       <c r="L471" s="4"/>
       <c r="M471" s="4"/>
       <c r="N471" s="68"/>
@@ -19618,7 +19704,7 @@
       <c r="H478" s="4"/>
       <c r="I478" s="4"/>
       <c r="J478" s="70"/>
-      <c r="K478" s="70"/>
+      <c r="K478" s="4"/>
       <c r="L478" s="4"/>
       <c r="M478" s="4"/>
       <c r="N478" s="4"/>
@@ -20256,7 +20342,7 @@
       <c r="H507" s="4"/>
       <c r="I507" s="4"/>
       <c r="J507" s="4"/>
-      <c r="K507" s="4"/>
+      <c r="K507" s="70"/>
       <c r="L507" s="4"/>
       <c r="M507" s="4"/>
       <c r="N507" s="4"/>
@@ -20366,7 +20452,7 @@
       <c r="H512" s="4"/>
       <c r="I512" s="4"/>
       <c r="J512" s="70"/>
-      <c r="K512" s="70"/>
+      <c r="K512" s="4"/>
       <c r="L512" s="4"/>
       <c r="M512" s="4"/>
       <c r="N512" s="4"/>
@@ -21246,7 +21332,7 @@
       <c r="H552" s="4"/>
       <c r="I552" s="4"/>
       <c r="J552" s="4"/>
-      <c r="K552" s="4"/>
+      <c r="K552" s="70"/>
       <c r="L552" s="4"/>
       <c r="M552" s="4"/>
       <c r="N552" s="4"/>
@@ -21356,7 +21442,7 @@
       <c r="H557" s="4"/>
       <c r="I557" s="4"/>
       <c r="J557" s="70"/>
-      <c r="K557" s="70"/>
+      <c r="K557" s="4"/>
       <c r="L557" s="4"/>
       <c r="M557" s="4"/>
       <c r="N557" s="4"/>
@@ -22918,7 +23004,7 @@
       <c r="H628" s="4"/>
       <c r="I628" s="4"/>
       <c r="J628" s="4"/>
-      <c r="K628" s="4"/>
+      <c r="K628" s="92"/>
       <c r="L628" s="4"/>
       <c r="M628" s="4"/>
       <c r="N628" s="4"/>
@@ -23072,7 +23158,7 @@
       <c r="H635" s="90"/>
       <c r="I635" s="91"/>
       <c r="J635" s="92"/>
-      <c r="K635" s="92"/>
+      <c r="K635" s="4"/>
       <c r="L635" s="89"/>
       <c r="M635" s="89"/>
       <c r="N635" s="94"/>
@@ -23204,7 +23290,7 @@
       <c r="H641" s="90"/>
       <c r="I641" s="91"/>
       <c r="J641" s="4"/>
-      <c r="K641" s="4"/>
+      <c r="K641" s="92"/>
       <c r="L641" s="4"/>
       <c r="M641" s="4"/>
       <c r="N641" s="94"/>
@@ -23270,7 +23356,7 @@
       <c r="H644" s="90"/>
       <c r="I644" s="91"/>
       <c r="J644" s="92"/>
-      <c r="K644" s="92"/>
+      <c r="K644" s="4"/>
       <c r="L644" s="89"/>
       <c r="M644" s="89"/>
       <c r="N644" s="87"/>
@@ -23534,7 +23620,7 @@
       <c r="H656" s="4"/>
       <c r="I656" s="4"/>
       <c r="J656" s="4"/>
-      <c r="K656" s="4"/>
+      <c r="K656" s="92"/>
       <c r="L656" s="89"/>
       <c r="M656" s="89"/>
       <c r="N656" s="87"/>
@@ -23622,7 +23708,7 @@
       <c r="H660" s="90"/>
       <c r="I660" s="91"/>
       <c r="J660" s="92"/>
-      <c r="K660" s="92"/>
+      <c r="K660" s="101"/>
       <c r="L660" s="89"/>
       <c r="M660" s="89"/>
       <c r="N660" s="87"/>
@@ -23644,7 +23730,7 @@
       <c r="H661" s="90"/>
       <c r="I661" s="91"/>
       <c r="J661" s="100"/>
-      <c r="K661" s="101"/>
+      <c r="K661" s="100"/>
       <c r="L661" s="102"/>
       <c r="M661" s="102"/>
       <c r="N661" s="87"/>
@@ -24194,7 +24280,7 @@
       <c r="H686" s="90"/>
       <c r="I686" s="103"/>
       <c r="J686" s="100"/>
-      <c r="K686" s="100"/>
+      <c r="K686" s="104"/>
       <c r="L686" s="102"/>
       <c r="M686" s="102"/>
       <c r="N686" s="87"/>
@@ -24216,7 +24302,7 @@
       <c r="H687" s="90"/>
       <c r="I687" s="103"/>
       <c r="J687" s="100"/>
-      <c r="K687" s="104"/>
+      <c r="K687" s="87"/>
       <c r="L687" s="102"/>
       <c r="M687" s="102"/>
       <c r="N687" s="87"/>
@@ -24238,7 +24324,7 @@
       <c r="H688" s="90"/>
       <c r="I688" s="103"/>
       <c r="J688" s="100"/>
-      <c r="K688" s="87"/>
+      <c r="K688" s="101"/>
       <c r="L688" s="102"/>
       <c r="M688" s="102"/>
       <c r="N688" s="87"/>
@@ -24326,7 +24412,7 @@
       <c r="H692" s="90"/>
       <c r="I692" s="103"/>
       <c r="J692" s="100"/>
-      <c r="K692" s="101"/>
+      <c r="K692" s="87"/>
       <c r="L692" s="102"/>
       <c r="M692" s="102"/>
       <c r="N692" s="87"/>
@@ -24348,7 +24434,7 @@
       <c r="H693" s="90"/>
       <c r="I693" s="91"/>
       <c r="J693" s="101"/>
-      <c r="K693" s="87"/>
+      <c r="K693" s="101"/>
       <c r="L693" s="102"/>
       <c r="M693" s="102"/>
       <c r="N693" s="87"/>
@@ -24436,7 +24522,7 @@
       <c r="H697" s="90"/>
       <c r="I697" s="103"/>
       <c r="J697" s="98"/>
-      <c r="K697" s="101"/>
+      <c r="K697" s="87"/>
       <c r="L697" s="102"/>
       <c r="M697" s="102"/>
       <c r="N697" s="87"/>
@@ -24458,7 +24544,7 @@
       <c r="H698" s="90"/>
       <c r="I698" s="103"/>
       <c r="J698" s="98"/>
-      <c r="K698" s="87"/>
+      <c r="K698" s="101"/>
       <c r="L698" s="102"/>
       <c r="M698" s="102"/>
       <c r="N698" s="87"/>
@@ -24546,7 +24632,7 @@
       <c r="H702" s="90"/>
       <c r="I702" s="103"/>
       <c r="J702" s="98"/>
-      <c r="K702" s="101"/>
+      <c r="K702" s="87"/>
       <c r="L702" s="102"/>
       <c r="M702" s="102"/>
       <c r="N702" s="87"/>
@@ -24568,7 +24654,7 @@
       <c r="H703" s="90"/>
       <c r="I703" s="103"/>
       <c r="J703" s="98"/>
-      <c r="K703" s="87"/>
+      <c r="K703" s="101"/>
       <c r="L703" s="102"/>
       <c r="M703" s="102"/>
       <c r="N703" s="87"/>
@@ -24656,7 +24742,7 @@
       <c r="H707" s="90"/>
       <c r="I707" s="103"/>
       <c r="J707" s="98"/>
-      <c r="K707" s="101"/>
+      <c r="K707" s="100"/>
       <c r="L707" s="102"/>
       <c r="M707" s="102"/>
       <c r="N707" s="87"/>
@@ -24766,7 +24852,7 @@
       <c r="H712" s="90"/>
       <c r="I712" s="91"/>
       <c r="J712" s="100"/>
-      <c r="K712" s="100"/>
+      <c r="K712" s="92"/>
       <c r="L712" s="102"/>
       <c r="M712" s="102"/>
       <c r="N712" s="87"/>
@@ -24942,7 +25028,7 @@
       <c r="H720" s="90"/>
       <c r="I720" s="91"/>
       <c r="J720" s="92"/>
-      <c r="K720" s="92"/>
+      <c r="K720" s="100"/>
       <c r="L720" s="89"/>
       <c r="M720" s="89"/>
       <c r="N720" s="87"/>
@@ -25382,7 +25468,7 @@
       <c r="H740" s="90"/>
       <c r="I740" s="91"/>
       <c r="J740" s="101"/>
-      <c r="K740" s="100"/>
+      <c r="K740" s="107"/>
       <c r="L740" s="102"/>
       <c r="M740" s="102"/>
       <c r="N740" s="87"/>
@@ -25426,7 +25512,7 @@
       <c r="H742" s="90"/>
       <c r="I742" s="4"/>
       <c r="J742" s="107"/>
-      <c r="K742" s="107"/>
+      <c r="K742" s="100"/>
       <c r="L742" s="66"/>
       <c r="M742" s="66"/>
       <c r="N742" s="4"/>
@@ -25646,7 +25732,7 @@
       <c r="H752" s="90"/>
       <c r="I752" s="103"/>
       <c r="J752" s="101"/>
-      <c r="K752" s="100"/>
+      <c r="K752" s="92"/>
       <c r="L752" s="102"/>
       <c r="M752" s="102"/>
       <c r="N752" s="87"/>
@@ -25822,7 +25908,7 @@
       <c r="H760" s="90"/>
       <c r="I760" s="91"/>
       <c r="J760" s="92"/>
-      <c r="K760" s="92"/>
+      <c r="K760" s="4"/>
       <c r="L760" s="89"/>
       <c r="M760" s="89"/>
       <c r="N760" s="109"/>
@@ -25998,7 +26084,7 @@
       <c r="H768" s="90"/>
       <c r="I768" s="4"/>
       <c r="J768" s="4"/>
-      <c r="K768" s="4"/>
+      <c r="K768" s="92"/>
       <c r="L768" s="89"/>
       <c r="M768" s="4"/>
       <c r="N768" s="109"/>
@@ -26174,7 +26260,7 @@
       <c r="H776" s="90"/>
       <c r="I776" s="91"/>
       <c r="J776" s="92"/>
-      <c r="K776" s="92"/>
+      <c r="K776" s="4"/>
       <c r="L776" s="89"/>
       <c r="M776" s="89"/>
       <c r="N776" s="109"/>
@@ -27980,7 +28066,6 @@
       <c r="H859" s="4"/>
       <c r="I859" s="4"/>
       <c r="J859" s="4"/>
-      <c r="K859" s="4"/>
       <c r="L859" s="4"/>
       <c r="M859" s="4"/>
       <c r="N859" s="4"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.intermet.2015.10.022`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CE054F-3B90-F44A-BED0-271B1B2A7CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89052B73-4204-DD4C-850C-71E70C6618D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="4100" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6320" yWindow="4100" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2263" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="347">
   <si>
     <r>
       <rPr>
@@ -1159,6 +1159,18 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2018.01.331</t>
+  </si>
+  <si>
+    <t>ScYLaTiZrHf</t>
+  </si>
+  <si>
+    <t>HCP+HCP</t>
+  </si>
+  <si>
+    <t>Y-rich HCP and Ti/Hf-rich HCP</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2015.10.022</t>
   </si>
 </sst>
 </file>
@@ -3503,8 +3515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E257" zoomScale="86" workbookViewId="0">
-      <selection activeCell="M283" sqref="M283"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B258" zoomScale="86" workbookViewId="0">
+      <selection activeCell="K280" sqref="K280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -15229,10 +15241,18 @@
     </row>
     <row r="275" spans="1:20" ht="18" customHeight="1">
       <c r="A275" s="64"/>
-      <c r="B275" s="73"/>
-      <c r="C275" s="4"/>
-      <c r="D275" s="4"/>
-      <c r="E275" s="9"/>
+      <c r="B275" s="111" t="s">
+        <v>343</v>
+      </c>
+      <c r="C275" s="155" t="s">
+        <v>344</v>
+      </c>
+      <c r="D275" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="E275" s="157" t="s">
+        <v>345</v>
+      </c>
       <c r="F275" s="4"/>
       <c r="G275" s="68"/>
       <c r="H275" s="4"/>
@@ -15241,7 +15261,9 @@
       <c r="K275" s="70"/>
       <c r="L275" s="68"/>
       <c r="M275" s="68"/>
-      <c r="N275" s="68"/>
+      <c r="N275" s="112" t="s">
+        <v>346</v>
+      </c>
       <c r="O275" s="9"/>
       <c r="P275" s="4"/>
       <c r="Q275" s="4"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1007/s11837-014-1085-x`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89052B73-4204-DD4C-850C-71E70C6618D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE9AF4A-B76A-C843-A9BE-CFBF42092DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="4100" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13660" yWindow="3400" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="352">
   <si>
     <r>
       <rPr>
@@ -1171,6 +1171,21 @@
   </si>
   <si>
     <t>10.1016/j.intermet.2015.10.022</t>
+  </si>
+  <si>
+    <t>YGdTbDyLu</t>
+  </si>
+  <si>
+    <t>GdTbDyTmLu</t>
+  </si>
+  <si>
+    <t>HCP</t>
+  </si>
+  <si>
+    <t>annealed at 1273K for 3.6ks and 1173K for 86.4ks; nanoscale inclusions persisted from the AC state</t>
+  </si>
+  <si>
+    <t>10.1007/s11837-014-1085-x</t>
   </si>
 </sst>
 </file>
@@ -3515,8 +3530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B258" zoomScale="86" workbookViewId="0">
-      <selection activeCell="K280" sqref="K280"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A259" zoomScale="86" workbookViewId="0">
+      <selection activeCell="M283" sqref="M283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -15273,9 +15288,15 @@
     </row>
     <row r="276" spans="1:20" ht="18" customHeight="1">
       <c r="A276" s="64"/>
-      <c r="B276" s="73"/>
-      <c r="C276" s="4"/>
-      <c r="D276" s="4"/>
+      <c r="B276" s="111" t="s">
+        <v>347</v>
+      </c>
+      <c r="C276" s="155" t="s">
+        <v>349</v>
+      </c>
+      <c r="D276" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E276" s="9"/>
       <c r="F276" s="4"/>
       <c r="G276" s="68"/>
@@ -15285,7 +15306,9 @@
       <c r="K276" s="70"/>
       <c r="L276" s="68"/>
       <c r="M276" s="68"/>
-      <c r="N276" s="68"/>
+      <c r="N276" s="112" t="s">
+        <v>351</v>
+      </c>
       <c r="O276" s="9"/>
       <c r="P276" s="4"/>
       <c r="Q276" s="4"/>
@@ -15295,9 +15318,15 @@
     </row>
     <row r="277" spans="1:20" ht="18" customHeight="1">
       <c r="A277" s="64"/>
-      <c r="B277" s="73"/>
-      <c r="C277" s="4"/>
-      <c r="D277" s="4"/>
+      <c r="B277" s="111" t="s">
+        <v>348</v>
+      </c>
+      <c r="C277" s="155" t="s">
+        <v>349</v>
+      </c>
+      <c r="D277" s="155" t="s">
+        <v>113</v>
+      </c>
       <c r="E277" s="9"/>
       <c r="F277" s="4"/>
       <c r="G277" s="68"/>
@@ -15307,7 +15336,9 @@
       <c r="K277" s="70"/>
       <c r="L277" s="68"/>
       <c r="M277" s="68"/>
-      <c r="N277" s="68"/>
+      <c r="N277" s="112" t="s">
+        <v>351</v>
+      </c>
       <c r="O277" s="9"/>
       <c r="P277" s="4"/>
       <c r="Q277" s="4"/>
@@ -15317,10 +15348,18 @@
     </row>
     <row r="278" spans="1:20" ht="18" customHeight="1">
       <c r="A278" s="64"/>
-      <c r="B278" s="73"/>
-      <c r="C278" s="4"/>
-      <c r="D278" s="4"/>
-      <c r="E278" s="9"/>
+      <c r="B278" s="111" t="s">
+        <v>348</v>
+      </c>
+      <c r="C278" s="155" t="s">
+        <v>349</v>
+      </c>
+      <c r="D278" s="155" t="s">
+        <v>187</v>
+      </c>
+      <c r="E278" s="157" t="s">
+        <v>350</v>
+      </c>
       <c r="F278" s="4"/>
       <c r="G278" s="68"/>
       <c r="H278" s="4"/>
@@ -15329,7 +15368,9 @@
       <c r="K278" s="70"/>
       <c r="L278" s="68"/>
       <c r="M278" s="68"/>
-      <c r="N278" s="68"/>
+      <c r="N278" s="112" t="s">
+        <v>351</v>
+      </c>
       <c r="O278" s="9"/>
       <c r="P278" s="4"/>
       <c r="Q278" s="4"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.2320/matertrans.M2016121`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE9AF4A-B76A-C843-A9BE-CFBF42092DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B643DF01-4914-AD45-B94E-6CF1ED0EF66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13660" yWindow="3400" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6100" yWindow="4980" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="359">
   <si>
     <r>
       <rPr>
@@ -1186,6 +1186,27 @@
   </si>
   <si>
     <t>10.1007/s11837-014-1085-x</t>
+  </si>
+  <si>
+    <t>10.2320/matertrans.M2016121</t>
+  </si>
+  <si>
+    <t>CoCuPdTiZrHf</t>
+  </si>
+  <si>
+    <t>CoCuFeTiZrHf</t>
+  </si>
+  <si>
+    <t>AgAuCuNiPdPt</t>
+  </si>
+  <si>
+    <t>Al4CoNiPdPt</t>
+  </si>
+  <si>
+    <t>after arc-melting alloys were homogenized in vacuum in quartz "as needed" at 1273K for 43.2ks</t>
+  </si>
+  <si>
+    <t>B2</t>
   </si>
 </sst>
 </file>
@@ -1998,7 +2019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2368,6 +2389,7 @@
     <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3530,8 +3552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A259" zoomScale="86" workbookViewId="0">
-      <selection activeCell="M283" sqref="M283"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A261" zoomScale="86" workbookViewId="0">
+      <selection activeCell="M288" sqref="M288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -15380,10 +15402,16 @@
     </row>
     <row r="279" spans="1:20" ht="18" customHeight="1">
       <c r="A279" s="64"/>
-      <c r="B279" s="73"/>
-      <c r="C279" s="4"/>
-      <c r="D279" s="4"/>
-      <c r="E279" s="9"/>
+      <c r="B279" s="111" t="s">
+        <v>353</v>
+      </c>
+      <c r="C279" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="D279" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="E279" s="157"/>
       <c r="F279" s="4"/>
       <c r="G279" s="68"/>
       <c r="H279" s="4"/>
@@ -15392,7 +15420,9 @@
       <c r="K279" s="70"/>
       <c r="L279" s="68"/>
       <c r="M279" s="68"/>
-      <c r="N279" s="68"/>
+      <c r="N279" s="112" t="s">
+        <v>352</v>
+      </c>
       <c r="O279" s="9"/>
       <c r="P279" s="4"/>
       <c r="Q279" s="4"/>
@@ -15402,10 +15432,16 @@
     </row>
     <row r="280" spans="1:20" ht="18" customHeight="1">
       <c r="A280" s="64"/>
-      <c r="B280" s="73"/>
-      <c r="C280" s="4"/>
-      <c r="D280" s="4"/>
-      <c r="E280" s="9"/>
+      <c r="B280" s="111" t="s">
+        <v>354</v>
+      </c>
+      <c r="C280" s="155" t="s">
+        <v>358</v>
+      </c>
+      <c r="D280" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="E280" s="157"/>
       <c r="F280" s="4"/>
       <c r="G280" s="68"/>
       <c r="H280" s="4"/>
@@ -15414,7 +15450,9 @@
       <c r="K280" s="70"/>
       <c r="L280" s="68"/>
       <c r="M280" s="68"/>
-      <c r="N280" s="68"/>
+      <c r="N280" s="112" t="s">
+        <v>352</v>
+      </c>
       <c r="O280" s="9"/>
       <c r="P280" s="4"/>
       <c r="Q280" s="4"/>
@@ -15424,10 +15462,16 @@
     </row>
     <row r="281" spans="1:20" ht="18" customHeight="1">
       <c r="A281" s="64"/>
-      <c r="B281" s="73"/>
-      <c r="C281" s="4"/>
-      <c r="D281" s="4"/>
-      <c r="E281" s="9"/>
+      <c r="B281" s="111" t="s">
+        <v>355</v>
+      </c>
+      <c r="C281" s="155" t="s">
+        <v>117</v>
+      </c>
+      <c r="D281" s="155" t="s">
+        <v>113</v>
+      </c>
+      <c r="E281" s="157"/>
       <c r="F281" s="4"/>
       <c r="G281" s="68"/>
       <c r="H281" s="4"/>
@@ -15436,7 +15480,9 @@
       <c r="K281" s="70"/>
       <c r="L281" s="68"/>
       <c r="M281" s="68"/>
-      <c r="N281" s="68"/>
+      <c r="N281" s="112" t="s">
+        <v>352</v>
+      </c>
       <c r="O281" s="9"/>
       <c r="P281" s="4"/>
       <c r="Q281" s="4"/>
@@ -15446,10 +15492,18 @@
     </row>
     <row r="282" spans="1:20" ht="18" customHeight="1">
       <c r="A282" s="64"/>
-      <c r="B282" s="73"/>
-      <c r="C282" s="4"/>
-      <c r="D282" s="4"/>
-      <c r="E282" s="9"/>
+      <c r="B282" s="111" t="s">
+        <v>356</v>
+      </c>
+      <c r="C282" s="159" t="s">
+        <v>358</v>
+      </c>
+      <c r="D282" s="155" t="s">
+        <v>195</v>
+      </c>
+      <c r="E282" s="157" t="s">
+        <v>357</v>
+      </c>
       <c r="F282" s="4"/>
       <c r="G282" s="68"/>
       <c r="H282" s="4"/>
@@ -15458,7 +15512,9 @@
       <c r="K282" s="70"/>
       <c r="L282" s="68"/>
       <c r="M282" s="68"/>
-      <c r="N282" s="68"/>
+      <c r="N282" s="112" t="s">
+        <v>352</v>
+      </c>
       <c r="O282" s="9"/>
       <c r="P282" s="4"/>
       <c r="Q282" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2022.144137`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B643DF01-4914-AD45-B94E-6CF1ED0EF66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8B4D9D-061B-9B43-A9A0-30B59DC8DB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="4980" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6700" yWindow="1580" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="377">
   <si>
     <r>
       <rPr>
@@ -1207,6 +1207,60 @@
   </si>
   <si>
     <t>B2</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2022.144137</t>
+  </si>
+  <si>
+    <t>AAM+H+WQ</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 20h and water quenched</t>
+  </si>
+  <si>
+    <t>(Ni2FeCoCr)17.65 Al5 Ti3 W1.5 Mo1.5 Nb0.75</t>
+  </si>
+  <si>
+    <t>AAM+H+WQ+CR</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 20h and water quenched; cold rolled to 80% reduction</t>
+  </si>
+  <si>
+    <t>AAM+H+WQ+CR+A+AT</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 20h and water quenched; cold rolled to 80% reduction; annealed at 1173K for 20min; agrd at 1023K for 24h</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H0</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 20h and water quenched; cold rolled to 80% reduction; annealed at 1198KK for 20min; agrd at 1023K for 24h</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 20h and water quenched; cold rolled to 80% reduction; annealed at 1223K for 20min; agrd at 1023K for 24h</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>(Ni2FeCoCr)17.65 Al5 Ti3 W1.5 Mo1.5 Nb0.76</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>(Ni2FeCoCr)17.65 Al5 Ti3 W1.5 Mo1.5 Nb0.77</t>
+  </si>
+  <si>
+    <t>FCC+sigma+L12</t>
+  </si>
+  <si>
+    <t>F4b</t>
   </si>
 </sst>
 </file>
@@ -3552,8 +3606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A261" zoomScale="86" workbookViewId="0">
-      <selection activeCell="M288" sqref="M288"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A273" zoomScale="86" workbookViewId="0">
+      <selection activeCell="K300" sqref="K300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -15524,19 +15578,39 @@
     </row>
     <row r="283" spans="1:20" ht="18" customHeight="1">
       <c r="A283" s="64"/>
-      <c r="B283" s="73"/>
-      <c r="C283" s="4"/>
-      <c r="D283" s="4"/>
-      <c r="E283" s="9"/>
-      <c r="F283" s="4"/>
-      <c r="G283" s="68"/>
-      <c r="H283" s="4"/>
-      <c r="I283" s="83"/>
-      <c r="J283" s="70"/>
+      <c r="B283" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C283" s="155" t="s">
+        <v>89</v>
+      </c>
+      <c r="D283" s="155" t="s">
+        <v>360</v>
+      </c>
+      <c r="E283" s="157" t="s">
+        <v>361</v>
+      </c>
+      <c r="F283" s="155" t="s">
+        <v>321</v>
+      </c>
+      <c r="G283" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H283" s="68"/>
+      <c r="I283" s="83">
+        <v>298</v>
+      </c>
+      <c r="J283" s="70">
+        <v>562000000</v>
+      </c>
       <c r="K283" s="70"/>
-      <c r="L283" s="68"/>
+      <c r="L283" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M283" s="68"/>
-      <c r="N283" s="68"/>
+      <c r="N283" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O283" s="9"/>
       <c r="P283" s="4"/>
       <c r="Q283" s="4"/>
@@ -15545,20 +15619,39 @@
       <c r="T283" s="9"/>
     </row>
     <row r="284" spans="1:20" ht="18" customHeight="1">
-      <c r="A284" s="64"/>
-      <c r="B284" s="73"/>
-      <c r="C284" s="4"/>
-      <c r="D284" s="4"/>
-      <c r="E284" s="9"/>
-      <c r="F284" s="4"/>
-      <c r="G284" s="68"/>
-      <c r="H284" s="4"/>
-      <c r="I284" s="83"/>
-      <c r="J284" s="70"/>
+      <c r="B284" s="111" t="s">
+        <v>372</v>
+      </c>
+      <c r="C284" s="155" t="s">
+        <v>89</v>
+      </c>
+      <c r="D284" s="155" t="s">
+        <v>360</v>
+      </c>
+      <c r="E284" s="157" t="s">
+        <v>361</v>
+      </c>
+      <c r="F284" s="155" t="s">
+        <v>323</v>
+      </c>
+      <c r="G284" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H284" s="68"/>
+      <c r="I284" s="83">
+        <v>298</v>
+      </c>
+      <c r="J284" s="70">
+        <v>865000000</v>
+      </c>
       <c r="K284" s="70"/>
-      <c r="L284" s="68"/>
+      <c r="L284" s="112" t="s">
+        <v>33</v>
+      </c>
       <c r="M284" s="68"/>
-      <c r="N284" s="68"/>
+      <c r="N284" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O284" s="9"/>
       <c r="P284" s="4"/>
       <c r="Q284" s="4"/>
@@ -15567,20 +15660,39 @@
       <c r="T284" s="9"/>
     </row>
     <row r="285" spans="1:20" ht="18" customHeight="1">
-      <c r="A285" s="64"/>
-      <c r="B285" s="73"/>
-      <c r="C285" s="4"/>
-      <c r="D285" s="4"/>
-      <c r="E285" s="9"/>
-      <c r="F285" s="4"/>
-      <c r="G285" s="68"/>
-      <c r="H285" s="4"/>
-      <c r="I285" s="83"/>
-      <c r="J285" s="70"/>
+      <c r="B285" s="111" t="s">
+        <v>374</v>
+      </c>
+      <c r="C285" s="155" t="s">
+        <v>89</v>
+      </c>
+      <c r="D285" s="155" t="s">
+        <v>360</v>
+      </c>
+      <c r="E285" s="157" t="s">
+        <v>361</v>
+      </c>
+      <c r="F285" s="155" t="s">
+        <v>322</v>
+      </c>
+      <c r="G285" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H285" s="68"/>
+      <c r="I285" s="83">
+        <v>298</v>
+      </c>
+      <c r="J285" s="70">
+        <v>44</v>
+      </c>
       <c r="K285" s="70"/>
-      <c r="L285" s="68"/>
+      <c r="L285" s="112" t="s">
+        <v>171</v>
+      </c>
       <c r="M285" s="68"/>
-      <c r="N285" s="68"/>
+      <c r="N285" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O285" s="9"/>
       <c r="P285" s="4"/>
       <c r="Q285" s="4"/>
@@ -15589,20 +15701,44 @@
       <c r="T285" s="9"/>
     </row>
     <row r="286" spans="1:20" ht="18" customHeight="1">
-      <c r="A286" s="64"/>
-      <c r="B286" s="73"/>
-      <c r="C286" s="4"/>
-      <c r="D286" s="4"/>
-      <c r="E286" s="9"/>
-      <c r="F286" s="4"/>
-      <c r="G286" s="68"/>
-      <c r="H286" s="4"/>
-      <c r="I286" s="83"/>
-      <c r="J286" s="70"/>
+      <c r="A286" s="116" t="s">
+        <v>368</v>
+      </c>
+      <c r="B286" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C286" s="155" t="s">
+        <v>233</v>
+      </c>
+      <c r="D286" s="155" t="s">
+        <v>363</v>
+      </c>
+      <c r="E286" s="157" t="s">
+        <v>364</v>
+      </c>
+      <c r="F286" s="155" t="s">
+        <v>321</v>
+      </c>
+      <c r="G286" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H286" s="68"/>
+      <c r="I286" s="83">
+        <v>298</v>
+      </c>
+      <c r="J286" s="70">
+        <v>1683000000</v>
+      </c>
       <c r="K286" s="70"/>
-      <c r="L286" s="68"/>
-      <c r="M286" s="68"/>
-      <c r="N286" s="68"/>
+      <c r="L286" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M286" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N286" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O286" s="9"/>
       <c r="P286" s="4"/>
       <c r="Q286" s="4"/>
@@ -15611,20 +15747,44 @@
       <c r="T286" s="9"/>
     </row>
     <row r="287" spans="1:20" ht="18" customHeight="1">
-      <c r="A287" s="64"/>
-      <c r="B287" s="73"/>
-      <c r="C287" s="4"/>
-      <c r="D287" s="4"/>
-      <c r="E287" s="9"/>
-      <c r="F287" s="4"/>
-      <c r="G287" s="68"/>
-      <c r="H287" s="4"/>
-      <c r="I287" s="83"/>
-      <c r="J287" s="70"/>
+      <c r="A287" s="116" t="s">
+        <v>367</v>
+      </c>
+      <c r="B287" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C287" s="155" t="s">
+        <v>375</v>
+      </c>
+      <c r="D287" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E287" s="157" t="s">
+        <v>366</v>
+      </c>
+      <c r="F287" s="155" t="s">
+        <v>321</v>
+      </c>
+      <c r="G287" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H287" s="68"/>
+      <c r="I287" s="83">
+        <v>298</v>
+      </c>
+      <c r="J287" s="70">
+        <v>1822000000</v>
+      </c>
       <c r="K287" s="70"/>
-      <c r="L287" s="68"/>
-      <c r="M287" s="68"/>
-      <c r="N287" s="68"/>
+      <c r="L287" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M287" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N287" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O287" s="9"/>
       <c r="P287" s="4"/>
       <c r="Q287" s="4"/>
@@ -15633,20 +15793,44 @@
       <c r="T287" s="9"/>
     </row>
     <row r="288" spans="1:20" ht="18" customHeight="1">
-      <c r="A288" s="64"/>
-      <c r="B288" s="73"/>
-      <c r="C288" s="4"/>
-      <c r="D288" s="4"/>
-      <c r="E288" s="9"/>
-      <c r="F288" s="4"/>
-      <c r="G288" s="68"/>
-      <c r="H288" s="4"/>
-      <c r="I288" s="83"/>
-      <c r="J288" s="70"/>
+      <c r="A288" s="116" t="s">
+        <v>371</v>
+      </c>
+      <c r="B288" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C288" s="155" t="s">
+        <v>375</v>
+      </c>
+      <c r="D288" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E288" s="157" t="s">
+        <v>369</v>
+      </c>
+      <c r="F288" s="155" t="s">
+        <v>321</v>
+      </c>
+      <c r="G288" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H288" s="68"/>
+      <c r="I288" s="83">
+        <v>298</v>
+      </c>
+      <c r="J288" s="70">
+        <v>1686000000</v>
+      </c>
       <c r="K288" s="70"/>
-      <c r="L288" s="68"/>
-      <c r="M288" s="68"/>
-      <c r="N288" s="68"/>
+      <c r="L288" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M288" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N288" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O288" s="9"/>
       <c r="P288" s="4"/>
       <c r="Q288" s="4"/>
@@ -15655,20 +15839,44 @@
       <c r="T288" s="9"/>
     </row>
     <row r="289" spans="1:20" ht="18" customHeight="1">
-      <c r="A289" s="64"/>
-      <c r="B289" s="73"/>
-      <c r="C289" s="4"/>
-      <c r="D289" s="4"/>
-      <c r="E289" s="9"/>
-      <c r="F289" s="4"/>
-      <c r="G289" s="68"/>
-      <c r="H289" s="4"/>
-      <c r="I289" s="83"/>
-      <c r="J289" s="70"/>
+      <c r="A289" s="116" t="s">
+        <v>373</v>
+      </c>
+      <c r="B289" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C289" s="155" t="s">
+        <v>375</v>
+      </c>
+      <c r="D289" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E289" s="157" t="s">
+        <v>370</v>
+      </c>
+      <c r="F289" s="155" t="s">
+        <v>321</v>
+      </c>
+      <c r="G289" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H289" s="68"/>
+      <c r="I289" s="83">
+        <v>298</v>
+      </c>
+      <c r="J289" s="70">
+        <v>1384000000</v>
+      </c>
       <c r="K289" s="70"/>
-      <c r="L289" s="68"/>
-      <c r="M289" s="68"/>
-      <c r="N289" s="68"/>
+      <c r="L289" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M289" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N289" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O289" s="9"/>
       <c r="P289" s="4"/>
       <c r="Q289" s="4"/>
@@ -15677,20 +15885,44 @@
       <c r="T289" s="9"/>
     </row>
     <row r="290" spans="1:20" ht="18" customHeight="1">
-      <c r="A290" s="64"/>
-      <c r="B290" s="73"/>
-      <c r="C290" s="4"/>
-      <c r="D290" s="4"/>
-      <c r="E290" s="9"/>
-      <c r="F290" s="4"/>
-      <c r="G290" s="68"/>
-      <c r="H290" s="4"/>
-      <c r="I290" s="83"/>
-      <c r="J290" s="70"/>
+      <c r="A290" s="116" t="s">
+        <v>368</v>
+      </c>
+      <c r="B290" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C290" s="155" t="s">
+        <v>233</v>
+      </c>
+      <c r="D290" s="155" t="s">
+        <v>363</v>
+      </c>
+      <c r="E290" s="157" t="s">
+        <v>364</v>
+      </c>
+      <c r="F290" s="155" t="s">
+        <v>323</v>
+      </c>
+      <c r="G290" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H290" s="68"/>
+      <c r="I290" s="83">
+        <v>298</v>
+      </c>
+      <c r="J290" s="70">
+        <v>1698000000</v>
+      </c>
       <c r="K290" s="70"/>
-      <c r="L290" s="68"/>
-      <c r="M290" s="68"/>
-      <c r="N290" s="68"/>
+      <c r="L290" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M290" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N290" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O290" s="9"/>
       <c r="P290" s="4"/>
       <c r="Q290" s="4"/>
@@ -15699,20 +15931,44 @@
       <c r="T290" s="9"/>
     </row>
     <row r="291" spans="1:20" ht="18" customHeight="1">
-      <c r="A291" s="64"/>
-      <c r="B291" s="73"/>
-      <c r="C291" s="4"/>
-      <c r="D291" s="4"/>
-      <c r="E291" s="9"/>
-      <c r="F291" s="4"/>
-      <c r="G291" s="68"/>
-      <c r="H291" s="4"/>
-      <c r="I291" s="83"/>
-      <c r="J291" s="70"/>
+      <c r="A291" s="116" t="s">
+        <v>367</v>
+      </c>
+      <c r="B291" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C291" s="155" t="s">
+        <v>375</v>
+      </c>
+      <c r="D291" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E291" s="157" t="s">
+        <v>366</v>
+      </c>
+      <c r="F291" s="155" t="s">
+        <v>323</v>
+      </c>
+      <c r="G291" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H291" s="68"/>
+      <c r="I291" s="83">
+        <v>298</v>
+      </c>
+      <c r="J291" s="70">
+        <v>1930000000</v>
+      </c>
       <c r="K291" s="70"/>
-      <c r="L291" s="68"/>
-      <c r="M291" s="68"/>
-      <c r="N291" s="68"/>
+      <c r="L291" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M291" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N291" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O291" s="9"/>
       <c r="P291" s="4"/>
       <c r="Q291" s="4"/>
@@ -15721,20 +15977,44 @@
       <c r="T291" s="9"/>
     </row>
     <row r="292" spans="1:20" ht="18" customHeight="1">
-      <c r="A292" s="64"/>
-      <c r="B292" s="73"/>
-      <c r="C292" s="4"/>
-      <c r="D292" s="4"/>
-      <c r="E292" s="9"/>
-      <c r="F292" s="4"/>
-      <c r="G292" s="4"/>
-      <c r="H292" s="4"/>
-      <c r="I292" s="83"/>
-      <c r="J292" s="70"/>
+      <c r="A292" s="116" t="s">
+        <v>371</v>
+      </c>
+      <c r="B292" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C292" s="155" t="s">
+        <v>375</v>
+      </c>
+      <c r="D292" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E292" s="157" t="s">
+        <v>369</v>
+      </c>
+      <c r="F292" s="155" t="s">
+        <v>323</v>
+      </c>
+      <c r="G292" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H292" s="68"/>
+      <c r="I292" s="83">
+        <v>298</v>
+      </c>
+      <c r="J292" s="70">
+        <v>1853000000</v>
+      </c>
       <c r="K292" s="70"/>
-      <c r="L292" s="68"/>
-      <c r="M292" s="68"/>
-      <c r="N292" s="68"/>
+      <c r="L292" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M292" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N292" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O292" s="9"/>
       <c r="P292" s="4"/>
       <c r="Q292" s="4"/>
@@ -15743,20 +16023,44 @@
       <c r="T292" s="9"/>
     </row>
     <row r="293" spans="1:20" ht="18" customHeight="1">
-      <c r="A293" s="64"/>
-      <c r="B293" s="73"/>
-      <c r="C293" s="4"/>
-      <c r="D293" s="4"/>
-      <c r="E293" s="9"/>
-      <c r="F293" s="4"/>
-      <c r="G293" s="4"/>
-      <c r="H293" s="4"/>
-      <c r="I293" s="83"/>
-      <c r="J293" s="70"/>
+      <c r="A293" s="116" t="s">
+        <v>373</v>
+      </c>
+      <c r="B293" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C293" s="155" t="s">
+        <v>375</v>
+      </c>
+      <c r="D293" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E293" s="157" t="s">
+        <v>370</v>
+      </c>
+      <c r="F293" s="155" t="s">
+        <v>323</v>
+      </c>
+      <c r="G293" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H293" s="68"/>
+      <c r="I293" s="83">
+        <v>298</v>
+      </c>
+      <c r="J293" s="70">
+        <v>1727000000</v>
+      </c>
       <c r="K293" s="70"/>
-      <c r="L293" s="68"/>
-      <c r="M293" s="68"/>
-      <c r="N293" s="68"/>
+      <c r="L293" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="M293" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N293" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O293" s="9"/>
       <c r="P293" s="4"/>
       <c r="Q293" s="4"/>
@@ -15765,20 +16069,44 @@
       <c r="T293" s="9"/>
     </row>
     <row r="294" spans="1:20" ht="18" customHeight="1">
-      <c r="A294" s="64"/>
-      <c r="B294" s="73"/>
-      <c r="C294" s="4"/>
-      <c r="D294" s="4"/>
-      <c r="E294" s="9"/>
-      <c r="F294" s="4"/>
-      <c r="G294" s="4"/>
-      <c r="H294" s="4"/>
-      <c r="I294" s="83"/>
-      <c r="J294" s="70"/>
+      <c r="A294" s="116" t="s">
+        <v>368</v>
+      </c>
+      <c r="B294" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C294" s="155" t="s">
+        <v>233</v>
+      </c>
+      <c r="D294" s="155" t="s">
+        <v>363</v>
+      </c>
+      <c r="E294" s="157" t="s">
+        <v>364</v>
+      </c>
+      <c r="F294" s="155" t="s">
+        <v>322</v>
+      </c>
+      <c r="G294" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H294" s="68"/>
+      <c r="I294" s="83">
+        <v>298</v>
+      </c>
+      <c r="J294" s="70">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="K294" s="70"/>
-      <c r="L294" s="68"/>
-      <c r="M294" s="68"/>
-      <c r="N294" s="68"/>
+      <c r="L294" s="112" t="s">
+        <v>171</v>
+      </c>
+      <c r="M294" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N294" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O294" s="9"/>
       <c r="P294" s="4"/>
       <c r="Q294" s="4"/>
@@ -15787,20 +16115,44 @@
       <c r="T294" s="9"/>
     </row>
     <row r="295" spans="1:20" ht="18" customHeight="1">
-      <c r="A295" s="64"/>
-      <c r="B295" s="73"/>
-      <c r="C295" s="4"/>
-      <c r="D295" s="4"/>
-      <c r="E295" s="9"/>
-      <c r="F295" s="4"/>
-      <c r="G295" s="4"/>
-      <c r="H295" s="4"/>
-      <c r="I295" s="83"/>
-      <c r="J295" s="70"/>
+      <c r="A295" s="116" t="s">
+        <v>367</v>
+      </c>
+      <c r="B295" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C295" s="155" t="s">
+        <v>375</v>
+      </c>
+      <c r="D295" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E295" s="157" t="s">
+        <v>366</v>
+      </c>
+      <c r="F295" s="155" t="s">
+        <v>322</v>
+      </c>
+      <c r="G295" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H295" s="68"/>
+      <c r="I295" s="83">
+        <v>298</v>
+      </c>
+      <c r="J295" s="70">
+        <v>11.4</v>
+      </c>
       <c r="K295" s="70"/>
-      <c r="L295" s="68"/>
-      <c r="M295" s="68"/>
-      <c r="N295" s="68"/>
+      <c r="L295" s="112" t="s">
+        <v>171</v>
+      </c>
+      <c r="M295" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N295" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O295" s="9"/>
       <c r="P295" s="4"/>
       <c r="Q295" s="4"/>
@@ -15809,20 +16161,44 @@
       <c r="T295" s="9"/>
     </row>
     <row r="296" spans="1:20" ht="18" customHeight="1">
-      <c r="A296" s="64"/>
-      <c r="B296" s="73"/>
-      <c r="C296" s="4"/>
-      <c r="D296" s="4"/>
-      <c r="E296" s="9"/>
-      <c r="F296" s="4"/>
-      <c r="G296" s="4"/>
-      <c r="H296" s="4"/>
-      <c r="I296" s="83"/>
-      <c r="J296" s="70"/>
+      <c r="A296" s="116" t="s">
+        <v>371</v>
+      </c>
+      <c r="B296" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C296" s="155" t="s">
+        <v>375</v>
+      </c>
+      <c r="D296" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E296" s="157" t="s">
+        <v>369</v>
+      </c>
+      <c r="F296" s="155" t="s">
+        <v>322</v>
+      </c>
+      <c r="G296" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H296" s="68"/>
+      <c r="I296" s="83">
+        <v>298</v>
+      </c>
+      <c r="J296" s="70">
+        <v>12.8</v>
+      </c>
       <c r="K296" s="70"/>
-      <c r="L296" s="68"/>
-      <c r="M296" s="68"/>
-      <c r="N296" s="68"/>
+      <c r="L296" s="112" t="s">
+        <v>171</v>
+      </c>
+      <c r="M296" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N296" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O296" s="9"/>
       <c r="P296" s="4"/>
       <c r="Q296" s="4"/>
@@ -15831,20 +16207,44 @@
       <c r="T296" s="9"/>
     </row>
     <row r="297" spans="1:20" ht="18" customHeight="1">
-      <c r="A297" s="64"/>
-      <c r="B297" s="73"/>
-      <c r="C297" s="4"/>
-      <c r="D297" s="4"/>
-      <c r="E297" s="9"/>
-      <c r="F297" s="4"/>
-      <c r="G297" s="4"/>
-      <c r="H297" s="4"/>
-      <c r="I297" s="83"/>
-      <c r="J297" s="70"/>
+      <c r="A297" s="116" t="s">
+        <v>373</v>
+      </c>
+      <c r="B297" s="111" t="s">
+        <v>362</v>
+      </c>
+      <c r="C297" s="155" t="s">
+        <v>375</v>
+      </c>
+      <c r="D297" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E297" s="157" t="s">
+        <v>370</v>
+      </c>
+      <c r="F297" s="155" t="s">
+        <v>322</v>
+      </c>
+      <c r="G297" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H297" s="68"/>
+      <c r="I297" s="83">
+        <v>298</v>
+      </c>
+      <c r="J297" s="70">
+        <v>19.5</v>
+      </c>
       <c r="K297" s="70"/>
-      <c r="L297" s="68"/>
-      <c r="M297" s="68"/>
-      <c r="N297" s="68"/>
+      <c r="L297" s="112" t="s">
+        <v>171</v>
+      </c>
+      <c r="M297" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N297" s="112" t="s">
+        <v>359</v>
+      </c>
       <c r="O297" s="9"/>
       <c r="P297" s="4"/>
       <c r="Q297" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1038/s41598-023-43085-y`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8B4D9D-061B-9B43-A9A0-30B59DC8DB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DAAEAB-DC2F-6F47-9302-EBA5F4AC690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="1580" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5980" yWindow="6320" windowWidth="22340" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2473" uniqueCount="380">
   <si>
     <r>
       <rPr>
@@ -1261,6 +1261,15 @@
   </si>
   <si>
     <t>F4b</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nb3Ta3MoWTh</t>
+  </si>
+  <si>
+    <t>superconducting transition temperature</t>
+  </si>
+  <si>
+    <t>10.1038/s41598-023-43085-y</t>
   </si>
 </sst>
 </file>
@@ -2328,6 +2337,62 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2388,62 +2453,6 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3606,8 +3615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A273" zoomScale="86" workbookViewId="0">
-      <selection activeCell="K300" sqref="K300"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A283" zoomScale="86" workbookViewId="0">
+      <selection activeCell="H304" sqref="H304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3664,19 +3673,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="118" t="s">
+      <c r="D2" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="119"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="123"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="126"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="145"/>
+      <c r="M2" s="145"/>
+      <c r="N2" s="148"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3692,17 +3701,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="130"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="151"/>
+      <c r="L3" s="149"/>
+      <c r="M3" s="149"/>
+      <c r="N3" s="152"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3743,43 +3752,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="131" t="s">
+      <c r="C5" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="133" t="s">
+      <c r="D5" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="133" t="s">
+      <c r="E5" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="133" t="s">
+      <c r="F5" s="155" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="133" t="s">
+      <c r="G5" s="155" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="134" t="s">
+      <c r="H5" s="156" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="133" t="s">
+      <c r="I5" s="155" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="133" t="s">
+      <c r="J5" s="155" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="133" t="s">
+      <c r="K5" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="133" t="s">
+      <c r="L5" s="155" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="133" t="s">
+      <c r="M5" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="133" t="s">
+      <c r="N5" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="138" t="s">
+      <c r="O5" s="123" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3795,19 +3804,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="137"/>
-      <c r="K6" s="137"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
-      <c r="O6" s="139"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="154"/>
+      <c r="E6" s="154"/>
+      <c r="F6" s="154"/>
+      <c r="G6" s="154"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="158"/>
+      <c r="J6" s="159"/>
+      <c r="K6" s="159"/>
+      <c r="L6" s="154"/>
+      <c r="M6" s="154"/>
+      <c r="N6" s="154"/>
+      <c r="O6" s="124"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3857,7 +3866,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="140"/>
+      <c r="O7" s="125"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -3872,35 +3881,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="142"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="143"/>
-      <c r="F8" s="144" t="s">
+      <c r="C8" s="127"/>
+      <c r="D8" s="127"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="145"/>
-      <c r="H8" s="145"/>
-      <c r="I8" s="146"/>
-      <c r="J8" s="147"/>
-      <c r="K8" s="147"/>
-      <c r="L8" s="148"/>
-      <c r="M8" s="149" t="s">
+      <c r="G8" s="130"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="131"/>
+      <c r="J8" s="132"/>
+      <c r="K8" s="132"/>
+      <c r="L8" s="133"/>
+      <c r="M8" s="134" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="150"/>
+      <c r="N8" s="135"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="151" t="s">
+      <c r="P8" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="152"/>
-      <c r="R8" s="153"/>
-      <c r="S8" s="153"/>
-      <c r="T8" s="154"/>
+      <c r="Q8" s="137"/>
+      <c r="R8" s="138"/>
+      <c r="S8" s="138"/>
+      <c r="T8" s="139"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="38" t="s">
@@ -14588,13 +14597,13 @@
         <v>327</v>
       </c>
       <c r="C257" s="4"/>
-      <c r="D257" s="155" t="s">
+      <c r="D257" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="E257" s="157" t="s">
+      <c r="E257" s="120" t="s">
         <v>329</v>
       </c>
-      <c r="F257" s="155" t="s">
+      <c r="F257" s="118" t="s">
         <v>326</v>
       </c>
       <c r="G257" s="112" t="s">
@@ -14604,7 +14613,7 @@
       <c r="I257" s="83">
         <v>298</v>
       </c>
-      <c r="J257" s="156">
+      <c r="J257" s="119">
         <v>0</v>
       </c>
       <c r="K257" s="70"/>
@@ -14628,13 +14637,13 @@
         <v>328</v>
       </c>
       <c r="C258" s="4"/>
-      <c r="D258" s="155" t="s">
+      <c r="D258" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="E258" s="157" t="s">
+      <c r="E258" s="120" t="s">
         <v>329</v>
       </c>
-      <c r="F258" s="155" t="s">
+      <c r="F258" s="118" t="s">
         <v>326</v>
       </c>
       <c r="G258" s="112" t="s">
@@ -14667,16 +14676,16 @@
       <c r="B259" s="111" t="s">
         <v>332</v>
       </c>
-      <c r="C259" s="155" t="s">
+      <c r="C259" s="118" t="s">
         <v>319</v>
       </c>
-      <c r="D259" s="155" t="s">
+      <c r="D259" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E259" s="111" t="s">
         <v>336</v>
       </c>
-      <c r="F259" s="155" t="s">
+      <c r="F259" s="118" t="s">
         <v>169</v>
       </c>
       <c r="G259" s="112" t="s">
@@ -14711,14 +14720,14 @@
       <c r="B260" s="111" t="s">
         <v>333</v>
       </c>
-      <c r="C260" s="155" t="s">
+      <c r="C260" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D260" s="155" t="s">
+      <c r="D260" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E260" s="9"/>
-      <c r="F260" s="155" t="s">
+      <c r="F260" s="118" t="s">
         <v>169</v>
       </c>
       <c r="G260" s="112" t="s">
@@ -14753,14 +14762,14 @@
       <c r="B261" s="111" t="s">
         <v>334</v>
       </c>
-      <c r="C261" s="155" t="s">
+      <c r="C261" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D261" s="155" t="s">
+      <c r="D261" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E261" s="9"/>
-      <c r="F261" s="155" t="s">
+      <c r="F261" s="118" t="s">
         <v>169</v>
       </c>
       <c r="G261" s="112" t="s">
@@ -14795,14 +14804,14 @@
       <c r="B262" s="111" t="s">
         <v>335</v>
       </c>
-      <c r="C262" s="155" t="s">
+      <c r="C262" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D262" s="155" t="s">
+      <c r="D262" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E262" s="9"/>
-      <c r="F262" s="155" t="s">
+      <c r="F262" s="118" t="s">
         <v>169</v>
       </c>
       <c r="G262" s="112" t="s">
@@ -14837,16 +14846,16 @@
       <c r="B263" s="111" t="s">
         <v>332</v>
       </c>
-      <c r="C263" s="155" t="s">
+      <c r="C263" s="118" t="s">
         <v>319</v>
       </c>
-      <c r="D263" s="155" t="s">
+      <c r="D263" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E263" s="111" t="s">
         <v>336</v>
       </c>
-      <c r="F263" s="155" t="s">
+      <c r="F263" s="118" t="s">
         <v>189</v>
       </c>
       <c r="G263" s="112" t="s">
@@ -14881,14 +14890,14 @@
       <c r="B264" s="111" t="s">
         <v>333</v>
       </c>
-      <c r="C264" s="155" t="s">
+      <c r="C264" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D264" s="155" t="s">
+      <c r="D264" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E264" s="9"/>
-      <c r="F264" s="155" t="s">
+      <c r="F264" s="118" t="s">
         <v>189</v>
       </c>
       <c r="G264" s="112" t="s">
@@ -14923,14 +14932,14 @@
       <c r="B265" s="111" t="s">
         <v>334</v>
       </c>
-      <c r="C265" s="155" t="s">
+      <c r="C265" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D265" s="155" t="s">
+      <c r="D265" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E265" s="9"/>
-      <c r="F265" s="155" t="s">
+      <c r="F265" s="118" t="s">
         <v>189</v>
       </c>
       <c r="G265" s="112" t="s">
@@ -14965,14 +14974,14 @@
       <c r="B266" s="111" t="s">
         <v>335</v>
       </c>
-      <c r="C266" s="155" t="s">
+      <c r="C266" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D266" s="155" t="s">
+      <c r="D266" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E266" s="9"/>
-      <c r="F266" s="155" t="s">
+      <c r="F266" s="118" t="s">
         <v>189</v>
       </c>
       <c r="G266" s="112" t="s">
@@ -15007,16 +15016,16 @@
       <c r="B267" s="111" t="s">
         <v>332</v>
       </c>
-      <c r="C267" s="155" t="s">
+      <c r="C267" s="118" t="s">
         <v>319</v>
       </c>
-      <c r="D267" s="155" t="s">
+      <c r="D267" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E267" s="111" t="s">
         <v>336</v>
       </c>
-      <c r="F267" s="155" t="s">
+      <c r="F267" s="118" t="s">
         <v>170</v>
       </c>
       <c r="G267" s="112" t="s">
@@ -15051,14 +15060,14 @@
       <c r="B268" s="111" t="s">
         <v>333</v>
       </c>
-      <c r="C268" s="155" t="s">
+      <c r="C268" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D268" s="155" t="s">
+      <c r="D268" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E268" s="9"/>
-      <c r="F268" s="155" t="s">
+      <c r="F268" s="118" t="s">
         <v>170</v>
       </c>
       <c r="G268" s="112" t="s">
@@ -15093,14 +15102,14 @@
       <c r="B269" s="111" t="s">
         <v>334</v>
       </c>
-      <c r="C269" s="155" t="s">
+      <c r="C269" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D269" s="155" t="s">
+      <c r="D269" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E269" s="9"/>
-      <c r="F269" s="155" t="s">
+      <c r="F269" s="118" t="s">
         <v>246</v>
       </c>
       <c r="G269" s="112" t="s">
@@ -15135,14 +15144,14 @@
       <c r="B270" s="111" t="s">
         <v>335</v>
       </c>
-      <c r="C270" s="155" t="s">
+      <c r="C270" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D270" s="155" t="s">
+      <c r="D270" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E270" s="9"/>
-      <c r="F270" s="155" t="s">
+      <c r="F270" s="118" t="s">
         <v>246</v>
       </c>
       <c r="G270" s="112" t="s">
@@ -15177,14 +15186,14 @@
       <c r="B271" s="111" t="s">
         <v>338</v>
       </c>
-      <c r="C271" s="155" t="s">
+      <c r="C271" s="118" t="s">
         <v>340</v>
       </c>
-      <c r="D271" s="155" t="s">
+      <c r="D271" s="118" t="s">
         <v>339</v>
       </c>
       <c r="E271" s="9"/>
-      <c r="F271" s="155" t="s">
+      <c r="F271" s="118" t="s">
         <v>341</v>
       </c>
       <c r="G271" s="112" t="s">
@@ -15215,14 +15224,14 @@
       <c r="B272" s="111" t="s">
         <v>338</v>
       </c>
-      <c r="C272" s="155" t="s">
+      <c r="C272" s="118" t="s">
         <v>340</v>
       </c>
-      <c r="D272" s="155" t="s">
+      <c r="D272" s="118" t="s">
         <v>339</v>
       </c>
       <c r="E272" s="9"/>
-      <c r="F272" s="155" t="s">
+      <c r="F272" s="118" t="s">
         <v>251</v>
       </c>
       <c r="G272" s="112" t="s">
@@ -15255,14 +15264,14 @@
       <c r="B273" s="111" t="s">
         <v>338</v>
       </c>
-      <c r="C273" s="155" t="s">
+      <c r="C273" s="118" t="s">
         <v>340</v>
       </c>
-      <c r="D273" s="155" t="s">
+      <c r="D273" s="118" t="s">
         <v>339</v>
       </c>
       <c r="E273" s="9"/>
-      <c r="F273" s="155" t="s">
+      <c r="F273" s="118" t="s">
         <v>251</v>
       </c>
       <c r="G273" s="112" t="s">
@@ -15272,7 +15281,7 @@
       <c r="I273" s="117">
         <v>140</v>
       </c>
-      <c r="J273" s="158">
+      <c r="J273" s="121">
         <v>1.17E-6</v>
       </c>
       <c r="K273" s="70"/>
@@ -15295,14 +15304,14 @@
       <c r="B274" s="111" t="s">
         <v>338</v>
       </c>
-      <c r="C274" s="155" t="s">
+      <c r="C274" s="118" t="s">
         <v>340</v>
       </c>
-      <c r="D274" s="155" t="s">
+      <c r="D274" s="118" t="s">
         <v>339</v>
       </c>
       <c r="E274" s="9"/>
-      <c r="F274" s="155" t="s">
+      <c r="F274" s="118" t="s">
         <v>251</v>
       </c>
       <c r="G274" s="112" t="s">
@@ -15335,13 +15344,13 @@
       <c r="B275" s="111" t="s">
         <v>343</v>
       </c>
-      <c r="C275" s="155" t="s">
+      <c r="C275" s="118" t="s">
         <v>344</v>
       </c>
-      <c r="D275" s="155" t="s">
+      <c r="D275" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="E275" s="157" t="s">
+      <c r="E275" s="120" t="s">
         <v>345</v>
       </c>
       <c r="F275" s="4"/>
@@ -15367,10 +15376,10 @@
       <c r="B276" s="111" t="s">
         <v>347</v>
       </c>
-      <c r="C276" s="155" t="s">
+      <c r="C276" s="118" t="s">
         <v>349</v>
       </c>
-      <c r="D276" s="155" t="s">
+      <c r="D276" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E276" s="9"/>
@@ -15397,10 +15406,10 @@
       <c r="B277" s="111" t="s">
         <v>348</v>
       </c>
-      <c r="C277" s="155" t="s">
+      <c r="C277" s="118" t="s">
         <v>349</v>
       </c>
-      <c r="D277" s="155" t="s">
+      <c r="D277" s="118" t="s">
         <v>113</v>
       </c>
       <c r="E277" s="9"/>
@@ -15427,13 +15436,13 @@
       <c r="B278" s="111" t="s">
         <v>348</v>
       </c>
-      <c r="C278" s="155" t="s">
+      <c r="C278" s="118" t="s">
         <v>349</v>
       </c>
-      <c r="D278" s="155" t="s">
+      <c r="D278" s="118" t="s">
         <v>187</v>
       </c>
-      <c r="E278" s="157" t="s">
+      <c r="E278" s="120" t="s">
         <v>350</v>
       </c>
       <c r="F278" s="4"/>
@@ -15459,13 +15468,13 @@
       <c r="B279" s="111" t="s">
         <v>353</v>
       </c>
-      <c r="C279" s="155" t="s">
+      <c r="C279" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="D279" s="155" t="s">
+      <c r="D279" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="E279" s="157"/>
+      <c r="E279" s="120"/>
       <c r="F279" s="4"/>
       <c r="G279" s="68"/>
       <c r="H279" s="4"/>
@@ -15489,13 +15498,13 @@
       <c r="B280" s="111" t="s">
         <v>354</v>
       </c>
-      <c r="C280" s="155" t="s">
+      <c r="C280" s="118" t="s">
         <v>358</v>
       </c>
-      <c r="D280" s="155" t="s">
+      <c r="D280" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="E280" s="157"/>
+      <c r="E280" s="120"/>
       <c r="F280" s="4"/>
       <c r="G280" s="68"/>
       <c r="H280" s="4"/>
@@ -15519,13 +15528,13 @@
       <c r="B281" s="111" t="s">
         <v>355</v>
       </c>
-      <c r="C281" s="155" t="s">
+      <c r="C281" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="D281" s="155" t="s">
+      <c r="D281" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="E281" s="157"/>
+      <c r="E281" s="120"/>
       <c r="F281" s="4"/>
       <c r="G281" s="68"/>
       <c r="H281" s="4"/>
@@ -15549,13 +15558,13 @@
       <c r="B282" s="111" t="s">
         <v>356</v>
       </c>
-      <c r="C282" s="159" t="s">
+      <c r="C282" s="122" t="s">
         <v>358</v>
       </c>
-      <c r="D282" s="155" t="s">
+      <c r="D282" s="118" t="s">
         <v>195</v>
       </c>
-      <c r="E282" s="157" t="s">
+      <c r="E282" s="120" t="s">
         <v>357</v>
       </c>
       <c r="F282" s="4"/>
@@ -15581,16 +15590,16 @@
       <c r="B283" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C283" s="155" t="s">
+      <c r="C283" s="118" t="s">
         <v>89</v>
       </c>
-      <c r="D283" s="155" t="s">
+      <c r="D283" s="118" t="s">
         <v>360</v>
       </c>
-      <c r="E283" s="157" t="s">
+      <c r="E283" s="120" t="s">
         <v>361</v>
       </c>
-      <c r="F283" s="155" t="s">
+      <c r="F283" s="118" t="s">
         <v>321</v>
       </c>
       <c r="G283" s="112" t="s">
@@ -15622,16 +15631,16 @@
       <c r="B284" s="111" t="s">
         <v>372</v>
       </c>
-      <c r="C284" s="155" t="s">
+      <c r="C284" s="118" t="s">
         <v>89</v>
       </c>
-      <c r="D284" s="155" t="s">
+      <c r="D284" s="118" t="s">
         <v>360</v>
       </c>
-      <c r="E284" s="157" t="s">
+      <c r="E284" s="120" t="s">
         <v>361</v>
       </c>
-      <c r="F284" s="155" t="s">
+      <c r="F284" s="118" t="s">
         <v>323</v>
       </c>
       <c r="G284" s="112" t="s">
@@ -15663,16 +15672,16 @@
       <c r="B285" s="111" t="s">
         <v>374</v>
       </c>
-      <c r="C285" s="155" t="s">
+      <c r="C285" s="118" t="s">
         <v>89</v>
       </c>
-      <c r="D285" s="155" t="s">
+      <c r="D285" s="118" t="s">
         <v>360</v>
       </c>
-      <c r="E285" s="157" t="s">
+      <c r="E285" s="120" t="s">
         <v>361</v>
       </c>
-      <c r="F285" s="155" t="s">
+      <c r="F285" s="118" t="s">
         <v>322</v>
       </c>
       <c r="G285" s="112" t="s">
@@ -15707,16 +15716,16 @@
       <c r="B286" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C286" s="155" t="s">
+      <c r="C286" s="118" t="s">
         <v>233</v>
       </c>
-      <c r="D286" s="155" t="s">
+      <c r="D286" s="118" t="s">
         <v>363</v>
       </c>
-      <c r="E286" s="157" t="s">
+      <c r="E286" s="120" t="s">
         <v>364</v>
       </c>
-      <c r="F286" s="155" t="s">
+      <c r="F286" s="118" t="s">
         <v>321</v>
       </c>
       <c r="G286" s="112" t="s">
@@ -15753,16 +15762,16 @@
       <c r="B287" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C287" s="155" t="s">
+      <c r="C287" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="D287" s="155" t="s">
+      <c r="D287" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="E287" s="157" t="s">
+      <c r="E287" s="120" t="s">
         <v>366</v>
       </c>
-      <c r="F287" s="155" t="s">
+      <c r="F287" s="118" t="s">
         <v>321</v>
       </c>
       <c r="G287" s="112" t="s">
@@ -15799,16 +15808,16 @@
       <c r="B288" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C288" s="155" t="s">
+      <c r="C288" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="D288" s="155" t="s">
+      <c r="D288" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="E288" s="157" t="s">
+      <c r="E288" s="120" t="s">
         <v>369</v>
       </c>
-      <c r="F288" s="155" t="s">
+      <c r="F288" s="118" t="s">
         <v>321</v>
       </c>
       <c r="G288" s="112" t="s">
@@ -15845,16 +15854,16 @@
       <c r="B289" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C289" s="155" t="s">
+      <c r="C289" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="D289" s="155" t="s">
+      <c r="D289" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="E289" s="157" t="s">
+      <c r="E289" s="120" t="s">
         <v>370</v>
       </c>
-      <c r="F289" s="155" t="s">
+      <c r="F289" s="118" t="s">
         <v>321</v>
       </c>
       <c r="G289" s="112" t="s">
@@ -15891,16 +15900,16 @@
       <c r="B290" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C290" s="155" t="s">
+      <c r="C290" s="118" t="s">
         <v>233</v>
       </c>
-      <c r="D290" s="155" t="s">
+      <c r="D290" s="118" t="s">
         <v>363</v>
       </c>
-      <c r="E290" s="157" t="s">
+      <c r="E290" s="120" t="s">
         <v>364</v>
       </c>
-      <c r="F290" s="155" t="s">
+      <c r="F290" s="118" t="s">
         <v>323</v>
       </c>
       <c r="G290" s="112" t="s">
@@ -15937,16 +15946,16 @@
       <c r="B291" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C291" s="155" t="s">
+      <c r="C291" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="D291" s="155" t="s">
+      <c r="D291" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="E291" s="157" t="s">
+      <c r="E291" s="120" t="s">
         <v>366</v>
       </c>
-      <c r="F291" s="155" t="s">
+      <c r="F291" s="118" t="s">
         <v>323</v>
       </c>
       <c r="G291" s="112" t="s">
@@ -15983,16 +15992,16 @@
       <c r="B292" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C292" s="155" t="s">
+      <c r="C292" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="D292" s="155" t="s">
+      <c r="D292" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="E292" s="157" t="s">
+      <c r="E292" s="120" t="s">
         <v>369</v>
       </c>
-      <c r="F292" s="155" t="s">
+      <c r="F292" s="118" t="s">
         <v>323</v>
       </c>
       <c r="G292" s="112" t="s">
@@ -16029,16 +16038,16 @@
       <c r="B293" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C293" s="155" t="s">
+      <c r="C293" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="D293" s="155" t="s">
+      <c r="D293" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="E293" s="157" t="s">
+      <c r="E293" s="120" t="s">
         <v>370</v>
       </c>
-      <c r="F293" s="155" t="s">
+      <c r="F293" s="118" t="s">
         <v>323</v>
       </c>
       <c r="G293" s="112" t="s">
@@ -16075,16 +16084,16 @@
       <c r="B294" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C294" s="155" t="s">
+      <c r="C294" s="118" t="s">
         <v>233</v>
       </c>
-      <c r="D294" s="155" t="s">
+      <c r="D294" s="118" t="s">
         <v>363</v>
       </c>
-      <c r="E294" s="157" t="s">
+      <c r="E294" s="120" t="s">
         <v>364</v>
       </c>
-      <c r="F294" s="155" t="s">
+      <c r="F294" s="118" t="s">
         <v>322</v>
       </c>
       <c r="G294" s="112" t="s">
@@ -16121,16 +16130,16 @@
       <c r="B295" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C295" s="155" t="s">
+      <c r="C295" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="D295" s="155" t="s">
+      <c r="D295" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="E295" s="157" t="s">
+      <c r="E295" s="120" t="s">
         <v>366</v>
       </c>
-      <c r="F295" s="155" t="s">
+      <c r="F295" s="118" t="s">
         <v>322</v>
       </c>
       <c r="G295" s="112" t="s">
@@ -16167,16 +16176,16 @@
       <c r="B296" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C296" s="155" t="s">
+      <c r="C296" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="D296" s="155" t="s">
+      <c r="D296" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="E296" s="157" t="s">
+      <c r="E296" s="120" t="s">
         <v>369</v>
       </c>
-      <c r="F296" s="155" t="s">
+      <c r="F296" s="118" t="s">
         <v>322</v>
       </c>
       <c r="G296" s="112" t="s">
@@ -16213,16 +16222,16 @@
       <c r="B297" s="111" t="s">
         <v>362</v>
       </c>
-      <c r="C297" s="155" t="s">
+      <c r="C297" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="D297" s="155" t="s">
+      <c r="D297" s="118" t="s">
         <v>365</v>
       </c>
-      <c r="E297" s="157" t="s">
+      <c r="E297" s="120" t="s">
         <v>370</v>
       </c>
-      <c r="F297" s="155" t="s">
+      <c r="F297" s="118" t="s">
         <v>322</v>
       </c>
       <c r="G297" s="112" t="s">
@@ -16254,19 +16263,35 @@
     </row>
     <row r="298" spans="1:20" ht="18" customHeight="1">
       <c r="A298" s="64"/>
-      <c r="B298" s="73"/>
-      <c r="C298" s="4"/>
-      <c r="D298" s="4"/>
+      <c r="B298" s="111" t="s">
+        <v>377</v>
+      </c>
+      <c r="C298" s="118" t="s">
+        <v>124</v>
+      </c>
+      <c r="D298" s="118" t="s">
+        <v>113</v>
+      </c>
       <c r="E298" s="9"/>
-      <c r="F298" s="4"/>
-      <c r="G298" s="4"/>
+      <c r="F298" s="118" t="s">
+        <v>378</v>
+      </c>
+      <c r="G298" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H298" s="4"/>
       <c r="I298" s="83"/>
-      <c r="J298" s="70"/>
+      <c r="J298" s="70">
+        <v>5.6</v>
+      </c>
       <c r="K298" s="70"/>
-      <c r="L298" s="68"/>
+      <c r="L298" s="112" t="s">
+        <v>249</v>
+      </c>
       <c r="M298" s="68"/>
-      <c r="N298" s="68"/>
+      <c r="N298" s="112" t="s">
+        <v>379</v>
+      </c>
       <c r="O298" s="9"/>
       <c r="P298" s="4"/>
       <c r="Q298" s="4"/>
@@ -16276,19 +16301,39 @@
     </row>
     <row r="299" spans="1:20" ht="18" customHeight="1">
       <c r="A299" s="64"/>
-      <c r="B299" s="73"/>
-      <c r="C299" s="4"/>
-      <c r="D299" s="4"/>
+      <c r="B299" s="111" t="s">
+        <v>377</v>
+      </c>
+      <c r="C299" s="118" t="s">
+        <v>124</v>
+      </c>
+      <c r="D299" s="118" t="s">
+        <v>113</v>
+      </c>
       <c r="E299" s="9"/>
-      <c r="F299" s="4"/>
-      <c r="G299" s="4"/>
+      <c r="F299" s="118" t="s">
+        <v>251</v>
+      </c>
+      <c r="G299" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H299" s="4"/>
-      <c r="I299" s="83"/>
-      <c r="J299" s="70"/>
+      <c r="I299" s="83">
+        <v>22</v>
+      </c>
+      <c r="J299" s="70">
+        <v>2.3300000000000001E-7</v>
+      </c>
       <c r="K299" s="70"/>
-      <c r="L299" s="68"/>
-      <c r="M299" s="68"/>
-      <c r="N299" s="68"/>
+      <c r="L299" s="112" t="s">
+        <v>252</v>
+      </c>
+      <c r="M299" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N299" s="112" t="s">
+        <v>379</v>
+      </c>
       <c r="O299" s="9"/>
       <c r="P299" s="4"/>
       <c r="Q299" s="4"/>
@@ -16298,19 +16343,39 @@
     </row>
     <row r="300" spans="1:20" ht="18" customHeight="1">
       <c r="A300" s="64"/>
-      <c r="B300" s="73"/>
-      <c r="C300" s="4"/>
-      <c r="D300" s="4"/>
+      <c r="B300" s="111" t="s">
+        <v>377</v>
+      </c>
+      <c r="C300" s="118" t="s">
+        <v>124</v>
+      </c>
+      <c r="D300" s="118" t="s">
+        <v>113</v>
+      </c>
       <c r="E300" s="9"/>
-      <c r="F300" s="4"/>
-      <c r="G300" s="4"/>
+      <c r="F300" s="118" t="s">
+        <v>251</v>
+      </c>
+      <c r="G300" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H300" s="4"/>
-      <c r="I300" s="83"/>
-      <c r="J300" s="70"/>
+      <c r="I300" s="117">
+        <v>140</v>
+      </c>
+      <c r="J300" s="70">
+        <v>3.8799999999999998E-7</v>
+      </c>
       <c r="K300" s="70"/>
-      <c r="L300" s="68"/>
-      <c r="M300" s="68"/>
-      <c r="N300" s="68"/>
+      <c r="L300" s="112" t="s">
+        <v>252</v>
+      </c>
+      <c r="M300" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N300" s="112" t="s">
+        <v>379</v>
+      </c>
       <c r="O300" s="9"/>
       <c r="P300" s="4"/>
       <c r="Q300" s="4"/>
@@ -16320,19 +16385,39 @@
     </row>
     <row r="301" spans="1:20" ht="18" customHeight="1">
       <c r="A301" s="64"/>
-      <c r="B301" s="73"/>
-      <c r="C301" s="4"/>
-      <c r="D301" s="4"/>
+      <c r="B301" s="111" t="s">
+        <v>377</v>
+      </c>
+      <c r="C301" s="118" t="s">
+        <v>124</v>
+      </c>
+      <c r="D301" s="118" t="s">
+        <v>113</v>
+      </c>
       <c r="E301" s="9"/>
-      <c r="F301" s="4"/>
-      <c r="G301" s="4"/>
+      <c r="F301" s="118" t="s">
+        <v>251</v>
+      </c>
+      <c r="G301" s="112" t="s">
+        <v>29</v>
+      </c>
       <c r="H301" s="4"/>
-      <c r="I301" s="83"/>
-      <c r="J301" s="70"/>
+      <c r="I301" s="83">
+        <v>298</v>
+      </c>
+      <c r="J301" s="70">
+        <v>5.7199999999999999E-7</v>
+      </c>
       <c r="K301" s="70"/>
-      <c r="L301" s="68"/>
-      <c r="M301" s="68"/>
-      <c r="N301" s="68"/>
+      <c r="L301" s="112" t="s">
+        <v>252</v>
+      </c>
+      <c r="M301" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="N301" s="112" t="s">
+        <v>379</v>
+      </c>
       <c r="O301" s="9"/>
       <c r="P301" s="4"/>
       <c r="Q301" s="4"/>
@@ -28596,11 +28681,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -28615,6 +28695,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.actamat.2023.118784`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C720FD39-0DD3-8A41-8CAC-3D15C7022D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1407F40-B186-EC4F-B923-87FFD3A840CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6080" windowWidth="34560" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4172" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4478" uniqueCount="653">
   <si>
     <r>
       <rPr>
@@ -2071,6 +2071,24 @@
   </si>
   <si>
     <t>10.20517/jmi.2022.03</t>
+  </si>
+  <si>
+    <t>Mo45 Nb35 Ta5 V15</t>
+  </si>
+  <si>
+    <t>Mo25 Nb50 V20 W5</t>
+  </si>
+  <si>
+    <t>Mo30 Nb35 Ta5 V25 W5</t>
+  </si>
+  <si>
+    <t>homogenized at 1925°C for 12h</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2023.118784</t>
   </si>
 </sst>
 </file>
@@ -3217,56 +3235,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3328,8 +3298,56 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4493,8 +4511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A442" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N489" sqref="N489"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A480" zoomScale="86" workbookViewId="0">
+      <selection activeCell="O513" sqref="O513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -4551,19 +4569,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="145" t="s">
+      <c r="D2" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="146"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
-      <c r="L2" s="150"/>
-      <c r="M2" s="150"/>
-      <c r="N2" s="153"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="137"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -4579,17 +4597,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="147"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="154"/>
-      <c r="M3" s="154"/>
-      <c r="N3" s="157"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="141"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -4630,43 +4648,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="142" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="160" t="s">
+      <c r="D5" s="144" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="160" t="s">
+      <c r="E5" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="160" t="s">
+      <c r="F5" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="160" t="s">
+      <c r="G5" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="161" t="s">
+      <c r="H5" s="145" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="160" t="s">
+      <c r="I5" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="160" t="s">
+      <c r="J5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="160" t="s">
+      <c r="K5" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="160" t="s">
+      <c r="L5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="160" t="s">
+      <c r="M5" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="160" t="s">
+      <c r="N5" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="128" t="s">
+      <c r="O5" s="149" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -4682,19 +4700,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="162"/>
-      <c r="I6" s="163"/>
-      <c r="J6" s="164"/>
-      <c r="K6" s="164"/>
-      <c r="L6" s="159"/>
-      <c r="M6" s="159"/>
-      <c r="N6" s="159"/>
-      <c r="O6" s="129"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="147"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="150"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -4744,7 +4762,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="130"/>
+      <c r="O7" s="151"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -4759,35 +4777,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="152" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="134" t="s">
+      <c r="C8" s="153"/>
+      <c r="D8" s="153"/>
+      <c r="E8" s="154"/>
+      <c r="F8" s="155" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="135"/>
-      <c r="H8" s="135"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="137"/>
-      <c r="K8" s="137"/>
-      <c r="L8" s="138"/>
-      <c r="M8" s="139" t="s">
+      <c r="G8" s="156"/>
+      <c r="H8" s="156"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="158"/>
+      <c r="L8" s="159"/>
+      <c r="M8" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="140"/>
+      <c r="N8" s="161"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="141" t="s">
+      <c r="P8" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="142"/>
-      <c r="R8" s="143"/>
-      <c r="S8" s="143"/>
-      <c r="T8" s="144"/>
+      <c r="Q8" s="163"/>
+      <c r="R8" s="164"/>
+      <c r="S8" s="164"/>
+      <c r="T8" s="165"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="38" t="s">
@@ -20829,7 +20847,7 @@
       <c r="D372" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E372" s="165" t="s">
+      <c r="E372" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F372" s="117" t="s">
@@ -20876,7 +20894,7 @@
       <c r="D373" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E373" s="165" t="s">
+      <c r="E373" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F373" s="117" t="s">
@@ -20923,7 +20941,7 @@
       <c r="D374" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E374" s="165" t="s">
+      <c r="E374" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F374" s="117" t="s">
@@ -20970,7 +20988,7 @@
       <c r="D375" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E375" s="165" t="s">
+      <c r="E375" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F375" s="117" t="s">
@@ -21017,7 +21035,7 @@
       <c r="D376" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E376" s="165" t="s">
+      <c r="E376" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F376" s="117" t="s">
@@ -21064,7 +21082,7 @@
       <c r="D377" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E377" s="165" t="s">
+      <c r="E377" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F377" s="117" t="s">
@@ -21111,7 +21129,7 @@
       <c r="D378" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E378" s="165" t="s">
+      <c r="E378" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F378" s="117" t="s">
@@ -21158,7 +21176,7 @@
       <c r="D379" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E379" s="165" t="s">
+      <c r="E379" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F379" s="117" t="s">
@@ -21205,7 +21223,7 @@
       <c r="D380" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E380" s="165" t="s">
+      <c r="E380" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F380" s="117" t="s">
@@ -21252,7 +21270,7 @@
       <c r="D381" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E381" s="165" t="s">
+      <c r="E381" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F381" s="117" t="s">
@@ -21299,7 +21317,7 @@
       <c r="D382" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E382" s="165" t="s">
+      <c r="E382" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F382" s="117" t="s">
@@ -21346,7 +21364,7 @@
       <c r="D383" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E383" s="165" t="s">
+      <c r="E383" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F383" s="117" t="s">
@@ -21393,7 +21411,7 @@
       <c r="D384" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E384" s="165" t="s">
+      <c r="E384" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F384" s="117" t="s">
@@ -21440,7 +21458,7 @@
       <c r="D385" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E385" s="165" t="s">
+      <c r="E385" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F385" s="117" t="s">
@@ -21487,7 +21505,7 @@
       <c r="D386" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E386" s="165" t="s">
+      <c r="E386" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F386" s="117" t="s">
@@ -21534,7 +21552,7 @@
       <c r="D387" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E387" s="165" t="s">
+      <c r="E387" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F387" s="117" t="s">
@@ -21581,7 +21599,7 @@
       <c r="D388" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E388" s="165" t="s">
+      <c r="E388" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F388" s="117" t="s">
@@ -21628,7 +21646,7 @@
       <c r="D389" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E389" s="165" t="s">
+      <c r="E389" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F389" s="117" t="s">
@@ -21675,7 +21693,7 @@
       <c r="D390" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E390" s="165" t="s">
+      <c r="E390" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F390" s="117" t="s">
@@ -21722,7 +21740,7 @@
       <c r="D391" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E391" s="165" t="s">
+      <c r="E391" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F391" s="117" t="s">
@@ -21769,7 +21787,7 @@
       <c r="D392" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E392" s="165" t="s">
+      <c r="E392" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F392" s="117" t="s">
@@ -21816,7 +21834,7 @@
       <c r="D393" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E393" s="165" t="s">
+      <c r="E393" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F393" s="117" t="s">
@@ -21863,7 +21881,7 @@
       <c r="D394" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E394" s="165" t="s">
+      <c r="E394" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F394" s="117" t="s">
@@ -21910,7 +21928,7 @@
       <c r="D395" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E395" s="165" t="s">
+      <c r="E395" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F395" s="117" t="s">
@@ -21957,7 +21975,7 @@
       <c r="D396" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E396" s="165" t="s">
+      <c r="E396" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F396" s="117" t="s">
@@ -22004,7 +22022,7 @@
       <c r="D397" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E397" s="165" t="s">
+      <c r="E397" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F397" s="117" t="s">
@@ -22051,7 +22069,7 @@
       <c r="D398" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E398" s="165" t="s">
+      <c r="E398" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F398" s="117" t="s">
@@ -22098,7 +22116,7 @@
       <c r="D399" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E399" s="165" t="s">
+      <c r="E399" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F399" s="117" t="s">
@@ -22145,7 +22163,7 @@
       <c r="D400" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E400" s="165" t="s">
+      <c r="E400" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F400" s="117" t="s">
@@ -22192,7 +22210,7 @@
       <c r="D401" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E401" s="165" t="s">
+      <c r="E401" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F401" s="117" t="s">
@@ -22239,7 +22257,7 @@
       <c r="D402" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E402" s="165" t="s">
+      <c r="E402" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F402" s="117" t="s">
@@ -22286,7 +22304,7 @@
       <c r="D403" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E403" s="165" t="s">
+      <c r="E403" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F403" s="117" t="s">
@@ -22333,7 +22351,7 @@
       <c r="D404" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E404" s="165" t="s">
+      <c r="E404" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F404" s="117" t="s">
@@ -22380,7 +22398,7 @@
       <c r="D405" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E405" s="165" t="s">
+      <c r="E405" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F405" s="117" t="s">
@@ -22427,7 +22445,7 @@
       <c r="D406" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E406" s="165" t="s">
+      <c r="E406" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F406" s="117" t="s">
@@ -22474,7 +22492,7 @@
       <c r="D407" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E407" s="165" t="s">
+      <c r="E407" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F407" s="117" t="s">
@@ -22521,7 +22539,7 @@
       <c r="D408" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E408" s="165" t="s">
+      <c r="E408" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F408" s="117" t="s">
@@ -22568,7 +22586,7 @@
       <c r="D409" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E409" s="165" t="s">
+      <c r="E409" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F409" s="117" t="s">
@@ -22615,7 +22633,7 @@
       <c r="D410" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E410" s="165" t="s">
+      <c r="E410" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F410" s="117" t="s">
@@ -22662,7 +22680,7 @@
       <c r="D411" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E411" s="165" t="s">
+      <c r="E411" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F411" s="117" t="s">
@@ -22709,7 +22727,7 @@
       <c r="D412" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E412" s="165" t="s">
+      <c r="E412" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F412" s="117" t="s">
@@ -22756,7 +22774,7 @@
       <c r="D413" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E413" s="165" t="s">
+      <c r="E413" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F413" s="117" t="s">
@@ -22803,7 +22821,7 @@
       <c r="D414" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E414" s="165" t="s">
+      <c r="E414" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F414" s="117" t="s">
@@ -22850,7 +22868,7 @@
       <c r="D415" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E415" s="165" t="s">
+      <c r="E415" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F415" s="117" t="s">
@@ -22897,7 +22915,7 @@
       <c r="D416" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E416" s="165" t="s">
+      <c r="E416" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F416" s="117" t="s">
@@ -22944,7 +22962,7 @@
       <c r="D417" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E417" s="165" t="s">
+      <c r="E417" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F417" s="117" t="s">
@@ -22991,7 +23009,7 @@
       <c r="D418" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E418" s="165" t="s">
+      <c r="E418" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F418" s="117" t="s">
@@ -23038,7 +23056,7 @@
       <c r="D419" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E419" s="165" t="s">
+      <c r="E419" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F419" s="117" t="s">
@@ -23085,7 +23103,7 @@
       <c r="D420" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E420" s="165" t="s">
+      <c r="E420" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F420" s="117" t="s">
@@ -23132,7 +23150,7 @@
       <c r="D421" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E421" s="165" t="s">
+      <c r="E421" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F421" s="117" t="s">
@@ -23179,7 +23197,7 @@
       <c r="D422" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E422" s="165" t="s">
+      <c r="E422" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F422" s="117" t="s">
@@ -23226,7 +23244,7 @@
       <c r="D423" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E423" s="165" t="s">
+      <c r="E423" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F423" s="117" t="s">
@@ -23273,7 +23291,7 @@
       <c r="D424" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E424" s="165" t="s">
+      <c r="E424" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F424" s="117" t="s">
@@ -23320,7 +23338,7 @@
       <c r="D425" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E425" s="165" t="s">
+      <c r="E425" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F425" s="117" t="s">
@@ -23367,7 +23385,7 @@
       <c r="D426" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E426" s="165" t="s">
+      <c r="E426" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F426" s="117" t="s">
@@ -23414,7 +23432,7 @@
       <c r="D427" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E427" s="165" t="s">
+      <c r="E427" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F427" s="117" t="s">
@@ -23461,7 +23479,7 @@
       <c r="D428" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E428" s="165" t="s">
+      <c r="E428" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F428" s="117" t="s">
@@ -23508,7 +23526,7 @@
       <c r="D429" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E429" s="165" t="s">
+      <c r="E429" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F429" s="117" t="s">
@@ -23555,7 +23573,7 @@
       <c r="D430" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E430" s="165" t="s">
+      <c r="E430" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F430" s="117" t="s">
@@ -23602,7 +23620,7 @@
       <c r="D431" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E431" s="165" t="s">
+      <c r="E431" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F431" s="117" t="s">
@@ -23649,7 +23667,7 @@
       <c r="D432" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E432" s="165" t="s">
+      <c r="E432" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F432" s="117" t="s">
@@ -23696,7 +23714,7 @@
       <c r="D433" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E433" s="165" t="s">
+      <c r="E433" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F433" s="117" t="s">
@@ -23743,7 +23761,7 @@
       <c r="D434" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E434" s="165" t="s">
+      <c r="E434" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F434" s="117" t="s">
@@ -23790,7 +23808,7 @@
       <c r="D435" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E435" s="165" t="s">
+      <c r="E435" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F435" s="117" t="s">
@@ -23837,7 +23855,7 @@
       <c r="D436" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E436" s="165" t="s">
+      <c r="E436" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F436" s="117" t="s">
@@ -23884,7 +23902,7 @@
       <c r="D437" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E437" s="165" t="s">
+      <c r="E437" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F437" s="117" t="s">
@@ -23931,7 +23949,7 @@
       <c r="D438" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E438" s="165" t="s">
+      <c r="E438" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F438" s="117" t="s">
@@ -23978,7 +23996,7 @@
       <c r="D439" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E439" s="165" t="s">
+      <c r="E439" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F439" s="117" t="s">
@@ -24025,7 +24043,7 @@
       <c r="D440" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E440" s="165" t="s">
+      <c r="E440" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F440" s="117" t="s">
@@ -24072,7 +24090,7 @@
       <c r="D441" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E441" s="165" t="s">
+      <c r="E441" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F441" s="117" t="s">
@@ -24119,7 +24137,7 @@
       <c r="D442" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E442" s="165" t="s">
+      <c r="E442" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F442" s="117" t="s">
@@ -24166,7 +24184,7 @@
       <c r="D443" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E443" s="165" t="s">
+      <c r="E443" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F443" s="117" t="s">
@@ -24213,7 +24231,7 @@
       <c r="D444" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E444" s="165" t="s">
+      <c r="E444" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F444" s="117" t="s">
@@ -24260,7 +24278,7 @@
       <c r="D445" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E445" s="165" t="s">
+      <c r="E445" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F445" s="117" t="s">
@@ -24307,7 +24325,7 @@
       <c r="D446" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E446" s="165" t="s">
+      <c r="E446" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F446" s="117" t="s">
@@ -24354,7 +24372,7 @@
       <c r="D447" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E447" s="165" t="s">
+      <c r="E447" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F447" s="117" t="s">
@@ -24401,7 +24419,7 @@
       <c r="D448" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E448" s="165" t="s">
+      <c r="E448" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F448" s="117" t="s">
@@ -24448,7 +24466,7 @@
       <c r="D449" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E449" s="165" t="s">
+      <c r="E449" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F449" s="117" t="s">
@@ -24495,7 +24513,7 @@
       <c r="D450" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E450" s="165" t="s">
+      <c r="E450" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F450" s="117" t="s">
@@ -24542,7 +24560,7 @@
       <c r="D451" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E451" s="165" t="s">
+      <c r="E451" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F451" s="117" t="s">
@@ -24589,7 +24607,7 @@
       <c r="D452" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E452" s="165" t="s">
+      <c r="E452" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F452" s="117" t="s">
@@ -24636,7 +24654,7 @@
       <c r="D453" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E453" s="165" t="s">
+      <c r="E453" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F453" s="117" t="s">
@@ -24683,7 +24701,7 @@
       <c r="D454" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E454" s="165" t="s">
+      <c r="E454" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F454" s="117" t="s">
@@ -24730,7 +24748,7 @@
       <c r="D455" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E455" s="165" t="s">
+      <c r="E455" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F455" s="117" t="s">
@@ -24777,7 +24795,7 @@
       <c r="D456" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E456" s="165" t="s">
+      <c r="E456" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F456" s="117" t="s">
@@ -24824,7 +24842,7 @@
       <c r="D457" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E457" s="165" t="s">
+      <c r="E457" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F457" s="117" t="s">
@@ -24871,7 +24889,7 @@
       <c r="D458" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E458" s="165" t="s">
+      <c r="E458" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F458" s="117" t="s">
@@ -24918,7 +24936,7 @@
       <c r="D459" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E459" s="165" t="s">
+      <c r="E459" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F459" s="117" t="s">
@@ -24965,7 +24983,7 @@
       <c r="D460" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E460" s="165" t="s">
+      <c r="E460" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F460" s="117" t="s">
@@ -25012,7 +25030,7 @@
       <c r="D461" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E461" s="165" t="s">
+      <c r="E461" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F461" s="117" t="s">
@@ -25059,7 +25077,7 @@
       <c r="D462" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E462" s="165" t="s">
+      <c r="E462" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F462" s="117" t="s">
@@ -25106,7 +25124,7 @@
       <c r="D463" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E463" s="165" t="s">
+      <c r="E463" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F463" s="117" t="s">
@@ -25153,7 +25171,7 @@
       <c r="D464" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E464" s="165" t="s">
+      <c r="E464" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F464" s="117" t="s">
@@ -25200,7 +25218,7 @@
       <c r="D465" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E465" s="165" t="s">
+      <c r="E465" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F465" s="117" t="s">
@@ -25247,7 +25265,7 @@
       <c r="D466" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E466" s="165" t="s">
+      <c r="E466" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F466" s="117" t="s">
@@ -25294,7 +25312,7 @@
       <c r="D467" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E467" s="165" t="s">
+      <c r="E467" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F467" s="117" t="s">
@@ -25341,7 +25359,7 @@
       <c r="D468" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E468" s="165" t="s">
+      <c r="E468" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F468" s="117" t="s">
@@ -25388,7 +25406,7 @@
       <c r="D469" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E469" s="165" t="s">
+      <c r="E469" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F469" s="117" t="s">
@@ -25435,7 +25453,7 @@
       <c r="D470" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E470" s="165" t="s">
+      <c r="E470" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F470" s="117" t="s">
@@ -25482,7 +25500,7 @@
       <c r="D471" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E471" s="165" t="s">
+      <c r="E471" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F471" s="117" t="s">
@@ -25529,7 +25547,7 @@
       <c r="D472" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E472" s="165" t="s">
+      <c r="E472" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F472" s="117" t="s">
@@ -25576,7 +25594,7 @@
       <c r="D473" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E473" s="165" t="s">
+      <c r="E473" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F473" s="117" t="s">
@@ -25623,7 +25641,7 @@
       <c r="D474" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E474" s="165" t="s">
+      <c r="E474" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F474" s="117" t="s">
@@ -25670,7 +25688,7 @@
       <c r="D475" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E475" s="165" t="s">
+      <c r="E475" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F475" s="117" t="s">
@@ -25717,7 +25735,7 @@
       <c r="D476" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E476" s="165" t="s">
+      <c r="E476" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F476" s="117" t="s">
@@ -25764,7 +25782,7 @@
       <c r="D477" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E477" s="165" t="s">
+      <c r="E477" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F477" s="117" t="s">
@@ -25811,7 +25829,7 @@
       <c r="D478" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E478" s="165" t="s">
+      <c r="E478" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F478" s="117" t="s">
@@ -25858,7 +25876,7 @@
       <c r="D479" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E479" s="165" t="s">
+      <c r="E479" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F479" s="117" t="s">
@@ -25905,7 +25923,7 @@
       <c r="D480" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E480" s="165" t="s">
+      <c r="E480" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F480" s="117" t="s">
@@ -25952,7 +25970,7 @@
       <c r="D481" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E481" s="165" t="s">
+      <c r="E481" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F481" s="117" t="s">
@@ -25999,7 +26017,7 @@
       <c r="D482" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="E482" s="165" t="s">
+      <c r="E482" s="128" t="s">
         <v>645</v>
       </c>
       <c r="F482" s="117" t="s">
@@ -26037,19 +26055,41 @@
     </row>
     <row r="483" spans="1:20" ht="15" customHeight="1">
       <c r="A483" s="4"/>
-      <c r="B483" s="73"/>
-      <c r="C483" s="4"/>
-      <c r="D483" s="4"/>
+      <c r="B483" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C483" s="117" t="s">
+        <v>305</v>
+      </c>
+      <c r="D483" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E483" s="9"/>
-      <c r="F483" s="4"/>
-      <c r="G483" s="4"/>
+      <c r="F483" s="117" t="s">
+        <v>90</v>
+      </c>
+      <c r="G483" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H483" s="4"/>
-      <c r="I483" s="4"/>
-      <c r="J483" s="4"/>
-      <c r="K483" s="4"/>
-      <c r="L483" s="4"/>
-      <c r="M483" s="4"/>
-      <c r="N483" s="4"/>
+      <c r="I483" s="4">
+        <v>298</v>
+      </c>
+      <c r="J483" s="106">
+        <v>6860000000</v>
+      </c>
+      <c r="K483" s="106">
+        <v>220000000</v>
+      </c>
+      <c r="L483" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M483" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N483" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O483" s="9"/>
       <c r="P483" s="4"/>
       <c r="Q483" s="4"/>
@@ -26059,19 +26099,41 @@
     </row>
     <row r="484" spans="1:20" ht="15" customHeight="1">
       <c r="A484" s="4"/>
-      <c r="B484" s="73"/>
-      <c r="C484" s="4"/>
-      <c r="D484" s="4"/>
+      <c r="B484" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C484" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D484" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E484" s="9"/>
-      <c r="F484" s="4"/>
-      <c r="G484" s="4"/>
+      <c r="F484" s="117" t="s">
+        <v>90</v>
+      </c>
+      <c r="G484" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H484" s="4"/>
-      <c r="I484" s="4"/>
-      <c r="J484" s="4"/>
-      <c r="K484" s="4"/>
-      <c r="L484" s="4"/>
-      <c r="M484" s="4"/>
-      <c r="N484" s="4"/>
+      <c r="I484" s="4">
+        <v>298</v>
+      </c>
+      <c r="J484" s="106">
+        <v>6850000000</v>
+      </c>
+      <c r="K484" s="106">
+        <v>90000000</v>
+      </c>
+      <c r="L484" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M484" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N484" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O484" s="9"/>
       <c r="P484" s="4"/>
       <c r="Q484" s="4"/>
@@ -26081,19 +26143,41 @@
     </row>
     <row r="485" spans="1:20" ht="15" customHeight="1">
       <c r="A485" s="4"/>
-      <c r="B485" s="73"/>
-      <c r="C485" s="4"/>
-      <c r="D485" s="4"/>
+      <c r="B485" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C485" s="117" t="s">
+        <v>305</v>
+      </c>
+      <c r="D485" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E485" s="9"/>
-      <c r="F485" s="4"/>
-      <c r="G485" s="4"/>
+      <c r="F485" s="117" t="s">
+        <v>90</v>
+      </c>
+      <c r="G485" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H485" s="4"/>
-      <c r="I485" s="4"/>
-      <c r="J485" s="4"/>
-      <c r="K485" s="4"/>
-      <c r="L485" s="4"/>
-      <c r="M485" s="4"/>
-      <c r="N485" s="4"/>
+      <c r="I485" s="4">
+        <v>298</v>
+      </c>
+      <c r="J485" s="106">
+        <v>7200000000</v>
+      </c>
+      <c r="K485" s="106">
+        <v>140000000</v>
+      </c>
+      <c r="L485" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M485" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N485" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O485" s="9"/>
       <c r="P485" s="4"/>
       <c r="Q485" s="4"/>
@@ -26103,19 +26187,41 @@
     </row>
     <row r="486" spans="1:20" ht="15" customHeight="1">
       <c r="A486" s="4"/>
-      <c r="B486" s="73"/>
-      <c r="C486" s="4"/>
-      <c r="D486" s="4"/>
+      <c r="B486" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C486" s="117" t="s">
+        <v>305</v>
+      </c>
+      <c r="D486" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E486" s="9"/>
-      <c r="F486" s="4"/>
-      <c r="G486" s="4"/>
+      <c r="F486" s="117" t="s">
+        <v>91</v>
+      </c>
+      <c r="G486" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H486" s="4"/>
-      <c r="I486" s="4"/>
-      <c r="J486" s="4"/>
-      <c r="K486" s="4"/>
-      <c r="L486" s="4"/>
-      <c r="M486" s="4"/>
-      <c r="N486" s="4"/>
+      <c r="I486" s="4">
+        <v>298</v>
+      </c>
+      <c r="J486" s="106">
+        <v>178000000000</v>
+      </c>
+      <c r="K486" s="106">
+        <v>6000000000</v>
+      </c>
+      <c r="L486" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M486" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N486" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O486" s="9"/>
       <c r="P486" s="4"/>
       <c r="Q486" s="4"/>
@@ -26125,19 +26231,41 @@
     </row>
     <row r="487" spans="1:20" ht="15" customHeight="1">
       <c r="A487" s="4"/>
-      <c r="B487" s="73"/>
-      <c r="C487" s="4"/>
-      <c r="D487" s="4"/>
+      <c r="B487" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C487" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D487" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E487" s="9"/>
-      <c r="F487" s="4"/>
-      <c r="G487" s="4"/>
+      <c r="F487" s="117" t="s">
+        <v>91</v>
+      </c>
+      <c r="G487" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H487" s="4"/>
-      <c r="I487" s="4"/>
-      <c r="J487" s="4"/>
-      <c r="K487" s="4"/>
-      <c r="L487" s="4"/>
-      <c r="M487" s="4"/>
-      <c r="N487" s="4"/>
+      <c r="I487" s="4">
+        <v>298</v>
+      </c>
+      <c r="J487" s="106">
+        <v>136000000000</v>
+      </c>
+      <c r="K487" s="106">
+        <v>3000000000</v>
+      </c>
+      <c r="L487" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M487" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N487" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O487" s="9"/>
       <c r="P487" s="4"/>
       <c r="Q487" s="4"/>
@@ -26147,19 +26275,41 @@
     </row>
     <row r="488" spans="1:20" ht="15" customHeight="1">
       <c r="A488" s="4"/>
-      <c r="B488" s="73"/>
-      <c r="C488" s="4"/>
-      <c r="D488" s="4"/>
+      <c r="B488" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C488" s="117" t="s">
+        <v>305</v>
+      </c>
+      <c r="D488" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E488" s="9"/>
-      <c r="F488" s="4"/>
-      <c r="G488" s="4"/>
+      <c r="F488" s="117" t="s">
+        <v>91</v>
+      </c>
+      <c r="G488" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H488" s="4"/>
-      <c r="I488" s="4"/>
-      <c r="J488" s="4"/>
-      <c r="K488" s="4"/>
-      <c r="L488" s="4"/>
-      <c r="M488" s="4"/>
-      <c r="N488" s="4"/>
+      <c r="I488" s="4">
+        <v>298</v>
+      </c>
+      <c r="J488" s="106">
+        <v>158000000000</v>
+      </c>
+      <c r="K488" s="106">
+        <v>4000000000</v>
+      </c>
+      <c r="L488" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M488" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N488" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O488" s="9"/>
       <c r="P488" s="4"/>
       <c r="Q488" s="4"/>
@@ -26169,85 +26319,191 @@
     </row>
     <row r="489" spans="1:20" ht="15" customHeight="1">
       <c r="A489" s="4"/>
-      <c r="B489" s="73"/>
-      <c r="C489" s="4"/>
-      <c r="D489" s="4"/>
-      <c r="E489" s="9"/>
-      <c r="F489" s="4"/>
-      <c r="G489" s="4"/>
+      <c r="B489" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C489" s="117" t="s">
+        <v>305</v>
+      </c>
+      <c r="D489" s="117" t="s">
+        <v>113</v>
+      </c>
+      <c r="E489" s="119"/>
+      <c r="F489" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G489" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H489" s="4"/>
-      <c r="I489" s="4"/>
-      <c r="J489" s="4"/>
-      <c r="K489" s="4"/>
-      <c r="L489" s="4"/>
-      <c r="M489" s="4"/>
-      <c r="N489" s="4"/>
+      <c r="I489" s="4">
+        <v>298</v>
+      </c>
+      <c r="J489" s="70">
+        <f t="shared" ref="J489:K491" si="12">P489*9807000</f>
+        <v>4932921000</v>
+      </c>
+      <c r="K489" s="70">
+        <f t="shared" si="12"/>
+        <v>88263000</v>
+      </c>
+      <c r="L489" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M489" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N489" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O489" s="9"/>
-      <c r="P489" s="4"/>
-      <c r="Q489" s="4"/>
+      <c r="P489" s="4">
+        <v>503</v>
+      </c>
+      <c r="Q489" s="4">
+        <v>9</v>
+      </c>
       <c r="R489" s="9"/>
       <c r="S489" s="9"/>
       <c r="T489" s="9"/>
     </row>
     <row r="490" spans="1:20" ht="15" customHeight="1">
       <c r="A490" s="4"/>
-      <c r="B490" s="73"/>
-      <c r="C490" s="4"/>
-      <c r="D490" s="4"/>
+      <c r="B490" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C490" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D490" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E490" s="9"/>
-      <c r="F490" s="4"/>
-      <c r="G490" s="4"/>
+      <c r="F490" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G490" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H490" s="4"/>
-      <c r="I490" s="4"/>
-      <c r="J490" s="4"/>
-      <c r="K490" s="4"/>
-      <c r="L490" s="4"/>
-      <c r="M490" s="4"/>
-      <c r="N490" s="4"/>
+      <c r="I490" s="4">
+        <v>298</v>
+      </c>
+      <c r="J490" s="70">
+        <f t="shared" si="12"/>
+        <v>4874079000</v>
+      </c>
+      <c r="K490" s="70">
+        <f t="shared" si="12"/>
+        <v>68649000</v>
+      </c>
+      <c r="L490" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M490" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N490" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O490" s="9"/>
-      <c r="P490" s="4"/>
-      <c r="Q490" s="4"/>
+      <c r="P490" s="4">
+        <v>497</v>
+      </c>
+      <c r="Q490" s="4">
+        <v>7</v>
+      </c>
       <c r="R490" s="9"/>
       <c r="S490" s="9"/>
       <c r="T490" s="9"/>
     </row>
     <row r="491" spans="1:20" ht="15" customHeight="1">
       <c r="A491" s="4"/>
-      <c r="B491" s="73"/>
-      <c r="C491" s="4"/>
-      <c r="D491" s="4"/>
+      <c r="B491" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C491" s="117" t="s">
+        <v>305</v>
+      </c>
+      <c r="D491" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E491" s="9"/>
-      <c r="F491" s="4"/>
-      <c r="G491" s="4"/>
+      <c r="F491" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G491" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H491" s="4"/>
-      <c r="I491" s="4"/>
-      <c r="J491" s="4"/>
-      <c r="K491" s="4"/>
-      <c r="L491" s="4"/>
-      <c r="M491" s="4"/>
-      <c r="N491" s="4"/>
+      <c r="I491" s="4">
+        <v>298</v>
+      </c>
+      <c r="J491" s="70">
+        <f t="shared" si="12"/>
+        <v>5099640000</v>
+      </c>
+      <c r="K491" s="70">
+        <f t="shared" si="12"/>
+        <v>78456000</v>
+      </c>
+      <c r="L491" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M491" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N491" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O491" s="9"/>
-      <c r="P491" s="4"/>
-      <c r="Q491" s="4"/>
+      <c r="P491" s="4">
+        <v>520</v>
+      </c>
+      <c r="Q491" s="4">
+        <v>8</v>
+      </c>
       <c r="R491" s="9"/>
       <c r="S491" s="9"/>
       <c r="T491" s="9"/>
     </row>
     <row r="492" spans="1:20" ht="15" customHeight="1">
       <c r="A492" s="4"/>
-      <c r="B492" s="73"/>
-      <c r="C492" s="4"/>
-      <c r="D492" s="4"/>
-      <c r="E492" s="9"/>
-      <c r="F492" s="4"/>
-      <c r="G492" s="4"/>
+      <c r="B492" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C492" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D492" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E492" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F492" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="G492" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H492" s="4"/>
-      <c r="I492" s="4"/>
-      <c r="J492" s="4"/>
+      <c r="I492" s="4">
+        <v>298</v>
+      </c>
+      <c r="J492" s="4">
+        <v>9411</v>
+      </c>
       <c r="K492" s="4"/>
-      <c r="L492" s="4"/>
-      <c r="M492" s="4"/>
-      <c r="N492" s="4"/>
+      <c r="L492" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="M492" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N492" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O492" s="9"/>
       <c r="P492" s="4"/>
       <c r="Q492" s="4"/>
@@ -26257,19 +26513,41 @@
     </row>
     <row r="493" spans="1:20" ht="15" customHeight="1">
       <c r="A493" s="4"/>
-      <c r="B493" s="73"/>
-      <c r="C493" s="4"/>
-      <c r="D493" s="4"/>
-      <c r="E493" s="9"/>
-      <c r="F493" s="4"/>
-      <c r="G493" s="4"/>
+      <c r="B493" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C493" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D493" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E493" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F493" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="G493" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H493" s="4"/>
-      <c r="I493" s="4"/>
-      <c r="J493" s="4"/>
+      <c r="I493" s="4">
+        <v>298</v>
+      </c>
+      <c r="J493" s="4">
+        <v>9085</v>
+      </c>
       <c r="K493" s="4"/>
-      <c r="L493" s="4"/>
-      <c r="M493" s="4"/>
-      <c r="N493" s="4"/>
+      <c r="L493" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="M493" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N493" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O493" s="9"/>
       <c r="P493" s="4"/>
       <c r="Q493" s="4"/>
@@ -26279,19 +26557,41 @@
     </row>
     <row r="494" spans="1:20" ht="15" customHeight="1">
       <c r="A494" s="4"/>
-      <c r="B494" s="73"/>
-      <c r="C494" s="4"/>
-      <c r="D494" s="4"/>
-      <c r="E494" s="9"/>
-      <c r="F494" s="4"/>
-      <c r="G494" s="4"/>
+      <c r="B494" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C494" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D494" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E494" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F494" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="G494" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H494" s="4"/>
-      <c r="I494" s="4"/>
-      <c r="J494" s="4"/>
+      <c r="I494" s="4">
+        <v>298</v>
+      </c>
+      <c r="J494" s="4">
+        <v>9441</v>
+      </c>
       <c r="K494" s="4"/>
-      <c r="L494" s="4"/>
-      <c r="M494" s="4"/>
-      <c r="N494" s="4"/>
+      <c r="L494" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="M494" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N494" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O494" s="9"/>
       <c r="P494" s="4"/>
       <c r="Q494" s="4"/>
@@ -26301,85 +26601,199 @@
     </row>
     <row r="495" spans="1:20" ht="15" customHeight="1">
       <c r="A495" s="4"/>
-      <c r="B495" s="73"/>
-      <c r="C495" s="4"/>
-      <c r="D495" s="4"/>
-      <c r="E495" s="9"/>
-      <c r="F495" s="4"/>
-      <c r="G495" s="4"/>
+      <c r="B495" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C495" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D495" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E495" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F495" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G495" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H495" s="4"/>
-      <c r="I495" s="4"/>
-      <c r="J495" s="4"/>
-      <c r="K495" s="4"/>
-      <c r="L495" s="4"/>
-      <c r="M495" s="4"/>
-      <c r="N495" s="4"/>
+      <c r="I495" s="4">
+        <v>298</v>
+      </c>
+      <c r="J495" s="70">
+        <f t="shared" ref="J495:K497" si="13">P495*9807000</f>
+        <v>4599483000</v>
+      </c>
+      <c r="K495" s="70">
+        <f t="shared" si="13"/>
+        <v>137298000</v>
+      </c>
+      <c r="L495" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M495" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N495" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O495" s="9"/>
-      <c r="P495" s="4"/>
-      <c r="Q495" s="4"/>
+      <c r="P495" s="4">
+        <v>469</v>
+      </c>
+      <c r="Q495" s="4">
+        <v>14</v>
+      </c>
       <c r="R495" s="9"/>
       <c r="S495" s="9"/>
       <c r="T495" s="9"/>
     </row>
     <row r="496" spans="1:20" ht="15" customHeight="1">
       <c r="A496" s="4"/>
-      <c r="B496" s="73"/>
-      <c r="C496" s="4"/>
-      <c r="D496" s="4"/>
-      <c r="E496" s="9"/>
-      <c r="F496" s="4"/>
-      <c r="G496" s="4"/>
+      <c r="B496" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C496" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D496" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E496" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F496" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G496" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H496" s="4"/>
-      <c r="I496" s="4"/>
-      <c r="J496" s="4"/>
-      <c r="K496" s="4"/>
-      <c r="L496" s="4"/>
-      <c r="M496" s="4"/>
-      <c r="N496" s="4"/>
+      <c r="I496" s="4">
+        <v>298</v>
+      </c>
+      <c r="J496" s="70">
+        <f t="shared" si="13"/>
+        <v>4677939000</v>
+      </c>
+      <c r="K496" s="70">
+        <f t="shared" si="13"/>
+        <v>88263000</v>
+      </c>
+      <c r="L496" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M496" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N496" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O496" s="9"/>
-      <c r="P496" s="4"/>
-      <c r="Q496" s="4"/>
+      <c r="P496" s="4">
+        <v>477</v>
+      </c>
+      <c r="Q496" s="4">
+        <v>9</v>
+      </c>
       <c r="R496" s="9"/>
       <c r="S496" s="9"/>
       <c r="T496" s="9"/>
     </row>
     <row r="497" spans="1:20" ht="15" customHeight="1">
       <c r="A497" s="4"/>
-      <c r="B497" s="73"/>
-      <c r="C497" s="4"/>
-      <c r="D497" s="4"/>
-      <c r="E497" s="9"/>
-      <c r="F497" s="4"/>
-      <c r="G497" s="4"/>
+      <c r="B497" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C497" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D497" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E497" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F497" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G497" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H497" s="4"/>
-      <c r="I497" s="4"/>
-      <c r="J497" s="4"/>
-      <c r="K497" s="4"/>
-      <c r="L497" s="4"/>
-      <c r="M497" s="4"/>
-      <c r="N497" s="4"/>
+      <c r="I497" s="4">
+        <v>298</v>
+      </c>
+      <c r="J497" s="70">
+        <f t="shared" si="13"/>
+        <v>4707360000</v>
+      </c>
+      <c r="K497" s="70">
+        <f t="shared" si="13"/>
+        <v>156912000</v>
+      </c>
+      <c r="L497" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M497" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N497" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O497" s="9"/>
-      <c r="P497" s="4"/>
-      <c r="Q497" s="4"/>
+      <c r="P497" s="4">
+        <v>480</v>
+      </c>
+      <c r="Q497" s="4">
+        <v>16</v>
+      </c>
       <c r="R497" s="9"/>
       <c r="S497" s="9"/>
       <c r="T497" s="9"/>
     </row>
     <row r="498" spans="1:20" ht="15" customHeight="1">
       <c r="A498" s="4"/>
-      <c r="B498" s="73"/>
-      <c r="C498" s="4"/>
-      <c r="D498" s="4"/>
-      <c r="E498" s="9"/>
-      <c r="F498" s="4"/>
-      <c r="G498" s="4"/>
-      <c r="H498" s="4"/>
-      <c r="I498" s="4"/>
-      <c r="J498" s="4"/>
+      <c r="B498" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C498" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D498" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E498" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F498" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G498" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H498" s="117" t="s">
+        <v>192</v>
+      </c>
+      <c r="I498" s="4">
+        <v>298</v>
+      </c>
+      <c r="J498" s="106">
+        <v>752000000</v>
+      </c>
       <c r="K498" s="4"/>
-      <c r="L498" s="4"/>
-      <c r="M498" s="4"/>
-      <c r="N498" s="4"/>
+      <c r="L498" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M498" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N498" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O498" s="9"/>
       <c r="P498" s="4"/>
       <c r="Q498" s="4"/>
@@ -26389,19 +26803,43 @@
     </row>
     <row r="499" spans="1:20" ht="15" customHeight="1">
       <c r="A499" s="4"/>
-      <c r="B499" s="73"/>
-      <c r="C499" s="4"/>
-      <c r="D499" s="4"/>
-      <c r="E499" s="9"/>
-      <c r="F499" s="4"/>
-      <c r="G499" s="4"/>
-      <c r="H499" s="4"/>
-      <c r="I499" s="4"/>
-      <c r="J499" s="4"/>
+      <c r="B499" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C499" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D499" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E499" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F499" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G499" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H499" s="117" t="s">
+        <v>192</v>
+      </c>
+      <c r="I499" s="4">
+        <v>298</v>
+      </c>
+      <c r="J499" s="106">
+        <v>974000000</v>
+      </c>
       <c r="K499" s="4"/>
-      <c r="L499" s="4"/>
-      <c r="M499" s="4"/>
-      <c r="N499" s="4"/>
+      <c r="L499" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M499" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N499" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O499" s="9"/>
       <c r="P499" s="4"/>
       <c r="Q499" s="4"/>
@@ -26411,19 +26849,43 @@
     </row>
     <row r="500" spans="1:20" ht="15" customHeight="1">
       <c r="A500" s="4"/>
-      <c r="B500" s="73"/>
-      <c r="C500" s="4"/>
-      <c r="D500" s="4"/>
-      <c r="E500" s="9"/>
-      <c r="F500" s="4"/>
-      <c r="G500" s="4"/>
-      <c r="H500" s="4"/>
-      <c r="I500" s="4"/>
-      <c r="J500" s="4"/>
+      <c r="B500" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C500" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D500" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E500" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F500" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G500" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H500" s="117" t="s">
+        <v>192</v>
+      </c>
+      <c r="I500" s="4">
+        <v>298</v>
+      </c>
+      <c r="J500" s="106">
+        <v>1053000000</v>
+      </c>
       <c r="K500" s="4"/>
-      <c r="L500" s="4"/>
-      <c r="M500" s="4"/>
-      <c r="N500" s="4"/>
+      <c r="L500" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M500" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N500" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O500" s="9"/>
       <c r="P500" s="4"/>
       <c r="Q500" s="4"/>
@@ -26433,19 +26895,43 @@
     </row>
     <row r="501" spans="1:20" ht="15" customHeight="1">
       <c r="A501" s="4"/>
-      <c r="B501" s="73"/>
-      <c r="C501" s="4"/>
-      <c r="D501" s="4"/>
-      <c r="E501" s="9"/>
-      <c r="F501" s="4"/>
-      <c r="G501" s="4"/>
-      <c r="H501" s="4"/>
-      <c r="I501" s="4"/>
-      <c r="J501" s="4"/>
+      <c r="B501" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C501" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D501" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E501" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F501" s="117" t="s">
+        <v>189</v>
+      </c>
+      <c r="G501" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H501" s="117" t="s">
+        <v>192</v>
+      </c>
+      <c r="I501" s="4">
+        <v>298</v>
+      </c>
+      <c r="J501" s="106">
+        <v>852000000</v>
+      </c>
       <c r="K501" s="4"/>
-      <c r="L501" s="4"/>
-      <c r="M501" s="4"/>
-      <c r="N501" s="4"/>
+      <c r="L501" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M501" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N501" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O501" s="9"/>
       <c r="P501" s="4"/>
       <c r="Q501" s="4"/>
@@ -26455,19 +26941,43 @@
     </row>
     <row r="502" spans="1:20" ht="15" customHeight="1">
       <c r="A502" s="4"/>
-      <c r="B502" s="73"/>
-      <c r="C502" s="4"/>
-      <c r="D502" s="4"/>
-      <c r="E502" s="9"/>
-      <c r="F502" s="4"/>
-      <c r="G502" s="4"/>
-      <c r="H502" s="4"/>
-      <c r="I502" s="4"/>
-      <c r="J502" s="4"/>
+      <c r="B502" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C502" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D502" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E502" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F502" s="117" t="s">
+        <v>189</v>
+      </c>
+      <c r="G502" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H502" s="117" t="s">
+        <v>192</v>
+      </c>
+      <c r="I502" s="4">
+        <v>298</v>
+      </c>
+      <c r="J502" s="106">
+        <v>1210000000</v>
+      </c>
       <c r="K502" s="4"/>
-      <c r="L502" s="4"/>
-      <c r="M502" s="4"/>
-      <c r="N502" s="4"/>
+      <c r="L502" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M502" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N502" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O502" s="9"/>
       <c r="P502" s="4"/>
       <c r="Q502" s="4"/>
@@ -26477,19 +26987,43 @@
     </row>
     <row r="503" spans="1:20" ht="15" customHeight="1">
       <c r="A503" s="4"/>
-      <c r="B503" s="73"/>
-      <c r="C503" s="4"/>
-      <c r="D503" s="4"/>
-      <c r="E503" s="9"/>
-      <c r="F503" s="4"/>
-      <c r="G503" s="4"/>
-      <c r="H503" s="4"/>
-      <c r="I503" s="4"/>
-      <c r="J503" s="4"/>
+      <c r="B503" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C503" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D503" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E503" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F503" s="117" t="s">
+        <v>189</v>
+      </c>
+      <c r="G503" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H503" s="117" t="s">
+        <v>192</v>
+      </c>
+      <c r="I503" s="4">
+        <v>298</v>
+      </c>
+      <c r="J503" s="106">
+        <v>1198000000</v>
+      </c>
       <c r="K503" s="4"/>
-      <c r="L503" s="4"/>
-      <c r="M503" s="4"/>
-      <c r="N503" s="4"/>
+      <c r="L503" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M503" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N503" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O503" s="9"/>
       <c r="P503" s="4"/>
       <c r="Q503" s="4"/>
@@ -26499,19 +27033,43 @@
     </row>
     <row r="504" spans="1:20" ht="15" customHeight="1">
       <c r="A504" s="4"/>
-      <c r="B504" s="73"/>
-      <c r="C504" s="4"/>
-      <c r="D504" s="4"/>
-      <c r="E504" s="9"/>
-      <c r="F504" s="4"/>
-      <c r="G504" s="4"/>
-      <c r="H504" s="4"/>
-      <c r="I504" s="4"/>
-      <c r="J504" s="4"/>
+      <c r="B504" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C504" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D504" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E504" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F504" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G504" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H504" s="117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I504" s="4">
+        <v>1573</v>
+      </c>
+      <c r="J504" s="106">
+        <v>263000000</v>
+      </c>
       <c r="K504" s="4"/>
-      <c r="L504" s="4"/>
-      <c r="M504" s="4"/>
-      <c r="N504" s="4"/>
+      <c r="L504" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M504" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N504" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O504" s="9"/>
       <c r="P504" s="4"/>
       <c r="Q504" s="4"/>
@@ -26521,19 +27079,43 @@
     </row>
     <row r="505" spans="1:20" ht="15" customHeight="1">
       <c r="A505" s="4"/>
-      <c r="B505" s="73"/>
-      <c r="C505" s="4"/>
-      <c r="D505" s="4"/>
-      <c r="E505" s="9"/>
-      <c r="F505" s="4"/>
-      <c r="G505" s="4"/>
-      <c r="H505" s="4"/>
-      <c r="I505" s="4"/>
-      <c r="J505" s="4"/>
+      <c r="B505" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C505" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D505" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E505" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F505" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G505" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H505" s="117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I505" s="4">
+        <v>1573</v>
+      </c>
+      <c r="J505" s="106">
+        <v>253000000</v>
+      </c>
       <c r="K505" s="4"/>
-      <c r="L505" s="4"/>
-      <c r="M505" s="4"/>
-      <c r="N505" s="4"/>
+      <c r="L505" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M505" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N505" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O505" s="9"/>
       <c r="P505" s="4"/>
       <c r="Q505" s="4"/>
@@ -26543,19 +27125,43 @@
     </row>
     <row r="506" spans="1:20" ht="15" customHeight="1">
       <c r="A506" s="4"/>
-      <c r="B506" s="73"/>
-      <c r="C506" s="4"/>
-      <c r="D506" s="4"/>
-      <c r="E506" s="9"/>
-      <c r="F506" s="4"/>
-      <c r="G506" s="4"/>
-      <c r="H506" s="4"/>
-      <c r="I506" s="4"/>
-      <c r="J506" s="4"/>
+      <c r="B506" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C506" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D506" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E506" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F506" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G506" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H506" s="117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I506" s="4">
+        <v>1573</v>
+      </c>
+      <c r="J506" s="106">
+        <v>480000000</v>
+      </c>
       <c r="K506" s="4"/>
-      <c r="L506" s="4"/>
-      <c r="M506" s="4"/>
-      <c r="N506" s="4"/>
+      <c r="L506" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M506" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N506" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O506" s="9"/>
       <c r="P506" s="4"/>
       <c r="Q506" s="4"/>
@@ -26565,19 +27171,43 @@
     </row>
     <row r="507" spans="1:20" ht="15" customHeight="1">
       <c r="A507" s="4"/>
-      <c r="B507" s="73"/>
-      <c r="C507" s="4"/>
-      <c r="D507" s="4"/>
-      <c r="E507" s="9"/>
-      <c r="F507" s="4"/>
-      <c r="G507" s="4"/>
-      <c r="H507" s="4"/>
-      <c r="I507" s="4"/>
-      <c r="J507" s="4"/>
+      <c r="B507" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C507" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D507" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E507" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F507" s="117" t="s">
+        <v>189</v>
+      </c>
+      <c r="G507" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H507" s="117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I507" s="4">
+        <v>1573</v>
+      </c>
+      <c r="J507" s="106">
+        <v>304000000</v>
+      </c>
       <c r="K507" s="70"/>
-      <c r="L507" s="4"/>
-      <c r="M507" s="4"/>
-      <c r="N507" s="4"/>
+      <c r="L507" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M507" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N507" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O507" s="9"/>
       <c r="P507" s="4"/>
       <c r="Q507" s="4"/>
@@ -26587,19 +27217,43 @@
     </row>
     <row r="508" spans="1:20" ht="15" customHeight="1">
       <c r="A508" s="4"/>
-      <c r="B508" s="73"/>
-      <c r="C508" s="4"/>
-      <c r="D508" s="4"/>
-      <c r="E508" s="9"/>
-      <c r="F508" s="4"/>
-      <c r="G508" s="4"/>
-      <c r="H508" s="4"/>
-      <c r="I508" s="4"/>
-      <c r="J508" s="70"/>
+      <c r="B508" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C508" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D508" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E508" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F508" s="117" t="s">
+        <v>189</v>
+      </c>
+      <c r="G508" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H508" s="117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I508" s="4">
+        <v>1573</v>
+      </c>
+      <c r="J508" s="70">
+        <v>270000000</v>
+      </c>
       <c r="K508" s="70"/>
-      <c r="L508" s="4"/>
-      <c r="M508" s="4"/>
-      <c r="N508" s="4"/>
+      <c r="L508" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M508" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N508" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O508" s="9"/>
       <c r="P508" s="4"/>
       <c r="Q508" s="4"/>
@@ -26609,19 +27263,43 @@
     </row>
     <row r="509" spans="1:20" ht="15" customHeight="1">
       <c r="A509" s="4"/>
-      <c r="B509" s="73"/>
-      <c r="C509" s="4"/>
-      <c r="D509" s="4"/>
-      <c r="E509" s="9"/>
-      <c r="F509" s="4"/>
-      <c r="G509" s="4"/>
-      <c r="H509" s="4"/>
-      <c r="I509" s="4"/>
-      <c r="J509" s="70"/>
+      <c r="B509" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C509" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D509" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E509" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F509" s="117" t="s">
+        <v>189</v>
+      </c>
+      <c r="G509" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H509" s="117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I509" s="4">
+        <v>1573</v>
+      </c>
+      <c r="J509" s="70">
+        <v>673000000</v>
+      </c>
       <c r="K509" s="70"/>
-      <c r="L509" s="4"/>
-      <c r="M509" s="4"/>
-      <c r="N509" s="4"/>
+      <c r="L509" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M509" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N509" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O509" s="9"/>
       <c r="P509" s="4"/>
       <c r="Q509" s="4"/>
@@ -26631,19 +27309,43 @@
     </row>
     <row r="510" spans="1:20" ht="15" customHeight="1">
       <c r="A510" s="4"/>
-      <c r="B510" s="73"/>
-      <c r="C510" s="4"/>
-      <c r="D510" s="4"/>
-      <c r="E510" s="9"/>
-      <c r="F510" s="4"/>
-      <c r="G510" s="4"/>
-      <c r="H510" s="4"/>
-      <c r="I510" s="4"/>
-      <c r="J510" s="70"/>
+      <c r="B510" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C510" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D510" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E510" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F510" s="117" t="s">
+        <v>170</v>
+      </c>
+      <c r="G510" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H510" s="117" t="s">
+        <v>192</v>
+      </c>
+      <c r="I510" s="4">
+        <v>298</v>
+      </c>
+      <c r="J510" s="4">
+        <v>1.08975712777191</v>
+      </c>
       <c r="K510" s="70"/>
-      <c r="L510" s="4"/>
-      <c r="M510" s="4"/>
-      <c r="N510" s="4"/>
+      <c r="L510" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M510" s="117" t="s">
+        <v>651</v>
+      </c>
+      <c r="N510" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O510" s="9"/>
       <c r="P510" s="4"/>
       <c r="Q510" s="4"/>
@@ -26653,19 +27355,43 @@
     </row>
     <row r="511" spans="1:20" ht="15" customHeight="1">
       <c r="A511" s="4"/>
-      <c r="B511" s="73"/>
-      <c r="C511" s="4"/>
-      <c r="D511" s="4"/>
-      <c r="E511" s="9"/>
-      <c r="F511" s="4"/>
-      <c r="G511" s="4"/>
-      <c r="H511" s="4"/>
-      <c r="I511" s="4"/>
-      <c r="J511" s="70"/>
+      <c r="B511" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C511" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D511" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E511" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F511" s="117" t="s">
+        <v>170</v>
+      </c>
+      <c r="G511" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H511" s="117" t="s">
+        <v>192</v>
+      </c>
+      <c r="I511" s="4">
+        <v>298</v>
+      </c>
+      <c r="J511" s="4">
+        <v>3.73178458289334</v>
+      </c>
       <c r="K511" s="70"/>
-      <c r="L511" s="4"/>
-      <c r="M511" s="4"/>
-      <c r="N511" s="4"/>
+      <c r="L511" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M511" s="117" t="s">
+        <v>651</v>
+      </c>
+      <c r="N511" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O511" s="9"/>
       <c r="P511" s="4"/>
       <c r="Q511" s="4"/>
@@ -26675,19 +27401,43 @@
     </row>
     <row r="512" spans="1:20" ht="15" customHeight="1">
       <c r="A512" s="4"/>
-      <c r="B512" s="73"/>
-      <c r="C512" s="4"/>
-      <c r="D512" s="4"/>
-      <c r="E512" s="9"/>
-      <c r="F512" s="4"/>
-      <c r="G512" s="4"/>
-      <c r="H512" s="4"/>
-      <c r="I512" s="4"/>
-      <c r="J512" s="70"/>
+      <c r="B512" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C512" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D512" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E512" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F512" s="117" t="s">
+        <v>170</v>
+      </c>
+      <c r="G512" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H512" s="117" t="s">
+        <v>192</v>
+      </c>
+      <c r="I512" s="4">
+        <v>298</v>
+      </c>
+      <c r="J512" s="4">
+        <v>5.2967265047518399</v>
+      </c>
       <c r="K512" s="4"/>
-      <c r="L512" s="4"/>
-      <c r="M512" s="4"/>
-      <c r="N512" s="4"/>
+      <c r="L512" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M512" s="117" t="s">
+        <v>651</v>
+      </c>
+      <c r="N512" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O512" s="9"/>
       <c r="P512" s="4"/>
       <c r="Q512" s="4"/>
@@ -26697,19 +27447,43 @@
     </row>
     <row r="513" spans="1:20" ht="15" customHeight="1">
       <c r="A513" s="4"/>
-      <c r="B513" s="73"/>
-      <c r="C513" s="4"/>
-      <c r="D513" s="4"/>
-      <c r="E513" s="9"/>
-      <c r="F513" s="4"/>
-      <c r="G513" s="4"/>
-      <c r="H513" s="4"/>
-      <c r="I513" s="4"/>
-      <c r="J513" s="4"/>
+      <c r="B513" s="110" t="s">
+        <v>647</v>
+      </c>
+      <c r="C513" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D513" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E513" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F513" s="117" t="s">
+        <v>170</v>
+      </c>
+      <c r="G513" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H513" s="117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I513" s="4">
+        <v>1573</v>
+      </c>
+      <c r="J513" s="1">
+        <v>12.991803278688501</v>
+      </c>
       <c r="K513" s="4"/>
-      <c r="L513" s="4"/>
-      <c r="M513" s="4"/>
-      <c r="N513" s="4"/>
+      <c r="L513" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M513" s="117" t="s">
+        <v>651</v>
+      </c>
+      <c r="N513" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O513" s="9"/>
       <c r="P513" s="4"/>
       <c r="Q513" s="4"/>
@@ -26719,19 +27493,43 @@
     </row>
     <row r="514" spans="1:20" ht="15" customHeight="1">
       <c r="A514" s="4"/>
-      <c r="B514" s="73"/>
-      <c r="C514" s="4"/>
-      <c r="D514" s="4"/>
-      <c r="E514" s="9"/>
-      <c r="F514" s="4"/>
-      <c r="G514" s="4"/>
-      <c r="H514" s="4"/>
-      <c r="I514" s="4"/>
-      <c r="J514" s="4"/>
+      <c r="B514" s="110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C514" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D514" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E514" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F514" s="117" t="s">
+        <v>170</v>
+      </c>
+      <c r="G514" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H514" s="117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I514" s="4">
+        <v>1573</v>
+      </c>
+      <c r="J514" s="1">
+        <v>6.9808743169398904</v>
+      </c>
       <c r="K514" s="4"/>
-      <c r="L514" s="4"/>
-      <c r="M514" s="4"/>
-      <c r="N514" s="4"/>
+      <c r="L514" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M514" s="117" t="s">
+        <v>651</v>
+      </c>
+      <c r="N514" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O514" s="9"/>
       <c r="P514" s="4"/>
       <c r="Q514" s="4"/>
@@ -26741,19 +27539,43 @@
     </row>
     <row r="515" spans="1:20" ht="15" customHeight="1">
       <c r="A515" s="4"/>
-      <c r="B515" s="73"/>
-      <c r="C515" s="4"/>
-      <c r="D515" s="4"/>
-      <c r="E515" s="9"/>
-      <c r="F515" s="4"/>
-      <c r="G515" s="4"/>
-      <c r="H515" s="4"/>
-      <c r="I515" s="4"/>
-      <c r="J515" s="4"/>
+      <c r="B515" s="110" t="s">
+        <v>649</v>
+      </c>
+      <c r="C515" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D515" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E515" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="F515" s="117" t="s">
+        <v>170</v>
+      </c>
+      <c r="G515" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="H515" s="117" t="s">
+        <v>290</v>
+      </c>
+      <c r="I515" s="4">
+        <v>1573</v>
+      </c>
+      <c r="J515" s="1">
+        <v>12.021857923497199</v>
+      </c>
       <c r="K515" s="4"/>
-      <c r="L515" s="4"/>
-      <c r="M515" s="4"/>
-      <c r="N515" s="4"/>
+      <c r="L515" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M515" s="117" t="s">
+        <v>651</v>
+      </c>
+      <c r="N515" s="117" t="s">
+        <v>652</v>
+      </c>
       <c r="O515" s="9"/>
       <c r="P515" s="4"/>
       <c r="Q515" s="4"/>
@@ -34309,6 +35131,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -34323,11 +35150,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s40194-024-01879-2`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1407F40-B186-EC4F-B923-87FFD3A840CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164603A8-C490-3048-AD9C-A1E0C4FD9932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6080" windowWidth="34560" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="8640" windowWidth="34560" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4478" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4522" uniqueCount="656">
   <si>
     <r>
       <rPr>
@@ -2089,6 +2089,15 @@
   </si>
   <si>
     <t>10.1016/j.actamat.2023.118784</t>
+  </si>
+  <si>
+    <t>Mn35 Co20 Ni20 Cu20 Ge5</t>
+  </si>
+  <si>
+    <t>Mn35 Co20 Ni20 Cu20 In5</t>
+  </si>
+  <si>
+    <t>10.1007/s40194-024-01879-2</t>
   </si>
 </sst>
 </file>
@@ -3238,6 +3247,57 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3297,57 +3357,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4511,8 +4520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A480" zoomScale="86" workbookViewId="0">
-      <selection activeCell="O513" sqref="O513"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A501" zoomScale="86" workbookViewId="0">
+      <selection activeCell="J526" sqref="J526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -4569,19 +4578,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="130"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="137"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="151"/>
+      <c r="M2" s="151"/>
+      <c r="N2" s="154"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -4597,17 +4606,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="141"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="155"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="157"/>
+      <c r="K3" s="157"/>
+      <c r="L3" s="155"/>
+      <c r="M3" s="155"/>
+      <c r="N3" s="158"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -4648,43 +4657,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="159" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="144" t="s">
+      <c r="D5" s="161" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="161" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="161" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="144" t="s">
+      <c r="G5" s="161" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="145" t="s">
+      <c r="H5" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="144" t="s">
+      <c r="I5" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="144" t="s">
+      <c r="J5" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="144" t="s">
+      <c r="K5" s="161" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="144" t="s">
+      <c r="L5" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="144" t="s">
+      <c r="M5" s="161" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="144" t="s">
+      <c r="N5" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="149" t="s">
+      <c r="O5" s="129" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -4700,19 +4709,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="150"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="160"/>
+      <c r="F6" s="160"/>
+      <c r="G6" s="160"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="164"/>
+      <c r="J6" s="165"/>
+      <c r="K6" s="165"/>
+      <c r="L6" s="160"/>
+      <c r="M6" s="160"/>
+      <c r="N6" s="160"/>
+      <c r="O6" s="130"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -4762,7 +4771,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="151"/>
+      <c r="O7" s="131"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -4777,35 +4786,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="153"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="155" t="s">
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="156"/>
-      <c r="H8" s="156"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="158"/>
-      <c r="K8" s="158"/>
-      <c r="L8" s="159"/>
-      <c r="M8" s="160" t="s">
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="161"/>
+      <c r="N8" s="141"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="162" t="s">
+      <c r="P8" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="163"/>
-      <c r="R8" s="164"/>
-      <c r="S8" s="164"/>
-      <c r="T8" s="165"/>
+      <c r="Q8" s="143"/>
+      <c r="R8" s="144"/>
+      <c r="S8" s="144"/>
+      <c r="T8" s="145"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="38" t="s">
@@ -27585,21 +27594,40 @@
     </row>
     <row r="516" spans="1:20" ht="15" customHeight="1">
       <c r="A516" s="4"/>
-      <c r="B516" s="73"/>
-      <c r="C516" s="4"/>
-      <c r="D516" s="4"/>
+      <c r="B516" s="110" t="s">
+        <v>654</v>
+      </c>
+      <c r="C516" s="117" t="s">
+        <v>102</v>
+      </c>
+      <c r="D516" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E516" s="9"/>
-      <c r="F516" s="4"/>
-      <c r="G516" s="4"/>
+      <c r="F516" s="117" t="s">
+        <v>250</v>
+      </c>
+      <c r="G516" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H516" s="4"/>
       <c r="I516" s="4"/>
-      <c r="J516" s="4"/>
+      <c r="J516" s="4">
+        <f>P516+273.15</f>
+        <v>1247.1500000000001</v>
+      </c>
       <c r="K516" s="4"/>
-      <c r="L516" s="4"/>
+      <c r="L516" s="117" t="s">
+        <v>249</v>
+      </c>
       <c r="M516" s="4"/>
-      <c r="N516" s="4"/>
+      <c r="N516" s="117" t="s">
+        <v>655</v>
+      </c>
       <c r="O516" s="9"/>
-      <c r="P516" s="4"/>
+      <c r="P516" s="4">
+        <v>974</v>
+      </c>
       <c r="Q516" s="4"/>
       <c r="R516" s="9"/>
       <c r="S516" s="9"/>
@@ -27607,21 +27635,40 @@
     </row>
     <row r="517" spans="1:20" ht="15" customHeight="1">
       <c r="A517" s="4"/>
-      <c r="B517" s="73"/>
-      <c r="C517" s="4"/>
-      <c r="D517" s="4"/>
+      <c r="B517" s="110" t="s">
+        <v>653</v>
+      </c>
+      <c r="C517" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="D517" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E517" s="9"/>
-      <c r="F517" s="4"/>
-      <c r="G517" s="4"/>
+      <c r="F517" s="117" t="s">
+        <v>250</v>
+      </c>
+      <c r="G517" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H517" s="4"/>
       <c r="I517" s="4"/>
-      <c r="J517" s="4"/>
+      <c r="J517" s="4">
+        <f t="shared" ref="J517:J519" si="14">P517+273.15</f>
+        <v>1226.4499999999998</v>
+      </c>
       <c r="K517" s="4"/>
-      <c r="L517" s="4"/>
+      <c r="L517" s="117" t="s">
+        <v>249</v>
+      </c>
       <c r="M517" s="4"/>
-      <c r="N517" s="4"/>
+      <c r="N517" s="117" t="s">
+        <v>655</v>
+      </c>
       <c r="O517" s="9"/>
-      <c r="P517" s="4"/>
+      <c r="P517" s="4">
+        <v>953.3</v>
+      </c>
       <c r="Q517" s="4"/>
       <c r="R517" s="9"/>
       <c r="S517" s="9"/>
@@ -27629,21 +27676,40 @@
     </row>
     <row r="518" spans="1:20" ht="15" customHeight="1">
       <c r="A518" s="4"/>
-      <c r="B518" s="73"/>
-      <c r="C518" s="4"/>
-      <c r="D518" s="4"/>
+      <c r="B518" s="110" t="s">
+        <v>654</v>
+      </c>
+      <c r="C518" s="117" t="s">
+        <v>102</v>
+      </c>
+      <c r="D518" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E518" s="9"/>
-      <c r="F518" s="4"/>
-      <c r="G518" s="4"/>
+      <c r="F518" s="117" t="s">
+        <v>248</v>
+      </c>
+      <c r="G518" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H518" s="4"/>
       <c r="I518" s="4"/>
-      <c r="J518" s="4"/>
+      <c r="J518" s="4">
+        <f t="shared" si="14"/>
+        <v>1362.15</v>
+      </c>
       <c r="K518" s="4"/>
-      <c r="L518" s="4"/>
+      <c r="L518" s="117" t="s">
+        <v>249</v>
+      </c>
       <c r="M518" s="4"/>
-      <c r="N518" s="4"/>
+      <c r="N518" s="117" t="s">
+        <v>655</v>
+      </c>
       <c r="O518" s="9"/>
-      <c r="P518" s="4"/>
+      <c r="P518" s="4">
+        <v>1089</v>
+      </c>
       <c r="Q518" s="4"/>
       <c r="R518" s="9"/>
       <c r="S518" s="9"/>
@@ -27651,21 +27717,40 @@
     </row>
     <row r="519" spans="1:20" ht="15" customHeight="1">
       <c r="A519" s="4"/>
-      <c r="B519" s="73"/>
-      <c r="C519" s="4"/>
-      <c r="D519" s="4"/>
+      <c r="B519" s="110" t="s">
+        <v>653</v>
+      </c>
+      <c r="C519" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="D519" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E519" s="9"/>
-      <c r="F519" s="4"/>
-      <c r="G519" s="4"/>
+      <c r="F519" s="117" t="s">
+        <v>248</v>
+      </c>
+      <c r="G519" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H519" s="4"/>
       <c r="I519" s="4"/>
-      <c r="J519" s="4"/>
+      <c r="J519" s="4">
+        <f t="shared" si="14"/>
+        <v>1373.75</v>
+      </c>
       <c r="K519" s="4"/>
-      <c r="L519" s="4"/>
+      <c r="L519" s="117" t="s">
+        <v>249</v>
+      </c>
       <c r="M519" s="4"/>
-      <c r="N519" s="4"/>
+      <c r="N519" s="117" t="s">
+        <v>655</v>
+      </c>
       <c r="O519" s="9"/>
-      <c r="P519" s="4"/>
+      <c r="P519" s="4">
+        <v>1100.5999999999999</v>
+      </c>
       <c r="Q519" s="4"/>
       <c r="R519" s="9"/>
       <c r="S519" s="9"/>
@@ -27673,19 +27758,41 @@
     </row>
     <row r="520" spans="1:20" ht="15" customHeight="1">
       <c r="A520" s="4"/>
-      <c r="B520" s="73"/>
-      <c r="C520" s="4"/>
-      <c r="D520" s="4"/>
+      <c r="B520" s="110" t="s">
+        <v>654</v>
+      </c>
+      <c r="C520" s="117" t="s">
+        <v>102</v>
+      </c>
+      <c r="D520" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E520" s="9"/>
-      <c r="F520" s="4"/>
-      <c r="G520" s="4"/>
+      <c r="F520" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G520" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H520" s="4"/>
-      <c r="I520" s="4"/>
-      <c r="J520" s="4"/>
-      <c r="K520" s="4"/>
-      <c r="L520" s="4"/>
-      <c r="M520" s="4"/>
-      <c r="N520" s="4"/>
+      <c r="I520" s="4">
+        <v>298</v>
+      </c>
+      <c r="J520" s="106">
+        <v>2402000000</v>
+      </c>
+      <c r="K520" s="106">
+        <v>20000000</v>
+      </c>
+      <c r="L520" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M520" s="117" t="s">
+        <v>299</v>
+      </c>
+      <c r="N520" s="117" t="s">
+        <v>655</v>
+      </c>
       <c r="O520" s="9"/>
       <c r="P520" s="4"/>
       <c r="Q520" s="4"/>
@@ -27695,19 +27802,41 @@
     </row>
     <row r="521" spans="1:20" ht="15" customHeight="1">
       <c r="A521" s="4"/>
-      <c r="B521" s="73"/>
-      <c r="C521" s="4"/>
-      <c r="D521" s="4"/>
+      <c r="B521" s="110" t="s">
+        <v>653</v>
+      </c>
+      <c r="C521" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="D521" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E521" s="9"/>
-      <c r="F521" s="4"/>
-      <c r="G521" s="4"/>
+      <c r="F521" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G521" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H521" s="4"/>
-      <c r="I521" s="4"/>
-      <c r="J521" s="4"/>
-      <c r="K521" s="4"/>
-      <c r="L521" s="4"/>
-      <c r="M521" s="4"/>
-      <c r="N521" s="4"/>
+      <c r="I521" s="4">
+        <v>298</v>
+      </c>
+      <c r="J521" s="106">
+        <v>1889500000</v>
+      </c>
+      <c r="K521" s="106">
+        <v>20000000</v>
+      </c>
+      <c r="L521" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M521" s="117" t="s">
+        <v>299</v>
+      </c>
+      <c r="N521" s="117" t="s">
+        <v>655</v>
+      </c>
       <c r="O521" s="9"/>
       <c r="P521" s="4"/>
       <c r="Q521" s="4"/>
@@ -35131,11 +35260,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -35150,6 +35274,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted structural data from `10.3390/met11121962`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164603A8-C490-3048-AD9C-A1E0C4FD9932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B359FF-27BF-E646-BD39-C262D9F74D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="8640" windowWidth="34560" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4522" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4546" uniqueCount="669">
   <si>
     <r>
       <rPr>
@@ -2098,6 +2098,45 @@
   </si>
   <si>
     <t>10.1007/s40194-024-01879-2</t>
+  </si>
+  <si>
+    <t>arc melting in helium not argon but assigned AAM for practical purposes; homogenized at 673K for 50h</t>
+  </si>
+  <si>
+    <t>TiZrHfNbCoNiAl</t>
+  </si>
+  <si>
+    <t>TiZrHfNbVCrMoMnFeCoNiAl</t>
+  </si>
+  <si>
+    <t>TiZrHfNbVCrMoMnFeCoNiAlSc</t>
+  </si>
+  <si>
+    <t>TiZrHfNbVCrMoMnFeCoNiAlBe</t>
+  </si>
+  <si>
+    <t>7x</t>
+  </si>
+  <si>
+    <t>12x</t>
+  </si>
+  <si>
+    <t>12x+Sc</t>
+  </si>
+  <si>
+    <t>12x+Be</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C14+?</t>
+  </si>
+  <si>
+    <t>C14+C15</t>
+  </si>
+  <si>
+    <t>10.3390/met11121962</t>
   </si>
 </sst>
 </file>
@@ -4520,8 +4559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A501" zoomScale="86" workbookViewId="0">
-      <selection activeCell="J526" sqref="J526"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A509" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N533" sqref="N533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -27845,11 +27884,21 @@
       <c r="T521" s="9"/>
     </row>
     <row r="522" spans="1:20" ht="15" customHeight="1">
-      <c r="A522" s="4"/>
-      <c r="B522" s="73"/>
-      <c r="C522" s="4"/>
-      <c r="D522" s="4"/>
-      <c r="E522" s="9"/>
+      <c r="A522" s="117" t="s">
+        <v>661</v>
+      </c>
+      <c r="B522" s="110" t="s">
+        <v>657</v>
+      </c>
+      <c r="C522" s="117" t="s">
+        <v>666</v>
+      </c>
+      <c r="D522" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E522" s="119" t="s">
+        <v>656</v>
+      </c>
       <c r="F522" s="4"/>
       <c r="G522" s="4"/>
       <c r="H522" s="4"/>
@@ -27858,7 +27907,9 @@
       <c r="K522" s="4"/>
       <c r="L522" s="4"/>
       <c r="M522" s="4"/>
-      <c r="N522" s="4"/>
+      <c r="N522" s="117" t="s">
+        <v>668</v>
+      </c>
       <c r="O522" s="9"/>
       <c r="P522" s="4"/>
       <c r="Q522" s="4"/>
@@ -27867,11 +27918,21 @@
       <c r="T522" s="9"/>
     </row>
     <row r="523" spans="1:20" ht="15" customHeight="1">
-      <c r="A523" s="4"/>
-      <c r="B523" s="73"/>
-      <c r="C523" s="4"/>
-      <c r="D523" s="4"/>
-      <c r="E523" s="9"/>
+      <c r="A523" s="117" t="s">
+        <v>662</v>
+      </c>
+      <c r="B523" s="110" t="s">
+        <v>658</v>
+      </c>
+      <c r="C523" s="117" t="s">
+        <v>665</v>
+      </c>
+      <c r="D523" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E523" s="119" t="s">
+        <v>656</v>
+      </c>
       <c r="F523" s="4"/>
       <c r="G523" s="4"/>
       <c r="H523" s="4"/>
@@ -27880,7 +27941,9 @@
       <c r="K523" s="4"/>
       <c r="L523" s="4"/>
       <c r="M523" s="4"/>
-      <c r="N523" s="4"/>
+      <c r="N523" s="117" t="s">
+        <v>668</v>
+      </c>
       <c r="O523" s="9"/>
       <c r="P523" s="4"/>
       <c r="Q523" s="4"/>
@@ -27889,11 +27952,21 @@
       <c r="T523" s="9"/>
     </row>
     <row r="524" spans="1:20" ht="15" customHeight="1">
-      <c r="A524" s="4"/>
-      <c r="B524" s="73"/>
-      <c r="C524" s="4"/>
-      <c r="D524" s="4"/>
-      <c r="E524" s="9"/>
+      <c r="A524" s="117" t="s">
+        <v>663</v>
+      </c>
+      <c r="B524" s="110" t="s">
+        <v>659</v>
+      </c>
+      <c r="C524" s="117" t="s">
+        <v>665</v>
+      </c>
+      <c r="D524" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E524" s="119" t="s">
+        <v>656</v>
+      </c>
       <c r="F524" s="4"/>
       <c r="G524" s="4"/>
       <c r="H524" s="4"/>
@@ -27902,7 +27975,9 @@
       <c r="K524" s="4"/>
       <c r="L524" s="4"/>
       <c r="M524" s="4"/>
-      <c r="N524" s="4"/>
+      <c r="N524" s="117" t="s">
+        <v>668</v>
+      </c>
       <c r="O524" s="9"/>
       <c r="P524" s="4"/>
       <c r="Q524" s="4"/>
@@ -27911,11 +27986,21 @@
       <c r="T524" s="9"/>
     </row>
     <row r="525" spans="1:20" ht="15" customHeight="1">
-      <c r="A525" s="4"/>
-      <c r="B525" s="73"/>
-      <c r="C525" s="4"/>
-      <c r="D525" s="4"/>
-      <c r="E525" s="9"/>
+      <c r="A525" s="117" t="s">
+        <v>664</v>
+      </c>
+      <c r="B525" s="110" t="s">
+        <v>660</v>
+      </c>
+      <c r="C525" s="117" t="s">
+        <v>667</v>
+      </c>
+      <c r="D525" s="117" t="s">
+        <v>195</v>
+      </c>
+      <c r="E525" s="119" t="s">
+        <v>656</v>
+      </c>
       <c r="F525" s="4"/>
       <c r="G525" s="4"/>
       <c r="H525" s="4"/>
@@ -27924,7 +28009,9 @@
       <c r="K525" s="4"/>
       <c r="L525" s="4"/>
       <c r="M525" s="4"/>
-      <c r="N525" s="4"/>
+      <c r="N525" s="117" t="s">
+        <v>668</v>
+      </c>
       <c r="O525" s="9"/>
       <c r="P525" s="4"/>
       <c r="Q525" s="4"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.jmrt.2024.12.204`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B359FF-27BF-E646-BD39-C262D9F74D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E146D057-15B5-4142-A9B7-8DE1F78E3BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="8640" windowWidth="34560" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="3300" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4546" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4636" uniqueCount="678">
   <si>
     <r>
       <rPr>
@@ -2137,6 +2137,33 @@
   </si>
   <si>
     <t>10.3390/met11121962</t>
+  </si>
+  <si>
+    <t>RHEA0</t>
+  </si>
+  <si>
+    <t>RHEA1</t>
+  </si>
+  <si>
+    <t>RHEA2</t>
+  </si>
+  <si>
+    <t>Ti25.00 V25.00 Nb25.00 Mo25.00</t>
+  </si>
+  <si>
+    <t>Ti20.00 V35.00 Nb35.00 Mo10.00</t>
+  </si>
+  <si>
+    <t>Ti35.00 V35.00 Nb10.00 Mo20.00</t>
+  </si>
+  <si>
+    <t>ST2</t>
+  </si>
+  <si>
+    <t>F14</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmrt.2024.12.204</t>
   </si>
 </sst>
 </file>
@@ -3286,57 +3313,6 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3396,6 +3372,57 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4559,8 +4586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A509" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N533" sqref="N533"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A511" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N538" sqref="N538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -4617,19 +4644,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="146" t="s">
+      <c r="D2" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="147"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="151"/>
-      <c r="M2" s="151"/>
-      <c r="N2" s="154"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="137"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -4645,17 +4672,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="155"/>
-      <c r="M3" s="155"/>
-      <c r="N3" s="158"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="141"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -4696,43 +4723,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="142" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="161" t="s">
+      <c r="D5" s="144" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="161" t="s">
+      <c r="E5" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="161" t="s">
+      <c r="F5" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="161" t="s">
+      <c r="G5" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="162" t="s">
+      <c r="H5" s="145" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="161" t="s">
+      <c r="I5" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="161" t="s">
+      <c r="J5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="161" t="s">
+      <c r="K5" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="161" t="s">
+      <c r="L5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="161" t="s">
+      <c r="M5" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="161" t="s">
+      <c r="N5" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="129" t="s">
+      <c r="O5" s="149" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -4748,19 +4775,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="160"/>
-      <c r="D6" s="160"/>
-      <c r="E6" s="160"/>
-      <c r="F6" s="160"/>
-      <c r="G6" s="160"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="164"/>
-      <c r="J6" s="165"/>
-      <c r="K6" s="165"/>
-      <c r="L6" s="160"/>
-      <c r="M6" s="160"/>
-      <c r="N6" s="160"/>
-      <c r="O6" s="130"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="147"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="150"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -4810,7 +4837,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="131"/>
+      <c r="O7" s="151"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -4825,35 +4852,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="152" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="135" t="s">
+      <c r="C8" s="153"/>
+      <c r="D8" s="153"/>
+      <c r="E8" s="154"/>
+      <c r="F8" s="155" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="137"/>
-      <c r="J8" s="138"/>
-      <c r="K8" s="138"/>
-      <c r="L8" s="139"/>
-      <c r="M8" s="140" t="s">
+      <c r="G8" s="156"/>
+      <c r="H8" s="156"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="158"/>
+      <c r="L8" s="159"/>
+      <c r="M8" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="141"/>
+      <c r="N8" s="161"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="142" t="s">
+      <c r="P8" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="143"/>
-      <c r="R8" s="144"/>
-      <c r="S8" s="144"/>
-      <c r="T8" s="145"/>
+      <c r="Q8" s="163"/>
+      <c r="R8" s="164"/>
+      <c r="S8" s="164"/>
+      <c r="T8" s="165"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="38" t="s">
@@ -28020,20 +28047,44 @@
       <c r="T525" s="9"/>
     </row>
     <row r="526" spans="1:20" ht="15" customHeight="1">
-      <c r="A526" s="4"/>
-      <c r="B526" s="73"/>
-      <c r="C526" s="4"/>
-      <c r="D526" s="4"/>
+      <c r="A526" s="117" t="s">
+        <v>669</v>
+      </c>
+      <c r="B526" s="110" t="s">
+        <v>672</v>
+      </c>
+      <c r="C526" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D526" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E526" s="9"/>
-      <c r="F526" s="4"/>
-      <c r="G526" s="4"/>
+      <c r="F526" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="G526" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H526" s="4"/>
-      <c r="I526" s="4"/>
-      <c r="J526" s="4"/>
-      <c r="K526" s="4"/>
-      <c r="L526" s="4"/>
-      <c r="M526" s="4"/>
-      <c r="N526" s="4"/>
+      <c r="I526" s="4">
+        <v>298</v>
+      </c>
+      <c r="J526" s="4">
+        <v>7330</v>
+      </c>
+      <c r="K526" s="4">
+        <v>10</v>
+      </c>
+      <c r="L526" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="M526" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="N526" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O526" s="9"/>
       <c r="P526" s="4"/>
       <c r="Q526" s="4"/>
@@ -28042,20 +28093,44 @@
       <c r="T526" s="9"/>
     </row>
     <row r="527" spans="1:20" ht="15" customHeight="1">
-      <c r="A527" s="4"/>
-      <c r="B527" s="73"/>
-      <c r="C527" s="4"/>
-      <c r="D527" s="4"/>
+      <c r="A527" s="117" t="s">
+        <v>670</v>
+      </c>
+      <c r="B527" s="110" t="s">
+        <v>673</v>
+      </c>
+      <c r="C527" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D527" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E527" s="9"/>
-      <c r="F527" s="4"/>
-      <c r="G527" s="4"/>
+      <c r="F527" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="G527" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H527" s="4"/>
-      <c r="I527" s="4"/>
-      <c r="J527" s="4"/>
-      <c r="K527" s="4"/>
-      <c r="L527" s="4"/>
-      <c r="M527" s="4"/>
-      <c r="N527" s="4"/>
+      <c r="I527" s="4">
+        <v>298</v>
+      </c>
+      <c r="J527" s="4">
+        <v>7040</v>
+      </c>
+      <c r="K527" s="4">
+        <v>30</v>
+      </c>
+      <c r="L527" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="M527" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="N527" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O527" s="9"/>
       <c r="P527" s="4"/>
       <c r="Q527" s="4"/>
@@ -28064,20 +28139,44 @@
       <c r="T527" s="9"/>
     </row>
     <row r="528" spans="1:20" ht="15" customHeight="1">
-      <c r="A528" s="4"/>
-      <c r="B528" s="73"/>
-      <c r="C528" s="4"/>
-      <c r="D528" s="4"/>
+      <c r="A528" s="117" t="s">
+        <v>671</v>
+      </c>
+      <c r="B528" s="110" t="s">
+        <v>674</v>
+      </c>
+      <c r="C528" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D528" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E528" s="9"/>
-      <c r="F528" s="4"/>
-      <c r="G528" s="4"/>
+      <c r="F528" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="G528" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H528" s="4"/>
-      <c r="I528" s="4"/>
-      <c r="J528" s="4"/>
-      <c r="K528" s="4"/>
-      <c r="L528" s="4"/>
-      <c r="M528" s="4"/>
-      <c r="N528" s="4"/>
+      <c r="I528" s="4">
+        <v>298</v>
+      </c>
+      <c r="J528" s="4">
+        <v>6610</v>
+      </c>
+      <c r="K528" s="4">
+        <v>10</v>
+      </c>
+      <c r="L528" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="M528" s="117" t="s">
+        <v>675</v>
+      </c>
+      <c r="N528" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O528" s="9"/>
       <c r="P528" s="4"/>
       <c r="Q528" s="4"/>
@@ -28086,86 +28185,183 @@
       <c r="T528" s="9"/>
     </row>
     <row r="529" spans="1:20" ht="15" customHeight="1">
-      <c r="A529" s="4"/>
-      <c r="B529" s="73"/>
-      <c r="C529" s="4"/>
-      <c r="D529" s="4"/>
+      <c r="A529" s="117" t="s">
+        <v>669</v>
+      </c>
+      <c r="B529" s="110" t="s">
+        <v>672</v>
+      </c>
+      <c r="C529" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D529" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E529" s="9"/>
-      <c r="F529" s="4"/>
-      <c r="G529" s="4"/>
+      <c r="F529" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G529" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H529" s="4"/>
-      <c r="I529" s="4"/>
-      <c r="J529" s="4"/>
+      <c r="I529" s="4">
+        <v>298</v>
+      </c>
+      <c r="J529" s="4">
+        <f>P529*J526*1000</f>
+        <v>975371532.84670854</v>
+      </c>
       <c r="K529" s="4"/>
-      <c r="L529" s="4"/>
-      <c r="M529" s="4"/>
-      <c r="N529" s="4"/>
+      <c r="L529" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M529" s="117" t="s">
+        <v>676</v>
+      </c>
+      <c r="N529" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O529" s="9"/>
-      <c r="P529" s="4"/>
+      <c r="P529" s="4">
+        <v>133.06569343065601</v>
+      </c>
       <c r="Q529" s="4"/>
       <c r="R529" s="9"/>
       <c r="S529" s="9"/>
       <c r="T529" s="9"/>
     </row>
     <row r="530" spans="1:20" ht="15" customHeight="1">
-      <c r="A530" s="4"/>
-      <c r="B530" s="73"/>
-      <c r="C530" s="4"/>
-      <c r="D530" s="4"/>
+      <c r="A530" s="117" t="s">
+        <v>670</v>
+      </c>
+      <c r="B530" s="110" t="s">
+        <v>673</v>
+      </c>
+      <c r="C530" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D530" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E530" s="9"/>
-      <c r="F530" s="4"/>
-      <c r="G530" s="4"/>
+      <c r="F530" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G530" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H530" s="4"/>
-      <c r="I530" s="4"/>
-      <c r="J530" s="4"/>
+      <c r="I530" s="4">
+        <v>298</v>
+      </c>
+      <c r="J530" s="4">
+        <f t="shared" ref="J530:J531" si="15">P530*J527*1000</f>
+        <v>946032116.78831685</v>
+      </c>
       <c r="K530" s="4"/>
-      <c r="L530" s="4"/>
-      <c r="M530" s="4"/>
-      <c r="N530" s="4"/>
+      <c r="L530" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M530" s="117" t="s">
+        <v>676</v>
+      </c>
+      <c r="N530" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O530" s="9"/>
-      <c r="P530" s="4"/>
+      <c r="P530" s="4">
+        <v>134.379562043795</v>
+      </c>
       <c r="Q530" s="4"/>
       <c r="R530" s="9"/>
       <c r="S530" s="9"/>
       <c r="T530" s="9"/>
     </row>
     <row r="531" spans="1:20" ht="15" customHeight="1">
-      <c r="A531" s="4"/>
-      <c r="B531" s="73"/>
-      <c r="C531" s="4"/>
-      <c r="D531" s="4"/>
+      <c r="A531" s="117" t="s">
+        <v>671</v>
+      </c>
+      <c r="B531" s="110" t="s">
+        <v>674</v>
+      </c>
+      <c r="C531" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D531" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E531" s="9"/>
-      <c r="F531" s="4"/>
-      <c r="G531" s="4"/>
+      <c r="F531" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G531" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H531" s="4"/>
-      <c r="I531" s="4"/>
-      <c r="J531" s="4"/>
+      <c r="I531" s="4">
+        <v>298</v>
+      </c>
+      <c r="J531" s="4">
+        <f t="shared" si="15"/>
+        <v>988122627.73722279</v>
+      </c>
       <c r="K531" s="4"/>
-      <c r="L531" s="4"/>
-      <c r="M531" s="4"/>
-      <c r="N531" s="4"/>
+      <c r="L531" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M531" s="117" t="s">
+        <v>676</v>
+      </c>
+      <c r="N531" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O531" s="9"/>
-      <c r="P531" s="4"/>
+      <c r="P531" s="4">
+        <v>149.48905109488999</v>
+      </c>
       <c r="Q531" s="4"/>
       <c r="R531" s="9"/>
       <c r="S531" s="9"/>
       <c r="T531" s="9"/>
     </row>
     <row r="532" spans="1:20" ht="15" customHeight="1">
-      <c r="A532" s="4"/>
-      <c r="B532" s="73"/>
-      <c r="C532" s="4"/>
-      <c r="D532" s="4"/>
+      <c r="A532" s="117" t="s">
+        <v>669</v>
+      </c>
+      <c r="B532" s="110" t="s">
+        <v>672</v>
+      </c>
+      <c r="C532" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D532" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E532" s="9"/>
-      <c r="F532" s="4"/>
-      <c r="G532" s="4"/>
+      <c r="F532" s="117" t="s">
+        <v>170</v>
+      </c>
+      <c r="G532" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H532" s="4"/>
-      <c r="I532" s="4"/>
-      <c r="J532" s="4"/>
+      <c r="I532" s="4">
+        <v>298</v>
+      </c>
+      <c r="J532" s="4">
+        <v>26</v>
+      </c>
       <c r="K532" s="4"/>
-      <c r="L532" s="4"/>
-      <c r="M532" s="4"/>
-      <c r="N532" s="4"/>
+      <c r="L532" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M532" s="117" t="s">
+        <v>676</v>
+      </c>
+      <c r="N532" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O532" s="9"/>
       <c r="P532" s="4"/>
       <c r="Q532" s="85"/>
@@ -28174,20 +28370,42 @@
       <c r="T532" s="9"/>
     </row>
     <row r="533" spans="1:20" ht="15" customHeight="1">
-      <c r="A533" s="4"/>
-      <c r="B533" s="73"/>
-      <c r="C533" s="4"/>
-      <c r="D533" s="4"/>
+      <c r="A533" s="117" t="s">
+        <v>670</v>
+      </c>
+      <c r="B533" s="110" t="s">
+        <v>673</v>
+      </c>
+      <c r="C533" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D533" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E533" s="9"/>
-      <c r="F533" s="4"/>
-      <c r="G533" s="4"/>
+      <c r="F533" s="117" t="s">
+        <v>246</v>
+      </c>
+      <c r="G533" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H533" s="4"/>
-      <c r="I533" s="4"/>
-      <c r="J533" s="4"/>
+      <c r="I533" s="4">
+        <v>298</v>
+      </c>
+      <c r="J533" s="4">
+        <v>50</v>
+      </c>
       <c r="K533" s="4"/>
-      <c r="L533" s="4"/>
-      <c r="M533" s="4"/>
-      <c r="N533" s="4"/>
+      <c r="L533" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M533" s="117" t="s">
+        <v>676</v>
+      </c>
+      <c r="N533" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O533" s="9"/>
       <c r="P533" s="4"/>
       <c r="Q533" s="85"/>
@@ -28196,20 +28414,42 @@
       <c r="T533" s="9"/>
     </row>
     <row r="534" spans="1:20" ht="15" customHeight="1">
-      <c r="A534" s="4"/>
-      <c r="B534" s="73"/>
-      <c r="C534" s="4"/>
-      <c r="D534" s="4"/>
+      <c r="A534" s="117" t="s">
+        <v>671</v>
+      </c>
+      <c r="B534" s="110" t="s">
+        <v>674</v>
+      </c>
+      <c r="C534" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D534" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E534" s="9"/>
-      <c r="F534" s="4"/>
-      <c r="G534" s="4"/>
+      <c r="F534" s="117" t="s">
+        <v>246</v>
+      </c>
+      <c r="G534" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H534" s="4"/>
-      <c r="I534" s="4"/>
-      <c r="J534" s="4"/>
+      <c r="I534" s="4">
+        <v>298</v>
+      </c>
+      <c r="J534" s="4">
+        <v>50</v>
+      </c>
       <c r="K534" s="4"/>
-      <c r="L534" s="4"/>
-      <c r="M534" s="4"/>
-      <c r="N534" s="4"/>
+      <c r="L534" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M534" s="117" t="s">
+        <v>676</v>
+      </c>
+      <c r="N534" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O534" s="9"/>
       <c r="P534" s="4"/>
       <c r="Q534" s="85"/>
@@ -28218,20 +28458,42 @@
       <c r="T534" s="9"/>
     </row>
     <row r="535" spans="1:20" ht="15" customHeight="1">
-      <c r="A535" s="4"/>
-      <c r="B535" s="73"/>
-      <c r="C535" s="4"/>
-      <c r="D535" s="4"/>
+      <c r="A535" s="117" t="s">
+        <v>669</v>
+      </c>
+      <c r="B535" s="110" t="s">
+        <v>672</v>
+      </c>
+      <c r="C535" s="117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D535" s="117" t="s">
+        <v>119</v>
+      </c>
       <c r="E535" s="9"/>
-      <c r="F535" s="4"/>
-      <c r="G535" s="4"/>
+      <c r="F535" s="117" t="s">
+        <v>189</v>
+      </c>
+      <c r="G535" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H535" s="4"/>
-      <c r="I535" s="4"/>
-      <c r="J535" s="4"/>
+      <c r="I535" s="4">
+        <v>298</v>
+      </c>
+      <c r="J535" s="106">
+        <v>1640000000</v>
+      </c>
       <c r="K535" s="4"/>
-      <c r="L535" s="4"/>
-      <c r="M535" s="4"/>
-      <c r="N535" s="4"/>
+      <c r="L535" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M535" s="117" t="s">
+        <v>676</v>
+      </c>
+      <c r="N535" s="117" t="s">
+        <v>677</v>
+      </c>
       <c r="O535" s="9"/>
       <c r="P535" s="4"/>
       <c r="Q535" s="85"/>
@@ -35347,6 +35609,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -35361,11 +35628,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.actamat.2016.12.021`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E146D057-15B5-4142-A9B7-8DE1F78E3BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254F37FF-E206-8D43-AC17-B8FEDE1FE61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="3300" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8900" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4636" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4734" uniqueCount="690">
   <si>
     <r>
       <rPr>
@@ -2164,6 +2164,42 @@
   </si>
   <si>
     <t>10.1016/j.jmrt.2024.12.204</t>
+  </si>
+  <si>
+    <t>Gd20Dy20Er20Ho20Tb20</t>
+  </si>
+  <si>
+    <t>Gd25Er25Ho25Tb25</t>
+  </si>
+  <si>
+    <t>Dy25Er25Ho25Tb25</t>
+  </si>
+  <si>
+    <t>ErHoTb</t>
+  </si>
+  <si>
+    <t>HCP+?</t>
+  </si>
+  <si>
+    <t>the unidentified phase had trigonal symmetry</t>
+  </si>
+  <si>
+    <t>neel temperature</t>
+  </si>
+  <si>
+    <t>peak magnetic entropy change</t>
+  </si>
+  <si>
+    <t>5T</t>
+  </si>
+  <si>
+    <t>3T</t>
+  </si>
+  <si>
+    <t>J/kgK</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2016.12.021</t>
   </si>
 </sst>
 </file>
@@ -3313,6 +3349,57 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3372,57 +3459,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4586,8 +4622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A511" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N538" sqref="N538"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A526" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N554" sqref="N554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -4644,19 +4680,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="130"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="137"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="151"/>
+      <c r="M2" s="151"/>
+      <c r="N2" s="154"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -4672,17 +4708,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="141"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="155"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="157"/>
+      <c r="K3" s="157"/>
+      <c r="L3" s="155"/>
+      <c r="M3" s="155"/>
+      <c r="N3" s="158"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -4723,43 +4759,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="159" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="144" t="s">
+      <c r="D5" s="161" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="161" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="161" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="144" t="s">
+      <c r="G5" s="161" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="145" t="s">
+      <c r="H5" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="144" t="s">
+      <c r="I5" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="144" t="s">
+      <c r="J5" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="144" t="s">
+      <c r="K5" s="161" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="144" t="s">
+      <c r="L5" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="144" t="s">
+      <c r="M5" s="161" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="144" t="s">
+      <c r="N5" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="149" t="s">
+      <c r="O5" s="129" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -4775,19 +4811,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="150"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="160"/>
+      <c r="F6" s="160"/>
+      <c r="G6" s="160"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="164"/>
+      <c r="J6" s="165"/>
+      <c r="K6" s="165"/>
+      <c r="L6" s="160"/>
+      <c r="M6" s="160"/>
+      <c r="N6" s="160"/>
+      <c r="O6" s="130"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -4837,7 +4873,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="151"/>
+      <c r="O7" s="131"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -4852,35 +4888,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="153"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="155" t="s">
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="156"/>
-      <c r="H8" s="156"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="158"/>
-      <c r="K8" s="158"/>
-      <c r="L8" s="159"/>
-      <c r="M8" s="160" t="s">
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="161"/>
+      <c r="N8" s="141"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="162" t="s">
+      <c r="P8" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="163"/>
-      <c r="R8" s="164"/>
-      <c r="S8" s="164"/>
-      <c r="T8" s="165"/>
+      <c r="Q8" s="143"/>
+      <c r="R8" s="144"/>
+      <c r="S8" s="144"/>
+      <c r="T8" s="145"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="38" t="s">
@@ -28503,19 +28539,37 @@
     </row>
     <row r="536" spans="1:20" ht="15" customHeight="1">
       <c r="A536" s="4"/>
-      <c r="B536" s="73"/>
-      <c r="C536" s="4"/>
-      <c r="D536" s="4"/>
+      <c r="B536" s="110" t="s">
+        <v>678</v>
+      </c>
+      <c r="C536" s="117" t="s">
+        <v>349</v>
+      </c>
+      <c r="D536" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E536" s="9"/>
-      <c r="F536" s="4"/>
-      <c r="G536" s="4"/>
+      <c r="F536" s="117" t="s">
+        <v>684</v>
+      </c>
+      <c r="G536" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H536" s="4"/>
       <c r="I536" s="4"/>
-      <c r="J536" s="4"/>
+      <c r="J536" s="4">
+        <v>186</v>
+      </c>
       <c r="K536" s="4"/>
-      <c r="L536" s="4"/>
-      <c r="M536" s="4"/>
-      <c r="N536" s="4"/>
+      <c r="L536" s="117" t="s">
+        <v>249</v>
+      </c>
+      <c r="M536" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N536" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O536" s="9"/>
       <c r="P536" s="4"/>
       <c r="Q536" s="85"/>
@@ -28525,19 +28579,39 @@
     </row>
     <row r="537" spans="1:20" ht="15" customHeight="1">
       <c r="A537" s="4"/>
-      <c r="B537" s="73"/>
-      <c r="C537" s="4"/>
-      <c r="D537" s="4"/>
-      <c r="E537" s="9"/>
-      <c r="F537" s="4"/>
-      <c r="G537" s="4"/>
+      <c r="B537" s="110" t="s">
+        <v>679</v>
+      </c>
+      <c r="C537" s="117" t="s">
+        <v>682</v>
+      </c>
+      <c r="D537" s="117" t="s">
+        <v>113</v>
+      </c>
+      <c r="E537" s="119" t="s">
+        <v>683</v>
+      </c>
+      <c r="F537" s="117" t="s">
+        <v>684</v>
+      </c>
+      <c r="G537" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H537" s="4"/>
       <c r="I537" s="4"/>
-      <c r="J537" s="4"/>
+      <c r="J537" s="4">
+        <v>139</v>
+      </c>
       <c r="K537" s="4"/>
-      <c r="L537" s="4"/>
-      <c r="M537" s="4"/>
-      <c r="N537" s="4"/>
+      <c r="L537" s="117" t="s">
+        <v>249</v>
+      </c>
+      <c r="M537" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N537" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O537" s="9"/>
       <c r="P537" s="4"/>
       <c r="Q537" s="4"/>
@@ -28547,19 +28621,39 @@
     </row>
     <row r="538" spans="1:20" ht="15" customHeight="1">
       <c r="A538" s="4"/>
-      <c r="B538" s="73"/>
-      <c r="C538" s="4"/>
-      <c r="D538" s="4"/>
-      <c r="E538" s="9"/>
-      <c r="F538" s="4"/>
-      <c r="G538" s="4"/>
+      <c r="B538" s="110" t="s">
+        <v>680</v>
+      </c>
+      <c r="C538" s="117" t="s">
+        <v>682</v>
+      </c>
+      <c r="D538" s="117" t="s">
+        <v>113</v>
+      </c>
+      <c r="E538" s="119" t="s">
+        <v>683</v>
+      </c>
+      <c r="F538" s="117" t="s">
+        <v>684</v>
+      </c>
+      <c r="G538" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H538" s="4"/>
       <c r="I538" s="4"/>
-      <c r="J538" s="4"/>
+      <c r="J538" s="4">
+        <v>52</v>
+      </c>
       <c r="K538" s="4"/>
-      <c r="L538" s="4"/>
-      <c r="M538" s="4"/>
-      <c r="N538" s="4"/>
+      <c r="L538" s="117" t="s">
+        <v>249</v>
+      </c>
+      <c r="M538" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N538" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O538" s="9"/>
       <c r="P538" s="4"/>
       <c r="Q538" s="4"/>
@@ -28569,19 +28663,39 @@
     </row>
     <row r="539" spans="1:20" ht="15" customHeight="1">
       <c r="A539" s="4"/>
-      <c r="B539" s="73"/>
-      <c r="C539" s="4"/>
-      <c r="D539" s="4"/>
-      <c r="E539" s="9"/>
-      <c r="F539" s="4"/>
-      <c r="G539" s="4"/>
+      <c r="B539" s="110" t="s">
+        <v>681</v>
+      </c>
+      <c r="C539" s="117" t="s">
+        <v>682</v>
+      </c>
+      <c r="D539" s="117" t="s">
+        <v>113</v>
+      </c>
+      <c r="E539" s="119" t="s">
+        <v>683</v>
+      </c>
+      <c r="F539" s="117" t="s">
+        <v>684</v>
+      </c>
+      <c r="G539" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H539" s="4"/>
       <c r="I539" s="4"/>
-      <c r="J539" s="4"/>
+      <c r="J539" s="4">
+        <v>88</v>
+      </c>
       <c r="K539" s="4"/>
-      <c r="L539" s="4"/>
-      <c r="M539" s="4"/>
-      <c r="N539" s="4"/>
+      <c r="L539" s="117" t="s">
+        <v>249</v>
+      </c>
+      <c r="M539" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N539" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O539" s="9"/>
       <c r="P539" s="4"/>
       <c r="Q539" s="4"/>
@@ -28591,19 +28705,39 @@
     </row>
     <row r="540" spans="1:20" ht="15" customHeight="1">
       <c r="A540" s="4"/>
-      <c r="B540" s="73"/>
-      <c r="C540" s="4"/>
-      <c r="D540" s="4"/>
+      <c r="B540" s="110" t="s">
+        <v>678</v>
+      </c>
+      <c r="C540" s="117" t="s">
+        <v>349</v>
+      </c>
+      <c r="D540" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E540" s="9"/>
-      <c r="F540" s="4"/>
-      <c r="G540" s="4"/>
-      <c r="H540" s="4"/>
+      <c r="F540" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="G540" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H540" s="4" t="s">
+        <v>686</v>
+      </c>
       <c r="I540" s="4"/>
-      <c r="J540" s="4"/>
+      <c r="J540" s="4">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="K540" s="4"/>
-      <c r="L540" s="4"/>
-      <c r="M540" s="4"/>
-      <c r="N540" s="4"/>
+      <c r="L540" s="117" t="s">
+        <v>688</v>
+      </c>
+      <c r="M540" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N540" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O540" s="9"/>
       <c r="P540" s="4"/>
       <c r="Q540" s="4"/>
@@ -28613,19 +28747,41 @@
     </row>
     <row r="541" spans="1:20" ht="15" customHeight="1">
       <c r="A541" s="4"/>
-      <c r="B541" s="73"/>
-      <c r="C541" s="4"/>
-      <c r="D541" s="4"/>
-      <c r="E541" s="9"/>
-      <c r="F541" s="4"/>
-      <c r="G541" s="4"/>
-      <c r="H541" s="4"/>
+      <c r="B541" s="110" t="s">
+        <v>679</v>
+      </c>
+      <c r="C541" s="117" t="s">
+        <v>682</v>
+      </c>
+      <c r="D541" s="117" t="s">
+        <v>113</v>
+      </c>
+      <c r="E541" s="119" t="s">
+        <v>683</v>
+      </c>
+      <c r="F541" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="G541" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H541" s="4" t="s">
+        <v>686</v>
+      </c>
       <c r="I541" s="4"/>
-      <c r="J541" s="4"/>
+      <c r="J541" s="4">
+        <v>4.8</v>
+      </c>
       <c r="K541" s="4"/>
-      <c r="L541" s="4"/>
-      <c r="M541" s="4"/>
-      <c r="N541" s="4"/>
+      <c r="L541" s="117" t="s">
+        <v>688</v>
+      </c>
+      <c r="M541" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N541" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O541" s="9"/>
       <c r="P541" s="4"/>
       <c r="Q541" s="4"/>
@@ -28635,19 +28791,41 @@
     </row>
     <row r="542" spans="1:20" ht="15" customHeight="1">
       <c r="A542" s="4"/>
-      <c r="B542" s="73"/>
-      <c r="C542" s="4"/>
-      <c r="D542" s="4"/>
-      <c r="E542" s="9"/>
-      <c r="F542" s="4"/>
-      <c r="G542" s="4"/>
-      <c r="H542" s="4"/>
+      <c r="B542" s="110" t="s">
+        <v>680</v>
+      </c>
+      <c r="C542" s="117" t="s">
+        <v>682</v>
+      </c>
+      <c r="D542" s="117" t="s">
+        <v>113</v>
+      </c>
+      <c r="E542" s="119" t="s">
+        <v>683</v>
+      </c>
+      <c r="F542" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="G542" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H542" s="117" t="s">
+        <v>687</v>
+      </c>
       <c r="I542" s="4"/>
-      <c r="J542" s="4"/>
+      <c r="J542" s="4">
+        <v>0.65</v>
+      </c>
       <c r="K542" s="4"/>
-      <c r="L542" s="4"/>
-      <c r="M542" s="4"/>
-      <c r="N542" s="4"/>
+      <c r="L542" s="117" t="s">
+        <v>688</v>
+      </c>
+      <c r="M542" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N542" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O542" s="9"/>
       <c r="P542" s="4"/>
       <c r="Q542" s="4"/>
@@ -28657,19 +28835,41 @@
     </row>
     <row r="543" spans="1:20" ht="15" customHeight="1">
       <c r="A543" s="4"/>
-      <c r="B543" s="73"/>
-      <c r="C543" s="4"/>
-      <c r="D543" s="4"/>
-      <c r="E543" s="9"/>
-      <c r="F543" s="4"/>
-      <c r="G543" s="4"/>
-      <c r="H543" s="4"/>
+      <c r="B543" s="110" t="s">
+        <v>681</v>
+      </c>
+      <c r="C543" s="117" t="s">
+        <v>682</v>
+      </c>
+      <c r="D543" s="117" t="s">
+        <v>113</v>
+      </c>
+      <c r="E543" s="119" t="s">
+        <v>683</v>
+      </c>
+      <c r="F543" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="G543" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H543" s="117" t="s">
+        <v>687</v>
+      </c>
       <c r="I543" s="4"/>
-      <c r="J543" s="4"/>
+      <c r="J543" s="4">
+        <v>3</v>
+      </c>
       <c r="K543" s="4"/>
-      <c r="L543" s="4"/>
-      <c r="M543" s="4"/>
-      <c r="N543" s="4"/>
+      <c r="L543" s="117" t="s">
+        <v>688</v>
+      </c>
+      <c r="M543" s="117" t="s">
+        <v>120</v>
+      </c>
+      <c r="N543" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O543" s="9"/>
       <c r="P543" s="4"/>
       <c r="Q543" s="4"/>
@@ -28679,19 +28879,39 @@
     </row>
     <row r="544" spans="1:20" ht="15" customHeight="1">
       <c r="A544" s="4"/>
-      <c r="B544" s="73"/>
-      <c r="C544" s="4"/>
-      <c r="D544" s="4"/>
+      <c r="B544" s="110" t="s">
+        <v>678</v>
+      </c>
+      <c r="C544" s="117" t="s">
+        <v>349</v>
+      </c>
+      <c r="D544" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E544" s="9"/>
-      <c r="F544" s="4"/>
-      <c r="G544" s="4"/>
+      <c r="F544" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="G544" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H544" s="4"/>
-      <c r="I544" s="4"/>
-      <c r="J544" s="4"/>
+      <c r="I544" s="4">
+        <v>298</v>
+      </c>
+      <c r="J544" s="106">
+        <v>258000000</v>
+      </c>
       <c r="K544" s="4"/>
-      <c r="L544" s="4"/>
-      <c r="M544" s="4"/>
-      <c r="N544" s="4"/>
+      <c r="L544" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M544" s="117" t="s">
+        <v>106</v>
+      </c>
+      <c r="N544" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O544" s="9"/>
       <c r="P544" s="4"/>
       <c r="Q544" s="4"/>
@@ -28701,19 +28921,39 @@
     </row>
     <row r="545" spans="1:20" ht="15" customHeight="1">
       <c r="A545" s="4"/>
-      <c r="B545" s="73"/>
-      <c r="C545" s="4"/>
-      <c r="D545" s="4"/>
+      <c r="B545" s="110" t="s">
+        <v>678</v>
+      </c>
+      <c r="C545" s="117" t="s">
+        <v>349</v>
+      </c>
+      <c r="D545" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E545" s="9"/>
-      <c r="F545" s="4"/>
-      <c r="G545" s="4"/>
+      <c r="F545" s="117" t="s">
+        <v>189</v>
+      </c>
+      <c r="G545" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H545" s="4"/>
-      <c r="I545" s="4"/>
-      <c r="J545" s="4"/>
+      <c r="I545" s="4">
+        <v>298</v>
+      </c>
+      <c r="J545" s="106">
+        <v>759000000</v>
+      </c>
       <c r="K545" s="4"/>
-      <c r="L545" s="4"/>
-      <c r="M545" s="4"/>
-      <c r="N545" s="4"/>
+      <c r="L545" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M545" s="117" t="s">
+        <v>106</v>
+      </c>
+      <c r="N545" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O545" s="9"/>
       <c r="P545" s="4"/>
       <c r="Q545" s="4"/>
@@ -28723,19 +28963,39 @@
     </row>
     <row r="546" spans="1:20" ht="15" customHeight="1">
       <c r="A546" s="4"/>
-      <c r="B546" s="73"/>
-      <c r="C546" s="4"/>
-      <c r="D546" s="4"/>
+      <c r="B546" s="110" t="s">
+        <v>678</v>
+      </c>
+      <c r="C546" s="117" t="s">
+        <v>349</v>
+      </c>
+      <c r="D546" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E546" s="9"/>
-      <c r="F546" s="4"/>
-      <c r="G546" s="4"/>
+      <c r="F546" s="117" t="s">
+        <v>170</v>
+      </c>
+      <c r="G546" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H546" s="4"/>
-      <c r="I546" s="4"/>
-      <c r="J546" s="4"/>
+      <c r="I546" s="4">
+        <v>298</v>
+      </c>
+      <c r="J546" s="4">
+        <v>24.8</v>
+      </c>
       <c r="K546" s="4"/>
-      <c r="L546" s="4"/>
-      <c r="M546" s="4"/>
-      <c r="N546" s="4"/>
+      <c r="L546" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="M546" s="117" t="s">
+        <v>106</v>
+      </c>
+      <c r="N546" s="117" t="s">
+        <v>689</v>
+      </c>
       <c r="O546" s="9"/>
       <c r="P546" s="4"/>
       <c r="Q546" s="4"/>
@@ -35609,11 +35869,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -35628,6 +35883,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.jallcom.2020.158357`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254F37FF-E206-8D43-AC17-B8FEDE1FE61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6F7627-5B56-6F4F-940A-B50520323B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8900" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6080" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4734" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4739" uniqueCount="693">
   <si>
     <r>
       <rPr>
@@ -2200,6 +2200,15 @@
   </si>
   <si>
     <t>10.1016/j.actamat.2016.12.021</t>
+  </si>
+  <si>
+    <t>MgAlTiFeNi</t>
+  </si>
+  <si>
+    <t>mechanical alloying by ball milling under Ar for 30h at 200rpm</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2020.158357</t>
   </si>
 </sst>
 </file>
@@ -3349,57 +3358,6 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3459,6 +3417,57 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4623,7 +4632,7 @@
   <dimension ref="A1:T859"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A526" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N554" sqref="N554"/>
+      <selection activeCell="G554" sqref="G554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -4680,19 +4689,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="146" t="s">
+      <c r="D2" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="147"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="151"/>
-      <c r="M2" s="151"/>
-      <c r="N2" s="154"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="137"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -4708,17 +4717,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="155"/>
-      <c r="M3" s="155"/>
-      <c r="N3" s="158"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="141"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -4759,43 +4768,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="142" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="161" t="s">
+      <c r="D5" s="144" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="161" t="s">
+      <c r="E5" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="161" t="s">
+      <c r="F5" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="161" t="s">
+      <c r="G5" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="162" t="s">
+      <c r="H5" s="145" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="161" t="s">
+      <c r="I5" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="161" t="s">
+      <c r="J5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="161" t="s">
+      <c r="K5" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="161" t="s">
+      <c r="L5" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="161" t="s">
+      <c r="M5" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="161" t="s">
+      <c r="N5" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="129" t="s">
+      <c r="O5" s="149" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -4811,19 +4820,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="160"/>
-      <c r="D6" s="160"/>
-      <c r="E6" s="160"/>
-      <c r="F6" s="160"/>
-      <c r="G6" s="160"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="164"/>
-      <c r="J6" s="165"/>
-      <c r="K6" s="165"/>
-      <c r="L6" s="160"/>
-      <c r="M6" s="160"/>
-      <c r="N6" s="160"/>
-      <c r="O6" s="130"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="147"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="150"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -4873,7 +4882,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="131"/>
+      <c r="O7" s="151"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -4888,35 +4897,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="152" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="135" t="s">
+      <c r="C8" s="153"/>
+      <c r="D8" s="153"/>
+      <c r="E8" s="154"/>
+      <c r="F8" s="155" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="137"/>
-      <c r="J8" s="138"/>
-      <c r="K8" s="138"/>
-      <c r="L8" s="139"/>
-      <c r="M8" s="140" t="s">
+      <c r="G8" s="156"/>
+      <c r="H8" s="156"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="158"/>
+      <c r="L8" s="159"/>
+      <c r="M8" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="141"/>
+      <c r="N8" s="161"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="142" t="s">
+      <c r="P8" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="143"/>
-      <c r="R8" s="144"/>
-      <c r="S8" s="144"/>
-      <c r="T8" s="145"/>
+      <c r="Q8" s="163"/>
+      <c r="R8" s="164"/>
+      <c r="S8" s="164"/>
+      <c r="T8" s="165"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="38" t="s">
@@ -29005,10 +29014,18 @@
     </row>
     <row r="547" spans="1:20" ht="15" customHeight="1">
       <c r="A547" s="4"/>
-      <c r="B547" s="73"/>
-      <c r="C547" s="4"/>
-      <c r="D547" s="4"/>
-      <c r="E547" s="9"/>
+      <c r="B547" s="110" t="s">
+        <v>690</v>
+      </c>
+      <c r="C547" s="117" t="s">
+        <v>358</v>
+      </c>
+      <c r="D547" s="117" t="s">
+        <v>173</v>
+      </c>
+      <c r="E547" s="119" t="s">
+        <v>691</v>
+      </c>
       <c r="F547" s="4"/>
       <c r="G547" s="4"/>
       <c r="H547" s="4"/>
@@ -29017,7 +29034,9 @@
       <c r="K547" s="4"/>
       <c r="L547" s="4"/>
       <c r="M547" s="4"/>
-      <c r="N547" s="4"/>
+      <c r="N547" s="117" t="s">
+        <v>692</v>
+      </c>
       <c r="O547" s="9"/>
       <c r="P547" s="4"/>
       <c r="Q547" s="4"/>
@@ -35869,6 +35888,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -35883,11 +35907,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msec.2019.110322`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6F7627-5B56-6F4F-940A-B50520323B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7400716D-863A-C245-8F70-1C3E64A14149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6080" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8840" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4739" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4783" uniqueCount="701">
   <si>
     <r>
       <rPr>
@@ -2209,6 +2209,30 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2020.158357</t>
+  </si>
+  <si>
+    <t>10.1016/j.msec.2019.110322</t>
+  </si>
+  <si>
+    <t>TiNbTaZr</t>
+  </si>
+  <si>
+    <t>TiNbTaZrV</t>
+  </si>
+  <si>
+    <t>TiNbTaZrMo</t>
+  </si>
+  <si>
+    <t>TiNbTaZrW</t>
+  </si>
+  <si>
+    <t>TiZrHfCr0.2Mo</t>
+  </si>
+  <si>
+    <t>TiZrHfCo0.07Cr0.07Mo</t>
+  </si>
+  <si>
+    <t>BCC+laves</t>
   </si>
 </sst>
 </file>
@@ -3358,6 +3382,57 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3417,57 +3492,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4631,8 +4655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A526" zoomScale="86" workbookViewId="0">
-      <selection activeCell="G554" sqref="G554"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A540" zoomScale="86" workbookViewId="0">
+      <selection activeCell="H564" sqref="H564"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -4689,19 +4713,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="130"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="137"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="151"/>
+      <c r="M2" s="151"/>
+      <c r="N2" s="154"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -4717,17 +4741,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="141"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="155"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="157"/>
+      <c r="K3" s="157"/>
+      <c r="L3" s="155"/>
+      <c r="M3" s="155"/>
+      <c r="N3" s="158"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -4768,43 +4792,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="159" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="144" t="s">
+      <c r="D5" s="161" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="161" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="161" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="144" t="s">
+      <c r="G5" s="161" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="145" t="s">
+      <c r="H5" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="144" t="s">
+      <c r="I5" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="144" t="s">
+      <c r="J5" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="144" t="s">
+      <c r="K5" s="161" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="144" t="s">
+      <c r="L5" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="144" t="s">
+      <c r="M5" s="161" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="144" t="s">
+      <c r="N5" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="149" t="s">
+      <c r="O5" s="129" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -4820,19 +4844,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="150"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="160"/>
+      <c r="F6" s="160"/>
+      <c r="G6" s="160"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="164"/>
+      <c r="J6" s="165"/>
+      <c r="K6" s="165"/>
+      <c r="L6" s="160"/>
+      <c r="M6" s="160"/>
+      <c r="N6" s="160"/>
+      <c r="O6" s="130"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -4882,7 +4906,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="151"/>
+      <c r="O7" s="131"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -4897,35 +4921,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="153"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="155" t="s">
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="156"/>
-      <c r="H8" s="156"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="158"/>
-      <c r="K8" s="158"/>
-      <c r="L8" s="159"/>
-      <c r="M8" s="160" t="s">
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="137"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="161"/>
+      <c r="N8" s="141"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="162" t="s">
+      <c r="P8" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="163"/>
-      <c r="R8" s="164"/>
-      <c r="S8" s="164"/>
-      <c r="T8" s="165"/>
+      <c r="Q8" s="143"/>
+      <c r="R8" s="144"/>
+      <c r="S8" s="144"/>
+      <c r="T8" s="145"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1">
       <c r="A9" s="38" t="s">
@@ -29046,132 +29070,292 @@
     </row>
     <row r="548" spans="1:20" ht="15" customHeight="1">
       <c r="A548" s="4"/>
-      <c r="B548" s="73"/>
+      <c r="B548" s="110" t="s">
+        <v>694</v>
+      </c>
       <c r="C548" s="4"/>
-      <c r="D548" s="4"/>
+      <c r="D548" s="117" t="s">
+        <v>238</v>
+      </c>
       <c r="E548" s="9"/>
-      <c r="F548" s="4"/>
-      <c r="G548" s="4"/>
+      <c r="F548" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G548" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H548" s="4"/>
-      <c r="I548" s="4"/>
-      <c r="J548" s="4"/>
-      <c r="K548" s="4"/>
-      <c r="L548" s="4"/>
-      <c r="M548" s="4"/>
-      <c r="N548" s="4"/>
+      <c r="I548" s="4">
+        <v>298</v>
+      </c>
+      <c r="J548" s="70">
+        <f t="shared" ref="J548:K553" si="16">P548*9807000</f>
+        <v>3069591000</v>
+      </c>
+      <c r="K548" s="70">
+        <f t="shared" si="16"/>
+        <v>86301600</v>
+      </c>
+      <c r="L548" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M548" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="N548" s="117" t="s">
+        <v>693</v>
+      </c>
       <c r="O548" s="9"/>
-      <c r="P548" s="4"/>
-      <c r="Q548" s="4"/>
+      <c r="P548" s="4">
+        <v>313</v>
+      </c>
+      <c r="Q548" s="4">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="R548" s="9"/>
       <c r="S548" s="9"/>
       <c r="T548" s="9"/>
     </row>
     <row r="549" spans="1:20" ht="15" customHeight="1">
       <c r="A549" s="4"/>
-      <c r="B549" s="73"/>
+      <c r="B549" s="110" t="s">
+        <v>695</v>
+      </c>
       <c r="C549" s="4"/>
-      <c r="D549" s="4"/>
+      <c r="D549" s="117" t="s">
+        <v>238</v>
+      </c>
       <c r="E549" s="9"/>
-      <c r="F549" s="4"/>
-      <c r="G549" s="4"/>
+      <c r="F549" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G549" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H549" s="4"/>
-      <c r="I549" s="4"/>
-      <c r="J549" s="4"/>
-      <c r="K549" s="4"/>
-      <c r="L549" s="4"/>
-      <c r="M549" s="4"/>
-      <c r="N549" s="4"/>
+      <c r="I549" s="4">
+        <v>298</v>
+      </c>
+      <c r="J549" s="70">
+        <f t="shared" si="16"/>
+        <v>4217010000</v>
+      </c>
+      <c r="K549" s="70">
+        <f t="shared" si="16"/>
+        <v>49035000</v>
+      </c>
+      <c r="L549" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M549" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="N549" s="117" t="s">
+        <v>693</v>
+      </c>
       <c r="O549" s="9"/>
-      <c r="P549" s="4"/>
-      <c r="Q549" s="4"/>
+      <c r="P549" s="4">
+        <v>430</v>
+      </c>
+      <c r="Q549" s="4">
+        <v>5</v>
+      </c>
       <c r="R549" s="9"/>
       <c r="S549" s="9"/>
       <c r="T549" s="9"/>
     </row>
     <row r="550" spans="1:20" ht="15" customHeight="1">
       <c r="A550" s="4"/>
-      <c r="B550" s="73"/>
+      <c r="B550" s="110" t="s">
+        <v>696</v>
+      </c>
       <c r="C550" s="4"/>
-      <c r="D550" s="4"/>
+      <c r="D550" s="117" t="s">
+        <v>238</v>
+      </c>
       <c r="E550" s="9"/>
-      <c r="F550" s="4"/>
-      <c r="G550" s="4"/>
+      <c r="F550" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G550" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H550" s="4"/>
-      <c r="I550" s="4"/>
-      <c r="J550" s="4"/>
-      <c r="K550" s="4"/>
-      <c r="L550" s="4"/>
-      <c r="M550" s="4"/>
-      <c r="N550" s="4"/>
+      <c r="I550" s="4">
+        <v>298</v>
+      </c>
+      <c r="J550" s="70">
+        <f t="shared" si="16"/>
+        <v>4677939000</v>
+      </c>
+      <c r="K550" s="70">
+        <f t="shared" si="16"/>
+        <v>76494600</v>
+      </c>
+      <c r="L550" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M550" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="N550" s="117" t="s">
+        <v>693</v>
+      </c>
       <c r="O550" s="9"/>
-      <c r="P550" s="4"/>
-      <c r="Q550" s="4"/>
+      <c r="P550" s="4">
+        <v>477</v>
+      </c>
+      <c r="Q550" s="4">
+        <v>7.8</v>
+      </c>
       <c r="R550" s="9"/>
       <c r="S550" s="9"/>
       <c r="T550" s="9"/>
     </row>
     <row r="551" spans="1:20" ht="15" customHeight="1">
       <c r="A551" s="4"/>
-      <c r="B551" s="73"/>
+      <c r="B551" s="110" t="s">
+        <v>697</v>
+      </c>
       <c r="C551" s="4"/>
-      <c r="D551" s="4"/>
+      <c r="D551" s="117" t="s">
+        <v>238</v>
+      </c>
       <c r="E551" s="9"/>
-      <c r="F551" s="4"/>
-      <c r="G551" s="4"/>
+      <c r="F551" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G551" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H551" s="4"/>
-      <c r="I551" s="4"/>
-      <c r="J551" s="4"/>
-      <c r="K551" s="4"/>
-      <c r="L551" s="4"/>
-      <c r="M551" s="4"/>
-      <c r="N551" s="4"/>
+      <c r="I551" s="4">
+        <v>298</v>
+      </c>
+      <c r="J551" s="70">
+        <f t="shared" si="16"/>
+        <v>5452692000</v>
+      </c>
+      <c r="K551" s="70">
+        <f t="shared" si="16"/>
+        <v>61784100</v>
+      </c>
+      <c r="L551" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M551" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="N551" s="117" t="s">
+        <v>693</v>
+      </c>
       <c r="O551" s="9"/>
-      <c r="P551" s="4"/>
-      <c r="Q551" s="4"/>
+      <c r="P551" s="4">
+        <v>556</v>
+      </c>
+      <c r="Q551" s="4">
+        <v>6.3</v>
+      </c>
       <c r="R551" s="9"/>
       <c r="S551" s="9"/>
       <c r="T551" s="9"/>
     </row>
     <row r="552" spans="1:20" ht="15" customHeight="1">
       <c r="A552" s="4"/>
-      <c r="B552" s="73"/>
-      <c r="C552" s="4"/>
-      <c r="D552" s="4"/>
+      <c r="B552" s="110" t="s">
+        <v>698</v>
+      </c>
+      <c r="C552" s="117" t="s">
+        <v>700</v>
+      </c>
+      <c r="D552" s="117" t="s">
+        <v>238</v>
+      </c>
       <c r="E552" s="9"/>
-      <c r="F552" s="4"/>
-      <c r="G552" s="4"/>
+      <c r="F552" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G552" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H552" s="4"/>
-      <c r="I552" s="4"/>
-      <c r="J552" s="4"/>
-      <c r="K552" s="70"/>
-      <c r="L552" s="4"/>
-      <c r="M552" s="4"/>
-      <c r="N552" s="4"/>
+      <c r="I552" s="4">
+        <v>298</v>
+      </c>
+      <c r="J552" s="70">
+        <f t="shared" si="16"/>
+        <v>5207517000</v>
+      </c>
+      <c r="K552" s="70">
+        <f t="shared" si="16"/>
+        <v>107877000</v>
+      </c>
+      <c r="L552" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M552" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="N552" s="117" t="s">
+        <v>693</v>
+      </c>
       <c r="O552" s="9"/>
-      <c r="P552" s="4"/>
-      <c r="Q552" s="4"/>
+      <c r="P552" s="4">
+        <v>531</v>
+      </c>
+      <c r="Q552" s="4">
+        <v>11</v>
+      </c>
       <c r="R552" s="9"/>
       <c r="S552" s="9"/>
       <c r="T552" s="9"/>
     </row>
     <row r="553" spans="1:20" ht="15" customHeight="1">
       <c r="A553" s="4"/>
-      <c r="B553" s="73"/>
-      <c r="C553" s="4"/>
-      <c r="D553" s="4"/>
+      <c r="B553" s="110" t="s">
+        <v>699</v>
+      </c>
+      <c r="C553" s="117" t="s">
+        <v>700</v>
+      </c>
+      <c r="D553" s="117" t="s">
+        <v>238</v>
+      </c>
       <c r="E553" s="9"/>
-      <c r="F553" s="4"/>
-      <c r="G553" s="4"/>
+      <c r="F553" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G553" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H553" s="4"/>
-      <c r="I553" s="4"/>
-      <c r="J553" s="70"/>
-      <c r="K553" s="70"/>
-      <c r="L553" s="4"/>
-      <c r="M553" s="4"/>
-      <c r="N553" s="4"/>
+      <c r="I553" s="4">
+        <v>298</v>
+      </c>
+      <c r="J553" s="70">
+        <f t="shared" si="16"/>
+        <v>5217324000</v>
+      </c>
+      <c r="K553" s="70">
+        <f t="shared" si="16"/>
+        <v>57861300</v>
+      </c>
+      <c r="L553" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M553" s="117" t="s">
+        <v>69</v>
+      </c>
+      <c r="N553" s="117" t="s">
+        <v>693</v>
+      </c>
       <c r="O553" s="9"/>
-      <c r="P553" s="85"/>
-      <c r="Q553" s="4"/>
+      <c r="P553" s="85">
+        <v>532</v>
+      </c>
+      <c r="Q553" s="4">
+        <v>5.9</v>
+      </c>
       <c r="R553" s="9"/>
       <c r="S553" s="9"/>
       <c r="T553" s="9"/>
@@ -35888,11 +36072,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -35907,6 +36086,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2011.01.072`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7400716D-863A-C245-8F70-1C3E64A14149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A1C09A-BF87-4243-B075-F4D41F738D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8840" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4783" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5188" uniqueCount="713">
   <si>
     <r>
       <rPr>
@@ -2233,6 +2233,42 @@
   </si>
   <si>
     <t>BCC+laves</t>
+  </si>
+  <si>
+    <t>AlCoFeMo0.5Ni</t>
+  </si>
+  <si>
+    <t>AlCoCr0.5FeMo0.5Ni</t>
+  </si>
+  <si>
+    <t>AlCoCr1.0FeMo0.5Ni</t>
+  </si>
+  <si>
+    <t>AlCoCr1.5FeMo0.5Ni</t>
+  </si>
+  <si>
+    <t>AlCoCr2.0FeMo0.5Ni</t>
+  </si>
+  <si>
+    <t>Cr0</t>
+  </si>
+  <si>
+    <t>Cr0.5</t>
+  </si>
+  <si>
+    <t>Cr1</t>
+  </si>
+  <si>
+    <t>Cr1.5</t>
+  </si>
+  <si>
+    <t>Cr2</t>
+  </si>
+  <si>
+    <t>B2+sigma</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2011.01.072</t>
   </si>
 </sst>
 </file>
@@ -4655,8 +4691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A540" zoomScale="86" workbookViewId="0">
-      <selection activeCell="H564" sqref="H564"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A552" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N606" sqref="N606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -29089,7 +29125,7 @@
         <v>298</v>
       </c>
       <c r="J548" s="70">
-        <f t="shared" ref="J548:K553" si="16">P548*9807000</f>
+        <f t="shared" ref="J548:K563" si="16">P548*9807000</f>
         <v>3069591000</v>
       </c>
       <c r="K548" s="70">
@@ -29361,1003 +29397,2101 @@
       <c r="T553" s="9"/>
     </row>
     <row r="554" spans="1:20" ht="15" customHeight="1">
-      <c r="A554" s="4"/>
-      <c r="B554" s="73"/>
-      <c r="C554" s="4"/>
-      <c r="D554" s="4"/>
+      <c r="A554" s="117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B554" s="110" t="s">
+        <v>701</v>
+      </c>
+      <c r="C554" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D554" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E554" s="9"/>
-      <c r="F554" s="4"/>
-      <c r="G554" s="4"/>
+      <c r="F554" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G554" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H554" s="4"/>
-      <c r="I554" s="4"/>
-      <c r="J554" s="70"/>
+      <c r="I554" s="4">
+        <v>298</v>
+      </c>
+      <c r="J554" s="70">
+        <f t="shared" si="16"/>
+        <v>5899404651.1627884</v>
+      </c>
       <c r="K554" s="70"/>
-      <c r="L554" s="4"/>
-      <c r="M554" s="4"/>
-      <c r="N554" s="4"/>
+      <c r="L554" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M554" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N554" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O554" s="9"/>
-      <c r="P554" s="85"/>
+      <c r="P554" s="9">
+        <v>601.55038759689899</v>
+      </c>
       <c r="Q554" s="4"/>
-      <c r="R554" s="9"/>
       <c r="S554" s="9"/>
       <c r="T554" s="9"/>
     </row>
     <row r="555" spans="1:20" ht="15" customHeight="1">
-      <c r="A555" s="4"/>
-      <c r="B555" s="73"/>
-      <c r="C555" s="4"/>
-      <c r="D555" s="4"/>
+      <c r="A555" s="117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B555" s="110" t="s">
+        <v>701</v>
+      </c>
+      <c r="C555" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D555" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E555" s="9"/>
-      <c r="F555" s="4"/>
-      <c r="G555" s="4"/>
+      <c r="F555" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G555" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H555" s="4"/>
-      <c r="I555" s="4"/>
-      <c r="J555" s="70"/>
+      <c r="I555" s="4">
+        <v>573</v>
+      </c>
+      <c r="J555" s="70">
+        <f t="shared" si="16"/>
+        <v>5260809302.3255739</v>
+      </c>
       <c r="K555" s="70"/>
-      <c r="L555" s="4"/>
-      <c r="M555" s="4"/>
-      <c r="N555" s="4"/>
+      <c r="L555" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M555" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N555" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O555" s="9"/>
-      <c r="P555" s="85"/>
+      <c r="P555" s="9">
+        <v>536.434108527131</v>
+      </c>
       <c r="Q555" s="4"/>
-      <c r="R555" s="9"/>
       <c r="S555" s="9"/>
       <c r="T555" s="9"/>
     </row>
     <row r="556" spans="1:20" ht="15" customHeight="1">
-      <c r="A556" s="4"/>
-      <c r="B556" s="73"/>
-      <c r="C556" s="4"/>
-      <c r="D556" s="4"/>
+      <c r="A556" s="117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B556" s="110" t="s">
+        <v>701</v>
+      </c>
+      <c r="C556" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D556" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E556" s="9"/>
-      <c r="F556" s="4"/>
-      <c r="G556" s="4"/>
+      <c r="F556" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G556" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H556" s="4"/>
-      <c r="I556" s="4"/>
-      <c r="J556" s="70"/>
+      <c r="I556" s="4">
+        <v>673</v>
+      </c>
+      <c r="J556" s="70">
+        <f t="shared" si="16"/>
+        <v>4909581860.4651089</v>
+      </c>
       <c r="K556" s="70"/>
-      <c r="L556" s="4"/>
-      <c r="M556" s="4"/>
-      <c r="N556" s="4"/>
+      <c r="L556" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M556" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N556" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O556" s="9"/>
-      <c r="P556" s="85"/>
+      <c r="P556" s="9">
+        <v>500.62015503875898</v>
+      </c>
       <c r="Q556" s="4"/>
-      <c r="R556" s="9"/>
       <c r="S556" s="9"/>
       <c r="T556" s="9"/>
     </row>
     <row r="557" spans="1:20" ht="15" customHeight="1">
-      <c r="A557" s="4"/>
-      <c r="B557" s="73"/>
-      <c r="C557" s="4"/>
-      <c r="D557" s="4"/>
+      <c r="A557" s="117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B557" s="110" t="s">
+        <v>701</v>
+      </c>
+      <c r="C557" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D557" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E557" s="9"/>
-      <c r="F557" s="4"/>
-      <c r="G557" s="4"/>
+      <c r="F557" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G557" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H557" s="4"/>
-      <c r="I557" s="4"/>
-      <c r="J557" s="70"/>
+      <c r="I557" s="4">
+        <v>773</v>
+      </c>
+      <c r="J557" s="70">
+        <f t="shared" si="16"/>
+        <v>4909581860.4651089</v>
+      </c>
       <c r="K557" s="4"/>
-      <c r="L557" s="4"/>
-      <c r="M557" s="4"/>
-      <c r="N557" s="4"/>
+      <c r="L557" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M557" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N557" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O557" s="9"/>
-      <c r="P557" s="85"/>
+      <c r="P557" s="9">
+        <v>500.62015503875898</v>
+      </c>
       <c r="Q557" s="4"/>
-      <c r="R557" s="9"/>
       <c r="S557" s="9"/>
       <c r="T557" s="9"/>
     </row>
     <row r="558" spans="1:20" ht="15" customHeight="1">
-      <c r="A558" s="4"/>
-      <c r="B558" s="73"/>
-      <c r="C558" s="4"/>
-      <c r="D558" s="4"/>
+      <c r="A558" s="117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B558" s="110" t="s">
+        <v>701</v>
+      </c>
+      <c r="C558" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D558" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E558" s="9"/>
-      <c r="F558" s="4"/>
-      <c r="G558" s="4"/>
+      <c r="F558" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G558" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H558" s="4"/>
-      <c r="I558" s="4"/>
-      <c r="J558" s="4"/>
+      <c r="I558" s="4">
+        <v>873</v>
+      </c>
+      <c r="J558" s="70">
+        <f t="shared" si="16"/>
+        <v>5047944186.0465059</v>
+      </c>
       <c r="K558" s="4"/>
-      <c r="L558" s="4"/>
-      <c r="M558" s="4"/>
-      <c r="N558" s="4"/>
+      <c r="L558" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M558" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N558" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O558" s="9"/>
-      <c r="P558" s="4"/>
+      <c r="P558" s="9">
+        <v>514.72868217054202</v>
+      </c>
       <c r="Q558" s="4"/>
-      <c r="R558" s="9"/>
       <c r="S558" s="9"/>
       <c r="T558" s="9"/>
     </row>
     <row r="559" spans="1:20" ht="15" customHeight="1">
-      <c r="A559" s="4"/>
-      <c r="B559" s="73"/>
-      <c r="C559" s="4"/>
-      <c r="D559" s="4"/>
+      <c r="A559" s="117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B559" s="110" t="s">
+        <v>701</v>
+      </c>
+      <c r="C559" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D559" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E559" s="9"/>
-      <c r="F559" s="4"/>
-      <c r="G559" s="4"/>
+      <c r="F559" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G559" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H559" s="4"/>
-      <c r="I559" s="4"/>
-      <c r="J559" s="4"/>
+      <c r="I559" s="4">
+        <v>973</v>
+      </c>
+      <c r="J559" s="70">
+        <f t="shared" si="16"/>
+        <v>4909581860.4651089</v>
+      </c>
       <c r="K559" s="4"/>
-      <c r="L559" s="4"/>
-      <c r="M559" s="4"/>
-      <c r="N559" s="4"/>
+      <c r="L559" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M559" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N559" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O559" s="9"/>
-      <c r="P559" s="4"/>
+      <c r="P559" s="9">
+        <v>500.62015503875898</v>
+      </c>
       <c r="Q559" s="4"/>
-      <c r="R559" s="9"/>
       <c r="S559" s="9"/>
       <c r="T559" s="9"/>
     </row>
     <row r="560" spans="1:20" ht="15" customHeight="1">
-      <c r="A560" s="4"/>
-      <c r="B560" s="73"/>
-      <c r="C560" s="4"/>
-      <c r="D560" s="4"/>
+      <c r="A560" s="117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B560" s="110" t="s">
+        <v>701</v>
+      </c>
+      <c r="C560" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D560" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E560" s="9"/>
-      <c r="F560" s="4"/>
-      <c r="G560" s="4"/>
+      <c r="F560" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G560" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H560" s="4"/>
-      <c r="I560" s="4"/>
-      <c r="J560" s="4"/>
+      <c r="I560" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J560" s="70">
+        <f t="shared" si="16"/>
+        <v>3781396744.1860447</v>
+      </c>
       <c r="K560" s="4"/>
-      <c r="L560" s="4"/>
-      <c r="M560" s="4"/>
-      <c r="N560" s="4"/>
+      <c r="L560" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M560" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N560" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O560" s="9"/>
-      <c r="P560" s="4"/>
+      <c r="P560" s="9">
+        <v>385.58139534883702</v>
+      </c>
       <c r="Q560" s="4"/>
-      <c r="R560" s="9"/>
       <c r="S560" s="9"/>
       <c r="T560" s="9"/>
     </row>
     <row r="561" spans="1:20" ht="15" customHeight="1">
-      <c r="A561" s="4"/>
-      <c r="B561" s="73"/>
-      <c r="C561" s="4"/>
-      <c r="D561" s="4"/>
+      <c r="A561" s="117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B561" s="110" t="s">
+        <v>701</v>
+      </c>
+      <c r="C561" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D561" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E561" s="9"/>
-      <c r="F561" s="4"/>
-      <c r="G561" s="4"/>
+      <c r="F561" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G561" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H561" s="4"/>
-      <c r="I561" s="4"/>
-      <c r="J561" s="4"/>
+      <c r="I561" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J561" s="70">
+        <f t="shared" si="16"/>
+        <v>2961866046.5116277</v>
+      </c>
       <c r="K561" s="4"/>
-      <c r="L561" s="4"/>
-      <c r="M561" s="4"/>
-      <c r="N561" s="4"/>
+      <c r="L561" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M561" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N561" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O561" s="9"/>
-      <c r="P561" s="4"/>
+      <c r="P561" s="9">
+        <v>302.01550387596899</v>
+      </c>
       <c r="Q561" s="4"/>
-      <c r="R561" s="9"/>
       <c r="S561" s="9"/>
       <c r="T561" s="9"/>
     </row>
     <row r="562" spans="1:20" ht="15" customHeight="1">
-      <c r="A562" s="4"/>
-      <c r="B562" s="73"/>
-      <c r="C562" s="4"/>
-      <c r="D562" s="4"/>
+      <c r="A562" s="117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B562" s="110" t="s">
+        <v>701</v>
+      </c>
+      <c r="C562" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D562" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E562" s="9"/>
-      <c r="F562" s="4"/>
-      <c r="G562" s="4"/>
+      <c r="F562" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G562" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H562" s="4"/>
-      <c r="I562" s="4"/>
-      <c r="J562" s="4"/>
+      <c r="I562" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J562" s="70">
+        <f t="shared" si="16"/>
+        <v>2355200465.1162701</v>
+      </c>
       <c r="K562" s="4"/>
-      <c r="L562" s="4"/>
-      <c r="M562" s="4"/>
-      <c r="N562" s="4"/>
+      <c r="L562" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M562" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N562" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O562" s="9"/>
-      <c r="P562" s="4"/>
+      <c r="P562" s="9">
+        <v>240.15503875968901</v>
+      </c>
       <c r="Q562" s="4"/>
-      <c r="R562" s="9"/>
       <c r="S562" s="9"/>
       <c r="T562" s="9"/>
     </row>
     <row r="563" spans="1:20" ht="15" customHeight="1">
-      <c r="A563" s="4"/>
-      <c r="B563" s="9"/>
-      <c r="C563" s="4"/>
-      <c r="D563" s="4"/>
+      <c r="A563" s="117" t="s">
+        <v>707</v>
+      </c>
+      <c r="B563" s="110" t="s">
+        <v>702</v>
+      </c>
+      <c r="C563" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D563" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E563" s="9"/>
-      <c r="F563" s="4"/>
-      <c r="G563" s="4"/>
+      <c r="F563" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G563" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H563" s="4"/>
-      <c r="I563" s="4"/>
-      <c r="J563" s="4"/>
+      <c r="I563" s="4">
+        <v>298</v>
+      </c>
+      <c r="J563" s="70">
+        <f t="shared" si="16"/>
+        <v>6005837209.3023176</v>
+      </c>
       <c r="K563" s="4"/>
-      <c r="L563" s="4"/>
-      <c r="M563" s="4"/>
-      <c r="N563" s="4"/>
+      <c r="L563" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M563" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N563" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O563" s="9"/>
-      <c r="P563" s="4"/>
+      <c r="P563" s="9">
+        <v>612.40310077519302</v>
+      </c>
       <c r="Q563" s="4"/>
-      <c r="R563" s="9"/>
       <c r="S563" s="9"/>
       <c r="T563" s="9"/>
     </row>
     <row r="564" spans="1:20" ht="15" customHeight="1">
-      <c r="A564" s="4"/>
-      <c r="B564" s="9"/>
-      <c r="C564" s="4"/>
-      <c r="D564" s="4"/>
+      <c r="A564" s="117" t="s">
+        <v>707</v>
+      </c>
+      <c r="B564" s="110" t="s">
+        <v>702</v>
+      </c>
+      <c r="C564" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D564" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E564" s="9"/>
-      <c r="F564" s="4"/>
-      <c r="G564" s="4"/>
+      <c r="F564" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G564" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H564" s="4"/>
-      <c r="I564" s="4"/>
-      <c r="J564" s="4"/>
+      <c r="I564" s="4">
+        <v>573</v>
+      </c>
+      <c r="J564" s="70">
+        <f t="shared" ref="J564:J598" si="17">P564*9807000</f>
+        <v>5335312093.0232553</v>
+      </c>
       <c r="K564" s="4"/>
-      <c r="L564" s="4"/>
-      <c r="M564" s="4"/>
-      <c r="N564" s="4"/>
+      <c r="L564" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M564" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N564" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O564" s="9"/>
-      <c r="P564" s="4"/>
+      <c r="P564" s="9">
+        <v>544.03100775193798</v>
+      </c>
       <c r="Q564" s="4"/>
-      <c r="R564" s="9"/>
       <c r="S564" s="9"/>
       <c r="T564" s="9"/>
     </row>
     <row r="565" spans="1:20" ht="15" customHeight="1">
-      <c r="A565" s="4"/>
-      <c r="B565" s="9"/>
-      <c r="C565" s="4"/>
-      <c r="D565" s="4"/>
+      <c r="A565" s="117" t="s">
+        <v>707</v>
+      </c>
+      <c r="B565" s="110" t="s">
+        <v>702</v>
+      </c>
+      <c r="C565" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D565" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E565" s="9"/>
-      <c r="F565" s="4"/>
-      <c r="G565" s="4"/>
+      <c r="F565" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G565" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H565" s="4"/>
-      <c r="I565" s="4"/>
-      <c r="J565" s="4"/>
+      <c r="I565" s="4">
+        <v>673</v>
+      </c>
+      <c r="J565" s="70">
+        <f t="shared" si="17"/>
+        <v>5335312093.0232553</v>
+      </c>
       <c r="K565" s="4"/>
-      <c r="L565" s="4"/>
-      <c r="M565" s="4"/>
-      <c r="N565" s="4"/>
+      <c r="L565" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M565" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N565" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O565" s="9"/>
-      <c r="P565" s="4"/>
+      <c r="P565" s="9">
+        <v>544.03100775193798</v>
+      </c>
       <c r="Q565" s="4"/>
-      <c r="R565" s="9"/>
       <c r="S565" s="9"/>
       <c r="T565" s="9"/>
     </row>
     <row r="566" spans="1:20" ht="15" customHeight="1">
-      <c r="A566" s="4"/>
-      <c r="B566" s="9"/>
-      <c r="C566" s="4"/>
-      <c r="D566" s="4"/>
+      <c r="A566" s="117" t="s">
+        <v>707</v>
+      </c>
+      <c r="B566" s="110" t="s">
+        <v>702</v>
+      </c>
+      <c r="C566" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D566" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E566" s="9"/>
-      <c r="F566" s="4"/>
-      <c r="G566" s="4"/>
+      <c r="F566" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G566" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H566" s="4"/>
-      <c r="I566" s="4"/>
-      <c r="J566" s="4"/>
+      <c r="I566" s="4">
+        <v>773</v>
+      </c>
+      <c r="J566" s="70">
+        <f t="shared" si="17"/>
+        <v>5345955348.8372049</v>
+      </c>
       <c r="K566" s="4"/>
-      <c r="L566" s="4"/>
-      <c r="M566" s="4"/>
-      <c r="N566" s="4"/>
+      <c r="L566" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M566" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N566" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O566" s="9"/>
-      <c r="P566" s="4"/>
+      <c r="P566" s="9">
+        <v>545.11627906976696</v>
+      </c>
       <c r="Q566" s="4"/>
-      <c r="R566" s="9"/>
       <c r="S566" s="9"/>
       <c r="T566" s="9"/>
     </row>
     <row r="567" spans="1:20" ht="15" customHeight="1">
-      <c r="A567" s="4"/>
-      <c r="B567" s="9"/>
-      <c r="C567" s="4"/>
-      <c r="D567" s="4"/>
+      <c r="A567" s="117" t="s">
+        <v>707</v>
+      </c>
+      <c r="B567" s="110" t="s">
+        <v>702</v>
+      </c>
+      <c r="C567" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D567" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E567" s="9"/>
-      <c r="F567" s="4"/>
-      <c r="G567" s="4"/>
+      <c r="F567" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G567" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H567" s="4"/>
-      <c r="I567" s="4"/>
-      <c r="J567" s="4"/>
+      <c r="I567" s="4">
+        <v>873</v>
+      </c>
+      <c r="J567" s="70">
+        <f t="shared" si="17"/>
+        <v>5133090232.558136</v>
+      </c>
       <c r="K567" s="4"/>
-      <c r="L567" s="4"/>
-      <c r="M567" s="4"/>
-      <c r="N567" s="4"/>
+      <c r="L567" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M567" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N567" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O567" s="9"/>
-      <c r="P567" s="4"/>
+      <c r="P567" s="9">
+        <v>523.41085271317797</v>
+      </c>
       <c r="Q567" s="4"/>
-      <c r="R567" s="9"/>
       <c r="S567" s="9"/>
       <c r="T567" s="9"/>
     </row>
     <row r="568" spans="1:20" ht="15" customHeight="1">
-      <c r="A568" s="4"/>
-      <c r="B568" s="9"/>
-      <c r="C568" s="4"/>
-      <c r="D568" s="4"/>
+      <c r="A568" s="117" t="s">
+        <v>707</v>
+      </c>
+      <c r="B568" s="110" t="s">
+        <v>702</v>
+      </c>
+      <c r="C568" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D568" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E568" s="9"/>
-      <c r="F568" s="4"/>
-      <c r="G568" s="4"/>
+      <c r="F568" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G568" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H568" s="4"/>
-      <c r="I568" s="4"/>
-      <c r="J568" s="4"/>
+      <c r="I568" s="4">
+        <v>973</v>
+      </c>
+      <c r="J568" s="70">
+        <f t="shared" si="17"/>
+        <v>4909581860.4651089</v>
+      </c>
       <c r="K568" s="4"/>
-      <c r="L568" s="4"/>
-      <c r="M568" s="4"/>
-      <c r="N568" s="4"/>
+      <c r="L568" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M568" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N568" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O568" s="9"/>
-      <c r="P568" s="4"/>
+      <c r="P568" s="9">
+        <v>500.62015503875898</v>
+      </c>
       <c r="Q568" s="4"/>
-      <c r="R568" s="9"/>
       <c r="S568" s="9"/>
       <c r="T568" s="9"/>
     </row>
     <row r="569" spans="1:20" ht="15" customHeight="1">
-      <c r="A569" s="4"/>
-      <c r="B569" s="9"/>
-      <c r="C569" s="4"/>
-      <c r="D569" s="4"/>
+      <c r="A569" s="117" t="s">
+        <v>707</v>
+      </c>
+      <c r="B569" s="110" t="s">
+        <v>702</v>
+      </c>
+      <c r="C569" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D569" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E569" s="9"/>
-      <c r="F569" s="4"/>
-      <c r="G569" s="4"/>
+      <c r="F569" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G569" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H569" s="4"/>
-      <c r="I569" s="4"/>
-      <c r="J569" s="4"/>
+      <c r="I569" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J569" s="70">
+        <f t="shared" si="17"/>
+        <v>3951688837.2092977</v>
+      </c>
       <c r="K569" s="4"/>
-      <c r="L569" s="4"/>
-      <c r="M569" s="4"/>
-      <c r="N569" s="4"/>
+      <c r="L569" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M569" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N569" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O569" s="9"/>
-      <c r="P569" s="4"/>
+      <c r="P569" s="9">
+        <v>402.94573643410803</v>
+      </c>
       <c r="Q569" s="4"/>
-      <c r="R569" s="9"/>
       <c r="S569" s="9"/>
       <c r="T569" s="9"/>
     </row>
     <row r="570" spans="1:20" ht="15" customHeight="1">
-      <c r="A570" s="4"/>
-      <c r="B570" s="9"/>
-      <c r="C570" s="4"/>
-      <c r="D570" s="4"/>
+      <c r="A570" s="117" t="s">
+        <v>707</v>
+      </c>
+      <c r="B570" s="110" t="s">
+        <v>702</v>
+      </c>
+      <c r="C570" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D570" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E570" s="9"/>
-      <c r="F570" s="4"/>
-      <c r="G570" s="4"/>
+      <c r="F570" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G570" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H570" s="4"/>
-      <c r="I570" s="4"/>
-      <c r="J570" s="4"/>
+      <c r="I570" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J570" s="70">
+        <f t="shared" si="17"/>
+        <v>2887363255.8139458</v>
+      </c>
       <c r="K570" s="4"/>
-      <c r="L570" s="4"/>
-      <c r="M570" s="4"/>
-      <c r="N570" s="4"/>
+      <c r="L570" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M570" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N570" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O570" s="9"/>
-      <c r="P570" s="4"/>
+      <c r="P570" s="9">
+        <v>294.41860465116201</v>
+      </c>
       <c r="Q570" s="4"/>
-      <c r="R570" s="9"/>
       <c r="S570" s="9"/>
       <c r="T570" s="9"/>
     </row>
     <row r="571" spans="1:20" ht="15" customHeight="1">
-      <c r="A571" s="4"/>
-      <c r="B571" s="9"/>
-      <c r="C571" s="4"/>
-      <c r="D571" s="4"/>
+      <c r="A571" s="117" t="s">
+        <v>707</v>
+      </c>
+      <c r="B571" s="110" t="s">
+        <v>702</v>
+      </c>
+      <c r="C571" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D571" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E571" s="9"/>
-      <c r="F571" s="4"/>
-      <c r="G571" s="4"/>
+      <c r="F571" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G571" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H571" s="4"/>
-      <c r="I571" s="4"/>
-      <c r="J571" s="4"/>
+      <c r="I571" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J571" s="70">
+        <f t="shared" si="17"/>
+        <v>2355200465.1162701</v>
+      </c>
       <c r="K571" s="4"/>
-      <c r="L571" s="4"/>
-      <c r="M571" s="4"/>
-      <c r="N571" s="4"/>
+      <c r="L571" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M571" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N571" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O571" s="9"/>
-      <c r="P571" s="4"/>
+      <c r="P571" s="9">
+        <v>240.15503875968901</v>
+      </c>
       <c r="Q571" s="4"/>
-      <c r="R571" s="9"/>
       <c r="S571" s="9"/>
       <c r="T571" s="9"/>
     </row>
     <row r="572" spans="1:20" ht="15" customHeight="1">
-      <c r="A572" s="4"/>
-      <c r="B572" s="9"/>
-      <c r="C572" s="4"/>
-      <c r="D572" s="4"/>
+      <c r="A572" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="B572" s="110" t="s">
+        <v>703</v>
+      </c>
+      <c r="C572" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D572" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E572" s="9"/>
-      <c r="F572" s="4"/>
-      <c r="G572" s="4"/>
+      <c r="F572" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G572" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H572" s="4"/>
-      <c r="I572" s="4"/>
-      <c r="J572" s="4"/>
+      <c r="I572" s="4">
+        <v>298</v>
+      </c>
+      <c r="J572" s="70">
+        <f t="shared" si="17"/>
+        <v>7144665581.3953419</v>
+      </c>
       <c r="K572" s="4"/>
-      <c r="L572" s="4"/>
-      <c r="M572" s="4"/>
-      <c r="N572" s="4"/>
+      <c r="L572" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M572" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N572" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O572" s="9"/>
-      <c r="P572" s="4"/>
+      <c r="P572" s="1">
+        <v>728.52713178294505</v>
+      </c>
       <c r="Q572" s="4"/>
-      <c r="R572" s="9"/>
       <c r="S572" s="9"/>
       <c r="T572" s="9"/>
     </row>
     <row r="573" spans="1:20" ht="15" customHeight="1">
-      <c r="A573" s="4"/>
-      <c r="B573" s="9"/>
-      <c r="C573" s="4"/>
-      <c r="D573" s="4"/>
+      <c r="A573" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="B573" s="110" t="s">
+        <v>703</v>
+      </c>
+      <c r="C573" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D573" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E573" s="9"/>
-      <c r="F573" s="4"/>
-      <c r="G573" s="4"/>
+      <c r="F573" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G573" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H573" s="4"/>
-      <c r="I573" s="4"/>
-      <c r="J573" s="4"/>
+      <c r="I573" s="4">
+        <v>573</v>
+      </c>
+      <c r="J573" s="70">
+        <f t="shared" si="17"/>
+        <v>6506070232.558136</v>
+      </c>
       <c r="K573" s="4"/>
-      <c r="L573" s="4"/>
-      <c r="M573" s="4"/>
-      <c r="N573" s="4"/>
+      <c r="L573" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M573" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N573" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O573" s="9"/>
-      <c r="P573" s="4"/>
+      <c r="P573" s="1">
+        <v>663.41085271317797</v>
+      </c>
       <c r="Q573" s="4"/>
-      <c r="R573" s="9"/>
       <c r="S573" s="9"/>
       <c r="T573" s="9"/>
     </row>
     <row r="574" spans="1:20" ht="15" customHeight="1">
-      <c r="A574" s="4"/>
-      <c r="B574" s="9"/>
-      <c r="C574" s="4"/>
-      <c r="D574" s="4"/>
+      <c r="A574" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="B574" s="110" t="s">
+        <v>703</v>
+      </c>
+      <c r="C574" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D574" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E574" s="9"/>
-      <c r="F574" s="4"/>
-      <c r="G574" s="4"/>
+      <c r="F574" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G574" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H574" s="4"/>
-      <c r="I574" s="4"/>
-      <c r="J574" s="4"/>
+      <c r="I574" s="4">
+        <v>673</v>
+      </c>
+      <c r="J574" s="70">
+        <f t="shared" si="17"/>
+        <v>6399637674.4185982</v>
+      </c>
       <c r="K574" s="4"/>
-      <c r="L574" s="4"/>
-      <c r="M574" s="4"/>
-      <c r="N574" s="4"/>
+      <c r="L574" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M574" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N574" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O574" s="9"/>
-      <c r="P574" s="4"/>
+      <c r="P574" s="1">
+        <v>652.55813953488303</v>
+      </c>
       <c r="Q574" s="4"/>
-      <c r="R574" s="9"/>
       <c r="S574" s="9"/>
       <c r="T574" s="9"/>
     </row>
     <row r="575" spans="1:20" ht="15" customHeight="1">
-      <c r="A575" s="4"/>
-      <c r="B575" s="9"/>
-      <c r="C575" s="4"/>
-      <c r="D575" s="4"/>
+      <c r="A575" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="B575" s="110" t="s">
+        <v>703</v>
+      </c>
+      <c r="C575" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D575" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E575" s="9"/>
-      <c r="F575" s="4"/>
-      <c r="G575" s="4"/>
+      <c r="F575" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G575" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H575" s="4"/>
-      <c r="I575" s="4"/>
-      <c r="J575" s="4"/>
+      <c r="I575" s="4">
+        <v>773</v>
+      </c>
+      <c r="J575" s="70">
+        <f t="shared" si="17"/>
+        <v>6271918604.6511602</v>
+      </c>
       <c r="K575" s="4"/>
-      <c r="L575" s="4"/>
-      <c r="M575" s="4"/>
-      <c r="N575" s="4"/>
+      <c r="L575" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M575" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N575" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O575" s="9"/>
-      <c r="P575" s="4"/>
+      <c r="P575" s="1">
+        <v>639.53488372093</v>
+      </c>
       <c r="Q575" s="4"/>
-      <c r="R575" s="9"/>
       <c r="S575" s="9"/>
       <c r="T575" s="9"/>
     </row>
     <row r="576" spans="1:20" ht="15" customHeight="1">
-      <c r="A576" s="4"/>
-      <c r="B576" s="9"/>
-      <c r="C576" s="4"/>
-      <c r="D576" s="4"/>
+      <c r="A576" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="B576" s="110" t="s">
+        <v>703</v>
+      </c>
+      <c r="C576" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D576" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E576" s="9"/>
-      <c r="F576" s="4"/>
-      <c r="G576" s="4"/>
+      <c r="F576" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G576" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H576" s="4"/>
-      <c r="I576" s="4"/>
-      <c r="J576" s="4"/>
+      <c r="I576" s="4">
+        <v>873</v>
+      </c>
+      <c r="J576" s="70">
+        <f t="shared" si="17"/>
+        <v>6005837209.3023176</v>
+      </c>
       <c r="K576" s="4"/>
-      <c r="L576" s="4"/>
-      <c r="M576" s="4"/>
-      <c r="N576" s="4"/>
+      <c r="L576" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M576" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N576" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O576" s="9"/>
-      <c r="P576" s="4"/>
+      <c r="P576" s="1">
+        <v>612.40310077519302</v>
+      </c>
       <c r="Q576" s="4"/>
-      <c r="R576" s="9"/>
       <c r="S576" s="9"/>
       <c r="T576" s="9"/>
     </row>
     <row r="577" spans="1:20" ht="15" customHeight="1">
-      <c r="A577" s="4"/>
-      <c r="B577" s="9"/>
-      <c r="C577" s="4"/>
-      <c r="D577" s="4"/>
+      <c r="A577" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="B577" s="110" t="s">
+        <v>703</v>
+      </c>
+      <c r="C577" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D577" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E577" s="9"/>
-      <c r="F577" s="4"/>
-      <c r="G577" s="4"/>
+      <c r="F577" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G577" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H577" s="4"/>
-      <c r="I577" s="4"/>
-      <c r="J577" s="4"/>
+      <c r="I577" s="4">
+        <v>973</v>
+      </c>
+      <c r="J577" s="70">
+        <f t="shared" si="17"/>
+        <v>5803615348.8372087</v>
+      </c>
       <c r="K577" s="4"/>
-      <c r="L577" s="4"/>
-      <c r="M577" s="4"/>
-      <c r="N577" s="4"/>
+      <c r="L577" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M577" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N577" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O577" s="9"/>
-      <c r="P577" s="4"/>
+      <c r="P577" s="1">
+        <v>591.78294573643404</v>
+      </c>
       <c r="Q577" s="4"/>
-      <c r="R577" s="9"/>
       <c r="S577" s="9"/>
       <c r="T577" s="9"/>
     </row>
     <row r="578" spans="1:20" ht="15" customHeight="1">
-      <c r="A578" s="4"/>
-      <c r="B578" s="9"/>
-      <c r="C578" s="4"/>
-      <c r="D578" s="4"/>
+      <c r="A578" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="B578" s="110" t="s">
+        <v>703</v>
+      </c>
+      <c r="C578" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D578" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E578" s="9"/>
-      <c r="F578" s="4"/>
-      <c r="G578" s="4"/>
+      <c r="F578" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G578" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H578" s="4"/>
-      <c r="I578" s="4"/>
-      <c r="J578" s="4"/>
+      <c r="I578" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J578" s="70">
+        <f t="shared" si="17"/>
+        <v>5165019999.9999933</v>
+      </c>
       <c r="K578" s="4"/>
-      <c r="L578" s="4"/>
-      <c r="M578" s="4"/>
-      <c r="N578" s="4"/>
+      <c r="L578" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M578" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N578" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O578" s="9"/>
-      <c r="P578" s="4"/>
+      <c r="P578" s="1">
+        <v>526.66666666666595</v>
+      </c>
       <c r="Q578" s="4"/>
-      <c r="R578" s="9"/>
       <c r="S578" s="9"/>
       <c r="T578" s="9"/>
     </row>
     <row r="579" spans="1:20" ht="15" customHeight="1">
-      <c r="A579" s="4"/>
-      <c r="B579" s="9"/>
-      <c r="C579" s="4"/>
-      <c r="D579" s="4"/>
+      <c r="A579" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="B579" s="110" t="s">
+        <v>703</v>
+      </c>
+      <c r="C579" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D579" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E579" s="9"/>
-      <c r="F579" s="4"/>
-      <c r="G579" s="4"/>
+      <c r="F579" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G579" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H579" s="4"/>
-      <c r="I579" s="4"/>
-      <c r="J579" s="4"/>
+      <c r="I579" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J579" s="70">
+        <f t="shared" si="17"/>
+        <v>4345489302.3255768</v>
+      </c>
       <c r="K579" s="4"/>
-      <c r="L579" s="4"/>
-      <c r="M579" s="4"/>
-      <c r="N579" s="4"/>
+      <c r="L579" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M579" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N579" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O579" s="9"/>
-      <c r="P579" s="4"/>
+      <c r="P579" s="1">
+        <v>443.10077519379797</v>
+      </c>
       <c r="Q579" s="4"/>
-      <c r="R579" s="9"/>
       <c r="S579" s="9"/>
       <c r="T579" s="9"/>
     </row>
     <row r="580" spans="1:20" ht="15" customHeight="1">
-      <c r="A580" s="4"/>
-      <c r="B580" s="9"/>
-      <c r="C580" s="4"/>
-      <c r="D580" s="4"/>
+      <c r="A580" s="117" t="s">
+        <v>708</v>
+      </c>
+      <c r="B580" s="110" t="s">
+        <v>703</v>
+      </c>
+      <c r="C580" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D580" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E580" s="9"/>
-      <c r="F580" s="4"/>
-      <c r="G580" s="4"/>
+      <c r="F580" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G580" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H580" s="4"/>
-      <c r="I580" s="4"/>
-      <c r="J580" s="4"/>
+      <c r="I580" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J580" s="70">
+        <f t="shared" si="17"/>
+        <v>3387596279.0697646</v>
+      </c>
       <c r="K580" s="4"/>
-      <c r="L580" s="4"/>
-      <c r="M580" s="4"/>
-      <c r="N580" s="4"/>
+      <c r="L580" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M580" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N580" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O580" s="9"/>
-      <c r="P580" s="4"/>
+      <c r="P580" s="1">
+        <v>345.42635658914702</v>
+      </c>
       <c r="Q580" s="4"/>
-      <c r="R580" s="9"/>
       <c r="S580" s="9"/>
       <c r="T580" s="9"/>
     </row>
     <row r="581" spans="1:20" ht="15" customHeight="1">
-      <c r="A581" s="68"/>
-      <c r="B581" s="9"/>
-      <c r="C581" s="4"/>
-      <c r="D581" s="4"/>
+      <c r="A581" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="B581" s="110" t="s">
+        <v>704</v>
+      </c>
+      <c r="C581" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D581" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E581" s="9"/>
-      <c r="F581" s="4"/>
-      <c r="G581" s="4"/>
+      <c r="F581" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G581" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H581" s="4"/>
-      <c r="I581" s="4"/>
-      <c r="J581" s="4"/>
+      <c r="I581" s="4">
+        <v>298</v>
+      </c>
+      <c r="J581" s="70">
+        <f t="shared" si="17"/>
+        <v>7974839534.8837175</v>
+      </c>
       <c r="K581" s="4"/>
-      <c r="L581" s="4"/>
-      <c r="M581" s="4"/>
-      <c r="N581" s="4"/>
+      <c r="L581" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M581" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N581" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O581" s="9"/>
-      <c r="P581" s="4"/>
+      <c r="P581" s="1">
+        <v>813.17829457364303</v>
+      </c>
       <c r="Q581" s="4"/>
       <c r="R581" s="9"/>
       <c r="S581" s="9"/>
       <c r="T581" s="9"/>
     </row>
     <row r="582" spans="1:20" ht="15" customHeight="1">
-      <c r="A582" s="68"/>
-      <c r="B582" s="9"/>
-      <c r="C582" s="4"/>
-      <c r="D582" s="4"/>
+      <c r="A582" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="B582" s="110" t="s">
+        <v>704</v>
+      </c>
+      <c r="C582" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D582" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E582" s="9"/>
-      <c r="F582" s="4"/>
-      <c r="G582" s="4"/>
+      <c r="F582" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G582" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H582" s="4"/>
-      <c r="I582" s="4"/>
-      <c r="J582" s="4"/>
+      <c r="I582" s="4">
+        <v>573</v>
+      </c>
+      <c r="J582" s="70">
+        <f t="shared" si="17"/>
+        <v>7336244186.0465117</v>
+      </c>
       <c r="K582" s="4"/>
-      <c r="L582" s="4"/>
-      <c r="M582" s="4"/>
-      <c r="N582" s="4"/>
+      <c r="L582" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M582" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N582" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O582" s="9"/>
-      <c r="P582" s="4"/>
+      <c r="P582" s="1">
+        <v>748.06201550387595</v>
+      </c>
       <c r="Q582" s="4"/>
       <c r="R582" s="9"/>
       <c r="S582" s="9"/>
       <c r="T582" s="9"/>
     </row>
     <row r="583" spans="1:20" ht="15" customHeight="1">
-      <c r="A583" s="68"/>
-      <c r="B583" s="9"/>
-      <c r="C583" s="4"/>
-      <c r="D583" s="4"/>
+      <c r="A583" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="B583" s="110" t="s">
+        <v>704</v>
+      </c>
+      <c r="C583" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D583" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E583" s="9"/>
-      <c r="F583" s="4"/>
-      <c r="G583" s="4"/>
+      <c r="F583" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G583" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H583" s="4"/>
-      <c r="I583" s="4"/>
-      <c r="J583" s="4"/>
+      <c r="I583" s="4">
+        <v>673</v>
+      </c>
+      <c r="J583" s="70">
+        <f t="shared" si="17"/>
+        <v>7176595348.8372087</v>
+      </c>
       <c r="K583" s="4"/>
-      <c r="L583" s="4"/>
-      <c r="M583" s="4"/>
-      <c r="N583" s="4"/>
+      <c r="L583" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M583" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N583" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O583" s="9"/>
-      <c r="P583" s="4"/>
+      <c r="P583" s="1">
+        <v>731.78294573643404</v>
+      </c>
       <c r="Q583" s="4"/>
       <c r="R583" s="9"/>
       <c r="S583" s="9"/>
       <c r="T583" s="9"/>
     </row>
     <row r="584" spans="1:20" ht="15" customHeight="1">
-      <c r="A584" s="68"/>
-      <c r="B584" s="9"/>
-      <c r="C584" s="4"/>
-      <c r="D584" s="4"/>
+      <c r="A584" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="B584" s="110" t="s">
+        <v>704</v>
+      </c>
+      <c r="C584" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D584" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E584" s="9"/>
-      <c r="F584" s="4"/>
-      <c r="G584" s="4"/>
+      <c r="F584" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G584" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H584" s="4"/>
-      <c r="I584" s="4"/>
-      <c r="J584" s="4"/>
+      <c r="I584" s="4">
+        <v>773</v>
+      </c>
+      <c r="J584" s="70">
+        <f t="shared" si="17"/>
+        <v>7080806046.5116282</v>
+      </c>
       <c r="K584" s="4"/>
-      <c r="L584" s="4"/>
-      <c r="M584" s="4"/>
-      <c r="N584" s="4"/>
+      <c r="L584" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M584" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N584" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O584" s="9"/>
-      <c r="P584" s="4"/>
+      <c r="P584" s="1">
+        <v>722.01550387596899</v>
+      </c>
       <c r="Q584" s="4"/>
       <c r="R584" s="9"/>
       <c r="S584" s="9"/>
       <c r="T584" s="9"/>
     </row>
     <row r="585" spans="1:20" ht="15" customHeight="1">
-      <c r="A585" s="68"/>
-      <c r="B585" s="9"/>
-      <c r="C585" s="4"/>
-      <c r="D585" s="4"/>
+      <c r="A585" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="B585" s="110" t="s">
+        <v>704</v>
+      </c>
+      <c r="C585" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D585" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E585" s="9"/>
-      <c r="F585" s="4"/>
-      <c r="G585" s="4"/>
+      <c r="F585" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G585" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H585" s="4"/>
-      <c r="I585" s="4"/>
-      <c r="J585" s="4"/>
+      <c r="I585" s="4">
+        <v>873</v>
+      </c>
+      <c r="J585" s="70">
+        <f t="shared" si="17"/>
+        <v>6772151627.90697</v>
+      </c>
       <c r="K585" s="4"/>
-      <c r="L585" s="4"/>
-      <c r="M585" s="4"/>
-      <c r="N585" s="4"/>
+      <c r="L585" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M585" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N585" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O585" s="9"/>
-      <c r="P585" s="4"/>
+      <c r="P585" s="1">
+        <v>690.54263565891404</v>
+      </c>
       <c r="Q585" s="4"/>
       <c r="R585" s="9"/>
       <c r="S585" s="9"/>
       <c r="T585" s="9"/>
     </row>
     <row r="586" spans="1:20" ht="15" customHeight="1">
-      <c r="A586" s="68"/>
-      <c r="B586" s="9"/>
-      <c r="C586" s="4"/>
-      <c r="D586" s="4"/>
+      <c r="A586" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="B586" s="110" t="s">
+        <v>704</v>
+      </c>
+      <c r="C586" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D586" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E586" s="9"/>
-      <c r="F586" s="4"/>
-      <c r="G586" s="4"/>
+      <c r="F586" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G586" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H586" s="4"/>
-      <c r="I586" s="4"/>
-      <c r="J586" s="4"/>
+      <c r="I586" s="4">
+        <v>973</v>
+      </c>
+      <c r="J586" s="70">
+        <f t="shared" si="17"/>
+        <v>6410280930.2325563</v>
+      </c>
       <c r="K586" s="4"/>
-      <c r="L586" s="4"/>
-      <c r="M586" s="4"/>
-      <c r="N586" s="4"/>
+      <c r="L586" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M586" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N586" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O586" s="9"/>
-      <c r="P586" s="4"/>
+      <c r="P586" s="1">
+        <v>653.64341085271303</v>
+      </c>
       <c r="Q586" s="4"/>
       <c r="R586" s="9"/>
       <c r="S586" s="9"/>
       <c r="T586" s="9"/>
     </row>
     <row r="587" spans="1:20" ht="15" customHeight="1">
-      <c r="A587" s="4"/>
-      <c r="B587" s="9"/>
-      <c r="C587" s="4"/>
-      <c r="D587" s="4"/>
+      <c r="A587" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="B587" s="110" t="s">
+        <v>704</v>
+      </c>
+      <c r="C587" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D587" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E587" s="9"/>
-      <c r="F587" s="4"/>
-      <c r="G587" s="4"/>
+      <c r="F587" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G587" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H587" s="4"/>
-      <c r="I587" s="4"/>
-      <c r="J587" s="4"/>
+      <c r="I587" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J587" s="70">
+        <f t="shared" si="17"/>
+        <v>5803615348.8372087</v>
+      </c>
       <c r="K587" s="4"/>
-      <c r="L587" s="4"/>
-      <c r="M587" s="4"/>
-      <c r="N587" s="4"/>
+      <c r="L587" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M587" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N587" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O587" s="9"/>
-      <c r="P587" s="4"/>
+      <c r="P587" s="1">
+        <v>591.78294573643404</v>
+      </c>
       <c r="Q587" s="4"/>
       <c r="R587" s="9"/>
       <c r="S587" s="9"/>
       <c r="T587" s="9"/>
     </row>
     <row r="588" spans="1:20" ht="15" customHeight="1">
-      <c r="A588" s="4"/>
-      <c r="B588" s="9"/>
-      <c r="C588" s="4"/>
-      <c r="D588" s="4"/>
+      <c r="A588" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="B588" s="110" t="s">
+        <v>704</v>
+      </c>
+      <c r="C588" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D588" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E588" s="9"/>
-      <c r="F588" s="4"/>
-      <c r="G588" s="4"/>
+      <c r="F588" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G588" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H588" s="4"/>
-      <c r="I588" s="4"/>
-      <c r="J588" s="4"/>
+      <c r="I588" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J588" s="70">
+        <f t="shared" si="17"/>
+        <v>4813792558.1395292</v>
+      </c>
       <c r="K588" s="4"/>
-      <c r="L588" s="4"/>
-      <c r="M588" s="4"/>
-      <c r="N588" s="4"/>
+      <c r="L588" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M588" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N588" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O588" s="9"/>
-      <c r="P588" s="4"/>
+      <c r="P588" s="1">
+        <v>490.85271317829398</v>
+      </c>
       <c r="Q588" s="4"/>
       <c r="R588" s="9"/>
       <c r="S588" s="9"/>
       <c r="T588" s="9"/>
     </row>
     <row r="589" spans="1:20" ht="15" customHeight="1">
-      <c r="A589" s="4"/>
-      <c r="B589" s="9"/>
-      <c r="C589" s="4"/>
-      <c r="D589" s="4"/>
+      <c r="A589" s="117" t="s">
+        <v>709</v>
+      </c>
+      <c r="B589" s="110" t="s">
+        <v>704</v>
+      </c>
+      <c r="C589" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D589" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E589" s="9"/>
-      <c r="F589" s="4"/>
-      <c r="G589" s="4"/>
+      <c r="F589" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G589" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H589" s="4"/>
-      <c r="I589" s="4"/>
-      <c r="J589" s="4"/>
+      <c r="I589" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J589" s="70">
+        <f t="shared" si="17"/>
+        <v>3674964186.0465055</v>
+      </c>
       <c r="K589" s="4"/>
-      <c r="L589" s="4"/>
-      <c r="M589" s="4"/>
-      <c r="N589" s="4"/>
+      <c r="L589" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M589" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N589" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O589" s="9"/>
-      <c r="P589" s="4"/>
+      <c r="P589" s="1">
+        <v>374.72868217054202</v>
+      </c>
       <c r="Q589" s="4"/>
       <c r="R589" s="9"/>
       <c r="S589" s="9"/>
       <c r="T589" s="9"/>
     </row>
     <row r="590" spans="1:20" ht="15" customHeight="1">
-      <c r="A590" s="4"/>
-      <c r="B590" s="9"/>
-      <c r="C590" s="4"/>
-      <c r="D590" s="4"/>
+      <c r="A590" s="117" t="s">
+        <v>710</v>
+      </c>
+      <c r="B590" s="110" t="s">
+        <v>705</v>
+      </c>
+      <c r="C590" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D590" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E590" s="9"/>
-      <c r="F590" s="4"/>
-      <c r="G590" s="4"/>
+      <c r="F590" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G590" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H590" s="4"/>
-      <c r="I590" s="4"/>
-      <c r="J590" s="4"/>
+      <c r="I590" s="4">
+        <v>298</v>
+      </c>
+      <c r="J590" s="70">
+        <f t="shared" si="17"/>
+        <v>8507002325.5813923</v>
+      </c>
       <c r="K590" s="4"/>
-      <c r="L590" s="4"/>
-      <c r="M590" s="4"/>
-      <c r="N590" s="4"/>
+      <c r="L590" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M590" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N590" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O590" s="9"/>
-      <c r="P590" s="4"/>
+      <c r="P590" s="9">
+        <v>867.44186046511595</v>
+      </c>
       <c r="Q590" s="4"/>
       <c r="R590" s="9"/>
       <c r="S590" s="9"/>
       <c r="T590" s="9"/>
     </row>
     <row r="591" spans="1:20" ht="15" customHeight="1">
-      <c r="A591" s="4"/>
-      <c r="B591" s="9"/>
-      <c r="C591" s="4"/>
-      <c r="D591" s="4"/>
+      <c r="A591" s="117" t="s">
+        <v>710</v>
+      </c>
+      <c r="B591" s="110" t="s">
+        <v>705</v>
+      </c>
+      <c r="C591" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D591" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E591" s="9"/>
-      <c r="F591" s="4"/>
-      <c r="G591" s="4"/>
+      <c r="F591" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G591" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H591" s="4"/>
-      <c r="I591" s="4"/>
-      <c r="J591" s="4"/>
+      <c r="I591" s="4">
+        <v>573</v>
+      </c>
+      <c r="J591" s="70">
+        <f t="shared" si="17"/>
+        <v>7612968837.2092943</v>
+      </c>
       <c r="K591" s="4"/>
-      <c r="L591" s="4"/>
-      <c r="M591" s="4"/>
-      <c r="N591" s="4"/>
+      <c r="L591" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M591" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N591" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O591" s="9"/>
-      <c r="P591" s="4"/>
+      <c r="P591" s="9">
+        <v>776.279069767441</v>
+      </c>
       <c r="Q591" s="4"/>
       <c r="R591" s="9"/>
       <c r="S591" s="9"/>
       <c r="T591" s="9"/>
     </row>
     <row r="592" spans="1:20" ht="15" customHeight="1">
-      <c r="A592" s="4"/>
-      <c r="B592" s="9"/>
-      <c r="C592" s="4"/>
-      <c r="D592" s="4"/>
+      <c r="A592" s="117" t="s">
+        <v>710</v>
+      </c>
+      <c r="B592" s="110" t="s">
+        <v>705</v>
+      </c>
+      <c r="C592" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D592" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E592" s="9"/>
-      <c r="F592" s="4"/>
-      <c r="G592" s="4"/>
+      <c r="F592" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G592" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H592" s="4"/>
-      <c r="I592" s="4"/>
-      <c r="J592" s="4"/>
+      <c r="I592" s="4">
+        <v>673</v>
+      </c>
+      <c r="J592" s="70">
+        <f t="shared" si="17"/>
+        <v>7304314418.6046448</v>
+      </c>
       <c r="K592" s="4"/>
-      <c r="L592" s="4"/>
-      <c r="M592" s="4"/>
-      <c r="N592" s="4"/>
+      <c r="L592" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M592" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N592" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O592" s="9"/>
-      <c r="P592" s="4"/>
+      <c r="P592" s="9">
+        <v>744.80620155038696</v>
+      </c>
       <c r="Q592" s="4"/>
       <c r="R592" s="9"/>
       <c r="S592" s="9"/>
       <c r="T592" s="9"/>
     </row>
     <row r="593" spans="1:20" ht="15" customHeight="1">
-      <c r="A593" s="4"/>
-      <c r="B593" s="9"/>
-      <c r="C593" s="4"/>
-      <c r="D593" s="4"/>
+      <c r="A593" s="117" t="s">
+        <v>710</v>
+      </c>
+      <c r="B593" s="110" t="s">
+        <v>705</v>
+      </c>
+      <c r="C593" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D593" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E593" s="9"/>
-      <c r="F593" s="4"/>
-      <c r="G593" s="4"/>
+      <c r="F593" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G593" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H593" s="4"/>
-      <c r="I593" s="4"/>
-      <c r="J593" s="4"/>
+      <c r="I593" s="4">
+        <v>773</v>
+      </c>
+      <c r="J593" s="70">
+        <f t="shared" si="17"/>
+        <v>6963730232.5581398</v>
+      </c>
       <c r="K593" s="4"/>
-      <c r="L593" s="4"/>
-      <c r="M593" s="4"/>
-      <c r="N593" s="4"/>
+      <c r="L593" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M593" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N593" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O593" s="9"/>
-      <c r="P593" s="4"/>
+      <c r="P593" s="9">
+        <v>710.07751937984494</v>
+      </c>
       <c r="Q593" s="4"/>
       <c r="R593" s="9"/>
       <c r="S593" s="9"/>
       <c r="T593" s="9"/>
     </row>
     <row r="594" spans="1:20" ht="15" customHeight="1">
-      <c r="A594" s="4"/>
-      <c r="B594" s="9"/>
-      <c r="C594" s="4"/>
-      <c r="D594" s="4"/>
+      <c r="A594" s="117" t="s">
+        <v>710</v>
+      </c>
+      <c r="B594" s="110" t="s">
+        <v>705</v>
+      </c>
+      <c r="C594" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D594" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E594" s="9"/>
-      <c r="F594" s="4"/>
-      <c r="G594" s="4"/>
+      <c r="F594" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G594" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H594" s="4"/>
-      <c r="I594" s="4"/>
-      <c r="J594" s="4"/>
+      <c r="I594" s="4">
+        <v>873</v>
+      </c>
+      <c r="J594" s="70">
+        <f t="shared" si="17"/>
+        <v>7123379069.7674332</v>
+      </c>
       <c r="K594" s="4"/>
-      <c r="L594" s="4"/>
-      <c r="M594" s="4"/>
-      <c r="N594" s="4"/>
+      <c r="L594" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M594" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N594" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O594" s="9"/>
-      <c r="P594" s="4"/>
+      <c r="P594" s="9">
+        <v>726.35658914728594</v>
+      </c>
       <c r="Q594" s="4"/>
       <c r="R594" s="9"/>
       <c r="S594" s="9"/>
       <c r="T594" s="9"/>
     </row>
     <row r="595" spans="1:20" ht="15" customHeight="1">
-      <c r="A595" s="4"/>
-      <c r="B595" s="9"/>
-      <c r="C595" s="4"/>
-      <c r="D595" s="4"/>
+      <c r="A595" s="117" t="s">
+        <v>710</v>
+      </c>
+      <c r="B595" s="110" t="s">
+        <v>705</v>
+      </c>
+      <c r="C595" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D595" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E595" s="9"/>
-      <c r="F595" s="4"/>
-      <c r="G595" s="4"/>
+      <c r="F595" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G595" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H595" s="4"/>
-      <c r="I595" s="4"/>
-      <c r="J595" s="4"/>
+      <c r="I595" s="4">
+        <v>973</v>
+      </c>
+      <c r="J595" s="70">
+        <f t="shared" si="17"/>
+        <v>6644432558.139533</v>
+      </c>
       <c r="K595" s="4"/>
-      <c r="L595" s="4"/>
-      <c r="M595" s="4"/>
-      <c r="N595" s="4"/>
+      <c r="L595" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M595" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N595" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O595" s="9"/>
-      <c r="P595" s="4"/>
+      <c r="P595" s="9">
+        <v>677.51937984496101</v>
+      </c>
       <c r="Q595" s="4"/>
       <c r="R595" s="9"/>
       <c r="S595" s="9"/>
       <c r="T595" s="9"/>
     </row>
     <row r="596" spans="1:20" ht="15" customHeight="1">
-      <c r="A596" s="4"/>
-      <c r="B596" s="9"/>
-      <c r="C596" s="4"/>
-      <c r="D596" s="4"/>
+      <c r="A596" s="117" t="s">
+        <v>710</v>
+      </c>
+      <c r="B596" s="110" t="s">
+        <v>705</v>
+      </c>
+      <c r="C596" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D596" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E596" s="9"/>
-      <c r="F596" s="4"/>
-      <c r="G596" s="4"/>
+      <c r="F596" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G596" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H596" s="4"/>
-      <c r="I596" s="4"/>
-      <c r="J596" s="4"/>
+      <c r="I596" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J596" s="70">
+        <f t="shared" si="17"/>
+        <v>6165486046.5116215</v>
+      </c>
       <c r="K596" s="4"/>
-      <c r="L596" s="4"/>
-      <c r="M596" s="4"/>
-      <c r="N596" s="4"/>
+      <c r="L596" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M596" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N596" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O596" s="9"/>
-      <c r="P596" s="4"/>
+      <c r="P596" s="9">
+        <v>628.68217054263505</v>
+      </c>
       <c r="Q596" s="4"/>
       <c r="R596" s="9"/>
       <c r="S596" s="9"/>
       <c r="T596" s="9"/>
     </row>
     <row r="597" spans="1:20" ht="15" customHeight="1">
-      <c r="A597" s="4"/>
-      <c r="B597" s="9"/>
-      <c r="C597" s="4"/>
-      <c r="D597" s="4"/>
+      <c r="A597" s="117" t="s">
+        <v>710</v>
+      </c>
+      <c r="B597" s="110" t="s">
+        <v>705</v>
+      </c>
+      <c r="C597" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D597" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E597" s="9"/>
-      <c r="F597" s="4"/>
-      <c r="G597" s="4"/>
+      <c r="F597" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G597" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H597" s="4"/>
-      <c r="I597" s="4"/>
-      <c r="J597" s="4"/>
+      <c r="I597" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J597" s="70">
+        <f t="shared" si="17"/>
+        <v>5548177209.3023243</v>
+      </c>
       <c r="K597" s="4"/>
-      <c r="L597" s="4"/>
-      <c r="M597" s="4"/>
-      <c r="N597" s="4"/>
+      <c r="L597" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M597" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N597" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O597" s="9"/>
-      <c r="P597" s="4"/>
+      <c r="P597" s="9">
+        <v>565.73643410852696</v>
+      </c>
       <c r="Q597" s="4"/>
       <c r="R597" s="9"/>
       <c r="S597" s="9"/>
       <c r="T597" s="9"/>
     </row>
     <row r="598" spans="1:20" ht="15" customHeight="1">
-      <c r="A598" s="4"/>
-      <c r="B598" s="9"/>
-      <c r="C598" s="4"/>
-      <c r="D598" s="4"/>
+      <c r="A598" s="117" t="s">
+        <v>710</v>
+      </c>
+      <c r="B598" s="110" t="s">
+        <v>705</v>
+      </c>
+      <c r="C598" s="117" t="s">
+        <v>711</v>
+      </c>
+      <c r="D598" s="117" t="s">
+        <v>113</v>
+      </c>
       <c r="E598" s="9"/>
-      <c r="F598" s="4"/>
-      <c r="G598" s="4"/>
+      <c r="F598" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G598" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H598" s="4"/>
-      <c r="I598" s="4"/>
-      <c r="J598" s="4"/>
+      <c r="I598" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J598" s="70">
+        <f t="shared" si="17"/>
+        <v>4430635348.8372078</v>
+      </c>
       <c r="K598" s="4"/>
-      <c r="L598" s="4"/>
-      <c r="M598" s="4"/>
-      <c r="N598" s="4"/>
+      <c r="L598" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M598" s="117" t="s">
+        <v>247</v>
+      </c>
+      <c r="N598" s="117" t="s">
+        <v>712</v>
+      </c>
       <c r="O598" s="9"/>
-      <c r="P598" s="4"/>
+      <c r="P598" s="9">
+        <v>451.78294573643399</v>
+      </c>
       <c r="Q598" s="4"/>
       <c r="R598" s="9"/>
       <c r="S598" s="9"/>
       <c r="T598" s="9"/>
     </row>
     <row r="599" spans="1:20" ht="15" customHeight="1">
-      <c r="A599" s="68"/>
-      <c r="B599" s="9"/>
-      <c r="C599" s="4"/>
-      <c r="D599" s="4"/>
+      <c r="A599" s="117"/>
+      <c r="B599" s="110"/>
+      <c r="C599" s="117"/>
+      <c r="D599" s="117"/>
       <c r="E599" s="9"/>
-      <c r="F599" s="4"/>
-      <c r="G599" s="4"/>
+      <c r="F599" s="117"/>
+      <c r="G599" s="117"/>
       <c r="H599" s="4"/>
       <c r="I599" s="4"/>
       <c r="J599" s="4"/>
@@ -30378,8 +31512,8 @@
       <c r="C600" s="4"/>
       <c r="D600" s="4"/>
       <c r="E600" s="9"/>
-      <c r="F600" s="4"/>
-      <c r="G600" s="4"/>
+      <c r="F600" s="117"/>
+      <c r="G600" s="117"/>
       <c r="H600" s="4"/>
       <c r="I600" s="4"/>
       <c r="J600" s="4"/>
@@ -30400,8 +31534,8 @@
       <c r="C601" s="4"/>
       <c r="D601" s="4"/>
       <c r="E601" s="9"/>
-      <c r="F601" s="4"/>
-      <c r="G601" s="4"/>
+      <c r="F601" s="117"/>
+      <c r="G601" s="117"/>
       <c r="H601" s="4"/>
       <c r="I601" s="4"/>
       <c r="J601" s="4"/>
@@ -30422,8 +31556,8 @@
       <c r="C602" s="4"/>
       <c r="D602" s="4"/>
       <c r="E602" s="9"/>
-      <c r="F602" s="4"/>
-      <c r="G602" s="4"/>
+      <c r="F602" s="117"/>
+      <c r="G602" s="117"/>
       <c r="H602" s="4"/>
       <c r="I602" s="4"/>
       <c r="J602" s="4"/>
@@ -30444,8 +31578,8 @@
       <c r="C603" s="4"/>
       <c r="D603" s="4"/>
       <c r="E603" s="9"/>
-      <c r="F603" s="4"/>
-      <c r="G603" s="4"/>
+      <c r="F603" s="117"/>
+      <c r="G603" s="117"/>
       <c r="H603" s="4"/>
       <c r="I603" s="4"/>
       <c r="J603" s="4"/>
@@ -30466,8 +31600,8 @@
       <c r="C604" s="4"/>
       <c r="D604" s="4"/>
       <c r="E604" s="9"/>
-      <c r="F604" s="4"/>
-      <c r="G604" s="4"/>
+      <c r="F604" s="117"/>
+      <c r="G604" s="117"/>
       <c r="H604" s="4"/>
       <c r="I604" s="4"/>
       <c r="J604" s="4"/>
@@ -30488,10 +31622,10 @@
       <c r="C605" s="4"/>
       <c r="D605" s="4"/>
       <c r="E605" s="9"/>
-      <c r="F605" s="4"/>
-      <c r="G605" s="4"/>
+      <c r="F605" s="117"/>
+      <c r="G605" s="117"/>
       <c r="H605" s="4"/>
-      <c r="I605" s="83"/>
+      <c r="I605" s="4"/>
       <c r="J605" s="4"/>
       <c r="K605" s="4"/>
       <c r="L605" s="4"/>
@@ -30510,10 +31644,10 @@
       <c r="C606" s="4"/>
       <c r="D606" s="4"/>
       <c r="E606" s="9"/>
-      <c r="F606" s="4"/>
-      <c r="G606" s="4"/>
+      <c r="F606" s="117"/>
+      <c r="G606" s="117"/>
       <c r="H606" s="4"/>
-      <c r="I606" s="83"/>
+      <c r="I606" s="4"/>
       <c r="J606" s="4"/>
       <c r="K606" s="4"/>
       <c r="L606" s="4"/>
@@ -30532,10 +31666,10 @@
       <c r="C607" s="4"/>
       <c r="D607" s="4"/>
       <c r="E607" s="9"/>
-      <c r="F607" s="4"/>
-      <c r="G607" s="4"/>
+      <c r="F607" s="117"/>
+      <c r="G607" s="117"/>
       <c r="H607" s="4"/>
-      <c r="I607" s="83"/>
+      <c r="I607" s="4"/>
       <c r="J607" s="4"/>
       <c r="K607" s="4"/>
       <c r="L607" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jallcom.2015.09.042`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Dec2024.xlsx
+++ b/MiscSmallUploads_Dec2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A1C09A-BF87-4243-B075-F4D41F738D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAC2ED3-1BE6-0B46-83FA-51B053DF9163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8840" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="4460" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5188" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5434" uniqueCount="729">
   <si>
     <r>
       <rPr>
@@ -2269,6 +2269,54 @@
   </si>
   <si>
     <t>10.1016/j.msea.2011.01.072</t>
+  </si>
+  <si>
+    <t>Co1.5CrFeNi1.5Ti0.5</t>
+  </si>
+  <si>
+    <t>Ti05</t>
+  </si>
+  <si>
+    <t>Al01Ti04</t>
+  </si>
+  <si>
+    <t>Al0.1Co1.5CrFeNi1.5Ti0.4</t>
+  </si>
+  <si>
+    <t>Al0.2Co1.5CrFeNi1.5Ti0.3</t>
+  </si>
+  <si>
+    <t>Al02Ti03</t>
+  </si>
+  <si>
+    <t>Al0.3Co1.5CrFeNi1.5Ti0.2</t>
+  </si>
+  <si>
+    <t>Al03Ti02</t>
+  </si>
+  <si>
+    <t>Al05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co1.5CrFeNi1.5Al0.5 </t>
+  </si>
+  <si>
+    <t>AAM+H+WQ+AT</t>
+  </si>
+  <si>
+    <t>homogenized at 1423K for 6h then quenched in water and aged for 50h at 1023K</t>
+  </si>
+  <si>
+    <t>FCC+D024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homogenized at 1423K for 6h then quenched in water and aged for 50h at 1023K; D024 is η-Ni3Ti phase </t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2015.09.042</t>
   </si>
 </sst>
 </file>
@@ -4691,8 +4739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A552" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N606" sqref="N606"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E591" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N626" sqref="N626"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -29881,7 +29929,7 @@
         <v>573</v>
       </c>
       <c r="J564" s="70">
-        <f t="shared" ref="J564:J598" si="17">P564*9807000</f>
+        <f t="shared" ref="J564:J622" si="17">P564*9807000</f>
         <v>5335312093.0232553</v>
       </c>
       <c r="K564" s="4"/>
@@ -31485,548 +31533,1184 @@
       <c r="T598" s="9"/>
     </row>
     <row r="599" spans="1:20" ht="15" customHeight="1">
-      <c r="A599" s="117"/>
-      <c r="B599" s="110"/>
-      <c r="C599" s="117"/>
-      <c r="D599" s="117"/>
-      <c r="E599" s="9"/>
-      <c r="F599" s="117"/>
-      <c r="G599" s="117"/>
+      <c r="A599" s="117" t="s">
+        <v>714</v>
+      </c>
+      <c r="B599" s="110" t="s">
+        <v>713</v>
+      </c>
+      <c r="C599" s="117" t="s">
+        <v>725</v>
+      </c>
+      <c r="D599" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E599" s="119" t="s">
+        <v>726</v>
+      </c>
+      <c r="F599" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G599" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H599" s="4"/>
-      <c r="I599" s="4"/>
-      <c r="J599" s="4"/>
+      <c r="I599" s="4">
+        <v>298</v>
+      </c>
+      <c r="J599" s="70">
+        <f t="shared" si="17"/>
+        <v>5165019999.9999933</v>
+      </c>
       <c r="K599" s="4"/>
-      <c r="L599" s="4"/>
-      <c r="M599" s="4"/>
-      <c r="N599" s="4"/>
+      <c r="L599" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M599" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N599" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O599" s="9"/>
-      <c r="P599" s="4"/>
-      <c r="Q599" s="4"/>
+      <c r="P599" s="4">
+        <v>526.66666666666595</v>
+      </c>
       <c r="R599" s="9"/>
       <c r="S599" s="9"/>
       <c r="T599" s="9"/>
     </row>
     <row r="600" spans="1:20" ht="15" customHeight="1">
-      <c r="A600" s="68"/>
-      <c r="B600" s="9"/>
-      <c r="C600" s="4"/>
-      <c r="D600" s="4"/>
-      <c r="E600" s="9"/>
-      <c r="F600" s="117"/>
-      <c r="G600" s="117"/>
+      <c r="A600" s="117" t="s">
+        <v>714</v>
+      </c>
+      <c r="B600" s="110" t="s">
+        <v>713</v>
+      </c>
+      <c r="C600" s="117" t="s">
+        <v>725</v>
+      </c>
+      <c r="D600" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E600" s="119" t="s">
+        <v>726</v>
+      </c>
+      <c r="F600" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G600" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H600" s="4"/>
-      <c r="I600" s="4"/>
-      <c r="J600" s="4"/>
+      <c r="I600" s="4">
+        <v>773</v>
+      </c>
+      <c r="J600" s="70">
+        <f t="shared" si="17"/>
+        <v>4357213777.7777748</v>
+      </c>
       <c r="K600" s="4"/>
-      <c r="L600" s="4"/>
-      <c r="M600" s="4"/>
-      <c r="N600" s="4"/>
+      <c r="L600" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M600" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N600" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O600" s="9"/>
-      <c r="P600" s="4"/>
-      <c r="Q600" s="4"/>
+      <c r="P600" s="4">
+        <v>444.29629629629602</v>
+      </c>
       <c r="R600" s="9"/>
       <c r="S600" s="9"/>
       <c r="T600" s="9"/>
     </row>
     <row r="601" spans="1:20" ht="15" customHeight="1">
-      <c r="A601" s="68"/>
-      <c r="B601" s="9"/>
-      <c r="C601" s="4"/>
-      <c r="D601" s="4"/>
-      <c r="E601" s="9"/>
-      <c r="F601" s="117"/>
-      <c r="G601" s="117"/>
+      <c r="A601" s="117" t="s">
+        <v>714</v>
+      </c>
+      <c r="B601" s="110" t="s">
+        <v>713</v>
+      </c>
+      <c r="C601" s="117" t="s">
+        <v>725</v>
+      </c>
+      <c r="D601" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E601" s="119" t="s">
+        <v>726</v>
+      </c>
+      <c r="F601" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G601" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H601" s="4"/>
-      <c r="I601" s="4"/>
-      <c r="J601" s="4"/>
+      <c r="I601" s="4">
+        <v>973</v>
+      </c>
+      <c r="J601" s="70">
+        <f t="shared" si="17"/>
+        <v>4101505333.3333311</v>
+      </c>
       <c r="K601" s="4"/>
-      <c r="L601" s="4"/>
-      <c r="M601" s="4"/>
-      <c r="N601" s="4"/>
+      <c r="L601" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M601" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N601" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O601" s="9"/>
-      <c r="P601" s="4"/>
-      <c r="Q601" s="4"/>
+      <c r="P601" s="4">
+        <v>418.222222222222</v>
+      </c>
       <c r="R601" s="9"/>
       <c r="S601" s="9"/>
       <c r="T601" s="9"/>
     </row>
     <row r="602" spans="1:20" ht="15" customHeight="1">
-      <c r="A602" s="68"/>
-      <c r="B602" s="9"/>
-      <c r="C602" s="4"/>
-      <c r="D602" s="4"/>
-      <c r="E602" s="9"/>
-      <c r="F602" s="117"/>
-      <c r="G602" s="117"/>
+      <c r="A602" s="117" t="s">
+        <v>714</v>
+      </c>
+      <c r="B602" s="110" t="s">
+        <v>713</v>
+      </c>
+      <c r="C602" s="117" t="s">
+        <v>725</v>
+      </c>
+      <c r="D602" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E602" s="119" t="s">
+        <v>726</v>
+      </c>
+      <c r="F602" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G602" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H602" s="4"/>
-      <c r="I602" s="4"/>
-      <c r="J602" s="4"/>
+      <c r="I602" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J602" s="70">
+        <f t="shared" si="17"/>
+        <v>3810927555.5555496</v>
+      </c>
       <c r="K602" s="4"/>
-      <c r="L602" s="4"/>
-      <c r="M602" s="4"/>
-      <c r="N602" s="4"/>
+      <c r="L602" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M602" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N602" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O602" s="9"/>
-      <c r="P602" s="4"/>
-      <c r="Q602" s="4"/>
+      <c r="P602" s="4">
+        <v>388.59259259259198</v>
+      </c>
       <c r="R602" s="9"/>
       <c r="S602" s="9"/>
       <c r="T602" s="9"/>
     </row>
     <row r="603" spans="1:20" ht="15" customHeight="1">
-      <c r="A603" s="68"/>
-      <c r="B603" s="9"/>
-      <c r="C603" s="4"/>
-      <c r="D603" s="4"/>
-      <c r="E603" s="9"/>
-      <c r="F603" s="117"/>
-      <c r="G603" s="117"/>
+      <c r="A603" s="117" t="s">
+        <v>714</v>
+      </c>
+      <c r="B603" s="110" t="s">
+        <v>713</v>
+      </c>
+      <c r="C603" s="117" t="s">
+        <v>725</v>
+      </c>
+      <c r="D603" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E603" s="119" t="s">
+        <v>726</v>
+      </c>
+      <c r="F603" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G603" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H603" s="4"/>
-      <c r="I603" s="4"/>
-      <c r="J603" s="4"/>
+      <c r="I603" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J603" s="70">
+        <f t="shared" si="17"/>
+        <v>3421553333.3333244</v>
+      </c>
       <c r="K603" s="4"/>
-      <c r="L603" s="4"/>
-      <c r="M603" s="4"/>
-      <c r="N603" s="4"/>
+      <c r="L603" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M603" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N603" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O603" s="9"/>
-      <c r="P603" s="4"/>
-      <c r="Q603" s="4"/>
+      <c r="P603" s="4">
+        <v>348.888888888888</v>
+      </c>
       <c r="R603" s="9"/>
       <c r="S603" s="9"/>
       <c r="T603" s="9"/>
     </row>
     <row r="604" spans="1:20" ht="15" customHeight="1">
-      <c r="A604" s="68"/>
-      <c r="B604" s="9"/>
-      <c r="C604" s="4"/>
-      <c r="D604" s="4"/>
-      <c r="E604" s="9"/>
-      <c r="F604" s="117"/>
-      <c r="G604" s="117"/>
+      <c r="A604" s="117" t="s">
+        <v>714</v>
+      </c>
+      <c r="B604" s="110" t="s">
+        <v>713</v>
+      </c>
+      <c r="C604" s="117" t="s">
+        <v>725</v>
+      </c>
+      <c r="D604" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E604" s="119" t="s">
+        <v>726</v>
+      </c>
+      <c r="F604" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G604" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H604" s="4"/>
-      <c r="I604" s="4"/>
-      <c r="J604" s="4"/>
+      <c r="I604" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J604" s="70">
+        <f t="shared" si="17"/>
+        <v>2631181777.7777753</v>
+      </c>
       <c r="K604" s="4"/>
-      <c r="L604" s="4"/>
-      <c r="M604" s="4"/>
-      <c r="N604" s="4"/>
+      <c r="L604" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M604" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N604" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O604" s="9"/>
-      <c r="P604" s="4"/>
-      <c r="Q604" s="4"/>
+      <c r="P604" s="4">
+        <v>268.29629629629602</v>
+      </c>
       <c r="R604" s="9"/>
       <c r="S604" s="9"/>
       <c r="T604" s="9"/>
     </row>
     <row r="605" spans="1:20" ht="15" customHeight="1">
-      <c r="A605" s="68"/>
-      <c r="B605" s="9"/>
-      <c r="C605" s="4"/>
-      <c r="D605" s="4"/>
-      <c r="E605" s="9"/>
-      <c r="F605" s="117"/>
-      <c r="G605" s="117"/>
+      <c r="A605" s="111" t="s">
+        <v>715</v>
+      </c>
+      <c r="B605" s="119" t="s">
+        <v>716</v>
+      </c>
+      <c r="C605" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D605" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E605" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F605" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G605" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H605" s="4"/>
-      <c r="I605" s="4"/>
-      <c r="J605" s="4"/>
+      <c r="I605" s="4">
+        <v>298</v>
+      </c>
+      <c r="J605" s="70">
+        <f t="shared" si="17"/>
+        <v>4351402222.2222157</v>
+      </c>
       <c r="K605" s="4"/>
-      <c r="L605" s="4"/>
-      <c r="M605" s="4"/>
-      <c r="N605" s="4"/>
+      <c r="L605" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M605" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N605" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O605" s="9"/>
-      <c r="P605" s="4"/>
-      <c r="Q605" s="4"/>
+      <c r="P605" s="4">
+        <v>443.70370370370301</v>
+      </c>
       <c r="R605" s="9"/>
       <c r="S605" s="9"/>
       <c r="T605" s="9"/>
     </row>
     <row r="606" spans="1:20" ht="15" customHeight="1">
-      <c r="A606" s="68"/>
-      <c r="B606" s="9"/>
-      <c r="C606" s="4"/>
-      <c r="D606" s="4"/>
-      <c r="E606" s="9"/>
-      <c r="F606" s="117"/>
-      <c r="G606" s="117"/>
+      <c r="A606" s="111" t="s">
+        <v>715</v>
+      </c>
+      <c r="B606" s="119" t="s">
+        <v>716</v>
+      </c>
+      <c r="C606" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D606" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E606" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F606" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G606" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H606" s="4"/>
-      <c r="I606" s="4"/>
-      <c r="J606" s="4"/>
+      <c r="I606" s="4">
+        <v>773</v>
+      </c>
+      <c r="J606" s="70">
+        <f t="shared" si="17"/>
+        <v>3828362222.2222185</v>
+      </c>
       <c r="K606" s="4"/>
-      <c r="L606" s="4"/>
-      <c r="M606" s="4"/>
-      <c r="N606" s="4"/>
+      <c r="L606" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M606" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N606" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O606" s="9"/>
-      <c r="P606" s="4"/>
-      <c r="Q606" s="4"/>
+      <c r="P606" s="4">
+        <v>390.37037037036998</v>
+      </c>
       <c r="R606" s="9"/>
       <c r="S606" s="9"/>
       <c r="T606" s="9"/>
     </row>
     <row r="607" spans="1:20" ht="15" customHeight="1">
-      <c r="A607" s="68"/>
-      <c r="B607" s="9"/>
-      <c r="C607" s="4"/>
-      <c r="D607" s="4"/>
-      <c r="E607" s="9"/>
-      <c r="F607" s="117"/>
-      <c r="G607" s="117"/>
+      <c r="A607" s="111" t="s">
+        <v>715</v>
+      </c>
+      <c r="B607" s="119" t="s">
+        <v>716</v>
+      </c>
+      <c r="C607" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D607" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E607" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F607" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G607" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H607" s="4"/>
-      <c r="I607" s="4"/>
-      <c r="J607" s="4"/>
+      <c r="I607" s="4">
+        <v>973</v>
+      </c>
+      <c r="J607" s="70">
+        <f t="shared" si="17"/>
+        <v>3473857333.3333311</v>
+      </c>
       <c r="K607" s="4"/>
-      <c r="L607" s="4"/>
-      <c r="M607" s="4"/>
-      <c r="N607" s="4"/>
+      <c r="L607" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M607" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N607" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O607" s="9"/>
-      <c r="P607" s="4"/>
-      <c r="Q607" s="4"/>
+      <c r="P607" s="4">
+        <v>354.222222222222</v>
+      </c>
       <c r="R607" s="9"/>
       <c r="S607" s="9"/>
       <c r="T607" s="9"/>
     </row>
     <row r="608" spans="1:20" ht="15" customHeight="1">
-      <c r="A608" s="68"/>
-      <c r="B608" s="9"/>
-      <c r="C608" s="4"/>
-      <c r="D608" s="4"/>
-      <c r="E608" s="9"/>
-      <c r="F608" s="4"/>
-      <c r="G608" s="4"/>
+      <c r="A608" s="111" t="s">
+        <v>715</v>
+      </c>
+      <c r="B608" s="119" t="s">
+        <v>716</v>
+      </c>
+      <c r="C608" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D608" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E608" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F608" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G608" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H608" s="4"/>
-      <c r="I608" s="83"/>
-      <c r="J608" s="4"/>
+      <c r="I608" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J608" s="70">
+        <f t="shared" si="17"/>
+        <v>3392495555.5555563</v>
+      </c>
       <c r="K608" s="4"/>
-      <c r="L608" s="4"/>
-      <c r="M608" s="4"/>
-      <c r="N608" s="4"/>
+      <c r="L608" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M608" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N608" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O608" s="9"/>
-      <c r="P608" s="4"/>
-      <c r="Q608" s="4"/>
+      <c r="P608" s="4">
+        <v>345.92592592592598</v>
+      </c>
       <c r="R608" s="9"/>
       <c r="S608" s="9"/>
       <c r="T608" s="9"/>
     </row>
     <row r="609" spans="1:20" ht="15" customHeight="1">
-      <c r="A609" s="68"/>
-      <c r="B609" s="9"/>
-      <c r="C609" s="4"/>
-      <c r="D609" s="4"/>
-      <c r="E609" s="9"/>
-      <c r="F609" s="4"/>
-      <c r="G609" s="4"/>
+      <c r="A609" s="111" t="s">
+        <v>715</v>
+      </c>
+      <c r="B609" s="119" t="s">
+        <v>716</v>
+      </c>
+      <c r="C609" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D609" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E609" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F609" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G609" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H609" s="4"/>
-      <c r="I609" s="83"/>
-      <c r="J609" s="4"/>
+      <c r="I609" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J609" s="70">
+        <f t="shared" si="17"/>
+        <v>2770659111.1111064</v>
+      </c>
       <c r="K609" s="4"/>
-      <c r="L609" s="4"/>
-      <c r="M609" s="4"/>
-      <c r="N609" s="4"/>
+      <c r="L609" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M609" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N609" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O609" s="9"/>
-      <c r="P609" s="4"/>
-      <c r="Q609" s="4"/>
+      <c r="P609" s="4">
+        <v>282.51851851851802</v>
+      </c>
       <c r="R609" s="9"/>
       <c r="S609" s="9"/>
       <c r="T609" s="9"/>
     </row>
     <row r="610" spans="1:20" ht="15" customHeight="1">
-      <c r="A610" s="68"/>
-      <c r="B610" s="9"/>
-      <c r="C610" s="4"/>
-      <c r="D610" s="4"/>
-      <c r="E610" s="9"/>
-      <c r="F610" s="4"/>
-      <c r="G610" s="4"/>
+      <c r="A610" s="111" t="s">
+        <v>715</v>
+      </c>
+      <c r="B610" s="119" t="s">
+        <v>716</v>
+      </c>
+      <c r="C610" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D610" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E610" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F610" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G610" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H610" s="4"/>
-      <c r="I610" s="83"/>
-      <c r="J610" s="4"/>
+      <c r="I610" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J610" s="70">
+        <f t="shared" si="17"/>
+        <v>2183691999.9999933</v>
+      </c>
       <c r="K610" s="4"/>
-      <c r="L610" s="4"/>
-      <c r="M610" s="4"/>
-      <c r="N610" s="4"/>
+      <c r="L610" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M610" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N610" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O610" s="9"/>
-      <c r="P610" s="4"/>
-      <c r="Q610" s="4"/>
+      <c r="P610" s="4">
+        <v>222.666666666666</v>
+      </c>
       <c r="R610" s="9"/>
       <c r="S610" s="9"/>
       <c r="T610" s="9"/>
     </row>
     <row r="611" spans="1:20" ht="15" customHeight="1">
-      <c r="A611" s="68"/>
-      <c r="B611" s="9"/>
-      <c r="C611" s="4"/>
-      <c r="D611" s="4"/>
-      <c r="E611" s="9"/>
-      <c r="F611" s="4"/>
-      <c r="G611" s="4"/>
+      <c r="A611" s="111" t="s">
+        <v>718</v>
+      </c>
+      <c r="B611" s="119" t="s">
+        <v>717</v>
+      </c>
+      <c r="C611" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D611" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E611" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F611" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G611" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H611" s="4"/>
-      <c r="I611" s="83"/>
-      <c r="J611" s="4"/>
+      <c r="I611" s="4">
+        <v>298</v>
+      </c>
+      <c r="J611" s="70">
+        <f t="shared" si="17"/>
+        <v>3508726666.6666589</v>
+      </c>
       <c r="K611" s="4"/>
-      <c r="L611" s="4"/>
-      <c r="M611" s="4"/>
-      <c r="N611" s="4"/>
+      <c r="L611" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M611" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N611" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O611" s="9"/>
-      <c r="P611" s="4"/>
-      <c r="Q611" s="4"/>
+      <c r="P611" s="4">
+        <v>357.77777777777698</v>
+      </c>
       <c r="R611" s="9"/>
       <c r="S611" s="9"/>
       <c r="T611" s="9"/>
     </row>
     <row r="612" spans="1:20" ht="15" customHeight="1">
-      <c r="A612" s="68"/>
-      <c r="B612" s="9"/>
-      <c r="C612" s="4"/>
-      <c r="D612" s="4"/>
-      <c r="E612" s="9"/>
-      <c r="F612" s="4"/>
-      <c r="G612" s="4"/>
+      <c r="A612" s="111" t="s">
+        <v>718</v>
+      </c>
+      <c r="B612" s="119" t="s">
+        <v>717</v>
+      </c>
+      <c r="C612" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D612" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E612" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F612" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G612" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H612" s="4"/>
-      <c r="I612" s="83"/>
-      <c r="J612" s="4"/>
+      <c r="I612" s="4">
+        <v>773</v>
+      </c>
+      <c r="J612" s="70">
+        <f t="shared" si="17"/>
+        <v>2968251999.9999933</v>
+      </c>
       <c r="K612" s="4"/>
-      <c r="L612" s="4"/>
-      <c r="M612" s="4"/>
-      <c r="N612" s="4"/>
+      <c r="L612" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M612" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N612" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O612" s="9"/>
-      <c r="P612" s="4"/>
-      <c r="Q612" s="4"/>
+      <c r="P612" s="4">
+        <v>302.666666666666</v>
+      </c>
       <c r="R612" s="9"/>
       <c r="S612" s="9"/>
       <c r="T612" s="9"/>
     </row>
     <row r="613" spans="1:20" ht="15" customHeight="1">
-      <c r="A613" s="68"/>
-      <c r="B613" s="9"/>
-      <c r="C613" s="4"/>
-      <c r="D613" s="4"/>
-      <c r="E613" s="9"/>
-      <c r="F613" s="4"/>
-      <c r="G613" s="4"/>
+      <c r="A613" s="111" t="s">
+        <v>718</v>
+      </c>
+      <c r="B613" s="119" t="s">
+        <v>717</v>
+      </c>
+      <c r="C613" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D613" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E613" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F613" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G613" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H613" s="4"/>
-      <c r="I613" s="83"/>
-      <c r="J613" s="4"/>
+      <c r="I613" s="4">
+        <v>973</v>
+      </c>
+      <c r="J613" s="70">
+        <f t="shared" si="17"/>
+        <v>2625370222.2222157</v>
+      </c>
       <c r="K613" s="4"/>
-      <c r="L613" s="4"/>
-      <c r="M613" s="4"/>
-      <c r="N613" s="4"/>
+      <c r="L613" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M613" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N613" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O613" s="9"/>
-      <c r="P613" s="4"/>
-      <c r="Q613" s="4"/>
+      <c r="P613" s="4">
+        <v>267.70370370370301</v>
+      </c>
       <c r="R613" s="9"/>
       <c r="S613" s="9"/>
       <c r="T613" s="9"/>
     </row>
     <row r="614" spans="1:20" ht="15" customHeight="1">
-      <c r="A614" s="68"/>
-      <c r="B614" s="9"/>
-      <c r="C614" s="4"/>
-      <c r="D614" s="4"/>
-      <c r="E614" s="9"/>
-      <c r="F614" s="4"/>
-      <c r="G614" s="4"/>
+      <c r="A614" s="111" t="s">
+        <v>718</v>
+      </c>
+      <c r="B614" s="119" t="s">
+        <v>717</v>
+      </c>
+      <c r="C614" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D614" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E614" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F614" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G614" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H614" s="4"/>
-      <c r="I614" s="83"/>
-      <c r="J614" s="4"/>
+      <c r="I614" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J614" s="70">
+        <f t="shared" si="17"/>
+        <v>2468458222.2222157</v>
+      </c>
       <c r="K614" s="4"/>
-      <c r="L614" s="4"/>
-      <c r="M614" s="4"/>
-      <c r="N614" s="4"/>
+      <c r="L614" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M614" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N614" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O614" s="9"/>
-      <c r="P614" s="4"/>
-      <c r="Q614" s="4"/>
+      <c r="P614" s="4">
+        <v>251.70370370370301</v>
+      </c>
       <c r="R614" s="9"/>
       <c r="S614" s="9"/>
       <c r="T614" s="9"/>
     </row>
     <row r="615" spans="1:20" ht="15" customHeight="1">
-      <c r="A615" s="68"/>
-      <c r="B615" s="9"/>
-      <c r="C615" s="4"/>
-      <c r="D615" s="4"/>
-      <c r="E615" s="9"/>
-      <c r="F615" s="4"/>
-      <c r="G615" s="4"/>
+      <c r="A615" s="111" t="s">
+        <v>718</v>
+      </c>
+      <c r="B615" s="119" t="s">
+        <v>717</v>
+      </c>
+      <c r="C615" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D615" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E615" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F615" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G615" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H615" s="4"/>
-      <c r="I615" s="83"/>
-      <c r="J615" s="4"/>
+      <c r="I615" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J615" s="70">
+        <f t="shared" si="17"/>
+        <v>2299923111.1111059</v>
+      </c>
       <c r="K615" s="4"/>
-      <c r="L615" s="4"/>
-      <c r="M615" s="4"/>
-      <c r="N615" s="4"/>
+      <c r="L615" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M615" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N615" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O615" s="9"/>
-      <c r="P615" s="4"/>
-      <c r="Q615" s="4"/>
+      <c r="P615" s="4">
+        <v>234.51851851851799</v>
+      </c>
       <c r="R615" s="9"/>
       <c r="S615" s="9"/>
       <c r="T615" s="9"/>
     </row>
     <row r="616" spans="1:20" ht="15" customHeight="1">
-      <c r="A616" s="68"/>
-      <c r="B616" s="9"/>
-      <c r="C616" s="4"/>
-      <c r="D616" s="4"/>
-      <c r="E616" s="9"/>
-      <c r="F616" s="4"/>
-      <c r="G616" s="4"/>
+      <c r="A616" s="111" t="s">
+        <v>718</v>
+      </c>
+      <c r="B616" s="119" t="s">
+        <v>717</v>
+      </c>
+      <c r="C616" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D616" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E616" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F616" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G616" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H616" s="4"/>
-      <c r="I616" s="83"/>
-      <c r="J616" s="4"/>
+      <c r="I616" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J616" s="70">
+        <f t="shared" si="17"/>
+        <v>1649028888.8888876</v>
+      </c>
       <c r="K616" s="4"/>
-      <c r="L616" s="4"/>
-      <c r="M616" s="4"/>
-      <c r="N616" s="4"/>
+      <c r="L616" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M616" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N616" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O616" s="9"/>
-      <c r="P616" s="4"/>
-      <c r="Q616" s="4"/>
+      <c r="P616" s="4">
+        <v>168.14814814814801</v>
+      </c>
       <c r="R616" s="9"/>
       <c r="S616" s="9"/>
       <c r="T616" s="9"/>
     </row>
     <row r="617" spans="1:20" ht="15" customHeight="1">
-      <c r="A617" s="68"/>
-      <c r="B617" s="9"/>
-      <c r="C617" s="4"/>
-      <c r="D617" s="4"/>
-      <c r="E617" s="9"/>
-      <c r="F617" s="4"/>
-      <c r="G617" s="4"/>
+      <c r="A617" s="111" t="s">
+        <v>720</v>
+      </c>
+      <c r="B617" s="119" t="s">
+        <v>719</v>
+      </c>
+      <c r="C617" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D617" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E617" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F617" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G617" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H617" s="4"/>
-      <c r="I617" s="83"/>
-      <c r="J617" s="4"/>
+      <c r="I617" s="4">
+        <v>298</v>
+      </c>
+      <c r="J617" s="70">
+        <f t="shared" si="17"/>
+        <v>3008932888.8888807</v>
+      </c>
       <c r="K617" s="4"/>
-      <c r="L617" s="4"/>
-      <c r="M617" s="4"/>
-      <c r="N617" s="4"/>
+      <c r="L617" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M617" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N617" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O617" s="9"/>
-      <c r="P617" s="4"/>
-      <c r="Q617" s="4"/>
+      <c r="P617" s="4">
+        <v>306.81481481481399</v>
+      </c>
       <c r="R617" s="9"/>
       <c r="S617" s="9"/>
       <c r="T617" s="9"/>
     </row>
     <row r="618" spans="1:20" ht="15" customHeight="1">
-      <c r="A618" s="68"/>
-      <c r="B618" s="9"/>
-      <c r="C618" s="4"/>
-      <c r="D618" s="4"/>
-      <c r="E618" s="9"/>
-      <c r="F618" s="4"/>
-      <c r="G618" s="4"/>
+      <c r="A618" s="111" t="s">
+        <v>720</v>
+      </c>
+      <c r="B618" s="119" t="s">
+        <v>719</v>
+      </c>
+      <c r="C618" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D618" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E618" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F618" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G618" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H618" s="4"/>
-      <c r="I618" s="83"/>
-      <c r="J618" s="4"/>
+      <c r="I618" s="4">
+        <v>773</v>
+      </c>
+      <c r="J618" s="70">
+        <f t="shared" si="17"/>
+        <v>2503327555.555553</v>
+      </c>
       <c r="K618" s="4"/>
-      <c r="L618" s="4"/>
-      <c r="M618" s="4"/>
-      <c r="N618" s="4"/>
+      <c r="L618" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M618" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N618" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O618" s="9"/>
-      <c r="P618" s="4"/>
-      <c r="Q618" s="4"/>
+      <c r="P618" s="4">
+        <v>255.25925925925901</v>
+      </c>
       <c r="R618" s="9"/>
       <c r="S618" s="9"/>
       <c r="T618" s="9"/>
     </row>
     <row r="619" spans="1:20" ht="15" customHeight="1">
-      <c r="A619" s="68"/>
-      <c r="B619" s="9"/>
-      <c r="C619" s="4"/>
-      <c r="D619" s="4"/>
-      <c r="E619" s="9"/>
-      <c r="F619" s="4"/>
-      <c r="G619" s="4"/>
+      <c r="A619" s="111" t="s">
+        <v>720</v>
+      </c>
+      <c r="B619" s="119" t="s">
+        <v>719</v>
+      </c>
+      <c r="C619" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D619" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E619" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F619" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G619" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H619" s="4"/>
-      <c r="I619" s="83"/>
-      <c r="J619" s="4"/>
+      <c r="I619" s="4">
+        <v>973</v>
+      </c>
+      <c r="J619" s="70">
+        <f t="shared" si="17"/>
+        <v>2352227111.1111026</v>
+      </c>
       <c r="K619" s="4"/>
-      <c r="L619" s="4"/>
-      <c r="M619" s="4"/>
-      <c r="N619" s="4"/>
+      <c r="L619" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M619" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N619" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O619" s="9"/>
-      <c r="P619" s="4"/>
-      <c r="Q619" s="4"/>
+      <c r="P619" s="4">
+        <v>239.85185185185099</v>
+      </c>
       <c r="R619" s="9"/>
       <c r="S619" s="9"/>
       <c r="T619" s="9"/>
     </row>
     <row r="620" spans="1:20" ht="15" customHeight="1">
-      <c r="A620" s="68"/>
-      <c r="B620" s="9"/>
-      <c r="C620" s="4"/>
-      <c r="D620" s="4"/>
-      <c r="E620" s="9"/>
-      <c r="F620" s="4"/>
-      <c r="G620" s="4"/>
+      <c r="A620" s="111" t="s">
+        <v>720</v>
+      </c>
+      <c r="B620" s="119" t="s">
+        <v>719</v>
+      </c>
+      <c r="C620" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D620" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E620" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F620" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G620" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H620" s="4"/>
-      <c r="I620" s="83"/>
-      <c r="J620" s="4"/>
+      <c r="I620" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J620" s="70">
+        <f t="shared" si="17"/>
+        <v>1957041333.333328</v>
+      </c>
       <c r="K620" s="4"/>
-      <c r="L620" s="4"/>
-      <c r="M620" s="4"/>
-      <c r="N620" s="4"/>
+      <c r="L620" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M620" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N620" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O620" s="9"/>
-      <c r="P620" s="4"/>
-      <c r="Q620" s="4"/>
+      <c r="P620" s="4">
+        <v>199.555555555555</v>
+      </c>
       <c r="R620" s="9"/>
       <c r="S620" s="9"/>
       <c r="T620" s="9"/>
     </row>
     <row r="621" spans="1:20" ht="15" customHeight="1">
-      <c r="A621" s="68"/>
-      <c r="B621" s="9"/>
-      <c r="C621" s="4"/>
-      <c r="D621" s="4"/>
-      <c r="E621" s="9"/>
-      <c r="F621" s="4"/>
-      <c r="G621" s="4"/>
+      <c r="A621" s="111" t="s">
+        <v>720</v>
+      </c>
+      <c r="B621" s="119" t="s">
+        <v>719</v>
+      </c>
+      <c r="C621" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D621" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E621" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F621" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G621" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H621" s="4"/>
-      <c r="I621" s="83"/>
-      <c r="J621" s="4"/>
+      <c r="I621" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J621" s="70">
+        <f t="shared" si="17"/>
+        <v>1538609333.3333247</v>
+      </c>
       <c r="K621" s="4"/>
-      <c r="L621" s="4"/>
-      <c r="M621" s="4"/>
-      <c r="N621" s="4"/>
+      <c r="L621" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M621" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N621" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O621" s="9"/>
-      <c r="P621" s="4"/>
-      <c r="Q621" s="4"/>
+      <c r="P621" s="4">
+        <v>156.888888888888</v>
+      </c>
       <c r="R621" s="9"/>
       <c r="S621" s="9"/>
       <c r="T621" s="9"/>
     </row>
     <row r="622" spans="1:20" ht="15" customHeight="1">
-      <c r="A622" s="68"/>
-      <c r="B622" s="9"/>
-      <c r="C622" s="4"/>
-      <c r="D622" s="4"/>
-      <c r="E622" s="9"/>
-      <c r="F622" s="4"/>
-      <c r="G622" s="4"/>
+      <c r="A622" s="111" t="s">
+        <v>720</v>
+      </c>
+      <c r="B622" s="119" t="s">
+        <v>719</v>
+      </c>
+      <c r="C622" s="117" t="s">
+        <v>287</v>
+      </c>
+      <c r="D622" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E622" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F622" s="117" t="s">
+        <v>77</v>
+      </c>
+      <c r="G622" s="117" t="s">
+        <v>29</v>
+      </c>
       <c r="H622" s="4"/>
-      <c r="I622" s="83"/>
-      <c r="J622" s="4"/>
+      <c r="I622" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J622" s="70">
+        <f t="shared" si="17"/>
+        <v>870280444.44444501</v>
+      </c>
       <c r="K622" s="4"/>
-      <c r="L622" s="4"/>
-      <c r="M622" s="4"/>
-      <c r="N622" s="4"/>
+      <c r="L622" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M622" s="117" t="s">
+        <v>727</v>
+      </c>
+      <c r="N622" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O622" s="9"/>
-      <c r="P622" s="4"/>
-      <c r="Q622" s="4"/>
+      <c r="P622" s="4">
+        <v>88.740740740740804</v>
+      </c>
       <c r="R622" s="9"/>
       <c r="S622" s="9"/>
       <c r="T622" s="9"/>
     </row>
     <row r="623" spans="1:20" ht="15" customHeight="1">
-      <c r="A623" s="4"/>
-      <c r="B623" s="9"/>
-      <c r="C623" s="4"/>
-      <c r="D623" s="4"/>
-      <c r="E623" s="9"/>
-      <c r="F623" s="4"/>
-      <c r="G623" s="4"/>
+      <c r="A623" s="117" t="s">
+        <v>721</v>
+      </c>
+      <c r="B623" s="119" t="s">
+        <v>722</v>
+      </c>
+      <c r="C623" s="117" t="s">
+        <v>83</v>
+      </c>
+      <c r="D623" s="117" t="s">
+        <v>723</v>
+      </c>
+      <c r="E623" s="119" t="s">
+        <v>724</v>
+      </c>
+      <c r="F623" s="117"/>
+      <c r="G623" s="117"/>
       <c r="H623" s="4"/>
       <c r="I623" s="4"/>
       <c r="J623" s="4"/>
       <c r="K623" s="4"/>
       <c r="L623" s="4"/>
       <c r="M623" s="4"/>
-      <c r="N623" s="4"/>
+      <c r="N623" s="117" t="s">
+        <v>728</v>
+      </c>
       <c r="O623" s="9"/>
       <c r="P623" s="4"/>
       <c r="Q623" s="4"/>
@@ -32035,13 +32719,13 @@
       <c r="T623" s="9"/>
     </row>
     <row r="624" spans="1:20" ht="15" customHeight="1">
-      <c r="A624" s="4"/>
-      <c r="B624" s="9"/>
-      <c r="C624" s="4"/>
-      <c r="D624" s="4"/>
-      <c r="E624" s="9"/>
-      <c r="F624" s="4"/>
-      <c r="G624" s="4"/>
+      <c r="A624" s="117"/>
+      <c r="B624" s="119"/>
+      <c r="C624" s="117"/>
+      <c r="D624" s="117"/>
+      <c r="E624" s="119"/>
+      <c r="F624" s="117"/>
+      <c r="G624" s="117"/>
       <c r="H624" s="4"/>
       <c r="I624" s="4"/>
       <c r="J624" s="4"/>
@@ -32057,13 +32741,13 @@
       <c r="T624" s="9"/>
     </row>
     <row r="625" spans="1:20" ht="15" customHeight="1">
-      <c r="A625" s="4"/>
-      <c r="B625" s="9"/>
-      <c r="C625" s="4"/>
-      <c r="D625" s="4"/>
-      <c r="E625" s="9"/>
-      <c r="F625" s="4"/>
-      <c r="G625" s="4"/>
+      <c r="A625" s="117"/>
+      <c r="B625" s="119"/>
+      <c r="C625" s="117"/>
+      <c r="D625" s="117"/>
+      <c r="E625" s="119"/>
+      <c r="F625" s="117"/>
+      <c r="G625" s="117"/>
       <c r="H625" s="4"/>
       <c r="I625" s="4"/>
       <c r="J625" s="4"/>
@@ -32079,13 +32763,13 @@
       <c r="T625" s="9"/>
     </row>
     <row r="626" spans="1:20" ht="15" customHeight="1">
-      <c r="A626" s="4"/>
-      <c r="B626" s="9"/>
-      <c r="C626" s="4"/>
-      <c r="D626" s="4"/>
-      <c r="E626" s="9"/>
-      <c r="F626" s="4"/>
-      <c r="G626" s="4"/>
+      <c r="A626" s="117"/>
+      <c r="B626" s="119"/>
+      <c r="C626" s="117"/>
+      <c r="D626" s="117"/>
+      <c r="E626" s="119"/>
+      <c r="F626" s="117"/>
+      <c r="G626" s="117"/>
       <c r="H626" s="4"/>
       <c r="I626" s="4"/>
       <c r="J626" s="4"/>
@@ -32101,13 +32785,13 @@
       <c r="T626" s="9"/>
     </row>
     <row r="627" spans="1:20" ht="15" customHeight="1">
-      <c r="A627" s="4"/>
-      <c r="B627" s="9"/>
-      <c r="C627" s="4"/>
-      <c r="D627" s="4"/>
-      <c r="E627" s="9"/>
-      <c r="F627" s="4"/>
-      <c r="G627" s="4"/>
+      <c r="A627" s="117"/>
+      <c r="B627" s="119"/>
+      <c r="C627" s="117"/>
+      <c r="D627" s="117"/>
+      <c r="E627" s="119"/>
+      <c r="F627" s="117"/>
+      <c r="G627" s="117"/>
       <c r="H627" s="4"/>
       <c r="I627" s="4"/>
       <c r="J627" s="4"/>
@@ -32123,13 +32807,13 @@
       <c r="T627" s="9"/>
     </row>
     <row r="628" spans="1:20" ht="15" customHeight="1">
-      <c r="A628" s="4"/>
-      <c r="B628" s="9"/>
-      <c r="C628" s="4"/>
-      <c r="D628" s="4"/>
-      <c r="E628" s="9"/>
-      <c r="F628" s="4"/>
-      <c r="G628" s="4"/>
+      <c r="A628" s="117"/>
+      <c r="B628" s="119"/>
+      <c r="C628" s="117"/>
+      <c r="D628" s="117"/>
+      <c r="E628" s="119"/>
+      <c r="F628" s="117"/>
+      <c r="G628" s="117"/>
       <c r="H628" s="4"/>
       <c r="I628" s="4"/>
       <c r="J628" s="4"/>

</xml_diff>